<commit_message>
Update CDC Press and COVID-19 Statistic on 20210629
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Press Title</t>
   </si>
@@ -31,13 +31,25 @@
     <t>Page Content</t>
   </si>
   <si>
+    <t>簡訊實聯制數據係以合法性、正當性、必要性進行使用，絕無違法情事</t>
+  </si>
+  <si>
+    <t>針對媒體報導「COVID-19疫苗接種外展服務，無法選擇疫苗廠牌，係為國產疫苗鋪路」 指揮中心澄清並非事實</t>
+  </si>
+  <si>
+    <t>新增54例COVID-19確定病例，均為本土個案</t>
+  </si>
+  <si>
+    <t>6月29日全國防疫會議後記者會報告</t>
+  </si>
+  <si>
     <t>新增60例COVID-19確定病例，均為本土個案</t>
   </si>
   <si>
     <t>本島各機場前往離島自願快篩而呈陽性反應之旅客，將進行PCR採檢陰性後，始允許登機</t>
   </si>
   <si>
-    <t>全球Delta變異株流行，即日起，入境旅客自機場前往檢疫地點應搭乘防疫車輛</t>
+    <t>全球Delta變異株流行，即日起，入境人士前往檢疫地點應搭乘防疫車輛</t>
   </si>
   <si>
     <t>網傳「mRNA疫苗會使接種者變成轉基因生物體」，指揮中心：疫苗品質安全把關，民眾用藥有保障</t>
@@ -49,16 +61,16 @@
     <t>指揮中心說明274萬劑莫德納(Moderna) COVID-19疫苗第一階段分配事宜</t>
   </si>
   <si>
-    <t>因應屏東Delta印度變異株群聚及相關感染事件，指揮中心已採取相關應變措施，避免感染擴大</t>
-  </si>
-  <si>
-    <t>新增78例本土COVID-19確定病例，另有2例境外移入</t>
-  </si>
-  <si>
-    <t>集中檢疫所開放高風險7國以外入境者自費入住</t>
-  </si>
-  <si>
-    <t>第二劑AZ COVID-19疫苗接種說明</t>
+    <t>/Bulletin/Detail/HS0hjvHxAOTCPtNPmDo7Bw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/LpD4TCQApQ9vv1V6scwESw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/1j8W3yYnAz6bFopxt7_Www?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/V6pewvqk9-nbn5aARuSARw?typeid=9</t>
   </si>
   <si>
     <t>/Bulletin/Detail/yaxkF9NPpjDvDsdKXaitsQ?typeid=9</t>
@@ -79,16 +91,16 @@
     <t>/Bulletin/Detail/nM5PTloj8i3dm5h_EI3lHA?typeid=9</t>
   </si>
   <si>
-    <t>/Bulletin/Detail/F95aOtuKwrsJ347Xslc-ZA?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/Ve2G8PYEHCAhycgrH0Q1PQ?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/ZgKW-VupBVtp_sGz2YXXaQ?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/auHSp7RyQ7EesQkbPZBoaA?typeid=9</t>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/HS0hjvHxAOTCPtNPmDo7Bw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/LpD4TCQApQ9vv1V6scwESw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/1j8W3yYnAz6bFopxt7_Www?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/V6pewvqk9-nbn5aARuSARw?typeid=9</t>
   </si>
   <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/yaxkF9NPpjDvDsdKXaitsQ?typeid=9</t>
@@ -109,16 +121,16 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/nM5PTloj8i3dm5h_EI3lHA?typeid=9</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/F95aOtuKwrsJ347Xslc-ZA?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/Ve2G8PYEHCAhycgrH0Q1PQ?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/ZgKW-VupBVtp_sGz2YXXaQ?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/auHSp7RyQ7EesQkbPZBoaA?typeid=9</t>
+    <t>發佈日期：2021-06-29\$\@\$中央流行疫情指揮中心今(29)日表示，簡訊實聯制的推出，係為方便民眾及商家落實實聯制措施、減少紙本紀錄的接觸，並有助於疫調人員掌握個案相關活動史及匡列接觸者等，相關數據之使用，均有其合法性、正當性、必要性，且絕無違法情事，說明如下：\$\@\$一、 合法性：衛福部依傳染病防治法第37條第1項第6款，公告「嚴重特殊傳染性肺炎(COVID-19)第三級疫情警戒標準及防疫措施裁罰規定」，規定外出時應全程佩戴口罩，並配合實聯制；行政院為遏止疫情擴散，並減少實聯制紙本填寫之接觸，推出「簡訊實聯制」，供民眾及商家使用。\$\@\$二、 正當性：簡訊實聯制係於經得使用人同意下，掃瞄QR code即完成實聯制措施；而「簡訊實聯制」並不會留下個資給店家，所留下的活動史簡訊，電信業者也只保留28天，且僅供指揮中心疫調使用，不會做目的外利用。\$\@\$三、 必要性：在疫調工作中，衛生單位人員須掌握確診個案相關之活動資訊，以即時展開接觸者匡列、環境清消等各項防疫措施，故適當的運用簡訊實聯制相關資訊，對防疫推動有實質的幫助。\$\@\$指揮中心進一步指出，簡訊實聯制自今(2021)年5月19日上線後，於6月3日起啟用實聯制資料調用機制，以供地方政府衛生局有疫情調查需求時，向指揮中心申請調閱，經審核通過後將調閱資料回復，大多數申請調用案件可於一日之內提供資料。截至6月29日，已有宜蘭縣、花蓮縣、南投縣、屏東縣、苗栗縣、桃園市、高雄市、基隆市、新北市、新竹縣、嘉義縣、彰化縣、臺中市、臺北市、臺南市、澎湖縣，共計16縣市政府衛生局調用303項資料，調用量前3名依序為桃園市衛生局、高雄市衛生局、臺中市衛生局。\$\@\$指揮中心強調，「簡訊實聯制」的推出，主要為提供民眾、商家、衛生單位不管是在配合防疫措施或執行疫調工作上便利的平臺，籲請民眾、商家配合，也請地方政府加強稽查，共同落實實聯制，完備疫調工作，達到防疫的目的。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-29\$\@\$針對媒體報導「COVID-19疫苗接種外展服務，無法選擇疫苗廠牌，係為國產疫苗鋪路」，中央流行疫情指揮中心今(29)日澄清，無法選擇疫苗廠牌，係因目前尚無法確認屆時可供應之疫苗廠牌與數量，並非為國產疫苗鋪路。\$\@\$指揮中心表示，為加速我國COVID-19疫苗接種作業，規劃辦理「COVID-19疫苗接種外展服務」，已於日前發文請各部會先行調查「規模1,000人以上企業」、「100人以上中央政府機關」等人員施打疫苗意願及進行造冊，並由各機關（構）自行評估是否有適合執行接種作業的地點及空間規劃等。\$\@\$有關媒體報導「該公文提到無法選擇疫苗廠牌，係為國產疫苗鋪路」，指揮中心澄清，係因目前尚無法確認屆時可供外展服務之疫苗廠牌與疫苗數量，並非為國產疫苗鋪路。待疫苗量充足，會依屆時可供應之疫苗廠牌與數量，再次詢問機關（構）參與外展服務與接種之意願。\$\@\$指揮中心進一步說明，有關「疫苗外展服務調查」，係為後續疫苗量充足且可全民接種時，疫苗需求量調查與分布之預先規劃。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-29\$\@\$中央流行疫情指揮中心今(29)日公布國內新增54例COVID-19確定病例，均為本土個案；另確診個案中新增8例死亡。\$\@\$指揮中心表示，今日新增之54例本土病例(其中17例為居家隔離期間或期滿檢驗陽性者)，為19例男性、35例女性，年齡介於未滿5歲至80多歲，發病日介於今(2021)年6月16日至6月28日。個案分布以新北市22例最多，其次為臺北市20例、桃園市及新竹縣各4例，彰化縣2例，基隆市及屏東縣各1例；其中31例為已知感染源、5例關聯不明、18例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增8例死亡個案，為5例男性、3例女性，年齡介於60多歲至80多歲，發病日介於5月9日至6月19日，確診日介於5月15日至6月20日，死亡日介於6月25日至6月27日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至6月27日累計公布13,435位確診個案中，已有10,086人解除隔離，解隔離人數達確診人數75.1%。\$\@\$指揮中心統計，截至目前國內累計1,311,961例新型冠狀病毒肺炎相關通報(含1,295,813例排除)，其中14,748例確診，分別為1,170例境外移入，13,525例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；個案中累計102例移除為空號。自2020年起累計643例COVID-19死亡病例，其中635例本土，個案居住縣市分布為新北市325例、臺北市245例、基隆市21例、桃園市18例、彰化縣10例、臺中市及新竹縣各4例、宜蘭縣及花蓮縣各2例，苗栗縣、臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月29日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-29\$\@\$中央流行疫情指揮中心表示，今(29)日上午與各縣市政府召開的「全國防疫會議」，決議如下：\$\@\$一、國內疫情雖持續下降，惟部分縣(市)仍持續爆發群聚事件，須密切注意監測，及早發現並介入防治；另國內出現Delta變異株群聚，應強化疫調早期圍堵，避免造成社區流行。\$\@\$1.雙北部分：臺北市疫情趨緩，惟轄內近期發生市場、機構及工地等群聚，須留意防範擴散至社區；新北市疫情亦趨緩，惟各行政區仍須留意後續疫情變化。\$\@\$2.屏東縣部分：因出現Delta變異株群聚，不排除未來一週仍可能檢出相關病例，請屏東縣落實精準疫調及接觸者匡列、追蹤，早期發現病例並介入防治。\$\@\$二、有關簡訊實聯制運用於疫調處理部分，鑒於簡訊實聯制推動主要作為輔助疫調之用，建置前提為民眾上傳資訊越少越好(僅有停留場所代碼及進入之時間點)，因此請各地方政府在疫情處理上仍應以精準疫調為主，簡訊實聯制為輔，地方政府如有實聯制資料運用於疫調之需求，指揮中心資訊組將會適時協助提供。\$\@\$三、針對Delta變異株之防範，有無需要調整醫療院所感染管制措施之部分，指揮中心參考比較國外感控措施，目前尚無需調整我國現行措施。至於相關確診者個案能否共同收治入院，建議地方政府在病房收治量能允許下，仍應以一人一室為主。</t>
   </si>
   <si>
     <t>發佈日期：2021-06-28\$\@\$中央流行疫情指揮中心今(28)日公布國內新增60例COVID-19確定病例，均為本土個案；另確診個案中新增3例死亡。\$\@\$指揮中心表示，今日新增之60例本土病例(其中31例為居家隔離期間或期滿檢驗陽性者)，為26例男性、34例女性，年齡介於未滿10歲至90多歲，發病日介於今(2021)年6月19日至6月27日。個案分佈以新北市33例最多，其次為臺北市22例、桃園市2例，基隆市、南投縣及彰化縣各1例；其中32例為已知感染源、3例關聯不明、25例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增3例死亡個案，為2例男性、1例女性，年齡介於70多歲至90多歲，發病日介於5月23日至6月22日，確診日介於5月26日至6月24日，死亡日介於6月25日至6月26日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前累計1,282,057例新型冠狀病毒肺炎相關通報(含1,265,704例排除)，其中14,694例確診，分別為1,170例境外移入，13,471例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計102例移除為空號。自2020年起累計635例COVID-19死亡病例，其中627例本土，個案居住縣市分布為新北市321例、臺北市243例、基隆市21例、桃園市17例、彰化縣10例、臺中市及新竹縣各4例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月28日新增死亡COVID-19確診個案表.pdf</t>
@@ -127,28 +139,10 @@
     <t>發佈日期：2021-06-27\$\@\$有關今(6/27)日上午飛往金門航班，某旅客於機場快篩站進行快篩，因第一次篩檢結果無法成為判定的依據，在取得當事人同意後，執行第二次篩檢，呈現陰性，判定快篩結果為陰性，應予放行，另同步通知金門航空站及金門縣衛生局，以確實掌握該旅客情況。該旅客抵達金門後立即執行PCR檢測，經採檢PCR結果亦為陰性。\$\@\$目前本島各機場針對前往離島旅客執行篩檢，仍屬自願性質，並無強迫性，不只顧及防疫，亦能爭取旅客信任，鼓勵更多旅客參與篩檢，對離島的防疫防線更有幫助。惟為避免造成地方疑慮，未來於各機場快篩呈陽性或弱陽性反應之旅客，不再考慮檢驗誤差問題，將進行PCR採檢陰性後，始允許登機。</t>
   </si>
   <si>
-    <t>發佈日期：2021-06-27\$\@\$中央流行疫情指揮中心今(27)日宣布，因應Delta變異株於全球日益擴散且其傳播力高，即日起若旅客自「重點高風險國家(巴西、印度、英國、祕魯、以色列、印尼及孟加拉)」入境，則請搭乘交通部安排之的防疫車輛前往集中檢疫所。若旅客並非由前述「重點高風險國家」入境，應自費搭乘防疫車輛(或自行駕車)前往防疫旅宿或自費集中檢疫所之檢疫地點。\$\@\$指揮中心強調，入境旅客之親友勿前往機場接機，以減少病毒傳播風險，共同保護親友及社區防疫安全。</t>
-  </si>
-  <si>
     <t>發佈日期：2021-06-27\$\@\$為保障健康安全，近日民眾踴躍接種COVID-19疫苗，關於疫苗接種後是否產生副作用也有諸多討論。針對網傳COVID-19 mRNA疫苗恐傷害人體，中央流行疫情指揮中心今（27）日澄清，疫苗中的mRNA並不會進入細胞核，不會以任何方式改變人體的DNA，或與DNA產生交互作用。而政府也會嚴格把關疫苗安全，民眾可安心接種。\$\@\$指揮中心表示，我國目前已核准緊急使用授權的COVID-19疫苗分為兩大類，其中所使用的COVID-19 mRNA疫苗，其作用原理是將含有一段可轉譯成SARS-CoV-2病毒棘蛋白的mRNA注射至體內，接種後會在人體細胞質內製造出SARS-CoV-2病毒棘蛋白，作為疫苗抗原，進而誘發人體產生免疫反應，以對抗SARS-CoV-2病毒，疫苗中的mRNA不會進入細胞核、不會改變人體的DNA，或與DNA產生交互作用。\$\@\$指揮中心重申，我國核准專案輸入的mRNA疫苗，例如莫德納疫苗，是經過衛生福利部食品藥物管理署審查廠商所提供的疫苗品質管制資料、非臨床藥毒理試驗及人體臨床試驗報告，確認疫苗的品質、安全及療效後，始予以核准。\$\@\$指揮中心表示，為確保COVID-19疫苗上市後廣泛臨床使用下國人用藥安全，我國已建立COVID-19疫苗安全資訊主動監控機制，除持續監控國外衛生主管機關發布之COVID-19疫苗安全警訊外，亦設有「疫苗不良事件通報系統(VAERS)」接受各界通報，蒐集、分析及評估我國COVID-19疫苗不良事件，並藉由收集相關安全資訊，監控其安全性，一旦發現具有未知或未預期之風險，立即啟動再評估機制，重新評估其療效與風險，並確認是否需採取相關風險管控措施。\$\@\$指揮中心再次提醒， COVID-19疫苗與其他藥品一樣，或多或少都具有一些副作用，如過敏反應等，民眾接種前應主動提供自己的身體狀況，包括是否對特定藥品過敏、慢性病或正在服用的藥品；女性則需告知是否(或可能)懷孕、準備懷孕或正在哺乳母乳等，供醫師審慎評估其臨床效益及風險。接種後則應關心身體變化，部分民眾接種COVID-19疫苗後，可能會發生接種部位疼痛、紅腫、疲倦、頭痛、肌肉痠痛、體溫升高、畏寒、關節痛及噁心等，這些症狀通常輕微並且數天內消失，但如發生嚴重持續性頭痛、視力改變或癲癇、嚴重且持續腹痛超過24小時以上、皮膚出現自發性出血點、瘀青、紫斑、嚴重胸痛或呼吸困難、下肢腫脹或疼痛等，請立即就醫，並說明疫苗接種史，同時請醫師通報當地衛生局或衛生福利部疾病管制署。</t>
   </si>
   <si>
-    <t>發佈日期：2021-06-27\$\@\$中央流行疫情指揮中心今(27)日公布國內新增89例COVID-19確定病例，分別為88例本土及1例境外移入；另確診個案中新增9例死亡。\$\@\$指揮中心表示，今日新增之88例本土病例(其中27例為居家隔離期間或期滿檢驗陽性者)，為48例男性、40例女性，年齡介於未滿5歲至90多歲，發病日介於今(2021)年6月10日至6月26日。個案分佈以新北市41例最多，其次為臺北市33例、臺南市8例、桃園市3例，屏東縣、南投縣及新竹市各1例；其中60例為已知感染源、2例關聯不明、26例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增9例死亡個案，為3例男性、6例女性，年齡介於40多歲至90多歲，發病日介於5月15日至6月22日，確診日介於5月20日至6月25日，死亡日介於6月22日至6月26日；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增1例境外移入個案(案14719)，為本國籍20多歲男性，5月3日曾在奧地利當地檢出COVID-19陽性，6月11日自奧地利返臺，持有搭機前3日內檢驗陰性證明，入境後至防疫旅館檢疫，6月24日進行檢疫期滿前採檢，於今日確診。個案在臺期間並無症狀，相關接觸者匡列中。\$\@\$指揮中心統計，截至目前國內累計1,266,904例新型冠狀病毒肺炎相關通報(含1,250,863例排除)，其中14,634例確診，分別為1,170例境外移入，13,411例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計102例移除為空號。自2020年起累計632例COVID-19死亡病例，其中624例本土，個案居住縣市分布為新北市319例、臺北市243例、基隆市20例、桃園市17例、彰化縣10例、臺中市及新竹縣各4例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月27日新增死亡COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
     <t>發佈日期：2021-06-26\$\@\$中央流行疫情指揮中心今(26)日表示，目前進口國內之274萬劑莫德納(Ｍoderna) COVID-19疫苗將陸續完成檢驗封緘，預計於今(2021)年7月1日起，陸續配送至地方政府衛生局及指定醫療院所，並開放第一類至第八類對象接種。第一階段預計分配各地方政府衛生局約106萬劑，分兩梯次配送，第一梯次配送約64.3萬劑，預計於7月1日陸續配達，第二梯次配送約41.8萬劑，預計７月８日陸續配達(如附件)。\$\@\$指揮中心指出，第一階段疫苗各地方政府分配數量係以下列原則核估，並將依各地方政府衛生局規劃，配送至衛生局或其指定醫療院所：\$\@\$一、各縣市第五類「居家式和社區式長照機構及身障服務照服員及服務對象」中，尚未接種疫苗之64歲以下與75歲以上服務對象及所有照服員人數總計之6成。\$\@\$二、各縣市第五類「其他機構(含矯正機關工作人員)」尚未接種人數。\$\@\$三、各縣市莫德納(Moderna)COVID-19疫苗已分配數。\$\@\$四、各縣市65-74歲長者30%人口數。\$\@\$另第二階段各地方政府分配數量則以65-74歲長者20%人口數所需疫苗數量核估，將視第一階段疫苗接種情形配發。\$\@\$指揮中心說明，有關第七類對象「維持國家安全及社會機能正常運作者」是經由各中央目的事業主管機關認定，並依據其感染風險決定為優先接種對象後進行造冊，列為首波接種之國家關鍵設施或維持設社會正常運作必要工作人員。上述對象的疫苗需求量，原則直接配送至各部會指定之COVID-19合約醫療院所，各醫療院所可視接種量能，透過原預約機制，或安排於特定時段集中接種。惟莫德納(Moderna) COVID-19疫苗於2-8℃配達後僅能保存28天，請第七類對象於預約日或接獲通知日期後，儘速前往接種，以利指揮中心視各醫療院所接種情形與庫存量，通知醫療院所逐續開放其他類對象接種，發揮COVID-19疫苗最大效益。\$\@\$指揮中心表示，第一階段配送之莫德納(Ｍoderna) COVID-19疫苗為美國提供之250萬劑其中一部分，將以2-8℃溫層配送，其包裝為每瓶14劑，10瓶一盒，接種單位可針對當日最後一瓶疫苗開瓶的剩餘劑，規劃候補名單機制，有效利用COVID-19疫苗。\$\@\$指揮中心提醒，為確保疫苗接種安全，建議先前曾因接種疫苗或任何注射治療後發生急性過敏反應的民眾，接種後請於接種處或附近留觀至少30分鐘，一般民眾則建議至少留觀15分鐘，並自我密切觀察15分鐘，以利即時處置該類急性過敏反應。\$\@\$指揮中心強調，依據各國疫苗上市後的安全性監測，曾有報告極少數年輕族群在接種mRNA 疫苗後發生心肌炎等不良反應事件，大多發生在接種後數天內，請民眾在接種mRNA 疫苗後如出現胸痛、喘或心悸等症狀，應立即就醫並說明疫苗接種史。 附件\$\@\$附件-274萬劑Moderna疫苗分配量.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-06-26\$\@\$中央流行疫情指揮中心今(26)日表示，有關屏東COVID-19 Delta印度變異株群聚及其相關感染事件，目前累計12例確定病例，其中6例經基因定序後，均為Delta印度變異株，分別為秘魯境外移入確診祖孫2人(案13332、13333)及案14298、14407、14408、14409。\$\@\$指揮中心指出，該起群聚事件指標個案為當地白牌司機(案14298)，經疫調及接觸者採檢後，發現1位工作接觸者(案14409)確診，而案14409之2位家人(案14407、14408)亦同時確診，其中案14407曾於6月11日、6月14日與秘魯境外移入案13332有短暫接觸，其餘事件相關確診個案均為家庭或活動之接觸者採檢後確診。為避免感染擴大，指揮中心已採取相關應變措施如下：\$\@\$一、精準疫調並擴大匡列接觸者及採檢，另接觸者安排防疫旅館落實隔離，並於居隔期滿前採檢，截至6月25日案14298群聚相關接觸者匡列136人、共居家隔離99人、自主健康管理匡列32人，自我健康監測5人，其中已採檢124人，PCR檢驗陽性9人、陰性115人，接觸者持續擴大匡列中。\$\@\$二、6月24日起於當地設置社區篩檢站，籲請足跡重疊民眾篩檢，並加強民眾溝通配合篩檢，截至6月25日PCR篩檢共419人皆為陰性；另針對確診個案公布社區足跡點，並完成公共場所消毒。\$\@\$三、當地醫療院所加強通報及感染管制措施，請醫師協助有疑似症狀就醫民眾轉介採檢院所通報及採檢。\$\@\$四、透過廣播系統呼籲民眾落實疫情三級警戒規範，外出與工作均要全程佩戴口罩，嚴查避免群聚，另針對當地超市、超商、餐飲業、傳統市場等場所關閉三天。\$\@\$五、給予確診個案妥善臨床照護處置，如符合單株抗體、瑞德西韋使用條件則即時使用；如有出現重症前兆，迅速進行處置及治療。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-06-26\$\@\$中央流行疫情指揮中心今(26)日公布國內新增80例COVID-19確定病例，其中78例為本土個案(39例為居家隔離期間或期滿檢驗陽性者)；另有2例境外移入。另，確診個案中新增13例死亡。\$\@\$指揮中心表示，今日新增之78例本土病例，為36例男性、42例女性，年齡介於未滿5歲至80多歲，發病日介於今(2021)年6月11日至6月25日。個案分佈以新北市36例最多，其次為臺北市30例、桃園市、基隆市及屏東縣各3例，苗栗縣、彰化縣及新竹縣各1例。其中雙北地區以外縣市12例中，10例為已知感染源、2例關聯不明；相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增13例死亡個案，為8例男性、5例女性，年齡介於40多歲至90多歲，發病日介於5月14日至6月20日，確診日介於5月19日至6月22日，死亡日介於6月21日至6月24日，詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至6月24日累計公布13,190位確診個案中，已有9,916人解除隔離，解隔離人數達確診人數75.1%。\$\@\$指揮中心表示，今日新增2例境外移入個案中，案14591為30多歲本國籍女性，6月11日自日本返臺，持有搭機前3日內檢驗陰性證明，居家檢疫期間並無症狀，6月25日進行期滿採檢，於今日確診。案14619為本國籍30多歲女性，6月11日自菲律賓返臺，持有搭機前3日內檢驗陰性證明，居家檢疫期間並無症狀，6月25日進行期滿採檢，於今日確診。2名個案檢疫期間均無接觸他人，故無匡列接觸者。\$\@\$指揮中心統計，國內累計1,243,683例新型冠狀病毒肺炎相關通報(含1,227,748例排除)，其中14,545例確診，分別為1,169例境外移入，13,323例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；累計102例移除為空號。自2020年起累計623例COVID-19死亡病例，其中615例本土，個案居住縣市分布為新北市313例、臺北市241例、基隆市20例、桃園市17例、彰化縣9例、臺中市及新竹縣各4例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月26日新增死亡COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-06-26\$\@\$中央流行疫情指揮中心今(26)日表示，為因應6月27日起，自COVID-19變異株「重點高風險7國(巴西、印度、英國、祕魯、以色列、印尼及孟加拉)」以外之國家入境旅客(過去14天旅遊史、含轉機)住宿需要，將開放集中檢疫所供民眾自費使用，於今日晚間8時開放訂房。\$\@\$指揮中心指出，目前全臺有49處集中檢疫所，分布於北、中、南等三區，包括各類公務人員訓練中心、軍營、停招的學校宿舍、旅館等，每人每日新臺幣2,000元整，12歲以下幼童與父或母同住一室者，不另外收費。\$\@\$指揮中心說明，民眾入住之檢疫所地點須由指揮中心分派，房內皆有網路、電視等相關設備，入住民眾亦可使用自己的手機電話與外界聯繫；集中檢疫場所均有提供三餐，餐飲會於固定時間送到檢疫房間外，再由民眾自行取用至自己的檢疫房間內用餐。\$\@\$指揮中心提醒，集中檢疫所預定今日晚間8時開放訂房，有意自費入住民眾可至「入境檢疫系統」網頁預約，預約者須於航班預計抵臺48小時前至入境檢疫系統預約、繳費，以取得預約訂房識別碼，作為入境登記使用。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-06-26\$\@\$中央流行疫情指揮中心今(26)日表示，5月9日前已完成第一劑AstraZeneca COVID-19疫苗接種之民眾，皆可於接種後第10至12週公費接種第二劑。專家建議AstraZeneca COVID-19疫苗接種間隔10至12週再接種第二劑疫苗，效益更佳。若有出國急迫性須於8至10週間接種者，亦可酌情提供接種。前述對象均可至各合約醫療院所預約接種，亦建議優先考量原接種醫院，或可至疾病管制署旅遊醫學合約醫院。\$\@\$指揮中心說明，截至6月24日止，已有3.3萬人完成兩劑AstraZeneca COVID-19疫苗接種，為使民眾獲得最大免疫保護力，請4月12日至5月9日期間已接種第一劑疫苗之民眾，於接種日起間隔第10-12週後，透過各醫院預約系統預約接種第二劑疫苗。為確保該等對象第二劑AstraZeneca COVID-19疫苗接種之權益，指揮中心將依據4月12日至5月9日每週AstraZeneca COVID-19疫苗接種量，自本週起4週內，每週配送至指揮中心指定之COVID-19疫苗合約醫療院所，預計全臺4週配送量約6.9萬劑。民眾可優先於原接種醫院預約，或可至疾管署旅遊醫學合約醫院接種（院所名單詳見附件，將視各院接種與開放情形適時調整）。\$\@\$指揮中心提醒，前往接種前務必確認備妥「COVID-19疫苗接種紀錄卡」及「健保卡」，若「COVID-19疫苗接種紀錄卡」已遺失，民眾可返回第一劑接種之醫療院所補發，並完成第二劑接種。指揮中心進一步說明，國外臨床試驗資料分析顯示，完成兩劑AstraZeneca COVID-19疫苗接種且間隔 12 週以上，保護力可達81%，籲請民眾可於第一劑接種10-12週後，完成第二劑接種，使疫苗發揮最大效益。 附件\$\@\$有開設旅遊醫學門診之醫療院所名單.pdf</t>
   </si>
 </sst>
 </file>
@@ -554,7 +548,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="2">
-        <v>44375</v>
+        <v>44376</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>25</v>
@@ -571,7 +565,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="2">
-        <v>44374</v>
+        <v>44376</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>26</v>
@@ -588,7 +582,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="2">
-        <v>44374</v>
+        <v>44376</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>27</v>
@@ -605,7 +599,7 @@
         <v>18</v>
       </c>
       <c r="C5" s="2">
-        <v>44374</v>
+        <v>44376</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>28</v>
@@ -622,7 +616,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="2">
-        <v>44374</v>
+        <v>44375</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>29</v>
@@ -639,7 +633,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="2">
-        <v>44373</v>
+        <v>44374</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>30</v>
@@ -656,13 +650,10 @@
         <v>21</v>
       </c>
       <c r="C8" s="2">
-        <v>44373</v>
+        <v>44374</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -673,13 +664,13 @@
         <v>22</v>
       </c>
       <c r="C9" s="2">
-        <v>44373</v>
+        <v>44374</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -690,13 +681,10 @@
         <v>23</v>
       </c>
       <c r="C10" s="2">
-        <v>44373</v>
+        <v>44374</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="E10" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -713,7 +701,7 @@
         <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20210630
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="325">
   <si>
     <t>Press Title</t>
   </si>
@@ -31,6 +31,15 @@
     <t>Page Content</t>
   </si>
   <si>
+    <t>指揮中心與農委會制定「批發市場防疫管理措施建議指引」 協助批發市場防疫</t>
+  </si>
+  <si>
+    <t>Moderna第三批採購疫苗41萬劑將於今(30)日下午抵臺</t>
+  </si>
+  <si>
+    <t>新增56例COVID-19確定病例，分別為55例本土及1例境外移入</t>
+  </si>
+  <si>
     <t>簡訊實聯制數據係以合法性、正當性、必要性進行使用，絕無違法情事</t>
   </si>
   <si>
@@ -61,6 +70,246 @@
     <t>指揮中心說明274萬劑莫德納(Moderna) COVID-19疫苗第一階段分配事宜</t>
   </si>
   <si>
+    <t>因應屏東Delta印度變異株群聚及相關感染事件，指揮中心已採取相關應變措施，避免感染擴大</t>
+  </si>
+  <si>
+    <t>新增78例本土COVID-19確定病例，另有2例境外移入</t>
+  </si>
+  <si>
+    <t>集中檢疫所開放高風險7國以外入境者自費入住</t>
+  </si>
+  <si>
+    <t>第二劑AZ COVID-19疫苗接種說明</t>
+  </si>
+  <si>
+    <t>6月25日全國防疫會議後記者會報告</t>
+  </si>
+  <si>
+    <t>為有效利用COVID-19疫苗 當日最後一瓶開瓶剩餘劑量將開放候補接種</t>
+  </si>
+  <si>
+    <t>因應全球Delta變異株流行，自6月27日零時起，全面提升入境人員檢疫措施</t>
+  </si>
+  <si>
+    <t>新增76例COVID-19確定病例，均為本土個案</t>
+  </si>
+  <si>
+    <t>民眾使用COVID-19家用快篩試劑流程與注意事項</t>
+  </si>
+  <si>
+    <t>新增130例COVID-19確定病例，分別為129例本土及1例境外移入</t>
+  </si>
+  <si>
+    <t>指揮中心與相關單位持續精進「市場專案」相關措施，達到社區清零目的</t>
+  </si>
+  <si>
+    <t>指揮中心維持全國疫情警戒第三級至7月12日止，希望國人共體時艱，共同抗疫</t>
+  </si>
+  <si>
+    <t>因應臺北農產運銷公司群聚感染事件，指揮中心啟動「市場專案」強化相關防疫作為</t>
+  </si>
+  <si>
+    <t>新增104例COVID-19確定病例，均為本土個案</t>
+  </si>
+  <si>
+    <t>指揮中心說明274萬劑莫德納(Moderna) COVID-19疫苗之分配規劃、第一批次分配原則與接種對象</t>
+  </si>
+  <si>
+    <t>因應印度變種病毒蔓延 居家檢疫及居家隔離期滿者均須進行PCR檢測 以維護國內社區安全</t>
+  </si>
+  <si>
+    <t>6月22日全國防疫會議後記者會報告</t>
+  </si>
+  <si>
+    <t>指揮中心說明「COVID-19疫苗公費接種對象」及現階段開放接種實施對象</t>
+  </si>
+  <si>
+    <t>新增78例COVID-19本土病例，另有1例境外移入</t>
+  </si>
+  <si>
+    <t>修正雇主聘僱移工防疫指引，明定雇主應落實防疫措施</t>
+  </si>
+  <si>
+    <t>新增75例COVID-19本土病例，均為本土個案</t>
+  </si>
+  <si>
+    <t>指揮中心持續監測疫苗接種後不良事件，提醒民眾待身體狀況穩定後再行安排接種</t>
+  </si>
+  <si>
+    <t>美國政府捐贈250萬劑Moderna COVID-19疫苗將於今(20)日傍晚抵臺</t>
+  </si>
+  <si>
+    <t>新增109例COVID-19病例，為107例本土、2例境外移入</t>
+  </si>
+  <si>
+    <t>指揮中心持續監測疫苗接種後不良事件，提醒民眾視身體狀況穩定後再行安排接種</t>
+  </si>
+  <si>
+    <t>已接種一劑AZ COVID-19疫苗之民眾，可陸續完成第二劑接種</t>
+  </si>
+  <si>
+    <t>新增128例COVID-19病例，為127例本土、1例境外移入</t>
+  </si>
+  <si>
+    <t>6月18日全國防疫會議後記者會報告</t>
+  </si>
+  <si>
+    <t>指揮中心持續監測疫苗接種後不良事件，並提醒高齡年長者接種疫苗之注意事項</t>
+  </si>
+  <si>
+    <t>為利醫療院所照護重症個案，指揮中心成立COVID-19重症個案臨床處置專家諮詢小組，自6月21日開始線上病例諮詢會議</t>
+  </si>
+  <si>
+    <t>Moderna疫苗24萬劑將於今(18)日下午抵臺</t>
+  </si>
+  <si>
+    <t>新增188例COVID-19病例，為187例本土、1例境外移入</t>
+  </si>
+  <si>
+    <t>接種COVID-19疫苗是預防感染、避免重症與死亡最有效的方式　指揮中心持續監測疫苗接種後不良事件</t>
+  </si>
+  <si>
+    <t>指揮中心公布新增175例COVID-19本土病例</t>
+  </si>
+  <si>
+    <t>指揮中心公布新增167例COVID-19本土病例，另有3例境外移入</t>
+  </si>
+  <si>
+    <t>國產疫苗審查皆以科學、專業為原則，並依法規程序採購</t>
+  </si>
+  <si>
+    <t>第二批莫德納(Moderna) COVID-19疫苗預計於6月18日起配送，請合約醫療院所開啟預約掛號服務，提供符合對象者預約接種</t>
+  </si>
+  <si>
+    <t>指揮中心說明疫苗接種第二類「中央及地方政府防疫人員」含括對象</t>
+  </si>
+  <si>
+    <t>日本提供我國AstraZeneca COVID-19疫苗第二次分配量說明</t>
+  </si>
+  <si>
+    <t>補助全國快速PCR檢驗儀 加速社區檢驗量能</t>
+  </si>
+  <si>
+    <t>指揮中心公布新增132例本土病例，另有3例境外移入</t>
+  </si>
+  <si>
+    <t>6月15日全國防疫會議後記者會報告</t>
+  </si>
+  <si>
+    <t>調整國籍航空公司機組員返臺檢疫措施，確保機組員職場健康安全及維護國內防疫安全</t>
+  </si>
+  <si>
+    <t>指揮中心公布新增185例COVID-19確定病例，均為本土個案</t>
+  </si>
+  <si>
+    <t>指揮中心說明「中央政府機關防疫相關人員之疫苗分配量寄放於各縣市」一事</t>
+  </si>
+  <si>
+    <t>網傳總統、副總統已接種COVID-19疫苗  指揮中心調閱接種系統查證均尚未接種</t>
+  </si>
+  <si>
+    <t>指揮中心公布新增174例COVID-19本土個案及1例境外移入</t>
+  </si>
+  <si>
+    <t>指揮中心：依公式計算配送各縣市疫苗數量  將視後續接種情形滾動檢討並加強配送</t>
+  </si>
+  <si>
+    <t>自6月12日起，首批莫德納疫苗開放尚未接種第一劑COVID-19疫苗的第一類醫事及非醫事人員接種</t>
+  </si>
+  <si>
+    <t>指揮中心公布新增250例本土個案，另有1例境外移入</t>
+  </si>
+  <si>
+    <t>為提升COVID-19疫苗接種效率，指揮中心與地方政府衛生局召開會議進行經驗交流與分享</t>
+  </si>
+  <si>
+    <t>6月11日全國防疫會議後記者會報告</t>
+  </si>
+  <si>
+    <t>為協助紓解重症醫療量能，指揮中心採購複合單株抗體藥物，提供具有重症風險因子之輕中度確診個案治療使用</t>
+  </si>
+  <si>
+    <t>指揮中心公布新增286例COVID-19本土確定病例及1例境外移入</t>
+  </si>
+  <si>
+    <t>全國疫情警戒第三級期間，持續執行「邊境嚴管」措施</t>
+  </si>
+  <si>
+    <t>指揮中心感謝我國企業及民間單位共同捐贈日製負壓隔離艙80座，公私協力共同防疫</t>
+  </si>
+  <si>
+    <t>疫苗接種政策為全體國民重要權益，資訊均公開透明，如有違法將嚴正法辦</t>
+  </si>
+  <si>
+    <t>指揮中心公布新增263例COVID-19本土確定病例，另有3例境外移入</t>
+  </si>
+  <si>
+    <t>指揮中心針對好心肝診所提供非開放接種對象接種疫苗案，將由司法單位依法徹查，還原真相，嚴正法辦</t>
+  </si>
+  <si>
+    <t>指揮中心說明配送至臺北市轄內合約醫院協助專案對象接種事宜</t>
+  </si>
+  <si>
+    <t>因應COVID-19疫情，調整COVID-19疫苗公費優先接種對象</t>
+  </si>
+  <si>
+    <t>指揮中心公布新增274例COVID-19本土確定病例，另有1例境外移入</t>
+  </si>
+  <si>
+    <t>COVID-19疫苗須依循指揮中心所訂之接種順序依序施打</t>
+  </si>
+  <si>
+    <t>6月8日全國防疫會議後記者會報告</t>
+  </si>
+  <si>
+    <t>指揮中心公布新增219例COVID-19確定病例，均為本土個案</t>
+  </si>
+  <si>
+    <t>國內出現自呼吸道疾病病人中分離出H1N2v流感病毒案例，病患已痊癒，疾管署呼籲民眾做好個人健康管理</t>
+  </si>
+  <si>
+    <t>加強訪查移工宿舍落實防疫工作  增訂企業因應員工確診應變處置</t>
+  </si>
+  <si>
+    <t>指揮中心公布新增211例本土COVID-19個案、3例境外移入</t>
+  </si>
+  <si>
+    <t>全國疫情警戒第三級延長至6月28日，相關防疫措施持續執行，嚴守社區防線</t>
+  </si>
+  <si>
+    <t>指揮中心澄清：目前我國COVID-19疫苗無自費接種規劃，並無所謂「自費負擔」之問題存在，而未來將依序開放全體國民公費接種，相關行政費用皆由政府負擔</t>
+  </si>
+  <si>
+    <t>指揮中心公布新增335例本土COVID-19個案，另有8例校正回歸個案</t>
+  </si>
+  <si>
+    <t>針對苗栗縣電子廠群聚感染案件，指揮中心說明前進指揮所協助防疫作為</t>
+  </si>
+  <si>
+    <t>指揮中心澄清：全民免費接種COVID-19疫苗公費疫苗順序，將由指揮中心陸續公布</t>
+  </si>
+  <si>
+    <t>指揮中心：政府已於特別預算編列40億，請合約醫療院所免費提供民眾接種公費COVID-19疫苗服務，自6月7日起實施</t>
+  </si>
+  <si>
+    <t>指揮中心澄清，有關網路及媒體報導全家6人確診COVID-19、母親病逝案，相關確診及死亡資訊都有公開</t>
+  </si>
+  <si>
+    <t>自即日起，暫停移工轉換雇主等作業以減少人員流動 防杜疫情擴散</t>
+  </si>
+  <si>
+    <t>苗栗縣2家電子廠發生群聚感染案件，前進指揮所已立即啟動相關防疫措施，避免感染擴大</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/QW-rc-JUvcOMq_9P2SjxLA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/pYQ-ddE0kOM_t_QJfc8xjw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/2_g7KcaGpuqcmjonS_tseQ?typeid=9</t>
+  </si>
+  <si>
     <t>/Bulletin/Detail/HS0hjvHxAOTCPtNPmDo7Bw?typeid=9</t>
   </si>
   <si>
@@ -91,6 +340,246 @@
     <t>/Bulletin/Detail/nM5PTloj8i3dm5h_EI3lHA?typeid=9</t>
   </si>
   <si>
+    <t>/Bulletin/Detail/F95aOtuKwrsJ347Xslc-ZA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Ve2G8PYEHCAhycgrH0Q1PQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/ZgKW-VupBVtp_sGz2YXXaQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/auHSp7RyQ7EesQkbPZBoaA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/5NpKu8jZAKdJssJnlGxTXA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/a_nNEk7-jcJcUMqE3M-Xeg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/zqUqseKSNKJint4YMEddiQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/9pKIzKzZOpp4HocU3uCl6g?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/c8C9gtHwUNnkywyMqWoLJQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/3A_GxvlYM4wkYEYTlozw6A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/0M4E0GxUuEj9_0rHwVlPAw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/3LyPF-Dt0AhduqNnRwp9zg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/kJJ5ZOZig6PA2ZAu2VMRQQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/mDFLj0aLsQztMI7vnMSy1w?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/HmZ7CIAda5ftC781xMTSKg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/zK5fwXiSohil4etG3pphhw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/NC6r7Z2A5ylk0AUMFxAkcA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/H95sl3L-tIrq1-o71rj8Gg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/7IX7KD-nM2TmIYgml7lDWg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/OakZRZ4dYRYEnX-_s__Dag?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Lby0PKwYfroFHd13wPbOdg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/ODtiZA3OtV7lf4IEVECBkA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/k9iJeEl5uPkgkCmCWtGZDg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/8QrfZwt787Bjeoh31UZztg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/B8Zac1K5GfDJSO8oDKcNfQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/4p1T6MpeJyRyu1syfZDUyw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/u9SuLf-DGkfywEXISH7pIw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/j5bFJQGngMHxaaQIK-j12w?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/hbSnCh8vhAKj2CsaFwbmZA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/tEf1nYt3fuARSRqFzbGbmw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/StnIZRaP2BZTFrduQfgCdg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/TAeqHS3g8G3Qbp3EGZkXSQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/f9isJQRtYK4rL9_Zmd4VUw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/3EaqopBnYL-XoDtMI8qQEA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/-bdXbaKzQLCvX8s69vQWQA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/gpzjNU57zwqDAfQJhI7fMA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/7ZPV_qpP_nL8FkiGNv1sbQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/R-DB5ro9NqAlSEStj_Uaxw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/2E5FJ55LFelexPtiSn3gbQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/84kDjSBTHU75sIoWKAdKcg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/DRnT39ZhmbVd21bWvHIEng?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/dmyxdxokdprJxTw9L5O5Bw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Aaw09pr_bNORqPc8F1fUSA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/832w8RYL7puxozPKMoTSAg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/A_4V_ZEYMJgH3nzjXxy21w?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/OOQWHbZwyOpZ-GpkKOgyYw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/iGXRaqo6rnJ0Gh9PFDovyg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/XUjGVcW2wV5HhfnxjVqg0w?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/eCpD5uFuWNjGpxhqMKIZ8A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/MHEOJlq75e2VYGkuBMGeJQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/-9laBujLZpjBzFaf_j8hcg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Z3woynaHMpHEAcv_YpZBHA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/6RR01Fye2xDT2mAOqhAoSg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/YCIJBF3p851kbsP5H1TZtw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/3iNNwroO0OrdsItewXo_GA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/itht4O09O7Hzx42_eMrmqw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/A_H9_tpR0cCtxnrn6ywmyg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/lMHQW2_3wdE5B0rVqMdwKA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/_O58a0Z72pKkvO77XRxTwg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/KklxR5Jvi8ZagDLpc8KhXg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/QT1poRzaqL7uU0eT1aAVFQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/WF6xlOaJgMr0POPnUwWvsw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/SPh-q2L4jdXq_e30j4qgMQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/iEPM5F7Kk_MMdZuFIF3xgA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/8UJd-2sMxGw-HAWQ6FJMSQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/6GaA6f7NZJ4vssTWjn2lsg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/07PCKLsTECw_vdl58CuklQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/R1FSxs02pQ9SbzB6uQQ8TA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/0SoUcz9h9xq6wfHsBCpV-g?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/CigUYrFf8immzExlBKZU7A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/JjN_NyCRNf6UTrNW6xvYhQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/c4MhZ18JVk_AQCy1McxIag?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/_dM67Z59iwBnM6hPn9W1uA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/aYrItM5MHeKmi1AQ2o0pzg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/nR4VlCvEVaDQd2QxrYxh5g?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/tlpf1qYwvYAgaVJbCaL1tg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/PPX8RUUDodGzAgui6fCasA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/QW-rc-JUvcOMq_9P2SjxLA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/pYQ-ddE0kOM_t_QJfc8xjw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/2_g7KcaGpuqcmjonS_tseQ?typeid=9</t>
+  </si>
+  <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/HS0hjvHxAOTCPtNPmDo7Bw?typeid=9</t>
   </si>
   <si>
@@ -121,12 +610,249 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/nM5PTloj8i3dm5h_EI3lHA?typeid=9</t>
   </si>
   <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/F95aOtuKwrsJ347Xslc-ZA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Ve2G8PYEHCAhycgrH0Q1PQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/ZgKW-VupBVtp_sGz2YXXaQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/auHSp7RyQ7EesQkbPZBoaA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/5NpKu8jZAKdJssJnlGxTXA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/a_nNEk7-jcJcUMqE3M-Xeg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/zqUqseKSNKJint4YMEddiQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/9pKIzKzZOpp4HocU3uCl6g?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/c8C9gtHwUNnkywyMqWoLJQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/3A_GxvlYM4wkYEYTlozw6A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/0M4E0GxUuEj9_0rHwVlPAw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/3LyPF-Dt0AhduqNnRwp9zg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/kJJ5ZOZig6PA2ZAu2VMRQQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/mDFLj0aLsQztMI7vnMSy1w?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/HmZ7CIAda5ftC781xMTSKg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/zK5fwXiSohil4etG3pphhw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/NC6r7Z2A5ylk0AUMFxAkcA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/H95sl3L-tIrq1-o71rj8Gg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/7IX7KD-nM2TmIYgml7lDWg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/OakZRZ4dYRYEnX-_s__Dag?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Lby0PKwYfroFHd13wPbOdg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/ODtiZA3OtV7lf4IEVECBkA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/k9iJeEl5uPkgkCmCWtGZDg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/8QrfZwt787Bjeoh31UZztg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/B8Zac1K5GfDJSO8oDKcNfQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/4p1T6MpeJyRyu1syfZDUyw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/u9SuLf-DGkfywEXISH7pIw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/j5bFJQGngMHxaaQIK-j12w?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/hbSnCh8vhAKj2CsaFwbmZA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/tEf1nYt3fuARSRqFzbGbmw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/StnIZRaP2BZTFrduQfgCdg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/TAeqHS3g8G3Qbp3EGZkXSQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/f9isJQRtYK4rL9_Zmd4VUw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/3EaqopBnYL-XoDtMI8qQEA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/-bdXbaKzQLCvX8s69vQWQA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/gpzjNU57zwqDAfQJhI7fMA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/7ZPV_qpP_nL8FkiGNv1sbQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/R-DB5ro9NqAlSEStj_Uaxw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/2E5FJ55LFelexPtiSn3gbQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/84kDjSBTHU75sIoWKAdKcg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/DRnT39ZhmbVd21bWvHIEng?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/dmyxdxokdprJxTw9L5O5Bw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Aaw09pr_bNORqPc8F1fUSA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/832w8RYL7puxozPKMoTSAg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/A_4V_ZEYMJgH3nzjXxy21w?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/OOQWHbZwyOpZ-GpkKOgyYw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/iGXRaqo6rnJ0Gh9PFDovyg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/XUjGVcW2wV5HhfnxjVqg0w?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/eCpD5uFuWNjGpxhqMKIZ8A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/MHEOJlq75e2VYGkuBMGeJQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/-9laBujLZpjBzFaf_j8hcg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Z3woynaHMpHEAcv_YpZBHA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/6RR01Fye2xDT2mAOqhAoSg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/YCIJBF3p851kbsP5H1TZtw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/3iNNwroO0OrdsItewXo_GA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/itht4O09O7Hzx42_eMrmqw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/A_H9_tpR0cCtxnrn6ywmyg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/lMHQW2_3wdE5B0rVqMdwKA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/_O58a0Z72pKkvO77XRxTwg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/KklxR5Jvi8ZagDLpc8KhXg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/QT1poRzaqL7uU0eT1aAVFQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/WF6xlOaJgMr0POPnUwWvsw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/SPh-q2L4jdXq_e30j4qgMQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/iEPM5F7Kk_MMdZuFIF3xgA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/8UJd-2sMxGw-HAWQ6FJMSQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/6GaA6f7NZJ4vssTWjn2lsg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/07PCKLsTECw_vdl58CuklQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/R1FSxs02pQ9SbzB6uQQ8TA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/0SoUcz9h9xq6wfHsBCpV-g?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/CigUYrFf8immzExlBKZU7A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/JjN_NyCRNf6UTrNW6xvYhQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/c4MhZ18JVk_AQCy1McxIag?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/_dM67Z59iwBnM6hPn9W1uA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/aYrItM5MHeKmi1AQ2o0pzg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/nR4VlCvEVaDQd2QxrYxh5g?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/tlpf1qYwvYAgaVJbCaL1tg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/PPX8RUUDodGzAgui6fCasA?typeid=9</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-30\$\@\$中央流行疫情指揮中心今(30)日表示，批發市場為供應民眾農、漁、畜等民生物資的重要營業場所，因應近期批發市場出現群聚感染事件，為確保相關場域工作人員、採購民眾自身與家人健康，指揮中心與農委會共同訂定「批發市場防疫管理措施建議指引」，呼籲各批發市場遵循，以避免群聚感染、疫情擴大。\$\@\$指揮中心進一步表示，「批發市場防疫管理措施建議指引」提供主管機關、場域管理單位及工作人員，依實際可行性與適用性，內化為適合個別場域所需的管理措施，供管理單位、從業人員及採購人員遵循辦理，以降低疫情在批發市場的發生機率、規模及社區傳播風險。\$\@\$指揮中心指出，「批發市場防疫管理措施建議指引」包含以下重點防疫措施，請各批發市場遵循，以降低疫情發生：\$\@\$人員健康管理：落實市場出入人員體溫量測、實聯制。盤點及造冊相關工作人員，落實健康狀況監測、定期篩檢及訂定健康監測計畫(包含人員名單及異常追蹤處理機制)，並鼓勵接種COVID-19疫苗。\$\@\$人流管制措施：調整市場攤位配置及營業時段，減少市場之出入口、劃定人員動線及分流措施，管制人數總量及單位時間人數。\$\@\$落實人員衛生行為：張貼標語、海報或透過廣播提醒顧客、從業人員等落實戴口罩及手部衛生，增加洗手設備可近性，並儘量使用非直接與顧客接觸之收付款方式。\$\@\$個人防護裝備建議：工作人員需佩戴口罩及面罩，視需要佩戴手套或穿著防水圍裙，拋棄式口罩不可重複使用；面罩若為可重複使用者，應確實清潔消毒後重複使用。\$\@\$環境清潔消毒：訂定環境清潔及消毒計畫，定時執行環境清潔及消毒，每天至少1次以上，並增加公共廁所衛生清潔及消毒頻率。\$\@\$出現確定病例之應變措施：訂定包括風險對象管理、風險區域管理及營運降載措施等3大應變措施，批發市場若發生確診者，應通報主管機關，風險區域須暫停營業，並視影響程度，通知供應人及承銷人至鄰近市場交易。\$\@\$指揮中心表示，農委會後續將與全國各批發市場及縣市政府召開視訊說明會，並請各縣市批發市場依據公布的指引自行訂定符合實際經營樣態的防疫作業規範，確保農產品穩定供應。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-30\$\@\$中央流行疫情指揮中心今(30)日表示，第三批Moderna疫苗41萬劑，已於歐洲時間6月29日晚上9時30分自阿姆斯特丹啟運，預定今日下午4時40分抵達桃園國際機場。\$\@\$指揮中心表示，本批疫苗為我國與供應商採購之一部分，首批15萬劑已於5月28日、第二批24萬劑也於6月18日分別到貨。今日抵臺疫苗待完成通關程序後，將直接運送至指定冷儲物流中心進行後續檢驗封緘作業，再提供COVID-19接種計畫所列實施對象接種。\$\@\$指揮中心指出，該中心已於今(2021)年2月8日與美國Moderna公司簽署505萬劑COVID-19疫苗供應合約，該疫苗為多劑型包裝(每瓶10人份)，存放於-20℃可保存6個月，於2-8℃之使用期限為30天，依臨床試驗結果，每人需施打2劑，2劑間隔28天以上，疫苗保護效力可達94%。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-30\$\@\$中央流行疫情指揮中心今(30)日公布國內新增56例COVID-19確定病例，分別為55例本土及1例境外移入；另確診個案中新增5例死亡。\$\@\$指揮中心表示，今日新增之55例本土病例(其中27例為居家隔離期間或期滿檢驗陽性者)，為30例男性、25例女性，年齡介於未滿5歲至80多歲，發病日介於今(2021)年6月20日至6月29日。個案分布以新北市23例最多，其次為臺北市22例、桃園市5例，高雄市及苗栗縣各2例、屏東縣1例；其中31例為已知感染源、2例關聯不明、22例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增5例死亡個案，為3例男性、2例女性，年齡介於60多歲至70多歲，發病日介於5月24日至6月16日，確診日介於5月25日至6月18日，死亡日介於6月25日至6月28日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至6月28日累計公布13,495位確診個案中，已有10,196人解除隔離，解隔離人數達確診人數75.6%。\$\@\$指揮中心表示，今日新增1例境外移入(案14875)，為印度籍30多歲男性，6月27日自印度來臺，持有搭機前3日內檢驗陰性報告，入境後至集中檢疫所檢疫並採檢送驗，於今日確診；個案在臺期間並無症狀，已匡列接觸者1人，因有適當防護，列自我健康監測。\$\@\$指揮中心統計，截至目前國內累計1,347,513例新型冠狀病毒肺炎相關通報(含1,331,329例排除)，其中14,804例確診，分別為1,172例境外移入(原6月28日公布之本土個案14755，經疫調採檢後改判為境外移入)，13,579例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計102例移除為空號。自2020年起累計 648例COVID-19死亡病例，其中640例本土，個案居住縣市分布為新北市329例、臺北市246例、基隆市21例、桃園市18例、彰化縣10例、臺中市及新竹縣各4例、宜蘭縣及花蓮縣各2例，苗栗縣、臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月30日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
     <t>發佈日期：2021-06-29\$\@\$中央流行疫情指揮中心今(29)日表示，簡訊實聯制的推出，係為方便民眾及商家落實實聯制措施、減少紙本紀錄的接觸，並有助於疫調人員掌握個案相關活動史及匡列接觸者等，相關數據之使用，均有其合法性、正當性、必要性，且絕無違法情事，說明如下：\$\@\$一、 合法性：衛福部依傳染病防治法第37條第1項第6款，公告「嚴重特殊傳染性肺炎(COVID-19)第三級疫情警戒標準及防疫措施裁罰規定」，規定外出時應全程佩戴口罩，並配合實聯制；行政院為遏止疫情擴散，並減少實聯制紙本填寫之接觸，推出「簡訊實聯制」，供民眾及商家使用。\$\@\$二、 正當性：簡訊實聯制係於經得使用人同意下，掃瞄QR code即完成實聯制措施；而「簡訊實聯制」並不會留下個資給店家，所留下的活動史簡訊，電信業者也只保留28天，且僅供指揮中心疫調使用，不會做目的外利用。\$\@\$三、 必要性：在疫調工作中，衛生單位人員須掌握確診個案相關之活動資訊，以即時展開接觸者匡列、環境清消等各項防疫措施，故適當的運用簡訊實聯制相關資訊，對防疫推動有實質的幫助。\$\@\$指揮中心進一步指出，簡訊實聯制自今(2021)年5月19日上線後，於6月3日起啟用實聯制資料調用機制，以供地方政府衛生局有疫情調查需求時，向指揮中心申請調閱，經審核通過後將調閱資料回復，大多數申請調用案件可於一日之內提供資料。截至6月29日，已有宜蘭縣、花蓮縣、南投縣、屏東縣、苗栗縣、桃園市、高雄市、基隆市、新北市、新竹縣、嘉義縣、彰化縣、臺中市、臺北市、臺南市、澎湖縣，共計16縣市政府衛生局調用303項資料，調用量前3名依序為桃園市衛生局、高雄市衛生局、臺中市衛生局。\$\@\$指揮中心強調，「簡訊實聯制」的推出，主要為提供民眾、商家、衛生單位不管是在配合防疫措施或執行疫調工作上便利的平臺，籲請民眾、商家配合，也請地方政府加強稽查，共同落實實聯制，完備疫調工作，達到防疫的目的。</t>
   </si>
   <si>
-    <t>發佈日期：2021-06-29\$\@\$針對媒體報導「COVID-19疫苗接種外展服務，無法選擇疫苗廠牌，係為國產疫苗鋪路」，中央流行疫情指揮中心今(29)日澄清，無法選擇疫苗廠牌，係因目前尚無法確認屆時可供應之疫苗廠牌與數量，並非為國產疫苗鋪路。\$\@\$指揮中心表示，為加速我國COVID-19疫苗接種作業，規劃辦理「COVID-19疫苗接種外展服務」，已於日前發文請各部會先行調查「規模1,000人以上企業」、「100人以上中央政府機關」等人員施打疫苗意願及進行造冊，並由各機關（構）自行評估是否有適合執行接種作業的地點及空間規劃等。\$\@\$有關媒體報導「該公文提到無法選擇疫苗廠牌，係為國產疫苗鋪路」，指揮中心澄清，係因目前尚無法確認屆時可供外展服務之疫苗廠牌與疫苗數量，並非為國產疫苗鋪路。待疫苗量充足，會依屆時可供應之疫苗廠牌與數量，再次詢問機關（構）參與外展服務與接種之意願。\$\@\$指揮中心進一步說明，有關「疫苗外展服務調查」，係為後續疫苗量充足且可全民接種時，疫苗需求量調查與分布之預先規劃。</t>
-  </si>
-  <si>
     <t>發佈日期：2021-06-29\$\@\$中央流行疫情指揮中心今(29)日公布國內新增54例COVID-19確定病例，均為本土個案；另確診個案中新增8例死亡。\$\@\$指揮中心表示，今日新增之54例本土病例(其中17例為居家隔離期間或期滿檢驗陽性者)，為19例男性、35例女性，年齡介於未滿5歲至80多歲，發病日介於今(2021)年6月16日至6月28日。個案分布以新北市22例最多，其次為臺北市20例、桃園市及新竹縣各4例，彰化縣2例，基隆市及屏東縣各1例；其中31例為已知感染源、5例關聯不明、18例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增8例死亡個案，為5例男性、3例女性，年齡介於60多歲至80多歲，發病日介於5月9日至6月19日，確診日介於5月15日至6月20日，死亡日介於6月25日至6月27日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至6月27日累計公布13,435位確診個案中，已有10,086人解除隔離，解隔離人數達確診人數75.1%。\$\@\$指揮中心統計，截至目前國內累計1,311,961例新型冠狀病毒肺炎相關通報(含1,295,813例排除)，其中14,748例確診，分別為1,170例境外移入，13,525例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；個案中累計102例移除為空號。自2020年起累計643例COVID-19死亡病例，其中635例本土，個案居住縣市分布為新北市325例、臺北市245例、基隆市21例、桃園市18例、彰化縣10例、臺中市及新竹縣各4例、宜蘭縣及花蓮縣各2例，苗栗縣、臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月29日新增死亡COVID-19確診個案表.pdf</t>
   </si>
   <si>
@@ -139,10 +865,130 @@
     <t>發佈日期：2021-06-27\$\@\$有關今(6/27)日上午飛往金門航班，某旅客於機場快篩站進行快篩，因第一次篩檢結果無法成為判定的依據，在取得當事人同意後，執行第二次篩檢，呈現陰性，判定快篩結果為陰性，應予放行，另同步通知金門航空站及金門縣衛生局，以確實掌握該旅客情況。該旅客抵達金門後立即執行PCR檢測，經採檢PCR結果亦為陰性。\$\@\$目前本島各機場針對前往離島旅客執行篩檢，仍屬自願性質，並無強迫性，不只顧及防疫，亦能爭取旅客信任，鼓勵更多旅客參與篩檢，對離島的防疫防線更有幫助。惟為避免造成地方疑慮，未來於各機場快篩呈陽性或弱陽性反應之旅客，不再考慮檢驗誤差問題，將進行PCR採檢陰性後，始允許登機。</t>
   </si>
   <si>
-    <t>發佈日期：2021-06-27\$\@\$為保障健康安全，近日民眾踴躍接種COVID-19疫苗，關於疫苗接種後是否產生副作用也有諸多討論。針對網傳COVID-19 mRNA疫苗恐傷害人體，中央流行疫情指揮中心今（27）日澄清，疫苗中的mRNA並不會進入細胞核，不會以任何方式改變人體的DNA，或與DNA產生交互作用。而政府也會嚴格把關疫苗安全，民眾可安心接種。\$\@\$指揮中心表示，我國目前已核准緊急使用授權的COVID-19疫苗分為兩大類，其中所使用的COVID-19 mRNA疫苗，其作用原理是將含有一段可轉譯成SARS-CoV-2病毒棘蛋白的mRNA注射至體內，接種後會在人體細胞質內製造出SARS-CoV-2病毒棘蛋白，作為疫苗抗原，進而誘發人體產生免疫反應，以對抗SARS-CoV-2病毒，疫苗中的mRNA不會進入細胞核、不會改變人體的DNA，或與DNA產生交互作用。\$\@\$指揮中心重申，我國核准專案輸入的mRNA疫苗，例如莫德納疫苗，是經過衛生福利部食品藥物管理署審查廠商所提供的疫苗品質管制資料、非臨床藥毒理試驗及人體臨床試驗報告，確認疫苗的品質、安全及療效後，始予以核准。\$\@\$指揮中心表示，為確保COVID-19疫苗上市後廣泛臨床使用下國人用藥安全，我國已建立COVID-19疫苗安全資訊主動監控機制，除持續監控國外衛生主管機關發布之COVID-19疫苗安全警訊外，亦設有「疫苗不良事件通報系統(VAERS)」接受各界通報，蒐集、分析及評估我國COVID-19疫苗不良事件，並藉由收集相關安全資訊，監控其安全性，一旦發現具有未知或未預期之風險，立即啟動再評估機制，重新評估其療效與風險，並確認是否需採取相關風險管控措施。\$\@\$指揮中心再次提醒， COVID-19疫苗與其他藥品一樣，或多或少都具有一些副作用，如過敏反應等，民眾接種前應主動提供自己的身體狀況，包括是否對特定藥品過敏、慢性病或正在服用的藥品；女性則需告知是否(或可能)懷孕、準備懷孕或正在哺乳母乳等，供醫師審慎評估其臨床效益及風險。接種後則應關心身體變化，部分民眾接種COVID-19疫苗後，可能會發生接種部位疼痛、紅腫、疲倦、頭痛、肌肉痠痛、體溫升高、畏寒、關節痛及噁心等，這些症狀通常輕微並且數天內消失，但如發生嚴重持續性頭痛、視力改變或癲癇、嚴重且持續腹痛超過24小時以上、皮膚出現自發性出血點、瘀青、紫斑、嚴重胸痛或呼吸困難、下肢腫脹或疼痛等，請立即就醫，並說明疫苗接種史，同時請醫師通報當地衛生局或衛生福利部疾病管制署。</t>
+    <t>發佈日期：2021-06-27\$\@\$中央流行疫情指揮中心今(27)日公布國內新增89例COVID-19確定病例，分別為88例本土及1例境外移入；另確診個案中新增9例死亡。\$\@\$指揮中心表示，今日新增之88例本土病例(其中27例為居家隔離期間或期滿檢驗陽性者)，為48例男性、40例女性，年齡介於未滿5歲至90多歲，發病日介於今(2021)年6月10日至6月26日。個案分佈以新北市41例最多，其次為臺北市33例、臺南市8例、桃園市3例，屏東縣、南投縣及新竹市各1例；其中60例為已知感染源、2例關聯不明、26例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增9例死亡個案，為3例男性、6例女性，年齡介於40多歲至90多歲，發病日介於5月15日至6月22日，確診日介於5月20日至6月25日，死亡日介於6月22日至6月26日；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增1例境外移入個案(案14719)，為本國籍20多歲男性，5月3日曾在奧地利當地檢出COVID-19陽性，6月11日自奧地利返臺，持有搭機前3日內檢驗陰性證明，入境後至防疫旅館檢疫，6月24日進行檢疫期滿前採檢，於今日確診。個案在臺期間並無症狀，相關接觸者匡列中。\$\@\$指揮中心統計，截至目前國內累計1,266,904例新型冠狀病毒肺炎相關通報(含1,250,863例排除)，其中14,634例確診，分別為1,170例境外移入，13,411例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計102例移除為空號。自2020年起累計632例COVID-19死亡病例，其中624例本土，個案居住縣市分布為新北市319例、臺北市243例、基隆市20例、桃園市17例、彰化縣10例、臺中市及新竹縣各4例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月27日新增死亡COVID-19確診個案表.pdf</t>
   </si>
   <si>
     <t>發佈日期：2021-06-26\$\@\$中央流行疫情指揮中心今(26)日表示，目前進口國內之274萬劑莫德納(Ｍoderna) COVID-19疫苗將陸續完成檢驗封緘，預計於今(2021)年7月1日起，陸續配送至地方政府衛生局及指定醫療院所，並開放第一類至第八類對象接種。第一階段預計分配各地方政府衛生局約106萬劑，分兩梯次配送，第一梯次配送約64.3萬劑，預計於7月1日陸續配達，第二梯次配送約41.8萬劑，預計７月８日陸續配達(如附件)。\$\@\$指揮中心指出，第一階段疫苗各地方政府分配數量係以下列原則核估，並將依各地方政府衛生局規劃，配送至衛生局或其指定醫療院所：\$\@\$一、各縣市第五類「居家式和社區式長照機構及身障服務照服員及服務對象」中，尚未接種疫苗之64歲以下與75歲以上服務對象及所有照服員人數總計之6成。\$\@\$二、各縣市第五類「其他機構(含矯正機關工作人員)」尚未接種人數。\$\@\$三、各縣市莫德納(Moderna)COVID-19疫苗已分配數。\$\@\$四、各縣市65-74歲長者30%人口數。\$\@\$另第二階段各地方政府分配數量則以65-74歲長者20%人口數所需疫苗數量核估，將視第一階段疫苗接種情形配發。\$\@\$指揮中心說明，有關第七類對象「維持國家安全及社會機能正常運作者」是經由各中央目的事業主管機關認定，並依據其感染風險決定為優先接種對象後進行造冊，列為首波接種之國家關鍵設施或維持設社會正常運作必要工作人員。上述對象的疫苗需求量，原則直接配送至各部會指定之COVID-19合約醫療院所，各醫療院所可視接種量能，透過原預約機制，或安排於特定時段集中接種。惟莫德納(Moderna) COVID-19疫苗於2-8℃配達後僅能保存28天，請第七類對象於預約日或接獲通知日期後，儘速前往接種，以利指揮中心視各醫療院所接種情形與庫存量，通知醫療院所逐續開放其他類對象接種，發揮COVID-19疫苗最大效益。\$\@\$指揮中心表示，第一階段配送之莫德納(Ｍoderna) COVID-19疫苗為美國提供之250萬劑其中一部分，將以2-8℃溫層配送，其包裝為每瓶14劑，10瓶一盒，接種單位可針對當日最後一瓶疫苗開瓶的剩餘劑，規劃候補名單機制，有效利用COVID-19疫苗。\$\@\$指揮中心提醒，為確保疫苗接種安全，建議先前曾因接種疫苗或任何注射治療後發生急性過敏反應的民眾，接種後請於接種處或附近留觀至少30分鐘，一般民眾則建議至少留觀15分鐘，並自我密切觀察15分鐘，以利即時處置該類急性過敏反應。\$\@\$指揮中心強調，依據各國疫苗上市後的安全性監測，曾有報告極少數年輕族群在接種mRNA 疫苗後發生心肌炎等不良反應事件，大多發生在接種後數天內，請民眾在接種mRNA 疫苗後如出現胸痛、喘或心悸等症狀，應立即就醫並說明疫苗接種史。 附件\$\@\$附件-274萬劑Moderna疫苗分配量.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-26\$\@\$中央流行疫情指揮中心今(26)日表示，有關屏東COVID-19 Delta印度變異株群聚及其相關感染事件，目前累計12例確定病例，其中6例經基因定序後，均為Delta印度變異株，分別為秘魯境外移入確診祖孫2人(案13332、13333)及案14298、14407、14408、14409。\$\@\$指揮中心指出，該起群聚事件指標個案為當地白牌司機(案14298)，經疫調及接觸者採檢後，發現1位工作接觸者(案14409)確診，而案14409之2位家人(案14407、14408)亦同時確診，其中案14407曾於6月11日、6月14日與秘魯境外移入案13332有短暫接觸，其餘事件相關確診個案均為家庭或活動之接觸者採檢後確診。為避免感染擴大，指揮中心已採取相關應變措施如下：\$\@\$一、精準疫調並擴大匡列接觸者及採檢，另接觸者安排防疫旅館落實隔離，並於居隔期滿前採檢，截至6月25日案14298群聚相關接觸者匡列136人、共居家隔離99人、自主健康管理匡列32人，自我健康監測5人，其中已採檢124人，PCR檢驗陽性9人、陰性115人，接觸者持續擴大匡列中。\$\@\$二、6月24日起於當地設置社區篩檢站，籲請足跡重疊民眾篩檢，並加強民眾溝通配合篩檢，截至6月25日PCR篩檢共419人皆為陰性；另針對確診個案公布社區足跡點，並完成公共場所消毒。\$\@\$三、當地醫療院所加強通報及感染管制措施，請醫師協助有疑似症狀就醫民眾轉介採檢院所通報及採檢。\$\@\$四、透過廣播系統呼籲民眾落實疫情三級警戒規範，外出與工作均要全程佩戴口罩，嚴查避免群聚，另針對當地超市、超商、餐飲業、傳統市場等場所關閉三天。\$\@\$五、給予確診個案妥善臨床照護處置，如符合單株抗體、瑞德西韋使用條件則即時使用；如有出現重症前兆，迅速進行處置及治療。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-26\$\@\$中央流行疫情指揮中心今(26)日表示，為因應6月27日起，自COVID-19變異株「重點高風險7國(巴西、印度、英國、祕魯、以色列、印尼及孟加拉)」以外之國家入境旅客(過去14天旅遊史、含轉機)住宿需要，將開放集中檢疫所供民眾自費使用，於今日晚間8時開放訂房。\$\@\$指揮中心指出，目前全臺有49處集中檢疫所，分布於北、中、南等三區，包括各類公務人員訓練中心、軍營、停招的學校宿舍、旅館等，每人每日新臺幣2,000元整，12歲以下幼童與父或母同住一室者，不另外收費。\$\@\$指揮中心說明，民眾入住之檢疫所地點須由指揮中心分派，房內皆有網路、電視等相關設備，入住民眾亦可使用自己的手機電話與外界聯繫；集中檢疫場所均有提供三餐，餐飲會於固定時間送到檢疫房間外，再由民眾自行取用至自己的檢疫房間內用餐。\$\@\$指揮中心提醒，集中檢疫所預定今日晚間8時開放訂房，有意自費入住民眾可至「入境檢疫系統」網頁預約，預約者須於航班預計抵臺48小時前至入境檢疫系統預約、繳費，以取得預約訂房識別碼，作為入境登記使用。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-26\$\@\$中央流行疫情指揮中心今(26)日表示，5月9日前已完成第一劑AstraZeneca COVID-19疫苗接種之民眾，皆可於接種後第10至12週公費接種第二劑。專家建議AstraZeneca COVID-19疫苗接種間隔10至12週再接種第二劑疫苗，效益更佳。若有出國急迫性須於8至10週間接種者，亦可酌情提供接種。前述對象均可至各合約醫療院所預約接種，亦建議優先考量原接種醫院，或可至疾病管制署旅遊醫學合約醫院。\$\@\$指揮中心說明，截至6月24日止，已有3.3萬人完成兩劑AstraZeneca COVID-19疫苗接種，為使民眾獲得最大免疫保護力，請4月12日至5月9日期間已接種第一劑疫苗之民眾，於接種日起間隔第10-12週後，透過各醫院預約系統預約接種第二劑疫苗。為確保該等對象第二劑AstraZeneca COVID-19疫苗接種之權益，指揮中心將依據4月12日至5月9日每週AstraZeneca COVID-19疫苗接種量，自本週起4週內，每週配送至指揮中心指定之COVID-19疫苗合約醫療院所，預計全臺4週配送量約6.9萬劑。民眾可優先於原接種醫院預約，或可至疾管署旅遊醫學合約醫院接種（院所名單詳見附件，將視各院接種與開放情形適時調整）。\$\@\$指揮中心提醒，前往接種前務必確認備妥「COVID-19疫苗接種紀錄卡」及「健保卡」，若「COVID-19疫苗接種紀錄卡」已遺失，民眾可返回第一劑接種之醫療院所補發，並完成第二劑接種。指揮中心進一步說明，國外臨床試驗資料分析顯示，完成兩劑AstraZeneca COVID-19疫苗接種且間隔 12 週以上，保護力可達81%，籲請民眾可於第一劑接種10-12週後，完成第二劑接種，使疫苗發揮最大效益。 附件\$\@\$有開設旅遊醫學門診之醫療院所名單.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-24\$\@\$中央流行疫情指揮中心今(24)日表示，「民眾使用COVID-19家用快篩試劑指引」已於6月19日公布(詳如新聞稿附件)。為利民眾居家正確自行檢測，指揮中心再次提醒民眾使用家用快篩試劑相關流程與注意事項。\$\@\$指揮中心指出，COVID-19家用快篩試劑可由醫療器材販賣業者、藥粧店、醫療器材行、便利商店等或藥局販售，民眾購買時，請確認產品名稱是否有「家用」、包裝是否刊載「防疫專案核准製造第XXXXXXXXXX號」或「防疫專案核准輸入第XXXXXXXXXX號」等字樣(已核准之家用快篩試劑名單可至衛生福利部食品藥物管理署[下稱食藥署]網站確認)、產品效期是否在有效期間或保存期限內，並依使用說明書或操作影片進行採檢及操作。對使用家用快篩試劑有任何疑問，可洽詢販售該產品之醫療器材商或藥局，或逕洽詢試劑廠商。\$\@\$指揮中心說明，居家隔離或居家檢疫者如測出結果為陽性時，請立即與當地衛生局聯繫，或撥打1922，依指示方式處理；非居家隔離且非居家檢疫者測出結果為陽性時，請戴好口罩，勿搭乘大眾運輸工具，儘速至鄰近的社區採檢院所進一步檢測，並將使用過之採檢器材用塑膠袋密封包好，一併攜帶至社區採檢院所，交予院所人員。當測出結果為陰性時，仍請遵循指揮中心的防疫規範，做好個人防護，持續自我健康管理，採檢完之家用快篩試劑及試劑棒勿任意棄置，請以塑膠袋密封包好，以一般垃圾處理。\$\@\$指揮中心提醒，若民眾已出現嚴重特殊傳染性肺炎相關症狀，不宜使用COVID-19家用快篩試劑自行在家檢測，應佩戴醫用口罩，儘速前往醫療院所就醫，且前往就醫時勿搭乘大眾運輸工具。另外，提醒居家快篩試劑測試結果可能出現偽陰性或偽陽性，仍需經認可實驗室所進行的「核酸檢測」作為診斷COVID-19感染之依據。COVID-19家用快篩試劑產品核准名單、說明書及操作影片均可至食藥署網站( http://www.fda.gov.tw )之業務專區 &gt; 醫療器材 &gt; COVID-19 防疫醫材專區 &gt; 家用新型冠狀病毒檢驗試劑專區查詢。 附件\$\@\$附件-民眾使用COVID-19家用快篩試劑檢驗指引.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-24\$\@\$中央流行疫情指揮中心今(24)日公布國內新增130例COVID-19確定病例，分別為129例本土個案及1例境外移入；另確診個案中新增6例死亡。\$\@\$指揮中心表示，今日新增之129例本土病例(其中73例為居家隔離/檢疫期間或期滿檢驗陽性者)，為64例男性、65例女性，年齡介於未滿5歲至90多歲，發病日介於今(2021)年6月4日至6月23日。個案分佈以新北市54例最多，其次為臺北市35例、基隆市9例、桃園市7例、屏東縣及高雄市各6例、苗栗縣及新竹縣各5例、南投縣2例。其中雙北地區以外縣市40例中，38例為已知感染源，2例關聯不明；相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增6例死亡個案，為男性5位、女性1位，年齡介於50多歲至90多歲，發病日介於5月11日至6月4日，確診日介於5月15日至6月5日，死亡日介於6月18日至6月23日，詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至6月22日累計公布12,958位確診個案中，已有9,288人解除隔離，解隔離人數達確診人數71.7%。\$\@\$指揮中心表示，案14386為本國籍60多歲女性，於6月9日自巴西返臺，持有登機前3日內檢驗陰性報告，入境後至集中檢疫所檢疫，6月22日檢疫期滿前採檢，於今日確診。個案在臺期間並無症狀，檢疫期間未與他人接觸，故無匡列接觸者。\$\@\$指揮中心統計，國內累計1,180,033例新型冠狀病毒肺炎相關通報(含1,164,226例排除)，其中14,389例確診，分別為1,167例境外移入，13,169例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另新增1例空號病例(案10029)，累計102例移除為空號。自2020年起累計605例COVID-19死亡病例，其中597例本土，個案居住縣市分布為新北市304例、臺北市237例、基隆市19例、桃園市15例、彰化縣9例、臺中市4例、宜蘭縣、新竹縣及花蓮縣各2例，臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月24日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-24\$\@\$中央流行疫情指揮中心今(24)日表示，為精進臺北農產運銷公司COVID-19群聚感染事件相關防疫作為，於昨(23)日晚間再次召開會議，與農委會、雙北市政府、雙北農產/果菜運銷公司進行專業溝通及討論「市場專案」各項細節，並於會中達成三點共識如下：\$\@\$一、自6月24日零時起，雙北批發市場所有從業人員未持有陰性檢驗證明者不得進場，請雙北市協調警力於現場維持秩序；另亦設置快篩站至6月24日零時，提供尚未篩檢者快篩服務。\$\@\$二、落實疫調、找出熱區：指揮中心將蒐集本案相關疫調資訊，並與雙北市政府、臺北農產運銷股份有限公司及新北市果菜運銷股份有限公司建立疫調資料交流機制，儘速釐清造成此波感染事件之問題及劃分疫情熱區，以利批發市場、零批市場及周遭傳統市場執行後續防疫因應作為。\$\@\$三、考量多有跨縣市至雙北批發市場之工作者，為即時發覺潛在個案，有效阻斷傳播鏈，確診個案由居住地縣市進行精準疫調及接觸者匡列作業，其中職場接觸者匡列由職場所在縣市進行。另疾管署將成立平台協助各地方政府整合資訊，讓疫調更加完整。\$\@\$指揮中心進一步說明，考量快篩或PCR檢驗陰性僅代表個案現階段不具病毒傳播力，雙北批發市場所有從業人員亦應持續落實動線分流、人員降載等相關防疫措施，減少傳播風險；另請臺北農產運銷股份有限公司、新北市果菜運銷股份有限公司針對從業人員進行健康監測，以及早掌握可能個案，並及時進行各項防治措施。\$\@\$指揮中心強調，本專案結束後，將持續設置篩檢站三週，提供周邊攤商及社區民眾就近篩檢，達到社區清零目的。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-23\$\@\$中央流行疫情指揮中心今(23)日表示，針對臺北農產運銷公司發生COVID-19群聚感染事件，指揮中心於昨(22)日召開會議，與農委會、臺北市政府、臺北農產運銷公司共同討論疫情狀況並研商「市場專案」強化相關防疫作為，積極協助地方政府及廠商進行防疫，避免感染擴大。相關措施如下：\$\@\$一、啟動「市場專案」快速全面篩檢，確保雙北批發市場從業人員防疫安全，避免傳播至家戶及社區之風險，並以社區儘速清零為目標。\$\@\$二、自6月24日零時起，雙北批發市場所有從業人員未持有6月20日以後檢驗陰性證明者不得進場，且規定須於完成篩檢後方得接種COVIID-19疫苗。\$\@\$三、為提升雙北批發市場各從業人員篩檢意願，篩檢站設置應鄰近市場並配合其作業時間；專案結束後，仍延長篩檢站設置時間，以利周邊攤商及社區民眾就近篩檢，以社區清零。\$\@\$四、為加快篩檢速度且減少偽陰性及偽陽性情形，建議僅進行PCR採檢，提升篩檢作業效率；如檢驗陽性者，請地方政府衛生局落實後續疫調及接觸者匡列工作，並請提供疾管署彙整轉送居住地縣市，以進行後續疫調及匡列作業。\$\@\$五、考量雙北批發市場貨車司機及隨車捆工停留於市場時間較短暫，該類人員之篩檢、疫調及接種作業，將請臺北農產運銷公司提供人員名冊，由指揮中心轉居住地縣市政府辦理。\$\@\$六、推動北北基桃批發市場從業人員逐步施打疫苗，以雙北批發市場優先實施，所需疫苗均由指揮中心提供。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-23\$\@\$中央流行疫情指揮中心今(23)日公布國內新增104例COVID-19確定病例，均為本土個案；另確診個案中新增24例死亡。\$\@\$指揮中心表示，今日新增之104例本土病例，為45例男性、59例女性，年齡介於未滿5歲至80多歲，發病日介於今(2021)年6月10日至6月22日。個案分佈以新北市45例最多，其次為臺北市22例，高雄市及新竹縣各9例，桃園市7例，苗栗縣4例，基隆市3例，宜蘭縣2例，彰化縣、南投縣及屏東縣各1例。其中雙北地區以外縣市37例中，28例為已知感染源，5例關聯不明，4例疫調中；相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增24例死亡個案，為男性15位、女性9位，年齡介於40多歲至80多歲，發病日介於4月11日至6月14日，確診日介於4月13日至6月16日，死亡日介於6月13日至6月21日，詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至6月21日累計公布12,879位確診個案中，已有9,041人解除隔離，解隔離人數達確診人數70.2%。\$\@\$指揮中心統計，截至目前國內累計1,148,916例新型冠狀病毒肺炎相關通報(含1,133,240例排除)，其中14,260例確診，分別為1,166例境外移入，13,041例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；新增1例空號病例(案14228)，累計101例移除為空號；自2020年起累計599例COVID-19死亡病例，其中591例本土，個案居住縣市分布為新北市301例、臺北市235例、基隆市19例、桃園市15例、彰化縣9例、臺中市4例、宜蘭縣及新竹縣各2例，臺東縣、雲林縣、高雄市及花蓮縣各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月23日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-22\$\@\$中央流行疫情指揮中心今(22)日表示，我國於今(2021)年6月18日及6月20日共計進口274萬劑莫德納(Moderna) COVID-19疫苗，預計於7月1日起配送至地方政府衛生局及指定醫療院所。自7月1日起，國內COVID-19疫苗接種對象(不限廠牌)擴增如下：\$\@\$1.第一類對象，醫事人員(包含醫事執登人員及醫事機構非醫事人員)\$\@\$2.第二類對象，中央及地方政府防疫人員、第一線處理大體之工作人員\$\@\$3.第三類對象，高接觸風險第一線工作人員\$\@\$4.第四類對象，因特殊情形必要出國者(因公出國者、外交駐臺員眷、代表國家出國之運動員或選手)\$\@\$5.第五類對象，包括「住宿型長照機構住民及其照護者」、「居家式和社區式長照機構及身障服務照服員及服務對象」、「其他機構(含矯正機關工作人員)」及洗腎患者，以及「矯正機關（構）工作人員」\$\@\$6.第六類對象，包括75歲以上長者及孕婦\$\@\$7.第七類對象，維持國家安全及社會機能正常運作者\$\@\$8.第八類對象，65-74歲長者\$\@\$9.已完成第一劑疫苗者，可依建議接種第二劑之時間，以同廠牌完成接種。\$\@\$指揮中心指出，第一批疫苗預計配送110萬劑，係以下列原則核估各縣市分配數量，並配送至各地方政府衛生局或其指定醫療院所：\$\@\$1.各縣市第五類「居家式和社區式長照機構及身障服務照服員及服務對象」與「其他機構(含矯正機關工作人員)」尚未接種人數\$\@\$2.各縣市莫德納(Moderna)COVID-19疫苗第一劑已分配數\$\@\$3.各縣市65-74歲長者30%人口數\$\@\$指揮中心說明，為確保維持國家及社會正常運作的相關基礎設施不受COVID-19疫情影響，第七類對象需經各中央主管機關認定並造冊，列為國家關鍵設施或維持設社會正常運作必要工作人員，並送指揮中心。經中央主管機關認定符合前述條件並造冊之對象，除了已陸續配送的國防軍事相關人員之外，包括高鐵、臺鐵、油氣水電與通訊等國家關鍵設施必要人員、全國第一線郵務處理人員、國家(含大考)等考試工作人員、高密度接觸孩童的幼兒園與國小安親班教育人員、托育機構人員、各類批發市場與屠宰市場工作人員、科學園區防疫工作人員、媒體第一線採訪工作人員、戶役政系統機房人員等。\$\@\$指揮中心表示，針對疫情較高風險的雙北等縣市，從事保母、計程車駕駛、外送員、國道客運司機、貨運司機、傳統市場合法攤商及賣場（含超商）收銀人員等，共計約50萬人，將特別納入此批COVID-19疫苗實施對象。上述對象的疫苗需求量將直接配送至各部會指定醫療院所。另，基於65-74歲長者一旦感染容易產生嚴重併發症或導致死亡，亦同時開放接種。\$\@\$指揮中心提醒，為確保疫苗接種安全，建議先前曾因接種疫苗或任何注射治療後發生急性過敏反應的民眾，接種後請於接種處或附近留觀至少30分鐘，一般民眾則建議至少留觀15分鐘，並自我密切觀察15分鐘，以利即時處置該類急性過敏反應。\$\@\$指揮中心強調，依據各國疫苗上市後的安全性監測，曾有報告極少數年輕族群在接種mRNA 疫苗後發生心肌炎等不良反應事件，大多發生在接種後數天內，請民眾在接種mRNA 疫苗後如出現胸痛、喘或心悸等症狀，應立即就醫並說明疫苗接種史。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-22\$\@\$中央流行疫情指揮中心今(22)日表示，已於今日上午與各縣市政府完成召開「全國防疫會議」。會議決議如下：\$\@\$一、在維持加強全國三級警戒等相關管制措施下，雙北市疫情已逐步趨緩，惟各縣市仍有零星爆發群聚事件發生，建議各縣市政府持續加強疫調及接觸者追蹤管理，以及早發現個案、控制疫情。另，端午節連假後對疫情之影響部分，目前尚未有相關影響發生，請各地方政府持續密切注意所轄區域疫情發展狀況，進一步強化社區篩檢及病例監測能力，以防止疫情反彈或新一波流行爆發出現。\$\@\$二、有關COVID-19疫情三級警戒期間，社區式長照服務雖暫時停止服務，但居家式長照服務及送餐服務仍會持續提供獨居失能長者。為因應防疫及持續關懷獨居長者生活與健康狀況，指揮中心就強化相關關懷服務訂定「COVID-19疫情三級警戒期間強化獨居長者關懷服務措施」，請各地方政府落實執行，重點包括：\$\@\$(一)強化服務機制部分：由地方政府整合社政、衛政、民政、警政單位及民間團體之力量，重新盤整資源，強化人力調度、支援及緊急處理機制。針對超過24小時聯繫未果之長者，建立緊急處理啟動機制結合網絡資源前往實地訪視。\$\@\$(二)加強關懷服務部分：針對列冊需關懷之獨居長者，由地方政府透過既有關懷服務體系，或協調由社區照顧關懷據點之專職人力及志工排班，每隔1日定時以電話或其他通訊方式關懷長者，了解其生活及健康狀況。針對暫未使用服務之長者，亦列為關懷對象，由地方政府協調照管中心、長照服務提供單位與鄰里資源，每隔1日定時以電話或其他通訊方式關懷長者。\$\@\$三、疫苗配發及接種：\$\@\$(一)指揮中心表示，有關各地方政府及外界關注之AZ疫苗自費施打第1劑之對象，其第2劑部分，以公費實施接種；另第1劑和第2劑施打不同廠牌疫苗部分，指揮中心目前建議第1劑、第2劑以施打同樣廠牌疫苗為主，不建議混合施打。\$\@\$(二)針對部分縣市將里鄰長納入第2類優先施打對象部分，指揮中心再次向地方政府説明，里鄰長等對象如確有實際執行居家檢疫、居家隔離等高風險對象之追蹤關懷、送餐、訪視等第一線工作，可納入第2類人員，請各地方政府確實查核，並應完成造冊作業。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-22\$\@\$中央流行疫情指揮中心今(22)日表示，衛生福利部傳染病防治諮詢會預防接種組(ACIP)於6月20日召開第3次臨時會議，專家針對COVID-19疫苗工作小組歷次會議進行確認，討論COVID-19疫苗公費接種對象，經考量孕婦為 COVID-19 感染後容易產生嚴重併發症或導致死亡之族群，為保障懷孕婦女及胎兒健康，建議孕婦應接種COVID-19 疫苗並納入第六類優先接種對象。\$\@\$指揮中心指出，依據現階段國內外疫情及疫苗供貨情形，目前開放實施對象包括第一類至第三類、第五類之「住宿型長照機構住民及其照護者」、「洗腎患者」及第六類「75歲以上長者」及「孕婦」。此外提醒已接種第一劑AZ COVID-19疫苗者，請於間隔10至12週後完成第二劑接種，使疫苗發揮最大效益；指揮中心亦將於6月23日再就4月12日至5月9日前已接種第一劑之人數進行疫苗配發，以使民眾可陸續完成第二劑接種。\$\@\$另指揮中心進一步說明，莫德納(Moderna) COVID-19疫苗現階段作業為開放第一類至第三類人員及孕婦接種，惟顧及孕婦胎兒狀況及多重健康狀況考量，建議孕婦接種前應與醫師就風險效益詳細評估後，擇適合廠牌進行接種。\$\@\$指揮中心強調，將持續視疫情狀況及疫苗供貨情形，滾動調整開放接種實施對象，保障民眾接種權益，守護民眾健康。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-22\$\@\$中央流行疫情指揮中心今(22)日公布國內新增79例COVID-19確定病例，其中78例為本土個案，另有1例境外移入；另確診個案中新增6例死亡。\$\@\$指揮中心表示，今日新增之78例本土病例，為35例男性、43例女性，年齡介於未滿5歲至90多歲，發病日介於今(2021)年6月14日至6月21日。個案分佈以新北市43例最多，其次為臺北市25例，南投縣3例，基隆市2例，苗栗縣、彰化縣、桃園市、臺中市及新竹縣各1例。其中雙北地區以外縣市10例中，8例為已知感染源，2例關聯不明；相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增6例死亡個案，為男性3位、女性3位，年齡介於50多歲至80多歲，發病日介於5月19日至6月19日，確診日介於5月28日至6月21日，死亡日介於6月17日至6月21日，詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至6月20日累計公布12,806位確診個案中，已有8,087人解除隔離，解隔離人數達確診人數63.2%。\$\@\$指揮中心表示，今日新增1例境外移入個案（案14257）為本國籍50多歲男性，長期於印尼工作，6月20日返臺，持有搭機前3日內檢驗陰性報告，入境後至防疫旅館居家檢疫，6月21日出現喉嚨痛等症狀，由衛生單位安排就醫採檢，於今日確診。個案檢疫期間無接觸他人，故無匡列接觸者。\$\@\$指揮中心統計，截至目前國內累計1,107,543例新型冠狀病毒肺炎相關通報(含1,091,972例排除)，其中14,157例確診，分別為1,166例境外移入，12,938例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；新增2例空號 (案10380、案14131)，累計100例移除為空號；自2020年起累計575例COVID-19死亡病例，其中568例本土，個案居住縣市分布為新北市291例、臺北市223例、基隆市18例、桃園市15例、彰化縣9例、臺中市4例、宜蘭縣及新竹縣各2例，臺東縣、雲林縣、高雄市及花蓮市各1例；另7例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月22日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-19\$\@\$中央流行疫情指揮中心今(19)日表示，將自今(2021)年6月23日起，陸續配發AZ COVID-19疫苗至地方政府衛生局，提供先前已接種第一劑AZ COVID-19疫苗的民眾完成兩劑疫苗接種，以提升免疫保護力。\$\@\$指揮中心說明，截至6月18日止，已有2.7萬名民眾完成兩劑AZ COVID-19疫苗接種，核估目前可調度的剩餘疫苗數量，可提供4月12日至5月9日以前約6.7萬名已接種第一劑疫苗的民眾繼續接種第二劑AZ COVID-19疫苗，並視疫苗供應及接種情形，適時調整疫苗配發進度。\$\@\$指揮中心表示，根據世界衛生組織( World Health Organization, WHO)與醫學期刊「刺胳針」(The Lancet)等國外臨床試驗資料分析顯示，完成兩劑AZ COVID-19疫苗(間隔 80 天)的追蹤結果證實，可預防6成以上有症狀感染之風險；當接種間隔 12 週以上且完成 2 劑接種，保護力可達 81%。基此，我國衛生福利部傳染病防治諮詢會預防接種組（ACIP）專家建議兩劑AZ COVID-19疫苗接種間隔至少8週，而間隔10至12週再接種第二劑疫苗的效益更佳，故指揮中心籲請民眾可於第一劑接種後10-12週完成第二劑接種，使疫苗發揮最大效益。\$\@\$指揮中心提醒，為確保疫苗接種安全，建議先前曾因接種疫苗或任何注射治療後發生急性過敏反應的民眾，於接種後請在接種處或附近留觀至少30分鐘，一般民眾則建議至少留觀15分鐘，並自我密切觀察15分鐘，以利即時處置該類急性過敏反應。\$\@\$指揮中心也提醒民眾，接種AZ COVID-19疫苗後的28天內，如有發生嚴重持續性頭痛、視力改變、癲癇、嚴重且持續腹痛超過24小時以上、嚴重胸痛或呼吸困難、下肢腫脹或疼痛、皮膚出現自發性出血點、瘀青、紫斑等任一症狀，應儘速就醫，並告知疫苗接種史，以利醫師及早釐清病因，並給予適當的臨床處置。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-19\$\@\$中央流行疫情指揮中心今(19)日公布國內新增128例COVID-19確定病例，分別為127例本土個案及1例境外移入；確診個案中新增20例死亡。\$\@\$指揮中心表示，今日新增之127例本土病例，為60例男性、67例女性，年齡介於未滿5歲至90多歲，發病日介於今(2021)年6月3日至6月18日。個案分佈以新北市81例最多，其次為臺北市30例，桃園市8例，新竹縣3例，新竹市、基隆市各2例，臺中市1例。其中雙北地區以外縣市16例中，12例為已知感染源、4例關聯不明；相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增20例死亡個案，為男性10位、女性10位，年齡介於50多歲至90多歲，發病日介於5月13日至6月12日，確診日介於5月20日至6月17日，死亡日介於6月10日至6月16日，詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至6月17日累計公布12,385位確診個案中，已有7,189人解除隔離，解隔離人數達確診人數58%。\$\@\$指揮中心表示，今日新增1例境外移入，為本國籍10多歲男性，5月25日曾於印度確診，6月5日自印度返臺，持有搭機前3日內檢驗陰性證明，入境時採檢陰性，後至集中檢疫所檢疫，6月18日檢疫期滿前採檢，於今日確診(Ct值37)。個案檢疫期間並無症狀，亦無接觸他人，故無框列接觸者。\$\@\$指揮中心統計，截至目前國內累計1,044,211例新型冠狀病毒肺炎相關通報(含1,028,898例排除)，其中13,896例確診，分別為1,163例境外移入，12,680例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另新增3例空號(案6822、案13764、案13800)，累計98例移除為空號。自2020年起累計538例COVID-19死亡病例，其中531例本土，個案居住縣市分布為新北市265例、臺北市215例、基隆市17例、桃園市15例、彰化縣8例、臺中市4例、宜蘭縣及新竹縣各2例，臺東縣、雲林縣及高雄市各1例；另7例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月19日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-18\$\@\$中央流行疫情指揮中心今(18)日表示，已於今日上午與各縣市政府完成召開「全國防疫會議」。會議決議如下：\$\@\$一、考量目前國內社區傳播風險仍然存在，請高風險地區持續辦理擴大社區篩檢，雙北部分，建議社區篩檢站設置可以民眾就醫可近性為考量，發生零星案例之地方政府建議加強接觸者追蹤管理，以防堵疫情擴散；另請地方政府持續強化輕症個案之健康監測與轉診效率，尤其針對弱勢族群及獨居老人應提供主動關懷。另對於目前確診病例數持續緩降，爰請各地方政府回復著重疫調及接觸者追蹤管理作業，以利及早發現個案，降低死亡發生。\$\@\$二、疑似感染 COVID-19 之死亡案例死因相驗原則：\$\@\$1.關於相驗，現行法規適用無疑。\$\@\$2.疫情期間猝死個案一律PCR採檢，現階段由雙北地區先施行。\$\@\$3.PCR採檢執行部分：行政相驗由醫師執行，司法相驗由法醫採檢。\$\@\$4.相關檢驗費用由公務預算支出。\$\@\$三、診所辦理自費快篩收治指引及收費標準：\$\@\$1.檢驗方法：以抗原快篩為初篩方法，若為抗原快篩陽性，需以核酸檢驗進行確認。\$\@\$2.檢驗試劑：經食藥署核准防疫專案製造或輸入的SARS-CoV-2抗原快速檢驗試劑，提醒在購買及使用皆須事先確認是否符合相關法規。\$\@\$3.採檢人員：依據傳染病防治法第46條第1項第1款，確定病例的檢體，應該由醫師採檢為原則；疑似病例或社區通報採檢病例的咽喉或鼻咽拭子等接觸者檢體，則不限由醫師採檢，得由醫師或其他醫事人員採檢。\$\@\$四、疫苗配撥及施打部分：\$\@\$1.再次重申疫苗施打目標族群請依指揮中心造冊之對象，依序進行施打，避免造成施打亂象。至於各地方政府提出納入COVID-19疫苗接種對象之相關建議部分，指揮中心均會就各類人員可能受感染風險狀況，作為納入公費施打對象之評估與考量。\$\@\$2.鑒於天氣炎熱，對於年長者施打疫苗部分，請各地方政府儘量安排在地區診所或社區注射站進行，也可運用機動快打方式為長者提供施打服務，避免讓年長者因行程往返造成身體不適情形。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-18\$\@\$中央流行疫情指揮中心今(18)日表示，為保障國人接種COVID-19疫苗權益，指揮中心持續監測疫苗接種後不良事件，並於今日邀集專家就「疫苗不良事件通報系統(VAERS)」通報的COVID-19疫苗接種後死亡個案進行討論。指揮中心表示，截至目前為止，尚未有死亡個案被判定為與疫苗相關。\$\@\$指揮中心統計，截至6月17日為止，國內接種AstraZeneca COVID-19疫苗共計1,273,121人次，其中229,566人次為75歲以上長者。又目前VAERS已收到25例接種AstraZeneca COVID-19疫苗後死亡之報告，其中20例發生在75歲以上長者，死亡個案絕大多數均為高齡長者且有慢性疾病；部分個案經司法相驗解剖後，初步死因與心血管疾病或慢性病史相關，惟迄目前為止，尚未有死亡個案被判定為與疫苗相關，指揮中心將持續監測疫苗接種後不良事件，偵測安全疑慮並做出因應。\$\@\$此外，指揮中心亦針對近期高齡者接種COVID-19疫苗，提供以下建議：\$\@\$1. 對於近期身體具狀況或慢性病情不穩定者，建議身體狀況較穩定後再接種。\$\@\$2. 近期天氣炎熱，考量長者身體狀況，建議避開高溫時段前往接種。\$\@\$3. 現有開放診所及衛生所可接種疫苗，建議就近前往接種。\$\@\$指揮中心提醒，所有符合目前開放疫苗接種順序的民眾，皆能依照各縣市政府的說明接種COVID-19疫苗，除了保護個人免於罹病，更可建立群體對COVID-19的免疫力，避免疾病傳播。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-16\$\@\$中央流行疫情指揮中心今(16)日指出，近日有媒體報導「國光在疫苗研發上，疑因試驗基準不公而慘遭淘汰」及「聯亞遭受衛福部刁難，所提的第三期臨床試驗替代方案遭漠視」等相關訊息，指揮中心嚴正澄清，衛生福利部食品藥物管理署(下稱「食藥署」)及財團法人醫藥品查驗中心(下稱「醫藥品查驗中心」)對於國內COVID-19疫苗臨床試驗計畫申請，皆採取一致性審查標準，包括諮詢輔導、召開週會及專家會議均一視同仁，秉持公平公正，提供最合適、最可行之法規科學建議，並無偏袒特定廠商。\$\@\$指揮中心表示，有關國光公司申請第二期臨床試驗一事，食藥署已於110年2月9日函復廠商審查結果，也於函中敘明食藥署之考量，絕無審查不公相關情事。另，有關報導所提聯亞公司提出「圈選接種 (Ring Vaccination)」的國內第三期臨床試驗規劃，食藥署及醫藥品查驗中心亦於諮詢週會給予相關建議，例如：如何選擇指標個案、樣本數估算、施打及追蹤時程、施打劑數之合理性等，供廠商進行相關評估，但截至目前食藥署仍未收到該廠商後續規劃及申請。\$\@\$指揮中心指出，考量疫情及國際公共衛生緊急需求，為加速國產疫苗及早上市，針對COVID-19疫苗研發及輔導，食藥署及醫藥品查驗中心採滾動式審查機制(rolling review)，並針對重要關鍵製程，派員駐廠監製，協助廠商於研發過程能符合法規要求，以縮短研發及審查時程，並確保疫苗品質、安全及療效。\$\@\$指揮中心表示，該中心採購COVID-19疫苗，包括先前採購國外疫苗，均為預採購模式。此次採購國產疫苗是依據政府採購法第105條第1項第2款「因人民之生命、身體、健康、財產遭遇緊急危難」辦理。惟採購合約細節基於保密要求，相關資訊暫不便對外透露。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-16\$\@\$中央流行疫情指揮中心今(16)日表示，將於6月18日起，配送第二批莫德納(Moderna) COVID-19疫苗73,200劑，同時開放第一類至第三類對象接種，請獲配之合約醫療院所開啟預約掛號服務，提供上述對象預約接種，提升群體免疫力。\$\@\$指揮中心說明，莫德納(Moderna) COVID-19疫苗已於6月9日起陸續提供第一類醫事及非醫事人員接種，截至昨(15)日累計接種3萬7,505人。為儘速提升第二類及第三類對象免疫保護力，將於6月18日起進行第二次配送，同時開放至第三類對象接種。本次疫苗配送量是以各縣市符合第一類至第三類對象中，尚未接種人數接種率４成核估，同時考量疫情風險程度，高風險縣市（臺北市、新北市）分配數量係以尚未接種人數接種率達5成以上計算，總計配送63,200劑。\$\@\$指揮中心表示，另10,000劑疫苗提供交通部認定之第二類及第三類對象所需疫苗量，其中分配給國籍航空機組員5,000劑，含長榮、立榮、華航、華信、台灣虎航、星宇及飛特立等7家公司的駕駛員、空服員與隨機維修員等；另外5,000劑分配給民航航空第一線人員，含桃園機場及相關廠商、民航局、航空站、航管人員、飛機維修、倉儲、地勤及空廚等人員。\$\@\$指揮中心提醒，為確保疫苗接種安全，建議先前曾因接種疫苗或任何注射治療後發生急性過敏反應之民眾，接種後請於接種處或附近留觀至少30分鐘，一般民眾則建議至少留觀15分鐘，並自我密切觀察15分鐘，以利即時處置該類急性過敏反應。另，依據各國疫苗上市後安全性監測，曾有報告極少數年輕族群在接種mRNA 疫苗後發生心肌炎等的不良反應事件，大多發生在接種後數天內，指揮中心特別提醒民眾，接種mRNA 疫苗後，應注意如出現胸痛、喘或心悸等症狀，請立即就醫並說明疫苗接種史。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-15\$\@\$中央流行疫情指揮中心今(15)日表示，有關COVID-19疫苗，在世界各國及世界衛生組織指引中，皆將防疫人員與醫護人員列在優先施打對象，目的是為了執行疾病防治工作保護民眾，維持社會安定；而我國也將此類人員列為優先施打的對象。\$\@\$指揮中心進一步指出，第二類中央及地方政府防疫人員包含對象為：「維持防疫體系運作之中央及地方政府重要官員」、「衛生單位第一線防疫人員」、「港埠執行邊境管制之海關檢查(Customs)、證照查驗(Immigration)、人員檢疫及動植物檢疫(Quarantine)、安全檢查及航空保安(Security)等第一線工作人員」、「實際執行居家檢疫與居家隔離者關懷服務工作可能接觸前開對象之第一線人員(含警察、提送餐等服務之村里長或村里幹事、垃圾清運之環保人員、心理諮商及特殊狀況親訪等人員)」、「實際執行救災、救護人員(指消防隊及民間救護車執行緊急救護技術之第一線人員)」、「第一線海巡、岸巡人員」、「實施空中救護勤務人員」及協助防疫工作之國軍人員，該項下截至6/15已造冊人數計約16.2萬人。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-13\$\@\$中央流行疫情指揮中心今(13)日公布國內新增175例COVID-19確定病例，分別為174例本土及1例境外移入；另確診個案中新增26例死亡。\$\@\$指揮中心表示，今日新增之174例本土病例，為79例男性、95例女性，年齡介於未滿5歲至90多歲，發病日介於今(2021)年5月23日至6月12日。個案分佈以新北市81例最多，其次為臺北市62例，桃園市16例，基隆市7例，彰化縣4例，新竹縣2例，臺中市及花蓮縣各1例。其中雙北地區以外縣市31例中，20例為已知感染源、7例關聯不明、4例調查中；相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增26例死亡個案，共計為男性15位、女性11位，年齡介於50多歲至90多歲，發病日介於5月6日至6月10日，確診日介於5月15日至6月12日，死亡日介於6月4日至6月12日，詳如新聞稿附件。\$\@\$指揮中心指出，今日新增1例境外移入個案(案12924)，為本國籍20多歲男性，4月曾在美國當地檢出COVID-19陽性，5月17日自美國返臺，持有搭機前3日內檢驗陰性報告，入境後至防疫旅館進行居家檢疫，6月11日自費採檢，於今日確診；個案在臺期間並無症狀，已匡列接觸者1人，列居家隔離。\$\@\$指揮中心統計，累計869,247例新型冠狀病毒肺炎相關通報(含846,797例排除)，其中12,921例確診，分別為1,155例境外移入，11,713例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中，另累計92例移除為空號。確診個案中437例死亡。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月13日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-12\$\@\$中央流行疫情指揮中心今(12)日表示，有關日本提供之124萬劑AZ疫苗，已於6月9日發布之新聞稿說明：預計自6月12日起，分階段陸續配送至各地方政府衛生局或指定醫療院所；而各地方政府分配數計算基礎如下（分配表如附件）：\$\@\$1、第一至三類未接種人數的六成。\$\@\$2、長照機構未接種人數的六成（離島加權至八成以上）。\$\@\$3、75歲以上人數的27%（離島加權至九成以上）。\$\@\$4、洗腎患者人數之全數。\$\@\$1至4項合計數扣除已配送莫德納疫苗數，即為各地方政府獲配疫苗數量。\$\@\$指揮中心重申，每批次疫苗配送各地方政府，是以疫情狀況、疫苗數量、接種情形等綜合評估後，訂定分配數計算基礎之公式，對各縣市依比例公平分配，指揮中心也會根據各自縣市之疫情及後續接種情形等狀況分析，滾動檢討並加強配送作業，全力協助地方政府推動疫苗接種作業。 附件\$\@\$附件-1100612-日本提供之124萬劑AZ疫苗各地方政府第一次配送分配表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-12\$\@\$中央流行疫情指揮中心今(12)日表示，首批莫德納（Moderna）疫苗15萬劑中，7.5萬劑已於6月9日配送提供全國COVID-19專責醫療院所(包括設置專責病房或負壓隔離病房或採檢院所)，以提供尚未接種COVID-19疫苗的第一線照顧病患醫事及非醫事人員接種服務，截至昨(11)日累計接種2萬4,869人。\$\@\$指揮中心指出，為使疫苗資源有效運用，並加速接種作業，自今日起同時開放所有第一類對象包含醫院、診所及其他醫事機構等執業登記醫事人員、非醫事工作人員，以及集中檢疫所非醫事人員接種莫德納疫苗。\$\@\$指揮中心表示，依據目前研究顯示，接種兩劑不同技術產製的COVID-19疫苗，第二劑接種後發生不良反應機率及嚴重程度較高，故不建議交替使用，惟若接種第一劑COVID-19疫苗發生嚴重過敏反應或產生任何(含對疫苗成分)嚴重的立即過敏或不良反應，並經通報疫苗不良事件通報系統(VAERS)判定為嚴重反應者，建議經醫師評估後接種不同技術產製的 COVID-19 疫苗，完成後續劑次。\$\@\$指揮中心進一步表示，另依美國疾病管制及預防中心近期針對COVID-19疫苗接種不良反應事件監測發現：「曾有報告極少數年輕族群在接種mRNA疫苗後發生心肌炎的不良反應事件，大多發生在接種後數天內」。由於莫德納COVID-19疫苗屬於mRNA疫苗的一種，因此會在接種意願書上加上下列說明「接種mRNA疫苗後應注意若有發生胸痛、喘或心悸等症狀，請立即就醫並說明疫苗接種史」。接種單位或地方政府衛生局如接獲相關不良反應事件通報，亦請依循相關作業進行通報，以利及時掌握。\$\@\$指揮中心指出，為利接種作業推動及維持社交距離避免群聚，COVID-19疫苗接種後調整留觀時間為15分鐘，自我密切觀察15分鐘；但針對先前曾經因接種疫苗或任何注射治療後發生急性過敏反應之民眾，接種後仍請於接種處或附近留觀至少30分鐘。倘持續發燒超過 48 小時、嚴重過敏反應如呼吸困難、氣喘、眩暈、心跳加速、全身紅疹等不適症狀，亦應儘速就醫，並說明疫苗接種史，以利醫師及早釐清病因，並給予適當臨床處置。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-11\$\@\$中央流行疫情指揮中心今(11)日表示，鑑於國內COVID-19疫情仍未穩定，為避免增加我國檢疫量能及醫療資源的負擔，全國疫情警戒第三級期間，將持續執行「邊境嚴管」措施。\$\@\$邊境嚴管措施，包括(一)未持有我國有效居留證之非本國籍人士，暫緩入境。緊急或人道考量等經專案許可者除外；(二)暫停旅客來臺轉機。指揮中心亦將視國內外疫情及社區防疫執行狀況，適時滾動調整。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-10\$\@\$中央流行疫情指揮中心今(10)日表示，鑒於近日國內疫情嚴峻，我國共計6家企業及民間單位（萬海航運、元大金控集團、臺灣證券交易所/臺灣期貨交易所/臺灣集中保管結算所/中華民國證券櫃檯買賣中心、光合基金會/大肚山產業創新基金會、富邦金控、急診醫學會）集資共同捐贈日本日立公司所生產之「負壓隔離艙」80座，將由衛生福利部轉交各急救責任醫院使用，盼能協助解決為各大急救責任醫院負壓隔離病房不足的問題，提供解決方案。\$\@\$指揮中心說明，經指揮中心醫療應變組王必勝副組長與代理商三顧股份有限公司交涉，日本日立公司鑒於臺灣疫情嚴峻，優先協調部分訂單給予我國採購，並由中華航空公司無償協助運輸工作，今日晚間首批10座已抵達臺灣，剩餘70座將分批於未來三周內陸續送達。\$\@\$指揮中心指出，「負壓隔離艙」可用於室內外、急診或加護病房等處，為確診或疑似病患提供緊急處置、暫留及轉出轉入空間，以減少醫護和病患直接接觸的機會，為我國第一線醫療資源提供直接的保護。正值此疫情艱難時刻，指揮中心感謝各方集結力量、團結抗疫，協助我國疫情防治工作，共同守護第一線醫療人員，指揮中心向各方表達誠摯的感謝，近日將儘快依各醫院需求及疫情狀況，調配運送至各醫院組裝啟用。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-10\$\@\$中央流行疫情指揮中心今（10）日表示，針對臺北市今日上午對COVID-19疫苗接種相關之言論，說明如下：\$\@\$一、    指揮中心指出，所謂4月21日之發文是指揮中心於4月14日與衛生局召開協調會之紀錄，其中一項決議為若合約醫院 COVID-19疫苗庫存量過多，評估無法於效期內用畢，為使疫苗有效運用，可在轄區衛生局人員協助下，將疫苗配送至其他合約醫院、非合約醫療院所或衛生所，需用者儘速使用，調度以一次為限，運送時應符合疫苗冷運冷藏相關規範等；惟當時狀況係因一批疫苗即將於5月底到期，當時開放之公費對象接種意願低，故將疫苗進行靈活配置，於效期前提供開放之公費對象中的需求者接種，以儘速適當使用疫苗。\$\@\$二、    指揮中心進一步說明，自5月下旬起，因疫情致疫苗接種需求大增，指揮中心為保障第一線醫護及防疫人員安全，依ACIP COVID-19疫苗工作小組會議決議，以電子郵件通知地方政府衛生局，自5/24起優先提供第一類至第三類人員接種，並視疫苗庫存量及接種規劃，提供3月22日至4月11日已完第一劑之醫護人員與因公務出國者接種第二劑，此外，必須暫緩「自費對象」以及「第一類至第三類同住者」接種；後續指揮中心撥配疫苗時亦皆限定接種對象，雙北地區以第一類至第三類未曾接種第一劑疫苗的醫事、防疫人員及高接觸風險者為優先接種對象，並未開放其他對象接種。有關好心肝診所接種疫苗的事件，疫苗效期至8月多，應無庫存量過多而無法使用之疑慮，且接種對象是否為開放接種之公費對象，為應釐清之重點。\$\@\$三、指揮中心重申，有關中央政府有850瓶COVID-19疫苗置於臺北市或轄內醫院一事，已於昨(9)日發布新聞稿說明，該等疫苗為指揮中心專案同意列冊施打對象，總計配送650瓶疫苗，其中差距之200瓶係為已送至臺北市立聯合醫院仁愛院區，提供華航機師及機組員接種之疫苗，另80瓶為指揮中心提供中心內各部會及疾管署人員施打，目前剩餘30瓶。\$\@\$四、有關疫苗接種預約系統部分，於這次124萬劑疫苗接種規劃，係以運用現行合約醫療院所預約模式提供民眾接種服務；至臺北市政府所提指揮中心規劃之預約系統，係為大規模接種措施使用，目前正積極測試中。\$\@\$指揮中心強調，疫苗接種政策為全體國民重要權益，相關規定、流程、接種對象及順序均公開透明，如有違法事項絕對依法徹查，嚴正法辦，絕不寬貸，有心人士切勿心存僥倖，以身試法。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-09\$\@\$有關COVID-19疫苗放置臺北市醫院，提供中央造冊之外國使節等施打一事，中央流行疫情指揮中心今(9)日表示，因特殊情形必要出國者，可由各該主管機關提具需求說明、預估接種人數及時程，向中央流行疫情指揮中心以專案方式，申請接種公費COVID-19疫苗。目前已專案申請接種對象包括我國因外交或公務需求奉派出國者、代表我國出國之運動員或參賽選手等。另基於互惠原則，駐臺外交人員及其在臺眷屬亦屬專案同意接種對象。針對此類專案指揮中心會視疫苗進口期程及供應量整體評估提供。\$\@\$指揮中心進一步說明，考量該類專案對象其工作地點多位於臺北市，且其工作性質需分批次接種，故依專案需求，撥配疫苗至單位指定院所，提供該類對象接種；目前撥配及接種狀況如下：\$\@\$一、疾病管制署庫存30瓶，係供該署尚未接種第一劑及須接種第二劑之防疫人員接種，本週預計接種30人次，並依照業務安排陸續完成接種。\$\@\$二、三軍總醫院附設民眾診療服務處計配送70瓶，提供國軍協助防疫旅館消毒之化學兵接種，已全數接種完畢。\$\@\$三、臺北市立仁愛醫院計配送180瓶，係提供華航機師及機組員接種，截至目前約250人尚未接種，預計本週完成接種。\$\@\$四、三軍總醫院北投分院計配送100瓶，供總統護衛等國安人員接種，截至目前，尚有250人未接種，庫存14 瓶，預計本週完成接種。\$\@\$五、臺北醫學大學附設醫院，係提供食品藥物管理署員工接種，已全數接種完畢。\$\@\$六、臺大醫院配送20瓶，供指揮中心委託研究計畫之研究對象使用，已全數接種完畢。\$\@\$七、指揮中心另請臺北市榮民總醫院協助接種外交使節、因公務需求有必要出國者及代表國家出國之運動選手疫苗接種事宜，目前約400人還未接種。\$\@\$指揮中心強調，針對上述指揮中心同意列冊施打對象，總計配送650瓶疫苗，目前已接種共計5,400人次，尚未接種為1,200人次。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-09\$\@\$中央流行疫情指揮中心今(9)日表示，昨(8)日衛生福利部傳染病防治諮詢會預防接種組(ACIP)召開專家會議，討論COVID-19疫苗優先接種順序。會中專家表示，因應國內正處於COVID-19社區流行階段現況，為使醫療、防疫業務正常運作，確保感染後易產生嚴重併發症或導致死亡之對象儘速獲得免疫保護力，同時確保社會及國家設施正常運作，降低疫情造成之衝擊，建議調整「COVID-19疫苗優先接種順序」，將「維持機構及社福照護系統運作」及「75歲以上長者」分別列於第五類及第六類對象，並將「經各主管機關認定之關鍵設施工作人員」、「運輸及倉儲業者」、「高中職以下學校教職員工與校內工作人員」及「幼兒園托育人員及托育機構專業人員」列入第七類「維持國家安全及社會機能正常運作」對象，需報指揮中心同意。\$\@\$指揮中心說明，日本提供我方之124萬劑AstraZeneca COVID-19疫苗完成檢驗封緘後，預計自6月12日起，分階段陸續配送至各地方政府衛生局或指定醫療院所，並依ACIP專家決議之優先接種順序，於本批疫苗開始供應後，同時開放「第一類至第三類尚未接種第一劑疫苗者」、「住宿式長照機構工作人員及住民」、「洗腎患者」及「75歲以上長者」，優先接種COVID-19疫苗。指揮中心將視疫苗供應期程、數量、優先接種對象接種情形及國內外疫情現況，適時調整疫苗分配數量及開放接種對象。\$\@\$指揮中心提醒，為確保疫苗接種安全，建議先前曾經因接種疫苗或任何注射治療後發生急性過敏反應之民眾，接種後請於接種處或附近留觀至少30分鐘，一般民眾則建議至少留觀15分鐘，並自我密切觀察15分鐘，以利即時處置該類急性過敏反應。接種AstraZeneca COVID-19疫苗後28天內，若出現嚴重持續性頭痛、視力改變、癲癇、嚴重且持續腹痛超過24小時以上、嚴重胸痛或呼吸困難、下肢腫脹或疼痛、皮膚出現自發性出血點、瘀青、紫斑等任一症狀，應盡速就醫，並告知疫苗接種史，以利醫師及早釐清病因，並給予適當臨床處置。\$\@\$指揮中心再次感謝日本政府於此疫情艱難，且全球疫苗產能供不應求之際，及時提供這批COVID-19疫苗，給予臺灣國內疫情防治極大幫助。指揮中心謹向日本政府與人民表達誠摯謝忱與感佩。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-09\$\@\$中央流行疫情指揮中心今(9)日澄清，有關媒體報導某臺北診所開放民眾連夜施打 COVID-19疫苗案，指揮中心重申，有關現階段COVID-19疫苗之撥配，係由各地方政府統籌分配予所轄合約醫療院所，針對於合約醫療院所提供接種服務，應符合目前公費接種對象優先順序，雙北地區以第一類至第三類未曾接種第一劑疫苗的醫事、防疫人員及高接觸風險者為優先接種對象；雙北以外之縣市，則以未曾接種疫苗的第一類醫事人員為接種對象，並將視疫苗接種進度，逐步開放至第二、三類及機構對象。另針對3月22日至4月11日已完成第一劑之公費對象，於間隔10至12週後，開放接種第二劑。\$\@\$指揮中心說明，針對媒體所報導之情事，已請臺北市政府衛生局進行瞭解及處理，另指揮中心聲明，合約醫療院所提供接種服務應符相關規範，並落實感染管制相關指引，同時應規劃維持社交距離避免群聚感染。如經查執行其接種作業有違指揮中心相關接種政策或實施對象者，可依傳染病防治法第29條處以30萬至200萬罰鍰；也再次強調中央與地方「標準一致、做法一致、腳步一致」防疫原則，請各地方政府及醫療院所依據指揮中心所訂之COVID-19疫苗接種順序，進行施打作業。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-08\$\@\$中央流行疫情指揮中心表示，今(8)日上午與各縣市政府召開的「全國防疫會議」，決議如下：\$\@\$一、近期國內疫情仍處高峰期，因感染而死亡的個案增加，指揮中心將持續與地方政府掌握及協調醫療資源，迅速應變，請地方政府衛生機關加強設置社區篩檢站，提高民眾採檢可近性，降低社區擴散風險。\$\@\$二、針對端午節連假前後，南北往返的大眾運輸系統購票率以及各觀光景點飯店住房率，指揮中心均與相關部會保持密切聯繫，持續掌握人流狀況，適時強化防疫措施；請各地方政府加強連假期間易造成人潮聚集區域的人流管控，同時呼籲民眾暫緩返鄉，減少人流移動。\$\@\$三、加強及落實移工防疫管理部分：\$\@\$(一) 針對北部電子工廠發生群聚感染案件，指揮中心已成立前進指揮所，協助相關廠區緊急應處，也請地方政府協助企業團體強化因應措施。\$\@\$(二) 勞動部昨(7)日已發布實施「暫停移工轉換至新雇主」，以及「暫緩雇主調派移工至其他廠區工作」作業，力求降低移工人流，並修訂「雇主聘僱移工指引」，增訂「企業因應疫情處置」；勞動部另將儘速發布補助要點，補助雇主因移工隔離以及宿舍降載，所須支出之必要防疫措施費用。\$\@\$四、針對大賣場及傳統市場的人流管制，屬高風險地區的地方政府已加強推動實聯制，並運用身分證單、雙號分流，進行人流管控。此外，經濟部已與地方政府研商擬訂5大措施，以加強傳統市場人流管制，請其他地方政府配合施行。\$\@\$五、針對COVID-19疫苗的分配與接種，請各地方政府及醫療院所依據指揮中心所訂之疫苗接種順序，進行施打作業。\$\@\$六、 經考量疫情進展與防疫量能餘裕，快篩陽性及輕症、無症狀確診者收治原則調整如下：\$\@\$(一) 快篩陽性尚未確診者：雖仍得採居家隔離一人一室，因考量收治量能餘裕已擴大，同意各縣市如量能足夠，得一律安排收住於集中檢疫場所，或加強型防疫旅館，並請地方政府再次盤點相關量能。\$\@\$(二) 輕症、無症狀確診者：應儘速收治於集中檢疫場所及加強型防疫旅館。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-08\$\@\$中央流行疫情指揮中心今(8)日公布國內新增219例COVID-19確定病例，均為本土個案。確診個案中新增22例死亡。\$\@\$指揮中心表示，今日新增之219例本土病例，為117例男性、102例女性，年齡介於未滿5歲至100多歲，發病日介於今(2021)年5月22日至6月7日。以新北市123例最多，其次為臺北市54例，苗栗縣16例，桃園市13例，基隆市8例，彰化縣2例，臺南市、新竹市及臺中市各1例。其中雙北地區以外縣市42例中，36例為已知感染源，6例關聯不明。相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增22例死亡個案，共計為男性15位、女性7位，年齡介於30多歲至100多歲，發病日介於5月13日至5月30日，確診日介於5月18日至6月4日，死亡日介於5月30日至6月7日，詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計698,373例新型冠狀病毒肺炎相關通報(含675,836例排除)，其中11,694例確診，分別為1,148例境外移入，10,493例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另新增16例空號 (案7378、9643、10704、10856、11304、11305、11306、11378、11379、11380、11382、11383、11385、11386、11393、11396)，累計65例移除為空號。確診個案中308例死亡。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月8日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-07\$\@\$疾病管制署今(7)日表示，本(2021)年4月接獲醫院通報，一名住中部之5歲女童流感輕症病患之呼吸道檢體分離出無法次分型之A型流感病毒，經該署進一步檢驗並進行基因定序為H1N2v流感病毒。經調查個案密切接觸者6名，其中3人有類流感症狀，經檢驗均未發現H1N2v流感病毒感染，經邀集農政單位及相關醫學與獸醫專家召開會議討論，依上述現有流行病學調查結果研判，本案應屬散發個案，與國際過去案例類似，無證據顯示有人傳人現象，衛生及農政單位亦將持續加強人類、動物與環境之監測。\$\@\$疾管署指出，這名女童未曾出國，家中從事禽畜養殖業，本年3月12日出現流鼻水及咳嗽症狀，3月13日開始發燒，3月14日因持續發燒而就醫，流感快篩為A型陽性，經醫師評估無需住院，開立流感抗病毒藥劑後返家，目前已康復。4月5日自該名女童呼吸道檢體分離出H1N2v流感病毒，另針對呼吸道感染常見病毒如腺病毒、呼吸道融合病毒、冠狀病毒、腸病毒及鼻病毒等進行檢測，均呈陰性反應。此外，農政單位亦自病例家族經營之養豬場豬隻採集檢體檢驗，結果未檢出H1N2流感病毒。\$\@\$國際間H1N2為存在豬隻的低病原性流感病毒，很少在人群中傳播，但偶爾有人類感染之報告，全球2012-2021年累計30例H1N2v流感確診病例，分布於美洲地區，以美國為多，其次為巴西，病例多具有豬隻暴露史或曾暴露於受汙染環境，並不會透過食用肉品而感染。本次由病患所分離之病毒基因序列，與本土過去於豬隻分離之H1N2流感病毒株最為接近，但不相同，對克流感及瑞樂沙等抗病毒藥物敏感。\$\@\$疾管署提醒，防範新型A型流感，民眾應遵守「5要6不」原則，「5要」：肉類及蛋要熟食、要以肥皂澈底洗手、出現症狀，要戴口罩速就醫並告知職業及接觸史、與禽畜長期接觸者要接種流感疫苗、要均衡飲食及適當運動；「6不」：不生食禽鳥蛋類或製品、不走私及購買來路不明肉品、不接觸或餵食動物、不野放及隨意丟棄動物、不將飼養動物與其他禽畜混居、不去空氣不流通或人潮壅擠的場所。相關資訊可至疾管署全球資訊網（https://www.cdc.gov.tw/），或撥打免費防疫專線1922（或0800-001922）洽詢。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-07\$\@\$中央流行疫情指揮中心今(7)日表示，為促使聘有移工企業落實防疫工作及員工確診應變處置，勞動部採取以下四大措施：\$\@\$一、增訂企業因應疫情之處置：將修訂「因應嚴重特殊傳染性肺炎雇主聘僱移工指引：移工工作、生活及外出管理注意事項」，並自下列規範公告之日起實施：\$\@\$（一）廠區未發生或部分廠區發生疫情時，應備有1人1室隔離空間、工作區及生活區應分艙分流，同產線移工應同一住宿地點、不得任意變動、每天進行員工健康監測由專人確認、追蹤及轉送疑似症狀者採檢並隔離。\$\@\$（二）廠區有1名員工確診後，應即匡列職場密切接觸者，並確實執行居家隔離於有單獨衛浴設備之套房。衍生隔離費用，必要時將由勞動部部分補貼。\$\@\$二、訪查潛在高風險企業：勞動部偕同地方政府已開始訪查，針對產業聘僱移工人數達50人以上宿舍共計1, 168家，預計6月10日訪查完畢。\$\@\$三、補助移工隔離及宿舍降載：勞動部將補助雇主必要防疫措施的部分費用，包括移工採檢後隔離期間費用，及鼓勵雇主降載移工每房居住人數轉住租賃建物、一般旅館或防疫旅館費用，並協調地方政府受理申請。\$\@\$四、加強宣導防疫措施：已於6月6日以「LINE@移點通」主動推播、發布新聞稿、移工權益網站、1955臉書及多國語廣播電臺，呼籲移工非必要不要外出，提醒桃竹苗地區之家事移工，注意自身健康情形，若有症狀或接觸史，儘速登記快篩。\$\@\$指揮中心表示，近期苗栗縣電子廠之移工群聚感染案件，勞動部已駐點前進指揮所現場，協助個案雇主與仲介公司，加強移工防疫及預防感染擴大：\$\@\$一、清理個案宿舍及進出管制：協助清空共用衛浴之移工宿舍，部分移工送集中檢疫所、部分隔離於其他有獨立衛浴房間，其餘人員禁止外出及限制出房門。\$\@\$二、實地關懷移工給予支持：自6月6日起，派駐雙語人員於前進指揮所，協助疫調翻譯，並每日早晚放送廣播關懷移工、關懷每日健康監測狀況，並啟動隔離移工關懷機制，由1955專線雙語人員主動電話關懷隔離移工情緒給予心理支持，及提供防疫包(溫度計、口罩、消毒用品、家鄉零食、1955專線電話、Line@移點通）。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-07\$\@\$中央流行疫情指揮中心今(7)日公布國內新增214例COVID-19確定病例，分別為211例本土個案及3例境外移入個案。確診個案中新增26例死亡。\$\@\$指揮中心表示，今日新增之211例本土病例，為106例男性、105例女性，年齡介於未滿10歲至90多歲，發病日介於今(2021)年5月21日至6月6日。個案分布地區以新北市82例最多，其次為臺北市60例，苗栗縣45例，彰化縣8例，新竹市、桃園市、澎湖縣及基隆市各3例，宜蘭縣、嘉義縣、屏東縣及新竹縣各1例。其中雙北地區以外縣市69例中，64例為已知感染源，1例有萬華區活動史，4例關聯不明。相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增26例死亡個案，共計為男性20位、女性6位，年齡介於50多歲至90多歲，發病日介於5月10日至6月2日，確診日介於5月12日至6月5日，死亡日介於5月31日至6月6日，詳如新聞稿附件。\$\@\$指揮中心表示，今日新增3例境外移入中，案11500、案11501分別為40多歲及20多歲菲律賓籍男性，5月15日來臺工作，持有搭機前3日內檢驗陰性報告，在臺期間並無症狀，6月5日自主健康管理期滿前自費採檢，於今日確診。案11052為本國籍40多歲男性，6月5日自印度返臺，持有搭機前3日內陰性報告，入境時無症狀，入境後至檢疫所集中檢疫並採檢送驗，於今日確診。\$\@\$指揮中心統計，截至目前國內累計671,160例新型冠狀病毒肺炎相關通報(含648,841例排除)，其中11,491例確診，分別為1,148例境外移入，10,290例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另49例(新增案10772、10826、10829、11143、11144、11146、11147、11148、11149、11155、11177、11179、11184、11190、11193、11194、11225、11227、11228、11229、11230)移除為空號。確診個案中286例死亡。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月7日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-07\$\@\$中央流行疫情指揮中心今(7)日宣布，因應本土疫情持續嚴峻，全國疫情警戒第三級延長至6月28日止，請全國民眾與政府共同持續努力，嚴守社區防線。相關措施如下：\$\@\$一、民眾外出應全程佩戴口罩，一經查獲有違反情事，將不再勸導，逕予開罰。\$\@\$二、經公告應關閉的休閒娛樂場所，將嚴查不得營業，並對違法營業的業者、現場執業人員、消費及聚會者，依法分別裁罰。\$\@\$三、全國餐飲業一律外帶，賣場及超市加強人流管制，並呼籲民眾少去多買，一次購足。\$\@\$四、結婚不宴客，喪禮不公祭。\$\@\$五、宗教集會活動全面暫停辦理，宗教場所暫不開放民眾進入。\$\@\$六、關閉休閒娛樂場、觀展觀賽場所及教育學習場域。\$\@\$七、停止室內5人以上、室外10人以上之家庭聚會(同住者不計)和社交聚會，並避免不必要移動、活動或集會。\$\@\$八、自我健康監測，有症狀應就醫。\$\@\$九、營業場所及洽公機關(構)應落實人流管制，戴口罩、保持社交距離。\$\@\$十、職場及工作處所應遵守企業持續營運指引的防疫規定，落實個人及工作場所衛生管理，啟動企業持續營運因應措施，如異地或遠距辦公、彈性時間上班。\$\@\$十一、公共場域、大眾運輸加強清消。\$\@\$指揮中心說明，針對近期醫院及長照機構感染事件，指揮中心已請全國醫院停止開放探病(例外情形除外)，住院病人的陪病者以1人為限，執行至全國三級警戒降級為止。至於長照機構，除停止開放機構住民探視，也要求非必要性特殊情況，盡量避免住民請假外出，並強化門禁管理，避免不必要的人員進出，同時持續落實每日工作人員、服務對象與陪住人員等體溫及健康監測，掌握其COVID-19暴露風險情形。\$\@\$指揮中心強調，現在是防疫的關鍵時刻，惟有民眾與政府互相配合、共同抗疫，才可控制疫情，維護全民健康。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-06\$\@\$中央流行疫情指揮中心今(6)日澄清，目前我國COVID-19疫苗優先提供公費對象接種，民眾不用負擔疫苗費用，6月7日起也無須負擔其他行政費用。未來將會依序逐漸擴大至全體國民皆能公費接種，目前更無自費接種規劃，並無所謂「自費負擔」之問題存在。今(2021)年5月31日經立法院三讀通過的「嚴重特殊傳染性肺炎防治及紓困振興特別條例」，加上去年所編列之疫苗預算，行政院已編列共約340億用來購買全民公費疫苗，今年則額外編列約40億元預算，用以負擔疫苗接種所需之醫療院所行政費用，讓符合公費資格者，在面對疫情挑戰時，不用擔心還要花錢施打疫苗。\$\@\$指揮中心表示，現階段開放的公費接種對象，以雙北地區屬於第一類至第三類未曾接種第一劑疫苗的醫事、防疫人員及高接觸風險者為優先接種對象；雙北以外之縣市則以未曾接種疫苗的第一類醫事人員為接種對象，並將視疫苗接種進度，逐步開放至第二、三類及機構對象。目前尚未開放的公費對象，也將視疫苗供應充裕情況，逐步列入公費接種。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-06\$\@\$中央流行疫情指揮中心今(6)日公布國內新增335例本土COVID-19確定病例，另有校正回歸本土個案8例，總計343例。確診個案中新增36例死亡。\$\@\$指揮中心表示，今日新增之335例本土病例，為189例男性、146例女性，年齡介於未滿5歲至90多歲，發病日介於今(2021)年5月24日至6月5日。另校正回歸個案8例中，為3例男性、5例女性，年齡介於20多歲至60多歲，發病日介於6月1日至6月2日。\$\@\$指揮中心指出，綜上所有本土個案共343例，分布地區以新北市160例最多，其次為苗栗縣75例、臺北市64例、桃園市16例、宜蘭縣9例、雲林縣、高雄市、彰化縣及新竹縣各3例，基隆市、臺中市及臺南市各2例，嘉義市1例。其中雙北地區以外縣市119例中，107例為已知感染源，7例關聯不明、5例疫調中。相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增36例死亡個案，共計為男性22位、女性14位，年齡介於50多歲至90多歲，發病日介於5月7日至6月1日，確診日介於5月13日至6月5日，死亡日介於5月28日至6月4日，詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計656,768例新型冠狀病毒肺炎相關通報(含634,762例排除)，其中11,298例確診，分別為1,145例境外移入，10,100例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另28例(新增案10494)移除為空號。確診個案中260例死亡。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月6日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-06\$\@\$中央流行疫情指揮中心今(6)日表示，針對苗栗縣電子公司廠房發生COVID-19群聚事件，指揮中心已即刻設立前進指揮所，積極協助地方政府及廠商進行防疫，避免感染擴大。相關措施如下：\$\@\$一、所有外籍移工停止上班，居家隔離，薪資照付。\$\@\$二、高風險區移工安排入住集中檢疫所；中低風險區就地居家隔離，並進行健康監控。\$\@\$三、本國籍員工確診者立即進行疫調，匡列接觸者，依規定進行隔離。其餘員工，加強健康監控。\$\@\$四、所有確診者皆已完成就醫安置。\$\@\$五、經工業局、防疫醫師及廠方進行會勘，依防疫計畫有條件降載復工。\$\@\$指揮中心指出，截至6月5日，第1家電子公司共計182案確診 (24名本國籍、158名外國籍），已匡列接觸者399名；第2家電子公司共計12案確診 (均為外國籍)；第3家電子公司共計12案確診 (2名本國籍、10名外國籍)。相關疫調持續進行中。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-06\$\@\$中央流行疫情指揮中心今(6)日澄清，有關昨(5)日公布之「自6月7日起，請合約醫療院所免費提供民眾接種公費COVID-19疫苗服務」新聞稿之內容，是指因應國內疫情嚴峻，指揮中心自6月7日起將依序提供符合「COVID-19疫苗接種計畫」之公費對象免費接種疫苗，相關施打順序將由指揮中心依據專家會議規定計畫，評估群體風險性，陸續開放施打。\$\@\$指揮中心表示，現階段開放之公費接種對象，以雙北地區屬於第一類至第三類未曾接種第一劑疫苗之醫事、防疫人員及高接觸風險者為優先接種對象；雙北以外之縣市則以未曾接種疫苗之第一類醫事人員為接種對象，並將視疫苗接種進度，逐步開放至第二、三類及機構對象。目前尚未開放之公費對象，也將於後續儘快開放公費接種。\$\@\$指揮中心強調，防疫相關政策皆秉持中央與地方「標準一致、做法一致、腳步一致」防疫原則，推動各項措施，也請相關單位及民眾主動積極配合，與政府共同努力，嚴守社區防線。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-05\$\@\$鑒於本土疫情嚴峻，應絕對禁止廠區和廠區間的移工流動。中央流行疫情指揮中心今(5)日表示， 地方政府及勞動部應協助苗栗某電子廠公司的移工避免離開宿舍，並於這段期間與地方政府合作，減少移工不必要的外出，以減少移工群聚發生。\$\@\$指揮中心指出，請雇主及仲介公司自即日起，配合辦理下列事項：\$\@\$一、自即日起針對移工非必要轉換至新雇主之作業，於第三級警戒期間暫緩作業。\$\@\$二、自即日起針對同一雇主不同廠區間的派工，於第三級警戒期間暫緩調派。\$\@\$三、確實依照勞動部發布嚴重特殊傳染性肺炎雇主聘僱移工指引，辦理防疫作業。\$\@\$指揮中心強調，基於國內防疫安全，近期將由勞動部與地方政府針對移工人數達五百人以上企業與百人以上大型移工宿舍進行訪查，實地督導雇主與仲介業者落實防疫指引，並請勞動部規劃補助企業改善宿舍防疫環境，以強化防疫量能。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-05\$\@\$中央流行疫情指揮中心今(5)日表示，針對苗栗縣2家電子公司廠房發生COVID-19群聚事件，指揮中心已於昨(4)日設立前進指揮所，積極協助地方政府及廠商進行防疫，避免感染擴大。相關作為如下：\$\@\$一、加速篩檢執行：昨日經動員後於第1家電子公司共開設18條篩檢線，每小時可執行350-500人次篩檢，截至昨日（6/3-6/4）共完成採檢4,599人，累計抗原快篩陽性59人，其中PCR檢驗共56人陽性確診、3人陰性。今日進行其餘約2,451人之採檢，截至中午尚餘約1,500人待採，將於今日完成採檢工作。\$\@\$二、宿舍、職場及外部風險評估及安置：針對第1家電子公司確診個案之宿舍及廠區分布，劃定風險區域，安排相關宿舍樓層之清空及人員區隔安置，密切接觸者送集中檢疫所或防疫旅館居家隔離，今日預計移出280位。另第2家電子公司之相關接觸者已匡列安排隔離安置及採檢，該公司亦於今天展開全員約4千人篩檢。\$\@\$三、由經濟部即刻派遣產業專家進駐前進指揮所，協助防疫醫師與電子場規劃廠區作業、休息及用餐等活動之分艙分流，如無法執行，即要求停工。\$\@\$四、由勞動部即刻派員確保仲介公司之移工管理，落實住宿人數降載及確保分艙分流，並就仍需共用衛浴之宿舍環境問題予以解決；移工宿舍人員禁止外出部分，加強管理並協調警政協處。\$\@\$五、為避免本國勞工將疫情帶入社區，請該公司緊急通知員工留置家中，如家庭環境無法落實一人一室者，公司應協助安排合適住宿地點。\$\@\$指揮中心指出，截至6月4日，第1家電子公司共計131案確診（14名本國籍、117名外國籍），已匡列接觸者323名，均已採檢；第2家電子公司共計9案確診。相關疫調持續進行中。</t>
   </si>
 </sst>
 </file>
@@ -517,7 +1363,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -545,16 +1391,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="C2" s="2">
-        <v>44376</v>
+        <v>44377</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -562,16 +1408,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="C3" s="2">
-        <v>44376</v>
+        <v>44377</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>26</v>
+        <v>186</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -579,16 +1425,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
       <c r="C4" s="2">
-        <v>44376</v>
+        <v>44377</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
+        <v>187</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -596,16 +1442,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="C5" s="2">
         <v>44376</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>188</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -613,16 +1459,13 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="C6" s="2">
-        <v>44375</v>
+        <v>44376</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -630,16 +1473,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C7" s="2">
-        <v>44374</v>
+        <v>44376</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>30</v>
+        <v>190</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -647,13 +1490,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="C8" s="2">
-        <v>44374</v>
+        <v>44376</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>31</v>
+        <v>191</v>
+      </c>
+      <c r="E8" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -661,16 +1507,16 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="C9" s="2">
-        <v>44374</v>
+        <v>44375</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>32</v>
+        <v>192</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -678,13 +1524,16 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>103</v>
       </c>
       <c r="C10" s="2">
         <v>44374</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>193</v>
+      </c>
+      <c r="E10" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -692,16 +1541,1259 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="2">
+        <v>44374</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="2">
+        <v>44374</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="2">
+        <v>44374</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E13" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="2">
+        <v>44373</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E14" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="2">
+        <v>44373</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E15" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="2">
+        <v>44373</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" s="2">
+        <v>44373</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="2">
+        <v>44373</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E18" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" s="2">
+        <v>44372</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="2">
+        <v>44372</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="2">
-        <v>44373</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="B21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" s="2">
+        <v>44372</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="2">
+        <v>44372</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" s="2">
+        <v>44371</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E23" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" s="2">
+        <v>44371</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E24" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" s="2">
+        <v>44371</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E25" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" s="2">
+        <v>44370</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="2">
+        <v>44370</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E27" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" s="2">
+        <v>44370</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E28" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" s="2">
+        <v>44369</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E29" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" s="2">
+        <v>44369</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
         <v>34</v>
       </c>
-      <c r="E11" t="s">
+      <c r="B31" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="2">
+        <v>44369</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E31" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" s="2">
+        <v>44369</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E32" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="2">
+        <v>44369</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E33" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" s="2">
+        <v>44368</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" s="2">
+        <v>44368</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" s="2">
+        <v>44367</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C37" s="2">
+        <v>44367</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" t="s">
+        <v>131</v>
+      </c>
+      <c r="C38" s="2">
+        <v>44367</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
         <v>42</v>
+      </c>
+      <c r="B39" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="2">
+        <v>44366</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" s="2">
+        <v>44366</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E40" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" s="2">
+        <v>44366</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E41" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" t="s">
+        <v>135</v>
+      </c>
+      <c r="C42" s="2">
+        <v>44365</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="E42" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
+        <v>136</v>
+      </c>
+      <c r="C43" s="2">
+        <v>44365</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="E43" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" t="s">
+        <v>137</v>
+      </c>
+      <c r="C44" s="2">
+        <v>44365</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="2">
+        <v>44365</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" t="s">
+        <v>139</v>
+      </c>
+      <c r="C46" s="2">
+        <v>44365</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" t="s">
+        <v>140</v>
+      </c>
+      <c r="C47" s="2">
+        <v>44364</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" t="s">
+        <v>141</v>
+      </c>
+      <c r="C48" s="2">
+        <v>44364</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" t="s">
+        <v>142</v>
+      </c>
+      <c r="C49" s="2">
+        <v>44363</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="2">
+        <v>44363</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E50" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" t="s">
+        <v>144</v>
+      </c>
+      <c r="C51" s="2">
+        <v>44363</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E51" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" t="s">
+        <v>145</v>
+      </c>
+      <c r="C52" s="2">
+        <v>44362</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E52" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" t="s">
+        <v>146</v>
+      </c>
+      <c r="C53" s="2">
+        <v>44362</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54" t="s">
+        <v>147</v>
+      </c>
+      <c r="C54" s="2">
+        <v>44362</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" t="s">
+        <v>148</v>
+      </c>
+      <c r="C55" s="2">
+        <v>44362</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" t="s">
+        <v>149</v>
+      </c>
+      <c r="C56" s="2">
+        <v>44362</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" t="s">
+        <v>150</v>
+      </c>
+      <c r="C57" s="2">
+        <v>44361</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" t="s">
+        <v>151</v>
+      </c>
+      <c r="C58" s="2">
+        <v>44361</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" t="s">
+        <v>152</v>
+      </c>
+      <c r="C59" s="2">
+        <v>44360</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" t="s">
+        <v>153</v>
+      </c>
+      <c r="C60" s="2">
+        <v>44360</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B61" t="s">
+        <v>154</v>
+      </c>
+      <c r="C61" s="2">
+        <v>44360</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="E61" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62" t="s">
+        <v>155</v>
+      </c>
+      <c r="C62" s="2">
+        <v>44359</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E62" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" t="s">
+        <v>156</v>
+      </c>
+      <c r="C63" s="2">
+        <v>44359</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E63" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" t="s">
+        <v>157</v>
+      </c>
+      <c r="C64" s="2">
+        <v>44359</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" t="s">
+        <v>158</v>
+      </c>
+      <c r="C65" s="2">
+        <v>44358</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" t="s">
+        <v>159</v>
+      </c>
+      <c r="C66" s="2">
+        <v>44358</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" t="s">
+        <v>160</v>
+      </c>
+      <c r="C67" s="2">
+        <v>44358</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68" t="s">
+        <v>161</v>
+      </c>
+      <c r="C68" s="2">
+        <v>44358</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" t="s">
+        <v>162</v>
+      </c>
+      <c r="C69" s="2">
+        <v>44358</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="E69" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70" t="s">
+        <v>163</v>
+      </c>
+      <c r="C70" s="2">
+        <v>44357</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E70" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" t="s">
+        <v>164</v>
+      </c>
+      <c r="C71" s="2">
+        <v>44357</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="E71" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>75</v>
+      </c>
+      <c r="B72" t="s">
+        <v>165</v>
+      </c>
+      <c r="C72" s="2">
+        <v>44357</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>76</v>
+      </c>
+      <c r="B73" t="s">
+        <v>166</v>
+      </c>
+      <c r="C73" s="2">
+        <v>44356</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>77</v>
+      </c>
+      <c r="B74" t="s">
+        <v>167</v>
+      </c>
+      <c r="C74" s="2">
+        <v>44356</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="E74" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>78</v>
+      </c>
+      <c r="B75" t="s">
+        <v>168</v>
+      </c>
+      <c r="C75" s="2">
+        <v>44356</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E75" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76" t="s">
+        <v>169</v>
+      </c>
+      <c r="C76" s="2">
+        <v>44356</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77" t="s">
+        <v>170</v>
+      </c>
+      <c r="C77" s="2">
+        <v>44356</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="E77" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78" t="s">
+        <v>171</v>
+      </c>
+      <c r="C78" s="2">
+        <v>44355</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E78" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>82</v>
+      </c>
+      <c r="B79" t="s">
+        <v>172</v>
+      </c>
+      <c r="C79" s="2">
+        <v>44355</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="E79" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>83</v>
+      </c>
+      <c r="B80" t="s">
+        <v>173</v>
+      </c>
+      <c r="C80" s="2">
+        <v>44354</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E80" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>84</v>
+      </c>
+      <c r="B81" t="s">
+        <v>174</v>
+      </c>
+      <c r="C81" s="2">
+        <v>44354</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="E81" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82" t="s">
+        <v>175</v>
+      </c>
+      <c r="C82" s="2">
+        <v>44354</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E82" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83" t="s">
+        <v>176</v>
+      </c>
+      <c r="C83" s="2">
+        <v>44354</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E83" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84" t="s">
+        <v>177</v>
+      </c>
+      <c r="C84" s="2">
+        <v>44353</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E84" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>88</v>
+      </c>
+      <c r="B85" t="s">
+        <v>178</v>
+      </c>
+      <c r="C85" s="2">
+        <v>44353</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E85" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>89</v>
+      </c>
+      <c r="B86" t="s">
+        <v>179</v>
+      </c>
+      <c r="C86" s="2">
+        <v>44353</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="E86" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>90</v>
+      </c>
+      <c r="B87" t="s">
+        <v>180</v>
+      </c>
+      <c r="C87" s="2">
+        <v>44353</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E87" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>91</v>
+      </c>
+      <c r="B88" t="s">
+        <v>181</v>
+      </c>
+      <c r="C88" s="2">
+        <v>44352</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>92</v>
+      </c>
+      <c r="B89" t="s">
+        <v>182</v>
+      </c>
+      <c r="C89" s="2">
+        <v>44352</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>93</v>
+      </c>
+      <c r="B90" t="s">
+        <v>183</v>
+      </c>
+      <c r="C90" s="2">
+        <v>44352</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E90" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>94</v>
+      </c>
+      <c r="B91" t="s">
+        <v>184</v>
+      </c>
+      <c r="C91" s="2">
+        <v>44352</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E91" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -716,6 +2808,86 @@
     <hyperlink ref="D9" r:id="rId8"/>
     <hyperlink ref="D10" r:id="rId9"/>
     <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="D12" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId12"/>
+    <hyperlink ref="D14" r:id="rId13"/>
+    <hyperlink ref="D15" r:id="rId14"/>
+    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D17" r:id="rId16"/>
+    <hyperlink ref="D18" r:id="rId17"/>
+    <hyperlink ref="D19" r:id="rId18"/>
+    <hyperlink ref="D20" r:id="rId19"/>
+    <hyperlink ref="D21" r:id="rId20"/>
+    <hyperlink ref="D22" r:id="rId21"/>
+    <hyperlink ref="D23" r:id="rId22"/>
+    <hyperlink ref="D24" r:id="rId23"/>
+    <hyperlink ref="D25" r:id="rId24"/>
+    <hyperlink ref="D26" r:id="rId25"/>
+    <hyperlink ref="D27" r:id="rId26"/>
+    <hyperlink ref="D28" r:id="rId27"/>
+    <hyperlink ref="D29" r:id="rId28"/>
+    <hyperlink ref="D30" r:id="rId29"/>
+    <hyperlink ref="D31" r:id="rId30"/>
+    <hyperlink ref="D32" r:id="rId31"/>
+    <hyperlink ref="D33" r:id="rId32"/>
+    <hyperlink ref="D34" r:id="rId33"/>
+    <hyperlink ref="D35" r:id="rId34"/>
+    <hyperlink ref="D36" r:id="rId35"/>
+    <hyperlink ref="D37" r:id="rId36"/>
+    <hyperlink ref="D38" r:id="rId37"/>
+    <hyperlink ref="D39" r:id="rId38"/>
+    <hyperlink ref="D40" r:id="rId39"/>
+    <hyperlink ref="D41" r:id="rId40"/>
+    <hyperlink ref="D42" r:id="rId41"/>
+    <hyperlink ref="D43" r:id="rId42"/>
+    <hyperlink ref="D44" r:id="rId43"/>
+    <hyperlink ref="D45" r:id="rId44"/>
+    <hyperlink ref="D46" r:id="rId45"/>
+    <hyperlink ref="D47" r:id="rId46"/>
+    <hyperlink ref="D48" r:id="rId47"/>
+    <hyperlink ref="D49" r:id="rId48"/>
+    <hyperlink ref="D50" r:id="rId49"/>
+    <hyperlink ref="D51" r:id="rId50"/>
+    <hyperlink ref="D52" r:id="rId51"/>
+    <hyperlink ref="D53" r:id="rId52"/>
+    <hyperlink ref="D54" r:id="rId53"/>
+    <hyperlink ref="D55" r:id="rId54"/>
+    <hyperlink ref="D56" r:id="rId55"/>
+    <hyperlink ref="D57" r:id="rId56"/>
+    <hyperlink ref="D58" r:id="rId57"/>
+    <hyperlink ref="D59" r:id="rId58"/>
+    <hyperlink ref="D60" r:id="rId59"/>
+    <hyperlink ref="D61" r:id="rId60"/>
+    <hyperlink ref="D62" r:id="rId61"/>
+    <hyperlink ref="D63" r:id="rId62"/>
+    <hyperlink ref="D64" r:id="rId63"/>
+    <hyperlink ref="D65" r:id="rId64"/>
+    <hyperlink ref="D66" r:id="rId65"/>
+    <hyperlink ref="D67" r:id="rId66"/>
+    <hyperlink ref="D68" r:id="rId67"/>
+    <hyperlink ref="D69" r:id="rId68"/>
+    <hyperlink ref="D70" r:id="rId69"/>
+    <hyperlink ref="D71" r:id="rId70"/>
+    <hyperlink ref="D72" r:id="rId71"/>
+    <hyperlink ref="D73" r:id="rId72"/>
+    <hyperlink ref="D74" r:id="rId73"/>
+    <hyperlink ref="D75" r:id="rId74"/>
+    <hyperlink ref="D76" r:id="rId75"/>
+    <hyperlink ref="D77" r:id="rId76"/>
+    <hyperlink ref="D78" r:id="rId77"/>
+    <hyperlink ref="D79" r:id="rId78"/>
+    <hyperlink ref="D80" r:id="rId79"/>
+    <hyperlink ref="D81" r:id="rId80"/>
+    <hyperlink ref="D82" r:id="rId81"/>
+    <hyperlink ref="D83" r:id="rId82"/>
+    <hyperlink ref="D84" r:id="rId83"/>
+    <hyperlink ref="D85" r:id="rId84"/>
+    <hyperlink ref="D86" r:id="rId85"/>
+    <hyperlink ref="D87" r:id="rId86"/>
+    <hyperlink ref="D88" r:id="rId87"/>
+    <hyperlink ref="D89" r:id="rId88"/>
+    <hyperlink ref="D90" r:id="rId89"/>
+    <hyperlink ref="D91" r:id="rId90"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20210708
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="333">
   <si>
     <t>Press Title</t>
   </si>
@@ -31,6 +31,15 @@
     <t>Page Content</t>
   </si>
   <si>
+    <t>指揮中心延長全國疫情警戒第三級至7月26日止，嚴守社區防線，並適度鬆綁部分措施</t>
+  </si>
+  <si>
+    <t>新增21例COVID-19確定病例，分別為18例本土及3例境外移入</t>
+  </si>
+  <si>
+    <t>針對媒體報導「指揮中心設局召開記者會」 指揮中心澄清並非事實</t>
+  </si>
+  <si>
     <t>指揮中心訂購第二批AZ疫苗62.6萬劑將於今(7)日下午抵臺</t>
   </si>
   <si>
@@ -61,6 +70,246 @@
     <t>新增80例COVID-19確定病例，分別為76例本土及4例境外移入</t>
   </si>
   <si>
+    <t>針對6月8日起曾在臺北市環南市場活動人員，將發送疫情警示簡訊</t>
+  </si>
+  <si>
+    <t>新增58例COVID-19確定病例，分別為57例本土及1例境外移入</t>
+  </si>
+  <si>
+    <t>7月2日全國防疫會議後記者會報告</t>
+  </si>
+  <si>
+    <t>因應全球Delta變異株流行，自7月2日中午12時加強國際港埠入境人員健康監測</t>
+  </si>
+  <si>
+    <t>國內新增2例日本腦炎病例，籲請民眾出入高風險場所加強防蚊，並按時帶幼兒接種疫苗</t>
+  </si>
+  <si>
+    <t>即日起，恢復家庭類移工轉換雇主，雇主應於接續當日安排移工檢驗PCR</t>
+  </si>
+  <si>
+    <t>新增50例COVID-19確定病例，分別為47例本土及3例境外移入</t>
+  </si>
+  <si>
+    <t>指揮中心與農委會制定「批發市場防疫管理措施建議指引」 協助批發市場防疫</t>
+  </si>
+  <si>
+    <t>Moderna第三批採購疫苗41萬劑將於今(30)日下午抵臺</t>
+  </si>
+  <si>
+    <t>新增56例COVID-19確定病例，分別為55例本土及1例境外移入</t>
+  </si>
+  <si>
+    <t>簡訊實聯制數據係以合法性、正當性、必要性進行使用，絕無違法情事</t>
+  </si>
+  <si>
+    <t>針對媒體報導「COVID-19疫苗接種外展服務，無法選擇疫苗廠牌，係為國產疫苗鋪路」 指揮中心澄清並非事實</t>
+  </si>
+  <si>
+    <t>新增54例COVID-19確定病例，均為本土個案</t>
+  </si>
+  <si>
+    <t>6月29日全國防疫會議後記者會報告</t>
+  </si>
+  <si>
+    <t>新增60例COVID-19確定病例，均為本土個案</t>
+  </si>
+  <si>
+    <t>本島各機場前往離島自願快篩而呈陽性反應之旅客，將進行PCR採檢陰性後，始允許登機</t>
+  </si>
+  <si>
+    <t>全球Delta變異株流行，即日起，入境人士前往檢疫地點應搭乘防疫車輛</t>
+  </si>
+  <si>
+    <t>網傳「mRNA疫苗會使接種者變成轉基因生物體」，指揮中心：疫苗品質安全把關，民眾用藥有保障</t>
+  </si>
+  <si>
+    <t>新增89例COVID-19確定病例，分別為88例本土及1例境外移入</t>
+  </si>
+  <si>
+    <t>指揮中心說明274萬劑莫德納(Moderna) COVID-19疫苗第一階段分配事宜</t>
+  </si>
+  <si>
+    <t>因應屏東Delta印度變異株群聚及相關感染事件，指揮中心已採取相關應變措施，避免感染擴大</t>
+  </si>
+  <si>
+    <t>新增78例本土COVID-19確定病例，另有2例境外移入</t>
+  </si>
+  <si>
+    <t>集中檢疫所開放高風險7國以外入境者自費入住</t>
+  </si>
+  <si>
+    <t>第二劑AZ COVID-19疫苗接種說明</t>
+  </si>
+  <si>
+    <t>6月25日全國防疫會議後記者會報告</t>
+  </si>
+  <si>
+    <t>為有效利用COVID-19疫苗 當日最後一瓶開瓶剩餘劑量將開放候補接種</t>
+  </si>
+  <si>
+    <t>因應全球Delta變異株流行，自6月27日零時起，全面提升入境人員檢疫措施</t>
+  </si>
+  <si>
+    <t>新增76例COVID-19確定病例，均為本土個案</t>
+  </si>
+  <si>
+    <t>民眾使用COVID-19家用快篩試劑流程與注意事項</t>
+  </si>
+  <si>
+    <t>新增130例COVID-19確定病例，分別為129例本土及1例境外移入</t>
+  </si>
+  <si>
+    <t>指揮中心與相關單位持續精進「市場專案」相關措施，達到社區清零目的</t>
+  </si>
+  <si>
+    <t>指揮中心維持全國疫情警戒第三級至7月12日止，希望國人共體時艱，共同抗疫</t>
+  </si>
+  <si>
+    <t>因應臺北農產運銷公司群聚感染事件，指揮中心啟動「市場專案」強化相關防疫作為</t>
+  </si>
+  <si>
+    <t>新增104例COVID-19確定病例，均為本土個案</t>
+  </si>
+  <si>
+    <t>指揮中心說明274萬劑莫德納(Moderna) COVID-19疫苗之分配規劃、第一批次分配原則與接種對象</t>
+  </si>
+  <si>
+    <t>因應印度變種病毒蔓延 居家檢疫及居家隔離期滿者均須進行PCR檢測 以維護國內社區安全</t>
+  </si>
+  <si>
+    <t>6月22日全國防疫會議後記者會報告</t>
+  </si>
+  <si>
+    <t>指揮中心說明「COVID-19疫苗公費接種對象」及現階段開放接種實施對象</t>
+  </si>
+  <si>
+    <t>新增78例COVID-19本土病例，另有1例境外移入</t>
+  </si>
+  <si>
+    <t>修正雇主聘僱移工防疫指引，明定雇主應落實防疫措施</t>
+  </si>
+  <si>
+    <t>新增75例COVID-19本土病例，均為本土個案</t>
+  </si>
+  <si>
+    <t>指揮中心持續監測疫苗接種後不良事件，提醒民眾待身體狀況穩定後再行安排接種</t>
+  </si>
+  <si>
+    <t>美國政府捐贈250萬劑Moderna COVID-19疫苗將於今(20)日傍晚抵臺</t>
+  </si>
+  <si>
+    <t>新增109例COVID-19病例，為107例本土、2例境外移入</t>
+  </si>
+  <si>
+    <t>指揮中心持續監測疫苗接種後不良事件，提醒民眾視身體狀況穩定後再行安排接種</t>
+  </si>
+  <si>
+    <t>已接種一劑AZ COVID-19疫苗之民眾，可陸續完成第二劑接種</t>
+  </si>
+  <si>
+    <t>新增128例COVID-19病例，為127例本土、1例境外移入</t>
+  </si>
+  <si>
+    <t>6月18日全國防疫會議後記者會報告</t>
+  </si>
+  <si>
+    <t>指揮中心持續監測疫苗接種後不良事件，並提醒高齡年長者接種疫苗之注意事項</t>
+  </si>
+  <si>
+    <t>為利醫療院所照護重症個案，指揮中心成立COVID-19重症個案臨床處置專家諮詢小組，自6月21日開始線上病例諮詢會議</t>
+  </si>
+  <si>
+    <t>Moderna疫苗24萬劑將於今(18)日下午抵臺</t>
+  </si>
+  <si>
+    <t>新增188例COVID-19病例，為187例本土、1例境外移入</t>
+  </si>
+  <si>
+    <t>接種COVID-19疫苗是預防感染、避免重症與死亡最有效的方式　指揮中心持續監測疫苗接種後不良事件</t>
+  </si>
+  <si>
+    <t>指揮中心公布新增175例COVID-19本土病例</t>
+  </si>
+  <si>
+    <t>指揮中心公布新增167例COVID-19本土病例，另有3例境外移入</t>
+  </si>
+  <si>
+    <t>國產疫苗審查皆以科學、專業為原則，並依法規程序採購</t>
+  </si>
+  <si>
+    <t>第二批莫德納(Moderna) COVID-19疫苗預計於6月18日起配送，請合約醫療院所開啟預約掛號服務，提供符合對象者預約接種</t>
+  </si>
+  <si>
+    <t>指揮中心說明疫苗接種第二類「中央及地方政府防疫人員」含括對象</t>
+  </si>
+  <si>
+    <t>日本提供我國AstraZeneca COVID-19疫苗第二次分配量說明</t>
+  </si>
+  <si>
+    <t>補助全國快速PCR檢驗儀 加速社區檢驗量能</t>
+  </si>
+  <si>
+    <t>指揮中心公布新增132例本土病例，另有3例境外移入</t>
+  </si>
+  <si>
+    <t>6月15日全國防疫會議後記者會報告</t>
+  </si>
+  <si>
+    <t>調整國籍航空公司機組員返臺檢疫措施，確保機組員職場健康安全及維護國內防疫安全</t>
+  </si>
+  <si>
+    <t>指揮中心公布新增185例COVID-19確定病例，均為本土個案</t>
+  </si>
+  <si>
+    <t>指揮中心說明「中央政府機關防疫相關人員之疫苗分配量寄放於各縣市」一事</t>
+  </si>
+  <si>
+    <t>網傳總統、副總統已接種COVID-19疫苗  指揮中心調閱接種系統查證均尚未接種</t>
+  </si>
+  <si>
+    <t>指揮中心公布新增174例COVID-19本土個案及1例境外移入</t>
+  </si>
+  <si>
+    <t>指揮中心：依公式計算配送各縣市疫苗數量  將視後續接種情形滾動檢討並加強配送</t>
+  </si>
+  <si>
+    <t>自6月12日起，首批莫德納疫苗開放尚未接種第一劑COVID-19疫苗的第一類醫事及非醫事人員接種</t>
+  </si>
+  <si>
+    <t>指揮中心公布新增250例本土個案，另有1例境外移入</t>
+  </si>
+  <si>
+    <t>為提升COVID-19疫苗接種效率，指揮中心與地方政府衛生局召開會議進行經驗交流與分享</t>
+  </si>
+  <si>
+    <t>6月11日全國防疫會議後記者會報告</t>
+  </si>
+  <si>
+    <t>為協助紓解重症醫療量能，指揮中心採購複合單株抗體藥物，提供具有重症風險因子之輕中度確診個案治療使用</t>
+  </si>
+  <si>
+    <t>指揮中心公布新增286例COVID-19本土確定病例及1例境外移入</t>
+  </si>
+  <si>
+    <t>全國疫情警戒第三級期間，持續執行「邊境嚴管」措施</t>
+  </si>
+  <si>
+    <t>指揮中心感謝我國企業及民間單位共同捐贈日製負壓隔離艙80座，公私協力共同防疫</t>
+  </si>
+  <si>
+    <t>疫苗接種政策為全體國民重要權益，資訊均公開透明，如有違法將嚴正法辦</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/aiGegg4ncYmMP9dTx4W_Zw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/h6gxof3idm6vTzGCwC7qJw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/65J6c1wTSqx-68NNaCRU5g?typeid=9</t>
+  </si>
+  <si>
     <t>/Bulletin/Detail/BlxZvHJU1w5vlVvV3EqlXg?typeid=9</t>
   </si>
   <si>
@@ -91,6 +340,246 @@
     <t>/Bulletin/Detail/75mzJEXQUlqOUK6jOkSFvw?typeid=9</t>
   </si>
   <si>
+    <t>/Bulletin/Detail/JfNJkibqwkf3ALmQsoqf9w?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/QdvjM3jxQOYglY2Gp2NgIQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/NQxqNqY1W6Y6z7xGQyKUvQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/0FIpdQsOY4ttnb_dXBT1sA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/4lJwtoH8B5KhGEctejJNZw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/O3bkuQKuH26ZV0XXbJYucQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/4V7Iv__GIhGG03D1ghBXOQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/QW-rc-JUvcOMq_9P2SjxLA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/pYQ-ddE0kOM_t_QJfc8xjw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/2_g7KcaGpuqcmjonS_tseQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/HS0hjvHxAOTCPtNPmDo7Bw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/LpD4TCQApQ9vv1V6scwESw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/1j8W3yYnAz6bFopxt7_Www?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/V6pewvqk9-nbn5aARuSARw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/yaxkF9NPpjDvDsdKXaitsQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/BIeGHTPRfBMrzrGAaJhH_Q?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/HzWKglQxOhCvZk1kKg0VyA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/W8nseTHzy75Qbnpgavjk-A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/CzOFlvhEpIoqdOEuGLOb8A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/nM5PTloj8i3dm5h_EI3lHA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/F95aOtuKwrsJ347Xslc-ZA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Ve2G8PYEHCAhycgrH0Q1PQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/ZgKW-VupBVtp_sGz2YXXaQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/auHSp7RyQ7EesQkbPZBoaA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/5NpKu8jZAKdJssJnlGxTXA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/a_nNEk7-jcJcUMqE3M-Xeg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/zqUqseKSNKJint4YMEddiQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/9pKIzKzZOpp4HocU3uCl6g?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/c8C9gtHwUNnkywyMqWoLJQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/3A_GxvlYM4wkYEYTlozw6A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/0M4E0GxUuEj9_0rHwVlPAw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/3LyPF-Dt0AhduqNnRwp9zg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/kJJ5ZOZig6PA2ZAu2VMRQQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/mDFLj0aLsQztMI7vnMSy1w?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/HmZ7CIAda5ftC781xMTSKg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/zK5fwXiSohil4etG3pphhw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/NC6r7Z2A5ylk0AUMFxAkcA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/H95sl3L-tIrq1-o71rj8Gg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/7IX7KD-nM2TmIYgml7lDWg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/OakZRZ4dYRYEnX-_s__Dag?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Lby0PKwYfroFHd13wPbOdg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/ODtiZA3OtV7lf4IEVECBkA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/k9iJeEl5uPkgkCmCWtGZDg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/8QrfZwt787Bjeoh31UZztg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/B8Zac1K5GfDJSO8oDKcNfQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/4p1T6MpeJyRyu1syfZDUyw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/u9SuLf-DGkfywEXISH7pIw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/j5bFJQGngMHxaaQIK-j12w?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/hbSnCh8vhAKj2CsaFwbmZA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/tEf1nYt3fuARSRqFzbGbmw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/StnIZRaP2BZTFrduQfgCdg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/TAeqHS3g8G3Qbp3EGZkXSQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/f9isJQRtYK4rL9_Zmd4VUw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/3EaqopBnYL-XoDtMI8qQEA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/-bdXbaKzQLCvX8s69vQWQA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/gpzjNU57zwqDAfQJhI7fMA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/7ZPV_qpP_nL8FkiGNv1sbQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/R-DB5ro9NqAlSEStj_Uaxw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/2E5FJ55LFelexPtiSn3gbQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/84kDjSBTHU75sIoWKAdKcg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/DRnT39ZhmbVd21bWvHIEng?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/dmyxdxokdprJxTw9L5O5Bw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Aaw09pr_bNORqPc8F1fUSA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/832w8RYL7puxozPKMoTSAg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/A_4V_ZEYMJgH3nzjXxy21w?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/OOQWHbZwyOpZ-GpkKOgyYw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/iGXRaqo6rnJ0Gh9PFDovyg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/XUjGVcW2wV5HhfnxjVqg0w?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/eCpD5uFuWNjGpxhqMKIZ8A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/MHEOJlq75e2VYGkuBMGeJQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/-9laBujLZpjBzFaf_j8hcg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Z3woynaHMpHEAcv_YpZBHA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/6RR01Fye2xDT2mAOqhAoSg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/YCIJBF3p851kbsP5H1TZtw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/3iNNwroO0OrdsItewXo_GA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/itht4O09O7Hzx42_eMrmqw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/A_H9_tpR0cCtxnrn6ywmyg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/aiGegg4ncYmMP9dTx4W_Zw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/h6gxof3idm6vTzGCwC7qJw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/65J6c1wTSqx-68NNaCRU5g?typeid=9</t>
+  </si>
+  <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/BlxZvHJU1w5vlVvV3EqlXg?typeid=9</t>
   </si>
   <si>
@@ -121,13 +610,253 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/75mzJEXQUlqOUK6jOkSFvw?typeid=9</t>
   </si>
   <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/JfNJkibqwkf3ALmQsoqf9w?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/QdvjM3jxQOYglY2Gp2NgIQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/NQxqNqY1W6Y6z7xGQyKUvQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/0FIpdQsOY4ttnb_dXBT1sA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/4lJwtoH8B5KhGEctejJNZw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/O3bkuQKuH26ZV0XXbJYucQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/4V7Iv__GIhGG03D1ghBXOQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/QW-rc-JUvcOMq_9P2SjxLA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/pYQ-ddE0kOM_t_QJfc8xjw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/2_g7KcaGpuqcmjonS_tseQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/HS0hjvHxAOTCPtNPmDo7Bw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/LpD4TCQApQ9vv1V6scwESw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/1j8W3yYnAz6bFopxt7_Www?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/V6pewvqk9-nbn5aARuSARw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/yaxkF9NPpjDvDsdKXaitsQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/BIeGHTPRfBMrzrGAaJhH_Q?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/HzWKglQxOhCvZk1kKg0VyA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/W8nseTHzy75Qbnpgavjk-A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/CzOFlvhEpIoqdOEuGLOb8A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/nM5PTloj8i3dm5h_EI3lHA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/F95aOtuKwrsJ347Xslc-ZA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Ve2G8PYEHCAhycgrH0Q1PQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/ZgKW-VupBVtp_sGz2YXXaQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/auHSp7RyQ7EesQkbPZBoaA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/5NpKu8jZAKdJssJnlGxTXA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/a_nNEk7-jcJcUMqE3M-Xeg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/zqUqseKSNKJint4YMEddiQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/9pKIzKzZOpp4HocU3uCl6g?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/c8C9gtHwUNnkywyMqWoLJQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/3A_GxvlYM4wkYEYTlozw6A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/0M4E0GxUuEj9_0rHwVlPAw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/3LyPF-Dt0AhduqNnRwp9zg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/kJJ5ZOZig6PA2ZAu2VMRQQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/mDFLj0aLsQztMI7vnMSy1w?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/HmZ7CIAda5ftC781xMTSKg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/zK5fwXiSohil4etG3pphhw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/NC6r7Z2A5ylk0AUMFxAkcA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/H95sl3L-tIrq1-o71rj8Gg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/7IX7KD-nM2TmIYgml7lDWg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/OakZRZ4dYRYEnX-_s__Dag?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Lby0PKwYfroFHd13wPbOdg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/ODtiZA3OtV7lf4IEVECBkA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/k9iJeEl5uPkgkCmCWtGZDg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/8QrfZwt787Bjeoh31UZztg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/B8Zac1K5GfDJSO8oDKcNfQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/4p1T6MpeJyRyu1syfZDUyw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/u9SuLf-DGkfywEXISH7pIw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/j5bFJQGngMHxaaQIK-j12w?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/hbSnCh8vhAKj2CsaFwbmZA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/tEf1nYt3fuARSRqFzbGbmw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/StnIZRaP2BZTFrduQfgCdg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/TAeqHS3g8G3Qbp3EGZkXSQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/f9isJQRtYK4rL9_Zmd4VUw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/3EaqopBnYL-XoDtMI8qQEA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/-bdXbaKzQLCvX8s69vQWQA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/gpzjNU57zwqDAfQJhI7fMA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/7ZPV_qpP_nL8FkiGNv1sbQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/R-DB5ro9NqAlSEStj_Uaxw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/2E5FJ55LFelexPtiSn3gbQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/84kDjSBTHU75sIoWKAdKcg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/DRnT39ZhmbVd21bWvHIEng?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/dmyxdxokdprJxTw9L5O5Bw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Aaw09pr_bNORqPc8F1fUSA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/832w8RYL7puxozPKMoTSAg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/A_4V_ZEYMJgH3nzjXxy21w?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/OOQWHbZwyOpZ-GpkKOgyYw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/iGXRaqo6rnJ0Gh9PFDovyg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/XUjGVcW2wV5HhfnxjVqg0w?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/eCpD5uFuWNjGpxhqMKIZ8A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/MHEOJlq75e2VYGkuBMGeJQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/-9laBujLZpjBzFaf_j8hcg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Z3woynaHMpHEAcv_YpZBHA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/6RR01Fye2xDT2mAOqhAoSg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/YCIJBF3p851kbsP5H1TZtw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/3iNNwroO0OrdsItewXo_GA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/itht4O09O7Hzx42_eMrmqw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/A_H9_tpR0cCtxnrn6ywmyg?typeid=9</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-08\$\@\$中央流行疫情指揮中心今(8)日表示，在國人共同努力配合下，國內疫情已在控制中，惟仍有部分感染事件發生，參酌世界各國管制作為及經驗，防疫措施鬆綁須逐步執行，才可穩定掌握疫情狀況，為確保國人健康，指揮中心經評估後決定，同步延長全國疫情警戒第三級至7月26日止，並適度鬆綁部分措施，說明如下：\$\@\$一、適度鬆綁措施：\$\@\$(一)    有條件鬆綁對象（地方政府得視防疫需要因時因地調整）：\$\@\$1.    戶外：國家公園、國家風景區、遊樂園區、休閒農場、森林遊樂區、植物園、文化園區、學校操場、駕訓班。\$\@\$2.    室內：美術館、博物館、電影院、表演場館(無觀眾)、社教機構、文化中心。\$\@\$3.    室內外運動場館(游泳池除外)、高爾夫球場。\$\@\$4.    餐飮場所(餐廳、傳統市場及夜市、百貨賣場 美食街、美食區等)符合指揮中心指引得內用。\$\@\$5.    國內小型旅行團(9人以下)、劇組拍攝。\$\@\$(二)    上述鬆綁須遵照通案性原則及主管機關指引：\$\@\$1.    實聯制、出入口管制、人流管控降載。\$\@\$2.    維持社交距離，除飮食外，全程戴口罩。\$\@\$3.    員工人員健康管理、確診事件即時應變。\$\@\$二、三級警戒延長仍須關閉之場所：\$\@\$(一)    休閒娛樂場所：\$\@\$歌廳、舞廳、夜總會、俱樂部、酒家、酒吧、酒店(廊)、錄影節目帶播映場所(MTV)、視聽歌唱場所(KTV)、理容院(觀光理髮、視聽理容)、指壓按摩場所、健身休閒中心(含提供指壓、三溫暖等設施之美容瘦身場所)、保齡球館、撞球場、室內螢幕式高爾夫練習場、遊藝場所、電子遊戲場、資訊休閒場所、休閒麻將館、自助選物販賣機營業場所、釣蝦場、桌遊場所及其他類似場所。\$\@\$(二)    教育學習場域：\$\@\$社區大學、樂齡學習中心、訓練班(駕訓班除外)、K書中心等其他類似場所。\$\@\$(三)    觀展觀賽場所：\$\@\$會展場館、游泳池等其他類似場所。\$\@\$指揮中心表示，鬆綁過程是疫情重要關鍵，籲請全國民眾持續落實遵循並積極配合三級警戒管制及鬆綁規定相關措施，與政府共同努力，嚴守社區防線。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-08\$\@\$中央流行疫情指揮中心今(8)日公布國內新增21例COVID-19確定病例，分別為18例本土及3例境外移入；另確診個案中新增3例死亡。\$\@\$指揮中心表示，今日新增之18例本土病例(其中6例為居家隔離期間或期滿檢驗陽性者)，為8例男性、10例女性，年齡介於未滿5歲至60多歲，發病日介於今(2021)年7月1日至7月7日。個案分布以臺北市12例最多，其次為新北市6例；其中9例為已知感染源、9例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增3例死亡個案，為2例男性、1例女性，年齡介於60多歲至70多歲，發病日介於5月27日至6月14日，確診日介於5月28日至6月17日，死亡日介於7月5日至7月6日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月6日累計公布13,889位確診個案中，已有11,456人解除隔離，解隔離人數達確診人數82.5%。\$\@\$指揮中心表示，今日新增3例境外移入中，案15252為本國籍30多歲男性，6月23日自泰國返臺，持有搭機前3日內檢驗陰性報告，入境後至防疫旅館檢疫，7月6日檢疫期滿前採檢，於今日確診；個案在臺期間並無症狀，且檢疫期間未與他人接觸，故無匡列接觸者。案15253為印尼籍20多歲男性漁工，5月10日自印尼來臺，持有搭機前3日內檢驗陰性報告，入境後至集中檢疫所檢疫，5月23日檢疫期滿前採檢結果為陰性，7月7日因有離境需求再次採檢，於今日確診；個案在臺期間並無症狀，已匡列接觸者221人，其中60人列居家隔離，餘161人列自我健康監測。案15254為本國籍10多歲女性，7月6日自美國返臺，持有搭機前3日內檢驗陰性報告，入境時在機場採檢，於今日確診；個案在臺期間並無症狀，相關接觸者匡列中。\$\@\$指揮中心統計，截至目前國內累計1,541,974例新型冠狀病毒肺炎相關通報(含1,525,372例排除)，其中15,149例確診，分別為1,193例境外移入，13,903例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計105例移除為空號。自2020年起累計 718例COVID-19死亡病例，其中710例本土，個案居住縣市分布為新北市363例、臺北市272例、基隆市24例、桃園市20例、彰化縣12例、新竹縣7例、臺中市4例、宜蘭縣及花蓮縣各2例，苗栗縣、臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月8日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-08\$\@\$針對媒體報導「指揮中心設局召開記者會」，中央流行疫情指揮中心今(8)日說明如下：\$\@\$一、針對臺北市環南市場進行大規模PCR篩檢且41人呈現陽性，顯示有群聚感染疫情，指揮中心於7月2日11:30前往環南市場現場召開記者會，並宣布與臺北市政府共同成立聯合前進指揮所。\$\@\$二、當日陳時中指揮官於9:45致電黃珊珊副市長，黃副市長將電話轉交給柯文哲市長，陳指揮官與柯市長直接通話，雙方對成立聯合前進指揮所達成共識，並在環南市場現場召開記者會。\$\@\$三、當日農委會陳吉仲主委於10:00多左右，親自致電二通予臺北市黃副市長，並於第二通電話中明確告知黃副市長，陳指揮官、經濟部王美花部長及農委會陳吉仲主委將至環南市場召開記者會，並邀請黃副市長出席，黃副市長表示柯市長也會出席。\$\@\$四、指揮中心表示，當日均依照指揮中心記者會程序，發布採訪通知；指揮中心幕僚抵達環南市場後，亦與臺北市市場處高副處長確認記者會場地、流程及雙方出席人員，同時與現場媒體溝通說明記者會流程，及預定出席人員。\$\@\$五、當日11:01，臺北市府陳智菡發言人於臺北市府群組發布採訪通知，說明柯市長、黃副市長皆會出席記者會； 11:20柯市長、黃副市長抵達環南市場。\$\@\$六、指揮中心說明，為儘快有效控制疫情，召開記者會說明防疫作為及因應措施，以利相關市場攤商、工作人員及周邊住民了解需配合之事項，並無「以開會名義設局召開記者會」一事。</t>
+  </si>
+  <si>
     <t>發佈日期：2021-07-07\$\@\$中央流行疫情指揮中心今(7)日表示，第二批AstraZeneca疫苗約62.6萬劑，預定今日下午3時40分抵達桃園國際機場。\$\@\$指揮中心說明，本批疫苗為我國與供應商(阿斯特捷利康公司)採購之一部分，首批11.7萬劑已於3月3日到貨，第二批今日抵臺疫苗完成通關程序後，將直接運送至指定冷儲物流中心進行後續檢驗封緘作業，再提供COVID-19接種計畫所列實施對象接種。\$\@\$指揮中心指出，該中心係於去(2020)年10月30日與臺灣阿斯特捷利康公司簽署1,000萬劑COVID-19疫苗供應合約，該公司也協助交付經由COVAX供應和日本捐贈的AstraZeneca疫苗。本次提供之疫苗係為多劑型包裝(每瓶10人份)，需存放於2-8℃的環境，本批效期至110年10月30日。</t>
   </si>
   <si>
-    <t>發佈日期：2021-07-07\$\@\$中央流行疫情指揮中心今(7)日公布國內新增40例COVID-19確定病例，分別為39例本土及1例境外移入；另確診個案中新增9例死亡。\$\@\$指揮中心表示，今日新增之39例本土病例(其中21例為居家隔離期間或期滿檢驗陽性者)，為21例男性、18例女性，年齡介於未滿10歲至80多歲，發病日介於今(2021)年6月26日至7月6日。個案分布以臺北市與新北市各14例最多、其次為桃園市11例；其中23例為已知感染源、4例關聯不明、12例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增9例死亡個案，為4例男性、5例女性，年齡介於40多歲至90多歲，發病日介於5月13日至6月27日，確診日介於5月18日至6月29日，死亡日介於7月3日至7月5日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月5日累計公布13,862位確診個案中，已有11,277人解除隔離，解隔離人數達確診人數81.4%。\$\@\$指揮中心表示，今日新增境外移入個案(案15208)，為本國籍40多歲女性，7月4日自泰國入境，持有搭機前3日內檢驗陰性報告，個案入境時並無症狀，於機場採檢後至檢疫旅館檢疫，於今日確診，衛生單位已匡列個案同班機前後2排座位旅客共7人，皆列居家隔離。\$\@\$指揮中心統計，截至目前國內累計1,532,252例新型冠狀病毒肺炎相關通報(含1,515,985例排除)，其中15,128例確診，分別為1,190例境外移入，13,885例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；無新增空號病例，累計105例移除為空號。自2020年起累計累計715例COVID-19死亡病例，其中707例本土，個案居住縣市分布為新北市361例、臺北市271例、基隆市24例、桃園市20例、彰化縣12例、新竹縣7例、臺中市4例、宜蘭縣及花蓮縣各2例，苗栗縣、臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月7日新增死亡COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-07\$\@\$網路謠傳「有1922回復，系統異常讓其他地區民眾預約登記、疾管署討論虛擬預約或取消方式處理、及正式預約開始要向1922確認」等資訊，中央流行疫情指揮中心今(7)日澄清，「COVID-19疫苗施打意願登記與預約系統」(1922.gov.tw)運作順暢並無異常，且已正式上線，並非虛擬預約，所有登記成功者皆已記錄在案，除非事後自行取消，否則已登記之紀錄並不會受到影響。前述相關網路訊息均非疾管署或1922防疫專線發布、回復，且內容多有不實，籲請民眾勿信、轉傳與散布。\$\@\$指揮中心說明，有關「COVID-19疫苗施打意願登記與預約系統」其設計目前為開放全國第9、10類對象民眾進行疫苗施打意願登記，故不限金馬澎地區登記意願；惟完成意願登記者，須符合當時公布開放預約之接種年齡及資格條件，系統平台會按疫苗分配情形以簡訊通知符合預約資格的民眾，收到簡訊通知者即可進行下一步預約接種。如有完成意願登記但不符合當時預約資格，則暫時不會收到預約接種簡訊且無法預約接種。而本次以離島金門、馬祖和澎湖先行試辦意願登記及預約接種，未來將再逐步開放到全國，截至今日8時，全國已有約148萬符合第9、10類接種對象完成意願登記，其中離島金門、馬祖及澎湖之意願登記人數約為4千5百人。\$\@\$指揮中心指出，目前全國1-8類對象已開放接種，符合該等對象資格者可依縣市政府規劃安排接種。昨日上線之「COVID-19疫苗施打意願登記與預約系統」，係為建立一個讓大量疫苗接種能依序穩定有效推行之機制，請符合第9、10類對象民眾先進行意願登記，再依簡訊通知，進行預約接種。\$\@\$指揮中心強調，網路謠傳「有1922回復，系統異常讓其他地區民眾預約登記、疾管署討論虛擬預約或取消方式處理、及正式預約開始要向1922確認」等資訊皆為不實訊息且均非發布自疾管署或1922防疫專線，籲請民眾勿信、轉傳與散布。</t>
+    <t>發佈日期：2021-07-07\$\@\$中央流行疫情指揮中心今(7)日公布國內新增40例COVID-19確定病例，分別為39例本土及1例境外移入；另確診個案中新增9例死亡。\$\@\$指揮中心表示，今日新增之39例本土病例(其中21例為居家隔離期間或期滿檢驗陽性者)，為21例男性、18例女性，年齡介於未滿10歲至80多歲，發病日介於今(2021)年6月26日至7月6日。個案分布以臺北市與新北市各14例最多、其次為桃園市11例；其中23例為已知感染源、4例關聯不明、12例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增9例死亡個案，為4例男性、5例女性，年齡介於40多歲至90多歲，發病日介於5月13日至6月27日，確診日介於5月18日至6月29日，死亡日介於7月1日至7月5日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月5日累計公布13,862位確診個案中，已有11,277人解除隔離，解隔離人數達確診人數81.4%。\$\@\$指揮中心表示，今日新增境外移入個案(案15208)，為本國籍40多歲女性，7月4日自泰國入境，持有搭機前3日內檢驗陰性報告，個案入境時並無症狀，於機場採檢後至檢疫旅館檢疫，於今日確診，衛生單位已匡列個案同班機前後2排座位旅客共7人，皆列居家隔離。\$\@\$指揮中心統計，截至目前國內累計1,532,252例新型冠狀病毒肺炎相關通報(含1,515,985例排除)，其中15,128例確診，分別為1,190例境外移入，13,885例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；無新增空號病例，累計105例移除為空號。自2020年起累計累計715例COVID-19死亡病例，其中707例本土，個案居住縣市分布為新北市361例、臺北市271例、基隆市24例、桃園市20例、彰化縣12例、新竹縣7例、臺中市4例、宜蘭縣及花蓮縣各2例，苗栗縣、臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月7日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-07\$\@\$網路謠傳「有1922回復，系統異常讓其他地區民眾預約登記、疾管署討論虛擬預約或取消方式處理、及正式預約開始要向1922確認」等資訊，中央流行疫情指揮中心今(7)日澄清，「COVID-19疫苗施打意願登記與預約系統」(1922.gov.tw)運作順暢並無異常，且已正式上線，並非虛擬預約，所有登記成功者皆已記錄在案，除非事後自行取消，否則已登記之紀錄並不會受到影響。前述相關網路訊息均非疾管署或1922防疫專線發布、回復，且內容多有不實，籲請民眾勿信、轉傳與散布。\$\@\$指揮中心說明，有關「COVID-19疫苗施打意願登記與預約系統」其設計目前為開放全國第9、10類對象民眾進行疫苗施打意願登記，故不限金馬澎地區登記意願；惟完成意願登記者，須符合當時公布開放預約之接種年齡及資格條件，系統平台會按疫苗分配情形以簡訊通知符合預約資格的民眾，收到簡訊通知者即可進行下一步預約接種。如有完成意願登記但不符合當時預約資格，則暫時不會收到預約接種簡訊且無法預約接種。而本次以離島金門、馬祖和澎湖先行試辦意願登記及預約接種，未來將再逐步開放到全國，截至今日8時，全國已有約148萬符合第9、10類接種對象完成意願登記，其中離島金門、馬祖及澎湖之意願登記人數約為4千5百人。\$\@\$指揮中心指出，目前全國1-8類對象已開放接種，符合該等對象資格者可依縣市政府規劃安排接種。昨日上線之「COVID-19疫苗施打意願登記與預約系統」，係為建立一個讓大量疫苗接種能依序穩定有效推行之機制，請符合第9、10類對象民眾先進行意願登記，再依簡訊通知，進行預約接種。\$\@\$指揮中心強調，網路謠傳「有1922回復，系統異常讓其他地區民眾預約登記、疾管署討論虛擬預約或取消方式處理、及正式預約開始要向1922確認」等資訊皆為不實訊息且均非發布自疾管署或1922防疫專線，籲請民眾勿信、轉傳與散布。 圖片 附件\$\@\$網傳COVID-19疫苗施打登記系統異常為不實訊息 全國第9、10類皆可登記且紀錄不會被消除.jpg</t>
   </si>
   <si>
     <t>發佈日期：2021-07-06\$\@\$中央流行疫情指揮中心今(6)日公布國內新增29例COVID-19確定病例，分別為27例本土及2例境外移入；另確診個案中新增17例死亡。\$\@\$指揮中心表示，今日新增之27例本土病例(其中15例為居家隔離期間或期滿檢驗陽性者)，為17例男性、10例女性，年齡介於未滿5歲至70多歲，發病日介於今(2021)年6月10日至7月5日。個案分布以臺北市14例最多，其次為新北市11例、屏東縣及彰化縣各1例；其中17例為已知感染源、10例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增17例死亡個案，為14位男性、3位女性，發病日介於5月16日至7月2日，確診日介於5月19日至7月5日，死亡日介於6月28日至7月5日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月4日累計公布13,831位確診個案中，已有11,180人解除隔離，解隔離人數達確診人數80.8%。\$\@\$指揮中心表示，今日新增境外移入個案中，案15180為本國籍10多歲男性，7月4日自美國入境，持有搭機前3日內檢驗陰性報告，入境時並無症狀，於機場採檢後至防疫旅館檢疫，7月5日出現嗅味覺異常等症狀，於今日確診，相關接觸者匡列中。案15185為本國籍30多歲男性，6月30日自印尼入境，持有搭機前3日內檢驗陰性報告，入境後至集中檢疫所檢疫並進行採檢，當日採檢結果為陰性；7月4日出現發燒、肌肉痠痛、流鼻水等症狀，7月5日由衛生單位採檢送驗，於今日確診，同班機旅客均已入境採檢並入住集中檢疫所。\$\@\$指揮中心統計，截至目前國內累計1,503,584例新型冠狀病毒肺炎相關通報(含1,487,019例排除)，其中15,088例確診，分別為1,189例境外移入，13,846例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另新增2例空號(案10180、案13124)，累計105例移除為空號。自2020年起累計706例COVID-19死亡病例，其中698例本土，個案居住縣市分布為新北市354例、臺北市269例、基隆市24例、桃園市20例、彰化縣12例、新竹縣7例、臺中市4例、宜蘭縣及花蓮縣各2例，苗栗縣、臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月6日新增死亡COVID-19確診個案表.pdf</t>
@@ -139,7 +868,151 @@
     <t>發佈日期：2021-07-06\$\@\$中央流行疫情指揮中心表示，今(6)日上午與各縣市政府召開的「全國防疫會議」，決議如下：\$\@\$一、國內疫情現況及評估\$\@\$1.疾病傳播能力雖呈現下降趨勢，惟部分縣市仍有群聚事件爆發，請各地方政府持續密切注意監測，早期發現並介入；另國內出現Delta變異株相關群聚，將強化國內病毒變異株基因監測外，鑒於該病毒株具高傳播力，未來可能成為主流病毒變異株，爰請各地方政府重新檢視病患收治轉送及醫療照護體系量能之整備。\$\@\$2.雙北部分，臺北市出現較大規模市場群聚，考量市場人流多屬不特定對象，請該市衛生機關加強轄內社區、市民及醫療院所警覺，並於市場周邊設置篩檢站；新北市亦有出現家禽市場群聚，請該市衛生機關持續留意後續疫情變化。\$\@\$二、疫苗施打意願登記與預約系統\$\@\$1.有關行政院唐鳳政務委員設計開發之「疫苗施打意願登記與預約系統」，重點如下：\$\@\$1)登記與預約四步驟：意願登記→1922以簡訊通知符合資格民眾→預約接種→接種疫苗。\$\@\$2)登記對象：第9類(18歲至64歲，患有高風險疾病、罕見疾病或重大傷病者)及第10類(50-64歲成人)符合公費疫苗接種對象。\$\@\$3)預約及登記平台：可採線上1922.gov.tw或手機app「健保快易通」(全名「全民健保行動快易通」)預約，或者持健保卡到超商、藥局、衛生所插卡預約。\$\@\$4)試辦時間及區域：7月6日上午10點至7日下午5點開放登記，7月8日上午10點至9日下午5點開放預約，於金門、馬祖、澎湖進行試辦。後續視試辦2週之成效後，再推動至全國。\$\@\$2.本系統啟動條件，以中央流行疫情指揮中心開放對象，進行逐步啟動，現行為第9及第10類民眾，另針對偏鄉或年長者意願及預約登記服務部分，請各地方政府各鄉鎮市公所提供協助作業。\$\@\$3.至於疫苗配撥安排，現階段以毎週提供單一品牌疫苗預約為原則，後續視疫苗到貨情況再行研議調整。\$\@\$三、針對第七類優先接種對象認定及疫苗配發施打作業，指揮中心依各專案主管部會造冊人數陸續進行疫苗核撥作業，鑒於造冊施打對象亦為各縣市的居民，且疫苗撥配量原則會多於專案造冊人數，爰請地方政府協助各部會疫苗依施打作業或計畫，進行各該對象之接種作業。</t>
   </si>
   <si>
+    <t>發佈日期：2021-07-05\$\@\$針對近日媒體報導「疾病管制署造冊人數，超過編制內人數」一事，中央流行疫情指揮中心今(5)日表示，為維持防疫體系運作，相關防疫人員與醫護人員均列為COVID-19公費疫苗接種的優先施打對象，包含第一類「維持醫療量能–醫事人員」及第二類「中央及地方政府防疫人員」，其中第二類對象為「維持防疫體系運作之中央及地方政府重要官員」、「衛生單位第一線防疫人員」以及「港埠執行邊境管制之海關檢查、證照查驗、人員檢疫及動植物檢疫、安全檢查及航空安全等第一線工作人員」等。\$\@\$指揮中心指出，疾管署為COVID-19防疫主責機關，負責疫情監控、邊境檢疫、社區防疫、感染管制及病毒檢驗事項等相關業務，該署造冊1,261人，其對象除了編制內人員(正式職員、聘僱人員、工級人員)850人外，尚有研發替代役、臨時人員、駐點及承攬人員等411人，該等人員負責協助支援各項業務推動，包含協勤保全人員、資訊委外駐點等，協助邊境檢疫作業及檢疫、隔離與預防接種等系統管理維運，均擔負重要職責，亦屬指揮中心公布之第一類「維持醫療量能–醫事人員」及第二類「維持防疫量能-中央及地方政府防疫人員」。\$\@\$指揮中心強調，因應COVID-19疫情，為維持防疫量能，又將防疫視同作戰，故以防疫業務推動與確保同仁防護能力為首要，進行相關人員接種作業，以避免影響防疫業務的正常運作。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-05\$\@\$中央流行疫情指揮中心今(5)日公布國內新增31例COVID-19確定病例，分別為28例本土及3例境外移入；另確診個案中新增1例死亡。\$\@\$指揮中心表示，今日新增之28例本土病例(其中13例為居家隔離期間或期滿檢驗陽性者)，為9例男性、19例女性，年齡介於未滿5歲至90多歲，發病日介於今(2021)年6月19日至7月4日。個案分布以臺北市15例最多，其次為新北市5例、桃園市3例、苗栗縣2例，屏東縣、基隆市及新竹縣各1例；其中16例為已知感染源、1例關聯不明、11例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增1例死亡個案(案12752)，為70多歲女性，具慢性病史及其他確診者接觸史；個案於6月11日出現發燒、呼吸困難症狀，同日就醫採檢並住院治療，6月12日確診，7月3日死亡。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月3日累計公布13,792位確診個案中，已有11,008人解除隔離，解隔離人數達確診人數79.8%。\$\@\$指揮中心表示，今日新增3例境外移入中，案15152為本國籍未滿5歲女童，6月21日自美國入境，持有搭機前3日內檢驗陰性報告，入境後於自宅進行居家檢疫，7月4日進行期滿前採檢，於今日確診(Ct值33)，個案在臺期間並無症狀，相關接觸者匡列中。案15155為本國籍20多歲男性，7月1日自英國返臺，持有搭機前3日內檢驗陰性報告，入境後至集中檢疫所檢疫並採檢，當日採檢結果為陰性，7月2日出現鼻塞、喉嚨癢、輕微發燒等症狀，7月4日通報衛生單位後安排採檢送驗，於今日確診(Ct值22)，相關接觸者匡列中。案15164為本國籍50多歲男性，7月2日自沙烏地阿拉伯返臺，持有搭機前3日內檢驗陰性報告，入境時在機場採檢後至防疫旅館檢疫，於今日確診；個案在臺期間並無症狀，相關接觸者匡列中。\$\@\$指揮中心統計，截至目前國內累計1,472,827例新型冠狀病毒肺炎相關通報(含1,455,971例排除)，其中15,061例確診，分別為1,187例境外移入(原7月4日公布之本土個案15109、15110 ，經疫調採檢後改判為境外移入)，13,821例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計103例移除為空號。自2020年起累計689例COVID-19死亡病例，其中681例本土，個案居住縣市分布為新北市349例、臺北市261例、基隆市22例、桃園市20例、彰化縣11例、新竹縣6例、臺中市4例、宜蘭縣及花蓮縣各2例，苗栗縣、臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。</t>
+  </si>
+  <si>
     <t>發佈日期：2021-07-04\$\@\$中央流行疫情指揮中心今(4)日公布國內新增39例COVID-19確定病例，分別為37例本土及2例境外移入；另確診個案中新增2例死亡。\$\@\$指揮中心表示，今日新增之37例本土病例(其中13例為居家隔離期間或期滿檢驗陽性者)，為12例男性、25例女性，年齡介於未滿5歲至90多歲，發病日介於今(2021)年6月17日至7月3日。個案分布以臺北市18例最多，其次為新北市11例、桃園市及彰化縣各3例、宜蘭縣2例；其中16例為已知感染源、3例關聯不明、18例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增2例死亡個案(案8089、12577)，分別為70多歲女性及80多歲男性，發病日為5月18日及6月9日，確診日為5月30日及6月11日，死亡日為7月2日及6月17日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月2日累計公布13,712位確診個案中，已有10,868人解除隔離，解隔離人數達確診人數79.3%。\$\@\$指揮中心表示，今日新增2例境外移入中，案15113為本國籍50多歲女性，7月2日自柬埔寨返臺，持有搭機前3日內檢驗陰性報告，入境時有發燒症狀，在機場採檢後送醫治療，於今日確診；相關接觸者匡列中。案15129為本國籍30多歲男性，6月30日起陸續出現頭痛、喉嚨痛及流鼻水等症狀，7月3日自印尼返臺，持有搭機前3日內檢驗陰性報告，入境時主動通報有症狀並在機場採檢，於今日確診；已掌握個案同行返臺之友人1名，其在臺期間並無症狀，檢體檢驗中，已列居家隔離，其餘同班機接觸者匡列中。\$\@\$指揮中心統計，截至目前國內累計1,459,913例新型冠狀病毒肺炎相關通報(含1,442,937例排除)，其中15,030例確診，分別為1,182例境外移入，13,795例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計103例移除為空號。自2020年起累計688例COVID-19死亡病例，其中680例本土，個案居住縣市分布為新北市349例、臺北市260例、基隆市22例、桃園市20例、彰化縣11例、新竹縣6例、臺中市4例、宜蘭縣及花蓮縣各2例，苗栗縣、臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月4日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-02\$\@\$中央流行疫情指揮中心今(2)日表示，因應臺北市環南市場疫情，將於今日針對6月8日起，曾於相關時間及地點出入之民眾，發送疫情警示簡訊，內容如下：\$\@\$[疫情警示]如您曾至環南市場，且6月8日之後曾有發燒、呼吸道症狀，腹瀉，或嗅、味覺異常等疑似症狀，請就醫評估或可至社區篩檢站採檢。\$\@\$指揮中心說明，收到簡訊者若有不適，務必正確佩戴外科口罩儘速就醫，不可搭乘大眾交通工具，就醫時應主動告知醫療人員相關暴露及接觸史。指定社區採檢院所醫院清單可至疾病管制署網站查詢：http://at.cdc.tw/5y262t。\$\@\$備註：本次簡訊發送範圍：\$\@\$北至：萬板大橋\$\@\$東至：西藏路\$\@\$南至：華翠大橋\$\@\$西至：環河快速道路</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-02\$\@\$中央流行疫情指揮中心今(2)日公布國內新增58例COVID-19確定病例，分別為57例本土及1例境外移入；另確診個案中新增15例死亡。\$\@\$指揮中心表示，今日新增之57例本土病例(其中22例為居家隔離期間或期滿檢驗陽性者)，為25例男性、32例女性，年齡介於未滿5歲至90多歲，發病日介於今(2021)年6月22日至7月1日。個案分布以臺北市29例最多，其次為新北市15例、新竹縣4例、桃園市及基隆市各3例、臺中市2例、新竹市1例；其中28例為已知感染源、6例關聯不明、23例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增15例死亡個案，為8例男性、7例女性，年齡介於40多歲至80多歲，發病日介於5月25日至6月21日，確診日介於5月28日至6月28日，死亡日介於6月3日至6月30日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至6月30日累計公布13,605位確診個案中，已有10,347人解除隔離，解隔離人數達確診人數76.1%。\$\@\$指揮中心表示，今日新增1例境外移入中(案14975)，為本國籍50多歲女性，6月28日自匈牙利返臺，持有搭機前3日內檢驗陰性報告，入境後至防疫旅館檢疫，7月1日申請外出奔喪，由衛生單位安排至醫院自費採檢，於今日確診；個案在臺期間並無症狀，相關接觸者匡列中。\$\@\$指揮中心統計，截至目前國內累計1,411,572例新型冠狀病毒肺炎相關通報(含1,395,446例排除)，其中14,911例確診，分別為1,176例境外移入，13,682例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計103例移除為空號。自2020年起累計676例COVID-19死亡病例，其中668例本土，個案居住縣市分布為新北市343例、臺北市256例、基隆市21例、桃園市20例、彰化縣11例、新竹縣5例、臺中市4例、宜蘭縣及花蓮縣各2例，苗栗縣、臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月2日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-02\$\@\$中央流行疫情指揮中心表示，今(2)日上午與各縣市政府召開的「全國防疫會議」，決議如下：\$\@\$一、鑒於國內仍有職場、機構、醫院、社區等場域群聚事件發生，請相關地方政府持續落實疫調及接觸者匡列、社區篩檢及監測，以利早期發現病例，早期介入；另近期人流有上升趨勢，請各地方政府加強宣導落實三級警戒注意事項。\$\@\$1.雙北部分：臺北市近期發生市場、機構及工地等群聚，須留意防範擴散至社區，並加強疫調及跨縣市疫情通報；另建議持續考量民眾就醫可近性，設置社區篩檢站。\$\@\$2.屏東縣部分：Delta變異株進入枋山社區，目前當地疫情雖已控制，仍請屏東縣政府擴大社區篩檢及居民健康監測，提升當地民眾及醫療院所防疫警覺。\$\@\$二、針對第七類「國家關鍵基礎設施及高風險接種人員等專案」對象疫苗配撥及接種作業，已請相關中央目的事業主管機關，於中央流行疫情指揮中心第86次大會(6月29日)中，就接種計畫進行報告，也請各部會與地方政府業務隸屬之局處聯繫，務必向縣市首長報告專案實施內容，讓縣市首長充分瞭解。\$\@\$三、有關地方政府建議擴大疫苗施打對象部分，指揮中心均會就疫情狀況、疫苗可分配數量、接種情形等持續綜合評估，滾動規劃後續納入施打之開放類別目標族群，請各地方政府配合指揮中心規劃，確實將撥配疫苗施打於優先開放之類別目標族群。\$\@\$四、有關地方政府關切Moderna疫苗後續撥發規劃部分，評估疫苗保存、解涷及配發至地方等作業所需時間，目前第二批撥配日期為7月5日。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-01\$\@\$中央流行疫情指揮中心今(1)日公布，鑑於Delta變異株於全球日益擴散且其傳播力強，為降低該病毒進入國內社區風險，自今(2021)年7月2日中午12時(航機抵臺時間)起，加強國際港埠入境人員健康監測，包含：\$\@\$一、14天內具「重點高風險國家」旅遊史之入境旅客，自空港或海港入境後，一律公費入住集中檢疫所14天，且須配合入住時、檢疫期滿進行COVID-19病毒核酸檢驗(PCR)檢測；另檢疫期間增加第10至12天以「家用快篩」採檢一次。\$\@\$二、14天內無「重點高風險國家」旅遊史之入境旅客，自空港或海港入境時皆須配合採深喉唾液及進行PCR檢測，並搭乘防疫車隊前往防疫旅宿或自費入住集中檢疫場所接續完成14天檢疫，且於檢疫期滿前(檢疫第12至14天)PCR檢測，另增加第10至12天以「家用快篩」採檢一次。\$\@\$三、所有入境旅客，檢驗為陽性者，均進行病毒基因定序。\$\@\$指揮中心強調，邊境管制為防範COVID-19疫情的重要關鍵，入境旅客抵臺時應主動配合邊境加強監測措施，並依指揮中心規定的交通方式前往檢疫地點及配合後續防疫相關措施。落實全民共同抗疫，將疫情阻絕於境外。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-01\$\@\$疾病管制署今(1)日公布國內新增2例日本腦炎確定病例，為彰化縣鹿港鎮本國籍50多歲男性及臺中市大安區越南籍20多歲男性，發病日分別為6月16日及6月24日，症狀包括發燒、頭痛、嘔吐及意識改變等，經就醫通報後確診，目前均仍住院治療中。\$\@\$疾管署表示，2名個案近期均無國內外旅遊史，平時活動地以居住地及工作地為主。衛生單位於2人活動地周邊發現有豬舍或水稻田等高風險場所，研判於活動地附近感染的可能性較高，並已前往個案活動地周邊進行環境滅蚊及誘蚊燈懸掛等防治措施，同時加強對當地民眾衛教宣導。\$\@\$疾管署監測資料顯示，國內今(2021)年截至目前共6例確定病例，個案居住地分別為基隆市、臺中市、彰化縣、臺南市、高雄市及屏東縣各1例，個案活動地附近均有高風險環境；2017至2020年全國同期確定病例數分別為12、25、12及13例，以40歲以上成人較多，惟各年齡層都有感染風險，民眾不可掉以輕心。\$\@\$疾管署指出，臺灣每年5至10月為日本腦炎流行季，其中6至7月為流行高峰。在臺灣以三斑家蚊、環紋家蚊及白頭家蚊為主要病媒蚊，常孳生於水稻田、池塘及灌溉溝渠等處，吸血高峰為黃昏與黎明時段。大部分的人感染日本腦炎後大多無明顯症狀，少數會有頭痛、發燒或無菌性腦膜炎，嚴重則可能出現意識改變、對人時地不能辨別、全身無力、腦神經功能損傷、輕癱等，甚至昏迷或死亡。請民眾儘量避免於病媒蚊吸血高峰時段，在上述易孳生病媒蚊之高風險環境附近活動；如果無法避免，應穿著淺色長袖衣褲，並於身體裸露處使用政府機關核可，含敵避(DEET)、派卡瑞丁(Picaridin)或伊默克(IR3535)成分的防蚊藥劑。\$\@\$疾管署呼籲，預防日本腦炎最有效的方法為接種日本腦炎疫苗，提醒民眾應按時帶家中滿15個月以上的幼兒至各地衛生所或合約院所接種疫苗，以避免因感染衍生嚴重後遺症。住家或活動地鄰近豬舍、水稻田等高風險環境的民眾應加強防蚊，如自覺有感染風險的成人，可前往旅遊醫學門診評估自費接種疫苗。相關資訊可至疾管署網站(https://www.cdc.gov.tw)或撥打免付費防疫專線1922(或0800-001922)洽詢。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-01\$\@\$中央流行疫情指揮中心今(1)日表示，本土確診案例連續1週低於百人，經考量失能者家庭照顧需求，及家庭較無其他替代人力，且不致有產業移工群聚擴大傳染風險等因素，自即日起優先恢復外籍家庭看護工及家庭幫傭，得轉換由家庭類雇主接續聘僱(含期滿轉換)；至於其他產業移工仍暫緩轉換，未來將視疫情再行檢討。\$\@\$指揮中心表示，家庭類雇主接續聘僱(含期滿轉換)家庭類移工應辦理以下事項：\$\@\$一、安排移工核酸檢驗（下稱PCR）：承接家庭類移工之新雇主應於接續聘僱（含期滿轉換）當日安排移工至合格醫療機構檢驗PCR，檢測費用應由新雇主支付。\$\@\$二、雇主應依指引辦理防疫措施：倘若接續聘僱移工檢測PCR確診時，新雇主應負雇主責任，並依勞動部「因應嚴重特殊傳染性肺炎雇主聘僱移工指引：移工工作、生活及外出管理注意事項」(下稱雇主指引)，配合衛生單位安排就醫或送集中檢疫所隔離治療，並依確診個案處置及解除隔離治療條件接續處理。倘若接續聘僱移工檢測PCR陰性，新雇主應依雇主指引，每日進行移工健康監測及記錄移工出入足跡。\$\@\$指揮中心進一步表示，新雇主若未於接續聘僱(含期滿轉換)當日，安排移工檢驗PCR，將依「就業服務法」第57條第9款規定，處新臺幣6萬至30萬元罰鍰，並不予核發接續聘僱許可及廢止名額。另雇主如果委託仲介公司辦理移工生活照顧，但仲介公司未善盡受任事務，違反防疫措施，仲介公司將被依「仲介公司違反就業服務法」規定，處新臺幣6萬元以上至30萬元以下罰鍰。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-30\$\@\$中央流行疫情指揮中心今(30)日表示，批發市場為供應民眾農、漁、畜等民生物資的重要營業場所，因應近期批發市場出現群聚感染事件，為確保相關場域工作人員、採購民眾自身與家人健康，指揮中心與農委會共同訂定「批發市場防疫管理措施建議指引」，呼籲各批發市場遵循，以避免群聚感染、疫情擴大。\$\@\$指揮中心進一步表示，「批發市場防疫管理措施建議指引」提供主管機關、場域管理單位及工作人員，依實際可行性與適用性，內化為適合個別場域所需的管理措施，供管理單位、從業人員及採購人員遵循辦理，以降低疫情在批發市場的發生機率、規模及社區傳播風險。\$\@\$指揮中心指出，「批發市場防疫管理措施建議指引」包含以下重點防疫措施，請各批發市場遵循，以降低疫情發生：\$\@\$人員健康管理：落實市場出入人員體溫量測、實聯制。盤點及造冊相關工作人員，落實健康狀況監測、定期篩檢及訂定健康監測計畫(包含人員名單及異常追蹤處理機制)，並鼓勵接種COVID-19疫苗。\$\@\$人流管制措施：調整市場攤位配置及營業時段，減少市場之出入口、劃定人員動線及分流措施，管制人數總量及單位時間人數。\$\@\$落實人員衛生行為：張貼標語、海報或透過廣播提醒顧客、從業人員等落實戴口罩及手部衛生，增加洗手設備可近性，並儘量使用非直接與顧客接觸之收付款方式。\$\@\$個人防護裝備建議：工作人員需佩戴口罩及面罩，視需要佩戴手套或穿著防水圍裙，拋棄式口罩不可重複使用；面罩若為可重複使用者，應確實清潔消毒後重複使用。\$\@\$環境清潔消毒：訂定環境清潔及消毒計畫，定時執行環境清潔及消毒，每天至少1次以上，並增加公共廁所衛生清潔及消毒頻率。\$\@\$出現確定病例之應變措施：訂定包括風險對象管理、風險區域管理及營運降載措施等3大應變措施，批發市場若發生確診者，應通報主管機關，風險區域須暫停營業，並視影響程度，通知供應人及承銷人至鄰近市場交易。\$\@\$指揮中心表示，農委會後續將與全國各批發市場及縣市政府召開視訊說明會，並請各縣市批發市場依據公布的指引自行訂定符合實際經營樣態的防疫作業規範，確保農產品穩定供應。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-30\$\@\$中央流行疫情指揮中心今(30)日表示，第三批Moderna疫苗41萬劑，已於歐洲時間6月29日晚上9時30分自阿姆斯特丹啟運，預定今日下午4時40分抵達桃園國際機場。\$\@\$指揮中心表示，本批疫苗為我國與供應商採購之一部分，首批15萬劑已於5月28日、第二批24萬劑也於6月18日分別到貨。今日抵臺疫苗待完成通關程序後，將直接運送至指定冷儲物流中心進行後續檢驗封緘作業，再提供COVID-19接種計畫所列實施對象接種。\$\@\$指揮中心指出，該中心已於今(2021)年2月8日與美國Moderna公司簽署505萬劑COVID-19疫苗供應合約，該疫苗為多劑型包裝(每瓶10人份)，存放於-20℃可保存至少6個月，於2-8℃之使用期限為30天，依臨床試驗結果，每人需施打2劑，2劑間隔28天以上，疫苗保護效力可達94%。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-29\$\@\$針對媒體報導「COVID-19疫苗接種外展服務，無法選擇疫苗廠牌，係為國產疫苗鋪路」，中央流行疫情指揮中心今(29)日澄清，無法選擇疫苗廠牌，係因目前尚無法確認屆時可供應之疫苗廠牌與數量，並非為國產疫苗鋪路。\$\@\$指揮中心表示，為加速我國COVID-19疫苗接種作業，規劃辦理「COVID-19疫苗接種外展服務」，已於日前發文請各部會先行調查「規模1,000人以上企業」、「100人以上中央政府機關」等人員施打疫苗意願及進行造冊，並由各機關（構）自行評估是否有適合執行接種作業的地點及空間規劃等。\$\@\$有關媒體報導「該公文提到無法選擇疫苗廠牌，係為國產疫苗鋪路」，指揮中心澄清，係因目前尚無法確認屆時可供外展服務之疫苗廠牌與疫苗數量，並非為國產疫苗鋪路。待疫苗量充足，會依屆時可供應之疫苗廠牌與數量，再次詢問機關（構）參與外展服務與接種之意願。\$\@\$指揮中心進一步說明，有關「疫苗外展服務調查」，係為後續疫苗量充足且可全民接種時，疫苗需求量調查與分布之預先規劃。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-29\$\@\$中央流行疫情指揮中心今(29)日公布國內新增54例COVID-19確定病例，均為本土個案；另確診個案中新增8例死亡。\$\@\$指揮中心表示，今日新增之54例本土病例(其中17例為居家隔離期間或期滿檢驗陽性者)，為19例男性、35例女性，年齡介於未滿5歲至80多歲，發病日介於今(2021)年6月16日至6月28日。個案分布以新北市22例最多，其次為臺北市20例、桃園市及新竹縣各4例，彰化縣2例，基隆市及屏東縣各1例；其中31例為已知感染源、5例關聯不明、18例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增8例死亡個案，為5例男性、3例女性，年齡介於60多歲至80多歲，發病日介於5月9日至6月19日，確診日介於5月15日至6月20日，死亡日介於6月25日至6月27日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至6月27日累計公布13,435位確診個案中，已有10,086人解除隔離，解隔離人數達確診人數75.1%。\$\@\$指揮中心統計，截至目前國內累計1,311,961例新型冠狀病毒肺炎相關通報(含1,295,813例排除)，其中14,748例確診，分別為1,170例境外移入，13,525例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；個案中累計102例移除為空號。自2020年起累計643例COVID-19死亡病例，其中635例本土，個案居住縣市分布為新北市325例、臺北市245例、基隆市21例、桃園市18例、彰化縣10例、臺中市及新竹縣各4例、宜蘭縣及花蓮縣各2例，苗栗縣、臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月29日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-29\$\@\$中央流行疫情指揮中心表示，今(29)日上午與各縣市政府召開的「全國防疫會議」，決議如下：\$\@\$一、國內疫情雖持續下降，惟部分縣(市)仍持續爆發群聚事件，須密切注意監測，及早發現並介入防治；另國內出現Delta變異株群聚，應強化疫調早期圍堵，避免造成社區流行。\$\@\$1.雙北部分：臺北市疫情趨緩，惟轄內近期發生市場、機構及工地等群聚，須留意防範擴散至社區；新北市疫情亦趨緩，惟各行政區仍須留意後續疫情變化。\$\@\$2.屏東縣部分：因出現Delta變異株群聚，不排除未來一週仍可能檢出相關病例，請屏東縣落實精準疫調及接觸者匡列、追蹤，早期發現病例並介入防治。\$\@\$二、有關簡訊實聯制運用於疫調處理部分，鑒於簡訊實聯制推動主要作為輔助疫調之用，建置前提為民眾上傳資訊越少越好(僅有停留場所代碼及進入之時間點)，因此請各地方政府在疫情處理上仍應以精準疫調為主，簡訊實聯制為輔，地方政府如有實聯制資料運用於疫調之需求，指揮中心資訊組將會適時協助提供。\$\@\$三、針對Delta變異株之防範，有無需要調整醫療院所感染管制措施之部分，指揮中心參考比較國外感控措施，目前尚無需調整我國現行措施。至於相關確診者個案能否共同收治入院，建議地方政府在病房收治量能允許下，仍應以一人一室為主。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-28\$\@\$中央流行疫情指揮中心今(28)日公布國內新增60例COVID-19確定病例，均為本土個案；另確診個案中新增3例死亡。\$\@\$指揮中心表示，今日新增之60例本土病例(其中31例為居家隔離期間或期滿檢驗陽性者)，為26例男性、34例女性，年齡介於未滿10歲至90多歲，發病日介於今(2021)年6月19日至6月27日。個案分佈以新北市33例最多，其次為臺北市22例、桃園市2例，基隆市、南投縣及彰化縣各1例；其中32例為已知感染源、3例關聯不明、25例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增3例死亡個案，為2例男性、1例女性，年齡介於70多歲至90多歲，發病日介於5月23日至6月22日，確診日介於5月26日至6月24日，死亡日介於6月25日至6月26日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前累計1,282,057例新型冠狀病毒肺炎相關通報(含1,265,704例排除)，其中14,694例確診，分別為1,170例境外移入，13,471例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計102例移除為空號。自2020年起累計635例COVID-19死亡病例，其中627例本土，個案居住縣市分布為新北市321例、臺北市243例、基隆市21例、桃園市17例、彰化縣10例、臺中市及新竹縣各4例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月28日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-27\$\@\$中央流行疫情指揮中心今(27)日宣布，因應Delta變異株於全球日益擴散且其傳播力高，即日起若旅客自「重點高風險國家(巴西、印度、英國、祕魯、以色列、印尼及孟加拉)」入境，則請搭乘交通部安排之的防疫車輛前往集中檢疫所。若旅客並非由前述「重點高風險國家」入境，應自費搭乘防疫車輛(或自行駕車)前往防疫旅宿或自費集中檢疫所之檢疫地點。\$\@\$指揮中心強調，入境人士之親友勿前往機場或港口接機，以減少病毒傳播風險，共同保護親友及社區防疫安全。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-27\$\@\$為保障健康安全，近日民眾踴躍接種COVID-19疫苗，關於疫苗接種後是否產生副作用也有諸多討論。針對網傳COVID-19 mRNA疫苗恐傷害人體，中央流行疫情指揮中心今（27）日澄清，疫苗中的mRNA並不會進入細胞核，不會以任何方式改變人體的DNA，或與DNA產生交互作用。而政府也會嚴格把關疫苗安全，民眾可安心接種。\$\@\$指揮中心表示，我國目前已核准緊急使用授權的COVID-19疫苗分為兩大類，其中所使用的COVID-19 mRNA疫苗，其作用原理是將含有一段可轉譯成SARS-CoV-2病毒棘蛋白的mRNA注射至體內，接種後會在人體細胞質內製造出SARS-CoV-2病毒棘蛋白，作為疫苗抗原，進而誘發人體產生免疫反應，以對抗SARS-CoV-2病毒，疫苗中的mRNA不會進入細胞核、不會改變人體的DNA，或與DNA產生交互作用。\$\@\$指揮中心重申，我國核准專案輸入的mRNA疫苗，例如莫德納疫苗，是經過衛生福利部食品藥物管理署審查廠商所提供的疫苗品質管制資料、非臨床藥毒理試驗及人體臨床試驗報告，確認疫苗的品質、安全及療效後，始予以核准。\$\@\$指揮中心表示，為確保COVID-19疫苗上市後廣泛臨床使用下國人用藥安全，我國已建立COVID-19疫苗安全資訊主動監控機制，除持續監控國外衛生主管機關發布之COVID-19疫苗安全警訊外，亦設有「疫苗不良事件通報系統(VAERS)」接受各界通報，蒐集、分析及評估我國COVID-19疫苗不良事件，並藉由收集相關安全資訊，監控其安全性，一旦發現具有未知或未預期之風險，立即啟動再評估機制，重新評估其療效與風險，並確認是否需採取相關風險管控措施。\$\@\$指揮中心再次提醒， COVID-19疫苗與其他藥品一樣，或多或少都具有一些副作用，如過敏反應等，民眾接種前應主動提供自己的身體狀況，包括是否對特定藥品過敏、慢性病或正在服用的藥品；女性則需告知是否(或可能)懷孕、準備懷孕或正在哺乳母乳等，供醫師審慎評估其臨床效益及風險。接種後則應關心身體變化，部分民眾接種COVID-19疫苗後，可能會發生接種部位疼痛、紅腫、疲倦、頭痛、肌肉痠痛、體溫升高、畏寒、關節痛及噁心等，這些症狀通常輕微並且數天內消失，但如發生嚴重持續性頭痛、視力改變或癲癇、嚴重且持續腹痛超過24小時以上、皮膚出現自發性出血點、瘀青、紫斑、嚴重胸痛或呼吸困難、下肢腫脹或疼痛等，請立即就醫，並說明疫苗接種史，同時請醫師通報當地衛生局或衛生福利部疾病管制署。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-27\$\@\$中央流行疫情指揮中心今(27)日公布國內新增89例COVID-19確定病例，分別為88例本土及1例境外移入；另確診個案中新增9例死亡。\$\@\$指揮中心表示，今日新增之88例本土病例(其中27例為居家隔離期間或期滿檢驗陽性者)，為48例男性、40例女性，年齡介於未滿5歲至90多歲，發病日介於今(2021)年6月10日至6月26日。個案分佈以新北市41例最多，其次為臺北市33例、臺南市8例、桃園市3例，屏東縣、南投縣及新竹市各1例；其中60例為已知感染源、2例關聯不明、26例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增9例死亡個案，為3例男性、6例女性，年齡介於40多歲至90多歲，發病日介於5月15日至6月22日，確診日介於5月20日至6月25日，死亡日介於6月22日至6月26日；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增1例境外移入個案(案14719)，為本國籍20多歲男性，5月3日曾在奧地利當地檢出COVID-19陽性，6月11日自奧地利返臺，持有搭機前3日內檢驗陰性證明，入境後至防疫旅館檢疫，6月24日進行檢疫期滿前採檢，於今日確診。個案在臺期間並無症狀，相關接觸者匡列中。\$\@\$指揮中心統計，截至目前國內累計1,266,904例新型冠狀病毒肺炎相關通報(含1,250,863例排除)，其中14,634例確診，分別為1,170例境外移入，13,411例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計102例移除為空號。自2020年起累計632例COVID-19死亡病例，其中624例本土，個案居住縣市分布為新北市319例、臺北市243例、基隆市20例、桃園市17例、彰化縣10例、臺中市及新竹縣各4例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月27日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-26\$\@\$中央流行疫情指揮中心今(26)日表示，目前進口國內之274萬劑莫德納(Ｍoderna) COVID-19疫苗將陸續完成檢驗封緘，預計於今(2021)年7月1日起，陸續配送至地方政府衛生局及指定醫療院所，並開放第一類至第八類對象接種。第一階段預計分配各地方政府衛生局約106萬劑，分兩梯次配送，第一梯次配送約64.3萬劑，預計於7月1日陸續配達，第二梯次配送約41.8萬劑，預計７月８日陸續配達(如附件)。\$\@\$指揮中心指出，第一階段疫苗各地方政府分配數量係以下列原則核估，並將依各地方政府衛生局規劃，配送至衛生局或其指定醫療院所：\$\@\$一、各縣市第五類「居家式和社區式長照機構及身障服務照服員及服務對象」中，尚未接種疫苗之64歲以下與75歲以上服務對象及所有照服員人數總計之6成。\$\@\$二、各縣市第五類「其他機構(含矯正機關工作人員)」尚未接種人數。\$\@\$三、各縣市莫德納(Moderna)COVID-19疫苗已分配數。\$\@\$四、各縣市65-74歲長者30%人口數。\$\@\$另第二階段各地方政府分配數量則以65-74歲長者20%人口數所需疫苗數量核估，將視第一階段疫苗接種情形配發。\$\@\$指揮中心說明，有關第七類對象「維持國家安全及社會機能正常運作者」是經由各中央目的事業主管機關認定，並依據其感染風險決定為優先接種對象後進行造冊，列為首波接種之國家關鍵設施或維持設社會正常運作必要工作人員。上述對象的疫苗需求量，原則直接配送至各部會指定之COVID-19合約醫療院所，各醫療院所可視接種量能，透過原預約機制，或安排於特定時段集中接種。惟莫德納(Moderna) COVID-19疫苗於2-8℃配達後僅能保存28天，請第七類對象於預約日或接獲通知日期後，儘速前往接種，以利指揮中心視各醫療院所接種情形與庫存量，通知醫療院所逐續開放其他類對象接種，發揮COVID-19疫苗最大效益。\$\@\$指揮中心表示，第一階段配送之莫德納(Ｍoderna) COVID-19疫苗為美國提供之250萬劑其中一部分，將以2-8℃溫層配送，其包裝為每瓶14劑，10瓶一盒，接種單位可針對當日最後一瓶疫苗開瓶的剩餘劑，規劃候補名單機制，有效利用COVID-19疫苗。\$\@\$指揮中心提醒，為確保疫苗接種安全，建議先前曾因接種疫苗或任何注射治療後發生急性過敏反應的民眾，接種後請於接種處或附近留觀至少30分鐘，一般民眾則建議至少留觀15分鐘，並自我密切觀察15分鐘，以利即時處置該類急性過敏反應。\$\@\$指揮中心強調，依據各國疫苗上市後的安全性監測，曾有報告極少數年輕族群在接種mRNA 疫苗後發生心肌炎等不良反應事件，大多發生在接種後數天內，請民眾在接種mRNA 疫苗後如出現胸痛、喘或心悸等症狀，應立即就醫並說明疫苗接種史。 附件\$\@\$附件-274萬劑Moderna疫苗分配量.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-26\$\@\$中央流行疫情指揮中心今(26)日公布國內新增80例COVID-19確定病例，其中78例為本土個案(39例為居家隔離期間或期滿檢驗陽性者)；另有2例境外移入。另，確診個案中新增13例死亡。\$\@\$指揮中心表示，今日新增之78例本土病例，為36例男性、42例女性，年齡介於未滿5歲至80多歲，發病日介於今(2021)年6月11日至6月25日。個案分佈以新北市36例最多，其次為臺北市30例、桃園市、基隆市及屏東縣各3例，苗栗縣、彰化縣及新竹縣各1例。其中雙北地區以外縣市12例中，10例為已知感染源、2例關聯不明；相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增13例死亡個案，為8例男性、5例女性，年齡介於40多歲至90多歲，發病日介於5月14日至6月20日，確診日介於5月19日至6月22日，死亡日介於6月21日至6月24日，詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至6月24日累計公布13,190位確診個案中，已有9,916人解除隔離，解隔離人數達確診人數75.1%。\$\@\$指揮中心表示，今日新增2例境外移入個案中，案14591為30多歲本國籍女性，6月11日自日本返臺，持有搭機前3日內檢驗陰性證明，居家檢疫期間並無症狀，6月25日進行期滿採檢，於今日確診。案14619為本國籍30多歲女性，6月11日自菲律賓返臺，持有搭機前3日內檢驗陰性證明，居家檢疫期間並無症狀，6月25日進行期滿採檢，於今日確診。2名個案檢疫期間均無接觸他人，故無匡列接觸者。\$\@\$指揮中心統計，國內累計1,243,683例新型冠狀病毒肺炎相關通報(含1,227,748例排除)，其中14,545例確診，分別為1,169例境外移入，13,323例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；累計102例移除為空號。自2020年起累計623例COVID-19死亡病例，其中615例本土，個案居住縣市分布為新北市313例、臺北市241例、基隆市20例、桃園市17例、彰化縣9例、臺中市及新竹縣各4例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月26日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-26\$\@\$中央流行疫情指揮中心今(26)日表示，為因應6月27日起，自COVID-19變異株「重點高風險7國(巴西、印度、英國、祕魯、以色列、印尼及孟加拉)」以外之國家入境旅客(過去14天旅遊史、含轉機)住宿需要，將開放集中檢疫所供民眾自費使用，於今日晚間8時開放訂房。\$\@\$指揮中心指出，目前全臺有49處集中檢疫所，分布於北、中、南等三區，包括各類公務人員訓練中心、軍營、停招的學校宿舍、旅館等，每人每日新臺幣2,000元整，12歲以下幼童與父或母同住一室者，不另外收費。\$\@\$指揮中心說明，民眾入住之檢疫所地點須由指揮中心分派，房內皆有網路、電視等相關設備，入住民眾亦可使用自己的手機電話與外界聯繫；集中檢疫場所均有提供三餐，餐飲會於固定時間送到檢疫房間外，再由民眾自行取用至自己的檢疫房間內用餐。\$\@\$指揮中心提醒，集中檢疫所預定今日晚間8時開放訂房，有意自費入住民眾可至「入境檢疫系統」網頁預約，預約者須於航班預計抵臺48小時前至入境檢疫系統預約、繳費，以取得預約訂房識別碼，作為入境登記使用。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-25\$\@\$中央流行疫情指揮中心表示，今(25)日上午與各縣市政府召開的「全國防疫會議」，決議如下：\$\@\$一、目前全國整體疫情雖有趨緩，惟仍有零星爆發群聚事件發生，建議各地方政府仍應加強社區篩檢、疫調及接觸者追蹤管理，且加強批發市場相關人員篩檢及健康監測，避免產銷營運受影響；另鑒於全球Delta病毒變異株流行擴大，指揮中心除持續加強國內變異株監測，並請地方政府配合同步監測。\$\@\$二、因應Delta病毒變異株於全球日益擴散且其傳播力高，自6/22起，確定病例之密切接觸者及自國外入境者，無論有無症狀，於居家隔離/檢疫期滿前1日，均須進行公費PCR檢測，若隔離/檢疫期間「有症狀者」及經疫調風險評估匡列之接觸者仍須立即採檢；另經專案許可入境對象(高級中等【含】以下學校之境外生、外籍移工、搭機入境之我國籍遠洋漁船僱用外籍船員/漁工、大專校院境外生、海外青年技術訓練班新生、境外非學位生等)，由原來的檢疫期滿後隔日採檢，調整為檢疫期滿前1日採檢。\$\@\$三、疫苗接種作業說明\$\@\$1、274萬劑Moderna疫苗，第一批110萬劑預計於6/30進行配送，並於7/1開放施打。\$\@\$2、COVID-19疫苗開瓶後有一定之保存時間，最後一瓶疫苗開瓶後剩餘劑量處理方式如下：\$\@\$(1)請接種單位公告COVID-19疫苗接種作業及開放候補名單登記。\$\@\$(2)剩餘劑量使用於非現行開放類別對象，請於該等人員之接種同意書空白處進行註記「剩餘劑量使用者」，該同意書由接種單位備查，並將接種資料上傳全國性預防接種資訊系統(NIIS)。\$\@\$3、目前國內供應各廠牌之COVID-19疫苗，其使用說明書皆載明每瓶疫苗抽取之最後一劑，若劑量不足1人分劑量則須丟棄，且為保障疫苗品質，不可與其他瓶疫苗混和抽取接種。\$\@\$4、針對已接種過第1劑COVID-19疫苗者，第2劑接種規劃如下\$\@\$(1)目前已開放5/9前已接種第1劑AZ COVID-19疫苗者，陸續於間隔10~12週時公費接種第2劑。並於7/1起開放所有已接種第1劑者，接種第2劑疫苗。\$\@\$(2)為第1至3類同住者，於5/3起開放COVID-19疫苗接種至暫停提供期間，已接種過第1劑的民眾，皆可於接種後第10至12週接種第2劑。專家建議兩劑AZ COVID-19疫苗接種間隔10至12週再接種第2劑疫苗的效益更佳。\$\@\$(3)在國外接種過第1劑COVID-19疫苗，在國內欲銜接接種第2劑疫苗時，須為已開放之公費對象方可提供接種。\$\@\$四、臺北區以外醫療院所，原則同意辦理專責病房數微調作業，請經傳染病防治醫療網區指揮官同意後報送指揮中心；後續仍應維持各項感染管控作業之進行，並視疫情持續滾動監測調整病房數。另，臺北區醫療院所之專責病房數維持不變，如先前所提供之專責病房數超過10%者，可優先進行微調；急診候床數需求量多者，亦可提出申請調整，惟上述相關調整案件請經傳染病防治醫療網網區指揮官同意後報送指揮中心。\$\@\$五、有關「市場專案」，請各地方政府務必確實落實相關防疫措施；另為利處理臺北市農產運銷群聚事件，包括第一果菜批發市場及環南市場，請儘速完成市場人員PCR採檢作業，並落實相關疫調之進行，以及確實匡列確診者之接觸者，進行隔離作業，並請各地方政府協助就轄區市場從業人員曾至臺北市上開市場作業者，進行營業市場地點、營業類型、攤商編號、姓名及電話等資訊之調查，並提供臺北市政府參考。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-25\$\@\$中央流行疫情指揮中心今(25)日表示，為有效利用COVID-19疫苗，針對當日最後一瓶疫苗開瓶的剩餘劑量，可由接種單位規劃候補名單機制，建議執行方式如下：\$\@\$一、 接種單位公告COVID-19疫苗接種作業及開放候補名單登記。\$\@\$二、請接種單位建立其他18歲以上接種對象候補名單。\$\@\$指揮中心指出，當剩餘劑量使用於非現行開放類別對象時，請於該等人員之接種同意書空白處進行註記「剩餘劑量使用者」，該同意書由接種單位備查，並將接種資料上傳。另針對接種站設站、至機構/洗腎診所接種或外展接種服務作業，亦比照上述原則事先規劃候補名單。接種單位可依上述建議事先規劃，以利有效並妥善的運用疫苗資源。有關尚未開放類別的公費接種對象，詳情可至網址 ( http://at.cdc.tw/1uq4dQ )查詢。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-25\$\@\$中央流行疫情指揮中心今(25)日表示，世界衛生組織(WHO)公布目前全球已有逾85個國家出現Delta變異株(印度變異株)病例，歐洲疾控中心(ECDC)評估其傳播力較Alpha(英國變異株)高40-60%。國際間部分疫苗接種率較佳的國家包括以色列及英國等，近期病例數回升，且發現Delta變異株病例佔比達七成以上。另國內亦出現自秘魯境外移入個案檢出Delta變異株，其鄰近的孟加拉、印尼等國該變異株佔比近期亦呈增加趨勢。\$\@\$指揮中心指出，因應 Delta變異株於全球日益擴散且其傳播力高，自今(110)年6月27日零時起(抵臺時間)，全面提升入境人員檢疫措施如下：\$\@\$一、「重點高風險國家」入境旅客(過去14天旅遊史、含轉機)之檢疫措施：自空港或海港入境後一律入住集中檢疫所14天，且須配合入住時、檢疫期滿進行PCR檢測，旅客不需支付檢疫所及採檢費用。目前「重點高風險國家」為巴西(巴西變異株)、印度，含本次新增英國、秘魯、以色列、印尼及孟加拉等共7國。\$\@\$二、前述7國旅遊史以外之所有入境旅客，入境後應入住防疫旅宿或自費入住集中檢疫所14天，且於居家檢疫期滿前配合進行PCR檢測。\$\@\$三、國籍航空公司機組員，自「重點高風險國家」航線航班返臺後，應入住防疫旅宿或符合規定之公司宿舍進行居家檢疫14天，且檢疫期滿進行PCR檢測。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-25\$\@\$中央流行疫情指揮中心今(25)日公布國內新增76例COVID-19確定病例，均為本土個案；其中34例為居家隔離/檢疫期間或期滿檢驗陽性者。另，確診個案中新增5例死亡。\$\@\$指揮中心表示，今日新增之76例本土病例，為39例男性、37例女性，年齡介於未滿5歲至80多歲，發病日介於今(2021)年5月18日至6月24日。個案分佈以新北市32例最多，其次為臺北市20例、桃園市10例、新竹縣4例、苗栗縣3例、彰化縣及高雄市各2例，宜蘭縣、基隆市及臺中市各1例。其中雙北地區以外縣市24例中，13例為已知感染源、2例關聯不明、9例疫調中；相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增5例死亡個案，為3例男性、2例女性，年齡介於70多歲至90多歲，發病日介於5月16日至6月19日，確診日介於5月29日至6月20日，死亡日介於6月21日至6月23日，詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至6月23日累計公布13,061位確診個案中，已有9,650人解除隔離，解隔離人數達確診人數73.9%。\$\@\$指揮中心統計，截至目前國內累計1,213,717例新型冠狀病毒肺炎相關通報(含1,197,732例排除)，其中14,465例確診，分別為1,167例境外移入，13,245例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計102例移除為空號。自2020年起累計610例COVID-19死亡病例，其中602例本土，個案居住縣市分布為新北市306例、臺北市238例、基隆市19例、桃園市16例、彰化縣9例、臺中市4例、新竹縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月25日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-24\$\@\$中央流行疫情指揮中心今(24)日表示，「民眾使用COVID-19家用快篩試劑指引」已於6月19日公布(詳如新聞稿附件)。為利民眾居家正確自行檢測，指揮中心再次提醒民眾使用家用快篩試劑相關流程與注意事項。\$\@\$指揮中心指出，COVID-19家用快篩試劑可由醫療器材販賣業者、藥粧店、醫療器材行、便利商店等或藥局販售，民眾購買時，請確認產品名稱是否有「家用」、包裝是否刊載「防疫專案核准製造第XXXXXXXXXX號」或「防疫專案核准輸入第XXXXXXXXXX號」等字樣(已核准之家用快篩試劑名單可至衛生福利部食品藥物管理署[下稱食藥署]網站確認)、產品效期是否在有效期間或保存期限內，並依使用說明書或操作影片進行採檢及操作。對使用家用快篩試劑有任何疑問，可洽詢販售該產品之醫療器材商或藥局，或逕洽詢試劑廠商。\$\@\$指揮中心說明，居家隔離或居家檢疫者如測出結果為陽性時，請立即與當地衛生局聯繫，或撥打1922，依指示方式處理；非居家隔離且非居家檢疫者測出結果為陽性時，請戴好口罩，勿搭乘大眾運輸工具，儘速至鄰近的社區採檢院所進一步檢測，並將使用過之採檢器材用塑膠袋密封包好，一併攜帶至社區採檢院所，交予院所人員。當測出結果為陰性時，仍請遵循指揮中心的防疫規範，做好個人防護，持續自我健康管理，採檢完之家用快篩試劑及試劑棒勿任意棄置，請以塑膠袋密封包好，以一般垃圾處理。\$\@\$指揮中心提醒，若民眾已出現嚴重特殊傳染性肺炎相關症狀，不宜使用COVID-19家用快篩試劑自行在家檢測，應佩戴醫用口罩，儘速前往醫療院所就醫，且前往就醫時勿搭乘大眾運輸工具。另外，提醒居家快篩試劑測試結果可能出現偽陰性或偽陽性，仍需經認可實驗室所進行的「核酸檢測」作為診斷COVID-19感染之依據。COVID-19家用快篩試劑產品核准名單、說明書及操作影片均可至食藥署網站( http://www.fda.gov.tw )之業務專區 &gt; 醫療器材 &gt; COVID-19 防疫醫材專區 &gt; 家用新型冠狀病毒檢驗試劑專區查詢。 附件\$\@\$附件-民眾使用COVID-19家用快篩試劑檢驗指引.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-23\$\@\$中央流行疫情指揮中心今(23)日表示，國內疫情由於國人的努力，得到良好控制，惟目前跨區傳播事件仍然存在，而世界各國因解封太快致疫情再起的經驗亦歷歷在目。為確保國人健康，指揮中心經評估後決定，全國再同步維持疫情三級警戒2週(至7月12日止)，用2週的時間換得國人平安，希望國人共體時艱，共同抗疫。\$\@\$指揮中心指出，考量社區感染風險尚未消除，指揮中心將持續與地方政府密切合作，加強落實以下管制措施，降低社區傳播風險，積極保障國人健康安全：\$\@\$一、針對確診個案精準疫調，儘速匡列相關接觸者並加強追蹤管理，及早阻斷病毒傳播鏈。\$\@\$二、針對居家檢疫及居家隔離者，無論有無症狀，均須於期滿前1日進行公費PCR檢測，以阻絕病毒進入社區。\$\@\$三、加速高風險族群疫苗接種作業，以減少其感染、或感染後產生嚴重併發症及死亡的機率。\$\@\$四、推動社區廣篩，鼓勵各地方政府設置社區篩檢站並加速檢驗時效，同時推廣企業快篩與居家快篩，以擴大篩檢量能並強化主動監測機制，儘速發掘社區內可能潛藏病例，有效斷絕所有感染鏈。\$\@\$五、強化重症醫療照護，透過COVID-19重症個案處置諮詢平臺，由多位專家諮詢委員線上提供醫院臨床重症個案處置意見，以降低個案死亡率、緩解重症醫療量能。\$\@\$六、啟動「民生供需產業健康監測專案」，針對果菜、家畜(肉品)、家禽、水產、綜合及其他類市場、超市、賣場及夜市等相關職業對象，由目的事業主管機關或地方政府進行人員健康監測，以及時進行各項防治措施，避免災害擴大，降低家戶傳播風險。\$\@\$指揮中心表示，現處疫情關鍵時刻，籲請全國民眾持續落實遵循並積極配合三級警戒管制措施，與政府共同努力，嚴守社區防線。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-22\$\@\$中央流行疫情指揮中心今(22)日公布國內新增79例COVID-19確定病例，其中78例為本土個案，另有1例境外移入；另確診個案中新增6例死亡。\$\@\$指揮中心表示，今日新增之78例本土病例，為35例男性、43例女性，年齡介於未滿5歲至90多歲，發病日介於今(2021)年6月14日至6月21日。個案分佈以新北市43例最多，其次為臺北市25例，南投縣3例，基隆市2例，苗栗縣、彰化縣、桃園市、臺中市及新竹縣各1例。其中雙北地區以外縣市10例中，8例為已知感染源，2例關聯不明；相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增6例死亡個案，為男性3位、女性3位，年齡介於50多歲至80多歲，發病日介於5月19日至6月19日，確診日介於5月28日至6月21日，死亡日介於6月17日至6月21日，詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至6月20日累計公布12,806位確診個案中，已有8,087人解除隔離，解隔離人數達確診人數63.2%。\$\@\$指揮中心表示，今日新增1例境外移入個案（案14257）為本國籍50多歲男性，長期於印尼工作，6月20日返臺，持有搭機前3日內檢驗陰性報告，入境後至防疫旅館居家檢疫，6月21日出現喉嚨痛等症狀，由衛生單位安排就醫採檢，於今日確診。個案檢疫期間無接觸他人，故無匡列接觸者。\$\@\$指揮中心統計，截至目前國內累計1,107,543例新型冠狀病毒肺炎相關通報(含1,091,972例排除)，其中14,157例確診，分別為1,166例境外移入，12,938例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；新增2例空號 (案10380、案14131)，累計100例移除為空號；自2020年起累計575例COVID-19死亡病例，其中568例本土，個案居住縣市分布為新北市291例、臺北市223例、基隆市18例、桃園市15例、彰化縣9例、臺中市4例、宜蘭縣及新竹縣各2例，臺東縣、雲林縣、高雄市及花蓮市各1例；另7例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月22日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-20\$\@\$中央流行疫情指揮中心今(20)日表示，為保障國人接種COVID-19疫苗權益，指揮中心持續監測疫苗接種後不良事件，截至今(2021)年6月19日止，國內接種AZ COVID-19疫苗共計1,446,608人次，其中314,487人次為75歲以上長者。目前疫苗不良事件通報系統(VAERS)已收到67例接種AZ COVID-19疫苗後死亡之報告。截至目前為止，尚無死亡個案被判定為與疫苗相關。\$\@\$指揮中心指出，昨(19)日接種後死亡案件新增18件，皆於接種後4日內發生，15例為75歲以上長者，死亡個案大多數為高齡且有慢性疾病。此外，目前已有9例死亡案件送司法相驗解剖，經初步研判，部分個案死因與心血管疾病(包括粥狀動脈硬化、主動脈瘤破裂及心肌梗塞等)或慢性病史(如支氣管性肺炎)相關。截至目前為止，死亡個案雖在時序上與疫苗接種相近，但尚無死亡個案被判定為與疫苗相關，後續仍待司法相驗解剖或回溯檢查等更精確資料，以釐清死因。指揮中心將持續監測疫苗接種後不良事件，偵測安全疑慮，並適時對外因應。\$\@\$指揮中心提醒，對於近期身體具狀況或慢性病情不穩定者，請於身體狀況較穩定後再安排接種。近期天氣炎熱，考量長者身體狀況，也建議避開高溫時段前往接種。另外，現在已開放診所及衛生所可接種疫苗，建議民眾就近前往接種，並注意防曬、補充水分。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-18\$\@\$中央流行疫情指揮中心今(18)日宣布，因應國內近期本土COVID-19確診病例疫情嚴峻，為利醫療院所照護重症個案、降低死亡率，將成立「COVID-19重症個案臨床處置專家諮詢小組」，由臺大醫院新竹臺大分院余忠仁院長擔任召集人，邀集全國22位重症個案臨床處置專家擔任諮詢委員，建立COVID-19重症個案處置諮詢平臺，並自6月21日(星期一)起，定期於星期一至星期五，每日晚間6時至8時，召開COVID-19線上重症病例諮詢會議，每日由3至5位諮詢委員，提供各醫療院所臨床重症個案處置意見，預定每次會議時間約為2小時。\$\@\$指揮中心表示，前已函請地方政府衛生局與相關學會轉知所屬醫療院所及會員，若醫療院所於診治COVID-19個案，有相關重症個案臨床處置諮詢需求，請於會議當日中午12時前，以電子郵件提交討論病例簡報、報告人姓名與聯繫資料至指揮中心醫療應變組公務信箱，以利會議討論。\$\@\$指揮中心說明，為降低重症個案死亡率，將「經鼻高流量濕化氧氣治療(Humidified high flow nasal cannula oxygen therapy, HFNCOT）」及「俯臥通氣治療(Prone positioning ventilation therapy)」，納入COVID-19確診個案公費給付項目，並回溯自5月1日起適用。\$\@\$指揮中心呼籲重症照護是團隊作戰，面對COVID-19疫情，重症照護團隊需照顧好自己及隊友，若有相關重症個案臨床處置諮詢需求，務必儘速提請討論，共同強化重症病人照護，保障病人安全。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-18\$\@\$中央流行疫情指揮中心今(18)日表示，第二批Moderna疫苗24萬劑，已於歐洲時間6月17日下午6時自盧森堡啟運，預定今日下午3時50分抵達桃園國際機場。本批疫苗為供應商承諾供應之一部分，待完成通關程序後，直接運送至指定冷儲物流中心進行後續檢驗封緘作業，再提供COVID-19接種計畫所列實施對象進行接種。\$\@\$指揮中心指出，該中心已於今(2021)年2月8日與美國Moderna公司簽署505萬劑COVID-19疫苗供應合約。該疫苗為多劑型包裝(每瓶10人份)，存放於-20℃可保存6個月，於2-8℃之使用期限為30天，依臨床試驗結果，每人需施打2劑，2劑間隔28天以上，疫苗保護效力可達94%。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-18\$\@\$中央流行疫情指揮中心今(18)日公布國內新增188例COVID-19確定病例，分別為187例本土個案及1例境外移入；確診個案中新增21例死亡。\$\@\$指揮中心表示，今日新增之187例本土病例，為83例男性、104例女性，年齡介於未滿5歲至90多歲，發病日介於今(2021)年5月29日至6月17日。個案分佈以新北市76例最多，其次為臺北市71例，苗栗縣26例，桃園市6例，基隆市4例，臺中市2例，花蓮縣及新竹縣各1例。其中雙北地區以外縣市40例中，38例為已知感染源、2例關聯不明；相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增21例死亡個案，為男性12位、女性9位，年齡介於50多歲至90多歲，發病日介於5月6日至6月13日，確診日介於5月19日至6月15日，死亡日介於6月10日至6月16日，詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至6月16日累計公布12,210位確診個案中，已有6,873人解除隔離，解隔離人數達確診人數56.3%。\$\@\$指揮中心指出，今日新增1例境外移入個案(案13801)，為印度籍30多歲男性船員，3月5日自印度來臺工作，4月3日登船出海工作，期間並無症狀，6月16日返回我國港口，因出境需要，於同日採檢，並於今日確診；個案在臺期間並無症狀，相關接觸者匡列中。\$\@\$指揮中心統計，截至目前國內累計1,011,097例新型冠狀病毒肺炎相關通報(含993,010例排除)，其中13,771例確診，分別為1,162例境外移入，12,556例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另新增1例空號(案13408)，累計95例移除為空號。自2020年起累計518例COVID-19死亡病例，其中511例本土，個案居住縣市分布為新北市255例、臺北市206例、基隆市17例、桃園市14例、彰化縣8例、臺中市4例、宜蘭縣及新竹縣各2例，臺東縣、雲林縣及高雄市各1例；另7例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月18日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-15\$\@\$中央流行疫情指揮中心今(15)日表示，為提升目前優先接種COVID-19疫苗對象之接種率，將於6月17日起，依各縣市75歲以上人口比率，進行第二次疫苗撥配，預計配送394,800劑。\$\@\$指揮中心說明，自6月12日起，已陸續撥配68.8萬劑(含高風險縣市及中高風險縣市額外撥配2.49萬劑)至各地方政府衛生局，提供第一類至第六類優先對象(包括「第一類至第三類尚未接種第一劑疫苗者」、「住宿式長照機構工作人員及住民」、「洗腎患者」及「75歲以上長者」)接種。為提升前揭對象接種率，本次疫苗配送量是以各縣市75歲以上長者人口數之26%核估，同時考量疫情風險程度，高風險縣市（臺北市、新北市）增配10%，中高風險縣市（桃園市、臺中市、基隆市、苗栗縣及彰化縣）增配5%，合計配送 385,800劑。加上前次疫苗撥配量，預估可讓全臺75歲以上長者接種率至少達53%。\$\@\$指揮中心指出，另考量部分縣市及離島縣市交通不便、疫苗配送不易且醫療資源相較不足，指揮中心規劃「離島-偏遠地區擴大接種計畫」，額外撥補臺東縣、屏東縣、澎湖縣、金門縣及連江縣共9,000劑疫苗，提供縣市依轄內接種需求規劃疫苗接種作業，其中連江縣撥配量將提前於6月16日配送。\$\@\$指揮中心特別提醒，為確保疫苗接種安全，建議先前曾因接種疫苗或任何注射治療後發生急性過敏反應之民眾，接種後請於接種處或附近留觀至少30分鐘，一般民眾則建議至少留觀15分鐘，並自我密切觀察15分鐘，以利即時處置該類急性過敏反應。接種AstraZeneca COVID-19疫苗後28天內，若出現嚴重持續性頭痛、視力改變、癲癇、嚴重且持續腹痛超過24小時以上、嚴重胸痛或呼吸困難、下肢腫脹或疼痛、皮膚出現自發性出血點、瘀青、紫斑等任一症狀，應儘速就醫，並告知疫苗接種史，以利醫師及早釐清病因，並給予適當臨床處置。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-15\$\@\$中央流行疫情指揮中心今(15)日表示，為儘速發掘社區內可能潛藏病例，並有效斷絕所有感染鏈，該中心已於10日公布「社區廣篩4大策略」；今日並宣布，將補助各地方社區篩檢站50臺PCR檢驗儀器，居家自採與企業快篩陽性民眾，將可就近至社區第一線進行快速PCR檢驗。\$\@\$指揮中心指出，在廣設社區篩檢站方面，截至6月13日止，全國各地已開設249社區篩檢站，為加速社區第一線檢驗量能篩檢，今日宣布將補助各地方社區篩檢站50臺PCR檢驗儀器，未來居家自採與企業快篩民眾，若快篩結果呈現陽性，可就近至有快速PCR檢驗的社區篩檢站進行檢驗，並依照PCR檢驗結果及有無症狀進行後續措施(如附表)，形成全國社區防疫網。\$\@\$指揮中心表示，目前持續鼓勵各地方政府設置社區篩檢站，並以「區域個案數」、「確診者足跡熱區」等盛行率較高的地區為考量，針對具有確診個案相關接觸史、活動史的無症狀民眾為主要篩檢對象。另為保全重度級急救責任醫院收治量能，請考量於社區健康中心、其他非重度級急救責任醫院及通風良好的場所，設置社區篩檢站。相關設置規定，可參考指揮中心訂頒的「各地方政府社區篩檢站設置指引」辦理。\$\@\$指揮中心再次提醒，所有篩檢工具皆有偽陰性、偽陽性的可能，檢驗陰性民眾仍應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施。 圖片 附件\$\@\$0615 COVID-19廣篩策略.jpg</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-15\$\@\$中央流行疫情指揮中心表示，今(15)日上午與各縣市政府召開的「全國防疫會議」，決議如下：\$\@\$一、目前全國推動加強三級警戒等管制措施，雙北疫情雖逐步趨緩，但指揮中心仍請雙北以外的部分縣市，密切注意疫情發展，須持續強化基層醫療檢驗及社區篩檢及病例監測之能力，針對弱勢族群及獨居老人更應提高注意，並加強疫調與接觸者管理及早發現個案，以防疫情反彈或出現新一波流行。\$\@\$二、有關疫苗配發及接種作業：\$\@\$(一)指揮中心再次向各地方政府說明，前一批COVAX分配之40.98萬劑及本次日本政府提供之124萬劑AZ疫苗，均以疫情狀況、疫苗可分配數量、接種情形等綜合評估後，訂定分配數計算基礎之公式，對各地方政府依比例公平、公開透明分配，指揮中心也會根據各地方政府之疫情及後續接種情形等狀況分析，滾動檢討並加強配送作業。\$\@\$(二)有關指揮中心已公布之目標接種族群，其疫苗施打不受戶籍地限制，請地方政府依序完成民眾預約接種作業；另地方政府建請指揮中心就目前開放施打對象重新評估研議部分，鑒於疫苗量有限，仍請各地方政府依造冊對象及接種計畫審慎作業，有關第七類施打對象部分，指揮中心正與相關機關進行盤點，也會參考地方政府建議，依實際狀況完備造冊作業。\$\@\$三、有關地方政府擬進行到宅接種作業，指揮中心尊重地方政府相關作業，惟請留意疫苗保存條件：須保存在2-8℃、開瓶後要在6小時內施打，避免晃動等。另應預先安排10人次進行施打，以利疫苗接種效率。\$\@\$四、針對出國留學之學生能否先予納入公費疫苗接種對象，鑒於國內疫苗供應需求，目前仍以臺灣社區防疫為主，暫不將上類人員納入公費施打對象。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-14\$\@\$國際疫情持續嚴峻且變化快速，為確保國籍航空機組員職場健康及維護國內防疫安全，關於國籍航空公司機組員接種COVID-19疫苗後之檢疫措施，於交通主管機關監督航空公司落實外站「零接觸」管理、機組員「機上全程防護」及返國檢疫措施下，調整說明如下：\$\@\$一、重點高風險國家航線航班之返臺機組員，居家檢疫14天(結束日PCR檢驗)。\$\@\$二、長程航班(入境旅遊疫情第三級地區)：\$\@\$1. 尚未接種疫苗及接種1劑疫苗未達兩週者：110/6/12起，採5天居家檢疫(結束日PCR檢驗)+9天加強版自主健康管理(第9、14天抗原快篩)。7/1起，採7天居家檢疫(結束日PCR檢驗)+7天加強版自主健康管理(第14天抗原快篩)。\$\@\$2. 接種1劑疫苗且滿兩週，但尚未具完整疫苗保護力：110/6/12起，採3天居家檢疫(結束日PCR檢驗)+11天自主健康管理(第9、14天抗原快篩)。7/1起，採5天居家檢疫(結束日PCR檢驗)+9加強版天自主健康管理(第9、14天抗原快篩)。\$\@\$3. 完整接種2劑疫苗達兩週且抗體檢測陽性(每3個月監測)：採7天自主健康管理(結束日PCR陰性)。\$\@\$三、短程航班(當班往返且未入境旅遊疫情第三級地區)：110/6/12起，\$\@\$1. 未完整接種疫苗達兩週及抗體檢測陰性者：採14天自主健康管理+每14天PCR監測。\$\@\$2. 完整接種疫苗滿兩週且抗體檢測陽性者(每3個月抗體監測)：自我健康監測+每14天PCR監測\$\@\$指揮中心表示，自疫情以來，機組員肩負疫苗及輸送物資進出口，以維持空運貨物運能，對機組員的付出表示感謝。目前國籍航空機組員多數已接種第1劑疫苗，後續將保留其第2劑疫苗，確保其能獲得疫苗保護力。指揮中心特別提醒，因病毒株變異及傳播力難以預測，具疫苗保護力的機組員於執勤時，仍應遵守民用航空局訂定之作業規範，於外站「零接觸當地人」、機上全程防護及加強手部衛生清消頻率等，以維護個人及家人防疫安全。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-14\$\@\$中央流行疫情指揮中心今(14)日公布國內新增185例COVID-19確定病例，均為本土個案；另確診個案中新增15例死亡。\$\@\$指揮中心表示，今日新增之185例本土病例，為83例男性、102例女性，年齡介於未滿5歲至90多歲，發病日介於今(2021)年5月28日至6月13日。個案分佈以新北市98例最多，其次為臺北市42例，基隆市14例，桃園市10例，苗栗縣7例，花蓮縣4例，彰化縣及新竹縣各3例，宜蘭縣2例，臺中市及雲林縣各1例。其中雙北地區以外縣市45例中，37例為已知感染源、5例關聯不明、3例調查中；相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增15例死亡個案，共計為男性9位、女性6位，年齡介於50多歲至90多歲，發病日介於5月10日至6月8日，確診日介於5月18日至6月13日，死亡日介於6月5日至6月13日，詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至6月12日累計公布11,547位確診個案中，已有5,802人解除隔離，解隔離人數達確診人數50.2%。\$\@\$指揮中心統計，截至目前國內累計886,014例新型冠狀病毒肺炎相關通報(含863,703例排除)，其中13,106例確診，分別為1,155例境外移入，11,898例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中，另累計92例移除為空號。確診個案中452例死亡。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月14日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-13\$\@\$中央流行疫情指揮中心今(13)日表示，有關網傳總統、副總統已接種COVID-19疫苗，經總統及副總統授權由中央流行疫情指揮中心調閱「全國性預防接種資訊管理系統(NIIS)」系統查證，蔡英文總統及賴清德副總統均尚未接種COVID-19疫苗。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-13\$\@\$中央流行疫情指揮中心今(13)日公布國內新增175例COVID-19確定病例，分別為174例本土及1例境外移入；另確診個案中新增26例死亡。\$\@\$指揮中心表示，今日新增之174例本土病例，為79例男性、95例女性，年齡介於未滿5歲至90多歲，發病日介於今(2021)年5月23日至6月12日。個案分佈以新北市81例最多，其次為臺北市62例，桃園市16例，基隆市7例，彰化縣4例，新竹縣2例，臺中市及花蓮縣各1例。其中雙北地區以外縣市31例中，20例為已知感染源、7例關聯不明、4例調查中；相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增26例死亡個案，共計為男性15位、女性11位，年齡介於50多歲至90多歲，發病日介於5月6日至6月10日，確診日介於5月15日至6月12日，死亡日介於6月4日至6月12日，詳如新聞稿附件。\$\@\$指揮中心指出，今日新增1例境外移入個案(案12924)，為本國籍20多歲男性，4月曾在美國當地檢出COVID-19陽性，5月17日自美國返臺，持有搭機前3日內檢驗陰性報告，入境後至防疫旅館進行居家檢疫，6月11日自費採檢，於今日確診；個案在臺期間並無症狀，已匡列接觸者1人，列居家隔離。\$\@\$指揮中心統計，累計869,247例新型冠狀病毒肺炎相關通報(含846,797例排除)，其中12,921例確診，分別為1,155例境外移入，11,713例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中，另累計92例移除為空號。確診個案中437例死亡。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月13日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-12\$\@\$中央流行疫情指揮中心今(12)日表示，有關日本提供之124萬劑AZ疫苗，已於6月9日發布之新聞稿說明：預計自6月12日起，分階段陸續配送至各地方政府衛生局或指定醫療院所；而各地方政府分配數計算基礎如下（分配表如附件）：\$\@\$1、第一至三類未接種人數的六成。\$\@\$2、長照機構未接種人數的六成（離島加權至八成以上）。\$\@\$3、75歲以上人數的27%（離島加權至九成以上）。\$\@\$4、洗腎患者人數之全數。\$\@\$1至4項合計數扣除已配送莫德納疫苗數，即為各地方政府獲配疫苗數量。\$\@\$指揮中心重申，每批次疫苗配送各地方政府，是以疫情狀況、疫苗數量、接種情形等綜合評估後，訂定分配數計算基礎之公式，對各縣市依比例公平分配，指揮中心也會根據各自縣市之疫情及後續接種情形等狀況分析，滾動檢討並加強配送作業，全力協助地方政府推動疫苗接種作業。 附件\$\@\$附件-1100612-日本提供之124萬劑AZ疫苗各地方政府第一次配送分配表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-12\$\@\$中央流行疫情指揮中心今(12)日表示，首批莫德納（Moderna）疫苗15萬劑中，7.5萬劑已於6月9日配送提供全國COVID-19專責醫療院所(包括設置專責病房或負壓隔離病房或採檢院所)，以提供尚未接種COVID-19疫苗的第一線照顧病患醫事及非醫事人員接種服務，截至昨(11)日累計接種2萬4,869人。\$\@\$指揮中心指出，為使疫苗資源有效運用，並加速接種作業，自今日起同時開放所有第一類對象包含醫院、診所及其他醫事機構等執業登記醫事人員、非醫事工作人員，以及集中檢疫所非醫事人員接種莫德納疫苗。\$\@\$指揮中心表示，依據目前研究顯示，接種兩劑不同技術產製的COVID-19疫苗，第二劑接種後發生不良反應機率及嚴重程度較高，故不建議交替使用，惟若接種第一劑COVID-19疫苗發生嚴重過敏反應或產生任何(含對疫苗成分)嚴重的立即過敏或不良反應，並經通報疫苗不良事件通報系統(VAERS)判定為嚴重反應者，建議經醫師評估後接種不同技術產製的 COVID-19 疫苗，完成後續劑次。\$\@\$指揮中心進一步表示，另依美國疾病管制及預防中心近期針對COVID-19疫苗接種不良反應事件監測發現：「曾有報告極少數年輕族群在接種mRNA疫苗後發生心肌炎的不良反應事件，大多發生在接種後數天內」。由於莫德納COVID-19疫苗屬於mRNA疫苗的一種，因此會在接種意願書上加上下列說明「接種mRNA疫苗後應注意若有發生胸痛、喘或心悸等症狀，請立即就醫並說明疫苗接種史」。接種單位或地方政府衛生局如接獲相關不良反應事件通報，亦請依循相關作業進行通報，以利及時掌握。\$\@\$指揮中心指出，為利接種作業推動及維持社交距離避免群聚，COVID-19疫苗接種後調整留觀時間為15分鐘，自我密切觀察15分鐘；但針對先前曾經因接種疫苗或任何注射治療後發生急性過敏反應之民眾，接種後仍請於接種處或附近留觀至少30分鐘。倘持續發燒超過 48 小時、嚴重過敏反應如呼吸困難、氣喘、眩暈、心跳加速、全身紅疹等不適症狀，亦應儘速就醫，並說明疫苗接種史，以利醫師及早釐清病因，並給予適當臨床處置。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-12\$\@\$中央流行疫情指揮中心今(12)日公布國內新增251例COVID-19確定病例，分別為250例本土及1例境外移入；另確診個案中新增26例死亡。\$\@\$指揮中心表示，今日新增之250例本土病例，為116例男性、134例女性，年齡介於未滿5歲至100多歲，發病日介於今(2021)年5月28日至6月11日。個案分佈以新北市133例最多，其次為臺北市65例，基隆市16例，桃園市13例，苗栗縣9例，花蓮縣3例，宜蘭縣、新竹市、彰化縣及臺中市各2例，高雄市、雲林縣、新竹縣各1例。其中雙北地區以外縣市52例中，45例為已知感染源，7例關聯不明。相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增26例死亡個案，共計為男性16位、女性10位，年齡介於40多歲至100多歲，發病日介於5月15日至6月9日，確診日介於5月18日至6月11日，死亡日介於6月4日至6月11日，詳如新聞稿附件。\$\@\$指揮中心指出，今日新增1例境外移入個案(案12698)，為本國籍40多歲女性，5月30日自中國返臺，持有搭機前3日內檢驗陰性報告，入境後至檢疫旅館進行居家檢疫，於6月9日出現發燒等症狀，6月10日由衛生單位安排採檢送驗，於今日確診。\$\@\$指揮中心統計，累計845,113例新型冠狀病毒肺炎相關通報(含821,956例排除)，其中12,746例確診，分別為1,154例境外移入，11,539例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另新增5例空號 (案9332、10323、10337、10353、12078)，累計92例移除為空號。確診個案中411例死亡。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月12日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-11\$\@\$中央流行疫情指揮中心表示，今(11)日下午由行政院秘書長李孟諺、指揮中心社區防疫組組長薛瑞元與各縣市政府衛生局召開「COVID-19疫苗接種作業推行協調會」，針對不同年齡與族群的疫苗接種策略，進行相關經驗交流與分享；會議重點如下：\$\@\$請地方衛生機關每日確實將接種名冊上傳，以利及時掌握接種進度及疫苗撥配相關事宜。\$\@\$日本政府提供我國的124萬劑AstraZeneca疫苗，開放75歲以上長者(含65歲以上具原住民身分者)施打，只要為民國35年12月31日(含)以前出生者，或具原住民身分之證明文件且為民國45年12月31日(含)以前出生者，均符合接種資格。同時，75歲以上長者，不限其居住地或戶籍地，均可就近完成接種作業。\$\@\$各地方政府的疫苗接種策略不同，大部分縣市採預先造冊、由民政單位通知方式辦理，另有部分縣市採用院所預約方式，惟請採預約方式之縣市，宜加速擴充電話線路及服務人力，使施打作業更為順暢。\$\@\$另，指揮中心提醒，目前第一類尚未完成接種COVID-19疫苗較多之縣市，請加速疫苗接種作業，使民眾儘早獲得疫苗保護力。\$\@\$為避免人潮擁擠，請各地方政府以分齡、分流、分批辦理，減少群聚風險。\$\@\$另，由於食品藥物管理署加速完成該批COVID-19疫苗檢驗封緘作業，以及物流業者鼎力協助提前於今日深夜開始配送，明(12)日將有50萬劑陸續運抵各地方政府，考量地方政府需前置作業時間，指揮中心表示，疫苗開打日仍以 6月15日為原則辦理。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-11\$\@\$中央流行疫情指揮中心表示，今(11)日上午與各縣市政府召開的「全國防疫會議」，決議如下：\$\@\$一、雙北疫情趨勢雖持平惟仍舊嚴峻，指揮中心持續鼓勵各縣市增設社區篩檢站，以便及早發掘潛在陽性個案，阻斷社區傳播鏈；另鑒於重症及死亡數攀升對社會之衝擊與影響較大，也請各地方政府持續掌握及協調醫療資源，迅速應變。\$\@\$二、針對疫苗配撥及施打作業：\$\@\$(一)指揮中心再次強調，中央與地方應秉持「標準一致、做法一致、腳步一致」防疫原則，請各地方政府及醫療院所依據指揮中心所訂「COVID-19疫苗接種順序」，進行施打作業。\$\@\$(二)有關各地方政府關切疫苗配撥量部分，指揮中心會儘速完成第一類至第六類符合施打對象之計算，並加速進行疫苗撥發作業。另鑒於現行國內疫苗量仍無法全數完成上開類別人員之施打，亦請各地方政府審慎妥予規劃相關施打作業之進行。\$\@\$(三)請地方衛生機關加強向合約醫療院所宣導，針對符合接種順序者，應讓其以最方便之方式就近完成接種作業，不侷限接種者居住地、工作地或戶籍地區分，避免造成人流移動情形；另有關疫苗施打類別，針對公費疫苗接種第七類有關維持國家安全及社會機能正常運作者之匡列部分，指揮中心將會再進一步研議，俾符實際運作狀況。\$\@\$三、衛生福利部醫事司與內政部消防署已協調民間18家救護車業者，自今日起投入防疫救護載運工作，將進行醫院、集中檢疫場所間，點到點之病患運送作業，預計至少有108部民間救護車加入防疫工作，以有效舒緩消防機關救護工作之壓力。\$\@\$四、請各地方政府鼓勵觀光飯店業者發動「暖心方案」，提供醫護人員以及相關醫事人員入住，讓第一線醫事人員可以獲得充分及妥適休息。\$\@\$五、鑒於暑假將屆，有關大專院校學生暑期生活管理作業，教育部前於5月26日及6月8日2度要求各級學校，應強化住宿生管理，並不得強制要求住宿學生返家。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-11\$\@\$中央流行疫情指揮中心今(11)日表示，指揮中心已採購複合單株抗體藥物，將提供具有重症風險因子之輕中度確診個案治療使用，以降低個案轉為重症需住院之風險，協助紓解重症醫療量能。\$\@\$指揮中心指出，依據國際研究顯示，新冠病毒感染患者輕症比率大約佔8成左右，但其中約9％的患者可能惡化為重症，主要的重症危險因子有高齡、肥胖、慢性腎病、心血管疾病/高血壓、慢性肺病、免疫抑制疾病/免疫抑制治療等影響免疫功能之疾病，以及懷孕等，且其病程演化迅速，甚至導致死亡。截至本(110)年6月10日監測資料，國內輕中度COVID-19確診病例約佔所有確診個案84%，死亡病例數佔確診病例2.7%。\$\@\$指揮中心表示，國內新冠肺炎(COVID-19)疫情持續嚴峻，重症醫療量能持續緊繃，鑒於單株抗體之療效及安全性已有部分證據支持，美國FDA及國際間已陸續發布緊急使用授權(EUA)核准於臨床使用，以治療輕度至中度SARS-CoV-2感染且有重症危險因子之高風險患者，降低個案轉為重症需住院之風險。指揮中心經諮詢專家，已將該藥物之使用建議納入我國新型冠狀病毒(SARS-CoV-2)感染臨床處置暫行指引，並著手採購儲備該藥物，規劃分配於集中檢疫場所之主責醫院，經醫師評估治療效益與風險，並充分告知後，給予符合條件個案注射治療。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-11\$\@\$中央流行疫情指揮中心今(11)日公布國內新增287例COVID-19確定病例，分別為286例本土及1例境外移入；另確診個案中新增24例死亡。\$\@\$指揮中心表示，今日新增之286例本土病例，為141例男性、145例女性，年齡介於未滿5歲至90多歲，發病日介於今(2021)年5月19日至6月10日。個案分佈以新北市120例最多，其次為苗栗縣56例、臺北市49例、桃園市19例、新竹縣12例、基隆市8例、彰化縣7例、臺中市4例、宜蘭縣及新竹市各3例、雲林縣及花蓮縣各2例、臺南市1例。其中雙北地區以外縣市117例中，109例為已知感染源，8例關聯不明。相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增24例死亡個案，共計為男性12位、女性12位，年齡介於50多歲至80多歲，發病日介於5月3日至6月8日，確診日介於5月15日至6月10日，死亡日介於6月2日至6月9日，詳如新聞稿附件。\$\@\$指揮中心指出，今日新增1例境外移入個案(案12479)，為泰國籍30多歲男性移工，2月7日曾在泰國當地檢出COVID-19陽性，3月23日自泰國來臺工作，持有搭機前3日內檢驗陰性報告，4月7日檢疫期滿採檢結果為陰性，6月8日出現發燒及咳嗽症狀，6月10日就醫採檢，於今日確診(Ct值31，次日再驗核酸檢測陰性，血清抗體陽性)；已匡列個案接觸者13人，皆列為居家隔離。\$\@\$指揮中心統計，累計804,931例新型冠狀病毒肺炎相關通報(含781,334例排除)，其中12,500例確診，分別為1,153例境外移入，11,294例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另新增9例空號 (案6616、9671、10339、10348、10350、10359、10452、11381、11865)，累計87例移除為空號。確診個案中385例死亡。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$6月11日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-11\$\@\$中央流行疫情指揮中心今(11)日表示，鑑於國內COVID-19疫情仍未穩定，為避免增加我國檢疫量能及醫療資源的負擔，全國疫情警戒第三級期間，將持續執行「邊境嚴管」措施。\$\@\$邊境嚴管措施，包括(一)未持有我國有效居留證之非本國籍人士，暫緩入境。緊急或人道考量等經專案許可者除外；(二)暫停旅客來臺轉機。指揮中心亦將視國內外疫情及社區防疫執行狀況，適時滾動調整。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-10\$\@\$中央流行疫情指揮中心今(10)日表示，鑒於近日國內疫情嚴峻，我國共計6家企業及民間單位（萬海航運、元大金控集團、臺灣證券交易所/臺灣期貨交易所/臺灣集中保管結算所/中華民國證券櫃檯買賣中心、光合基金會/大肚山產業創新基金會、富邦金控、急診醫學會）集資共同捐贈日本日立公司所生產之「負壓隔離艙」80座，將由衛生福利部轉交各急救責任醫院使用，盼能協助解決為各大急救責任醫院負壓隔離病房不足的問題，提供解決方案。\$\@\$指揮中心說明，經指揮中心醫療應變組王必勝副組長與代理商三顧股份有限公司交涉，日本日立公司鑒於臺灣疫情嚴峻，優先協調部分訂單給予我國採購，並由中華航空公司無償協助運輸工作，今日晚間首批10座已抵達臺灣，剩餘70座將分批於未來三周內陸續送達。\$\@\$指揮中心指出，「負壓隔離艙」可用於室內外、急診或加護病房等處，為確診或疑似病患提供緊急處置、暫留及轉出轉入空間，以減少醫護和病患直接接觸的機會，為我國第一線醫療資源提供直接的保護。正值此疫情艱難時刻，指揮中心感謝各方集結力量、團結抗疫，協助我國疫情防治工作，共同守護第一線醫療人員，指揮中心向各方表達誠摯的感謝，近日將儘快依各醫院需求及疫情狀況，調配運送至各醫院組裝啟用。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-10\$\@\$中央流行疫情指揮中心今（10）日表示，針對臺北市今日上午對COVID-19疫苗接種相關之言論，說明如下：\$\@\$一、    指揮中心指出，所謂4月21日之發文是指揮中心於4月14日與衛生局召開協調會之紀錄，其中一項決議為若合約醫院 COVID-19疫苗庫存量過多，評估無法於效期內用畢，為使疫苗有效運用，可在轄區衛生局人員協助下，將疫苗配送至其他合約醫院、非合約醫療院所或衛生所，需用者儘速使用，調度以一次為限，運送時應符合疫苗冷運冷藏相關規範等；惟當時狀況係因一批疫苗即將於5月底到期，當時開放之公費對象接種意願低，故將疫苗進行靈活配置，於效期前提供開放之公費對象中的需求者接種，以儘速適當使用疫苗。\$\@\$二、    指揮中心進一步說明，自5月下旬起，因疫情致疫苗接種需求大增，指揮中心為保障第一線醫護及防疫人員安全，依ACIP COVID-19疫苗工作小組會議決議，以電子郵件通知地方政府衛生局，自5/24起優先提供第一類至第三類人員接種，並視疫苗庫存量及接種規劃，提供3月22日至4月11日已完第一劑之醫護人員與因公務出國者接種第二劑，此外，必須暫緩「自費對象」以及「第一類至第三類同住者」接種；後續指揮中心撥配疫苗時亦皆限定接種對象，雙北地區以第一類至第三類未曾接種第一劑疫苗的醫事、防疫人員及高接觸風險者為優先接種對象，並未開放其他對象接種。有關好心肝診所接種疫苗的事件，疫苗效期至8月多，應無庫存量過多而無法使用之疑慮，且接種對象是否為開放接種之公費對象，為應釐清之重點。\$\@\$三、指揮中心重申，有關中央政府有850瓶COVID-19疫苗置於臺北市或轄內醫院一事，已於昨(9)日發布新聞稿說明，該等疫苗為指揮中心專案同意列冊施打對象，總計配送650瓶疫苗，其中差距之200瓶係為已送至臺北市立聯合醫院仁愛院區，提供華航機師及機組員接種之疫苗，另80瓶為指揮中心提供中心內各部會及疾管署人員施打，目前剩餘30瓶。\$\@\$四、有關疫苗接種預約系統部分，於這次124萬劑疫苗接種規劃，係以運用現行合約醫療院所預約模式提供民眾接種服務；至臺北市政府所提指揮中心規劃之預約系統，係為大規模接種措施使用，目前正積極測試中。\$\@\$指揮中心強調，疫苗接種政策為全體國民重要權益，相關規定、流程、接種對象及順序均公開透明，如有違法事項絕對依法徹查，嚴正法辦，絕不寬貸，有心人士切勿心存僥倖，以身試法。</t>
   </si>
 </sst>
 </file>
@@ -514,7 +1387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -542,16 +1415,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="C2" s="2">
-        <v>44384</v>
+        <v>44385</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -559,16 +1432,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="C3" s="2">
-        <v>44384</v>
+        <v>44385</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>26</v>
+        <v>186</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -576,16 +1449,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
       <c r="C4" s="2">
-        <v>44384</v>
+        <v>44385</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
+        <v>187</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -593,16 +1466,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
       <c r="C5" s="2">
-        <v>44383</v>
+        <v>44384</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>188</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -610,16 +1483,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="C6" s="2">
-        <v>44383</v>
+        <v>44384</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>29</v>
+        <v>189</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -627,16 +1500,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="C7" s="2">
-        <v>44383</v>
+        <v>44384</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>30</v>
+        <v>190</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -644,13 +1517,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>101</v>
       </c>
       <c r="C8" s="2">
-        <v>44382</v>
+        <v>44383</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>31</v>
+        <v>191</v>
+      </c>
+      <c r="E8" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -658,13 +1534,16 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="C9" s="2">
-        <v>44382</v>
+        <v>44383</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>32</v>
+        <v>192</v>
+      </c>
+      <c r="E9" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -672,16 +1551,16 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>103</v>
       </c>
       <c r="C10" s="2">
-        <v>44381</v>
+        <v>44383</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>193</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -689,13 +1568,1280 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="2">
+        <v>44382</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="2">
+        <v>44382</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E12" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="2">
+        <v>44381</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E13" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="2">
+        <v>44380</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="2">
+        <v>44379</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E15" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="2">
+        <v>44379</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E16" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" s="2">
+        <v>44379</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E17" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="2">
+        <v>44378</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E18" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" s="2">
+        <v>44378</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E19" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="2">
+        <v>44378</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="2">
-        <v>44380</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="B21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" s="2">
+        <v>44378</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="2">
+        <v>44377</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E22" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C23" s="2">
+        <v>44377</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E23" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" s="2">
+        <v>44377</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" s="2">
+        <v>44376</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" s="2">
+        <v>44376</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E26" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="2">
+        <v>44376</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E27" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" s="2">
+        <v>44376</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E28" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" s="2">
+        <v>44375</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E29" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" s="2">
+        <v>44374</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
         <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="2">
+        <v>44374</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E31" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" s="2">
+        <v>44374</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E32" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="2">
+        <v>44374</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E33" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" s="2">
+        <v>44373</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E34" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" s="2">
+        <v>44373</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" s="2">
+        <v>44373</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E36" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C37" s="2">
+        <v>44373</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E37" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" t="s">
+        <v>131</v>
+      </c>
+      <c r="C38" s="2">
+        <v>44373</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="2">
+        <v>44372</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="E39" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" s="2">
+        <v>44372</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E40" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" s="2">
+        <v>44372</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E41" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" t="s">
+        <v>135</v>
+      </c>
+      <c r="C42" s="2">
+        <v>44372</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="E42" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
+        <v>136</v>
+      </c>
+      <c r="C43" s="2">
+        <v>44371</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="E43" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" t="s">
+        <v>137</v>
+      </c>
+      <c r="C44" s="2">
+        <v>44371</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="2">
+        <v>44371</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" t="s">
+        <v>139</v>
+      </c>
+      <c r="C46" s="2">
+        <v>44370</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E46" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" t="s">
+        <v>140</v>
+      </c>
+      <c r="C47" s="2">
+        <v>44370</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" t="s">
+        <v>141</v>
+      </c>
+      <c r="C48" s="2">
+        <v>44370</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" t="s">
+        <v>142</v>
+      </c>
+      <c r="C49" s="2">
+        <v>44369</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="2">
+        <v>44369</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" t="s">
+        <v>144</v>
+      </c>
+      <c r="C51" s="2">
+        <v>44369</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" t="s">
+        <v>145</v>
+      </c>
+      <c r="C52" s="2">
+        <v>44369</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" t="s">
+        <v>146</v>
+      </c>
+      <c r="C53" s="2">
+        <v>44369</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="E53" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54" t="s">
+        <v>147</v>
+      </c>
+      <c r="C54" s="2">
+        <v>44368</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" t="s">
+        <v>148</v>
+      </c>
+      <c r="C55" s="2">
+        <v>44368</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" t="s">
+        <v>149</v>
+      </c>
+      <c r="C56" s="2">
+        <v>44367</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E56" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57" t="s">
+        <v>150</v>
+      </c>
+      <c r="C57" s="2">
+        <v>44367</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" t="s">
+        <v>151</v>
+      </c>
+      <c r="C58" s="2">
+        <v>44367</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>62</v>
+      </c>
+      <c r="B59" t="s">
+        <v>152</v>
+      </c>
+      <c r="C59" s="2">
+        <v>44366</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" t="s">
+        <v>153</v>
+      </c>
+      <c r="C60" s="2">
+        <v>44366</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B61" t="s">
+        <v>154</v>
+      </c>
+      <c r="C61" s="2">
+        <v>44366</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62" t="s">
+        <v>155</v>
+      </c>
+      <c r="C62" s="2">
+        <v>44365</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" t="s">
+        <v>156</v>
+      </c>
+      <c r="C63" s="2">
+        <v>44365</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" t="s">
+        <v>157</v>
+      </c>
+      <c r="C64" s="2">
+        <v>44365</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E64" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65" t="s">
+        <v>158</v>
+      </c>
+      <c r="C65" s="2">
+        <v>44365</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E65" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" t="s">
+        <v>159</v>
+      </c>
+      <c r="C66" s="2">
+        <v>44365</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E66" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" t="s">
+        <v>160</v>
+      </c>
+      <c r="C67" s="2">
+        <v>44364</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68" t="s">
+        <v>161</v>
+      </c>
+      <c r="C68" s="2">
+        <v>44364</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" t="s">
+        <v>162</v>
+      </c>
+      <c r="C69" s="2">
+        <v>44363</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70" t="s">
+        <v>163</v>
+      </c>
+      <c r="C70" s="2">
+        <v>44363</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" t="s">
+        <v>164</v>
+      </c>
+      <c r="C71" s="2">
+        <v>44363</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>75</v>
+      </c>
+      <c r="B72" t="s">
+        <v>165</v>
+      </c>
+      <c r="C72" s="2">
+        <v>44362</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>76</v>
+      </c>
+      <c r="B73" t="s">
+        <v>166</v>
+      </c>
+      <c r="C73" s="2">
+        <v>44362</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E73" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>77</v>
+      </c>
+      <c r="B74" t="s">
+        <v>167</v>
+      </c>
+      <c r="C74" s="2">
+        <v>44362</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="E74" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>78</v>
+      </c>
+      <c r="B75" t="s">
+        <v>168</v>
+      </c>
+      <c r="C75" s="2">
+        <v>44362</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76" t="s">
+        <v>169</v>
+      </c>
+      <c r="C76" s="2">
+        <v>44362</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="E76" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>80</v>
+      </c>
+      <c r="B77" t="s">
+        <v>170</v>
+      </c>
+      <c r="C77" s="2">
+        <v>44361</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="E77" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78" t="s">
+        <v>171</v>
+      </c>
+      <c r="C78" s="2">
+        <v>44361</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E78" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>82</v>
+      </c>
+      <c r="B79" t="s">
+        <v>172</v>
+      </c>
+      <c r="C79" s="2">
+        <v>44360</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>83</v>
+      </c>
+      <c r="B80" t="s">
+        <v>173</v>
+      </c>
+      <c r="C80" s="2">
+        <v>44360</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E80" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>84</v>
+      </c>
+      <c r="B81" t="s">
+        <v>174</v>
+      </c>
+      <c r="C81" s="2">
+        <v>44360</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="E81" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82" t="s">
+        <v>175</v>
+      </c>
+      <c r="C82" s="2">
+        <v>44359</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E82" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83" t="s">
+        <v>176</v>
+      </c>
+      <c r="C83" s="2">
+        <v>44359</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E83" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84" t="s">
+        <v>177</v>
+      </c>
+      <c r="C84" s="2">
+        <v>44359</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E84" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>88</v>
+      </c>
+      <c r="B85" t="s">
+        <v>178</v>
+      </c>
+      <c r="C85" s="2">
+        <v>44358</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E85" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>89</v>
+      </c>
+      <c r="B86" t="s">
+        <v>179</v>
+      </c>
+      <c r="C86" s="2">
+        <v>44358</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="E86" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>90</v>
+      </c>
+      <c r="B87" t="s">
+        <v>180</v>
+      </c>
+      <c r="C87" s="2">
+        <v>44358</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E87" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>91</v>
+      </c>
+      <c r="B88" t="s">
+        <v>181</v>
+      </c>
+      <c r="C88" s="2">
+        <v>44358</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="E88" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>92</v>
+      </c>
+      <c r="B89" t="s">
+        <v>182</v>
+      </c>
+      <c r="C89" s="2">
+        <v>44358</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E89" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>93</v>
+      </c>
+      <c r="B90" t="s">
+        <v>183</v>
+      </c>
+      <c r="C90" s="2">
+        <v>44357</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E90" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>94</v>
+      </c>
+      <c r="B91" t="s">
+        <v>184</v>
+      </c>
+      <c r="C91" s="2">
+        <v>44357</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E91" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -710,6 +2856,86 @@
     <hyperlink ref="D9" r:id="rId8"/>
     <hyperlink ref="D10" r:id="rId9"/>
     <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="D12" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId12"/>
+    <hyperlink ref="D14" r:id="rId13"/>
+    <hyperlink ref="D15" r:id="rId14"/>
+    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D17" r:id="rId16"/>
+    <hyperlink ref="D18" r:id="rId17"/>
+    <hyperlink ref="D19" r:id="rId18"/>
+    <hyperlink ref="D20" r:id="rId19"/>
+    <hyperlink ref="D21" r:id="rId20"/>
+    <hyperlink ref="D22" r:id="rId21"/>
+    <hyperlink ref="D23" r:id="rId22"/>
+    <hyperlink ref="D24" r:id="rId23"/>
+    <hyperlink ref="D25" r:id="rId24"/>
+    <hyperlink ref="D26" r:id="rId25"/>
+    <hyperlink ref="D27" r:id="rId26"/>
+    <hyperlink ref="D28" r:id="rId27"/>
+    <hyperlink ref="D29" r:id="rId28"/>
+    <hyperlink ref="D30" r:id="rId29"/>
+    <hyperlink ref="D31" r:id="rId30"/>
+    <hyperlink ref="D32" r:id="rId31"/>
+    <hyperlink ref="D33" r:id="rId32"/>
+    <hyperlink ref="D34" r:id="rId33"/>
+    <hyperlink ref="D35" r:id="rId34"/>
+    <hyperlink ref="D36" r:id="rId35"/>
+    <hyperlink ref="D37" r:id="rId36"/>
+    <hyperlink ref="D38" r:id="rId37"/>
+    <hyperlink ref="D39" r:id="rId38"/>
+    <hyperlink ref="D40" r:id="rId39"/>
+    <hyperlink ref="D41" r:id="rId40"/>
+    <hyperlink ref="D42" r:id="rId41"/>
+    <hyperlink ref="D43" r:id="rId42"/>
+    <hyperlink ref="D44" r:id="rId43"/>
+    <hyperlink ref="D45" r:id="rId44"/>
+    <hyperlink ref="D46" r:id="rId45"/>
+    <hyperlink ref="D47" r:id="rId46"/>
+    <hyperlink ref="D48" r:id="rId47"/>
+    <hyperlink ref="D49" r:id="rId48"/>
+    <hyperlink ref="D50" r:id="rId49"/>
+    <hyperlink ref="D51" r:id="rId50"/>
+    <hyperlink ref="D52" r:id="rId51"/>
+    <hyperlink ref="D53" r:id="rId52"/>
+    <hyperlink ref="D54" r:id="rId53"/>
+    <hyperlink ref="D55" r:id="rId54"/>
+    <hyperlink ref="D56" r:id="rId55"/>
+    <hyperlink ref="D57" r:id="rId56"/>
+    <hyperlink ref="D58" r:id="rId57"/>
+    <hyperlink ref="D59" r:id="rId58"/>
+    <hyperlink ref="D60" r:id="rId59"/>
+    <hyperlink ref="D61" r:id="rId60"/>
+    <hyperlink ref="D62" r:id="rId61"/>
+    <hyperlink ref="D63" r:id="rId62"/>
+    <hyperlink ref="D64" r:id="rId63"/>
+    <hyperlink ref="D65" r:id="rId64"/>
+    <hyperlink ref="D66" r:id="rId65"/>
+    <hyperlink ref="D67" r:id="rId66"/>
+    <hyperlink ref="D68" r:id="rId67"/>
+    <hyperlink ref="D69" r:id="rId68"/>
+    <hyperlink ref="D70" r:id="rId69"/>
+    <hyperlink ref="D71" r:id="rId70"/>
+    <hyperlink ref="D72" r:id="rId71"/>
+    <hyperlink ref="D73" r:id="rId72"/>
+    <hyperlink ref="D74" r:id="rId73"/>
+    <hyperlink ref="D75" r:id="rId74"/>
+    <hyperlink ref="D76" r:id="rId75"/>
+    <hyperlink ref="D77" r:id="rId76"/>
+    <hyperlink ref="D78" r:id="rId77"/>
+    <hyperlink ref="D79" r:id="rId78"/>
+    <hyperlink ref="D80" r:id="rId79"/>
+    <hyperlink ref="D81" r:id="rId80"/>
+    <hyperlink ref="D82" r:id="rId81"/>
+    <hyperlink ref="D83" r:id="rId82"/>
+    <hyperlink ref="D84" r:id="rId83"/>
+    <hyperlink ref="D85" r:id="rId84"/>
+    <hyperlink ref="D86" r:id="rId85"/>
+    <hyperlink ref="D87" r:id="rId86"/>
+    <hyperlink ref="D88" r:id="rId87"/>
+    <hyperlink ref="D89" r:id="rId88"/>
+    <hyperlink ref="D90" r:id="rId89"/>
+    <hyperlink ref="D91" r:id="rId90"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20210713
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Press Title</t>
   </si>
@@ -31,6 +31,12 @@
     <t>Page Content</t>
   </si>
   <si>
+    <t>新增29例COVID-19確定病例，分別為28例本土及1例境外移入</t>
+  </si>
+  <si>
+    <t>COVID-19公費疫苗預約平臺  即日起開放18歲(含)以上民眾進行第三輪意願登記</t>
+  </si>
+  <si>
     <t>為儘速提升第一劑COVID-19疫苗涵蓋率，第二劑Moderna疫苗接種間隔調整自第10週起接種</t>
   </si>
   <si>
@@ -61,6 +67,36 @@
     <t>針對媒體報導「指揮中心設局召開記者會」 指揮中心澄清並非事實</t>
   </si>
   <si>
+    <t>指揮中心延長全國疫情警戒第三級至7月26日止，嚴守社區防線，並自7月13日起適度鬆綁部分措施</t>
+  </si>
+  <si>
+    <t>指揮中心訂購第二批AZ疫苗62.6萬劑將於今(7)日下午抵臺</t>
+  </si>
+  <si>
+    <t>新增40例COVID-19確定病例，分別為39例本土及1例境外移入</t>
+  </si>
+  <si>
+    <t>網傳COVID-19疫苗施打登記系統異常為不實訊息 全國第9、10類皆可登記且紀錄不會被消除</t>
+  </si>
+  <si>
+    <t>新增29例COVID-19確定病例，分別為27例本土及2例境外移入</t>
+  </si>
+  <si>
+    <t>日本政府提供113萬劑AstraZeneca COVID-19疫苗將於7月8日下午抵臺</t>
+  </si>
+  <si>
+    <t>7月6日全國防疫會議後記者會報告</t>
+  </si>
+  <si>
+    <t>報載「疾病管制署造冊人數，超過編制內人數」 指揮中心說明：人員皆符合規定 以利防疫運作</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/mdt2oCvvps_-TB8TSliKag?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/RACDgdJ7AErNus7J2j37iw?typeid=9</t>
+  </si>
+  <si>
     <t>/Bulletin/Detail/vu8IYJ-y67cc4ZpemyPBTA?typeid=9</t>
   </si>
   <si>
@@ -91,6 +127,36 @@
     <t>/Bulletin/Detail/65J6c1wTSqx-68NNaCRU5g?typeid=9</t>
   </si>
   <si>
+    <t>/Bulletin/Detail/aiGegg4ncYmMP9dTx4W_Zw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/BlxZvHJU1w5vlVvV3EqlXg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/2Rt1n0uftGTcpzceVxt5Zg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/o2v7FN9aRKyxQMLbSEh6Sg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/UDshrp3kzpPt0FBWObobWQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/FS-2y4B6C2TqLutsQbWlzQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/eW2VeHdKNhOsJIjrzEIQlA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/PrfZ05Bfggkz1sUAAWohbg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/mdt2oCvvps_-TB8TSliKag?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/RACDgdJ7AErNus7J2j37iw?typeid=9</t>
+  </si>
+  <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/vu8IYJ-y67cc4ZpemyPBTA?typeid=9</t>
   </si>
   <si>
@@ -121,6 +187,36 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/65J6c1wTSqx-68NNaCRU5g?typeid=9</t>
   </si>
   <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/aiGegg4ncYmMP9dTx4W_Zw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/BlxZvHJU1w5vlVvV3EqlXg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/2Rt1n0uftGTcpzceVxt5Zg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/o2v7FN9aRKyxQMLbSEh6Sg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/UDshrp3kzpPt0FBWObobWQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/FS-2y4B6C2TqLutsQbWlzQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/eW2VeHdKNhOsJIjrzEIQlA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/PrfZ05Bfggkz1sUAAWohbg?typeid=9</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-13\$\@\$中央流行疫情指揮中心今(13)日公布國內新增29例COVID-19確定病例，分別為28例本土及1例境外移入；另確診個案中新增6例死亡。\$\@\$指揮中心表示，今日新增之28例本土病例(其中11例為居家隔離期間或期滿檢驗陽性者)，為18例男性、10例女性，年齡介於未滿10歲至80多歲，發病日介於今(2021)年6月26日至7月12日。個案分布以新北市15例為最多，其次為臺北市9例，桃園市2例，苗栗縣及臺中市各1例；其中16例為已知感染源、3例關聯不明、9例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增6例死亡個案，為4例男性、2例女性，年齡介於60多歲至80多歲，發病日介於5月12日至6月18日，確診日介於5月16日至6月19日，死亡日介於7月4日至7月12日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月11日累計公布14,050位確診個案中，已有11,901人解除隔離，解隔離人數達確診人數84.7%。\$\@\$指揮中心表示，今日新增1例境外移入個案(案15387)，為本國籍40多歲男性，6月30日自印尼入境，持搭機前3日內檢驗陰性報告，入境後至集中檢疫所檢疫並採檢，7月1日結果為陰性；7月8日出現輕微發燒與肌肉痠痛等症狀，7月11日仍未緩解，由衛生單位安排採檢，於今日確診。個案檢疫期間無接觸他人，同機旅客均已入住集中檢疫所，故無匡列接觸者。\$\@\$指揮中心統計，截至目前國內累計1,661,153例新型冠狀病毒肺炎相關通報(含1,644,686例排除)，其中15,302例確診，分別為1,204例境外移入，14,045例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；確診個案中，累計105例移除為空號。2020年起累計747例COVID-19死亡病例，其中739例本土，個案居住縣市分布為新北市370例、臺北市286例、基隆市25例、桃園市21例、彰化縣13例、新竹縣10例、臺中市4例、宜蘭縣、苗栗縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月13日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-13\$\@\$中央流行疫情指揮中心今(13)日表示，為順利推動我國COVID-19疫苗接種作業，自即(7/13)日起開放18歲(含)以上民眾，於「疫苗施打意願登記與預約系統」( https://1922.gov.tw/）進行第三輪意願登記，相關說明如下：\$\@\$一、意願登記時間：即日起至7月15日17時，並同步進行第三輪結算。\$\@\$二、簡訊通知時間：7月16日至7月18日將陸續以簡訊通知符合資格的民眾；收到簡訊者，才能進行預約。本輪可接種疫苗為AZ疫苗。\$\@\$三、為協助不便使用「COVID-19疫苗施打意願登記與預約系統」的民眾登記意願，請地方政府設置因地制宜的服務專線或指定人員，協助不便使用系統的民眾進行意願登記。\$\@\$指揮中心進一步表示，第二輪的意願登記已於昨(12)日17時截止，全國約有285萬人登記，其中約114萬人有意願接種AZ疫苗。系統平臺將自7月13日上午，陸續以簡訊通知符合資格的民眾，提醒收到簡訊民眾記得進行預約；施打期間為7月16日至7月22日，籲請民眾準時前往接種。\$\@\$指揮中心提醒，「COVID-19疫苗施打意願登記與預約系統」須先完成意願登記，才能在接到通知後進行預約。系統平臺會按疫苗分配情形、參照民眾所登記的意願，通知符合預約資格的民眾，收到簡訊通知者即可進行下一步預約接種。尚未收到簡訊的民眾，會於後續符合預約資格後，收到簡訊通知，所有資料皆會完整保存，請民眾放心。\$\@\$指揮中心強調，「COVID-19疫苗施打意願登記與預約系統」是為建立讓大量疫苗接種能依序穩定有效推行的機制，中央與地方腳步一致，加強疫苗接種推動，提升群體保護力，維護國人健康。</t>
+  </si>
+  <si>
     <t>發佈日期：2021-07-12\$\@\$中央流行疫情指揮中心今(12)日表示，為儘速提升國人COVID-19疫苗第一劑涵蓋率及我國群體保護力，並因應政策需要，昨(11)日經衛生福利部傳染病防治諮詢會預防接種組(ACIP)會議第4次臨時會議決議，自即日起調整現階段Moderna COVID-19疫苗之第一、二劑接種間隔，除第一類接種對象、國籍航空機組員及孕婦的第二劑Moderna疫苗維持於間隔至少28天後接種外，其餘對象均調整第一劑與第二劑接種間隔10至12週，並依疫苗供貨情形滾動調整。\$\@\$指揮中心指出，截至昨(11)日COVID-19疫苗(包含Moderna及AstraZeneca)累計接種3,565,840人次，疫苗涵蓋率約14.87%。依據國外臨床試驗資料分析顯示，Moderna COVID-19疫苗完成接種第一劑14天後保護力約為81%，另依據WHO建議接種間隔最晚可至12週，指揮中心考量政策需要並參考ACIP建議，亦將Moderna COVID-19疫苗接種間隔調整為10至12週，並持續視疫情狀況及疫苗供貨情形，滾動調整接種政策。\$\@\$指揮中心提醒，前往接種第二劑疫苗前，請確認備妥「COVID-19疫苗接種紀錄卡」及「健保卡」，若「COVID-19疫苗接種紀錄卡」已遺失，民眾可返回第一劑接種之醫療院所補發，再完成第二劑接種。此外，籲請民眾完成疫苗接種後，須持續積極配合各項防疫措施，並落實勤洗手、戴口罩及保持社交距離等個人防護，以全面保護自我與家人的健康，有效降低染疫風險。</t>
   </si>
   <si>
@@ -139,10 +235,22 @@
     <t>發佈日期：2021-07-10\$\@\$中央流行疫情指揮中心今(10)日公布國內新增33例COVID-19確定病例，分別為31例本土及2例境外移入；另確診個案中新增6例死亡。\$\@\$指揮中心表示，今日新增之31例本土病例(其中19例為居家隔離期間或期滿檢驗陽性者)，為17例男性、14例女性，年齡介於10多歲至70多歲，發病日介於今(2021)年6月22日至7月9日。個案分布以臺北市及新北市各13例最多，其次為桃園市4例，基隆市1例；其中21例為已知感染源、2例關聯不明、8例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增6例死亡個案，為2例男性、4例女性，年齡介於30多歲至80多歲，發病日介於6月3日至6月24日，確診日介於6月4日至6月25日，死亡日介於7月6日至7月8日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月8日累計公布13,950位確診個案中，已有11,698人解除隔離，解隔離人數達確診人數83.9%。\$\@\$指揮中心表示，今日新增2例境外移入中，案15299為本國籍30多歲女性，6月25日自義大利入境，持搭機前3日內檢驗陰性報告，入境後至自宅居家檢疫，7月8日進行期滿前採檢，於今日確診，個案在臺期間並無症狀，檢疫期間無接觸他人，故無匡列接觸者。案15319為本國籍20多歲男性，6月26日自比利時入境，持搭機前3日內檢驗陰性報告，入境後於自宅居家檢疫，7月8日進行期滿前採檢，於今日確診，個案在臺期間並無症狀，檢疫期間無接觸他人，故無匡列接觸者。\$\@\$指揮中心統計，截至目前國內累計1,606,389例新型冠狀病毒肺炎相關通報(含1,589,769例排除)，其中15,218例確診，分別為1,199例境外移入，13,966例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；個案中累計105例移除為空號。自2020年起累計736例COVID-19死亡病例，其中728例本土，個案居住縣市分布為新北市368例、臺北市279例、基隆市25例、桃園市21例、彰化縣12例、新竹縣9例、臺中市4例、宜蘭縣、苗栗縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月10日新增死亡COVID-19確診個案表.pdf</t>
   </si>
   <si>
-    <t>發佈日期：2021-07-09\$\@\$中央流行疫情指揮中心今(9)日公布國內新增36例COVID-19確定病例，分別為32例本土及4例境外移入；另確診個案中新增12例死亡。\$\@\$指揮中心表示，今日新增之32例本土病例(其中13例為居家隔離期間或期滿檢驗陽性者)，為17例男性、15例女性，年齡介於未滿5歲至70多歲，發病日介於今(2021)年7月1日至7月8日。個案分布以臺北市19例最多，其次為新北市11例、桃園市2例；其中14例為已知感染源、1例關聯不明、17例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增12例死亡個案，為8例男性、4例女性，年齡介於40多歲至80多歲，發病日介於5月12日至7月4日，確診日介於5月16日至7月7日，死亡日介於6月30日至7月8日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月7日累計公布13,929位確診個案中，已有11,536人解除隔離，解隔離人數達確診人數82.8%。\$\@\$指揮中心表示，今日新增4例境外移入中，案15270為本國籍60多歲女性，6月25日自土耳其返臺，持有搭機前3日內檢驗陰性報告，入境後於自宅進行居家檢疫，7月7日檢疫期滿前採檢，於今日確診；個案在臺期間並無症狀，且檢疫期間未與他人接觸，故無匡列接觸者。案15283為本國籍30多歲女性，7月7日自美國返臺，持有搭機前3日內檢驗陰性報告，入境後在機場採檢，於今日確診；個案在臺期間並無症狀，已匡列同班機前後2排旅客共6人，均列居家隔離。案15289、15290皆為本國籍20多歲女性，7月7日自捷克搭乘同班機返臺，均持有搭機前3日內檢驗陰性報告，入境後在機場採檢，於今日確診；2人在臺期間並無症狀，相關接觸者匡列中。\$\@\$指揮中心統計，截至目前國內累計1,582,844例新型冠狀病毒肺炎相關通報(含1,566,436例排除)，其中15,185例確診，分別為1,197例境外移入，13,935例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計105例移除為空號。自2020年起累計730例COVID-19死亡病例，其中722例本土，個案居住縣市分布為新北市367例、臺北市277例、基隆市24例、桃園市21例、彰化縣12例、新竹縣8例、臺中市4例、宜蘭縣、苗栗縣及花蓮縣各2例，臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月9日新增死亡COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
     <t>發佈日期：2021-07-08\$\@\$中央流行疫情指揮中心今(8)日表示，為順利推動我國COVID-19疫苗接種作業，指揮中心於昨(7)日下午邀集各地方政府代表共同召開「疫苗施打意願登記與預約系統」討論會議，達成共識及決議如下：\$\@\$一、指揮中心將自即日起，開放全國第9類及第10類對象意願登記，並正式啟用「COVID-19疫苗施打意願登記與預約系統」，請符合資格民眾可先行意願登記：\$\@\$(一) 意願登記：即日起至7月12日下午5時止。\$\@\$(二) 為保障65歲以上長者疫苗接種權益，若希望使用該系統進行意願登記，請依時程辦理。\$\@\$二、為協助不便使用「COVID-19疫苗施打意願登記與預約系統」之民眾進行意願登記，請地方政府設置因地制宜之服務專線或指定人員，協助不便使用系統民眾進行意願登記。\$\@\$指揮中心提醒，「COVID-19疫苗施打意願登記與預約系統」須先完成意願登記後，才能在接到通知後進行預約。系統平臺會按疫苗分配情形參照民眾所登記之意願，通知符合預約資格的民眾，收到簡訊通知者即可進行下一步預約接種。尚未收到簡訊之民眾，會於後續符合預約資格後，收到簡訊通知，所有資料皆會完整保存，請民眾放心。指揮中心也強調，「COVID-19疫苗施打意願登記與預約系統」是為建立一個讓大量疫苗接種能依序穩定有效推行之機制，中央與地方腳步一致，加強疫苗接種推動，提升群體保護力，維護國人健康。\$\@\$備註:\$\@\$第9類對象為18-64歲具有易導致嚴重疾病之高風險疾病者、罕見疾病及重大傷病者。\$\@\$高風險疾病者定義： https://reurl.cc/R02Qx6\$\@\$罕見疾病定義： https://reurl.cc/Nr2E36\$\@\$重大傷病者請依健保卡註記或重大傷病卡為主\$\@\$第10類對象為50-64歲成人。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-08\$\@\$中央流行疫情指揮中心今(8)日公布國內新增21例COVID-19確定病例，分別為18例本土及3例境外移入；另確診個案中新增3例死亡。\$\@\$指揮中心表示，今日新增之18例本土病例(其中6例為居家隔離期間或期滿檢驗陽性者)，為8例男性、10例女性，年齡介於未滿5歲至60多歲，發病日介於今(2021)年7月1日至7月7日。個案分布以臺北市12例最多，其次為新北市6例；其中9例為已知感染源、9例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增3例死亡個案，為2例男性、1例女性，年齡介於60多歲至70多歲，發病日介於5月27日至6月14日，確診日介於5月28日至6月17日，死亡日介於7月5日至7月6日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月6日累計公布13,889位確診個案中，已有11,456人解除隔離，解隔離人數達確診人數82.5%。\$\@\$指揮中心表示，今日新增3例境外移入中，案15252為本國籍30多歲男性，6月23日自泰國返臺，持有搭機前3日內檢驗陰性報告，入境後至防疫旅館檢疫，7月6日檢疫期滿前採檢，於今日確診；個案在臺期間並無症狀，且檢疫期間未與他人接觸，故無匡列接觸者。案15253為印尼籍20多歲男性漁工，5月10日自印尼來臺，持有搭機前3日內檢驗陰性報告，入境後至集中檢疫所檢疫，5月23日檢疫期滿前採檢結果為陰性，7月7日因有離境需求再次採檢，於今日確診；個案在臺期間並無症狀，已匡列接觸者221人，其中60人列居家隔離，餘161人列自我健康監測。案15254為本國籍10多歲女性，7月6日自美國返臺，持有搭機前3日內檢驗陰性報告，入境時在機場採檢，於今日確診；個案在臺期間並無症狀，相關接觸者匡列中。\$\@\$指揮中心統計，截至目前國內累計1,541,974例新型冠狀病毒肺炎相關通報(含1,525,372例排除)，其中15,149例確診，分別為1,193例境外移入，13,903例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計105例移除為空號。自2020年起累計 718例COVID-19死亡病例，其中710例本土，個案居住縣市分布為新北市363例、臺北市272例、基隆市24例、桃園市20例、彰化縣12例、新竹縣7例、臺中市4例、宜蘭縣及花蓮縣各2例，苗栗縣、臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月8日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-08\$\@\$針對媒體報導「指揮中心設局召開記者會」，中央流行疫情指揮中心今(8)日說明如下：\$\@\$一、針對臺北市環南市場進行大規模PCR篩檢且41人呈現陽性，顯示有群聚感染疫情，指揮中心於7月2日11:30前往環南市場現場召開記者會，並宣布與臺北市政府共同成立聯合前進指揮所。\$\@\$二、當日陳時中指揮官於9:45致電黃珊珊副市長，黃副市長將電話轉交給柯文哲市長，陳指揮官與柯市長直接通話，雙方對成立聯合前進指揮所達成共識，並在環南市場現場召開記者會。\$\@\$三、當日農委會陳吉仲主委於10:00多左右，親自致電二通予臺北市黃副市長，並於第二通電話中明確告知黃副市長，陳指揮官、經濟部王美花部長及農委會陳吉仲主委將至環南市場召開記者會，並邀請黃副市長出席，黃副市長表示柯市長也會出席。\$\@\$四、指揮中心表示，當日均依照指揮中心記者會程序，發布採訪通知；指揮中心幕僚抵達環南市場後，亦與臺北市市場處高副處長確認記者會場地、流程及雙方出席人員，同時與現場媒體溝通說明記者會流程，及預定出席人員。\$\@\$五、當日11:01，臺北市府陳智菡發言人於臺北市府群組發布採訪通知，說明柯市長、黃副市長皆會出席記者會； 11:20柯市長、黃副市長抵達環南市場。\$\@\$六、指揮中心說明，為儘快有效控制疫情，召開記者會說明防疫作為及因應措施，以利相關市場攤商、工作人員及周邊住民了解需配合之事項，並無「以開會名義設局召開記者會」一事。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-08\$\@\$中央流行疫情指揮中心今(8)日表示，在國人共同努力配合下，國內疫情已在控制中，惟仍有部分感染事件發生，參酌世界各國管制作為及經驗，防疫措施鬆綁須逐步執行，才可穩定掌握疫情狀況，為確保國人健康，指揮中心經評估後決定，同步延長全國疫情警戒第三級至7月26日止，並自7月13日起適度鬆綁部分措施，說明如下：\$\@\$一、適度鬆綁措施：\$\@\$(一)    有條件鬆綁對象（地方政府得視防疫需要因時因地調整）：\$\@\$1.    戶外：國家公園、國家風景區、遊樂園區、休閒農場、森林遊樂區、植物園、文化園區、學校操場、駕訓班。\$\@\$2.    室內：美術館、博物館、電影院、表演場館(無觀眾)、社教機構、文化中心。\$\@\$3.    室內外運動場館(游泳池除外)、高爾夫球場。\$\@\$4.    餐飮場所(餐廳、傳統市場及夜市、百貨賣場 美食街、美食區等)符合指揮中心指引得內用。\$\@\$5.    國內小型旅行團(9人以下)、劇組拍攝。\$\@\$(二)    上述鬆綁須遵照通案性原則及主管機關指引：\$\@\$1.    實聯制、出入口管制、人流管控降載。\$\@\$2.    維持社交距離，除飮食外，全程戴口罩。\$\@\$3.    員工人員健康管理、確診事件即時應變。\$\@\$二、三級警戒延長仍須關閉之場所：\$\@\$(一)    休閒娛樂場所：\$\@\$歌廳、舞廳、夜總會、俱樂部、酒家、酒吧、酒店(廊)、錄影節目帶播映場所(MTV)、視聽歌唱場所(KTV)、理容院(觀光理髮、視聽理容)、指壓按摩場所、健身休閒中心(含提供指壓、三溫暖等設施之美容瘦身場所)、保齡球館、撞球場、室內螢幕式高爾夫練習場、遊藝場所、電子遊戲場、資訊休閒場所、休閒麻將館、自助選物販賣機營業場所、釣蝦場、桌遊場所及其他類似場所。\$\@\$(二)    教育學習場域：\$\@\$社區大學、樂齡學習中心、訓練班(駕訓班除外)、K書中心等其他類似場所。\$\@\$(三)    觀展觀賽場所：\$\@\$會展場館、游泳池等其他類似場所。\$\@\$指揮中心表示，鬆綁過程是疫情重要關鍵，籲請全國民眾持續落實遵循並積極配合三級警戒管制及鬆綁規定相關措施，與政府共同努力，嚴守社區防線。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-07\$\@\$網路謠傳「有1922回復，系統異常讓其他地區民眾預約登記、疾管署討論虛擬預約或取消方式處理、及正式預約開始要向1922確認」等資訊，中央流行疫情指揮中心今(7)日澄清，「COVID-19疫苗施打意願登記與預約系統」(1922.gov.tw)運作順暢並無異常，且已正式上線，並非虛擬預約，所有登記成功者皆已記錄在案，除非事後自行取消，否則已登記之紀錄並不會受到影響。前述相關網路訊息均非疾管署或1922防疫專線發布、回復，且內容多有不實，籲請民眾勿信、轉傳與散布。\$\@\$指揮中心說明，有關「COVID-19疫苗施打意願登記與預約系統」其設計目前為開放全國第9、10類對象民眾進行疫苗施打意願登記，故不限金馬澎地區登記意願；惟完成意願登記者，須符合當時公布開放預約之接種年齡及資格條件，系統平台會按疫苗分配情形以簡訊通知符合預約資格的民眾，收到簡訊通知者即可進行下一步預約接種。如有完成意願登記但不符合當時預約資格，則暫時不會收到預約接種簡訊且無法預約接種。而本次以離島金門、馬祖和澎湖先行試辦意願登記及預約接種，未來將再逐步開放到全國，截至今日8時，全國已有約148萬符合第9、10類接種對象完成意願登記，其中離島金門、馬祖及澎湖之意願登記人數約為4千5百人。\$\@\$指揮中心指出，目前全國1-8類對象已開放接種，符合該等對象資格者可依縣市政府規劃安排接種。昨日上線之「COVID-19疫苗施打意願登記與預約系統」，係為建立一個讓大量疫苗接種能依序穩定有效推行之機制，請符合第9、10類對象民眾先進行意願登記，再依簡訊通知，進行預約接種。\$\@\$指揮中心強調，網路謠傳「有1922回復，系統異常讓其他地區民眾預約登記、疾管署討論虛擬預約或取消方式處理、及正式預約開始要向1922確認」等資訊皆為不實訊息且均非發布自疾管署或1922防疫專線，籲請民眾勿信、轉傳與散布。 圖片 附件\$\@\$網傳COVID-19疫苗施打登記系統異常為不實訊息 全國第9、10類皆可登記且紀錄不會被消除.jpg</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-06\$\@\$中央流行疫情指揮中心今(6)日公布國內新增29例COVID-19確定病例，分別為27例本土及2例境外移入；另確診個案中新增17例死亡。\$\@\$指揮中心表示，今日新增之27例本土病例(其中15例為居家隔離期間或期滿檢驗陽性者)，為17例男性、10例女性，年齡介於未滿5歲至70多歲，發病日介於今(2021)年6月10日至7月5日。個案分布以臺北市14例最多，其次為新北市11例、屏東縣及彰化縣各1例；其中17例為已知感染源、10例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增17例死亡個案，為14位男性、3位女性，發病日介於5月16日至7月2日，確診日介於5月19日至7月5日，死亡日介於6月28日至7月5日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月4日累計公布13,831位確診個案中，已有11,180人解除隔離，解隔離人數達確診人數80.8%。\$\@\$指揮中心表示，今日新增境外移入個案中，案15180為本國籍10多歲男性，7月4日自美國入境，持有搭機前3日內檢驗陰性報告，入境時並無症狀，於機場採檢後至防疫旅館檢疫，7月5日出現嗅味覺異常等症狀，於今日確診，相關接觸者匡列中。案15185為本國籍30多歲男性，6月30日自印尼入境，持有搭機前3日內檢驗陰性報告，入境後至集中檢疫所檢疫並進行採檢，當日採檢結果為陰性；7月4日出現發燒、肌肉痠痛、流鼻水等症狀，7月5日由衛生單位採檢送驗，於今日確診，同班機旅客均已入境採檢並入住集中檢疫所。\$\@\$指揮中心統計，截至目前國內累計1,503,584例新型冠狀病毒肺炎相關通報(含1,487,019例排除)，其中15,088例確診，分別為1,189例境外移入，13,846例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另新增2例空號(案10180、案13124)，累計105例移除為空號。自2020年起累計706例COVID-19死亡病例，其中698例本土，個案居住縣市分布為新北市354例、臺北市269例、基隆市24例、桃園市20例、彰化縣12例、新竹縣7例、臺中市4例、宜蘭縣及花蓮縣各2例，苗栗縣、臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月6日新增死亡COVID-19確診個案表.pdf</t>
   </si>
 </sst>
 </file>
@@ -517,7 +625,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -545,16 +653,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2">
-        <v>44389</v>
+        <v>44390</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -562,16 +670,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2">
-        <v>44389</v>
+        <v>44390</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -579,16 +687,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2">
         <v>44389</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -596,16 +704,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2">
-        <v>44388</v>
+        <v>44389</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -613,16 +721,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2">
-        <v>44388</v>
+        <v>44389</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -630,16 +738,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2">
-        <v>44387</v>
+        <v>44388</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -647,16 +755,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C8" s="2">
-        <v>44386</v>
+        <v>44388</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -664,16 +772,16 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C9" s="2">
-        <v>44385</v>
+        <v>44387</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -681,13 +789,13 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2">
-        <v>44385</v>
+        <v>44386</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -695,13 +803,171 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C11" s="2">
         <v>44385</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>34</v>
+        <v>54</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2">
+        <v>44385</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="2">
+        <v>44385</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2">
+        <v>44385</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="2">
+        <v>44384</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="2">
+        <v>44384</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="2">
+        <v>44384</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="2">
+        <v>44383</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="2">
+        <v>44383</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="2">
+        <v>44383</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="2">
+        <v>44382</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -716,6 +982,16 @@
     <hyperlink ref="D9" r:id="rId8"/>
     <hyperlink ref="D10" r:id="rId9"/>
     <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="D12" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId12"/>
+    <hyperlink ref="D14" r:id="rId13"/>
+    <hyperlink ref="D15" r:id="rId14"/>
+    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D17" r:id="rId16"/>
+    <hyperlink ref="D18" r:id="rId17"/>
+    <hyperlink ref="D19" r:id="rId18"/>
+    <hyperlink ref="D20" r:id="rId19"/>
+    <hyperlink ref="D21" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20210715
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Press Title</t>
   </si>
@@ -31,6 +31,21 @@
     <t>Page Content</t>
   </si>
   <si>
+    <t>153萬劑AstraZeneca疫苗及35萬劑Moderna疫苗將於今(15)日下午抵臺</t>
+  </si>
+  <si>
+    <t>新增18例COVID-19確定病例，分別為14例本土及4例境外移入</t>
+  </si>
+  <si>
+    <t>社區式服務之衛生福利機構可依照相關防疫管理指引，逐步恢復提供服務</t>
+  </si>
+  <si>
+    <t>新增27例COVID-19確定病例，分別為17例本土及10例境外移入</t>
+  </si>
+  <si>
+    <t>7月13日全國防疫會議後記者會報告</t>
+  </si>
+  <si>
     <t>新增29例COVID-19確定病例，分別為28例本土及1例境外移入</t>
   </si>
   <si>
@@ -46,49 +61,19 @@
     <t>自7月13日起恢復移工轉換雇主，雇主需於承接日前3日內安排移工檢驗PCR</t>
   </si>
   <si>
-    <t>籲請50歲(含)以上及18歲(含)以上第9類對象至COVID-19公費疫苗預約平臺登記意願  7月13日起陸續簡訊通知進行預約</t>
-  </si>
-  <si>
-    <t>新增31例COVID-19確定病例，分別為28例本土及3例境外移入</t>
-  </si>
-  <si>
-    <t>新增33例COVID-19確定病例，分別為31例本土及2例境外移入</t>
-  </si>
-  <si>
-    <t>新增36例COVID-19確定病例，分別為32例本土及4例境外移入</t>
-  </si>
-  <si>
-    <t>即日起開放全國第9及第10類對象意願登記</t>
-  </si>
-  <si>
-    <t>新增21例COVID-19確定病例，分別為18例本土及3例境外移入</t>
-  </si>
-  <si>
-    <t>針對媒體報導「指揮中心設局召開記者會」 指揮中心澄清並非事實</t>
-  </si>
-  <si>
-    <t>指揮中心延長全國疫情警戒第三級至7月26日止，嚴守社區防線，並自7月13日起適度鬆綁部分措施</t>
-  </si>
-  <si>
-    <t>指揮中心訂購第二批AZ疫苗62.6萬劑將於今(7)日下午抵臺</t>
-  </si>
-  <si>
-    <t>新增40例COVID-19確定病例，分別為39例本土及1例境外移入</t>
-  </si>
-  <si>
-    <t>網傳COVID-19疫苗施打登記系統異常為不實訊息 全國第9、10類皆可登記且紀錄不會被消除</t>
-  </si>
-  <si>
-    <t>新增29例COVID-19確定病例，分別為27例本土及2例境外移入</t>
-  </si>
-  <si>
-    <t>日本政府提供113萬劑AstraZeneca COVID-19疫苗將於7月8日下午抵臺</t>
-  </si>
-  <si>
-    <t>7月6日全國防疫會議後記者會報告</t>
-  </si>
-  <si>
-    <t>報載「疾病管制署造冊人數，超過編制內人數」 指揮中心說明：人員皆符合規定 以利防疫運作</t>
+    <t>/Bulletin/Detail/TRxFQmh7DNXlnYJdF8qV-A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Ppvh82lbGAf4mdyYY3JanQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/djglefBeFAgAOPL4Kq7-0A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/yZAmavXm44dCHkOMtcPprQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/zOQiiCl-yK8YpiAj15rDNA?typeid=9</t>
   </si>
   <si>
     <t>/Bulletin/Detail/mdt2oCvvps_-TB8TSliKag?typeid=9</t>
@@ -106,49 +91,19 @@
     <t>/Bulletin/Detail/3UJq0hJLq-ru0x_ktDM0tg?typeid=9</t>
   </si>
   <si>
-    <t>/Bulletin/Detail/LFEwMGAQQaE-q0wQ6ioHkQ?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/IWGDujzOX0GnYxtf2TCw5Q?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/1dFCXuBsiBFoOW0i9YDK9g?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/RlZy77CwVu9UhVlsIbpnVg?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/-ZC75bJni8eECGyL4uEuYA?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/h6gxof3idm6vTzGCwC7qJw?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/65J6c1wTSqx-68NNaCRU5g?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/aiGegg4ncYmMP9dTx4W_Zw?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/BlxZvHJU1w5vlVvV3EqlXg?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/2Rt1n0uftGTcpzceVxt5Zg?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/o2v7FN9aRKyxQMLbSEh6Sg?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/UDshrp3kzpPt0FBWObobWQ?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/FS-2y4B6C2TqLutsQbWlzQ?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/eW2VeHdKNhOsJIjrzEIQlA?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/PrfZ05Bfggkz1sUAAWohbg?typeid=9</t>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/TRxFQmh7DNXlnYJdF8qV-A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Ppvh82lbGAf4mdyYY3JanQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/djglefBeFAgAOPL4Kq7-0A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/yZAmavXm44dCHkOMtcPprQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/zOQiiCl-yK8YpiAj15rDNA?typeid=9</t>
   </si>
   <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/mdt2oCvvps_-TB8TSliKag?typeid=9</t>
@@ -166,49 +121,19 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/3UJq0hJLq-ru0x_ktDM0tg?typeid=9</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/LFEwMGAQQaE-q0wQ6ioHkQ?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/IWGDujzOX0GnYxtf2TCw5Q?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/1dFCXuBsiBFoOW0i9YDK9g?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/RlZy77CwVu9UhVlsIbpnVg?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/-ZC75bJni8eECGyL4uEuYA?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/h6gxof3idm6vTzGCwC7qJw?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/65J6c1wTSqx-68NNaCRU5g?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/aiGegg4ncYmMP9dTx4W_Zw?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/BlxZvHJU1w5vlVvV3EqlXg?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/2Rt1n0uftGTcpzceVxt5Zg?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/o2v7FN9aRKyxQMLbSEh6Sg?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/UDshrp3kzpPt0FBWObobWQ?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/FS-2y4B6C2TqLutsQbWlzQ?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/eW2VeHdKNhOsJIjrzEIQlA?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/PrfZ05Bfggkz1sUAAWohbg?typeid=9</t>
+    <t>發佈日期：2021-07-15\$\@\$中央流行疫情指揮中心今(15)日表示，日本政府提供第三批的97萬劑AstraZeneca疫苗及我國自行採購的第三批56萬劑AstraZeneca疫苗與第四批35萬劑Moderna疫苗將於今日下午陸續運抵桃園國際機場，待完成通關程序後，將直接運送至指定冷儲物流中心進行後續檢驗封縅作業，再提供COVID-19疫苗接種計畫所列實施對象進行接種。\$\@\$指揮中心說明，日本提供我國AstraZeneca疫苗分別為6月4日124萬劑、7月6日113萬劑與本批97萬劑，共334萬劑；我國與供應商(阿斯特捷利康公司)採購AstraZeneca疫苗分別為3月3日11.7萬劑、7月7日62.6萬劑與本批56萬劑，共130.03萬劑到貨。另，我國與Moderna供應商採購部分分別為5月28日15萬劑、6月18日24萬劑、6月30日41萬劑與本批35萬劑，共115萬劑。\$\@\$指揮中心再次感謝日本政府伸出援手提供第三批COVID-19疫苗，加上我國自行採購之AstraZeneca疫苗與Moderna疫苗陸續到貨，將有助提升我國疫苗覆蓋率。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-15\$\@\$中央流行疫情指揮中心今(15)日公布國內新增18例COVID-19確定病例，分別為14例本土及4例境外移入；另確診個案中新增6例死亡。\$\@\$指揮中心表示，今日新增之14例本土病例(其中7例為居家隔離期間或期滿檢驗陽性者)，為8例男性、6例女性，年齡介於未滿10歲至60多歲，發病日介於今(2021)年7月7日至7月14日。個案分布以臺北市9例為最多，其次為桃園市3例、新北市2例；其中11例為已知感染源、3例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增6例死亡個案，為1例男性、5例女性，年齡介於60多歲至80多歲，發病日介於5月15日至6月29日，確診日介於5月26日至6月30日，死亡日介於7月6日至7月13日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月13日累計公布14,103位確診個案中，已有12,083人解除隔離，解隔離人數達確診人數85.7%。\$\@\$指揮中心表示，今日新增4例境外移入個案中，案15437為阿富汗籍40多歲男性，7月1日自阿富汗來臺工作，持有搭機前3日內檢驗陰性報告，入境後至防疫旅館居家檢疫，7月13日檢疫期滿前採檢，於今日確診；個案在臺期間並無症狀，且檢疫期間未與他人接觸，故無匡列接觸者。案15446、案15447均為印尼籍20多歲男性漁工，受雇於同一公司，5月12日搭乘同班機自印尼來臺，皆持有搭機前3日內檢驗陰性報告，入境後均至防疫旅館完成居家檢疫並持續隔離至7月12日，7月13日由公司安排自費採檢，皆於今日確診；2人在臺期間並無症狀且無外出，已匡列接觸者4人，因有適當防護，均列自我健康監測。案15452為荷蘭籍40多歲男性，7月13日自阿拉伯聯合大公國(杜拜)來臺工作，持有搭機前3日內檢驗陰性報告，入境時在機場採檢後至防疫旅館檢疫，於今日確診；個案在臺期間並無症狀，相關接觸者匡列中。\$\@\$指揮中心統計，截至目前國內累計1,707,362例新型冠狀病毒肺炎相關通報(含1,690,141例排除)，其中15,346例確診，分別為1,218例境外移入，14,075例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計106例移除為空號。2020年起累計759例COVID-19死亡病例，其中751例本土，個案居住縣市分布為新北市377例、臺北市288例、基隆市26例、桃園市22例、彰化縣13例、新竹縣10例、臺中市4例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月15日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-14\$\@\$中央流行疫情指揮中心今(14)日表示，COVID-19疫情三級警戒期間，為降低失能者及身心障礙者群聚及傳染風險，社區式機構均暫停提供服務。現因應國內疫情趨緩，指揮中心宣布社區式機構可在工作人員疫苗施打率達8成且做好防疫整備工作的狀態下，適度鬆綁，逐步恢復提供服務。\$\@\$指揮中心說明，為確保服務對象健康，衛生福利部特訂定「衛生福利機構(社區型)因應COVID-19防疫管理指引」，針對「服務條件」、「自主防疫管理措施」、「具有COVID-19感染風險者之應變措施及發生確診病例應變處置」等管理事項，提供社區式服務機構依循辦理，地方政府應輔導轄內機構依本指引提供服務，並填具檢核表報地方政府備查，在完備防疫工作的前提下逐步恢復提供服務。\$\@\$本指引適用提供社區式服務之衛生福利機構，包括：社區式服務類長期照顧機構(日間照顧、小規模多機能)、附設於住宿機構之日間照顧服務、身心障礙日間型服務(含社區日間作業設施、社區式日間照顧、日間服務機構)、精神復健機構(日間型)、早期療育機構。本指引重點包括：\$\@\$一、服務條件\$\@\$(一)機構提供服務條件：\$\@\$1.整體工作人員疫苗施打率達8成，方可提供服務。\$\@\$2.未接種疫苗、接種第一劑疫苗未滿14日者，服務前應自費提供3日內SARS-CoV-2抗原快篩(以下簡稱抗原快篩)陰性證明，於三級警戒期間須配合每週自費提供抗原快篩陰性證明。\$\@\$(二)服務對象接受服務條件(未成年者不適用)：\$\@\$1.建議服務對象接種第一劑疫苗滿14日後，再前往接受服務。\$\@\$2.未接種疫苗、接種第一劑疫苗未滿14日者，接受服務前應自費提供3日內抗原快篩陰性證明或解除隔離證明，於三級警戒期間須配合每週自費提供抗原快篩陰性證明。\$\@\$二、自主防疫管理措施：\$\@\$(一)工作人員及服務對象之健康管理部分，若為確診、居家檢疫、居家隔離、自主健康管理、抗原快篩陽性者均不可提供或使用服務。\$\@\$(二)規劃服務動線、分區空間及隔離空間，建立分艙分流及分組活動、用餐機制。\$\@\$(三)交通服務管理，每車以10人(含司機)為限，車內禁止用餐、飲水。\$\@\$(四)加強環境(含交通接送車輛)清潔消毒，每日至少2次。\$\@\$三、具有COVID-19感染風險者之應變措施及發生確診病例應變處置：\$\@\$(一)發現疑似病例，機構應於24小時內通報，疑似病例應各自於隔離空間等候就醫或返家，且不得搭乘大眾交通工具。\$\@\$(二)任1位工作人員或服務對象為確定病例時，應暫停服務且立即通報地方主管機關，機構應進行相關人員造冊，並向該等人員宣導請其確實配合疫調。\$\@\$(三)立即就已知資訊先通知確定病例及可能與其有接觸之人員，等待衛生單位調查與聯繫。\$\@\$另家庭托顧服務部分，因照顧規模較小，且工作人員及服務對象皆屬公費疫苗第五類施打對象，較不易發生大規模群聚感染情形；雖不在指引適用範圍，但仍應在家庭托顧員完成疫苗第一劑接種且滿14日的前提下，參考社區式服務防疫管理指引加強人員健康監測、維持社交距離、增加環境清潔消毒次數、建立疑似個案通報轉送及確診病例應變處置機制，落實防疫規範下恢復營運。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-14\$\@\$中央流行疫情指揮中心今(14)日公布國內新增27例COVID-19確定病例，分別為17例本土及10例境外移入；另確診個案中新增6例死亡。\$\@\$指揮中心表示，今日新增之17例本土病例(其中9例為居家隔離期間或期滿檢驗陽性者)，為11例男性、6例女性，年齡介於未滿10歲至80多歲，發病日介於今(2021)年7月7日至7月13日。個案分布以臺北市10例為最多，其次為桃園市3例、新北市及臺中市各2例；其中10例為已知感染源、3例關聯不明、4例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增6例死亡個案，為5例男性、1例女性，年齡介於50多歲至80多歲，發病日介於5月15日至7月3日，確診日介於5月19日至7月5日，死亡日介於7月10日至7月12日；詳如新聞稿附件1。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月12日累計公布14,074位確診個案中，已有11,964人解除隔離，解隔離人數達確診人數85.0%。\$\@\$指揮中心表示，今日新增10例境外移入個案，為9例男性、1例女性，年齡介於10多歲至70多歲，分別自緬甸(6例，為同一班機乘客)、英國、日本、印尼及茅利塔尼亞入境，均持有搭機前3日內檢驗陰性報告，入境日介於6月30日至7月11日；詳如新聞稿附件2。\$\@\$指揮中心統計，截至目前國內累計1,686,311例新型冠狀病毒肺炎相關通報(含1,669,801例排除)，其中15,328例確診，分別為1,214例境外移入，14,061例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；新增1例空號病例(案15282)，共累計106例移除為空號。2020年起累計753例COVID-19死亡病例，其中745例本土，個案居住縣市分布為新北市374例、臺北市287例、基隆市25例、桃園市21例、彰化縣13例、新竹縣10例、臺中市4例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月14日新增死亡COVID-19確診個案表.pdf\$\@\$7月14日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-13\$\@\$中央流行疫情指揮中心表示，今(13)日上午與各縣市政府召開的「全國防疫會議」，決議如下：\$\@\$一、國內疫情現況及評估\$\@\$1.自實施全國加強三級警戒等相關管制措施下，Rt值已逐步下降，疫情持續趨緩，本週開始進行部分管制措施鬆綁，請各地方政府密切注意後續效應、及時應處。另全國三級警戒將延長至7月26日，考量各項防疫措施可能對民眾生活經濟、心理健康造成壓力，建議各地方政府進一步規劃相關關懷及配套方案，以舒緩民眾身心壓力。\$\@\$2.境外移入病例隨國外疫情上升有增加趨勢外，入境全面篩檢亦有陸續發現變異株相關個案，其中不乏病毒量高之病例，建議各地方政府持續加強疫情監控；雙北近期發生家庭群聚及職場群聚事件，仍請雙北地方政府除持續考量民眾就醫可近性設置社區篩檢站外，亦強化疫調作業，以利及早掌握病例，妥善應處。\$\@\$二、各直轄市、縣(市)政府「居家隔離/居家檢疫期滿前採檢政策」執行現況\$\@\$1.因應新型冠狀病毒Delta變異株於全球日益擴散且傳播力高，自今(2021)年6月22日起，確定病例之密切接觸者及自國外入境者，無論有無症狀，於居家隔離/檢疫之期滿前，須由各地方政府協助安排於隔離或檢疫期滿前1-3日(即接觸或入境迄日起第12-14日)內，搭乘防疫計程車前往醫療院所進行採檢，並確保於期滿前可取得檢驗報告。\$\@\$2.政策實施迄今，經期滿採檢計發現4名居家隔離、14名居家檢疫者採檢為確定病例，顯見於隔離或檢疫期滿前落實採檢措施，可避免COVID-19病毒進入社區，降低社區傳播風險，仍請各地方政府持續落實居家隔離/檢疫之期滿前採檢措施，共同守護社區防疫安全。\$\@\$三、衛生福利部為利疫情期間日照服務機構業務執行，業研議「衛生福利機構(社區型)因應COVID-19防疫管理指引」，相關重點請各地方政府協助檢視，近期將對外發布，重點包括：\$\@\$1.適用範圍：社區式服務類長期照顧機構(日間照顧、小規模多機能家庭托顧)、附設於一般護理之家、精神護理之家、老人福利機構、身心障礙福利機構之日間照顧服務、身心障礙日間型服務(社區日間作業設施、社區式日間照顧、家庭托顧、日間服務機構)、精神復健機構（日間型）、早期療育機構。\$\@\$2.服務條件\$\@\$(1)機構提供服務條件：\$\@\$整體工作人員疫苗施打率達8成，方可提供服務。\$\@\$未接種疫苗、接種第一劑疫苗未滿14日者，服務前應自費提供3日內SARS-CoV-2抗原快篩陰性證明或解除隔離證明，於三級警戒期間須配合每週自費提供抗原快篩陰性證明。\$\@\$地方政府應輔導轄內機構依本指引提供服務，機構須填具檢核表報地方政府備查，並配合後續抽核。\$\@\$(2)服務對象(含陪同照顧者)接受服務條件(未成年者不適用)：\$\@\$建議服務對象接種第一劑疫苗滿14日後，再前往接受服務。\$\@\$未接種疫苗、接種第一劑疫苗未滿14日者，接受服務前應自費提供3日內SARS-CoV-2抗原快篩陰性證明或解除隔離證明，於三級警戒期間須配合每週自費提供抗原快篩陰性證明。\$\@\$3.自主防疫管理措施：\$\@\$(1)工作人員及服務對象之健康管理部分，若為居家檢疫、居家隔離、自主健康管理者均不可提供或使用服務。\$\@\$(2)規劃服務動線、分區空間及隔離空間，建立分艙分流及活動分組進行機制。\$\@\$(3)交通服務管理，每車以10人（含司機）為限\$\@\$4.疑似確診應變措施：\$\@\$(1)任1位工作人員或服務對象為確定病例時，應暫停服務且立即通報地方社（衛）政主管機關，機構應進行相關人員造冊，並向該等人員宣導請其確實配合疫調。\$\@\$(2)立即就已知資訊先通知確定病例及可能與其有接觸之人員，等待衛生單位調查與聯繫。\$\@\$四、針對地方政府疫調資料調閱部分\$\@\$1.各地方政府如有確診軌跡調閱之需求，可透過各區管中心向指揮中心調閱，並將儘速於1天內提供。\$\@\$2.指揮中心已完成個案軌跡、熱區查詢、及簡訊實聯制疫調查詢功能，近日內提供各地方政府直接由線上進行查詢。另簡訊實聯制資料僅限制疫調查詢為主，相關查詢均有紀錄及配套機制，以確保使用範圍。\$\@\$3.以臺北市為例，近日向指揮中心調閱近1,000筆資料，除提供資料，指揮中心也提供線上查詢功能，並將和臺北市資訊局洽談介接與合作事宜。</t>
   </si>
   <si>
     <t>發佈日期：2021-07-13\$\@\$中央流行疫情指揮中心今(13)日公布國內新增29例COVID-19確定病例，分別為28例本土及1例境外移入；另確診個案中新增6例死亡。\$\@\$指揮中心表示，今日新增之28例本土病例(其中11例為居家隔離期間或期滿檢驗陽性者)，為18例男性、10例女性，年齡介於未滿10歲至80多歲，發病日介於今(2021)年6月26日至7月12日。個案分布以新北市15例為最多，其次為臺北市9例，桃園市2例，苗栗縣及臺中市各1例；其中16例為已知感染源、3例關聯不明、9例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增6例死亡個案，為4例男性、2例女性，年齡介於60多歲至80多歲，發病日介於5月12日至6月18日，確診日介於5月16日至6月19日，死亡日介於7月4日至7月12日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月11日累計公布14,050位確診個案中，已有11,901人解除隔離，解隔離人數達確診人數84.7%。\$\@\$指揮中心表示，今日新增1例境外移入個案(案15387)，為本國籍40多歲男性，6月30日自印尼入境，持搭機前3日內檢驗陰性報告，入境後至集中檢疫所檢疫並採檢，7月1日結果為陰性；7月8日出現輕微發燒與肌肉痠痛等症狀，7月11日仍未緩解，由衛生單位安排採檢，於今日確診。個案檢疫期間無接觸他人，同機旅客均已入住集中檢疫所，故無匡列接觸者。\$\@\$指揮中心統計，截至目前國內累計1,661,153例新型冠狀病毒肺炎相關通報(含1,644,686例排除)，其中15,302例確診，分別為1,204例境外移入，14,045例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；確診個案中，累計105例移除為空號。2020年起累計747例COVID-19死亡病例，其中739例本土，個案居住縣市分布為新北市370例、臺北市286例、基隆市25例、桃園市21例、彰化縣13例、新竹縣10例、臺中市4例、宜蘭縣、苗栗縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月13日新增死亡COVID-19確診個案表.pdf</t>
@@ -221,36 +146,6 @@
   </si>
   <si>
     <t>發佈日期：2021-07-12\$\@\$中央流行疫情指揮中心今(12)日公布國內新增24例COVID-19確定病例，分別為23例本土及1例境外移入；另確診個案中新增1例死亡。\$\@\$指揮中心表示，今日新增之23例本土病例(其中9例為居家隔離期間或期滿檢驗陽性者)，為13例男性、10例女性，年齡介於未滿10歲至90多歲，發病日介於今(2021)年6月20日至7月11日。個案分布以新北市10例為最多，其次為臺北市9例，基隆市、桃園市、新竹市及臺中市各1例；其中17例為已知感染源、4例關聯不明、2例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增1例死亡個案(案2598)，為60多歲男性，具慢性病史及其他確診者接觸史；個案於5月11日出現發燒等症狀，5月19日就醫採檢，5月20日確診並住院治療，6月11日解除隔離並出院。7月10日因其他原因死亡。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月10日累計公布14,019位確診個案中，已有11,850人解除隔離，解隔離人數達確診人數84.5%。\$\@\$指揮中心表示，今日新增1例境外移入個案(案15370)，為克羅埃西亞籍未滿10歲女童，6月28日自瑞士入境，持搭機前3日內檢驗陰性報告，入境後至防疫旅館檢疫，7月10日進行檢疫期滿前採檢，於今日確診(Ct值33)。個案在臺期間並無症狀，相關接觸者匡列中。\$\@\$指揮中心統計，截至目前國內累計1,639,921例新型冠狀病毒肺炎相關通報(含1,622,834例排除)，其中15,273例確診，分別為1,203例境外移入，14,017例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；確診個案中，累計105例移除為空號。自2020年起累計741例COVID-19死亡病例，其中733例本土，個案居住縣市分布為新北市369例、臺北市283例、基隆市25例、桃園市21例、彰化縣12例、新竹縣9例、臺中市4例、宜蘭縣、苗栗縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-12\$\@\$中央流行疫情指揮中心今(12)日表示，本土確診案例自今(2021)年7月2日起已連續低於50人，為兼顧國內產業用人需求及移工工作權益，爰自7月13日起恢復移工轉換雇主或工作。至於移工調派及工作延伸，考量移工流動性較高，仍暫緩解封，未來將視疫情再行檢討。\$\@\$指揮中心說明，7月1日已公佈優先恢復家庭類移工轉換至家庭類雇主，新雇主需為移工安排檢驗PCR。近期評估國內整體疫情及產業發展需要，將自7月13日起恢復家庭類以外類別之移工辦理轉換雇主，新雇主接續聘僱(含期滿轉換)移工應辦理以下事項：\$\@\$一、安排移工核酸檢驗（下稱PCR）：承接移工之新雇主應於接續聘僱日（含期滿轉換）前3日內安排移工檢驗PCR。但工作所在地之醫療院所假日期間未提供檢驗服務或檢驗能量已額滿者，得例外延後至接續聘僱日起3日內檢驗PCR。等待檢驗PCR結果期間，新雇主應安排移工1人1室，落實防疫措施，檢驗費用應由新雇主支付。\$\@\$二、雇主應依指引辦理防疫措施：倘若接續聘僱移工檢測PCR確診時，新雇主應負雇主責任，並依勞動部「因應嚴重特殊傳染性肺炎雇主聘僱移工指引：移工工作、生活及外出管理注意事項」(下稱雇主指引)，配合衛生單位安排就醫或送集中檢疫所隔離治療，並依確診個案處置及解除隔離治療條件續處。倘若接續聘僱移工檢測PCR陰性，新雇主應依雇主指引，每日進行移工健康監測及記錄移工出入足跡。\$\@\$指揮中心進一步表示，新雇主接續聘僱(含期滿轉換)移工，如未於上開規定期限內安排移工檢驗PCR，或於等待PCR檢驗結果期間，未落實移工1人1室，將依就業服務法規定，處新臺幣6萬至30萬元罰鍰及不予核發接續聘僱許可。另雇主如委託仲介公司辦理移工生活照顧，因仲介公司未善盡受任事務，違反防疫措施，將依仲介公司違反就業服務法規定，處新臺幣6萬元以上至30萬元以下罰鍰。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-11\$\@\$中央流行疫情指揮中心今(11)日表示，為順利推動我國COVID-19疫苗接種作業，自即日起全國50歲(含)以上及18歲(含)以上第9類具有易導致嚴重疾病之高風險疾病者、罕見疾病及重大傷病者均可於「疫苗施打意願登記與預約系統」（ https://1922.gov.tw/ ）進行意願登記，相關說明如下：\$\@\$一、意願登記時間：即日起至7月12日17時，並同步進行第一輪結算。\$\@\$二、簡訊通知時間：7月13日至7月15日將陸續以簡訊通知符合資格的民眾；收到簡訊者，才能進行預約。\$\@\$三、最快將於7月16日進行接種，未來三週均為AZ疫苗。\$\@\$四、為協助不便使用「COVID-19疫苗施打意願登記與預約系統」的民眾登記意願，請地方政府設置因地制宜的服務專線或指定人員，協助不便使用系統的民眾進行意願登記。\$\@\$指揮中心提醒，「COVID-19疫苗施打意願登記與預約系統」須先完成意願登記後，才能在接到通知後進行預約。系統平臺會按疫苗分配情形、參照民眾所登記的意願，通知符合預約資格的民眾，收到簡訊通知者即可進行下一步預約接種。尚未收到簡訊的民眾，會於後續符合預約資格後，收到簡訊通知，所有資料皆會完整保存，請民眾放心。\$\@\$指揮中心強調，「COVID-19疫苗施打意願登記與預約系統」是為建立讓大量疫苗接種能依序穩定有效推行的機制，中央與地方腳步一致，加強疫苗接種推動，提升群體保護力，維護國人健康。\$\@\$備註：\$\@\$1. 第9類對象為18-64歲具有易導致嚴重疾病之高風險疾病者、罕見疾病及重大傷病者。\$\@\$(1) 高風險疾病者定義： https://reurl.cc/R02Qx6\$\@\$(2) 罕見疾病定義： https://reurl.cc/Nr2E36\$\@\$(3) 重大傷病者請依健保卡註記或重大傷病卡為主\$\@\$2. 第10類對象為50-64歲成人。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-11\$\@\$中央流行疫情指揮中心今(11)日公布國內新增31例COVID-19確定病例，分別為28例本土及3例境外移入；另確診個案中新增4例死亡。\$\@\$指揮中心表示，今日新增之28例本土病例(其中10例為居家隔離期間或期滿檢驗陽性者)，為15例男性、13例女性，年齡介於未滿5歲至90多歲，發病日介於今(2021)年6月26日至7月10日。個案分布以新北市12例為最多，其次為臺北市11例、桃園市2例，新竹縣、彰化縣及臺中市各1例；其中15例為已知感染源、9例關聯不明、4例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增4例死亡個案，為2例男性、2例女性，年齡介於40多歲至70多歲，發病日介於5月22日至6月22日，確診日介於5月25日至7月6日，死亡日介於7月7日至7月9日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月9日累計公布13,986位確診個案中，已有11,802人解除隔離，解隔離人數達確診人數84.4%。\$\@\$指揮中心表示，今日新增3例境外移入個案中，案15342為本國籍30多歲男性，7月8日自沙烏地阿拉伯返臺，持有搭機前3日內檢驗陰性報告，入境後在機場採檢，並入住防疫旅館，於今日確診；個案在臺期間並無症狀，相關接觸者匡列中。案15351為菲律賓籍30多歲船員，5月17日自菲律賓來臺工作，持有搭機前3日內檢驗陰性報告，入境後至集中檢疫所檢疫，檢疫期滿前採檢結果為陰性即登船出海工作，7月10日返臺並採檢，於今日確診；個案出海工作及在臺期間並無症狀，相關接觸者匡列中。案15353為本國籍40多歲男性，7月10日自印尼返臺，持有搭機前3日內檢驗陰性報告，入境後在機場採檢，於今日確診；個案7月11日出現發燒症狀，已於醫院隔離治療，相關接觸者匡列中。\$\@\$指揮中心統計，截至目前國內累計1,625,351例新型冠狀病毒肺炎相關通報(含1,608,702例排除)，其中15,249例確診，分別為1,202例境外移入，13,994例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計105例移除為空號。自2020年起累計740例COVID-19死亡病例，其中732例本土，個案居住縣市分布為新北市368例、臺北市283例、基隆市25例、桃園市21例、彰化縣12例、新竹縣9例、臺中市4例、宜蘭縣、苗栗縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月11日新增死亡COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-10\$\@\$中央流行疫情指揮中心今(10)日公布國內新增33例COVID-19確定病例，分別為31例本土及2例境外移入；另確診個案中新增6例死亡。\$\@\$指揮中心表示，今日新增之31例本土病例(其中19例為居家隔離期間或期滿檢驗陽性者)，為17例男性、14例女性，年齡介於10多歲至70多歲，發病日介於今(2021)年6月22日至7月9日。個案分布以臺北市及新北市各13例最多，其次為桃園市4例，基隆市1例；其中21例為已知感染源、2例關聯不明、8例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增6例死亡個案，為2例男性、4例女性，年齡介於30多歲至80多歲，發病日介於6月3日至6月24日，確診日介於6月4日至6月25日，死亡日介於7月6日至7月8日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月8日累計公布13,950位確診個案中，已有11,698人解除隔離，解隔離人數達確診人數83.9%。\$\@\$指揮中心表示，今日新增2例境外移入中，案15299為本國籍30多歲女性，6月25日自義大利入境，持搭機前3日內檢驗陰性報告，入境後至自宅居家檢疫，7月8日進行期滿前採檢，於今日確診，個案在臺期間並無症狀，檢疫期間無接觸他人，故無匡列接觸者。案15319為本國籍20多歲男性，6月26日自比利時入境，持搭機前3日內檢驗陰性報告，入境後於自宅居家檢疫，7月8日進行期滿前採檢，於今日確診，個案在臺期間並無症狀，檢疫期間無接觸他人，故無匡列接觸者。\$\@\$指揮中心統計，截至目前國內累計1,606,389例新型冠狀病毒肺炎相關通報(含1,589,769例排除)，其中15,218例確診，分別為1,199例境外移入，13,966例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；個案中累計105例移除為空號。自2020年起累計736例COVID-19死亡病例，其中728例本土，個案居住縣市分布為新北市368例、臺北市279例、基隆市25例、桃園市21例、彰化縣12例、新竹縣9例、臺中市4例、宜蘭縣、苗栗縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月10日新增死亡COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-08\$\@\$中央流行疫情指揮中心今(8)日表示，為順利推動我國COVID-19疫苗接種作業，指揮中心於昨(7)日下午邀集各地方政府代表共同召開「疫苗施打意願登記與預約系統」討論會議，達成共識及決議如下：\$\@\$一、指揮中心將自即日起，開放全國第9類及第10類對象意願登記，並正式啟用「COVID-19疫苗施打意願登記與預約系統」，請符合資格民眾可先行意願登記：\$\@\$(一) 意願登記：即日起至7月12日下午5時止。\$\@\$(二) 為保障65歲以上長者疫苗接種權益，若希望使用該系統進行意願登記，請依時程辦理。\$\@\$二、為協助不便使用「COVID-19疫苗施打意願登記與預約系統」之民眾進行意願登記，請地方政府設置因地制宜之服務專線或指定人員，協助不便使用系統民眾進行意願登記。\$\@\$指揮中心提醒，「COVID-19疫苗施打意願登記與預約系統」須先完成意願登記後，才能在接到通知後進行預約。系統平臺會按疫苗分配情形參照民眾所登記之意願，通知符合預約資格的民眾，收到簡訊通知者即可進行下一步預約接種。尚未收到簡訊之民眾，會於後續符合預約資格後，收到簡訊通知，所有資料皆會完整保存，請民眾放心。指揮中心也強調，「COVID-19疫苗施打意願登記與預約系統」是為建立一個讓大量疫苗接種能依序穩定有效推行之機制，中央與地方腳步一致，加強疫苗接種推動，提升群體保護力，維護國人健康。\$\@\$備註:\$\@\$第9類對象為18-64歲具有易導致嚴重疾病之高風險疾病者、罕見疾病及重大傷病者。\$\@\$高風險疾病者定義： https://reurl.cc/R02Qx6\$\@\$罕見疾病定義： https://reurl.cc/Nr2E36\$\@\$重大傷病者請依健保卡註記或重大傷病卡為主\$\@\$第10類對象為50-64歲成人。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-08\$\@\$中央流行疫情指揮中心今(8)日公布國內新增21例COVID-19確定病例，分別為18例本土及3例境外移入；另確診個案中新增3例死亡。\$\@\$指揮中心表示，今日新增之18例本土病例(其中6例為居家隔離期間或期滿檢驗陽性者)，為8例男性、10例女性，年齡介於未滿5歲至60多歲，發病日介於今(2021)年7月1日至7月7日。個案分布以臺北市12例最多，其次為新北市6例；其中9例為已知感染源、9例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增3例死亡個案，為2例男性、1例女性，年齡介於60多歲至70多歲，發病日介於5月27日至6月14日，確診日介於5月28日至6月17日，死亡日介於7月5日至7月6日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月6日累計公布13,889位確診個案中，已有11,456人解除隔離，解隔離人數達確診人數82.5%。\$\@\$指揮中心表示，今日新增3例境外移入中，案15252為本國籍30多歲男性，6月23日自泰國返臺，持有搭機前3日內檢驗陰性報告，入境後至防疫旅館檢疫，7月6日檢疫期滿前採檢，於今日確診；個案在臺期間並無症狀，且檢疫期間未與他人接觸，故無匡列接觸者。案15253為印尼籍20多歲男性漁工，5月10日自印尼來臺，持有搭機前3日內檢驗陰性報告，入境後至集中檢疫所檢疫，5月23日檢疫期滿前採檢結果為陰性，7月7日因有離境需求再次採檢，於今日確診；個案在臺期間並無症狀，已匡列接觸者221人，其中60人列居家隔離，餘161人列自我健康監測。案15254為本國籍10多歲女性，7月6日自美國返臺，持有搭機前3日內檢驗陰性報告，入境時在機場採檢，於今日確診；個案在臺期間並無症狀，相關接觸者匡列中。\$\@\$指揮中心統計，截至目前國內累計1,541,974例新型冠狀病毒肺炎相關通報(含1,525,372例排除)，其中15,149例確診，分別為1,193例境外移入，13,903例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計105例移除為空號。自2020年起累計 718例COVID-19死亡病例，其中710例本土，個案居住縣市分布為新北市363例、臺北市272例、基隆市24例、桃園市20例、彰化縣12例、新竹縣7例、臺中市4例、宜蘭縣及花蓮縣各2例，苗栗縣、臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月8日新增死亡COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-08\$\@\$針對媒體報導「指揮中心設局召開記者會」，中央流行疫情指揮中心今(8)日說明如下：\$\@\$一、針對臺北市環南市場進行大規模PCR篩檢且41人呈現陽性，顯示有群聚感染疫情，指揮中心於7月2日11:30前往環南市場現場召開記者會，並宣布與臺北市政府共同成立聯合前進指揮所。\$\@\$二、當日陳時中指揮官於9:45致電黃珊珊副市長，黃副市長將電話轉交給柯文哲市長，陳指揮官與柯市長直接通話，雙方對成立聯合前進指揮所達成共識，並在環南市場現場召開記者會。\$\@\$三、當日農委會陳吉仲主委於10:00多左右，親自致電二通予臺北市黃副市長，並於第二通電話中明確告知黃副市長，陳指揮官、經濟部王美花部長及農委會陳吉仲主委將至環南市場召開記者會，並邀請黃副市長出席，黃副市長表示柯市長也會出席。\$\@\$四、指揮中心表示，當日均依照指揮中心記者會程序，發布採訪通知；指揮中心幕僚抵達環南市場後，亦與臺北市市場處高副處長確認記者會場地、流程及雙方出席人員，同時與現場媒體溝通說明記者會流程，及預定出席人員。\$\@\$五、當日11:01，臺北市府陳智菡發言人於臺北市府群組發布採訪通知，說明柯市長、黃副市長皆會出席記者會； 11:20柯市長、黃副市長抵達環南市場。\$\@\$六、指揮中心說明，為儘快有效控制疫情，召開記者會說明防疫作為及因應措施，以利相關市場攤商、工作人員及周邊住民了解需配合之事項，並無「以開會名義設局召開記者會」一事。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-08\$\@\$中央流行疫情指揮中心今(8)日表示，在國人共同努力配合下，國內疫情已在控制中，惟仍有部分感染事件發生，參酌世界各國管制作為及經驗，防疫措施鬆綁須逐步執行，才可穩定掌握疫情狀況，為確保國人健康，指揮中心經評估後決定，同步延長全國疫情警戒第三級至7月26日止，並自7月13日起適度鬆綁部分措施，說明如下：\$\@\$一、適度鬆綁措施：\$\@\$(一)    有條件鬆綁對象（地方政府得視防疫需要因時因地調整）：\$\@\$1.    戶外：國家公園、國家風景區、遊樂園區、休閒農場、森林遊樂區、植物園、文化園區、學校操場、駕訓班。\$\@\$2.    室內：美術館、博物館、電影院、表演場館(無觀眾)、社教機構、文化中心。\$\@\$3.    室內外運動場館(游泳池除外)、高爾夫球場。\$\@\$4.    餐飮場所(餐廳、傳統市場及夜市、百貨賣場 美食街、美食區等)符合指揮中心指引得內用。\$\@\$5.    國內小型旅行團(9人以下)、劇組拍攝。\$\@\$(二)    上述鬆綁須遵照通案性原則及主管機關指引：\$\@\$1.    實聯制、出入口管制、人流管控降載。\$\@\$2.    維持社交距離，除飮食外，全程戴口罩。\$\@\$3.    員工人員健康管理、確診事件即時應變。\$\@\$二、三級警戒延長仍須關閉之場所：\$\@\$(一)    休閒娛樂場所：\$\@\$歌廳、舞廳、夜總會、俱樂部、酒家、酒吧、酒店(廊)、錄影節目帶播映場所(MTV)、視聽歌唱場所(KTV)、理容院(觀光理髮、視聽理容)、指壓按摩場所、健身休閒中心(含提供指壓、三溫暖等設施之美容瘦身場所)、保齡球館、撞球場、室內螢幕式高爾夫練習場、遊藝場所、電子遊戲場、資訊休閒場所、休閒麻將館、自助選物販賣機營業場所、釣蝦場、桌遊場所及其他類似場所。\$\@\$(二)    教育學習場域：\$\@\$社區大學、樂齡學習中心、訓練班(駕訓班除外)、K書中心等其他類似場所。\$\@\$(三)    觀展觀賽場所：\$\@\$會展場館、游泳池等其他類似場所。\$\@\$指揮中心表示，鬆綁過程是疫情重要關鍵，籲請全國民眾持續落實遵循並積極配合三級警戒管制及鬆綁規定相關措施，與政府共同努力，嚴守社區防線。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-07\$\@\$網路謠傳「有1922回復，系統異常讓其他地區民眾預約登記、疾管署討論虛擬預約或取消方式處理、及正式預約開始要向1922確認」等資訊，中央流行疫情指揮中心今(7)日澄清，「COVID-19疫苗施打意願登記與預約系統」(1922.gov.tw)運作順暢並無異常，且已正式上線，並非虛擬預約，所有登記成功者皆已記錄在案，除非事後自行取消，否則已登記之紀錄並不會受到影響。前述相關網路訊息均非疾管署或1922防疫專線發布、回復，且內容多有不實，籲請民眾勿信、轉傳與散布。\$\@\$指揮中心說明，有關「COVID-19疫苗施打意願登記與預約系統」其設計目前為開放全國第9、10類對象民眾進行疫苗施打意願登記，故不限金馬澎地區登記意願；惟完成意願登記者，須符合當時公布開放預約之接種年齡及資格條件，系統平台會按疫苗分配情形以簡訊通知符合預約資格的民眾，收到簡訊通知者即可進行下一步預約接種。如有完成意願登記但不符合當時預約資格，則暫時不會收到預約接種簡訊且無法預約接種。而本次以離島金門、馬祖和澎湖先行試辦意願登記及預約接種，未來將再逐步開放到全國，截至今日8時，全國已有約148萬符合第9、10類接種對象完成意願登記，其中離島金門、馬祖及澎湖之意願登記人數約為4千5百人。\$\@\$指揮中心指出，目前全國1-8類對象已開放接種，符合該等對象資格者可依縣市政府規劃安排接種。昨日上線之「COVID-19疫苗施打意願登記與預約系統」，係為建立一個讓大量疫苗接種能依序穩定有效推行之機制，請符合第9、10類對象民眾先進行意願登記，再依簡訊通知，進行預約接種。\$\@\$指揮中心強調，網路謠傳「有1922回復，系統異常讓其他地區民眾預約登記、疾管署討論虛擬預約或取消方式處理、及正式預約開始要向1922確認」等資訊皆為不實訊息且均非發布自疾管署或1922防疫專線，籲請民眾勿信、轉傳與散布。 圖片 附件\$\@\$網傳COVID-19疫苗施打登記系統異常為不實訊息 全國第9、10類皆可登記且紀錄不會被消除.jpg</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-06\$\@\$中央流行疫情指揮中心今(6)日公布國內新增29例COVID-19確定病例，分別為27例本土及2例境外移入；另確診個案中新增17例死亡。\$\@\$指揮中心表示，今日新增之27例本土病例(其中15例為居家隔離期間或期滿檢驗陽性者)，為17例男性、10例女性，年齡介於未滿5歲至70多歲，發病日介於今(2021)年6月10日至7月5日。個案分布以臺北市14例最多，其次為新北市11例、屏東縣及彰化縣各1例；其中17例為已知感染源、10例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增17例死亡個案，為14位男性、3位女性，發病日介於5月16日至7月2日，確診日介於5月19日至7月5日，死亡日介於6月28日至7月5日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月4日累計公布13,831位確診個案中，已有11,180人解除隔離，解隔離人數達確診人數80.8%。\$\@\$指揮中心表示，今日新增境外移入個案中，案15180為本國籍10多歲男性，7月4日自美國入境，持有搭機前3日內檢驗陰性報告，入境時並無症狀，於機場採檢後至防疫旅館檢疫，7月5日出現嗅味覺異常等症狀，於今日確診，相關接觸者匡列中。案15185為本國籍30多歲男性，6月30日自印尼入境，持有搭機前3日內檢驗陰性報告，入境後至集中檢疫所檢疫並進行採檢，當日採檢結果為陰性；7月4日出現發燒、肌肉痠痛、流鼻水等症狀，7月5日由衛生單位採檢送驗，於今日確診，同班機旅客均已入境採檢並入住集中檢疫所。\$\@\$指揮中心統計，截至目前國內累計1,503,584例新型冠狀病毒肺炎相關通報(含1,487,019例排除)，其中15,088例確診，分別為1,189例境外移入，13,846例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另新增2例空號(案10180、案13124)，累計105例移除為空號。自2020年起累計706例COVID-19死亡病例，其中698例本土，個案居住縣市分布為新北市354例、臺北市269例、基隆市24例、桃園市20例、彰化縣12例、新竹縣7例、臺中市4例、宜蘭縣及花蓮縣各2例，苗栗縣、臺東縣、雲林縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月6日新增死亡COVID-19確診個案表.pdf</t>
   </si>
 </sst>
 </file>
@@ -625,7 +520,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -653,16 +548,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2">
+        <v>44392</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="2">
-        <v>44390</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -670,16 +565,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2">
+        <v>44392</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="2">
-        <v>44390</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -687,16 +582,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2">
+        <v>44391</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="2">
-        <v>44389</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -704,16 +599,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2">
+        <v>44391</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="2">
-        <v>44389</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -721,16 +616,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2">
+        <v>44390</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="2">
-        <v>44389</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -738,16 +633,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2">
+        <v>44390</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="2">
-        <v>44388</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -755,16 +650,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2">
+        <v>44390</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="2">
-        <v>44388</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -772,16 +667,16 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2">
+        <v>44389</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="2">
-        <v>44387</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -789,13 +684,16 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2">
+        <v>44389</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="2">
-        <v>44386</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>53</v>
+      <c r="E10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -803,171 +701,13 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2">
+        <v>44389</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="C11" s="2">
-        <v>44385</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="2">
-        <v>44385</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="2">
-        <v>44385</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="2">
-        <v>44385</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="2">
-        <v>44384</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="2">
-        <v>44384</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="2">
-        <v>44384</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="2">
-        <v>44383</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="2">
-        <v>44383</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="2">
-        <v>44383</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="2">
-        <v>44382</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -982,16 +722,6 @@
     <hyperlink ref="D9" r:id="rId8"/>
     <hyperlink ref="D10" r:id="rId9"/>
     <hyperlink ref="D11" r:id="rId10"/>
-    <hyperlink ref="D12" r:id="rId11"/>
-    <hyperlink ref="D13" r:id="rId12"/>
-    <hyperlink ref="D14" r:id="rId13"/>
-    <hyperlink ref="D15" r:id="rId14"/>
-    <hyperlink ref="D16" r:id="rId15"/>
-    <hyperlink ref="D17" r:id="rId16"/>
-    <hyperlink ref="D18" r:id="rId17"/>
-    <hyperlink ref="D19" r:id="rId18"/>
-    <hyperlink ref="D20" r:id="rId19"/>
-    <hyperlink ref="D21" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20210716
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Press Title</t>
   </si>
@@ -31,6 +31,21 @@
     <t>Page Content</t>
   </si>
   <si>
+    <t>近期城市汙水廠採驗結果皆為陰性，指揮中心將持續進行環境監測</t>
+  </si>
+  <si>
+    <t>新增32例COVID-19確定病例，分別為29例本土及3例境外移入</t>
+  </si>
+  <si>
+    <t>指揮中心持續監測全球Delta變異株流行情形，自7月18日零時起增列緬甸為「重點高風險國家」</t>
+  </si>
+  <si>
+    <t>COVID-19公費疫苗預約平臺第二輪預約接種自明(7/16)日開打，第三輪「意願登記」結算將延長至7月19日中午12時止</t>
+  </si>
+  <si>
+    <t>暴露後狂犬病免疫製劑接種適用對象，新增黃喉貂，並自本(110)年7月1日起適用</t>
+  </si>
+  <si>
     <t>153萬劑AstraZeneca疫苗及35萬劑Moderna疫苗將於今(15)日下午抵臺</t>
   </si>
   <si>
@@ -46,19 +61,19 @@
     <t>7月13日全國防疫會議後記者會報告</t>
   </si>
   <si>
-    <t>新增29例COVID-19確定病例，分別為28例本土及1例境外移入</t>
-  </si>
-  <si>
-    <t>COVID-19公費疫苗預約平臺  即日起開放18歲(含)以上民眾進行第三輪意願登記</t>
-  </si>
-  <si>
-    <t>為儘速提升第一劑COVID-19疫苗涵蓋率，第二劑Moderna疫苗接種間隔調整自第10週起接種</t>
-  </si>
-  <si>
-    <t>新增24例COVID-19確定病例，分別為23例本土及1例境外移入</t>
-  </si>
-  <si>
-    <t>自7月13日起恢復移工轉換雇主，雇主需於承接日前3日內安排移工檢驗PCR</t>
+    <t>/Bulletin/Detail/0_5hYtFaIW9kmfkkRHA0fQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/B34H9oWmz6AnDmYSsCIHHg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/kA2aOz-R6HIFy232juX3FQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/8J0zKvCwRhnEIxcDO93kog?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/qSj5Zk3qZf_2Om9XsxHj7A?typeid=9</t>
   </si>
   <si>
     <t>/Bulletin/Detail/TRxFQmh7DNXlnYJdF8qV-A?typeid=9</t>
@@ -76,19 +91,19 @@
     <t>/Bulletin/Detail/zOQiiCl-yK8YpiAj15rDNA?typeid=9</t>
   </si>
   <si>
-    <t>/Bulletin/Detail/mdt2oCvvps_-TB8TSliKag?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/RACDgdJ7AErNus7J2j37iw?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/vu8IYJ-y67cc4ZpemyPBTA?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/1FS11QWUMT5jcui6nxcIvw?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/3UJq0hJLq-ru0x_ktDM0tg?typeid=9</t>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/0_5hYtFaIW9kmfkkRHA0fQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/B34H9oWmz6AnDmYSsCIHHg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/kA2aOz-R6HIFy232juX3FQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/8J0zKvCwRhnEIxcDO93kog?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/qSj5Zk3qZf_2Om9XsxHj7A?typeid=9</t>
   </si>
   <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/TRxFQmh7DNXlnYJdF8qV-A?typeid=9</t>
@@ -106,22 +121,22 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/zOQiiCl-yK8YpiAj15rDNA?typeid=9</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/mdt2oCvvps_-TB8TSliKag?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/RACDgdJ7AErNus7J2j37iw?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/vu8IYJ-y67cc4ZpemyPBTA?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/1FS11QWUMT5jcui6nxcIvw?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/3UJq0hJLq-ru0x_ktDM0tg?typeid=9</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-15\$\@\$中央流行疫情指揮中心今(15)日表示，日本政府提供第三批的97萬劑AstraZeneca疫苗及我國自行採購的第三批56萬劑AstraZeneca疫苗與第四批35萬劑Moderna疫苗將於今日下午陸續運抵桃園國際機場，待完成通關程序後，將直接運送至指定冷儲物流中心進行後續檢驗封縅作業，再提供COVID-19疫苗接種計畫所列實施對象進行接種。\$\@\$指揮中心說明，日本提供我國AstraZeneca疫苗分別為6月4日124萬劑、7月6日113萬劑與本批97萬劑，共334萬劑；我國與供應商(阿斯特捷利康公司)採購AstraZeneca疫苗分別為3月3日11.7萬劑、7月7日62.6萬劑與本批56萬劑，共130.03萬劑到貨。另，我國與Moderna供應商採購部分分別為5月28日15萬劑、6月18日24萬劑、6月30日41萬劑與本批35萬劑，共115萬劑。\$\@\$指揮中心再次感謝日本政府伸出援手提供第三批COVID-19疫苗，加上我國自行採購之AstraZeneca疫苗與Moderna疫苗陸續到貨，將有助提升我國疫苗覆蓋率。</t>
+    <t>發佈日期：2021-07-16\$\@\$中央流行疫情指揮中心今(16)日表示，為配合世界衛生組織(WHO)推動的根除小兒麻痺病毒之環境監測調查計畫，且為防堵國際疫情威脅與國內疫苗預防接種政策的改變，疾病管制署自(2012)年7月起即建立環境監測系統，透過從污水處理系統收集而來的污水樣本，檢測一個群體中是否有來自未知病患的小兒麻痺病毒，用以評估環境中野生株及疫苗株小兒麻痺病毒的流通傳播。自去(2020)年1月起，因應COVID-19疫情，於前揭計畫下加驗SARS-CoV-2病毒。\$\@\$指揮中心說明，環境監測調查作業的監測頻率為每月2次，將採集汙水廠的汙水樣本，濃縮後進行核酸檢驗；疾管署持續監測採檢11處城市汙水匯流的汙水廠，目前僅於今(2021)年6月1日監測採檢2處驗出COVID-19陽性。惟截至目前為止(含6月中與7月初)，11處（包含前揭該2處）城市汙水廠之污水監測SARS-CoV-2病毒檢測結果皆為陰性。\$\@\$指揮中心強調，未來將持續監測全臺大都會共11間汙水廠，並視疫情狀況調整環境汙水SARS-CoV-2病毒監測作業。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-16\$\@\$中央流行疫情指揮中心今(16)日公布國內新增32例COVID-19確定病例，分別為29例本土及3例境外移入；另確診個案中新增4例死亡。\$\@\$指揮中心表示，今日新增之29例本土病例(其中7例為居家隔離期間或期滿檢驗陽性者)，為17例男性、12例女性，年齡介於未滿5歲至60多歲，發病日介於今(2021)年7月5日至7月15日。個案分布以臺北市14例為最多，其次為新北市11例、桃園市2例、宜蘭縣及彰化縣各1例；其中21例為已知感染源、4例關聯不明、4例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增4例死亡個案，均為男性，年齡介於60多歲至90多歲，發病日介於5月24日至6月16日，確診日介於5月26日至6月24日，死亡日介於7月9日至7月14日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月14日累計公布14,130位確診個案中，已有12,131人解除隔離，解隔離人數達確診人數85.9%。\$\@\$指揮中心表示，今日新增3例境外移入個案中，案15468為美國籍50多歲男性，7月2日自美國來臺工作，持有搭機前3日內檢驗陰性報告，入境後至防疫旅館居家檢疫，7月14日檢疫期滿前採檢，於今日確診；個案在臺期間並無症狀，且檢疫期間未與他人接觸，故無匡列接觸者。案15472為本國籍未滿10歲女童，7月2日自美國返臺，持有搭機前3日內檢驗陰性報告，入境後至防疫旅館居家檢疫，7月14日檢疫期滿前採檢，於今日確診；個案在臺期間並無症狀，已匡列接觸者2人，列居家隔離。案15480為菲律賓籍30多歲男性漁工，4月30日自菲律賓來臺，持有搭機前3日內檢驗陰性報告，入境後至防疫旅館居家檢疫，檢疫期滿與自主健康管理期滿採檢結果均為陰性，5月22日登船工作後未再下船，7月14日因有出海作業需求，由公司安排自費採檢，於今日確診；個案在臺期間並無症狀，已匡列接觸者18人，其中17人列居家隔離、1人列自我健康監測。\$\@\$指揮中心統計，截至目前國內累計1,727,787例新型冠狀病毒肺炎相關通報(含1,710,974例排除)，其中15,378例確診，分別為1,221例境外移入，14,104例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計106例移除為空號。2020年起累計763例COVID-19死亡病例，其中755例本土，個案居住縣市分布為新北市379例、臺北市289例、基隆市26例、桃園市23例、彰化縣13例、新竹縣10例、臺中市4例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月16日新增死亡COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-16\$\@\$中央流行疫情指揮中心今(16)日宣布，考量緬甸疫情現況及風險，於「重點高風險國家」增列緬甸。自7月18日零時起(抵臺時間)，自海港或空港入境我國人士，如過去14天有緬甸旅遊史(含轉機)者，入境後均應至集中檢疫所進行14天檢疫，且須配合於入住時與檢疫期滿分別進行PCR檢測，另檢疫期間第10至12天以「家用快篩」採檢一次；旅客不需支付集中檢疫所及採檢費用；此外，國籍航空公司機組員亦維持自「重點高風險國家」航線航班返臺後，應入住防疫旅宿或符合規定之公司宿舍檢疫14天，且檢疫期滿進行PCR檢測。\$\@\$指揮中心表示，緬甸近1個多月疫情再度遽升，近1週日增確診數由50例以下，上升至逾4,000例，新增確診及死亡數均續創新高，檢驗陽性率已逾30%；迄今累計逾20萬例確診病例，逾4千例死亡，致死率2%。此波疫情初期病例多來自鄰近印度邊境之實皆省(Sagaing)及欽邦(Chin)，爾後與印度接壤之多個社區陸續爆發疫情，並監測到Delta變異株。該國已於部分地區實施居家令，因醫療體系之篩檢量及檢測能力不足，實際疫情可能比官方公布更為嚴峻。\$\@\$指揮中心指出，現行「重點高風險國家」為巴西(Gamma巴西變異株)、印度、英國、秘魯、以色列、印尼、孟加拉及本次新增之緬甸(Delta印度變異株)等，共8國。\$\@\$指揮中心說明，邊境管制為防範COVID-19疫情之重要關鍵，指揮中心已全面提升入境人士檢疫措施、持續監測境外移入檢出變異株情形，同時籲請入境人士抵臺時應主動配合邊境檢疫措施，並依指揮中心規定之交通方式前往檢疫地點及配合後續防疫措施，落實全民共同抗疫，將疫情阻絕於境外。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-15\$\@\$中央流行疫情指揮中心今(15)日表示，「COVID-19疫苗施打意願登記與預約系統」第二輪共計約94.1萬人已完成預約接種，將自明(16)日起開始施打，請民眾攜帶健保卡，如為第二劑接種者，亦請攜帶接種紀錄卡，於預約時間準時至預約地點接種疫苗。如民眾錯過預約時段，可於當日告知現場人員，另擇同日之其他時段接種；如無法於預約當日接種，須等候下一輪簡訊通知後，再至系統重新預約接種。\$\@\$指揮中心指出，第三輪意願登記原訂於7月15日下午5時進行第三輪結算，將延長至7月19日中午12時進行第三輪結算，並自7月20日起陸續以簡訊通知符合資格的民眾進行預約接種；本輪可接種疫苗為AZ疫苗。\$\@\$指揮中心提醒，「COVID-19疫苗施打意願登記與預約系統」須先完成意願登記，才能在接到簡訊通知後進行預約。系統平臺會按疫苗分配情形、參照民眾登記之意願，通知符合預約資格的民眾，收到簡訊通知者才可進行下一步預約接種。尚未收到簡訊的民眾，會於後續符合預約資格後收到簡訊通知，所有資料皆會完整保存，請民眾放心。\$\@\$指揮中心強調，「COVID-19疫苗施打意願登記與預約系統」是為了建立大量疫苗接種能依序穩定有效推行的機制，中央與地方腳步一致，加強推動疫苗接種，提升群體保護力，守護國人健康。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-15\$\@\$疾病管制署今(15)日表示，因應行政院農業委員會動植物防疫檢疫局本(2021)年6月30日發布，國內檢出首例黃喉貂狂犬病陽性案例，為維護國內民眾健康及安全，降低感染風險，疾管署修訂「疑似狂犬病或麗沙病毒動物抓咬傷臨床處置指引」，調整暴露後預防接種對象，增列遭「黃喉貂」咬傷者，經評估傷口暴露等級為第2及第3類者，應接種暴露後狂犬病免疫球蛋白及疫苗，並自本年7月1日起適用。\$\@\$疾管署說明，國內每年均接獲數起食肉目野生動物抓咬傷民眾通報案件，今年迄今有8起，其中3件動物檢驗為狂犬病陽性，去（2020）年同期為11起，全年則有14起，其中5件檢驗為狂犬病陽性、4件陰性、5件未送驗，陽性案件分布範圍為南投縣3件，屏東縣、嘉義縣各1件。\$\@\$狂犬病是由狂犬病病毒引起的一種急性腦脊髓炎，狂犬病毒從已感染動物的唾液隨著抓、咬傷所造成之傷口進入人體，潛伏期約1至3個月，初期症狀有發熱、喉嚨痛、發冷、厭食、嘔吐、呼吸困難、咳嗽、頭痛或咬傷部位異樣感，數天後出現興奮及恐懼現象，然後麻痺、吞嚥困難，咽喉部痙攣，並引起恐水現象(又稱恐水症)，隨後會發生精神錯亂及抽搐等情況，如不採取醫療措施，患者常因呼吸麻痺導致死亡，致死率近100%，但如能在遭動物咬傷後及時就醫，並接受狂犬病暴露後預防接種，可以降低發病的風險。\$\@\$疾管署再次呼籲，民眾應避免接觸及捕捉野生動物，每年須帶家中犬、貓等寵物施打狂犬病疫苗；如不慎遭野生哺乳類動物抓咬傷，請以肥皂及大量清水沖洗傷口15分鐘，再以優碘或70%酒精消毒後，儘速前往就醫，經醫師評估如有感染狂犬病風險，應儘速接種免疫球蛋白，並依時程(接種第一劑當天為第0天、3、7及第14天)接種4劑人用狂犬病疫苗，降低發病風險。相關資訊請參閱疾管署全球資訊網(https://www.cdc.gov.tw)或撥打免費防疫專線1922(或0800-001922)洽詢。 圖片 附件\$\@\$鼬獾.jpg\$\@\$黃喉貂.jpg\$\@\$白鼻心.jpg\$\@\$疑似狂犬病或麗沙病毒感染動物抓咬傷臨床處置指引_0715.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-15\$\@\$中央流行疫情指揮中心今(15)日表示，日本政府提供第三批的97萬劑AstraZeneca疫苗及我國自行採購的第三批56萬劑AstraZeneca疫苗與第四批35萬劑Moderna疫苗將於今日下午陸續運抵桃園國際機場，待完成通關程序後，將直接運送至指定冷儲物流中心進行後續檢驗封緘作業，再提供COVID-19疫苗接種計畫所列實施對象進行接種。\$\@\$指揮中心說明，日本提供我國AstraZeneca疫苗分別為6月4日124萬劑、7月8日113萬劑與本批97萬劑，共334萬劑；我國與供應商(阿斯特捷利康公司)採購AstraZeneca疫苗分別為3月3日11.7萬劑、7月7日62.6萬劑與本批56萬劑，共130.3萬劑到貨。另，我國與Moderna供應商採購部分分別為5月28日15萬劑、6月18日24萬劑、6月30日41萬劑與本批35萬劑，共115萬劑。\$\@\$指揮中心再次感謝日本政府伸出援手提供第三批COVID-19疫苗，加上我國自行採購之AstraZeneca疫苗與Moderna疫苗陸續到貨，將有助提升我國疫苗覆蓋率。</t>
   </si>
   <si>
     <t>發佈日期：2021-07-15\$\@\$中央流行疫情指揮中心今(15)日公布國內新增18例COVID-19確定病例，分別為14例本土及4例境外移入；另確診個案中新增6例死亡。\$\@\$指揮中心表示，今日新增之14例本土病例(其中7例為居家隔離期間或期滿檢驗陽性者)，為8例男性、6例女性，年齡介於未滿10歲至60多歲，發病日介於今(2021)年7月7日至7月14日。個案分布以臺北市9例為最多，其次為桃園市3例、新北市2例；其中11例為已知感染源、3例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增6例死亡個案，為1例男性、5例女性，年齡介於60多歲至80多歲，發病日介於5月15日至6月29日，確診日介於5月26日至6月30日，死亡日介於7月6日至7月13日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月13日累計公布14,103位確診個案中，已有12,083人解除隔離，解隔離人數達確診人數85.7%。\$\@\$指揮中心表示，今日新增4例境外移入個案中，案15437為阿富汗籍40多歲男性，7月1日自阿富汗來臺工作，持有搭機前3日內檢驗陰性報告，入境後至防疫旅館居家檢疫，7月13日檢疫期滿前採檢，於今日確診；個案在臺期間並無症狀，且檢疫期間未與他人接觸，故無匡列接觸者。案15446、案15447均為印尼籍20多歲男性漁工，受雇於同一公司，5月12日搭乘同班機自印尼來臺，皆持有搭機前3日內檢驗陰性報告，入境後均至防疫旅館完成居家檢疫並持續隔離至7月12日，7月13日由公司安排自費採檢，皆於今日確診；2人在臺期間並無症狀且無外出，已匡列接觸者4人，因有適當防護，均列自我健康監測。案15452為荷蘭籍40多歲男性，7月13日自阿拉伯聯合大公國(杜拜)來臺工作，持有搭機前3日內檢驗陰性報告，入境時在機場採檢後至防疫旅館檢疫，於今日確診；個案在臺期間並無症狀，相關接觸者匡列中。\$\@\$指揮中心統計，截至目前國內累計1,707,362例新型冠狀病毒肺炎相關通報(含1,690,141例排除)，其中15,346例確診，分別為1,218例境外移入，14,075例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計106例移除為空號。2020年起累計759例COVID-19死亡病例，其中751例本土，個案居住縣市分布為新北市377例、臺北市288例、基隆市26例、桃園市22例、彰化縣13例、新竹縣10例、臺中市4例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月15日新增死亡COVID-19確診個案表.pdf</t>
@@ -134,18 +149,6 @@
   </si>
   <si>
     <t>發佈日期：2021-07-13\$\@\$中央流行疫情指揮中心表示，今(13)日上午與各縣市政府召開的「全國防疫會議」，決議如下：\$\@\$一、國內疫情現況及評估\$\@\$1.自實施全國加強三級警戒等相關管制措施下，Rt值已逐步下降，疫情持續趨緩，本週開始進行部分管制措施鬆綁，請各地方政府密切注意後續效應、及時應處。另全國三級警戒將延長至7月26日，考量各項防疫措施可能對民眾生活經濟、心理健康造成壓力，建議各地方政府進一步規劃相關關懷及配套方案，以舒緩民眾身心壓力。\$\@\$2.境外移入病例隨國外疫情上升有增加趨勢外，入境全面篩檢亦有陸續發現變異株相關個案，其中不乏病毒量高之病例，建議各地方政府持續加強疫情監控；雙北近期發生家庭群聚及職場群聚事件，仍請雙北地方政府除持續考量民眾就醫可近性設置社區篩檢站外，亦強化疫調作業，以利及早掌握病例，妥善應處。\$\@\$二、各直轄市、縣(市)政府「居家隔離/居家檢疫期滿前採檢政策」執行現況\$\@\$1.因應新型冠狀病毒Delta變異株於全球日益擴散且傳播力高，自今(2021)年6月22日起，確定病例之密切接觸者及自國外入境者，無論有無症狀，於居家隔離/檢疫之期滿前，須由各地方政府協助安排於隔離或檢疫期滿前1-3日(即接觸或入境迄日起第12-14日)內，搭乘防疫計程車前往醫療院所進行採檢，並確保於期滿前可取得檢驗報告。\$\@\$2.政策實施迄今，經期滿採檢計發現4名居家隔離、14名居家檢疫者採檢為確定病例，顯見於隔離或檢疫期滿前落實採檢措施，可避免COVID-19病毒進入社區，降低社區傳播風險，仍請各地方政府持續落實居家隔離/檢疫之期滿前採檢措施，共同守護社區防疫安全。\$\@\$三、衛生福利部為利疫情期間日照服務機構業務執行，業研議「衛生福利機構(社區型)因應COVID-19防疫管理指引」，相關重點請各地方政府協助檢視，近期將對外發布，重點包括：\$\@\$1.適用範圍：社區式服務類長期照顧機構(日間照顧、小規模多機能家庭托顧)、附設於一般護理之家、精神護理之家、老人福利機構、身心障礙福利機構之日間照顧服務、身心障礙日間型服務(社區日間作業設施、社區式日間照顧、家庭托顧、日間服務機構)、精神復健機構（日間型）、早期療育機構。\$\@\$2.服務條件\$\@\$(1)機構提供服務條件：\$\@\$整體工作人員疫苗施打率達8成，方可提供服務。\$\@\$未接種疫苗、接種第一劑疫苗未滿14日者，服務前應自費提供3日內SARS-CoV-2抗原快篩陰性證明或解除隔離證明，於三級警戒期間須配合每週自費提供抗原快篩陰性證明。\$\@\$地方政府應輔導轄內機構依本指引提供服務，機構須填具檢核表報地方政府備查，並配合後續抽核。\$\@\$(2)服務對象(含陪同照顧者)接受服務條件(未成年者不適用)：\$\@\$建議服務對象接種第一劑疫苗滿14日後，再前往接受服務。\$\@\$未接種疫苗、接種第一劑疫苗未滿14日者，接受服務前應自費提供3日內SARS-CoV-2抗原快篩陰性證明或解除隔離證明，於三級警戒期間須配合每週自費提供抗原快篩陰性證明。\$\@\$3.自主防疫管理措施：\$\@\$(1)工作人員及服務對象之健康管理部分，若為居家檢疫、居家隔離、自主健康管理者均不可提供或使用服務。\$\@\$(2)規劃服務動線、分區空間及隔離空間，建立分艙分流及活動分組進行機制。\$\@\$(3)交通服務管理，每車以10人（含司機）為限\$\@\$4.疑似確診應變措施：\$\@\$(1)任1位工作人員或服務對象為確定病例時，應暫停服務且立即通報地方社（衛）政主管機關，機構應進行相關人員造冊，並向該等人員宣導請其確實配合疫調。\$\@\$(2)立即就已知資訊先通知確定病例及可能與其有接觸之人員，等待衛生單位調查與聯繫。\$\@\$四、針對地方政府疫調資料調閱部分\$\@\$1.各地方政府如有確診軌跡調閱之需求，可透過各區管中心向指揮中心調閱，並將儘速於1天內提供。\$\@\$2.指揮中心已完成個案軌跡、熱區查詢、及簡訊實聯制疫調查詢功能，近日內提供各地方政府直接由線上進行查詢。另簡訊實聯制資料僅限制疫調查詢為主，相關查詢均有紀錄及配套機制，以確保使用範圍。\$\@\$3.以臺北市為例，近日向指揮中心調閱近1,000筆資料，除提供資料，指揮中心也提供線上查詢功能，並將和臺北市資訊局洽談介接與合作事宜。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-13\$\@\$中央流行疫情指揮中心今(13)日公布國內新增29例COVID-19確定病例，分別為28例本土及1例境外移入；另確診個案中新增6例死亡。\$\@\$指揮中心表示，今日新增之28例本土病例(其中11例為居家隔離期間或期滿檢驗陽性者)，為18例男性、10例女性，年齡介於未滿10歲至80多歲，發病日介於今(2021)年6月26日至7月12日。個案分布以新北市15例為最多，其次為臺北市9例，桃園市2例，苗栗縣及臺中市各1例；其中16例為已知感染源、3例關聯不明、9例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增6例死亡個案，為4例男性、2例女性，年齡介於60多歲至80多歲，發病日介於5月12日至6月18日，確診日介於5月16日至6月19日，死亡日介於7月4日至7月12日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月11日累計公布14,050位確診個案中，已有11,901人解除隔離，解隔離人數達確診人數84.7%。\$\@\$指揮中心表示，今日新增1例境外移入個案(案15387)，為本國籍40多歲男性，6月30日自印尼入境，持搭機前3日內檢驗陰性報告，入境後至集中檢疫所檢疫並採檢，7月1日結果為陰性；7月8日出現輕微發燒與肌肉痠痛等症狀，7月11日仍未緩解，由衛生單位安排採檢，於今日確診。個案檢疫期間無接觸他人，同機旅客均已入住集中檢疫所，故無匡列接觸者。\$\@\$指揮中心統計，截至目前國內累計1,661,153例新型冠狀病毒肺炎相關通報(含1,644,686例排除)，其中15,302例確診，分別為1,204例境外移入，14,045例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；確診個案中，累計105例移除為空號。2020年起累計747例COVID-19死亡病例，其中739例本土，個案居住縣市分布為新北市370例、臺北市286例、基隆市25例、桃園市21例、彰化縣13例、新竹縣10例、臺中市4例、宜蘭縣、苗栗縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月13日新增死亡COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-13\$\@\$中央流行疫情指揮中心今(13)日表示，為順利推動我國COVID-19疫苗接種作業，自即(7/13)日起開放18歲(含)以上民眾，於「疫苗施打意願登記與預約系統」( https://1922.gov.tw/）進行第三輪意願登記，相關說明如下：\$\@\$一、意願登記時間：即日起至7月15日17時，並同步進行第三輪結算。\$\@\$二、簡訊通知時間：7月16日至7月18日將陸續以簡訊通知符合資格的民眾；收到簡訊者，才能進行預約。本輪可接種疫苗為AZ疫苗。\$\@\$三、為協助不便使用「COVID-19疫苗施打意願登記與預約系統」的民眾登記意願，請地方政府設置因地制宜的服務專線或指定人員，協助不便使用系統的民眾進行意願登記。\$\@\$指揮中心進一步表示，第二輪的意願登記已於昨(12)日17時截止，全國約有285萬人登記，其中約114萬人有意願接種AZ疫苗。系統平臺將自7月13日上午，陸續以簡訊通知符合資格的民眾，提醒收到簡訊民眾記得進行預約；施打期間為7月16日至7月22日，籲請民眾準時前往接種。\$\@\$指揮中心提醒，「COVID-19疫苗施打意願登記與預約系統」須先完成意願登記，才能在接到通知後進行預約。系統平臺會按疫苗分配情形、參照民眾所登記的意願，通知符合預約資格的民眾，收到簡訊通知者即可進行下一步預約接種。尚未收到簡訊的民眾，會於後續符合預約資格後，收到簡訊通知，所有資料皆會完整保存，請民眾放心。\$\@\$指揮中心強調，「COVID-19疫苗施打意願登記與預約系統」是為建立讓大量疫苗接種能依序穩定有效推行的機制，中央與地方腳步一致，加強疫苗接種推動，提升群體保護力，維護國人健康。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-12\$\@\$中央流行疫情指揮中心今(12)日表示，為儘速提升國人COVID-19疫苗第一劑涵蓋率及我國群體保護力，並因應政策需要，昨(11)日經衛生福利部傳染病防治諮詢會預防接種組(ACIP)會議第4次臨時會議決議，自即日起調整現階段Moderna COVID-19疫苗之第一、二劑接種間隔，除第一類接種對象、國籍航空機組員及孕婦的第二劑Moderna疫苗維持於間隔至少28天後接種外，其餘對象均調整第一劑與第二劑接種間隔10至12週，並依疫苗供貨情形滾動調整。\$\@\$指揮中心指出，截至昨(11)日COVID-19疫苗(包含Moderna及AstraZeneca)累計接種3,565,840人次，疫苗涵蓋率約14.87%。依據國外臨床試驗資料分析顯示，Moderna COVID-19疫苗完成接種第一劑14天後保護力約為81%，另依據WHO建議接種間隔最晚可至12週，指揮中心考量政策需要並參考ACIP建議，亦將Moderna COVID-19疫苗接種間隔調整為10至12週，並持續視疫情狀況及疫苗供貨情形，滾動調整接種政策。\$\@\$指揮中心提醒，前往接種第二劑疫苗前，請確認備妥「COVID-19疫苗接種紀錄卡」及「健保卡」，若「COVID-19疫苗接種紀錄卡」已遺失，民眾可返回第一劑接種之醫療院所補發，再完成第二劑接種。此外，籲請民眾完成疫苗接種後，須持續積極配合各項防疫措施，並落實勤洗手、戴口罩及保持社交距離等個人防護，以全面保護自我與家人的健康，有效降低染疫風險。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-12\$\@\$中央流行疫情指揮中心今(12)日公布國內新增24例COVID-19確定病例，分別為23例本土及1例境外移入；另確診個案中新增1例死亡。\$\@\$指揮中心表示，今日新增之23例本土病例(其中9例為居家隔離期間或期滿檢驗陽性者)，為13例男性、10例女性，年齡介於未滿10歲至90多歲，發病日介於今(2021)年6月20日至7月11日。個案分布以新北市10例為最多，其次為臺北市9例，基隆市、桃園市、新竹市及臺中市各1例；其中17例為已知感染源、4例關聯不明、2例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增1例死亡個案(案2598)，為60多歲男性，具慢性病史及其他確診者接觸史；個案於5月11日出現發燒等症狀，5月19日就醫採檢，5月20日確診並住院治療，6月11日解除隔離並出院。7月10日因其他原因死亡。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月10日累計公布14,019位確診個案中，已有11,850人解除隔離，解隔離人數達確診人數84.5%。\$\@\$指揮中心表示，今日新增1例境外移入個案(案15370)，為克羅埃西亞籍未滿10歲女童，6月28日自瑞士入境，持搭機前3日內檢驗陰性報告，入境後至防疫旅館檢疫，7月10日進行檢疫期滿前採檢，於今日確診(Ct值33)。個案在臺期間並無症狀，相關接觸者匡列中。\$\@\$指揮中心統計，截至目前國內累計1,639,921例新型冠狀病毒肺炎相關通報(含1,622,834例排除)，其中15,273例確診，分別為1,203例境外移入，14,017例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；確診個案中，累計105例移除為空號。自2020年起累計741例COVID-19死亡病例，其中733例本土，個案居住縣市分布為新北市369例、臺北市283例、基隆市25例、桃園市21例、彰化縣12例、新竹縣9例、臺中市4例、宜蘭縣、苗栗縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。</t>
   </si>
 </sst>
 </file>
@@ -551,7 +554,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="2">
-        <v>44392</v>
+        <v>44393</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>25</v>
@@ -568,7 +571,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="2">
-        <v>44392</v>
+        <v>44393</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>26</v>
@@ -585,7 +588,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="2">
-        <v>44391</v>
+        <v>44393</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>27</v>
@@ -602,7 +605,7 @@
         <v>18</v>
       </c>
       <c r="C5" s="2">
-        <v>44391</v>
+        <v>44392</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>28</v>
@@ -619,7 +622,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="2">
-        <v>44390</v>
+        <v>44392</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>29</v>
@@ -636,7 +639,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="2">
-        <v>44390</v>
+        <v>44392</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>30</v>
@@ -653,7 +656,7 @@
         <v>21</v>
       </c>
       <c r="C8" s="2">
-        <v>44390</v>
+        <v>44392</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>31</v>
@@ -670,7 +673,7 @@
         <v>22</v>
       </c>
       <c r="C9" s="2">
-        <v>44389</v>
+        <v>44391</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>32</v>
@@ -687,7 +690,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="2">
-        <v>44389</v>
+        <v>44391</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>33</v>
@@ -704,10 +707,13 @@
         <v>24</v>
       </c>
       <c r="C11" s="2">
-        <v>44389</v>
+        <v>44390</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20210719
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Press Title</t>
   </si>
@@ -31,6 +31,18 @@
     <t>Page Content</t>
   </si>
   <si>
+    <t>COVID-19公費疫苗預約平臺第三輪意願登記截止，並自明(7/20)日上10時起預約接種</t>
+  </si>
+  <si>
+    <t>衛福部核准高端MVC-COV1901新冠肺炎疫苗專案製造</t>
+  </si>
+  <si>
+    <t>新增21例COVID-19確定病例，分別為15例本土及6例境外移入</t>
+  </si>
+  <si>
+    <t>自110年7月20日起恢復調派移工變更工作場所 雇主需於調派日前3日內安排移工檢驗PCR</t>
+  </si>
+  <si>
     <t>為使疫苗資源有效運用，Moderna疫苗第二劑接種對象擴及至第二類及三類，請各縣市及合約醫療院所加強推動符合資格民眾接種</t>
   </si>
   <si>
@@ -79,16 +91,16 @@
     <t>為儘速提升第一劑COVID-19疫苗涵蓋率，第二劑Moderna疫苗接種間隔調整自第10週起接種</t>
   </si>
   <si>
-    <t>新增24例COVID-19確定病例，分別為23例本土及1例境外移入</t>
-  </si>
-  <si>
-    <t>自7月13日起恢復移工轉換雇主，雇主需於承接日前3日內安排移工檢驗PCR</t>
-  </si>
-  <si>
-    <t>籲請50歲(含)以上及18歲(含)以上第9類對象至COVID-19公費疫苗預約平臺登記意願  7月13日起陸續簡訊通知進行預約</t>
-  </si>
-  <si>
-    <t>新增31例COVID-19確定病例，分別為28例本土及3例境外移入</t>
+    <t>/Bulletin/Detail/QZnxN-D_mKhbpnDTSRB2YQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/gzkfXTnBuktqDJ3BXhI54w?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/au9qBuU-ft4ueA56WlXGPQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/fJu3NrBv5eVgPKLyZxGvyQ?typeid=9</t>
   </si>
   <si>
     <t>/Bulletin/Detail/7Ct5hMov8Tbtg1FNdufD7g?typeid=9</t>
@@ -139,16 +151,16 @@
     <t>/Bulletin/Detail/vu8IYJ-y67cc4ZpemyPBTA?typeid=9</t>
   </si>
   <si>
-    <t>/Bulletin/Detail/1FS11QWUMT5jcui6nxcIvw?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/3UJq0hJLq-ru0x_ktDM0tg?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/LFEwMGAQQaE-q0wQ6ioHkQ?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/IWGDujzOX0GnYxtf2TCw5Q?typeid=9</t>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/QZnxN-D_mKhbpnDTSRB2YQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/gzkfXTnBuktqDJ3BXhI54w?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/au9qBuU-ft4ueA56WlXGPQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/fJu3NrBv5eVgPKLyZxGvyQ?typeid=9</t>
   </si>
   <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/7Ct5hMov8Tbtg1FNdufD7g?typeid=9</t>
@@ -199,19 +211,19 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/vu8IYJ-y67cc4ZpemyPBTA?typeid=9</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/1FS11QWUMT5jcui6nxcIvw?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/3UJq0hJLq-ru0x_ktDM0tg?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/LFEwMGAQQaE-q0wQ6ioHkQ?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/IWGDujzOX0GnYxtf2TCw5Q?typeid=9</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-18\$\@\$中央流行疫情指揮中心(18)日表示，Moderna疫苗自解凍後，可使用期間為30天(配送各縣市後以28天計算)，自7月1、5、8及9日陸續配送至各地方政府衛生局或合約醫療院所的Moderna疫苗目前尚餘21萬570劑，將在7月29日至8月6日間到期，請各地方政府衛生局及合約醫療院所加強推動，針對原已符合第二劑接種間隔為至少28天的第一類、機組人員及孕婦等對象提供接種。\$\@\$指揮中心指出，為使疫苗資源有效運用，經統計自6月9日至7月9日為止，已接種第一劑Moderna疫苗之第一類至第三類對象及孕婦，共計18萬9,788人可於8月6日之前(接種間隔至少28天)接種第二劑Moderna疫苗，故目前各地方政府及合約醫療院所剩餘量，尚足以提供該等對象第二劑接種使用。為使高風險第一線防疫人員及相關工作人員能夠儘速獲得保護力，讓疫苗資源有效運用，自即日起除第一類、機組人員及孕婦等對象以外，第二及第三類對象於接種第一劑Moderna疫苗後滿28天，亦可接種第二劑。\$\@\$另指揮中心提醒，5月11日至5月23日已接種第一劑AstraZeneca 疫苗的民眾，將陸續自下週起間隔滿10週，可透過COVID-19疫苗預約系統意願登記接種第二劑，或至COVID-19疫苗合約醫療院所預約。請地方政府衛生局偕同合約醫療院所提供前述對象完成二劑疫苗接種，以提升第二劑疫苗覆蓋率。指揮中心亦將持續視疫情狀況及疫苗供貨情形，滾動調整接種政策。\$\@\$指揮中心提醒，民眾前往接種COVID-19第二劑疫苗前，請備妥「COVID-19疫苗接種紀錄卡」及「健保卡」。若「COVID-19疫苗接種紀錄卡」已遺失，民眾可返回第一劑接種的醫療院所申請補發，再繼續完成第二劑接種。接種單位於接種前需核對民眾身分資料、主動詢問民眾疫苗接種史，檢視疫苗接種紀錄卡紀錄及健保卡註記貼紙資料，如均無相關接種證明或資訊者，除可使用網路連線全國性預防接種資訊管理系統(NIIS)查詢子系統查詢疫苗接種史，合約醫療院所亦可透過雲端藥歷系統等連結查詢，以確認疫苗接種間隔及廠牌是否符合規範。</t>
+    <t>發佈日期：2021-07-19\$\@\$中央流行疫情指揮中心今(19)日表示，「COVID-19疫苗施打意願登記與預約系統」第三輪的意願登記已於今日中午12時截止，全國約有887萬人登記，其中約495萬人有意願接種AZ疫苗。該系統平臺自7月20日上午10時起，將針對第六、八、九、十類及1973年12月31日(含)以前出生民眾，約170萬人會陸續收到簡訊，預約接種期程至7月22日中午12時截止；本輪可接種疫苗為AZ疫苗，施打期間為7月23日至7月29日，籲請民眾準時前往接種。未來將視疫苗到貨量，每周二發送簡訊，提醒民眾預約接種。如接獲簡訊，但沒有完成預約者，將自動加入下一次簡訊通知名單。\$\@\$指揮中心進一步說明，該系統平臺自今日中午12時以後將先暫停意願登記，後續視疫苗新到貨量後重開意願登記。此外，重新開啟後，增勾或改勾AZ疫苗者，將於第三輪意願登記接種AZ疫苗之495萬人優先處理後，再接續處理。\$\@\$指揮中心提醒，請民眾須先於「COVID-19疫苗施打意願登記與預約系統」完成意願登記，才能在接到簡訊通知後進行預約。系統平臺會按疫苗分配情形、參照民眾登記之意願，通知符合預約資格的民眾，收到簡訊通知者才可進行下一步預約接種。尚未收到簡訊的民眾，會於後續符合預約資格後，收到簡訊通知，所有資料皆會完整保存，請民眾放心。\$\@\$指揮中心強調，「COVID-19疫苗施打意願登記與預約系統」是為了建立讓大量疫苗接種能依序且穩定有效推行的機制，中央與地方腳步一致，加強推動疫苗接種，提升群體保護力，守護國人健康。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-19\$\@\$衛生福利部食品藥物管理署(以下簡稱食藥署)為積極因應新型冠狀病毒疾病(以下簡稱COVID-19)疫情防疫需求，於110年7月18日邀請國內化學製造管制、藥學、毒理學、臨床醫學、公衛、法律及醫學倫理專家召開會議，討論高端MVC-COV1901新冠肺炎疫苗(以下簡稱高端疫苗)專案製造申請案。\$\@\$經過一天充分的審查與討論，鑑於高端疫苗的中和抗體數據已證明不劣於國人接種AZ疫苗的中和抗體結果，達成食藥署公告之「新冠疫苗專案製造或輸入技術性資料審查基準」要求，且安全性數據顯示無重大安全疑慮：\$\@\$1.高端疫苗組與AZ疫苗組之原型株活病毒中和抗體幾何平均效價比值(geometric mean titer ratio, GMTR)的95%信賴區間下限為3.4倍，遠大於標準要求0.67倍。\$\@\$2.高端疫苗組的血清反應比率(sero-response rate)的95%信賴區間下限為95.5%，遠大於標準要求50%。\$\@\$基於疾病管制署認定國內確有疫情及疫苗緊急公共衛生需求之前提，評估整體醫療利益與風險平衡，與會專家出席21人，主席不參與投票，18人同意，1人補件再議，1人不同意。\$\@\$食藥署依「藥事法第48條之2規定」，核准高端疫苗專案製造，適用於20歲以上成人之主動免疫接種，接種兩劑，間隔28天，以預防COVID-19。另針對專家會議建議，該疫苗於專案核准製造期間，藥商須每月提供安全性監測報告，並於核准後一年內檢送國內外執行疫苗保護效益(effectiveness)報告，以保障國人用藥安全。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-19\$\@\$中央流行疫情指揮中心今(19)日公布國內新增21例COVID-19確定病例，分別為15例本土及6例境外移入；另確診個案中新增1例死亡。\$\@\$指揮中心表示，今日新增之15例本土病例(其中7例為居家隔離期間或期滿檢驗陽性者)，為8例男性、7例女性，年齡介於未滿5歲至80多歲，發病日介於今(2021)年7月14日至7月17日。個案分布以新北市11例為最多，其次為桃園市3例、臺北市1例；其中9例為已知感染源，餘6例關聯不明，將持續進行疫情調查，以釐清感染源。\$\@\$指揮中心說明，今日新增1例死亡個案(案13852)，為80多歲男性，有慢性病，因有其他確診者接觸史，6月17日安排採檢，採檢時無症狀，檢驗結果為陽性，同日收治住院，6月18日確診，7月9日解除隔離，7月17日因其他原因死亡。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月17日累計公布14,192位確診個案中，已有12,268人解除隔離，解隔離人數達確診人數86.4%。\$\@\$指揮中心表示，今日新增6例境外移入個案，為5男 1女，年齡介於20多歲至50多歲，分別自阿根廷、阿拉伯聯合大公國、柬埔寨、波蘭、丹麥、美國入境，均持有搭機前3日內檢驗陰性報告，入境日介於5月28日至7月17日；詳如新聞稿附件。\$\@\$指揮中心統計，累計1,778,511例新型冠狀病毒肺炎相關通報(含1,761,879例排除)，其中15,429例確診，分別為1,235例境外移入，14,141例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計106例移除為空號。2020年起累計769例COVID-19死亡病例，其中761例本土，個案居住縣市分布為新北市382例、臺北市291例、基隆市27例、桃園市23例、彰化縣13例、新竹縣10例、臺中市4例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月19日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-19\$\@\$中央流行疫情指揮中心今(19)日表示，國內疫情已較為穩定，為兼顧國內妥善安排人力及實務上業務需求，自今(2021)年7月20日起恢復移工調派至同一雇主之其他工作場所。至於工作延伸(即雇主指派移工至客戶契約履行地工作)，考量移工流動性較高及染疫風險，仍暫緩解封，未來將視疫情再行檢討。\$\@\$指揮中心說明，近期評估國內整體疫情及產業發展需要，將自7月20日起恢復調派移工變更工作場所，雇主符合下列情形，得調派移工變更工作場所單次達60日以上，其餘單次未達60日以上者仍不得調派：\$\@\$一、安排移工核酸檢驗（下稱PCR）且PCR結果須為陰性：如為須向勞動部申請調派許可者(如營造業)，須於申請日(含)前3日內安排移工檢驗PCR，且PCR結果須為陰性，始得向勞動部提出申請。另其他工作類別無須經勞動部許可得逕調派者，須於調派日(含)前3日內安排移工檢驗PCR，且PCR結果須為陰性，始得調派移工，又調派前應先將PCR檢驗結果送當地勞工主管機關備查。\$\@\$二、雇主應依指引辦理防疫措施：倘若移工檢測PCR確診時，雇主應善盡雇主責任，並依勞動部「因應嚴重特殊傳染性肺炎雇主聘僱移工指引：移工工作、生活及外出管理注意事項」，配合衛生單位安排就醫或送集中檢疫所隔離治療，並依確診個案處置及解除隔離治療條件續處。倘若移工檢測PCR陰性，雇主調派移工仍應依指引，每日進行移工健康監測及記錄移工出入足跡。\$\@\$指揮中心進一步表示，雇主調派移工變更工作場所單次達60日以上者，如未於上開規定期限內安排移工檢驗PCR，未依規定向勞動部申請或未送當地勞工主管機關備查，將依「就業服務法」第57條第4款及第68條第1項規定，處新臺幣3萬至15萬元罰鍰；若違反2次以上，將廢止雇主聘僱許可及管制聘僱移工名額。另雇主如委託仲介公司辦理移工生活照顧，因仲介公司未善盡受任事務，違反上開防疫措施，將依仲介公司違反「就業服務法」規定，處新臺幣6萬元以上至30萬元以下罰鍰。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-18\$\@\$中央流行疫情指揮中心今(18)日表示，Moderna疫苗自解凍後，可使用期間為30天(配送各縣市後以28天計算)，自7月1、5、8及9日陸續配送至各地方政府衛生局或合約醫療院所的Moderna疫苗目前尚餘21萬570劑，將在7月29日至8月6日間到期，請各地方政府衛生局及合約醫療院所加強推動，針對原已符合第二劑接種間隔為至少28天的第一類、機組人員及孕婦等對象提供接種。\$\@\$指揮中心指出，為使疫苗資源有效運用，經統計自6月9日至7月9日為止，已接種第一劑Moderna疫苗之第一類至第三類對象及孕婦，共計18萬9,788人可於8月6日之前(接種間隔至少28天)接種第二劑Moderna疫苗，故目前各地方政府及合約醫療院所剩餘量，尚足以提供該等對象第二劑接種使用。為使高風險第一線防疫人員及相關工作人員能夠儘速獲得保護力，讓疫苗資源有效運用，自即日起除第一類、機組人員及孕婦等對象以外，第二及第三類對象於接種第一劑Moderna疫苗後滿28天，亦可接種第二劑。\$\@\$另指揮中心提醒，5月11日至5月23日已接種第一劑AstraZeneca 疫苗的民眾，將陸續自下週起間隔滿10週，可透過COVID-19疫苗預約系統意願登記接種第二劑，或至COVID-19疫苗合約醫療院所預約。請地方政府衛生局偕同合約醫療院所提供前述對象完成二劑疫苗接種，以提升第二劑疫苗覆蓋率。指揮中心亦將持續視疫情狀況及疫苗供貨情形，滾動調整接種政策。\$\@\$指揮中心提醒，民眾前往接種COVID-19第二劑疫苗前，請備妥「COVID-19疫苗接種紀錄卡」及「健保卡」。若「COVID-19疫苗接種紀錄卡」已遺失，民眾可返回第一劑接種的醫療院所申請補發，再繼續完成第二劑接種。接種單位於接種前需核對民眾身分資料、主動詢問民眾疫苗接種史，檢視疫苗接種紀錄卡紀錄及健保卡註記貼紙資料，如均無相關接種證明或資訊者，除可使用網路連線全國性預防接種資訊管理系統(NIIS)查詢子系統查詢疫苗接種史，合約醫療院所亦可透過雲端藥歷系統等連結查詢，以確認疫苗接種間隔及廠牌是否符合規範。</t>
   </si>
   <si>
     <t>發佈日期：2021-07-18\$\@\$中央流行疫情指揮中心今(18)日公布國內新增18例COVID-19確定病例，分別為15例本土及3例境外移入；另確診個案中新增4例死亡。\$\@\$指揮中心表示，今日新增之15例本土病例(其中6例為居家隔離期間或期滿檢驗陽性者)，為9例男性、6例女性，年齡介於20多歲至90多歲，發病日介於今(2021)年7月10日至7月17日。個案分布以新北市7例為最多，其次為臺北市5例、桃園市3例；其中9例為已知感染源，餘6例關聯不明，將持續進行疫情調查，以釐清感染源。\$\@\$指揮中心說明，今日新增4例死亡個案，為3例男性、1例女性，年齡介於40多歲至80多歲，發病日介於5月26日至6月13日，確診日介於6月3日至6月16日，死亡日介於7月13日至7月15日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月16日累計公布14,180位確診個案中，已有12,243人解除隔離，解隔離人數達確診人數86.3%。\$\@\$指揮中心表示，今日新增3例境外移入個案中，案15507為本國籍20多歲男性，7月15日自西班牙返臺，持有搭機前3日內檢驗陰性報告，入境時在機場採檢後至防疫旅館檢疫，於今日確診；個案在臺期間並無症狀，相關接觸者匡列中。案15508為英國籍20多歲男性，7月15日自英國來臺工作，持有搭機前3日內檢驗陰性報告，入境後至集中檢疫所檢疫並採檢，於今日確診；個案在臺期間並無症狀，相關接觸者匡列中。案15512為本國籍50多歲女性，7月16日自美國返臺，持有搭機前3日內檢驗陰性報告，入境時無症狀，在機場採檢後至防疫旅館檢疫，同日出現流鼻水、喉嚨痛、喉嚨癢及頭暈症狀，7月17日由衛生單位安排至集中檢疫所隔離，並於今日確診；已匡列接觸者19人，其中10人為同班機前後兩排旅客，列居家隔離，餘9人為同班機機組員，列自主健康管理。\$\@\$指揮中心統計，截至目前國內累計1,765,532例新型冠狀病毒肺炎相關通報(含1,747,814例排除)，其中15,408例確診，分別為1,229例境外移入，14,126例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計106例移除為空號。2020年起累計768例COVID-19死亡病例，其中760例本土，個案居住縣市分布為新北市382例、臺北市291例、基隆市26例、桃園市23例、彰化縣13例、新竹縣10例、臺中市4例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月18日新增死亡COVID-19確診個案表.pdf</t>
@@ -226,40 +238,16 @@
     <t>發佈日期：2021-07-16\$\@\$中央流行疫情指揮中心今(16)日公布國內新增32例COVID-19確定病例，分別為29例本土及3例境外移入；另確診個案中新增4例死亡。\$\@\$指揮中心表示，今日新增之29例本土病例(其中7例為居家隔離期間或期滿檢驗陽性者)，為17例男性、12例女性，年齡介於未滿5歲至60多歲，發病日介於今(2021)年7月5日至7月15日。個案分布以臺北市14例為最多，其次為新北市11例、桃園市2例、宜蘭縣及彰化縣各1例；其中21例為已知感染源、4例關聯不明、4例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增4例死亡個案，均為男性，年齡介於60多歲至90多歲，發病日介於5月24日至6月16日，確診日介於5月26日至6月24日，死亡日介於7月9日至7月14日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月14日累計公布14,130位確診個案中，已有12,131人解除隔離，解隔離人數達確診人數85.9%。\$\@\$指揮中心表示，今日新增3例境外移入個案中，案15468為美國籍50多歲男性，7月2日自美國來臺工作，持有搭機前3日內檢驗陰性報告，入境後至防疫旅館居家檢疫，7月14日檢疫期滿前採檢，於今日確診；個案在臺期間並無症狀，且檢疫期間未與他人接觸，故無匡列接觸者。案15472為本國籍未滿10歲女童，7月2日自美國返臺，持有搭機前3日內檢驗陰性報告，入境後至防疫旅館居家檢疫，7月14日檢疫期滿前採檢，於今日確診；個案在臺期間並無症狀，已匡列接觸者2人，列居家隔離。案15480為菲律賓籍30多歲男性漁工，4月30日自菲律賓來臺，持有搭機前3日內檢驗陰性報告，入境後至防疫旅館居家檢疫，檢疫期滿與自主健康管理期滿採檢結果均為陰性，5月22日登船工作後未再下船，7月14日因有出海作業需求，由公司安排自費採檢，於今日確診；個案在臺期間並無症狀，已匡列接觸者18人，其中17人列居家隔離、1人列自我健康監測。\$\@\$指揮中心統計，截至目前國內累計1,727,787例新型冠狀病毒肺炎相關通報(含1,710,974例排除)，其中15,378例確診，分別為1,221例境外移入，14,104例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計106例移除為空號。2020年起累計763例COVID-19死亡病例，其中755例本土，個案居住縣市分布為新北市379例、臺北市289例、基隆市26例、桃園市23例、彰化縣13例、新竹縣10例、臺中市4例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月16日新增死亡COVID-19確診個案表.pdf</t>
   </si>
   <si>
-    <t>發佈日期：2021-07-16\$\@\$中央流行疫情指揮中心今(16)日宣布，考量緬甸疫情現況及風險，於「重點高風險國家」增列緬甸。自7月18日零時起(抵臺時間)，自海港或空港入境我國人士，如過去14天有緬甸旅遊史(含轉機)者，入境後均應至集中檢疫所進行14天檢疫，且須配合於入住時與檢疫期滿分別進行PCR檢測，另檢疫期間第10至12天以「家用快篩」採檢一次；旅客不需支付集中檢疫所及採檢費用；此外，國籍航空公司機組員亦維持自「重點高風險國家」航線航班返臺後，應入住防疫旅宿或符合規定之公司宿舍檢疫14天，且檢疫期滿進行PCR檢測。\$\@\$指揮中心表示，緬甸近1個多月疫情再度遽升，近1週日增確診數由50例以下，上升至逾4,000例，新增確診及死亡數均續創新高，檢驗陽性率已逾30%；迄今累計逾20萬例確診病例，逾4千例死亡，致死率2%。此波疫情初期病例多來自鄰近印度邊境之實皆省(Sagaing)及欽邦(Chin)，爾後與印度接壤之多個社區陸續爆發疫情，並監測到Delta變異株。該國已於部分地區實施居家令，因醫療體系之篩檢量及檢測能力不足，實際疫情可能比官方公布更為嚴峻。\$\@\$指揮中心指出，現行「重點高風險國家」為巴西(Gamma巴西變異株)、印度、英國、秘魯、以色列、印尼、孟加拉及本次新增之緬甸(Delta印度變異株)等，共8國。\$\@\$指揮中心說明，邊境管制為防範COVID-19疫情之重要關鍵，指揮中心已全面提升入境人士檢疫措施、持續監測境外移入檢出變異株情形，同時籲請入境人士抵臺時應主動配合邊境檢疫措施，並依指揮中心規定之交通方式前往檢疫地點及配合後續防疫措施，落實全民共同抗疫，將疫情阻絕於境外。</t>
-  </si>
-  <si>
     <t>發佈日期：2021-07-15\$\@\$中央流行疫情指揮中心今(15)日表示，「COVID-19疫苗施打意願登記與預約系統」第二輪共計約94.1萬人已完成預約接種，將自明(16)日起開始施打，請民眾攜帶健保卡，如為第二劑接種者，亦請攜帶接種紀錄卡，於預約時間準時至預約地點接種疫苗。如民眾錯過預約時段，可於當日告知現場人員，另擇同日之其他時段接種；如無法於預約當日接種，須等候下一輪簡訊通知後，再至系統重新預約接種。\$\@\$指揮中心指出，第三輪意願登記原訂於7月15日下午5時進行第三輪結算，將延長至7月19日中午12時進行第三輪結算，並自7月20日起陸續以簡訊通知符合資格的民眾進行預約接種；本輪可接種疫苗為AZ疫苗。\$\@\$指揮中心提醒，「COVID-19疫苗施打意願登記與預約系統」須先完成意願登記，才能在接到簡訊通知後進行預約。系統平臺會按疫苗分配情形、參照民眾登記之意願，通知符合預約資格的民眾，收到簡訊通知者才可進行下一步預約接種。尚未收到簡訊的民眾，會於後續符合預約資格後收到簡訊通知，所有資料皆會完整保存，請民眾放心。\$\@\$指揮中心強調，「COVID-19疫苗施打意願登記與預約系統」是為了建立大量疫苗接種能依序穩定有效推行的機制，中央與地方腳步一致，加強推動疫苗接種，提升群體保護力，守護國人健康。</t>
   </si>
   <si>
-    <t>發佈日期：2021-07-15\$\@\$疾病管制署今(15)日表示，因應行政院農業委員會動植物防疫檢疫局本(2021)年6月30日發布，國內檢出首例黃喉貂狂犬病陽性案例，為維護國內民眾健康及安全，降低感染風險，疾管署修訂「疑似狂犬病或麗沙病毒動物抓咬傷臨床處置指引」，調整暴露後預防接種對象，增列遭「黃喉貂」咬傷者，經評估傷口暴露等級為第2及第3類者，應接種暴露後狂犬病免疫球蛋白及疫苗，並自本年7月1日起適用。\$\@\$疾管署說明，國內每年均接獲數起食肉目野生動物抓咬傷民眾通報案件，今年迄今有8起，其中3件動物檢驗為狂犬病陽性，去（2020）年同期為11起，全年則有14起，其中5件檢驗為狂犬病陽性、4件陰性、5件未送驗，陽性案件分布範圍為南投縣3件，屏東縣、嘉義縣各1件。\$\@\$狂犬病是由狂犬病病毒引起的一種急性腦脊髓炎，狂犬病毒從已感染動物的唾液隨著抓、咬傷所造成之傷口進入人體，潛伏期約1至3個月，初期症狀有發熱、喉嚨痛、發冷、厭食、嘔吐、呼吸困難、咳嗽、頭痛或咬傷部位異樣感，數天後出現興奮及恐懼現象，然後麻痺、吞嚥困難，咽喉部痙攣，並引起恐水現象(又稱恐水症)，隨後會發生精神錯亂及抽搐等情況，如不採取醫療措施，患者常因呼吸麻痺導致死亡，致死率近100%，但如能在遭動物咬傷後及時就醫，並接受狂犬病暴露後預防接種，可以降低發病的風險。\$\@\$疾管署再次呼籲，民眾應避免接觸及捕捉野生動物，每年須帶家中犬、貓等寵物施打狂犬病疫苗；如不慎遭野生哺乳類動物抓咬傷，請以肥皂及大量清水沖洗傷口15分鐘，再以優碘或70%酒精消毒後，儘速前往就醫，經醫師評估如有感染狂犬病風險，應儘速接種免疫球蛋白，並依時程(接種第一劑當天為第0天、3、7及第14天)接種4劑人用狂犬病疫苗，降低發病風險。相關資訊請參閱疾管署全球資訊網(https://www.cdc.gov.tw)或撥打免費防疫專線1922(或0800-001922)洽詢。 圖片 附件\$\@\$鼬獾.jpg\$\@\$黃喉貂.jpg\$\@\$白鼻心.jpg\$\@\$疑似狂犬病或麗沙病毒感染動物抓咬傷臨床處置指引_0715.pdf</t>
+    <t>發佈日期：2021-07-15\$\@\$中央流行疫情指揮中心今(15)日表示，日本政府提供第三批的97萬劑AstraZeneca疫苗及我國自行採購的第三批56萬劑AstraZeneca疫苗與第四批35萬劑Moderna疫苗將於今日下午陸續運抵桃園國際機場，待完成通關程序後，將直接運送至指定冷儲物流中心進行後續檢驗封緘作業，再提供COVID-19疫苗接種計畫所列實施對象進行接種。\$\@\$指揮中心說明，日本提供我國AstraZeneca疫苗分別為6月4日124萬劑、7月8日113萬劑與本批97萬劑，共334萬劑；我國與供應商(阿斯特捷利康公司)採購AstraZeneca疫苗分別為3月3日11.7萬劑、7月7日62.6萬劑與本批56萬劑，共130.3萬劑到貨。另，我國與Moderna供應商採購部分分別為5月28日15萬劑、6月18日24萬劑、6月30日41萬劑與本批35萬劑，共115萬劑。\$\@\$指揮中心再次感謝日本政府伸出援手提供第三批COVID-19疫苗，加上我國自行採購之AstraZeneca疫苗與Moderna疫苗陸續到貨，將有助提升我國疫苗覆蓋率。</t>
   </si>
   <si>
     <t>發佈日期：2021-07-15\$\@\$中央流行疫情指揮中心今(15)日公布國內新增18例COVID-19確定病例，分別為14例本土及4例境外移入；另確診個案中新增6例死亡。\$\@\$指揮中心表示，今日新增之14例本土病例(其中7例為居家隔離期間或期滿檢驗陽性者)，為8例男性、6例女性，年齡介於未滿10歲至60多歲，發病日介於今(2021)年7月7日至7月14日。個案分布以臺北市9例為最多，其次為桃園市3例、新北市2例；其中11例為已知感染源、3例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增6例死亡個案，為1例男性、5例女性，年齡介於60多歲至80多歲，發病日介於5月15日至6月29日，確診日介於5月26日至6月30日，死亡日介於7月6日至7月13日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月13日累計公布14,103位確診個案中，已有12,083人解除隔離，解隔離人數達確診人數85.7%。\$\@\$指揮中心表示，今日新增4例境外移入個案中，案15437為阿富汗籍40多歲男性，7月1日自阿富汗來臺工作，持有搭機前3日內檢驗陰性報告，入境後至防疫旅館居家檢疫，7月13日檢疫期滿前採檢，於今日確診；個案在臺期間並無症狀，且檢疫期間未與他人接觸，故無匡列接觸者。案15446、案15447均為印尼籍20多歲男性漁工，受雇於同一公司，5月12日搭乘同班機自印尼來臺，皆持有搭機前3日內檢驗陰性報告，入境後均至防疫旅館完成居家檢疫並持續隔離至7月12日，7月13日由公司安排自費採檢，皆於今日確診；2人在臺期間並無症狀且無外出，已匡列接觸者4人，因有適當防護，均列自我健康監測。案15452為荷蘭籍40多歲男性，7月13日自阿拉伯聯合大公國(杜拜)來臺工作，持有搭機前3日內檢驗陰性報告，入境時在機場採檢後至防疫旅館檢疫，於今日確診；個案在臺期間並無症狀，相關接觸者匡列中。\$\@\$指揮中心統計，截至目前國內累計1,707,362例新型冠狀病毒肺炎相關通報(含1,690,141例排除)，其中15,346例確診，分別為1,218例境外移入，14,075例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計106例移除為空號。2020年起累計759例COVID-19死亡病例，其中751例本土，個案居住縣市分布為新北市377例、臺北市288例、基隆市26例、桃園市22例、彰化縣13例、新竹縣10例、臺中市4例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月15日新增死亡COVID-19確診個案表.pdf</t>
   </si>
   <si>
-    <t>發佈日期：2021-07-14\$\@\$中央流行疫情指揮中心今(14)日表示，COVID-19疫情三級警戒期間，為降低失能者及身心障礙者群聚及傳染風險，社區式機構均暫停提供服務。現因應國內疫情趨緩，指揮中心宣布社區式機構可在工作人員疫苗施打率達8成且做好防疫整備工作的狀態下，適度鬆綁，逐步恢復提供服務。\$\@\$指揮中心說明，為確保服務對象健康，衛生福利部特訂定「衛生福利機構(社區型)因應COVID-19防疫管理指引」，針對「服務條件」、「自主防疫管理措施」、「具有COVID-19感染風險者之應變措施及發生確診病例應變處置」等管理事項，提供社區式服務機構依循辦理，地方政府應輔導轄內機構依本指引提供服務，並填具檢核表報地方政府備查，在完備防疫工作的前提下逐步恢復提供服務。\$\@\$本指引適用提供社區式服務之衛生福利機構，包括：社區式服務類長期照顧機構(日間照顧、小規模多機能)、附設於住宿機構之日間照顧服務、身心障礙日間型服務(含社區日間作業設施、社區式日間照顧、日間服務機構)、精神復健機構(日間型)、早期療育機構。本指引重點包括：\$\@\$一、服務條件\$\@\$(一)機構提供服務條件：\$\@\$1.整體工作人員疫苗施打率達8成，方可提供服務。\$\@\$2.未接種疫苗、接種第一劑疫苗未滿14日者，服務前應自費提供3日內SARS-CoV-2抗原快篩(以下簡稱抗原快篩)陰性證明，於三級警戒期間須配合每週自費提供抗原快篩陰性證明。\$\@\$(二)服務對象接受服務條件(未成年者不適用)：\$\@\$1.建議服務對象接種第一劑疫苗滿14日後，再前往接受服務。\$\@\$2.未接種疫苗、接種第一劑疫苗未滿14日者，接受服務前應自費提供3日內抗原快篩陰性證明或解除隔離證明，於三級警戒期間須配合每週自費提供抗原快篩陰性證明。\$\@\$二、自主防疫管理措施：\$\@\$(一)工作人員及服務對象之健康管理部分，若為確診、居家檢疫、居家隔離、自主健康管理、抗原快篩陽性者均不可提供或使用服務。\$\@\$(二)規劃服務動線、分區空間及隔離空間，建立分艙分流及分組活動、用餐機制。\$\@\$(三)交通服務管理，每車以10人(含司機)為限，車內禁止用餐、飲水。\$\@\$(四)加強環境(含交通接送車輛)清潔消毒，每日至少2次。\$\@\$三、具有COVID-19感染風險者之應變措施及發生確診病例應變處置：\$\@\$(一)發現疑似病例，機構應於24小時內通報，疑似病例應各自於隔離空間等候就醫或返家，且不得搭乘大眾交通工具。\$\@\$(二)任1位工作人員或服務對象為確定病例時，應暫停服務且立即通報地方主管機關，機構應進行相關人員造冊，並向該等人員宣導請其確實配合疫調。\$\@\$(三)立即就已知資訊先通知確定病例及可能與其有接觸之人員，等待衛生單位調查與聯繫。\$\@\$另家庭托顧服務部分，因照顧規模較小，且工作人員及服務對象皆屬公費疫苗第五類施打對象，較不易發生大規模群聚感染情形；雖不在指引適用範圍，但仍應在家庭托顧員完成疫苗第一劑接種且滿14日的前提下，參考社區式服務防疫管理指引加強人員健康監測、維持社交距離、增加環境清潔消毒次數、建立疑似個案通報轉送及確診病例應變處置機制，落實防疫規範下恢復營運。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-14\$\@\$中央流行疫情指揮中心今(14)日公布國內新增27例COVID-19確定病例，分別為17例本土及10例境外移入；另確診個案中新增6例死亡。\$\@\$指揮中心表示，今日新增之17例本土病例(其中9例為居家隔離期間或期滿檢驗陽性者)，為11例男性、6例女性，年齡介於未滿10歲至80多歲，發病日介於今(2021)年7月7日至7月13日。個案分布以臺北市10例為最多，其次為桃園市3例、新北市及臺中市各2例；其中10例為已知感染源、3例關聯不明、4例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增6例死亡個案，為5例男性、1例女性，年齡介於50多歲至80多歲，發病日介於5月15日至7月3日，確診日介於5月19日至7月5日，死亡日介於7月10日至7月12日；詳如新聞稿附件1。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月12日累計公布14,074位確診個案中，已有11,964人解除隔離，解隔離人數達確診人數85.0%。\$\@\$指揮中心表示，今日新增10例境外移入個案，為9例男性、1例女性，年齡介於10多歲至70多歲，分別自緬甸(6例，為同一班機乘客)、英國、日本、印尼及茅利塔尼亞入境，均持有搭機前3日內檢驗陰性報告，入境日介於6月30日至7月11日；詳如新聞稿附件2。\$\@\$指揮中心統計，截至目前國內累計1,686,311例新型冠狀病毒肺炎相關通報(含1,669,801例排除)，其中15,328例確診，分別為1,214例境外移入，14,061例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；新增1例空號病例(案15282)，共累計106例移除為空號。2020年起累計753例COVID-19死亡病例，其中745例本土，個案居住縣市分布為新北市374例、臺北市287例、基隆市25例、桃園市21例、彰化縣13例、新竹縣10例、臺中市4例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月14日新增死亡COVID-19確診個案表.pdf\$\@\$7月14日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-13\$\@\$中央流行疫情指揮中心今(13)日公布國內新增29例COVID-19確定病例，分別為28例本土及1例境外移入；另確診個案中新增6例死亡。\$\@\$指揮中心表示，今日新增之28例本土病例(其中11例為居家隔離期間或期滿檢驗陽性者)，為18例男性、10例女性，年齡介於未滿10歲至80多歲，發病日介於今(2021)年6月26日至7月12日。個案分布以新北市15例為最多，其次為臺北市9例，桃園市2例，苗栗縣及臺中市各1例；其中16例為已知感染源、3例關聯不明、9例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增6例死亡個案，為4例男性、2例女性，年齡介於60多歲至80多歲，發病日介於5月12日至6月18日，確診日介於5月16日至6月19日，死亡日介於7月4日至7月12日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月11日累計公布14,050位確診個案中，已有11,901人解除隔離，解隔離人數達確診人數84.7%。\$\@\$指揮中心表示，今日新增1例境外移入個案(案15387)，為本國籍40多歲男性，6月30日自印尼入境，持搭機前3日內檢驗陰性報告，入境後至集中檢疫所檢疫並採檢，7月1日結果為陰性；7月8日出現輕微發燒與肌肉痠痛等症狀，7月11日仍未緩解，由衛生單位安排採檢，於今日確診。個案檢疫期間無接觸他人，同機旅客均已入住集中檢疫所，故無匡列接觸者。\$\@\$指揮中心統計，截至目前國內累計1,661,153例新型冠狀病毒肺炎相關通報(含1,644,686例排除)，其中15,302例確診，分別為1,204例境外移入，14,045例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；確診個案中，累計105例移除為空號。2020年起累計747例COVID-19死亡病例，其中739例本土，個案居住縣市分布為新北市370例、臺北市286例、基隆市25例、桃園市21例、彰化縣13例、新竹縣10例、臺中市4例、宜蘭縣、苗栗縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月13日新增死亡COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
     <t>發佈日期：2021-07-13\$\@\$中央流行疫情指揮中心今(13)日表示，為順利推動我國COVID-19疫苗接種作業，自即(7/13)日起開放18歲(含)以上民眾，於「疫苗施打意願登記與預約系統」( https://1922.gov.tw/）進行第三輪意願登記，相關說明如下：\$\@\$一、意願登記時間：即日起至7月15日17時，並同步進行第三輪結算。\$\@\$二、簡訊通知時間：7月16日至7月18日將陸續以簡訊通知符合資格的民眾；收到簡訊者，才能進行預約。本輪可接種疫苗為AZ疫苗。\$\@\$三、為協助不便使用「COVID-19疫苗施打意願登記與預約系統」的民眾登記意願，請地方政府設置因地制宜的服務專線或指定人員，協助不便使用系統的民眾進行意願登記。\$\@\$指揮中心進一步表示，第二輪的意願登記已於昨(12)日17時截止，全國約有285萬人登記，其中約114萬人有意願接種AZ疫苗。系統平臺將自7月13日上午，陸續以簡訊通知符合資格的民眾，提醒收到簡訊民眾記得進行預約；施打期間為7月16日至7月22日，籲請民眾準時前往接種。\$\@\$指揮中心提醒，「COVID-19疫苗施打意願登記與預約系統」須先完成意願登記，才能在接到通知後進行預約。系統平臺會按疫苗分配情形、參照民眾所登記的意願，通知符合預約資格的民眾，收到簡訊通知者即可進行下一步預約接種。尚未收到簡訊的民眾，會於後續符合預約資格後，收到簡訊通知，所有資料皆會完整保存，請民眾放心。\$\@\$指揮中心強調，「COVID-19疫苗施打意願登記與預約系統」是為建立讓大量疫苗接種能依序穩定有效推行的機制，中央與地方腳步一致，加強疫苗接種推動，提升群體保護力，維護國人健康。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-12\$\@\$中央流行疫情指揮中心今(12)日公布國內新增24例COVID-19確定病例，分別為23例本土及1例境外移入；另確診個案中新增1例死亡。\$\@\$指揮中心表示，今日新增之23例本土病例(其中9例為居家隔離期間或期滿檢驗陽性者)，為13例男性、10例女性，年齡介於未滿10歲至90多歲，發病日介於今(2021)年6月20日至7月11日。個案分布以新北市10例為最多，其次為臺北市9例，基隆市、桃園市、新竹市及臺中市各1例；其中17例為已知感染源、4例關聯不明、2例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增1例死亡個案(案2598)，為60多歲男性，具慢性病史及其他確診者接觸史；個案於5月11日出現發燒等症狀，5月19日就醫採檢，5月20日確診並住院治療，6月11日解除隔離並出院。7月10日因其他原因死亡。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月10日累計公布14,019位確診個案中，已有11,850人解除隔離，解隔離人數達確診人數84.5%。\$\@\$指揮中心表示，今日新增1例境外移入個案(案15370)，為克羅埃西亞籍未滿10歲女童，6月28日自瑞士入境，持搭機前3日內檢驗陰性報告，入境後至防疫旅館檢疫，7月10日進行檢疫期滿前採檢，於今日確診(Ct值33)。個案在臺期間並無症狀，相關接觸者匡列中。\$\@\$指揮中心統計，截至目前國內累計1,639,921例新型冠狀病毒肺炎相關通報(含1,622,834例排除)，其中15,273例確診，分別為1,203例境外移入，14,017例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；確診個案中，累計105例移除為空號。自2020年起累計741例COVID-19死亡病例，其中733例本土，個案居住縣市分布為新北市369例、臺北市283例、基隆市25例、桃園市21例、彰化縣12例、新竹縣9例、臺中市4例、宜蘭縣、苗栗縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-12\$\@\$中央流行疫情指揮中心今(12)日表示，本土確診案例自今(2021)年7月2日起已連續低於50人，為兼顧國內產業用人需求及移工工作權益，爰自7月13日起恢復移工轉換雇主或工作。至於移工調派及工作延伸，考量移工流動性較高，仍暫緩解封，未來將視疫情再行檢討。\$\@\$指揮中心說明，7月1日已公佈優先恢復家庭類移工轉換至家庭類雇主，新雇主需為移工安排檢驗PCR。近期評估國內整體疫情及產業發展需要，將自7月13日起恢復家庭類以外類別之移工辦理轉換雇主，新雇主接續聘僱(含期滿轉換)移工應辦理以下事項：\$\@\$一、安排移工核酸檢驗（下稱PCR）：承接移工之新雇主應於接續聘僱日（含期滿轉換）前3日內安排移工檢驗PCR。但工作所在地之醫療院所假日期間未提供檢驗服務或檢驗能量已額滿者，得例外延後至接續聘僱日起3日內檢驗PCR。等待檢驗PCR結果期間，新雇主應安排移工1人1室，落實防疫措施，檢驗費用應由新雇主支付。\$\@\$二、雇主應依指引辦理防疫措施：倘若接續聘僱移工檢測PCR確診時，新雇主應負雇主責任，並依勞動部「因應嚴重特殊傳染性肺炎雇主聘僱移工指引：移工工作、生活及外出管理注意事項」(下稱雇主指引)，配合衛生單位安排就醫或送集中檢疫所隔離治療，並依確診個案處置及解除隔離治療條件續處。倘若接續聘僱移工檢測PCR陰性，新雇主應依雇主指引，每日進行移工健康監測及記錄移工出入足跡。\$\@\$指揮中心進一步表示，新雇主接續聘僱(含期滿轉換)移工，如未於上開規定期限內安排移工檢驗PCR，或於等待PCR檢驗結果期間，未落實移工1人1室，將依就業服務法規定，處新臺幣6萬至30萬元罰鍰及不予核發接續聘僱許可。另雇主如委託仲介公司辦理移工生活照顧，因仲介公司未善盡受任事務，違反防疫措施，將依仲介公司違反就業服務法規定，處新臺幣6萬元以上至30萬元以下罰鍰。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-11\$\@\$中央流行疫情指揮中心今(11)日表示，為順利推動我國COVID-19疫苗接種作業，自即日起全國50歲(含)以上及18歲(含)以上第9類具有易導致嚴重疾病之高風險疾病者、罕見疾病及重大傷病者均可於「疫苗施打意願登記與預約系統」（ https://1922.gov.tw/ ）進行意願登記，相關說明如下：\$\@\$一、意願登記時間：即日起至7月12日17時，並同步進行第一輪結算。\$\@\$二、簡訊通知時間：7月13日至7月15日將陸續以簡訊通知符合資格的民眾；收到簡訊者，才能進行預約。\$\@\$三、最快將於7月16日進行接種，未來三週均為AZ疫苗。\$\@\$四、為協助不便使用「COVID-19疫苗施打意願登記與預約系統」的民眾登記意願，請地方政府設置因地制宜的服務專線或指定人員，協助不便使用系統的民眾進行意願登記。\$\@\$指揮中心提醒，「COVID-19疫苗施打意願登記與預約系統」須先完成意願登記後，才能在接到通知後進行預約。系統平臺會按疫苗分配情形、參照民眾所登記的意願，通知符合預約資格的民眾，收到簡訊通知者即可進行下一步預約接種。尚未收到簡訊的民眾，會於後續符合預約資格後，收到簡訊通知，所有資料皆會完整保存，請民眾放心。\$\@\$指揮中心強調，「COVID-19疫苗施打意願登記與預約系統」是為建立讓大量疫苗接種能依序穩定有效推行的機制，中央與地方腳步一致，加強疫苗接種推動，提升群體保護力，維護國人健康。\$\@\$備註：\$\@\$1. 第9類對象為18-64歲具有易導致嚴重疾病之高風險疾病者、罕見疾病及重大傷病者。\$\@\$(1) 高風險疾病者定義： https://reurl.cc/R02Qx6\$\@\$(2) 罕見疾病定義： https://reurl.cc/Nr2E36\$\@\$(3) 重大傷病者請依健保卡註記或重大傷病卡為主\$\@\$2. 第10類對象為50-64歲成人。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-11\$\@\$中央流行疫情指揮中心今(11)日公布國內新增31例COVID-19確定病例，分別為28例本土及3例境外移入；另確診個案中新增4例死亡。\$\@\$指揮中心表示，今日新增之28例本土病例(其中10例為居家隔離期間或期滿檢驗陽性者)，為15例男性、13例女性，年齡介於未滿5歲至90多歲，發病日介於今(2021)年6月26日至7月10日。個案分布以新北市12例為最多，其次為臺北市11例、桃園市2例，新竹縣、彰化縣及臺中市各1例；其中15例為已知感染源、9例關聯不明、4例調查中，相關疫情調查持續進行中。\$\@\$指揮中心說明，今日新增4例死亡個案，為2例男性、2例女性，年齡介於40多歲至70多歲，發病日介於5月22日至6月22日，確診日介於5月25日至7月6日，死亡日介於7月7日至7月9日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至7月9日累計公布13,986位確診個案中，已有11,802人解除隔離，解隔離人數達確診人數84.4%。\$\@\$指揮中心表示，今日新增3例境外移入個案中，案15342為本國籍30多歲男性，7月8日自沙烏地阿拉伯返臺，持有搭機前3日內檢驗陰性報告，入境後在機場採檢，並入住防疫旅館，於今日確診；個案在臺期間並無症狀，相關接觸者匡列中。案15351為菲律賓籍30多歲船員，5月17日自菲律賓來臺工作，持有搭機前3日內檢驗陰性報告，入境後至集中檢疫所檢疫，檢疫期滿前採檢結果為陰性即登船出海工作，7月10日返臺並採檢，於今日確診；個案出海工作及在臺期間並無症狀，相關接觸者匡列中。案15353為本國籍40多歲男性，7月10日自印尼返臺，持有搭機前3日內檢驗陰性報告，入境後在機場採檢，於今日確診；個案7月11日出現發燒症狀，已於醫院隔離治療，相關接觸者匡列中。\$\@\$指揮中心統計，截至目前國內累計1,625,351例新型冠狀病毒肺炎相關通報(含1,608,702例排除)，其中15,249例確診，分別為1,202例境外移入，13,994例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計105例移除為空號。自2020年起累計740例COVID-19死亡病例，其中732例本土，個案居住縣市分布為新北市368例、臺北市283例、基隆市25例、桃園市21例、彰化縣12例、新竹縣9例、臺中市4例、宜蘭縣、苗栗縣及花蓮縣各2例，臺東縣、雲林縣、南投縣及高雄市各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$7月11日新增死亡COVID-19確診個案表.pdf</t>
   </si>
 </sst>
 </file>
@@ -665,7 +653,7 @@
         <v>25</v>
       </c>
       <c r="C2" s="2">
-        <v>44395</v>
+        <v>44396</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>45</v>
@@ -682,7 +670,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="2">
-        <v>44395</v>
+        <v>44396</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>46</v>
@@ -699,7 +687,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="2">
-        <v>44394</v>
+        <v>44396</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>47</v>
@@ -716,7 +704,7 @@
         <v>28</v>
       </c>
       <c r="C5" s="2">
-        <v>44393</v>
+        <v>44396</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>48</v>
@@ -733,7 +721,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="2">
-        <v>44393</v>
+        <v>44395</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>49</v>
@@ -750,7 +738,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="2">
-        <v>44393</v>
+        <v>44395</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>50</v>
@@ -767,7 +755,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="2">
-        <v>44392</v>
+        <v>44394</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>51</v>
@@ -784,7 +772,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="2">
-        <v>44392</v>
+        <v>44393</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>52</v>
@@ -801,10 +789,13 @@
         <v>33</v>
       </c>
       <c r="C10" s="2">
-        <v>44392</v>
+        <v>44393</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>53</v>
+      </c>
+      <c r="E10" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -815,13 +806,10 @@
         <v>34</v>
       </c>
       <c r="C11" s="2">
-        <v>44392</v>
+        <v>44393</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="E11" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -832,7 +820,7 @@
         <v>35</v>
       </c>
       <c r="C12" s="2">
-        <v>44391</v>
+        <v>44392</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>55</v>
@@ -849,13 +837,10 @@
         <v>36</v>
       </c>
       <c r="C13" s="2">
-        <v>44391</v>
+        <v>44392</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="E13" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -866,10 +851,13 @@
         <v>37</v>
       </c>
       <c r="C14" s="2">
-        <v>44390</v>
+        <v>44392</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>57</v>
+      </c>
+      <c r="E14" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -880,7 +868,7 @@
         <v>38</v>
       </c>
       <c r="C15" s="2">
-        <v>44390</v>
+        <v>44392</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>58</v>
@@ -897,13 +885,10 @@
         <v>39</v>
       </c>
       <c r="C16" s="2">
-        <v>44390</v>
+        <v>44391</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="E16" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -914,7 +899,7 @@
         <v>40</v>
       </c>
       <c r="C17" s="2">
-        <v>44389</v>
+        <v>44391</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>60</v>
@@ -928,13 +913,10 @@
         <v>41</v>
       </c>
       <c r="C18" s="2">
-        <v>44389</v>
+        <v>44390</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="E18" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -945,13 +927,10 @@
         <v>42</v>
       </c>
       <c r="C19" s="2">
-        <v>44389</v>
+        <v>44390</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="E19" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -962,13 +941,13 @@
         <v>43</v>
       </c>
       <c r="C20" s="2">
-        <v>44388</v>
+        <v>44390</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -979,13 +958,10 @@
         <v>44</v>
       </c>
       <c r="C21" s="2">
-        <v>44388</v>
+        <v>44389</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="E21" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20210826
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
   <si>
     <t>Press Title</t>
   </si>
@@ -31,6 +31,12 @@
     <t>Page Content</t>
   </si>
   <si>
+    <t>新增8例COVID-19確定病例，分別為2例本土及6例境外移入</t>
+  </si>
+  <si>
+    <t>公私協力積極爭取  期盼首批BNT疫苗提早到貨</t>
+  </si>
+  <si>
     <t>針對8月23日至8月29日完成第一劑接種高端疫苗民眾，後續第二劑接種說明</t>
   </si>
   <si>
@@ -61,6 +67,33 @@
     <t>因應帛琉出現確診個案，指揮中心啟動相關檢疫應變措施</t>
   </si>
   <si>
+    <t>COVID-19公費疫苗預約平台增加開放8月16日以後新增或加選登記高端疫苗民眾預約，於8月27日起施打</t>
+  </si>
+  <si>
+    <t>因應國內疫情趨緩，重啟境外生專案入境作業</t>
+  </si>
+  <si>
+    <t>指揮中心自8月24日至9月6日維持疫情警戒標準為第二級，請民眾持續配合防疫措施，共同維護國內社區安全</t>
+  </si>
+  <si>
+    <t>新增10例COVID-19確定病例，分別為2例本土及8例境外移入</t>
+  </si>
+  <si>
+    <t>新增9例COVID-19確定病例，分別為6例本土及3例境外移入</t>
+  </si>
+  <si>
+    <t>COVID-19公費疫苗預約平台增加開放35歲至20歲(含)民眾預約高端疫苗，於8月23日起施打</t>
+  </si>
+  <si>
+    <t>新增11例COVID-19確定病例，分別為6例本土及5例境外移入</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/MCsgPQYHX-7Y1rwdp37gRg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/aJJeOsDDOxac6JVfv7Rihw?typeid=9</t>
+  </si>
+  <si>
     <t>/Bulletin/Detail/En4toBxZv-IRT1rsaV5HRg?typeid=9</t>
   </si>
   <si>
@@ -91,6 +124,36 @@
     <t>/Bulletin/Detail/20df0rka3uytDe64smiXPw?typeid=9</t>
   </si>
   <si>
+    <t>/Bulletin/Detail/JwqUNrkd3UJjTrh__G1IWg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/s8vqd-5p3fAMcsi6juI9qQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/CH9ulKnJV8KjzHAoNAS49g?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/TMBzM2ScpzGt4E13V2gfiA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/zrW7NHh2Fvz07rrCKMjwkw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/ec1AizBRzil-FR1eJbYJGA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/WtKfUsA_vl63jWz7H9vufw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/MCSodz6QzYMEGxgwoZMdYg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/MCsgPQYHX-7Y1rwdp37gRg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/aJJeOsDDOxac6JVfv7Rihw?typeid=9</t>
+  </si>
+  <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/En4toBxZv-IRT1rsaV5HRg?typeid=9</t>
   </si>
   <si>
@@ -121,6 +184,36 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/20df0rka3uytDe64smiXPw?typeid=9</t>
   </si>
   <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/JwqUNrkd3UJjTrh__G1IWg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/s8vqd-5p3fAMcsi6juI9qQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/CH9ulKnJV8KjzHAoNAS49g?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/TMBzM2ScpzGt4E13V2gfiA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/zrW7NHh2Fvz07rrCKMjwkw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/ec1AizBRzil-FR1eJbYJGA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/WtKfUsA_vl63jWz7H9vufw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/MCSodz6QzYMEGxgwoZMdYg?typeid=9</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-08-26\$\@\$中央流行疫情指揮中心今(26)日公布國內新增8例COVID-19確定病例，分別為2例本土及6例境外移入；另確診個案中新增2例死亡。\$\@\$指揮中心表示，今日新增2例本土病例中，案16055為越南籍30多歲男性，因曾接觸確診者(案16006)， 8月19日由衛生單位安排採檢(核酸檢驗結果為陰性)並進行居家隔離，8月25日出現喉嚨痛、喉嚨癢及頭痛症狀，由衛生單位安排就醫採檢，於今日確診(Ct值14.9)。案16056為本國籍20多歲女性，因曾接觸確診者(案15969)，8月16日由衛生單位安排採檢(核酸檢驗結果為陰性)並進行居家隔離，8月17日出現喉嚨癢及咳嗽症狀，並於隔日緩解，8月25日接受隔離期滿前採檢，於今日確診(Ct值24)。由於2例個案隔離期間未與他人接觸，且就醫期間之相關接觸者均有適當防護，故皆無匡列接觸者。\$\@\$指揮中心說明，今日新增2例死亡個案中，案14517為80多歲男性，具慢性病史、無相關活動接觸史；6月23日因發燒就醫，6月24日採檢並住院隔離治療，6月25日確診，8月4日解除隔離，8月20日死亡。案14837為70多歲男性，具慢性病史及其他確診個案接觸史；6月27日因出現咳嗽、疲倦症狀就醫採檢，6月28日住院隔離治療，6月29日確診，7月14日解除隔離並出院，8月20日因其他原因死亡。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至8月24日累計公布14,739位確診個案中，已有13,644人解除隔離，解隔離人數達確診人數92.6%。\$\@\$指揮中心說明，今日新增6例境外移入個案，為3例男性、3例女性，年齡介於10多歲至50多歲，分別自美國(案16050、16052、16057)、日本(案16051、16053)及中國(案16054)入境，入境日介於8月2日至8月24日，均持有搭機前3日內檢驗陰性報告；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計2,573,538例新型冠狀病毒肺炎相關通報(含2,556,336例排除)，其中15,947例確診，分別為1,385例境外移入，14,509例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計110例移除為空號。2020年起累計832例COVID-19死亡病例，其中824例本土，個案居住縣市分布為新北市409例、臺北市315例、基隆市28例、桃園市26例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、臺南市、南投縣、高雄市及屏東縣各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$8月26日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-08-25\$\@\$中央流行疫情指揮中心今(25)日表示，日前接獲台積電主動告知，鴻海永齡亦提供相關訊息表示，有另一批上海復星代理的BNT原廠疫苗，將於8月下旬出廠，而這批疫苗比捐贈單位預定的首批供應期程還要早，許多國家都在積極爭取，若臺灣不爭取，這批疫苗可能將送往其他國家。\$\@\$指揮中心表示，基於BNT疫苗可以施打12-18歲的青少年學生族群，而9月又即將開學，只要這批疫苗能夠確認是原廠出貨，而且經過安全檢驗，政府當然願意爭取這批疫苗，而疫苗早一天進來，讓學生能早日施打，家長、老師、學生都可以早一天安心。\$\@\$指揮中心指出，這批復星公司另案代理本要銷往他處的疫苗，在外盒包裝印有復必泰的品名，瓶身上則有復星醫藥等中文字樣，雖然這與原約定的標示方式不同，但政府仍願意積極爭取這批可以提早到來的疫苗，而且這批疫苗仍然是原廠製造、包裝並直送臺灣，只要確保疫苗品質安全無虞，當可在標示方式上給予彈性，所以政府接受可以照原來印的標示供貨，以利爭取這批疫苗早日供應國人使用。\$\@\$指揮中心表示，政府很感謝台積電的協助，也很感謝鴻海創辦人郭台銘先生，人在歐洲的這段期間也努力幫忙爭取，後續相關進度會再跟大家報告。從洽購疫苗，到爭取首批BNT的疫苗提早到貨，這都是官民合作的成果，對於包括鴻海永齡、台積電、慈濟三個企業和民間團體的協助，政府要再次表達由衷的感謝。\$\@\$指揮中心強調，防疫是政府唯一的考量，重要的是這個疫苗的內容物是安全有效的，輸入臺灣之後，仍要經過食藥署的檢驗封緘，確實有達到標準、安全無虞，才會開放讓民眾接種。</t>
+  </si>
+  <si>
     <t>發佈日期：2021-08-25\$\@\$中央流行疫情指揮中心今(25)日表示，自8月23日至8月29日完成第一劑高端COVID-19疫苗接種之民眾，COVID-19公費疫苗預約平台預計於9月27日提供接種第二劑，屆時符合預約資格或收到簡訊提醒者即可預約接種。另若有出國急迫性須於第一劑後滿28天接種者，請地方政府衛生局指定轄內合約醫療院所於預約平台開打(9月27日)前酌情提供接種。\$\@\$指揮中心指出，高端疫苗目前第二劑接種間隔至少28天，已於國內接種第一劑高端COVID-19疫苗之民眾，若因緊急出國需提前接種第二劑疫苗者，可提供具有付款紀錄之機票與出國日程及留學入學證明或公司外派出國等證明文件，至指定之合約醫療院所，經醫師評估後進行接種。\$\@\$指揮中心提醒，民眾前往接種COVID-19第二劑疫苗前，請備妥「COVID-19疫苗接種紀錄卡」及「健保卡」，若「COVID-19疫苗接種紀錄卡」已遺失，民眾可返回第一劑接種之醫療院所補發，再完成第二劑接種。於接種前，接種單位需核對民眾身分資料、主動詢問民眾疫苗接種史，檢視民眾COVID-19疫苗接種紀錄卡紀錄及健保卡註記貼紙資料，如均無相關接種證明或資訊者，除可使用網路連線「全國性預防接種資訊管理系統」(NIIS)查詢子系統查詢疫苗接種史，合約醫療院所亦可透過雲端藥歷系統等連結查詢，以確認疫苗接種間隔及廠牌是否符合規範。</t>
   </si>
   <si>
@@ -139,10 +232,40 @@
     <t>發佈日期：2021-08-24\$\@\$中央流行疫情指揮中心今(24)日公布國內新增6例COVID-19確定病例，分別為1例本土及5例境外移入；另確診個案中新增1例死亡。\$\@\$指揮中心表示，今日新增之1例本土病例(案16044)，為本國籍70多歲男性，8月22日因其他原因就醫，採檢後於今日確診(Ct值37.7)；衛生單位已啟動醫院及社區調查與防治，目前匡列家庭接觸者1人，列居家隔離，其餘接觸者匡列中。\$\@\$指揮中心說明，今日新增1例死亡個案(案15877)，為80多歲女性，具慢性病史及其他確診個案接觸史，7月27日出現食慾不振症狀，並於同日死亡；後因同住家人確診(案15851)，故於8月5日進行採檢，8月6日確診(Ct值23.8)。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至8月22日累計公布14,727位確診個案中，已有13,621人解除隔離，解隔離人數達確診人數92.5%。\$\@\$今日新增5例境外移入個案均為男性，年齡介於10多歲至40多歲，分別自日本(案16043、16045、16048)、印度(案16046)、土耳其(16047)入境，均持有搭機前3日內檢驗陰性報告，入境日介於8月12日至8月22日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計2,524,269例新型冠狀病毒肺炎相關通報(含2,507,456例排除)，其中15,938例確診，分別為1,378例境外移入，14,507例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計110例移除為空號。2020年起累計829例COVID-19死亡病例，其中821例本土，個案居住縣市分布為新北市408例、臺北市314例、基隆市28例、桃園市26例、彰化縣15例、新竹縣12例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、臺南市、南投縣、高雄市及屏東縣各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$8月24日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
+    <t>發佈日期：2021-08-23\$\@\$中央流行疫情指揮中心今(23)日表示，全球Delta變異株日益擴散且其傳播力強，我國境外移入病例有增加趨勢，為降低該病毒進入國內社區風險，與及時偵測國內病例阻斷傳播鏈，擬定COVID-19加強監測方案如下：\$\@\$(一)社區加強監測：8月30日將配置公費COVID-19家用快篩試劑於各縣市合約診所，由醫師判斷對具高風險民眾提供試劑，由民眾自行居家篩檢並回報快篩結果。檢驗為陽性時，再前往社區採檢站或採檢院所進行PCR檢測複驗，以強化基層診所監測能力。\$\@\$(二)國際機場特定高風險工作人員重點監測：8月30日起於桃園、臺北、臺中與高雄等四個國際機場之特定高風險工作人員，每7天以公費家用快篩試劑採檢一次，如檢驗為陽性者，再進行公費PCR檢測，以強化邊境監測能力。\$\@\$(三)廢汙水監測：擴大全國汙水SARS-CoV-2病毒監測範圍，由11處擴充為22處，以早期偵測社區中SARS-CoV-2病毒傳播狀況。\$\@\$(四)捐血人血清抗體陽性盛行率調查：針對110年4-7月份臺灣地區捐血中心捐血人之血液存檔樣本，抽樣5,000個檢體進行抗核蛋白及棘蛋白抗體檢測，以分析自然感染或接種疫苗的抗體陽性比例之地理分布及趨勢變化。\$\@\$(五)邊境進口冷凍食品包裝監測：持續在邊境採樣檢驗進口冷凍肉品、水產品及水果之內、外包裝，監控進口冷凍食品內、外包裝之SARS-CoV-2病毒污染狀況及評估消毒作業效果，以防止病毒透過進口食品包裝污染而入境我國。\$\@\$指揮中心進一步指出，目前國內疫情雖穩定控制中，但面臨Delta病毒變異株的威脅無可避免，需持續強化邊境與社區監測及各項防疫作為，避免病毒入侵社區。指揮中心未來將持續觀察疫情態勢，適度調整加強監測方案。</t>
+  </si>
+  <si>
     <t>發佈日期：2021-08-23\$\@\$中央流行疫情指揮中心今(23)日公布國內新增6例COVID-19確定病例，分別為4例本土及2例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增之4例本土病例(其中2例為居家隔離期間陽性者)，為2例男性、2例女性，年齡介於20多歲至70多歲，其中2例發病日分別為今(2021)年8月15日、8月20日，餘2例為無症狀感染。個案分布均在新北市；其中2例為已知感染源、2例關聯不明，將持續進行疫情調查，以釐清感染源。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至8月21日累計公布14,717位確診個案中，已有13,601人解除隔離，解隔離人數達確診人數92.4%。\$\@\$指揮中心說明，今日新增2例境外移入個案中，案16037為俄羅斯籍20多歲女性，未接種COVID-19疫苗，8月11日自俄羅斯來臺就學，持搭機3日內檢驗陰性證明，個案入境於機場採檢結果陰性，至防疫旅館檢疫，8月20日有鼻塞等症狀，8月21日由衛生單位安排採檢，於今日確診。個案檢疫期間無接觸他人，故無匡列接觸者。案16038為40多歲立陶宛籍男性，未接種COVID-19疫苗，8月13日自立陶宛來臺工作，持搭機3日內檢驗陰性證明，個案入境於機場採檢結果陰性，至防疫旅館檢疫，8月21日出現發燒、咳嗽等症狀，由衛生單位安排採檢，於今日確診。個案檢疫期間無接觸他人，故無匡列接觸者。\$\@\$指揮中心統計，截至目前國內累計2,502,861例新型冠狀病毒肺炎相關通報(含2,485,203例排除)，其中15,932例確診，分別為1,373例境外移入，14,506例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計110例移除為空號。2020年起累計828例COVID-19死亡病例，其中820例本土，個案居住縣市分布為新北市407例、臺北市314例、基隆市28例、桃園市26例、彰化縣15例、新竹縣12例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、臺南市、南投縣、高雄市及屏東縣各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。</t>
   </si>
   <si>
     <t>發佈日期：2021-08-22\$\@\$中央流行疫情指揮中心今(22)日公布國內新增10例COVID-19確定病例，分別為6例本土及4例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增之6例本土病例(其中2例為居家隔離期間或期滿檢驗陽性者)，為3例男性、3例女性，年齡介於未滿5歲至90多歲，其中1例發病日為今(2021)年8月21日、餘5例為無症狀感染。個案分布為臺北市3例，新北市、桃園市及雲林縣各1例；其中3例為已知感染源、1例關聯不明、2例疫調中，將持續進行疫情調查，以釐清感染源。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至8月20日累計公布14,707位確診個案中，已有13,580人解除隔離，解隔離人數達確診人數92.3%。\$\@\$指揮中心說明，今日新增4例境外移入個案，為2例男性、2例女性，年齡介於30多歲至50多歲，分別自日本(案16028)、德國(案16029)、南非(案16030)及印度(案16036)入境，入境日介於8月8日至8月20日，均持有搭機前3日內檢驗陰性報告；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計2,489,074例新型冠狀病毒肺炎相關通報(含2,471,769例排除)，其中15,926例確診，分別為1,371例境外移入，14,502例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計110例移除為空號。2020年起累計828例COVID-19死亡病例，其中820例本土，個案居住縣市分布為新北市407例、臺北市314例、基隆市28例、桃園市26例、彰化縣15例、新竹縣12例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、臺南市、南投縣、高雄市及屏東縣各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$8月22日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-08-21\$\@\$中央流行疫情指揮中心今(21)日表示，帛琉衛生部於今日上午發布新聞稿表示，當地2位帛琉籍民眾自8月15日自關島入境，於入境後第5日COVID-19採檢檢驗陽性。帛國政府已立即採取隔離及接觸者採檢等應變措施，目前所有人員檢驗結果均為陰性，該國並將在第10天的隔離規定後再次採檢，2位進入帛琉後活動範圍不大，初步研判帛國疫情似並未擴散。此外，帛國政府已於本日重啟「緊急應變中心」（Emergency Operations Center），擴大執行疫調並追蹤詳細接觸史，密切監控疫情發展。外交部、我國駐帛琉大使館及相關單位持續掌握此案發展，並與該國保持密切聯繫。\$\@\$指揮中心說明，因應此次帛琉出現確診個案，自帛琉入境旅客，除維持自帛琉返臺入境時於機場配合採深喉唾液PCR檢測，參加臺帛旅遊泡泡之旅客於機場應落實與其他國際旅客分流，並於檢驗陰性後採「5+9」模式，於入境第0日至第5日進行加強自主健康管理，第5日自費進行PCR檢測取得陰性報告後，最快第6日起改一般自主健康管理外，另增加入境後第12-14日須公費進行PCR檢測。\$\@\$指揮中心進一步指出，加強自主健康管理期間，除一起前往旅遊及返臺者外，應入住防疫旅宿或符合1人1室之居所，且需有單獨房間與專用衛浴，共同生活者應一起採取適當防護措施，包含佩戴口罩，保持社交距離，不可共食。若沒有出現任何症狀，可以外出，但僅能從事固定且有限度之活動，且不可搭乘大眾運輸，禁止至人潮擁擠場所，採實名制，需記錄每日活動及接觸人員，不可接觸不特定人士，且應全程佩戴口罩及保持社交距離，並於入境後14天內遵守自主健康管理應注意事項。\$\@\$指揮中心提醒，欲赴帛琉旅客，同樣搭機當日於機場採檢PCR陰性，始得搭機，若檢出陽性者應配合疫情調查，其密切接觸者(如：同行家人等)亦應暫緩搭機；防疫期間赴帛琉旅遊，務請確實遵守指揮中心及帛國的防疫措施，如佩戴口罩、勤洗手及保持社交距離等規範，以維護自身的健康安全。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-08-21\$\@\$中央流行疫情指揮中心今(21)日表示，「COVID-19公費疫苗預約平台」將於今(2021)年8月21日中午12時進行意願登記結算，並於8月23日上午10時至8月24日下午6時止，增加開放8月16日下午2時以後新登記或加選意願登記為高端疫苗之民眾進行預約。\$\@\$指揮中心說明，本期可接種疫苗為高端疫苗，上述符合預約資格者，即得於開放預約期間進行預約，亦將於開放預約後，陸續收到提醒簡訊，請記得進行預約。此次增加開放對象預定於8月27日至8月29日施打，並視疫苗供應期程調整接種場次，籲請民眾屆時準時前往接種。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-08-21\$\@\$中央流行疫情指揮中心今(21)日表示，今(2021)年5月17日考量國內及國際COVID-19疫情升溫，宣布自5月19日開始，暫停未持居留證之非本國籍人士入境，因此教育部配合指揮中心邊境嚴管措施，暫停境外學生入境申請作業。現經評估國內疫情趨緩，且110學年度開學在即，教育部專案簽請指揮中心8月20日同意，重新開放110學年度境外學位生及華語受獎生等申請入境。\$\@\$指揮中心說明，有關重啟境外生專案入境作業，重要原則如下，並請學校預為通知境外生準備：\$\@\$一、入境前：\$\@\$1.新生及未持有效簽證/居留證/中華民國入境許可證之學生，由學校先行造冊送部函轉外交部領事事務局及內政部移民署受理學生辦理簽證或入出境許可證。\$\@\$2.學生取得簽證後，訂妥班機及檢疫場所後，通知學校透過線上申請取得同意函，並於登機前應檢具3日內COVID-19核酸檢驗陰性報告。\$\@\$二、入境後：依規定於入境時採深喉唾液PCR檢測，並於檢疫場所進行居家檢疫14天，檢疫期滿前(檢疫第12至14天)PCR檢測，此外第10至12天須以「家用快篩」採檢一次。\$\@\$三、檢疫結束後：須再進行7天自主健康管理，期滿後始得入校。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-08-21\$\@\$中央流行疫情指揮中心今(21)日表示，考量國內疫情雖趨緩但仍有零星不明感染源之本土病例，經與相關單位溝通討論及評估後，宣布自今(2021)年8月24日至9月6日維持疫情警戒標準為第二級，並將維持或調整相關管制規定如下：\$\@\$一、通案性原則：\$\@\$1. 除飲食外，外出全程佩戴口罩。\$\@\$2. 實聯制、保持社交安全距離。\$\@\$3. 營業場所及公共場域人流控管或總量管制：室內空間至少1.5米/人(2.25平方米/人)，室外空間至少1米/人(1平方米/人)。\$\@\$4. 集會活動人數上限：放寬為室內80人，室外300人，若超額則向地方主管機關提報防疫計畫。\$\@\$5. 婚宴、公祭：\$\@\$(1). 公祭遵守內政部相關防疫規定處理。\$\@\$(2). 婚宴遵守每一隔間室內80人、室外300人上限，並遵守餐飲指引不得逐桌敬酒。\$\@\$6. 餐飲管理：依照衛福部規定處理，新增同住親友聚餐不受限使用隔板、梅花座及專人分菜。\$\@\$7. 醫院探病：開放加護病房、安寧病房、呼吸照護病房、精神科病房、兒童病房、身心障礙、病況危急及住院天數達7天以上者之探病；探病者須遵守探病時段、人數限制及出具篩檢陰性證明等規定。\$\@\$8. 符合主管機關防疫管理指引或規範得開放：K書中心、室內遊樂園、海釣場、海泳/浮潛等水域活動。\$\@\$二、仍須關閉之場所：\$\@\$1. 歌廳、舞廳、夜總會、俱樂部、酒家、酒吧、酒店(廊)、錄影節目帶播映場所(MTV)、視聽歌唱場所(KTV)、理容院(觀光理髮、視聽理容)。\$\@\$2. 遊藝場所、電子遊戲場、資訊休閒場所、休閒麻將館及其他類似場所。\$\@\$指揮中心說明，目前國內疫情穩定控制中，為兼顧防疫與民眾的生活品質，未來將持續觀察疫情態勢，循序漸進，適度放寬管制措施；面對病毒變異株的威脅，將持續強化邊境監測及防疫作為，籲請民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-08-21\$\@\$中央流行疫情指揮中心今(21)日公布國內新增10例COVID-19確定病例，分別為2例本土及8例境外移入；另確診個案中新增1例死亡。\$\@\$指揮中心表示，今日新增之2例本土病例(均非居家隔離期間檢驗陽性者)，為新北市40多歲男性及50多歲女性，分別於8月16日及8月19日發病；其中1例關聯不明、1例疫調中，將持續進行疫情調查，以釐清感染源。\$\@\$指揮中心說明，今日新增1例死亡個案(案9244)，為60多歲男性，具慢性病史，無相關接觸史，5月25日出現發燒、流鼻涕等症狀，5月28日就醫採檢，檢驗陽性後於6月1日住院治療，6月2日確診，6月12日死亡。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至8月19日累計公布14,698位確診個案中，已有13,581人解除隔離，解隔離人數達確診人數92.4%。\$\@\$指揮中心說明，今日新增8例境外移入個案，為7例男性、1例女性，年齡介於10多歲至60多歲，分別自美國(案16018)、印度(案16019)、印尼(案16020至16022)、南非(案16023)、日本(案16024)、阿爾巴尼亞(案16025)入境，入境日介於8月18日至8月19日，均持有搭機前3日內檢驗陰性報告；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計2,472,606例新型冠狀病毒肺炎相關通報(含2,455,074例排除)，其中15,916例確診，分別為1,367例境外移入，14,496例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計110例移除為空號。2020年起累計828例COVID-19死亡病例，其中820例本土，個案居住縣市分布為新北市407例、臺北市314例、基隆市28例、桃園市26例、彰化縣15例、新竹縣12例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、臺南市、南投縣、高雄市及屏東縣各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$8月21日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-08-20\$\@\$中央流行疫情指揮中心今(20)日公布國內新增9例COVID-19確定病例，分別為6例本土及3例境外移入；另確診個案中新增1例死亡。\$\@\$指揮中心表示，今日新增之6例本土病例(其中2例為居家隔離期間檢驗陽性者)，為4例男性、2例女性，年齡介於未滿5歲至60多歲，其中3例發病日為今(2021)年8月18日、餘3例為無症狀感染。個案分布為新北市3例、臺北市2例及彰化縣1例；其中2例為已知感染源、2例關聯不明、2例疫調中，將持續進行疫情調查，以釐清感染源。\$\@\$指揮中心說明，今日新增1例死亡個案(案15492)，為60多歲男性，具慢性病史及其他確診個案接觸史，7月9日出現咳嗽症狀，7月16日因發燒及意識不清送醫並住院隔離治療，7月17日確診，8月18日死亡。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至8月18日累計公布14,692位確診個案中，已有13,550人解除隔離，解隔離人數達確診人數92.2%。\$\@\$指揮中心說明，今日新增3例境外移入個案，為2例男性、1例女性，年齡介於20多歲至40多歲，分別自羅馬尼亞(案16011)、孟加拉(案16012)及英國(案16013)入境，入境日介於8月6日至8月17日，均持有搭機前3日內檢驗陰性報告；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計2,450,350例新型冠狀病毒肺炎相關通報(含2,433,271例排除)，其中15,906例確診，分別為1,359例境外移入，14,494例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計110例移除為空號。2020年起累計827例COVID-19死亡病例，其中819例本土，個案居住縣市分布為新北市406例、臺北市314例、基隆市28例、桃園市26例、彰化縣15例、新竹縣12例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、臺南市、南投縣、高雄市及屏東縣各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$8月20日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-08-19\$\@\$中央流行疫情指揮中心今(19)日公布國內新增6例COVID-19確定病例，分別為1例本土及5例境外移入；另確診個案中新增5例死亡。\$\@\$指揮中心表示，今日新增之1例本土病例(案16006)，為本國籍50多歲男性，近期無國內外旅遊史，今(2021)年8月18日陪家人就醫，因家人需住院治療，故於同日接受陪病者採檢，於今日確診(Ct值22.7)；個案為無症狀感染，衛生單位已啟動醫院及社區調查與防治，相關接觸者匡列中。\$\@\$指揮中心說明，今日新增5例死亡個案，為3例男性、2例女性，年齡介於60多歲至80多歲，發病日介5月24日至6月13日，確診日介於6月2日至6月15日，死亡日介於8月13日至8月17日；詳如新聞稿附件1。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至8月17日累計公布14,681位確診個案中，已有13,545人解除隔離，解隔離人數達確診人數92.3%。\$\@\$指揮中心說明，今日新增5例境外移入個案，為4例男性、1例女性，年齡介於20多歲至50多歲，分別自美國(案16002)、立陶宛(案16003)、越南(案16004)、阿拉伯聯合大公國(杜拜) (案16005)及伊朗(案16007)入境，均持有搭機前3日內檢驗陰性報告，入境日介於8月6日至8月17日；詳如新聞稿附件2。\$\@\$指揮中心統計，截至目前國內累計2,429,464例新型冠狀病毒肺炎相關通報(含2,411,951例排除)，其中15,897例確診，分別為1,356例境外移入，14,488例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計110例移除為空號。2020年起累計826例COVID-19死亡病例，其中818例本土，個案居住縣市分布為新北市406例、臺北市314例、基隆市28例、桃園市26例、彰化縣15例、新竹縣12例、臺中市4例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、臺南市、南投縣、高雄市及屏東縣各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$附件1-8月19日新增死亡COVID-19確診個案表.pdf\$\@\$附件2-8月19日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-08-18\$\@\$中央流行疫情指揮中心今(18)日表示，「COVID-19公費疫苗預約平台」( https://1922.gov.tw/ )自8月16日10時起，已開放高端疫苗預約，至今日12時截止，總計約41.9萬人完成預約，並將於8月23日至8月29日施打。惟為利疫苗資源有效利用，將自8月18日16時至8月20日12時止，增加開放「8月13日12時以前意願登記，且為35歲至20歲(含)[即2001年8月23日(含)以前出生]民眾預約，估計約有29.8萬人。\$\@\$指揮中心說明，請符合上述預約接種資格者，可於開放預約期間進行預約，亦將於開放預約後，陸續收到提醒簡訊，請記得進行預約。此次增加開放對象同樣預定於8月23日至8月29日施打，並視疫苗供應期程調整接種場次，籲請民眾屆時準時前往接種。\$\@\$指揮中心提醒，前次(8月16日10時至8月18日12時止)已宣布之符合預約資格對象，包含「65歲以上長者」、「64歲至20歲(含)第九類對象」以及「64歲至36歲(含)民眾」，依原預約時間，已於8月18日中午12時停止預約及修改；8月18日16時至8月20日12時，則僅開放上述增加開放對象進行預約。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-08-18\$\@\$中央流行疫情指揮中心今(18)日公布國內新增11例COVID-19確定病例，分別為6例本土及5例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增之6例本土病例(均非居家隔離期間陽性者)，為2例男性、4例女性，年齡介於20多歲至80多歲，其中1例8月14日發病，餘均為無症狀感染，個案分布為臺北市4例、新北市2例；其中2例為已知感染源、4例關聯不明，將持續進行疫情調查，以釐清感染源。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至8月16日累計公布14,663位確診個案中，已有13,214人解除隔離，解隔離人數達確診人數90.1%。\$\@\$指揮中心說明，今日新增5例境外移入個案，為1名男性、4名女性，年齡介於20多歲至40多歲，分別自美國(案15996、案15998)、阿拉伯聯合大公國(杜拜)(案15997)、印度(案15999)、法國(案16000)入境，入境日介於5月17日至8月15日，均持有搭機前3日內檢驗陰性報告。詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計2,407,073例新型冠狀病毒肺炎相關通報(含2,389,646例排除)，其中15,891例確診，分別為1,351例境外移入，14,487例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計110例移除為空號。2020年起累計821例COVID-19死亡病例，其中813例本土，個案居住縣市分布為新北市402例、臺北市313例、基隆市28例、桃園市26例、彰化縣15例、新竹縣12例、臺中市4例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、臺南市、南投縣、高雄市及屏東縣各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$8月18日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
 </sst>
 </file>
@@ -517,7 +640,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -545,16 +668,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2">
-        <v>44433</v>
+        <v>44434</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -562,16 +685,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2">
         <v>44433</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -579,16 +702,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2">
         <v>44433</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -596,16 +719,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2">
-        <v>44432</v>
+        <v>44433</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -613,16 +736,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C6" s="2">
-        <v>44432</v>
+        <v>44433</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -630,16 +753,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C7" s="2">
         <v>44432</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -647,13 +770,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2">
-        <v>44431</v>
+        <v>44432</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>31</v>
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -661,16 +787,16 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2">
-        <v>44431</v>
+        <v>44432</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -678,16 +804,16 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2">
-        <v>44430</v>
+        <v>44431</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -695,13 +821,186 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2">
+        <v>44431</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2">
+        <v>44430</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="2">
         <v>44429</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>34</v>
+      <c r="D13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2">
+        <v>44429</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="2">
+        <v>44429</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="2">
+        <v>44429</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="2">
+        <v>44429</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="2">
+        <v>44428</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="2">
+        <v>44427</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="2">
+        <v>44426</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="2">
+        <v>44426</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -716,6 +1015,16 @@
     <hyperlink ref="D9" r:id="rId8"/>
     <hyperlink ref="D10" r:id="rId9"/>
     <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="D12" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId12"/>
+    <hyperlink ref="D14" r:id="rId13"/>
+    <hyperlink ref="D15" r:id="rId14"/>
+    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D17" r:id="rId16"/>
+    <hyperlink ref="D18" r:id="rId17"/>
+    <hyperlink ref="D19" r:id="rId18"/>
+    <hyperlink ref="D20" r:id="rId19"/>
+    <hyperlink ref="D21" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20210910
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="157">
   <si>
     <t>Press Title</t>
   </si>
@@ -31,6 +31,15 @@
     <t>Page Content</t>
   </si>
   <si>
+    <t>新增7例COVID-19確定病例，分別為2例本土及5例境外移入</t>
+  </si>
+  <si>
+    <t>指揮中心訂購AstraZeneca疫苗45.8萬劑將於今(10)日下午抵臺</t>
+  </si>
+  <si>
+    <t>國籍航空公司機組人員防疫健康管控措施作業原則會議說明</t>
+  </si>
+  <si>
     <t>台積電、鴻海永齡、慈濟三間企業和民間團體捐贈之第二批BNT疫苗91萬劑於9月9日上午抵臺</t>
   </si>
   <si>
@@ -139,13 +148,13 @@
     <t>針對8月23日至8月29日完成第一劑接種高端疫苗民眾，後續第二劑接種說明</t>
   </si>
   <si>
-    <t>新增1例境外移入COVID-19病例，自南非入境</t>
-  </si>
-  <si>
-    <t>我國COVID-19科技防疫APEC視訊國際研討會首登場，增進亞太地區團結抗疫及應變能力</t>
-  </si>
-  <si>
-    <t>指揮中心宣布自8月27日零時起，入境旅客前往檢疫地點均應搭乘「防疫車輛」，不得自行駕車前往</t>
+    <t>/Bulletin/Detail/rFB5EmwGsyKbpr0QYSaR1Q?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/v691B_c9aAFGvjZj9jes1A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/0xS-kPajD0nRI51CKtOqsA?typeid=9</t>
   </si>
   <si>
     <t>/Bulletin/Detail/82Hu5ddU8Al22gNK_wAq2Q?typeid=9</t>
@@ -259,13 +268,13 @@
     <t>/Bulletin/Detail/En4toBxZv-IRT1rsaV5HRg?typeid=9</t>
   </si>
   <si>
-    <t>/Bulletin/Detail/uqw6Rnia5LLT408IUDG9Bw?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/CdKpu9coN7HNgaRFiwz2uA?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/r99mP45_fbYuhr1y_Y7ChA?typeid=9</t>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/rFB5EmwGsyKbpr0QYSaR1Q?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/v691B_c9aAFGvjZj9jes1A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/0xS-kPajD0nRI51CKtOqsA?typeid=9</t>
   </si>
   <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/82Hu5ddU8Al22gNK_wAq2Q?typeid=9</t>
@@ -379,13 +388,13 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/En4toBxZv-IRT1rsaV5HRg?typeid=9</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/uqw6Rnia5LLT408IUDG9Bw?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/CdKpu9coN7HNgaRFiwz2uA?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/r99mP45_fbYuhr1y_Y7ChA?typeid=9</t>
+    <t>發佈日期：2021-09-10\$\@\$中央流行疫情指揮中心今(10)日公布國內新增7例COVID-19確定病例，分別為2例本土及5例境外移入；另確診個案中新增1例死亡。\$\@\$指揮中心說明，今日新增2例本土病例中，案16173為60多歲男性，9月7日出現胸痛、輕微噁心、肌肉痠痛等症狀，9月8日就醫並採檢，於今日確診，已匡列接觸者6人，列居家隔離，餘匡列中。案16179為10多歲男性， 9月8日出現胸痛、呼吸痛等症狀，9月9日就醫採檢，於今日確診，已匡列接觸者51人，列居家隔離，餘匡列中。衛生單位將持續進行疫情調查及防治，以釐清感染源。\$\@\$指揮中心表示，今日新增5例境外移入個案，分別自美國(案16174、案16175)、土耳其(案16176)、日本(案16177)、亞美尼亞(案16178)入境，入境日介於8月26日至9月8日，均持有搭機前3日內檢驗陰性報告，詳如新聞稿附件。\$\@\$指揮中心指出，今日新增1例死亡個案(案10387)，為70多歲男性，具慢性病史及其他確診者接觸史，6月3日因其他原因就醫，同日出現發燒、咳嗽等症狀，採檢後住院治療，於6月4日確診，8月26日解除隔離，9月5日死亡。\$\@\$指揮中心統計，截至目前國內累計2,938,839例新型冠狀病毒肺炎相關通報(含2,921,268例排除)，其中16,069例確診，分別為1,452例境外移入，14,563例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另累計110例移除為空號。2020年起累計839例COVID-19死亡病例，其中829例本土，個案居住縣市分布為新北市411例、臺北市318例、基隆市28例、桃園市26例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、臺南市、南投縣、高雄市及屏東縣各1例；另10例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$9月10日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-09-10\$\@\$中央流行疫情指揮中心今(10)日表示，約45.8萬劑AstraZeneca疫苗預定於今日下午3時40分抵達桃園國際機場，待完成通關程序後，直接運送至指定冷儲物流中心進行後續檢驗封緘作業，再提供COVID-19接種計畫所列實施對象接種。\$\@\$指揮中心指出，該中心係於去(2020)年10月30日與臺灣阿斯特捷利康公司簽署1,000萬劑COVID-19疫苗供應合約，截至目前總計到貨約372.7萬劑，分別為3月3日11.7萬劑、7月7日62.6萬劑、7月15日56萬劑、7月27日58.2萬劑、8月12日52.4萬劑、8月27日26.5萬劑、8月31日59.5萬劑，及本次提供第八批45.8萬疫苗。本次提供的疫苗係為多劑型包裝(每瓶10人份)，需存放於2-8℃的環境，依臨床試驗每人需施打2劑，本批效期至110年12月31日。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-09-09\$\@\$中央流行疫情指揮中心今(9)日表示，為精進國籍航空公司機組員人員防疫作為，於今日晚間召開會議，與桃園市機師職業工會、桃園市空服員職業工會、中華航空企業工會、長榮航空公司企業工會、長榮航空關係企業工會、交通部及民航局進行專業溝通及討論，說明如下：\$\@\$一、就醫問題：將與各醫師公會溝通，加強宣導醫療人員不可無故拒絕機組人員就醫。\$\@\$二、國籍航空公司機組員人員接種第三劑疫苗：將納入未來施打規劃考量，惟目前各國施打間隔不一，有6個月與9個月，需提至專家會議進行討論。\$\@\$三、機組員防護裝備問題：民航局已編列防疫經費補助航空公司採購個人防護裝備，指揮中心建議比照去年防疫經驗再行檢視，並請航空公司按民航局指示配合處理。\$\@\$指揮中心說明，為確保機組人員執勤健康及安全，將持續與相關部會進行討論，強化機組人員防疫措施，並加強職業安全衛生管理，以共同維護機組員身心健康；同時，機組員執勤時應遵守民航局訂定之相關作業規範，提高自我警覺，落實各項防疫措施、自我健康監測及異常通報機制，以維護自身及親友之健康安全。</t>
   </si>
   <si>
     <t>發佈日期：2021-09-09\$\@\$中央流行疫情指揮中心今(9)日表示，台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的第二批BNT疫苗91萬劑，已於今日上午6時18分順利運抵桃園國際機場，並在完成通關程序後，直接運送至指定冷儲物流中心進行後續檢驗封緘作業。\$\@\$指揮中心說明，由台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的BNT疫苗1,500萬劑，目前共計到貨184萬劑，分別為首批於9月2日送達的93萬劑，以及於今日送達的91萬劑。本批疫苗效期至111年1月17日，將由指揮中心統籌運用，優先開放給12歲至17歲(含)青少年族群造冊接種；其餘將優先提供已意願登記，且尚未接種過疫苗的18至22歲(含)民眾；後續將再視疫情趨勢、接種狀況及疫苗到貨情形等綜合評估，開放其他對象接種。\$\@\$對於台積電、鴻海暨永齡基金會、慈濟基金會三間企業和民間團體積極協助，提供更多的疫苗讓民眾接種，加速提升臺灣疫苗覆蓋率，指揮中心再次表達由衷的謝意。</t>
@@ -460,9 +469,6 @@
     <t>發佈日期：2021-08-31\$\@\$中央流行疫情指揮中心今(31)日公布國內新增4例COVID-19確定病例，分別為3例本土及1例境外移入；另確診個案中新增1例死亡。\$\@\$指揮中心表示，今日新增之3例本土病例(均非居家隔離期間陽性者)，為2例男性、1例女性，年齡介於30多歲至60多歲，其中1例於今(2021)年 8月16日發病，另2例於8月30日發病。個案分布為新北市2例、台北市1例；其中2例關聯不明，1例疫調中，將持續進行疫情調查，以釐清感染源。\$\@\$指揮中心說明，今日新增1例死亡個案(案16093)，為本國籍60多歲男性，8月8日於越南確診，8月28日搭乘醫療專機返臺後至醫院採檢並治療，8月29日確診，8月30日死亡。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至8月29日累計公布14,784位確診個案中，已有13,676人解除隔離，解隔離人數達確診人數92.5%。\$\@\$指揮中心表示，今日新增1例境外移入個案(案16105)，為英國籍30多歲男性，未接種COVID-19疫苗，自述6月曾於英國確診，8月17日持搭機前三日內檢驗陰性報告來臺工作，入境後至集中檢疫所採檢陰性並檢疫，8月30日進行期滿前採檢，於今日確診。個案在臺期間並無症狀，集中檢疫期間無接觸他人，故無匡列接觸者。\$\@\$指揮中心統計，截至目前國內累計2,677,839例新型冠狀病毒肺炎相關通報(含2,660,833例排除)，其中15,995例確診，分別為1,414例境外移入，14,528例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計110例移除為空號。2020年起累計835例COVID-19死亡病例，其中825例本土，個案居住縣市分布為新北市410例、臺北市315例、基隆市28例、桃園市26例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、臺南市、南投縣、高雄市及屏東縣各1例；另10例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。</t>
   </si>
   <si>
-    <t>發佈日期：2021-08-31\$\@\$中央流行疫情指揮中心今(31)日表示，約59.5萬劑AstraZeneca疫苗預定於今日下午3時40分抵達桃園國際機場，待完成通關程序後，直接運送至指定冷儲物流中心，進行後續檢驗封緘作業，再提供COVID-19接種計畫所列實施對象接種。\$\@\$指揮中心指出，該中心於去(2020)年10月30日與臺灣阿斯特捷利康公司簽署1,000萬劑COVID-19疫苗供應合約，先前已陸續到貨，分別為3月3日11.7萬劑、7月7日62.6萬劑、7月15日56萬劑、7月27日58.2萬劑、8月12日52.4萬劑、8月27日26.5萬劑，本次提供第七批疫苗，截至目前總計約327萬劑到貨。本次提供的疫苗為多劑型包裝(每瓶10人份)，需存放於2-8℃的環境，依臨床試驗每人需施打2劑，本批效期至110年12月31日。</t>
-  </si>
-  <si>
     <t>發佈日期：2021-08-30\$\@\$中央流行疫情指揮中心今(30)日表示，為降低Delta變異株進入社區風險，及時偵測國內病例以阻斷隱性傳播鏈，指揮中心即日起啟動COVID-19社區加強監測方案，透過一群守護社區健康之基層診所醫師，協助評估就醫民眾臨床症狀，視需要提供公費COVID-19家用快篩試劑，由民眾自行居家篩檢並自主回報篩檢結果，為強化偵測社區病例注入新力量。\$\@\$指揮中心表示，COVID-19社區加強監測方案將自今日開始執行至今(2021)年12月31日，目前全國18個縣市共計82家診所參與，診所名單詳如新聞稿附件；未來將視執行情形及疫情變化，調整公費快篩試劑發放診所家數。民眾如為2歲以上出現呼吸道症狀的病患至公費快篩試劑發放診所掛號就醫，經醫師判斷後，發放公費家用快篩試劑及注意事項說明單張，如為2歲以下幼兒的陪同看診者，亦由醫師判斷後發放。\$\@\$指揮中心說明，民眾領取試劑後，請配合依注意事項說明內容儘速採檢，並至線上(https://forms.gle/8gh7Kb3ZkYE5aArW7)填寫試劑領取診所名稱及快篩結果等資料，此為匿名方式收集，無須擔心個人資料外洩情形。\$\@\$指揮中心呼籲，如快篩檢驗為陽性者請儘速至鄰近的社區採檢院所( https://reurl.cc/MArG1L )進一步PCR檢驗。提醒民眾前往社區採檢院所時，請戴好口罩、勿搭乘大眾運輸工具，對於使用過之採檢器材請用塑膠袋密封包好，並攜帶至社區採檢院所，交予院所人員處理。 附件\$\@\$附件-20210830公費COVID-19家用快篩試劑發送社區定點診所名單.pdf</t>
   </si>
   <si>
@@ -472,40 +478,13 @@
     <t>發佈日期：2021-08-29\$\@\$中央流行疫情指揮中心今(29)日表示，捷克政府於7月26日宣布捐贈我國3萬劑COVID-19疫苗，經捷克衛生部與我國駐捷克代表處之通力合作安排，已於臺北時間8月27日凌晨自布拉格機場啟運，預計8月29日下午抵達桃園國際機場。該批Moderna疫苗抵臺後，將於完成通關程序後，直接運送至指定冷儲物流中心進行後續檢驗封緘作業，提供COVID-19接種計畫所列實施對象進行接種。\$\@\$指揮中心說明，值此全球疫苗供不應求時刻，捷克伸出援手提供這批COVID-19疫苗，給予國内疫情防治極大幫助，指揮中心謹向捷克政府與民眾至上誠摯謝意。</t>
   </si>
   <si>
-    <t>發佈日期：2021-08-29\$\@\$中央流行疫情指揮中心今(29)日公布國內新增23例COVID-19確定病例，分別為13例本土及10例境外移入；另確診個案中新增1例死亡。\$\@\$指揮中心表示，今日新增之13例本土病例(其中9例為居家隔離期間陽性者)，為6例男性、7例女性，年齡介於未滿5歲至50多歲，發病日介於今(2021)年8月16日至8月28日，個案分布為新北市11例、臺北市2例；其中9例為已知感染源、4例關聯不明，將持續進行疫情調查，以釐清感染源。\$\@\$指揮中心說明，今日新增1例死亡個案(案16067)，為菲律賓籍60多歲男性，8月26日出現發燒症狀，8月27日入境我國後即送醫採檢確診，並於同日死亡。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至8月27日累計公布14,755位確診個案中，已有13,673人解除隔離，解隔離人數達確診人數92.7%。\$\@\$指揮中心表示，今日新增10例境外移入個案，為7例男性、3例女性，年齡介於10多歲至60多歲，分別自中國(案16071)、柬埔寨(案16074、16075)、美國(案16076)、緬甸(案16088、16089、16090、16091)、巴基斯坦(案16092)及越南(案16093)入境，入境日介於8月15日至8月28日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計2,637,402例新型冠狀病毒肺炎相關通報(含2,619,709例排除)，其中15,983例確診，分別為1,408例境外移入，14,522例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計110例移除為空號。2020年起累計834例COVID-19死亡病例，其中825例本土，個案居住縣市分布為新北市410例、臺北市315例、基隆市28例、桃園市26例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、臺南市、南投縣、高雄市及屏東縣各1例；另9例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$8月29日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
     <t>發佈日期：2021-08-28\$\@\$中央流行疫情指揮中心今(28)日表示，「COVID-19公費疫苗預約平臺」 ( https://1922.gov.tw/ ) 自8月28日起將BNT疫苗納入意願登記選項，並維持開放18歲(含)以上民眾登記，請有意願民眾把握機會進行登記；至於12歲至17歲(含)對象，目前規劃採行流感疫苗接種模式，以校園集中接種或依通知書至地方政府衛生局指定合約醫療院所方式接種，暫不納入意願登記。另第七期將提供接種AZ疫苗，預約時間自8月29日上午10時至8月31日中午12時截止。\$\@\$指揮中心說明，第七期預約將提供於7月19日前已意願登記選擇AZ疫苗，且尚未接種過疫苗之29歲(含)以上對象[即1992年12月31日(含)以前出生]及滿18歲以上[即2003年9月3日(含)前出生]第九類對象進行接種；施打期間預計自9月3日至9月10日止，並視疫苗供應期程調整接種場次，籲請民眾屆時準時前往接種。此外，提醒符合第七期AZ疫苗預約資格對象如欲增加選擇BNT疫苗，須於8月31日下午4時後始可加選。另已符合AZ疫苗第二劑接種間隔之民眾，將另行開放接種。\$\@\$指揮中心再次提醒，請民眾於「COVID-19公費疫苗預約平臺」開放意願登記時，先進行意願登記，後續符合預約資格者才可進行下一步預約接種。系統平臺會按疫苗分配情形、參照民眾登記之意願，提供符合預約資格者進行預約接種，所有資料皆會完整保存，請民眾放心。</t>
   </si>
   <si>
-    <t>發佈日期：2021-08-28\$\@\$中央流行疫情指揮中心今(28)日公布國內新增6例境外移入COVID-19病例，分別自法國、美國、越南、巴基斯坦、柬埔寨及其他國家移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增6例境外移入個案，為3例男性、3例女性，年齡介於10多歲至60多歲，分別自法國(案16065)、美國(案16066)、其他(案16067)、越南(案16068)、巴基斯坦(案16069)、柬埔寨(案16070)入境，入境日介於今(2021)年8月7日至8月27日；詳如新聞稿附件。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至8月26日累計公布14,748位確診個案中，已有13,674人解除隔離，解隔離人數達確診人數92.7%。\$\@\$指揮中心統計，截至目前國內累計2,618,184例新型冠狀病毒肺炎相關通報(含2,600,433例排除)，其中15,960例確診，分別為1,398例境外移入，14,509例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計110例移除為空號。 2020年起累計833例COVID-19死亡病例，其中825例本土，個案居住縣市分布為新北市410例、臺北市315例、基隆市28例、桃園市26例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、臺南市、南投縣、高雄市及屏東縣各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$8月28日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-08-27\$\@\$中央流行疫情指揮中心今(27)日表示，本土疫情趨緩，指揮中心宣布8月24日至9月6日維持疫情警戒標準為第二級，考量疫情維持穩定及住宿式長照機構住民探視之需求，前已於8月10日宣布，全國住宿式長照機構除臺北市及新北市維持暫停訪客(除例外情形)外，其他縣市則有條件開放探視。\$\@\$現經指揮中心評估，臺北市及新北市的社區感染風險等級已調降至中風險，故自8月31日起，可比照其他縣市開放訪客，說明如下：\$\@\$一、訪客須出具訪視前3天內採檢之自費篩檢陰性證明；若訪客為「確診者取得解除隔離治療通知書且距發病日未滿3個月者」或「完成2劑COVID-19疫苗接種達14天(含)以上者」，可免除前述篩檢之要求。\$\@\$二、探視應遵循「衛生福利機構與榮譽國民之家因應COVID-19訪客管理作業原則」辦理，包括：落實預約制、實聯制、詢問TOCC及限制有感染症狀者進入、每位住民每次訪客人數不可超過3人、不同住民訪客間維持社交距離、進入住房探視每住房每時段原則上僅開放1位住民接受訪客探視、全程佩戴口罩等。\$\@\$指揮中心提醒，住宿式長照機構相關管理將視疫情發展，滾動修正。</t>
-  </si>
-  <si>
     <t>發佈日期：2021-08-27\$\@\$中央流行疫情指揮中心今(27)日公布國內新增7例境外移入COVID-19病例，分別自瑞典、美國、印尼(3例)及印度(2例)入境；另確診個案中新增1例死亡。\$\@\$指揮中心表示，今日新增7例境外移入個案，為3例男性、4例女性，年齡介於20多歲至40多歲，分別自瑞典(案16058)、美國(案16059)、印尼(案16060、16061、16062)及印度(案16063、16064)入境，入境日介於今(2021)年8月13日至8月25日，均持有搭機前3日內檢驗陰性報告；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增1例死亡個案(案14879)，為60多歲男性，具慢性病史及其他確診個案接觸史；3月12日因其他原因住院，6月26日出現發燒、咳嗽及腹瀉症狀，6月29日採檢，6月30日確診，8月18日死亡。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至8月25日累計公布14,740位確診個案中，已有13,669人解除隔離，解隔離人數達確診人數92.7%。\$\@\$指揮中心統計，截至目前國內累計2,596,704例新型冠狀病毒肺炎相關通報(含2,579,632例排除)，其中15,954例確診，分別為1,392例境外移入，14,509例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計110例移除為空號。2020年起累計833例COVID-19死亡病例，其中825例本土，個案居住縣市分布為新北市410例、臺北市315例、基隆市28例、桃園市26例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、臺南市、南投縣、高雄市及屏東縣各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$8月27日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
-    <t>發佈日期：2021-08-27\$\@\$中央流行疫情指揮中心今(27)日表示，26.5萬劑AstraZeneca疫苗已於今(27)日上午11時37分抵達桃園國際機場，待完成通關程序後，直接運送至指定冷儲物流中心，進行後續檢驗封緘作業，再提供COVID-19接種計畫所列實施對象接種。\$\@\$指揮中心指出，該中心係於去(2020)年10月30日與臺灣阿斯特捷利康公司簽署1,000萬劑COVID-19疫苗供應合約，先前已陸續到貨，分為3月3日11.7萬劑、7月7日62.6萬劑、7月15日56萬劑、7月27日58.2萬劑、8月12日52.4萬劑，本次提供第六批疫苗，截至目前總計約267.4萬劑到貨。本次提供的疫苗係為多劑型包裝(每瓶10人份)，需存放於2-8℃環境，依臨床試驗每人需施打2劑，本批效期至今(2021)年12月7日。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-08-26\$\@\$中央流行疫情指揮中心今(26)日公布國內新增8例COVID-19確定病例，分別為2例本土及6例境外移入；另確診個案中新增2例死亡。\$\@\$指揮中心表示，今日新增2例本土病例中，案16055為越南籍30多歲男性，因曾接觸確診者(案16006)， 8月19日由衛生單位安排採檢(核酸檢驗結果為陰性)並進行居家隔離，8月25日出現喉嚨痛、喉嚨癢及頭痛症狀，由衛生單位安排就醫採檢，於今日確診(Ct值14.9)。案16056為本國籍20多歲女性，因曾接觸確診者(案15969)，8月16日由衛生單位安排採檢(核酸檢驗結果為陰性)並進行居家隔離，8月17日出現喉嚨癢及咳嗽症狀，並於隔日緩解，8月25日接受隔離期滿前採檢，於今日確診(Ct值24)。由於2例個案隔離期間未與他人接觸，且就醫期間之相關接觸者均有適當防護，故皆無匡列接觸者。\$\@\$指揮中心說明，今日新增2例死亡個案中，案14517為80多歲男性，具慢性病史、無相關活動接觸史；6月23日因發燒就醫，6月24日採檢並住院隔離治療，6月25日確診，8月4日解除隔離，8月20日死亡。案14837為70多歲男性，具慢性病史及其他確診個案接觸史；6月27日因出現咳嗽、疲倦症狀就醫採檢，6月28日住院隔離治療，6月29日確診，7月14日解除隔離並出院，8月20日因其他原因死亡。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至8月24日累計公布14,739位確診個案中，已有13,644人解除隔離，解隔離人數達確診人數92.6%。\$\@\$指揮中心說明，今日新增6例境外移入個案，為3例男性、3例女性，年齡介於10多歲至50多歲，分別自美國(案16050、16052、16057)、日本(案16051、16053)及中國(案16054)入境，入境日介於8月2日至8月24日，均持有搭機前3日內檢驗陰性報告；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計2,573,538例新型冠狀病毒肺炎相關通報(含2,556,336例排除)，其中15,947例確診，分別為1,385例境外移入，14,509例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計110例移除為空號。2020年起累計832例COVID-19死亡病例，其中824例本土，個案居住縣市分布為新北市409例、臺北市315例、基隆市28例、桃園市26例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、臺南市、南投縣、高雄市及屏東縣各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$8月26日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-08-25\$\@\$中央流行疫情指揮中心今(25)日表示，日前接獲台積電主動告知，鴻海永齡亦提供相關訊息表示，有另一批上海復星代理的BNT原廠疫苗，將於8月下旬出廠，而這批疫苗比捐贈單位預定的首批供應期程還要早，許多國家都在積極爭取，若臺灣不爭取，這批疫苗可能將送往其他國家。\$\@\$指揮中心表示，基於BNT疫苗可以施打12-18歲的青少年學生族群，而9月又即將開學，只要這批疫苗能夠確認是原廠出貨，而且經過安全檢驗，政府當然願意爭取這批疫苗，而疫苗早一天進來，讓學生能早日施打，家長、老師、學生都可以早一天安心。\$\@\$指揮中心指出，這批復星公司另案代理本要銷往他處的疫苗，在外盒包裝印有復必泰的品名，瓶身上則有復星醫藥等中文字樣，雖然這與原約定的標示方式不同，但政府仍願意積極爭取這批可以提早到來的疫苗，而且這批疫苗仍然是原廠製造、包裝並直送臺灣，只要確保疫苗品質安全無虞，當可在標示方式上給予彈性，所以政府接受可以照原來印的標示供貨，以利爭取這批疫苗早日供應國人使用。\$\@\$指揮中心表示，政府很感謝台積電的協助，也很感謝鴻海創辦人郭台銘先生，人在歐洲的這段期間也努力幫忙爭取，後續相關進度會再跟大家報告。從洽購疫苗，到爭取首批BNT的疫苗提早到貨，這都是官民合作的成果，對於包括鴻海永齡、台積電、慈濟三個企業和民間團體的協助，政府要再次表達由衷的感謝。\$\@\$指揮中心強調，防疫是政府唯一的考量，重要的是這個疫苗的內容物是安全有效的，輸入臺灣之後，仍要經過食藥署的檢驗封緘，確實有達到標準、安全無虞，才會開放讓民眾接種。</t>
-  </si>
-  <si>
     <t>發佈日期：2021-08-25\$\@\$中央流行疫情指揮中心今(25)日表示，自8月23日至8月29日完成第一劑高端COVID-19疫苗接種之民眾，COVID-19公費疫苗預約平台預計於9月27日提供接種第二劑，屆時符合預約資格或收到簡訊提醒者即可預約接種。另若有出國急迫性須於第一劑後滿28天接種者，請地方政府衛生局指定轄內合約醫療院所於預約平台開打(9月27日)前酌情提供接種。\$\@\$指揮中心指出，高端疫苗目前第二劑接種間隔至少28天，已於國內接種第一劑高端COVID-19疫苗之民眾，若因緊急出國需提前接種第二劑疫苗者，可提供具有付款紀錄之機票與出國日程及留學入學證明或公司外派出國等證明文件，至指定之合約醫療院所，經醫師評估後進行接種。\$\@\$指揮中心提醒，民眾前往接種COVID-19第二劑疫苗前，請備妥「COVID-19疫苗接種紀錄卡」及「健保卡」，若「COVID-19疫苗接種紀錄卡」已遺失，民眾可返回第一劑接種之醫療院所補發，再完成第二劑接種。於接種前，接種單位需核對民眾身分資料、主動詢問民眾疫苗接種史，檢視民眾COVID-19疫苗接種紀錄卡紀錄及健保卡註記貼紙資料，如均無相關接種證明或資訊者，除可使用網路連線「全國性預防接種資訊管理系統」(NIIS)查詢子系統查詢疫苗接種史，合約醫療院所亦可透過雲端藥歷系統等連結查詢，以確認疫苗接種間隔及廠牌是否符合規範。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-08-25\$\@\$中央流行疫情指揮中心今(25)日公布國內新增1例境外移入COVID-19病例(案16049)，自南非入境；另確診個案中新增1例死亡。\$\@\$指揮中心表示，案16049為南非籍20多歲男性，未接種COVID-19疫苗，於今(2021)年8月22日來臺工作，持有搭機前3日內檢驗陰性報告，入境時在機場採檢後至防疫旅館居家檢疫，於今日確診。個案在臺期間並無症狀，衛生單位已匡列同班機接觸者3人，均列居家隔離；其餘接觸者匡列中。\$\@\$指揮中心說明，新增之死亡個案(案15845)，為70多歲女性，具慢性病史及其他確診個案接觸史，7月1日因其他原因住院，8月2日因醫院有病患確診，故安排個案進行採檢，8月4日確診，8月22日死亡。\$\@\$指揮中心指出，近期確診個案解隔離情形，5月11日至8月23日累計公布14,733位確診個案中，已有13,626人解除隔離，解隔離人數達確診人數92.5%。\$\@\$指揮中心統計，截至目前國內累計2,548,825例新型冠狀病毒肺炎相關通報(含2,531,924例排除)，其中15,939例確診，分別為1,379例境外移入，14,507例本土病例，36例敦睦艦隊、2例航空器感染、1例不明及14例調查中；另累計110例移除為空號。2020年起累計830例COVID-19死亡病例，其中822例本土，個案居住縣市分布為新北市409例、臺北市314例、基隆市28例、桃園市26例、彰化縣15例、新竹縣12例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，臺東縣、雲林縣、臺南市、南投縣、高雄市及屏東縣各1例；另8例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-08-25\$\@\$疾病管制署今(25)日表示，我國運用科技進行傳染病防治工作成果獲得亞太經合會（APEC）經濟體高度肯定，並於本（110）年8月25日及26日上午9時，舉辦「APEC亞太地區傳染病數位工具應用：挑戰與機會國際研討會( Digital Tools for Addressing Infectious Disease in the Asia-Pacific Region: Challenges and Opportunities）」，由衛生福利部薛瑞元政務次長、中央研究院陳建仁院士、疾病管制署周志浩署長偕我國與18國產官學專家，於線上分享運用科技工具攜手抗疫經驗，期能增進亞太區域團結抗疫及應變能力。\$\@\$疾管署指出，COVID-19疫情在全球及亞太區域大流行，不僅對健康亦對社會與經濟發展造成重大衝擊及影響。面對疫情的威脅，薛次長致詞中表示，為因應COVID-19疫情的高度變異性，防疫亦須及時調整，單以傳統防治方式恐無法快速應對，所幸科技進步，全球數位科技已廣泛運用於COVID-19疫情監測與應變，協助防疫工作推動更順暢；期望本次研討會可強化APEC經濟體間抗疫協作與夥伴關係發展，互相交流，共同攜手合作，成功抗疫。\$\@\$疾管署說明，本研討會由陳建仁院士擔任專題講座，會中分享我國運用數位科技輔助防疫及檢疫經驗，如健保雲端系統建置「TOCC」(旅遊史、職業別、接觸史及是否群聚)提示機制、電子圍籬居家隔離系統、口罩實名制等，並由歐美亞太等18國逾40位及國內110位專家同步連線參與討論，就傳染病監測、社區防治動員、產官學合作發展創新技術及資料隱私保護等議題進行交流與分享，共同為COVID-19科技防疫工作注入新力量。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-08-24\$\@\$中央流行疫情指揮中心今(24)日表示，因應全球COVID-19疫情持續升溫，鄰近多國仍處於嚴峻或再創新高狀況，且Delta變異株流行範圍持續擴大，為阻絕疫情由境外擴散，指揮中心宣布自8月27日零時起（航班抵臺時間），入境旅客應搭乘「防疫車輛」逕至檢疫處所，不得自行駕車前往。\$\@\$指揮中心說明，前述措施將避免旅客自行駕車前往檢疫地點之路程中，接觸其他民眾的機會，減少病毒傳播風險，籲請民眾務必配合，維護我國社區防疫安全。</t>
   </si>
 </sst>
 </file>
@@ -911,7 +890,7 @@
         <v>44</v>
       </c>
       <c r="C2" s="2">
-        <v>44448</v>
+        <v>44449</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>84</v>
@@ -928,7 +907,7 @@
         <v>45</v>
       </c>
       <c r="C3" s="2">
-        <v>44448</v>
+        <v>44449</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>85</v>
@@ -945,7 +924,7 @@
         <v>46</v>
       </c>
       <c r="C4" s="2">
-        <v>44447</v>
+        <v>44448</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>86</v>
@@ -962,7 +941,7 @@
         <v>47</v>
       </c>
       <c r="C5" s="2">
-        <v>44446</v>
+        <v>44448</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>87</v>
@@ -979,7 +958,7 @@
         <v>48</v>
       </c>
       <c r="C6" s="2">
-        <v>44446</v>
+        <v>44448</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>88</v>
@@ -996,7 +975,7 @@
         <v>49</v>
       </c>
       <c r="C7" s="2">
-        <v>44446</v>
+        <v>44447</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>89</v>
@@ -1013,7 +992,7 @@
         <v>50</v>
       </c>
       <c r="C8" s="2">
-        <v>44445</v>
+        <v>44446</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>90</v>
@@ -1030,7 +1009,7 @@
         <v>51</v>
       </c>
       <c r="C9" s="2">
-        <v>44445</v>
+        <v>44446</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>91</v>
@@ -1047,7 +1026,7 @@
         <v>52</v>
       </c>
       <c r="C10" s="2">
-        <v>44445</v>
+        <v>44446</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>92</v>
@@ -1064,7 +1043,7 @@
         <v>53</v>
       </c>
       <c r="C11" s="2">
-        <v>44444</v>
+        <v>44445</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>93</v>
@@ -1081,7 +1060,7 @@
         <v>54</v>
       </c>
       <c r="C12" s="2">
-        <v>44444</v>
+        <v>44445</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>94</v>
@@ -1098,7 +1077,7 @@
         <v>55</v>
       </c>
       <c r="C13" s="2">
-        <v>44444</v>
+        <v>44445</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>95</v>
@@ -1115,7 +1094,7 @@
         <v>56</v>
       </c>
       <c r="C14" s="2">
-        <v>44443</v>
+        <v>44444</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>96</v>
@@ -1132,7 +1111,7 @@
         <v>57</v>
       </c>
       <c r="C15" s="2">
-        <v>44443</v>
+        <v>44444</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>97</v>
@@ -1149,7 +1128,7 @@
         <v>58</v>
       </c>
       <c r="C16" s="2">
-        <v>44442</v>
+        <v>44444</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>98</v>
@@ -1166,7 +1145,7 @@
         <v>59</v>
       </c>
       <c r="C17" s="2">
-        <v>44442</v>
+        <v>44443</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>99</v>
@@ -1177,13 +1156,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
         <v>60</v>
       </c>
       <c r="C18" s="2">
-        <v>44442</v>
+        <v>44443</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>100</v>
@@ -1194,13 +1173,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
         <v>61</v>
       </c>
       <c r="C19" s="2">
-        <v>44441</v>
+        <v>44442</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>101</v>
@@ -1211,13 +1190,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
         <v>62</v>
       </c>
       <c r="C20" s="2">
-        <v>44441</v>
+        <v>44442</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>102</v>
@@ -1228,13 +1207,13 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>63</v>
       </c>
       <c r="C21" s="2">
-        <v>44441</v>
+        <v>44442</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>103</v>
@@ -1251,7 +1230,7 @@
         <v>64</v>
       </c>
       <c r="C22" s="2">
-        <v>44440</v>
+        <v>44441</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>104</v>
@@ -1268,7 +1247,7 @@
         <v>65</v>
       </c>
       <c r="C23" s="2">
-        <v>44440</v>
+        <v>44441</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>105</v>
@@ -1285,7 +1264,7 @@
         <v>66</v>
       </c>
       <c r="C24" s="2">
-        <v>44439</v>
+        <v>44441</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>106</v>
@@ -1302,7 +1281,7 @@
         <v>67</v>
       </c>
       <c r="C25" s="2">
-        <v>44439</v>
+        <v>44440</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>107</v>
@@ -1319,7 +1298,7 @@
         <v>68</v>
       </c>
       <c r="C26" s="2">
-        <v>44439</v>
+        <v>44440</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>108</v>
@@ -1336,7 +1315,7 @@
         <v>69</v>
       </c>
       <c r="C27" s="2">
-        <v>44438</v>
+        <v>44439</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>109</v>
@@ -1353,7 +1332,7 @@
         <v>70</v>
       </c>
       <c r="C28" s="2">
-        <v>44438</v>
+        <v>44439</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>110</v>
@@ -1370,13 +1349,10 @@
         <v>71</v>
       </c>
       <c r="C29" s="2">
-        <v>44437</v>
+        <v>44439</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="E29" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1387,13 +1363,13 @@
         <v>72</v>
       </c>
       <c r="C30" s="2">
-        <v>44437</v>
+        <v>44438</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>112</v>
       </c>
       <c r="E30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1404,13 +1380,13 @@
         <v>73</v>
       </c>
       <c r="C31" s="2">
-        <v>44436</v>
+        <v>44438</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>113</v>
       </c>
       <c r="E31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1421,13 +1397,13 @@
         <v>74</v>
       </c>
       <c r="C32" s="2">
-        <v>44436</v>
+        <v>44437</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>114</v>
       </c>
       <c r="E32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1438,13 +1414,10 @@
         <v>75</v>
       </c>
       <c r="C33" s="2">
-        <v>44435</v>
+        <v>44437</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="E33" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1455,13 +1428,13 @@
         <v>76</v>
       </c>
       <c r="C34" s="2">
-        <v>44435</v>
+        <v>44436</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>116</v>
       </c>
       <c r="E34" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1472,13 +1445,10 @@
         <v>77</v>
       </c>
       <c r="C35" s="2">
-        <v>44435</v>
+        <v>44436</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="E35" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1489,13 +1459,10 @@
         <v>78</v>
       </c>
       <c r="C36" s="2">
-        <v>44434</v>
+        <v>44435</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="E36" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1506,13 +1473,13 @@
         <v>79</v>
       </c>
       <c r="C37" s="2">
-        <v>44433</v>
+        <v>44435</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>119</v>
       </c>
       <c r="E37" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1523,13 +1490,10 @@
         <v>80</v>
       </c>
       <c r="C38" s="2">
-        <v>44433</v>
+        <v>44435</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="E38" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1540,13 +1504,10 @@
         <v>81</v>
       </c>
       <c r="C39" s="2">
-        <v>44433</v>
+        <v>44434</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="E39" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1562,9 +1523,6 @@
       <c r="D40" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E40" t="s">
-        <v>162</v>
-      </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
@@ -1574,13 +1532,13 @@
         <v>83</v>
       </c>
       <c r="C41" s="2">
-        <v>44432</v>
+        <v>44433</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>123</v>
       </c>
       <c r="E41" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20220108
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Press Title</t>
   </si>
@@ -31,6 +31,9 @@
     <t>Page Content</t>
   </si>
   <si>
+    <t>新增44例COVID-19確定病例，分別為2例本土及42例境外移入</t>
+  </si>
+  <si>
     <t>即日起請已接種兩劑COVID-19疫苗且滿12週並滿18歲民眾，儘速接種疫苗追加劑</t>
   </si>
   <si>
@@ -58,7 +61,7 @@
     <t>針對桃園機場群聚感染案件，指揮中心今日成立前進指揮所協助防疫作為</t>
   </si>
   <si>
-    <t>1月5日起至1月31日止，地方政府可提供民眾200元(含)以下衛教品，以提升接種意願</t>
+    <t>/Bulletin/Detail/QcNPHHjaJVEr-bnW4hG5RQ?typeid=9</t>
   </si>
   <si>
     <t>/Bulletin/Detail/DViInYHA83okHIasbqONZQ?typeid=9</t>
@@ -88,7 +91,7 @@
     <t>/Bulletin/Detail/Y4fwruTZG4YQclQTSYPT-w?typeid=9</t>
   </si>
   <si>
-    <t>/Bulletin/Detail/Q-xhjZ6c709hJ-9GQXtFFw?typeid=9</t>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/QcNPHHjaJVEr-bnW4hG5RQ?typeid=9</t>
   </si>
   <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/DViInYHA83okHIasbqONZQ?typeid=9</t>
@@ -118,10 +121,10 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/Y4fwruTZG4YQclQTSYPT-w?typeid=9</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/Q-xhjZ6c709hJ-9GQXtFFw?typeid=9</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-07\$\@\$中央流行疫情指揮中心今(7)日表示，因應國內發生Omicron變異株本土確診病例，社區感染風險提升，衛生福利部傳染病防治諮詢會預防接種組(ACIP)決議，已接種兩劑COVID-19疫苗且間隔滿12週(84天)以上之滿18歲民眾，應儘速接種1劑COVID-19疫苗追加劑，以提升免疫保護力。\$\@\$指揮中心說明，昨(6)日召開ACIP會議討論COVID-19疫苗接種策略，考量國內外COVID-19疫情升溫，為降低社區傳播風險，專家指出，建議滿18歲以上民眾於完整接種COVID-19疫苗基礎劑12週後，應接種1劑追加劑，以提升個人及群體免疫力。追加劑接種廠牌建議如下：\$\@\$一、以mRNA疫苗(如Moderna、BNT)或蛋白質次單元疫苗(如高端)完成基礎劑：追加劑可以選擇接種Moderna(半劑量)、BNT、高端或AZ疫苗。\$\@\$二、以AZ完成基礎劑：追加劑可選擇接種mRNA或蛋白質次單元疫苗。\$\@\$指揮中心指出，目前國內疫苗庫存充足，將請地方政府衛生局儘速擴充接種量能，符合接種間隔的民眾可透過「COVID-19疫苗防治一網通」( https://antiflu.cdc.gov.tw/Covid19 )或地方政府衛生局公告，查詢鄰近合約醫療院所提供施打之疫苗廠牌及接種時間。</t>
+    <t>發佈日期：2022-01-08\$\@\$中央流行疫情指揮中心今(8)日公布國內新增44例COVID-19確定病例，分別為2例本土個案(案17414-17415)及42例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，本土個案(案17414-17415)分別為本國籍1例男性、1例女性，年齡均為50多歲，均為桃園機場感染事件相關個案；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增42例境外移入個案，性別為25例男性、16例女性、1例調查中，年齡介於未滿10至70多歲，分別自美國(23例)、越南(4例)、法國(2例)、阿根廷、澳大利亞、菲律賓、加拿大、阿拉伯聯合大公國、泰國、巴西、西班牙、印度、義大利及德國(各1例)入境，另有2例調查中，入境日介於去(2021)年12月15日至今(2022)年1月7日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,074,946例新型冠狀病毒肺炎相關通報(含5,055,445例排除)，其中17,302例確診，分別為2,630例境外移入，14,618例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計113例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月8日新增本土COVID-19確診個案表.pdf\$\@\$1月8日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-07\$\@\$中央流行疫情指揮中心今(7)日表示，因應國內發生Omicron變異株本土確診病例，社區感染風險提升，衛生福利部傳染病防治諮詢會預防接種組(ACIP)決議，已接種兩劑COVID-19疫苗且間隔滿12週(84天)以上之滿18歲民眾，應儘速接種1劑COVID-19疫苗追加劑，以提升免疫保護力。\$\@\$指揮中心說明，昨(6)日召開ACIP會議討論COVID-19疫苗接種策略，考量國內外COVID-19疫情升溫，為降低社區傳播風險，專家指出，建議滿18歲以上民眾於完整接種COVID-19疫苗基礎劑12週後，應接種1劑追加劑，以提升個人及群體免疫力。追加劑接種廠牌建議如下：\$\@\$一、以mRNA疫苗(如Moderna、BNT)或蛋白質次單元疫苗(如高端)完成基礎劑：追加劑可以選擇接種Moderna(半劑量)、BNT、高端或AZ疫苗。\$\@\$二、以AZ完成基礎劑：追加劑可選擇接種mRNA或蛋白質次單元疫苗。\$\@\$指揮中心指出，目前國內疫苗庫存充足，將請地方政府衛生局儘速擴充接種量能，符合接種間隔的民眾可透過「COVID-19疫苗防治一網通」( https://antiflu.cdc.gov.tw/Covid19 )或地方政府衛生局公告，查詢鄰近合約醫療院所提供施打之疫苗廠牌及接種時間。\$\@\$*備註：國外接種疫苗者，接種追加劑說明：\$\@\$一、於國外曾接種WHO EUL 之COVID-19疫苗 返國後請先至就近衛生所或健康服務中心補登國外疫苗接種紀錄，並妥善保存國外接種紀錄。\$\@\$二、符合現行追加劑接種間隔者(至少12週)，可攜國外接種紀錄、健保卡或相關身分證明文件，至鄰近COVID-19疫苗合約院所掛號接種。\$\@\$三、如接種非WHO EUL COVID-19疫苗, 視同無效劑次, 可於與最後一劑COVID-19疫苗間隔28天後, 於國內先完成COVID-19疫苗基礎劑接種，再依規定接種追加劑。</t>
   </si>
   <si>
     <t>發佈日期：2022-01-07\$\@\$中央流行疫情指揮中心今(7)日公布國內新增62例COVID-19確定病例，分別為4例本土個案(案17368-17371)及58例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，本土個案(案17368-17371)分別為本國籍1例男性、3例女性，年齡介於20至50多歲，均為桃園機場感染事件相關個案；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增58例境外移入個案，為29例男性、29例女性，年齡介於10多歲至70多歲，分別自美國(35例)、法國(4例)、英國(3例)、瑞士、越南及印度(各2例)、奧地利、智利、德國、加拿大、愛爾蘭、孟加拉、奈及利亞、墨西哥、西班牙及哥斯大黎加(各1例)入境，入境日介於去(2021)年12月22日至今(2022)年1月6日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,055,274例新型冠狀病毒肺炎相關通報(含5,035,769例排除)，其中17,258例確診，分別為2,588例境外移入，14,616例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另新增2例空號病例(案17271，案17272與舊案重複，改列空號)，累計113例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月7日新增本土COVID-19確診個案表.pdf\$\@\$1月7日新增境外移入COVID-19確診個案表.pdf</t>
@@ -133,16 +136,19 @@
     <t>發佈日期：2022-01-06\$\@\$中央流行疫情指揮中心今(6)日表示，考量目前國際COVID-19疫情嚴峻，請長者及其他 COVID-19感染後容易產生嚴重併發症之族群，儘速完成COVID-19疫苗基礎劑接種，提升保護力。\$\@\$指揮中心表示，目前我國75歲以上長者第1劑接種率僅約73%，第2劑接種率僅約67%，仍需再積極提升，為維護長者及風險族群健康，降低因感染COVID-19造成之重症、住院或死亡風險，家中長輩如尚未接種COVID-19疫苗第1、2劑，請於其身體狀況較穩定時，協助陪同至各地方政府衛生局安排或指定之合約醫療院所接種。\$\@\$指揮中心說明，疫苗接種後可能發生副作用，通常輕微並於數天內消失，並隨年齡層增加而減少，若擔心接種疫苗後所產生之副作用，可先與醫師討論，經諮詢評估選擇合適的疫苗接種。\$\@\$指揮中心表示，若為行動不便者，各地方政府衛生局亦設有到宅接種服務，有需求者可向各地方政府衛生局洽詢。另為鼓勵18歲以上尚未接種第1劑、第2劑COVID-19疫苗接種者儘速踴躍前往接種，於2022年1月5日至1月31日前接種COVID-19疫苗者，可獲得地方政府發放之200元(含)以下衛教品，鼓勵民眾儘速接種，獲得保護力。\$\@\$指揮中心提醒，依我國衛生福利部傳染病防治諮詢會預防接種組(ACIP)建議，接種COVID-19疫苗應與流感疫苗等其他疫苗間隔至少7天，亦請民眾前往接種COVID-19疫苗前，應備妥健保卡或其他可證明身分之證件，如為接種第2劑COVID-19疫苗者，請記得攜帶「COVID-19疫苗接種紀錄卡」，並於接種前評估時，說明過往疫苗接種史，以利醫生評估。另近期天氣多變，對於近期身體具狀況或慢性病情不穩定者，請於身體狀況較穩定後就近前往接種。接種後亦請多加留意身體狀況，多喝水多休息，亦請家人協助注意，如有持續發燒超過48小時、嚴重過敏反應如呼吸困難、氣喘、眩暈、心跳加速、全身紅疹等不適症狀，應儘速就醫釐清病因。</t>
   </si>
   <si>
+    <t>發佈日期：2022-01-06\$\@\$中央流行疫情指揮中心今(6)日表示，因應國際COVID-19疫情嚴峻及Omicron新型變異株威脅，考量春節入境人潮且近期COVID-19境外移入確診個案增加，為確保國內醫療院所對疫情的因應及保全醫療量能，即日起調整醫療機構醫療應變作為，說明如下：\$\@\$一、全國專責病房及負壓隔離病房調整收治病人條件，專責病房僅收治疑似或確診COVID-19病人；負壓隔離病室則以收治疑似或確診COVID-19及其他空氣傳染之法定傳染病病人為原則，清空非必要(如非空氣傳染防護隔離治療)入住於負壓隔離病房的病人。\$\@\$二、臺北市、新北市、基隆市、桃園市之應變醫院，於3日內恢復開設急性一般病床總數之20%作為專責病房(開設床數含負壓隔離病床)，收治疑似或確診個案。\$\@\$三、臺北市、新北市、基隆市、宜蘭縣、桃園市、新竹市、新竹縣及苗栗縣之急性一般病床總數500床以上之急救責任醫院，於3日內恢復開設急性一般病床總數之5%作為專責病房(開設床數含負壓隔離病床)，收治疑似或確診個案。\$\@\$四、專責病房收治疑似或確診COVID-19病人應以一人一室為原則(家人、同住者、同行者等如均為確診個案且知情同意，得兩人一室)，並有適當動線規劃，分流分艙安置住院病人；落實固定照護團隊與服務區塊化，避免人員頻繁輪替或跨單位工作；配置適當且固定之工作人員(含清潔人員、傳送人員及照顧服務員等)，以防範院內感染傳播風險。\$\@\$指揮中心呼籲醫療機構落實感染管制、強化門禁管制及工作人員健康監測、加強員工使用適當個人防護裝備，以預防並降低醫院群聚感染風險。由於Omicron新型變異株可能造成突破性感染，降低疫苗之保護力，指揮中心籲請可接種追加劑疫苗之醫院工作人員儘速接種追加劑疫苗，以確保人員健康安全。指揮中心將持續監測國內外疫情發展，確實掌握病床數及相關醫療資源分配，滾動修正相關應變策略，完善醫療照護體系，確保醫療量能充足以因應疫情。</t>
+  </si>
+  <si>
     <t>發佈日期：2022-01-05\$\@\$中央流行疫情指揮中心今(5)日公布國內新增3例COVID-19本土確定病例(尚未取號)，為擴大採檢清潔外包人員，於今日晚間檢驗陽性。\$\@\$指揮中心表示，3名個案均為女性，年齡分別為1例50多歲及2例60多歲，Ct值分別為33.8、23.4及19.5，為案17230、案17238、案17239及17266同職場工作人員，相關疫情調查、接觸者匡列及防治工作刻正進行中。\$\@\$指揮中心說明，因應桃園機場感染事件，指揮中心於第一時間針對外包清潔人員進行擴大採檢，已匡列861人，截至今日晚間，已有4例陽性（案17266及前述3例陽性）、855例陰性、1例檢驗中、1例待採檢。總計清潔外包人員已確診共7人（案17230、案17238-17239、17266、及前述3例）。\$\@\$指揮中心說明，因應今日晚間新增3位本土確診病例，前進指揮所立即啟動緊急作為如下：\$\@\$1. 針對清潔外包公司航廈夜班人員共93人，全數送集中檢疫所集中隔離。\$\@\$2. 該公司其餘未隔離員工，共768人，明後兩日（1月6日-1月7日）每日以家用快篩自我檢測，並彙整報告提供前進指揮所。1月8日將再度安排全員PCR檢驗。\$\@\$3. 已責成外包清潔公司嚴格確實執行員工健康監測，確保員工健康，以及早處理可能事件。</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-05\$\@\$中央流行疫情指揮中心今(5)日公布國內新增26例COVID-19確定病例，分別為1例(案17266)本土及25例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，案17266為本國籍50多歲女性，已接種2劑莫德納疫苗(為突破性感染)，與案17230、案17238及案17239為同職場工作人員，曾與前述個案搭乘同路線交通車，原定於今(2022)年1月5日採檢，1月3日出現乾咳、喉嚨不適等症狀，1月4日自行前往採檢站採檢後於今日確診，相關疫情調查、接觸者匡列及防治工作刻正進行中。\$\@\$指揮中心表示，今日新增25例境外移入個案，為12例男性、13例女性，年齡介於未滿5歲至70多歲，分別自美國(11例，案17241-17243、案17250、案17252、案17254、案17256-17259、案17265)、法國(3例，案17244、案17246、案17253)、加拿大(案17245)、丹麥(案17247)、英國(17248)、玻利維亞(案17249)、德國(案17251)、史瓦帝尼王國(案17255)、澳洲(案17260)、巴拿馬(2例，案17261-17262)、瑞典(案17263)及印尼(案17264)入境，入境日介於去(2021)年11月14日至今(2022)年1月4日；詳如新聞稿附件。\$\@\$另1月2日公布之案17181境外移入病例經疫調後改判為本土病例，為案16941之相關感染。\$\@\$指揮中心統計，截至目前國內累計5,017,456例新型冠狀病毒肺炎相關通報(含4,998,328例排除)，其中17,155例確診，分別為2,493例境外移入，14,608例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月5日新增境外移入COVID-19確診個案表.pdf</t>
+    <t>發佈日期：2022-01-05\$\@\$中央流行疫情指揮中心今(5)日公布國內新增26例COVID-19確定病例，分別為1例(案17266)本土及25例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，案17266為本國籍50多歲女性，已接種2劑莫德納疫苗(為突破性感染)，與案17230、案17238及案17239為同職場工作人員，曾與前述個案搭乘同路線交通車，原定於今(2022)年1月5日採檢，1月3日出現乾咳、喉嚨不適等症狀，1月4日自行前往採檢站採檢後於今日確診，相關疫情調查、接觸者匡列及防治工作刻正進行中。\$\@\$指揮中心表示，今日新增25例境外移入個案，為12例男性、13例女性，年齡介於未滿5歲至70多歲，分別自美國(12例，案17241-17243、案17245、案17250、案17252、案17254、案17256-17259、案17265)、法國(3例，案17244、案17246、案17253)、丹麥(案17247)、英國(17248)、玻利維亞(案17249)、德國(案17251)、史瓦帝尼王國(案17255)、澳洲(案17260)、巴拿馬(2例，案17261-17262)、瑞典(案17263)及印尼(案17264)入境，入境日介於去(2021)年11月14日至今(2022)年1月4日；詳如新聞稿附件。\$\@\$另1月2日公布之案17181境外移入病例經疫調後改判為本土病例，為案16941之相關感染。\$\@\$指揮中心統計，截至目前國內累計5,017,456例新型冠狀病毒肺炎相關通報(含4,998,328例排除)，其中17,155例確診，分別為2,493例境外移入，14,608例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月5日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
     <t>發佈日期：2022-01-05\$\@\$疾管署今(5)日宣布，為提升疫苗接種人口涵蓋率，發揮疫苗最大效益，自2022年1月6日起，公費流感疫苗擴大提供全國6個月以上尚未接種之民眾接種，至疫苗用罄為止，疾管署呼籲尚未接種的計畫對象，尤其是65歲以上長者、學齡前幼兒及醫事人員等重點族群儘快接種，以保障自身及周遭人員的健康。\$\@\$疾管署表示，2021年度公費流感疫苗分2階段施打，除50至64歲無高風險慢性病成人於第二階段11月15日開打外，其於對象均為10月1日開打。截至2022年1月4日，公費疫苗總接種數約562萬劑，整體疫苗使用率逾91.9%，剩餘量約49萬劑；目前全國約有3,700餘家合約院所(含部分衛生所)提供接種服務，建議民眾可先透過各地方政府衛生局網頁、疾管署流感防治一網通(https://antiflu.cdc.gov.tw/)、疾管家或1922防疫諮詢專線，查詢鄰近合約院所名單，並向合約院所預約，以確保可施打到疫苗。\$\@\$另公費流感疫苗接種期間，COVID-19疫苗接種作業持續進行，依衛生福利部傳染病防治諮詢會預防接種組專家建議，2種疫苗接種間隔應至少7天，避免發生疫苗接種不良事件無法釐清。疾管署提醒民眾於預約或接種前主動告知疫苗接種史，合約院所應於接種區建立動線分流，並請相關工作人員於接種前落實檢核接種紀錄，接種後於健保卡黏貼流感疫苗接種貼紙。\$\@\$疾管署提醒，國內流感疫情仍處低點尚未進入流行期，民眾可儘速接種，以於流感疫情達高峰前獲得足夠保護力。近期氣溫偏低，為防範流感及COVID-19疫情雙重衝擊，民眾除接種疫苗，應養成良好衛生習慣，出現類流感症狀儘速戴口罩就醫，並在家休息，減少病毒傳播機會。如有流感疫苗或流感防治相關疑問，可至疾管署全球資訊網(https://www.cdc.gov.tw)，或撥打免付費防疫專線1922(或0800-001922)洽詢。</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-04\$\@\$中央流行疫情指揮中心今(4)日表示，為加速國人完成2劑接種，提升尚未接種第1、2劑COVID-19疫苗民眾之接種意願，各地方政府自2022年1月5日至1月31日前，可提供18歲以上民眾200元(含)以下衛教品，以鼓勵民眾踴躍完成接種2劑COVID-19疫苗，儘速獲得完整免疫保護力。\$\@\$指揮中心表示，截至2022年1月3日為止，我國COVID-19疫苗第一劑接種率約80%，第二劑接種率約69%，為因應國際疫情持續嚴峻及Omicron新型變異株之威脅增加，接種涵蓋率仍須再提升，目前COVID-19疫苗由地方政府衛生局指定/安排之合約醫療院所或衛生所進行接種，鼓勵尚未接種過任何1劑COVID-19疫苗及符合接種間隔但尚未完成2劑COVID-19疫苗接種之民眾，請儘速前往COVID-19疫苗合約醫療院所接種。\$\@\$指揮中心說明，目前國內各廠牌COVID-19疫苗供應充分，民眾可至衛生福利部疾病管制署全球資訊網，「COVID-19疫苗接種院所單元」（https://www.cdc.gov.tw/Category/List/u4l1b_gHhf9WDjhEtRmRRw），運用「COVID-19接種院所地圖」及各地方政府衛生局公告之COVID-19疫苗接種合約醫療院所以及車站等隨到隨打疫苗接種站，就近前往接種。\$\@\$指揮中心提醒， 18歲至未滿20歲民眾，如自行前往接種，請持家長簽具之意願同意書。若由家長陪同前往接種，請本人與家長於現場共同簽署意願同意書。另依衛生福利部傳染病防治諮詢會預防接種組(ACIP)建議，接種COVID-19疫苗應與流感疫苗等其他疫苗間隔至少7天，亦請民眾前往接種COVID-19疫苗前，應備妥健保卡或其他可證明身分之證件，如為接種第2劑COVID-19疫苗者亦請攜帶「COVID-19疫苗接種紀錄卡」，並於接種前評估時說明過往疫苗接種史，以利醫生評估。</t>
+    <t>發佈日期：2022-01-04\$\@\$中央流行疫情指揮中心今(4)日表示，為因應桃園機場群聚感染案件，陳時中指揮官於今日下午協同醫療應變組王必勝副組長、桃園市政府衛生局王文彥局長、衛生福利部疾病管制署北區管制中心及機場公司航運中心工作人員，實地進行入境旅客動線勘查，評估釐清風險，檢視第一線人員防護裝備及消毒情形，並啟動下列防疫作為：\$\@\$一、 成立前進指揮所，由醫療應變組王必勝副組長擔任指揮官，統籌指揮相關防疫工作，進行跨單位溝通協調，並評估各單位現場作業風險，提出相關改善計畫。\$\@\$二、 針對高風險旅客(14天內有症狀)之入境動線，重新釐清評估風險，避免與其他民眾、工作人員接觸，降低傳播可能性。\$\@\$三、 配合桃園市政府衛生局採檢規劃「擴大、快速」戰略概念，擴大評估可能有在個案活動地(如清潔的廁所)活動之其他人員，快速進行相關篩檢。</t>
   </si>
 </sst>
 </file>
@@ -548,7 +554,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="2">
-        <v>44568</v>
+        <v>44569</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>25</v>
@@ -582,7 +588,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="2">
-        <v>44567</v>
+        <v>44568</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>27</v>
@@ -621,6 +627,9 @@
       <c r="D6" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
@@ -630,13 +639,13 @@
         <v>20</v>
       </c>
       <c r="C7" s="2">
-        <v>44566</v>
+        <v>44567</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -653,7 +662,7 @@
         <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -670,7 +679,7 @@
         <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -681,10 +690,13 @@
         <v>23</v>
       </c>
       <c r="C10" s="2">
-        <v>44565</v>
+        <v>44566</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -701,7 +713,7 @@
         <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20220109
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="202">
   <si>
     <t>Press Title</t>
   </si>
@@ -49,16 +49,151 @@
     <t>因應春節入境人潮及COVID-19境外移入確診個案增加，指揮中心擴大開設專責病房及調整醫療機構應變策略</t>
   </si>
   <si>
-    <t>新增3例COVID-19本土確定病例，衛生單位已啟動疫情調查及防治作為</t>
-  </si>
-  <si>
-    <t>新增26例COVID-19確定病例，分別為1例本土及25例境外移入</t>
-  </si>
-  <si>
-    <t>自2022年1月6日起，公費流感疫苗開放全民接種至疫苗用罄</t>
-  </si>
-  <si>
-    <t>針對桃園機場群聚感染案件，指揮中心今日成立前進指揮所協助防疫作為</t>
+    <t>網傳「三級警戒微解封的不可思議之處」指揮中心： 原同住家人就不受限制，謠言邏輯誤導且比喻失當，請勿輕信轉傳，造成防疫困擾</t>
+  </si>
+  <si>
+    <t>網傳「政府讓人民施打未受認證且保護力低之國產疫苗」  指揮中心：會把關國產疫苗品質、安全及療效</t>
+  </si>
+  <si>
+    <t>網傳「代工(AZ疫苗)三億劑嫌太多賣不出去」，指揮中心：有心人刻意扭曲語意</t>
+  </si>
+  <si>
+    <t>網傳「臺中太原路復健醫院被徵收為方艙醫院」 指揮中心：假訊息勿轉傳</t>
+  </si>
+  <si>
+    <t>網路販售「新冠病毒快篩試劑」，指揮中心：已觸法，警方偵辦中</t>
+  </si>
+  <si>
+    <t>網現偽冒教育部網站  指揮中心：境外假網頁勿輕信</t>
+  </si>
+  <si>
+    <t>因應結核菌液態培養(MGIT)檢驗試劑暫時性缺貨，為利早期診斷結核病，針對疑似結核病送驗初查痰3套，請務必再進行結核分枝桿菌核酸增幅(NAA)檢驗(疾病管制署致醫界通函第470號)</t>
+  </si>
+  <si>
+    <t>COVID-19專家諮詢會因應變異株流行，更新治療指引藥物適用原則(疾病管制署致醫界通函第469號)</t>
+  </si>
+  <si>
+    <t>因應COVID-19 Omicron變異株威脅，籲請社區定點診所加強發放公費COVID-19家用快篩試劑予高風險民眾(疾病管制署致醫界通函第468號)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COVID-19專家諮詢會參照最新實證與藥物適應症，更新治療指引藥物適用對象並重申制定原則(疾病管制署致醫界通函第467號) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">近期登革熱隱藏期平均超過3日，籲請醫師對具登革熱流行地區旅遊史之疑似病例提高警覺，加強診斷及通報(疾病管制署致醫界通函第466號) </t>
+  </si>
+  <si>
+    <t>10月1日起擴大2歲以上兒童使用丙型干擾素釋放試驗(IGRA)，以提升潛伏結核感染(LTBI)檢驗準確性及守護幼童健康(疾病管制署致醫界通函第465號)</t>
+  </si>
+  <si>
+    <t>111年潛伏結核感染治療HP複方藥品.pdf(另開新視窗)</t>
+  </si>
+  <si>
+    <t>「111年人體測溫用紅外線熱影像儀維護保養」採購案.pdf(另開新視窗)</t>
+  </si>
+  <si>
+    <t>111年細胞培養及分生試劑乙批.pdf(另開新視窗)</t>
+  </si>
+  <si>
+    <t>111年疫情統計分析R系統維護及諮詢服務.pdf(另開新視窗)</t>
+  </si>
+  <si>
+    <t>111-112年 COVID-19疫苗4,000萬劑倉儲物流與配送.pdf(另開新視窗)</t>
+  </si>
+  <si>
+    <t>高屏區管制中心111年國際港埠檢體收送.pdf(另開新視窗)</t>
+  </si>
+  <si>
+    <t>助理研究員(預估缺)</t>
+  </si>
+  <si>
+    <t>師(三)級護理師</t>
+  </si>
+  <si>
+    <t>約聘護理師</t>
+  </si>
+  <si>
+    <t>約用護理師(徵才案號：1521延長公告)</t>
+  </si>
+  <si>
+    <t>約用助理(徵才案號：1522延長公告)</t>
+  </si>
+  <si>
+    <t>111年地方衛生機關防疫業務考評作業手冊</t>
+  </si>
+  <si>
+    <t>公告本署慢性傳染病組約用人員徵才案(徵才案號：0309)初審合格名單及甄試事宜。</t>
+  </si>
+  <si>
+    <t>公告本署公共關係室約用人員徵才案(徵才案號：0708)初審合格名單及甄試事宜。</t>
+  </si>
+  <si>
+    <t>公告本署檢驗及疫苗研製中心約用人員徵才案(徵才案號：1057、1058)初審合格名單及甄試事宜。</t>
+  </si>
+  <si>
+    <t>公告本署師(三)級護理師甄選之口試日程相關事宜(口試名單公告)。</t>
+  </si>
+  <si>
+    <t>公告本署急性傳染病組約用人員徵才案(徵才案號：1105)初審合格名單及甄試事宜。</t>
+  </si>
+  <si>
+    <t>1月5日起至1月31日止，地方政府可提供民眾200元(含)以下衛教品，以提升接種意願</t>
+  </si>
+  <si>
+    <t>新增34例COVID-19確定病例，分別為4例本土及30例境外移入</t>
+  </si>
+  <si>
+    <t>新增1例COVID-19本土確定病例，衛生單位已啟動疫情調查及防治作為</t>
+  </si>
+  <si>
+    <t>新增25例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>新增20例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>新增21例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>新增41例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>指揮中心重申，兩岸應以防疫優先，才能維護兩岸民眾健康</t>
+  </si>
+  <si>
+    <t>受聘僱外國人健康檢查管理辦法部分條文修正案自111年1月1日起實施，確保社區防疫安全</t>
+  </si>
+  <si>
+    <t>指揮中心增加公費COVID-19家用快篩試劑發放點，早期偵測，防範病毒進入社區</t>
+  </si>
+  <si>
+    <t>新增24例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>台積電、鴻海永齡、慈濟三間企業和民間團體捐贈之第十五批BNT疫苗93.83萬劑於今(30)日上午抵臺</t>
+  </si>
+  <si>
+    <t>新增14例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>新增19例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>為因應我國民眾能加速入境歐盟等國家，我國「數位新冠病毒健康證明」於12月28日上午8時開放下載</t>
+  </si>
+  <si>
+    <t>因應國際Omicron變異株疫情迅速擴散，指揮中心入境旅客PCR檢驗報告調整為「2日內」報告並改以「採檢日」為計算基準</t>
+  </si>
+  <si>
+    <t>移工轉換雇主及雇主調派移工變更工作地點，如已完整接種COVID-19疫苗，即日起無須事前檢驗PCR</t>
+  </si>
+  <si>
+    <t>有條件放寬陪病人數上限至2人，並調整陪病者COVID-19疫苗接種規範及篩檢措施</t>
+  </si>
+  <si>
+    <t>新增16例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>12月28日至1月10日維持疫情警戒標準為第二級，請民眾配合跨年大型活動等防疫準備注意事項</t>
   </si>
   <si>
     <t>/Bulletin/Detail/QcNPHHjaJVEr-bnW4hG5RQ?typeid=9</t>
@@ -79,16 +214,154 @@
     <t>/Bulletin/Detail/u0vHFZX2nzlhWBifQl3x5Q?typeid=9</t>
   </si>
   <si>
-    <t>/Bulletin/Detail/jK3GN-Hw8x_ELLciTmfwQg?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/xR3EWQ6aKrqsQwfI_iNxqg?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/oHyBMuXSjeea-EJ0olgdRQ?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/Y4fwruTZG4YQclQTSYPT-w?typeid=9</t>
+    <t>/Bulletin/Detail/ftv6FPFis84j5uHWTq4lNA?typeid=8772</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/PmSCiSjM5YpCUxXqoS81RA?typeid=8772</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/QCmwPRiL1nKrc8-AuqSEGg?typeid=8772</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/IO3F02JMs4pToOM84aXopQ?typeid=8772</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/zjF-6vCLlbYe1RhTXKlq1Q?typeid=8772</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/IU5CMLLt8bQqXWHQhil0Aw?typeid=8772</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/KaqzyT5RqFOuOQFGpEYLgA?typeid=48</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/zUiCR7uM2Ox39wGHOkzhMw?typeid=48</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/tun0Es9fOoIJqDFToylh6Q?typeid=48</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/1pVYYgWzE_U3RlTuctsioQ?typeid=48</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/HU4mCbrzZQlHC-VhwBiJOg?typeid=48</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/DyZ6ZOuk-VLQSHiQ6xhqoQ?typeid=48</t>
+  </si>
+  <si>
+    <t>/Uploads/files/2eca6680-fdde-4a38-934a-6da1c2dd8b8b.pdf</t>
+  </si>
+  <si>
+    <t>/Uploads/files/575633c9-11a3-4d2c-a5df-3bc675a198dc.pdf</t>
+  </si>
+  <si>
+    <t>/Uploads/files/a022ad25-9fb8-433f-a588-a93c1e5f9d9c.pdf</t>
+  </si>
+  <si>
+    <t>/Uploads/files/557f2695-c3ee-4d00-aa33-5d0dc36f7f09.pdf</t>
+  </si>
+  <si>
+    <t>/Uploads/files/a22b63a6-c6cb-463f-940d-26f4c11b17bc.pdf</t>
+  </si>
+  <si>
+    <t>/Uploads/files/0516860c-da1c-4620-ae05-79a01343a4d6.pdf</t>
+  </si>
+  <si>
+    <t>/HireList/Detail?hireId=kLNv1XH1fB8TlCZo6RSNGw</t>
+  </si>
+  <si>
+    <t>/HireList/Detail?hireId=7afE7y_q_0a-FLqnxHIjIA</t>
+  </si>
+  <si>
+    <t>/HireList/Detail?hireId=0i1H55b5Pqk0ahyBe-cr-A</t>
+  </si>
+  <si>
+    <t>/HireList/Detail?hireId=2tmdwtNL8GDuj002O3_QsA</t>
+  </si>
+  <si>
+    <t>/HireList/Detail?hireId=3FDssdDwiCeDzVB2w5R-gA</t>
+  </si>
+  <si>
+    <t>/HireList/Detail?hireId=HnyAaEpJjNTAhTgoRupHfg</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Y_cTXA-RBSS1MjAEFDP3TQ?typeid=11</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/vN_TxnDuv7GamvGxnZXEdw?typeid=11</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/7UJRpdDRbQNIZWyyEfHdHQ?typeid=11</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/u9ej71cxiu9bJqO0gMxdOQ?typeid=11</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/_EjXyzKBrURN93eoTpH45Q?typeid=11</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/6_WqkhWC-GJV1mcZ8hGpEg?typeid=11</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Q-xhjZ6c709hJ-9GQXtFFw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/NQf6AVY3GBaKX9pYZ5jA3Q?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/8XzxB5KZNJhy0ITApU7wWg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/wPYoUO5Fv8bYEL0fGvlwrw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/7wbCdR_N1PJc783mP_mtlQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/mj5H52pb8ivr0RcjQ-N9cw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/L32CQqYyDVXO-DF7hgHyAQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/pr-CblnPk9vL2ApdEOo_dQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/jOxiIwl9CpcNJxP8dckk6A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/ijxgB4PqNSwT9jxZQotXIQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/AjUkrlWXkxOqou5W9tgVpw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/WIMrcWpPk8g16xjOZR_e4g?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/uC2CvyAZKpXLB4pbfUDEwA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Vr-xa_jxF7CS4mlKHSpHgw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/-rE5uMCRLrzdP16Sf7m5UA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/_VRX4ciyxXBAZZrWlce-FQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Cd_p1u_CUNlo8A-6VywrYA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/frAq9bxqUXeg-8CrHH-M_w?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Q8YCgoN6l70alReqqr5Wmw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/nIdKcbV265_Oy19NRrVK0g?typeid=9</t>
   </si>
   <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/QcNPHHjaJVEr-bnW4hG5RQ?typeid=9</t>
@@ -109,16 +382,154 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/u0vHFZX2nzlhWBifQl3x5Q?typeid=9</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/jK3GN-Hw8x_ELLciTmfwQg?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/xR3EWQ6aKrqsQwfI_iNxqg?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/oHyBMuXSjeea-EJ0olgdRQ?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/Y4fwruTZG4YQclQTSYPT-w?typeid=9</t>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/ftv6FPFis84j5uHWTq4lNA?typeid=8772</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/PmSCiSjM5YpCUxXqoS81RA?typeid=8772</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/QCmwPRiL1nKrc8-AuqSEGg?typeid=8772</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/IO3F02JMs4pToOM84aXopQ?typeid=8772</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/zjF-6vCLlbYe1RhTXKlq1Q?typeid=8772</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/IU5CMLLt8bQqXWHQhil0Aw?typeid=8772</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/KaqzyT5RqFOuOQFGpEYLgA?typeid=48</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/zUiCR7uM2Ox39wGHOkzhMw?typeid=48</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/tun0Es9fOoIJqDFToylh6Q?typeid=48</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/1pVYYgWzE_U3RlTuctsioQ?typeid=48</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/HU4mCbrzZQlHC-VhwBiJOg?typeid=48</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/DyZ6ZOuk-VLQSHiQ6xhqoQ?typeid=48</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Uploads/files/2eca6680-fdde-4a38-934a-6da1c2dd8b8b.pdf</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Uploads/files/575633c9-11a3-4d2c-a5df-3bc675a198dc.pdf</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Uploads/files/a022ad25-9fb8-433f-a588-a93c1e5f9d9c.pdf</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Uploads/files/557f2695-c3ee-4d00-aa33-5d0dc36f7f09.pdf</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Uploads/files/a22b63a6-c6cb-463f-940d-26f4c11b17bc.pdf</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Uploads/files/0516860c-da1c-4620-ae05-79a01343a4d6.pdf</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=kLNv1XH1fB8TlCZo6RSNGw</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=7afE7y_q_0a-FLqnxHIjIA</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=0i1H55b5Pqk0ahyBe-cr-A</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=2tmdwtNL8GDuj002O3_QsA</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=3FDssdDwiCeDzVB2w5R-gA</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=HnyAaEpJjNTAhTgoRupHfg</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Y_cTXA-RBSS1MjAEFDP3TQ?typeid=11</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/vN_TxnDuv7GamvGxnZXEdw?typeid=11</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/7UJRpdDRbQNIZWyyEfHdHQ?typeid=11</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/u9ej71cxiu9bJqO0gMxdOQ?typeid=11</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/_EjXyzKBrURN93eoTpH45Q?typeid=11</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/6_WqkhWC-GJV1mcZ8hGpEg?typeid=11</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Q-xhjZ6c709hJ-9GQXtFFw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/NQf6AVY3GBaKX9pYZ5jA3Q?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/8XzxB5KZNJhy0ITApU7wWg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/wPYoUO5Fv8bYEL0fGvlwrw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/7wbCdR_N1PJc783mP_mtlQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/mj5H52pb8ivr0RcjQ-N9cw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/L32CQqYyDVXO-DF7hgHyAQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/pr-CblnPk9vL2ApdEOo_dQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/jOxiIwl9CpcNJxP8dckk6A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/ijxgB4PqNSwT9jxZQotXIQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/AjUkrlWXkxOqou5W9tgVpw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/WIMrcWpPk8g16xjOZR_e4g?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/uC2CvyAZKpXLB4pbfUDEwA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Vr-xa_jxF7CS4mlKHSpHgw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/-rE5uMCRLrzdP16Sf7m5UA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/_VRX4ciyxXBAZZrWlce-FQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Cd_p1u_CUNlo8A-6VywrYA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/frAq9bxqUXeg-8CrHH-M_w?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Q8YCgoN6l70alReqqr5Wmw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/nIdKcbV265_Oy19NRrVK0g?typeid=9</t>
   </si>
   <si>
     <t>發佈日期：2022-01-08\$\@\$中央流行疫情指揮中心今(8)日公布國內新增44例COVID-19確定病例，分別為2例本土個案(案17414-17415)及42例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，本土個案(案17414-17415)分別為本國籍1例男性、1例女性，年齡均為50多歲，均為桃園機場感染事件相關個案；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增42例境外移入個案，性別為25例男性、16例女性、1例調查中，年齡介於未滿10至70多歲，分別自美國(23例)、越南(4例)、法國(2例)、阿根廷、澳大利亞、菲律賓、加拿大、阿拉伯聯合大公國、泰國、巴西、西班牙、印度、義大利及德國(各1例)入境，另有2例調查中，入境日介於去(2021)年12月15日至今(2022)年1月7日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,074,946例新型冠狀病毒肺炎相關通報(含5,055,445例排除)，其中17,302例確診，分別為2,630例境外移入，14,618例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計113例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月8日新增本土COVID-19確診個案表.pdf\$\@\$1月8日新增境外移入COVID-19確診個案表.pdf</t>
@@ -127,28 +538,88 @@
     <t>發佈日期：2022-01-07\$\@\$中央流行疫情指揮中心今(7)日表示，因應國內發生Omicron變異株本土確診病例，社區感染風險提升，衛生福利部傳染病防治諮詢會預防接種組(ACIP)決議，已接種兩劑COVID-19疫苗且間隔滿12週(84天)以上之滿18歲民眾，應儘速接種1劑COVID-19疫苗追加劑，以提升免疫保護力。\$\@\$指揮中心說明，昨(6)日召開ACIP會議討論COVID-19疫苗接種策略，考量國內外COVID-19疫情升溫，為降低社區傳播風險，專家指出，建議滿18歲以上民眾於完整接種COVID-19疫苗基礎劑12週後，應接種1劑追加劑，以提升個人及群體免疫力。追加劑接種廠牌建議如下：\$\@\$一、以mRNA疫苗(如Moderna、BNT)或蛋白質次單元疫苗(如高端)完成基礎劑：追加劑可以選擇接種Moderna(半劑量)、BNT、高端或AZ疫苗。\$\@\$二、以AZ完成基礎劑：追加劑可選擇接種mRNA或蛋白質次單元疫苗。\$\@\$指揮中心指出，目前國內疫苗庫存充足，將請地方政府衛生局儘速擴充接種量能，符合接種間隔的民眾可透過「COVID-19疫苗防治一網通」( https://antiflu.cdc.gov.tw/Covid19 )或地方政府衛生局公告，查詢鄰近合約醫療院所提供施打之疫苗廠牌及接種時間。\$\@\$*備註：國外接種疫苗者，接種追加劑說明：\$\@\$一、於國外曾接種WHO EUL 之COVID-19疫苗 返國後請先至就近衛生所或健康服務中心補登國外疫苗接種紀錄，並妥善保存國外接種紀錄。\$\@\$二、符合現行追加劑接種間隔者(至少12週)，可攜國外接種紀錄、健保卡或相關身分證明文件，至鄰近COVID-19疫苗合約院所掛號接種。\$\@\$三、如接種非WHO EUL COVID-19疫苗, 視同無效劑次, 可於與最後一劑COVID-19疫苗間隔28天後, 於國內先完成COVID-19疫苗基礎劑接種，再依規定接種追加劑。</t>
   </si>
   <si>
+    <t>發佈日期：2022-01-06\$\@\$中央流行疫情指揮中心今(6)日表示，因應國際COVID-19疫情嚴峻及Omicron新型變異株威脅，考量春節入境人潮且近期COVID-19境外移入確診個案增加，為確保國內醫療院所對疫情的因應及保全醫療量能，即日起調整醫療機構醫療應變作為，說明如下：\$\@\$一、全國專責病房及負壓隔離病房調整收治病人條件，專責病房僅收治疑似或確診COVID-19病人；負壓隔離病室則以收治疑似或確診COVID-19及其他空氣傳染之法定傳染病病人為原則，清空非必要(如非空氣傳染防護隔離治療)入住於負壓隔離病房的病人。\$\@\$二、臺北市、新北市、基隆市、桃園市之應變醫院，於3日內恢復開設急性一般病床總數之20%作為專責病房(開設床數含負壓隔離病床)，收治疑似或確診個案。\$\@\$三、臺北市、新北市、基隆市、宜蘭縣、桃園市、新竹市、新竹縣及苗栗縣之急性一般病床總數500床以上之急救責任醫院，於3日內恢復開設急性一般病床總數之5%作為專責病房(開設床數含負壓隔離病床)，收治疑似或確診個案。\$\@\$四、專責病房收治疑似或確診COVID-19病人應以一人一室為原則(家人、同住者、同行者等如均為確診個案且知情同意，得兩人一室)，並有適當動線規劃，分流分艙安置住院病人；落實固定照護團隊與服務區塊化，避免人員頻繁輪替或跨單位工作；配置適當且固定之工作人員(含清潔人員、傳送人員及照顧服務員等)，以防範院內感染傳播風險。\$\@\$指揮中心呼籲醫療機構落實感染管制、強化門禁管制及工作人員健康監測、加強員工使用適當個人防護裝備，以預防並降低醫院群聚感染風險。由於Omicron新型變異株可能造成突破性感染，降低疫苗之保護力，指揮中心籲請可接種追加劑疫苗之醫院工作人員儘速接種追加劑疫苗，以確保人員健康安全。指揮中心將持續監測國內外疫情發展，確實掌握病床數及相關醫療資源分配，滾動修正相關應變策略，完善醫療照護體系，確保醫療量能充足以因應疫情。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-10\$\@\$中央流行疫情指揮中心今（10）日表示，近日有網友散布「三級警戒微解封的不可思議之處，新冠肺炎病毒只會攻擊家人」等訊息，相關內容多有誤導，且在錯誤基礎上進行不當類比，指揮中心再次強調，相關防疫指引已清楚說明，原本同住家人可以繼續維持生活，相關指引都是針對日常非同住者間的行為互動加以規範，呼籲民眾勿輕信或隨意散播、轉傳錯誤訊息，造成防疫困擾。\$\@\$指揮中心指出，有關7月13號以後針對部分場所將適度鬆綁，但仍須遵守防疫相關指引及規範，而此波疫情中，不少個案均為家戶群聚感染，由於室內密切接觸風險較高，因此對於室內社交人數須有較嚴格規範，但不包含原本同住的家人，也無需限制同住家人不能在家打麻將、看電影、吃飯等。 圖片 附件\$\@\$0710指揮中心：勿輕信「三級警戒微解封的不可思議之處」之網傳.jpg</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-13\$\@\$近日有網友在臉書FB以自製圖文方式散布「政府讓人民施打未受認證且保護力低之國產疫苗」、「國產疫苗的中和抗體效價比國外疫苗差」、「國產疫苗為什麼不向國際提出緊急授權」，中央流行疫情指揮中心(下稱指揮中心)今（13）日嚴正澄清表示，目前國產疫苗臨床試驗尚在進行中，最終結果須等廠商提出EUA 申請，經專家會議審查疫苗的製程管控、藥毒理試驗及臨床試驗結果，在緊急公衛的需求下，確認疫苗使用效益大於風險，才會核准緊急授權使用。\$\@\$指揮中心指出，目前國產疫苗廠商皆已積極規劃，以取得國際認證為目標。國產疫苗需經食藥署和專家會議嚴謹審查，在緊急公衛需求，並確認效益大於風險，才會核准緊急授權使用。此外，各家廠牌的疫苗所使用的檢驗實驗室及檢驗方式不同且無協和，無法直接由各實驗室產生數值進行比較。國產疫苗仍需等廠商提出申請，經過中央主管機關嚴格把關及審查通過後，確認品質、安全、療效後，品質沒有問題，疫苗方可供民眾施打。\$\@\$指揮中心再次提醒，民眾接獲來源不明的訊息時，應先進行查證，切勿隨意散播、轉傳，以免觸法。 圖片 附件\$\@\$0613網傳「政府讓人民施打未受認證且保護力低之國產疫苗」-1.jpg\$\@\$0613網傳「政府讓人民施打未受認證且保護力低之國產疫苗」-2.jpg</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-12\$\@\$中央流行疫情指揮中心今(12)日嚴正澄清，近日於社群平台流傳「代工三億劑嫌太多賣不出去」等訊息，指揮中心於6月10日記者會已公開說明，與AstraZeneca原廠洽談授權製造事宜時，我方提出可年產一億劑之規劃，但原廠要求需年產三億劑，經評估，對我方產能過於沉重，並無以「賣不出去」為由拒絕原廠授權製造，卻被有心人刻意扭曲語意。此圖文與事實不符，指揮中心特此澄清。\$\@\$指揮中心重申，防疫相關資訊應以中央流行疫情指揮中心公布內容為主。提醒民眾，收到來路不明訊息多加留意、查證，切勿轉傳散播。詳情請上官網查詢 (http://at.cdc.tw/Q7S2Vt)。 圖片 附件\$\@\$20210612澄清.jpg</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-05-25\$\@\$中央流行疫情指揮中心今(25)日表示，近日網路出現偽冒教育部網站，杜撰「全國各級學校因應疫情停課時程資訊」等訊息，意圖造成民眾困惑，此為境外假網頁不實訊息，請民眾勿輕信。\$\@\$指揮中心副指揮官陳宗彥表示，該網站假冒教育部傳達不實防疫訊息，刑事警察局已成立專案小組偵辦，經調查其為境外IP。\$\@\$指揮中心指出，教育部全球資訊網正確的網址是https://www.edu.tw/ ，民眾收到任何連結時，可以先觀察連結網址，是否跟官方網址一樣。例如，教育部官方網址的網域，就會是「edu.tw」結尾。\$\@\$指揮中心強調，散播假訊息構成犯罪，會被判處最高三年有期徒刑或併科三百萬元罰金。提醒民眾，收到來路不明訊息多加留意、查證，切勿轉傳散播，以免觸法。 圖片 附件\$\@\$0525指揮中心指出，網路出現偽冒教育部網站並杜撰假訊息，請民眾勿輕信.jpg\$\@\$勿散播不實訊息，以免觸法受罰.jpg</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-06\$\@\$為提供結核病患即時診斷，疾病管制署結核病診治指引自104年已加重結核分枝桿菌核酸增幅(nucleic acid amplification, NAA)檢驗於診斷結核病之角色。NAA檢驗具快速、高敏感度及高特異性，可大幅縮短傳統培養檢驗方法所需等待結果時間，有利及早診斷及治療結核病。\$\@\$因應近期結核菌液態培養(MGIT)檢驗發生添加劑(營養劑併抑制細菌生長的抗生素成分)供貨短缺情形，為避免延遲發現疑似結核病個案，依本署110年12月24日「衛生福利部傳染病防治諮詢會(結核病防治組)」會議決議，於供貨短缺期間，對於社區型肺炎尚未通報結核病者，於診斷送驗3套初查痰執行塗片耐酸性染色鏡檢(Acid fast stain)及分枝桿菌培養時，其中1套請務必同時開立NAA檢驗。另考量實驗室短期內MGIT痰培養試劑有限，對於管理中的結核病患追蹤複查痰，請採1套進行培養檢驗，暫時避免重複送驗檢體，此因應作為停止施行時間將於缺貨狀況緩解後再函週知。\$\@\$有關「結核病診治指引」可至疾病管制署全球資訊網(https://www.cdc.gov.tw)&gt;傳染病與防疫專題&gt;傳染病介紹&gt;第三類定傳染病&gt;結核病&gt;重要指引及教材項下查閱。\$\@\$感謝您與我們共同維護全民的健康安全。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-24\$\@\$一、考評單位：衛生福利部疾病管制署。\$\@\$二、考評目的：客觀衡量地方政府衛生局111年防疫業務之施政績效。\$\@\$三、受評機關：地方政府衛生局。\$\@\$四、受評期間：111年1月至12月\$\@\$五、考評架構與權重：9項考評指標，共計200分。\$\@\$六、考評方式：\$\@\$(一)   防疫業務相關管理系統之統計結果及書面考核。\$\@\$本手冊考評指標資料，如須受評機關提供始得評分者，請於112年1月13日前備函逕送考評執行單位進行評核。\$\@\$考評單位於指定日期前完成分數統計及成績評定。\$\@\$考評單位完成考評並請地方政府衛生局確認後，於111年3月17日前將考評結果送衛生福利部綜合規劃司備查。\$\@\$(二)   考評單位得視需要辦理實地查核。 附件\$\@\$111年地方衛生機關業務考評作業手冊-防疫類.pdf\$\@\$111年地方衛生機關業務考評作業手冊-防疫類.docx</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-20\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$公共關係室\$\@\$約用公關助理\$\@\$(徵才案號：0708)\$\@\$(計5名)\$\@\$王○琴(F22546****)\$\@\$李○怡(A22422****)\$\@\$李○達(F12468****)\$\@\$鍾○婷(T22347****)\$\@\$廖○儀(T22036****)\$\@\$二、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一)口試：\$\@\$1、報到時間：110年12月30日星期四09:50~10:00，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署1樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：10:00~11:30。\$\@\$(二)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(三)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於110年12月29日下午5點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3823)，俾利安排應試座位。\$\@\$(四)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(五)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-04\$\@\$中央流行疫情指揮中心今(4)日表示，為加速國人完成2劑接種，提升尚未接種第1、2劑COVID-19疫苗民眾之接種意願，各地方政府自2022年1月5日至1月31日前，可提供18歲以上民眾200元(含)以下衛教品，以鼓勵民眾踴躍完成接種2劑COVID-19疫苗，儘速獲得完整免疫保護力。\$\@\$指揮中心表示，截至2022年1月3日為止，我國COVID-19疫苗第一劑接種率約80%，第二劑接種率約69%，為因應國際疫情持續嚴峻及Omicron新型變異株之威脅增加，接種涵蓋率仍須再提升，目前COVID-19疫苗由地方政府衛生局指定/安排之合約醫療院所或衛生所進行接種，鼓勵尚未接種過任何1劑COVID-19疫苗及符合接種間隔但尚未完成2劑COVID-19疫苗接種之民眾，請儘速前往COVID-19疫苗合約醫療院所接種。\$\@\$指揮中心說明，目前國內各廠牌COVID-19疫苗供應充分，民眾可至衛生福利部疾病管制署全球資訊網，「COVID-19疫苗接種院所單元」（https://www.cdc.gov.tw/Category/List/u4l1b_gHhf9WDjhEtRmRRw），運用「COVID-19接種院所地圖」及各地方政府衛生局公告之COVID-19疫苗接種合約醫療院所以及車站等隨到隨打疫苗接種站，就近前往接種。\$\@\$指揮中心提醒， 18歲至未滿20歲民眾，如自行前往接種，請持家長簽具之意願同意書。若由家長陪同前往接種，請本人與家長於現場共同簽署意願同意書。另依衛生福利部傳染病防治諮詢會預防接種組(ACIP)建議，接種COVID-19疫苗應與流感疫苗等其他疫苗間隔至少7天，亦請民眾前往接種COVID-19疫苗前，應備妥健保卡或其他可證明身分之證件，如為接種第2劑COVID-19疫苗者亦請攜帶「COVID-19疫苗接種紀錄卡」，並於接種前評估時說明過往疫苗接種史，以利醫生評估。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-04\$\@\$中央流行疫情指揮中心今(4)日公布國內新增34例COVID-19確定病例，分別為4例(案17230、案17238-17240)本土及30例境外移入，其中案17230為昨(3)日公布之尚未取號本土個案；另確診個案中無新增死亡。\$\@\$指揮中心表示，案17238-17240為本國籍，1例男性、2例女性，年齡均為50多歲，皆已接種2劑疫苗，為案17230接觸者。案17238及案17239均為同職場工作人員，通勤時搭乘同班交通車，案17239於1月1日起陸續出現疲倦、咳嗽、流鼻水症狀；案17240為防疫計程車司機，1月1日出現咳嗽症狀，3人經衛生單位安排採檢後於今日確診，相關疫情調查、接觸者匡列及防治工作刻正進行中。\$\@\$指揮中心表示，今日新增30例境外移入個案，為16例男性、14例女性，年齡介於未滿5歲至70多歲，分別自美國(22例，案17207、案17210-17219、案17221、案17223-17228、案17231-17232、案17235-17236)、法國(案17208)、挪威(案17209)、南非(案17220)、阿拉伯聯合大公國(案17222)、英國(案17229)、波蘭(案17234)及烏茲別克(案17237)入境，另1例(案17233)調查中，入境日介於去(2021)年11月20日至今(2022)年1月3日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,998,949例新型冠狀病毒肺炎相關通報(含4,979,641例排除)，其中17,129例確診，分別為2,469例境外移入，14,606例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月4日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-03\$\@\$中央流行疫情指揮中心今(3)日公布國內新增1例COVID-19本土確定病例(尚未取號)，為本國籍40多歲女性，任機場停車場清潔人員，近期無出入境紀錄，已接種2劑AZ疫苗。個案於今(2022)年1/2出現發燒、畏寒、咳嗽、流鼻水、喉嚨痛等症狀，並於今日進行快篩，結果為陽性，同時採檢後確診。桃園市政府衛生局即刻啟動疫情調查，並立即通知同住家人就讀之兩校，分別預防性停課一天。\$\@\$指揮中心說明，桃園市政府在接獲醫院通報個案後，已通知個案家人就讀之兩校，分別預防性停課一天。並立即針對6名家人，已於今晚完成採檢，並以急件進行核酸檢驗，檢驗結果確認均為陰性，請兩校師生及家長不需擔憂。並對於個案之工作場域相關接觸者，現正擴大匡列採檢中，包括召回數百名防疫計程車司機將漏夜進行採檢，及針對個案所服務工作場域將進行清消。\$\@\$指揮中心進一步說明，個案另曾於去(2021)年12/30、12/31兩日上午9時至12時有至忠貞市場(中壢前龍街路段)擺攤賣小孩耳環、公仔、髪圈等，衛生單位將針對該市場進行疫調及接觸者匡列，並進行清消作業。\$\@\$指揮中心呼籲，民眾若曾於該段時間出入該場所，應請進行自我健康監測，若於1/14前出現發燒、上呼吸道、腹瀉、嗅味覺異常等症狀，應佩戴醫用口罩，儘速至社區採檢站或各指定採檢院所，接受採檢及評估。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-03\$\@\$中央流行疫情指揮中心今(3)日公布國內新增25例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增25例境外移入個案，為9例男性、16例女性，年齡介於未滿5歲至70多歲，分別自美國(15例，案17182-17183、案17186-17191、案17196-17197、案17199、案17201-17203、案17205)、土耳其(4例，案17192-17195)、德國(案17184)、加拿大(案17185)、義大利(案17198)、菲律賓(案17200)、亞美尼亞(案17204)及千里達及托巴哥(案17206)入境，入境日介於去(2021)年12月19日至今(2022)年1月1日；詳如新聞稿附件。\$\@\$另去年12月28日及12月30日公布之2例(案17058、案17099)境外移入病例經疫調後改判為本土病例，為案17085之相關感染。\$\@\$指揮中心統計，截至目前國內累計4,982,263例新型冠狀病毒肺炎相關通報(含4,962,860例排除)，其中17,095例確診，分別為2,439例境外移入，14,602例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月3日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-01\$\@\$中央流行疫情指揮中心今(1)日公布國內新增21例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增21例境外移入個案，為15例男性、6例女性，年齡介於20多歲至70多歲，分別自美國(9例，案17141、案17148、案17149、案17151、案17154、案17156、案17159-17161)、越南(6例，案17142、案17145、案17147、案17150、案17152、案17153)、埃及(案17143)、寮國(案17144)、瓜地馬拉(案17146)、羅馬尼亞(案17155)、烏克蘭(案17157)及德國(案17158)入境，入境日介於去(2021)年12月17日至12月31日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,961,497例新型冠狀病毒肺炎相關通報(含4,942,271例排除)，其中17,050例確診，分別為2,396例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月1日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-31\$\@\$中央流行疫情指揮中心今(31)日公布國內新增41例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增41例境外移入個案，為16例男性、25例女性，年齡介於20多歲至70多歲，分別自美國(14例，案17104-17106、案17112、案17113、案17115、案17116、案17118-17122、案17131、案17139)、菲律賓(2例，案17125、案17132)、法國(2例，案17117、案17124)、義大利(案17114)、肯亞(案17123)、喀麥隆(案17126)、瑞士(案17127)、印度(案17128)、阿拉伯聯合大公國(案17129)、烏克蘭(案17130)、越南(案17133)及柬埔寨(案17138)入境，另14例(案17100-17103、案17107-17111、案17134-17137、案17140)調查中，入境日介於今(2021)年12月16日至12月30日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,946,919例新型冠狀病毒肺炎相關通報(含4,927,473例排除)，其中17,029例確診，分別為2,375例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月31日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-30\$\@\$衛生福利部疾病管制署今（30）日公布「受聘僱外國人健康檢查管理辦法」部分條文修正案，並預訂於111年1月1日實施。本次修法重點包括「修正移工申請結核病都治條件」及「防疫期間調整移工健檢期限之法源依據」等事項，確保社區防疫安全。\$\@\$疾管署說明，結核病為結核桿菌感染所造成的慢性傳染病，目前抗結核藥物效果良好，連續服藥14天後的傳染力可大幅下降；透過移工主動配合、雇主支持，再加上結核病都治關懷員等衛生單位人員持續關心移工確實規則服藥，幾乎可以痊癒，且治療期間亦可正常工作與生活作息；此外，罹患結核病之移工若於國內完成治療，除能避免疾病持續傳播，維護員工健康外，亦不影響雇主勞動力需求。本辦法修正後，移工確診為肺結核、結核性肋膜炎（多重抗藥性結核病個案除外）或漢生病，且本人同意留臺配合按規治療者，雇主應於收受診斷證明書之次日起15日內，檢具「診斷證明書」及「受聘僱外國人接受衛生單位安排都治服務同意書」送縣市政府衛生局申請都治服務，共同落實社區防疫。\$\@\$疾管署指出，本辦法另增訂「中央流行疫情指揮中心成立期間，中央衛生主管機關得依國內疫情防治所需，調整移工健檢期限」及「自聘僱許可生效日起滿6、18及30個月之日與最近一次健檢日間隔未滿3個月者，免辦該次定期健檢」等規定；且回溯至自110年5月19日施行，以避免部分移工需於短期間內重複健檢，並能兼顧防疫安全。\$\@\$為利雇主（仲介）能瞭解本辦法修正後實務作業，疾病管制署提供「移工罹患結核病申請留臺治療」宣導海報、「認識結核病的問與答」多國語言宣導單張及宣導影片等相關衛教素材，並建置於該署全球資訊網（http://www.cdc.gov.tw ； 首頁&gt;國際旅遊與健康&gt;外國人健康管理&gt;受聘僱外國人健檢&gt;最新消息）供下載瀏覽。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-30\$\@\$中央流行疫情指揮中心今（30）日表示，由於國際疫情嚴峻及Omicron新型變異株之威脅日益擴散，近期入境人數及COVID-19境外移入個案增加，為強化社區監測，自明(2022)年1月1日起擴大辦理COVID-19社區加強監測方案，全國由86家定點診所發放公費COVID-19家用快篩試劑增加至272家，由各縣市人口數較多之鄉鎮市區基層診所協助發放試劑，因COVID-19症狀與一般感冒相似，提醒民眾如有出現呼吸道症狀，可多加前往該等診所，由醫師評估發放試劑後自行檢驗。\$\@\$指揮中心說明，今(2021)年8月30日起規劃推動COVID-19社區加強監測方案，迄今已發放1萬餘劑公費COVID-19家用快篩試劑，考量近期COVID-19社區傳播風險提升，為提高民眾取得公費家用快篩試劑可近性與及早發現自身感染之可能，將自明年1月1日起於全國21個縣市增加至272個診所試劑發放點，診所名單詳如新聞稿附件。\$\@\$指揮中心呼籲，現值呼吸道病毒活躍期，請民眾多加留意自身健康，如出現呼吸道症狀，可前往本計畫定點診所；民眾如為2歲以上出現呼吸道症狀的病患至公費快篩試劑發放診所掛號就醫，經醫師評估後發放試劑及注意事項說明單張，如為2歲以下幼兒的陪同看診者，亦由醫師評估後發放。民眾領取試劑後，請配合依注意事項說明內容儘速採檢，並至線上(https://forms.gle/8gh7Kb3ZkYE5aArW7)填寫試劑領取診所名稱及快篩結果等資料，此為匿名方式收集，無須擔心個人資料外洩情形。\$\@\$指揮中心提醒，如居家快篩檢驗為陽性時，請勿慌張並儘速至鄰近的社區採檢院所( https://reurl.cc/MArG1L )進一步PCR檢驗。民眾前往社區採檢院所時，請戴好口罩、勿搭乘大眾運輸工具，對於使用過之採檢器材請用塑膠袋密封包好，並攜帶至社區採檢院所，交予院所人員處理。 附件\$\@\$附件-配合辦理發放公費COVID-19家用快篩試劑社區定點診所名單.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-30\$\@\$中央流行疫情指揮中心今(30)日表示，台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的第十五批BNT疫苗93.83萬劑，已於今日上午順利運抵桃園國際機場，並在完成通關程序後，直接運送至指定冷儲物流中心進行後續檢驗封緘作業。\$\@\$指揮中心說明，由台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的BNT疫苗1,500萬劑，目前共計到貨1333.62萬劑，分別為首批9月2日93萬劑、第二批9月9日91萬劑、第三批9月30日54萬劑、第四批10月1日67萬劑、第五批10月4日27萬劑、第六批10月7日88.92萬劑、第七批10月8日88.92萬劑、第八批10月14日82.7萬劑、第九批10月28日90.21萬劑、第十批10月29日91.03萬劑、第十一批11月5日87.17萬劑、第十二批11月12日92.66萬劑、第十三批11月25日93.83萬劑、第十四批12月9日192.35萬劑，以及本批93.83萬劑。本批疫苗效期至2022年3月28日，將由指揮中心統籌運用，儘速提供民眾接種。\$\@\$對於台積電、鴻海暨永齡基金會、慈濟基金會三間企業和民間團體積極協助，提供更多的疫苗讓民眾接種，加速提升臺灣疫苗覆蓋率，指揮中心再次表達由衷的謝意。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-29\$\@\$中央流行疫情指揮中心今(29)日公布國內新增14例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增14例境外移入個案，為6例男性、8例女性，年齡介於10多歲至70多歲，分別自美國(10例，案17063-17070、案17072、案17073)、德國(案17062)、泰國(案17071)、香港(案17074)及越南(案17075)入境，入境日介於今(2021)年12月14日至12月27日；詳如新聞稿附件。\$\@\$指揮中心統計，累計4,917,481例新型冠狀病毒肺炎相關通報(含4,898,907例排除)，其中16,964例確診，分別為2,310例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月29日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-28\$\@\$中央流行疫情指揮中心今(28)日公布國內新增19例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增19例境外移入個案，為9例男性、10例女性，年齡介於未滿10歲至80多歲，分別自美國(8例，案17043、案17045-17049、案17051、案17056)、瑞士(案17044)、寮國(案17050)、越南(案17052)、柬埔寨(案17053)、加拿大(2例，案17054、案17061)、哈薩克(案17055)、香港(案17057)、中國(案17058)及阿根廷(2例，案17059、案17060)入境，入境日介於今(2021)年12月14日至12月26日；詳如新聞稿附件。\$\@\$指揮中心統計，累計4,901,375例新型冠狀病毒肺炎相關通報(含4,882,616例排除)，其中16,950例確診，分別為2,296例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月28日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-27\$\@\$中央流行疫情指揮中心今(27)日表示，近期考量國內整體疫情趨緩及配合疫苗接種政策，為兼顧國內產業用人需求及移工工作權益，因此適度鬆綁管制措施，自110年12月27日起，移工轉換新雇主及同一雇主調派移工變更工作地點，如移工已完整接種COVID-19疫苗，無須再事前安排移工檢驗PCR，但雇主及移工仍應落實指揮中心及勞動部規定的相關防疫措施。\$\@\$指揮中心表示，鼓勵在臺移工接種疫苗，以提升疫苗覆蓋率，降低群聚感染可能性。另取消PCR相關規定後，雇主仍應依規定落實強化宿舍管理、分艙分流、健康監測等其他防疫規定，若未落實防疫，仍將依就業服務法相關規定，處新臺幣6萬至30萬元罰鍰及不予核發接續聘僱許可。另雇主如委託仲介公司辦理移工生活照顧，因仲介公司未善盡受任事務，違反防疫措施，將依仲介公司違反就業服務法規定，處新臺幣6萬元以上至30萬元以下罰鍰。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-27\$\@\$中央流行疫情指揮中心今(27)日公布國內新增16例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增16例境外移入個案，為12例男性、4例女性，年齡介於10多歲至60多歲，分別自美國(8例，案17027-案17028、案17031、案17033-案17037)、越南(案17029)、匈牙利(案17030)、哈薩克(案17032)、菲律賓(案17038)、寮國(案17039)、英國(案17040)、德國(案17041)及印尼(案17042)入境，入境日介於今(2021)年12月12日至12月26日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,884,004例新型冠狀病毒肺炎相關通報(含4,864,380例排除)，其中16,931例確診，分別為2,277例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月27日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
     <t>發佈日期：2022-01-07\$\@\$中央流行疫情指揮中心今(7)日公布國內新增62例COVID-19確定病例，分別為4例本土個案(案17368-17371)及58例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，本土個案(案17368-17371)分別為本國籍1例男性、3例女性，年齡介於20至50多歲，均為桃園機場感染事件相關個案；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增58例境外移入個案，為29例男性、29例女性，年齡介於10多歲至70多歲，分別自美國(35例)、法國(4例)、英國(3例)、瑞士、越南及印度(各2例)、奧地利、智利、德國、加拿大、愛爾蘭、孟加拉、奈及利亞、墨西哥、西班牙及哥斯大黎加(各1例)入境，入境日介於去(2021)年12月22日至今(2022)年1月6日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,055,274例新型冠狀病毒肺炎相關通報(含5,035,769例排除)，其中17,258例確診，分別為2,588例境外移入，14,616例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另新增2例空號病例(案17271，案17272與舊案重複，改列空號)，累計113例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月7日新增本土COVID-19確診個案表.pdf\$\@\$1月7日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-06\$\@\$中央流行疫情指揮中心今(6)日公布國內新增43例COVID-19確定病例，為昨(5)日公布尚未取號的3例本土個案(案17307-17309)及40例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，案17307-17309為本國籍女性，年齡介於50至60多歲，皆已接種2劑疫苗，為案17230、案17238、案17239及案17266同職場工作人員；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增40例境外移入個案，為20例男性、20例女性，年齡介於未滿5歲至70多歲，分別自美國(24例，案17267、案17270、案17273-17275、案17277-17282、案17284-17289、案17291-17292、案17300、案17302、案17304-17306)、印度(3例，案17290、案17296、案17303)、巴拿馬(2例，案17271-17272)、荷蘭(案17268)、阿拉伯聯合大公國(2例，案17283、案17301)、加拿大(案17269)、菲律賓(案17276)、義大利(案17293)、英國(案17295)、中國(案17298)及法國(案17299)入境，另有2例(案17294、案17297)調查中，入境日介於去(2021)年12月26日至今(2022)年1月5日；詳如新聞稿附件。\$\@\$另去年12月31日公布之案17127境外移入病例經疫調後改判為本土病例，為案17073之相關感染。\$\@\$指揮中心統計，截至目前國內累計5,036,659例新型冠狀病毒肺炎相關通報(含5,016,638例排除)，其中17,198例確診，分別為2,532例境外移入，14,612例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月6日新增境外移入COVID-19確診個案表.pdf\$\@\$1月6日新增本土COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
     <t>發佈日期：2022-01-06\$\@\$中央流行疫情指揮中心今(6)日表示，考量目前國際COVID-19疫情嚴峻，請長者及其他 COVID-19感染後容易產生嚴重併發症之族群，儘速完成COVID-19疫苗基礎劑接種，提升保護力。\$\@\$指揮中心表示，目前我國75歲以上長者第1劑接種率僅約73%，第2劑接種率僅約67%，仍需再積極提升，為維護長者及風險族群健康，降低因感染COVID-19造成之重症、住院或死亡風險，家中長輩如尚未接種COVID-19疫苗第1、2劑，請於其身體狀況較穩定時，協助陪同至各地方政府衛生局安排或指定之合約醫療院所接種。\$\@\$指揮中心說明，疫苗接種後可能發生副作用，通常輕微並於數天內消失，並隨年齡層增加而減少，若擔心接種疫苗後所產生之副作用，可先與醫師討論，經諮詢評估選擇合適的疫苗接種。\$\@\$指揮中心表示，若為行動不便者，各地方政府衛生局亦設有到宅接種服務，有需求者可向各地方政府衛生局洽詢。另為鼓勵18歲以上尚未接種第1劑、第2劑COVID-19疫苗接種者儘速踴躍前往接種，於2022年1月5日至1月31日前接種COVID-19疫苗者，可獲得地方政府發放之200元(含)以下衛教品，鼓勵民眾儘速接種，獲得保護力。\$\@\$指揮中心提醒，依我國衛生福利部傳染病防治諮詢會預防接種組(ACIP)建議，接種COVID-19疫苗應與流感疫苗等其他疫苗間隔至少7天，亦請民眾前往接種COVID-19疫苗前，應備妥健保卡或其他可證明身分之證件，如為接種第2劑COVID-19疫苗者，請記得攜帶「COVID-19疫苗接種紀錄卡」，並於接種前評估時，說明過往疫苗接種史，以利醫生評估。另近期天氣多變，對於近期身體具狀況或慢性病情不穩定者，請於身體狀況較穩定後就近前往接種。接種後亦請多加留意身體狀況，多喝水多休息，亦請家人協助注意，如有持續發燒超過48小時、嚴重過敏反應如呼吸困難、氣喘、眩暈、心跳加速、全身紅疹等不適症狀，應儘速就醫釐清病因。</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-06\$\@\$中央流行疫情指揮中心今(6)日表示，因應國際COVID-19疫情嚴峻及Omicron新型變異株威脅，考量春節入境人潮且近期COVID-19境外移入確診個案增加，為確保國內醫療院所對疫情的因應及保全醫療量能，即日起調整醫療機構醫療應變作為，說明如下：\$\@\$一、全國專責病房及負壓隔離病房調整收治病人條件，專責病房僅收治疑似或確診COVID-19病人；負壓隔離病室則以收治疑似或確診COVID-19及其他空氣傳染之法定傳染病病人為原則，清空非必要(如非空氣傳染防護隔離治療)入住於負壓隔離病房的病人。\$\@\$二、臺北市、新北市、基隆市、桃園市之應變醫院，於3日內恢復開設急性一般病床總數之20%作為專責病房(開設床數含負壓隔離病床)，收治疑似或確診個案。\$\@\$三、臺北市、新北市、基隆市、宜蘭縣、桃園市、新竹市、新竹縣及苗栗縣之急性一般病床總數500床以上之急救責任醫院，於3日內恢復開設急性一般病床總數之5%作為專責病房(開設床數含負壓隔離病床)，收治疑似或確診個案。\$\@\$四、專責病房收治疑似或確診COVID-19病人應以一人一室為原則(家人、同住者、同行者等如均為確診個案且知情同意，得兩人一室)，並有適當動線規劃，分流分艙安置住院病人；落實固定照護團隊與服務區塊化，避免人員頻繁輪替或跨單位工作；配置適當且固定之工作人員(含清潔人員、傳送人員及照顧服務員等)，以防範院內感染傳播風險。\$\@\$指揮中心呼籲醫療機構落實感染管制、強化門禁管制及工作人員健康監測、加強員工使用適當個人防護裝備，以預防並降低醫院群聚感染風險。由於Omicron新型變異株可能造成突破性感染，降低疫苗之保護力，指揮中心籲請可接種追加劑疫苗之醫院工作人員儘速接種追加劑疫苗，以確保人員健康安全。指揮中心將持續監測國內外疫情發展，確實掌握病床數及相關醫療資源分配，滾動修正相關應變策略，完善醫療照護體系，確保醫療量能充足以因應疫情。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-05\$\@\$中央流行疫情指揮中心今(5)日公布國內新增3例COVID-19本土確定病例(尚未取號)，為擴大採檢清潔外包人員，於今日晚間檢驗陽性。\$\@\$指揮中心表示，3名個案均為女性，年齡分別為1例50多歲及2例60多歲，Ct值分別為33.8、23.4及19.5，為案17230、案17238、案17239及17266同職場工作人員，相關疫情調查、接觸者匡列及防治工作刻正進行中。\$\@\$指揮中心說明，因應桃園機場感染事件，指揮中心於第一時間針對外包清潔人員進行擴大採檢，已匡列861人，截至今日晚間，已有4例陽性（案17266及前述3例陽性）、855例陰性、1例檢驗中、1例待採檢。總計清潔外包人員已確診共7人（案17230、案17238-17239、17266、及前述3例）。\$\@\$指揮中心說明，因應今日晚間新增3位本土確診病例，前進指揮所立即啟動緊急作為如下：\$\@\$1. 針對清潔外包公司航廈夜班人員共93人，全數送集中檢疫所集中隔離。\$\@\$2. 該公司其餘未隔離員工，共768人，明後兩日（1月6日-1月7日）每日以家用快篩自我檢測，並彙整報告提供前進指揮所。1月8日將再度安排全員PCR檢驗。\$\@\$3. 已責成外包清潔公司嚴格確實執行員工健康監測，確保員工健康，以及早處理可能事件。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-05\$\@\$中央流行疫情指揮中心今(5)日公布國內新增26例COVID-19確定病例，分別為1例(案17266)本土及25例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，案17266為本國籍50多歲女性，已接種2劑莫德納疫苗(為突破性感染)，與案17230、案17238及案17239為同職場工作人員，曾與前述個案搭乘同路線交通車，原定於今(2022)年1月5日採檢，1月3日出現乾咳、喉嚨不適等症狀，1月4日自行前往採檢站採檢後於今日確診，相關疫情調查、接觸者匡列及防治工作刻正進行中。\$\@\$指揮中心表示，今日新增25例境外移入個案，為12例男性、13例女性，年齡介於未滿5歲至70多歲，分別自美國(12例，案17241-17243、案17245、案17250、案17252、案17254、案17256-17259、案17265)、法國(3例，案17244、案17246、案17253)、丹麥(案17247)、英國(17248)、玻利維亞(案17249)、德國(案17251)、史瓦帝尼王國(案17255)、澳洲(案17260)、巴拿馬(2例，案17261-17262)、瑞典(案17263)及印尼(案17264)入境，入境日介於去(2021)年11月14日至今(2022)年1月4日；詳如新聞稿附件。\$\@\$另1月2日公布之案17181境外移入病例經疫調後改判為本土病例，為案16941之相關感染。\$\@\$指揮中心統計，截至目前國內累計5,017,456例新型冠狀病毒肺炎相關通報(含4,998,328例排除)，其中17,155例確診，分別為2,493例境外移入，14,608例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月5日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-05\$\@\$疾管署今(5)日宣布，為提升疫苗接種人口涵蓋率，發揮疫苗最大效益，自2022年1月6日起，公費流感疫苗擴大提供全國6個月以上尚未接種之民眾接種，至疫苗用罄為止，疾管署呼籲尚未接種的計畫對象，尤其是65歲以上長者、學齡前幼兒及醫事人員等重點族群儘快接種，以保障自身及周遭人員的健康。\$\@\$疾管署表示，2021年度公費流感疫苗分2階段施打，除50至64歲無高風險慢性病成人於第二階段11月15日開打外，其於對象均為10月1日開打。截至2022年1月4日，公費疫苗總接種數約562萬劑，整體疫苗使用率逾91.9%，剩餘量約49萬劑；目前全國約有3,700餘家合約院所(含部分衛生所)提供接種服務，建議民眾可先透過各地方政府衛生局網頁、疾管署流感防治一網通(https://antiflu.cdc.gov.tw/)、疾管家或1922防疫諮詢專線，查詢鄰近合約院所名單，並向合約院所預約，以確保可施打到疫苗。\$\@\$另公費流感疫苗接種期間，COVID-19疫苗接種作業持續進行，依衛生福利部傳染病防治諮詢會預防接種組專家建議，2種疫苗接種間隔應至少7天，避免發生疫苗接種不良事件無法釐清。疾管署提醒民眾於預約或接種前主動告知疫苗接種史，合約院所應於接種區建立動線分流，並請相關工作人員於接種前落實檢核接種紀錄，接種後於健保卡黏貼流感疫苗接種貼紙。\$\@\$疾管署提醒，國內流感疫情仍處低點尚未進入流行期，民眾可儘速接種，以於流感疫情達高峰前獲得足夠保護力。近期氣溫偏低，為防範流感及COVID-19疫情雙重衝擊，民眾除接種疫苗，應養成良好衛生習慣，出現類流感症狀儘速戴口罩就醫，並在家休息，減少病毒傳播機會。如有流感疫苗或流感防治相關疑問，可至疾管署全球資訊網(https://www.cdc.gov.tw)，或撥打免付費防疫專線1922(或0800-001922)洽詢。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-04\$\@\$中央流行疫情指揮中心今(4)日表示，為因應桃園機場群聚感染案件，陳時中指揮官於今日下午協同醫療應變組王必勝副組長、桃園市政府衛生局王文彥局長、衛生福利部疾病管制署北區管制中心及機場公司航運中心工作人員，實地進行入境旅客動線勘查，評估釐清風險，檢視第一線人員防護裝備及消毒情形，並啟動下列防疫作為：\$\@\$一、 成立前進指揮所，由醫療應變組王必勝副組長擔任指揮官，統籌指揮相關防疫工作，進行跨單位溝通協調，並評估各單位現場作業風險，提出相關改善計畫。\$\@\$二、 針對高風險旅客(14天內有症狀)之入境動線，重新釐清評估風險，避免與其他民眾、工作人員接觸，降低傳播可能性。\$\@\$三、 配合桃園市政府衛生局採檢規劃「擴大、快速」戰略概念，擴大評估可能有在個案活動地(如清潔的廁所)活動之其他人員，快速進行相關篩檢。</t>
+    <t>發佈日期：2021-06-01\$\@\$中央流行疫情指揮中心今(1)日指出，近日有網友在通訊軟體LINE散布「臺中市太原路復健醫院被徵收為方艙醫院」，臺中市政府衛生局已澄清為不實訊息，請民眾勿再轉傳與散布，以免觸法遭罰。\$\@\$指揮中心表示，臺中市政府已對外澄清，此復健醫院近期進行搬遷作業，是為了提升醫療品質，正以BOT方式規劃市立綜合醫院，並非徵用作為方艙醫院。\$\@\$指揮中心副指揮官陳宗彥指出，因應疫情變化，各地方政府規劃應變醫院及專責醫院收治患者，民眾接獲來源不明的訊息時，應先進行查證，切勿隨意散播、轉傳，以免觸法。\$\@\$指揮中心重申，防疫相關資訊應以中央流行疫情指揮中心公布內容為主，散播假訊息構成犯罪，會被判處最高三年有期徒刑或併科三百萬元罰金。提醒民眾，收到來路不明訊息多加留意、查證，切勿轉傳散播，以免觸法。詳情請上官網查詢(http://at.cdc.tw/Q7S2Vt)。 圖片 附件\$\@\$網傳「臺中市太原路復健醫院被徵收為方艙醫院」為不實訊息勿轉傳.jpg\$\@\$勿散播不實訊息，以免觸法受罰.jpg</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-05-28\$\@\$近期國內疫情升溫，警方發現網路上有不肖人士販售「新冠病毒快篩試劑」，中央流行疫情指揮中心副指揮官陳宗彥今(28)日表示，擅自在網路販售新冠病毒檢驗試劑等第三級醫療器材已違反「醫療器材管理法」，目前警方已進行偵辦，提醒民眾切勿購買檢測，除有效性及檢測結果正確性均無法確認外，還可能危害自身健康。\$\@\$指揮中心指出，新冠病毒檢驗試劑是第三級醫療器材，依據「醫療器材管理法」規定，只有醫療器材商及藥局可以販賣，且國內並未開放可使用通訊方式在網路、電話、社群媒體等販售。\$\@\$指揮中心強調，不肖人士在網路擅自販售專案核准的新冠病毒檢驗試劑已違「醫療器材管理法」，會被罰3萬以上100萬以下罰鍰，如果民眾發現有類似狀況，可打1919專線或是向地方衛生局檢舉。 圖片 附件\$\@\$0528網路販售「新冠病毒快篩試劑」已觸法，警方偵辦中.jpg\$\@\$勿散播不實訊息，以免觸法受罰.jpg</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-09-28\$\@\$各位醫界朋友，您好：\$\@\$我國現行潛伏結核感染(LTBI)檢驗方式依受檢者年齡區分，未滿5歲以皮膚結核菌素試驗(TST)，5歲(含)以上抽血執行丙型干擾素釋放試驗(IGRA)。經參考世界衛生組織(WHO)、美國兒科醫學會(AAP)及國內臨床兒科醫師建議，並考量國際間已有相關研究指出IGRA可適用於2歲以上兒童，爰自本(110)年10月1日起擴大IGRA適用對象至2歲(含)以上兒童。\$\@\$IGRA檢驗方式較TST可減少兒童接種卡介苗造成的偽陽性結果，避免因環境非結核分枝桿菌(NTM)或卡介苗造成的TST增強效應(booster effect)，提升檢驗準確性，及早給予治療。倘2歲(含)至未滿5歲兒童無法執行IGRA檢驗，得維持使用TST方式。另，考量2歲以下因缺乏相關實證資料故暫不建議使用IGRA檢驗，仍維持TST方式檢測。\$\@\$此外，考量未滿5歲之結核病接觸者發病風險高，應於指標個案確診後儘速完成胸部X光攝影及LTBI檢驗，其中陽性者排除活動性結核病後應提供LTBI治療；陰性者可能處於LTBI空窗期，請LTBI合作醫師先提供預防性治療(prophylaxis)，俟接觸者與指標個案終止有效暴露滿8週後之LTBI檢驗結果，再決定是否停止預防性治療或完成LTBI治療，以降低發病風險。有關LTBI檢驗與治療資訊，請參考疾病管制署全球資訊網(https://www.cdc.gov.tw)&gt;傳染病與防疫專題&gt;傳染病介紹&gt;第三類法定傳染病&gt;結核病&gt;治療照護&gt;潛伏結核感染專區。\$\@\$感謝您與我們共同守護民眾的健康。 附件\$\@\$附件1-110年IGRA檢驗適用對象擴大至2歲以上兒童問答集.pdf\$\@\$附件2-未滿5歲結核病接觸者LTBI檢驗流程建議.pdf\$\@\$附件3-結核病接觸者就醫轉介單更新版.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-24\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$慢性傳染病組\$\@\$約用助理\$\@\$(徵才案號：0309)\$\@\$(計3名)\$\@\$林○萱(B22260****)\$\@\$陳○瑜(Q22389****)\$\@\$陳○君(F22674****)\$\@\$二、實作、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一)實作：\$\@\$1、報到時間：111年1月7日星期五13:20。\$\@\$2、報到地點：衛生福利部疾病管制署1樓(臺北市中正區林森南路6號)。\$\@\$3、實作時間：13:40~15:10。實作開始鈴響(13:40)未到者，喪失應考資格。\$\@\$(二)口試：\$\@\$1、報到時間：111年1月7日星期五15:20，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署1樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：15:30~16:30。\$\@\$(三)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(四)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於111年1月6日下午5點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3823)，俾利安排應試座位。\$\@\$(五)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(六)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。\$\@\$三、試場規則：\$\@\$(一)第一試為實作測驗，題型為資料串接統計分析，應試者得自行攜帶筆記型電腦，並預先安裝欲於測驗時使用的統計分析軟體(可選擇使用SAS、R、Excel等其他統計分析軟體)；未自行攜帶筆記型電腦者，則由本署提供公務電腦於測驗時使用(僅具Excel功能且無法安裝軟體)。\$\@\$(二)測驗中途不容許離場，並於考試時間過半後始得離場，離場後不得再進入試場。\$\@\$(三)測驗期間不允許上網、隨身攜帶手機(含智慧手環)、行動網卡、無線網路分享器等電子用品，並請關閉網路、手機、聲音及振動(含鬧鐘)，考試過程中如有上網、發出聲音及震動，均喪失應考資格。\$\@\$(四)個人用品(如書包等)置於考場前後，桌面上僅可放置必要文具(墊板須為透明；水杯、飲料亦禁止放置)。\$\@\$(五)有下列各款情事之一者，予以扣考並不予計分或不得繼續應考：\$\@\$1、冒名頂替。\$\@\$2、持用偽造或變造之證件。\$\@\$3、互換座位或試卷。\$\@\$4、傳遞文稿、參考資料、書寫有關文字之物件或有關信號。\$\@\$5、夾帶書籍文件。\$\@\$6、故意不繳交試卷或破壞試卷彌封。\$\@\$7、在桌椅、文具或肢體上或其他處所，書寫有關文字。\$\@\$8、電子通訊舞弊行為。\$\@\$9、窺視他人試卷、答案卷、作答結果或互相交談。\$\@\$10、在答案卷上書寫姓名、座號或其他不應有之文字、標記或自備稿紙書寫。\$\@\$11、其他破壞試場秩序事項。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-11-15\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$檢驗及疫苗研製中心\$\@\$約用助理\$\@\$(徵才案號：1057)\$\@\$(計3名)\$\@\$張○睿(I10045****)\$\@\$方○媃(Q22405****)\$\@\$洪○貞(E22306****)\$\@\$檢驗及疫苗研製中心\$\@\$約用研究助理\$\@\$(徵才案號：1058)\$\@\$(計4名)\$\@\$蘇○瑜(A22867****)\$\@\$李○志(P12320****)\$\@\$陳○均(F23000****)\$\@\$陳○君(C22130****)\$\@\$二、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一)口試：\$\@\$1、報到時間：110年11月25日星期四08:50~09:00，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署7樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：09:00~11:00。\$\@\$(二)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(三)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於110年11月24日下午3點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3823)，俾利安排應試座位。\$\@\$(四)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(五)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
   </si>
 </sst>
 </file>
@@ -523,7 +994,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -551,16 +1022,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="C2" s="2">
         <v>44569</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>116</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -568,16 +1039,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="C3" s="2">
         <v>44568</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>26</v>
+        <v>117</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -585,16 +1056,13 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="C4" s="2">
         <v>44568</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s">
-        <v>37</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -602,16 +1070,13 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="C5" s="2">
         <v>44567</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -619,16 +1084,13 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="C6" s="2">
         <v>44567</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -636,16 +1098,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="C7" s="2">
         <v>44567</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -653,16 +1115,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="C8" s="2">
-        <v>44566</v>
+        <v>44387</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>31</v>
+        <v>122</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -670,16 +1132,16 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="C9" s="2">
-        <v>44566</v>
+        <v>44360</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>32</v>
+        <v>123</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -687,16 +1149,16 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="C10" s="2">
-        <v>44566</v>
+        <v>44359</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>124</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -704,16 +1166,1254 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="2">
+        <v>44348</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="2">
+        <v>44344</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="2">
+        <v>44341</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="2">
+        <v>44567</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="2">
+        <v>44567</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="2">
+        <v>44560</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="2">
+        <v>44491</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="2">
+        <v>44469</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="2">
+        <v>44467</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="2">
+        <v>44568</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="2">
+      <c r="B21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="2">
+        <v>44567</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="2">
+        <v>44567</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="2">
+        <v>44566</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="2">
+        <v>44566</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="2">
+        <v>44566</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="2">
+        <v>44568</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="2">
+        <v>44568</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="2">
+        <v>44568</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="2">
+        <v>44567</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="2">
+        <v>44566</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="2">
+        <v>44566</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" s="2">
+        <v>44554</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="2">
+        <v>44554</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="2">
+        <v>44550</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E34" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="2">
+        <v>44515</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="2">
+        <v>44496</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="2">
+        <v>44494</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="2">
         <v>44565</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D38" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E38" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="2">
+        <v>44565</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E39" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" s="2">
+        <v>44564</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E40" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="2">
+        <v>44564</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E41" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" s="2">
+        <v>44563</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="2">
+        <v>44562</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E43" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="2">
+        <v>44561</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E44" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" t="s">
+        <v>103</v>
+      </c>
+      <c r="C45" s="2">
+        <v>44561</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46" s="2">
+        <v>44560</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E46" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" t="s">
+        <v>105</v>
+      </c>
+      <c r="C47" s="2">
+        <v>44560</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E47" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48" s="2">
+        <v>44560</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" t="s">
+        <v>107</v>
+      </c>
+      <c r="C49" s="2">
+        <v>44560</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E49" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" t="s">
+        <v>108</v>
+      </c>
+      <c r="C50" s="2">
+        <v>44559</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E50" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" t="s">
+        <v>109</v>
+      </c>
+      <c r="C51" s="2">
+        <v>44558</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E51" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" t="s">
+        <v>110</v>
+      </c>
+      <c r="C52" s="2">
+        <v>44557</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" t="s">
+        <v>111</v>
+      </c>
+      <c r="C53" s="2">
+        <v>44557</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" s="2">
+        <v>44557</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E54" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="2">
+        <v>44557</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" s="2">
+        <v>44557</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E56" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57" s="2">
+        <v>44557</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" t="s">
+        <v>60</v>
+      </c>
+      <c r="C58" s="2">
+        <v>44569</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E58" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" t="s">
+        <v>61</v>
+      </c>
+      <c r="C59" s="2">
+        <v>44568</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" t="s">
+        <v>62</v>
+      </c>
+      <c r="C60" s="2">
+        <v>44568</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E60" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>8</v>
+      </c>
+      <c r="B61" t="s">
+        <v>63</v>
+      </c>
+      <c r="C61" s="2">
+        <v>44567</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>9</v>
+      </c>
+      <c r="B62" t="s">
+        <v>64</v>
+      </c>
+      <c r="C62" s="2">
+        <v>44567</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E62" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63" t="s">
+        <v>65</v>
+      </c>
+      <c r="C63" s="2">
+        <v>44567</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E63" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>11</v>
+      </c>
+      <c r="B64" t="s">
+        <v>66</v>
+      </c>
+      <c r="C64" s="2">
+        <v>44387</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65" s="2">
+        <v>44360</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E65" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>13</v>
+      </c>
+      <c r="B66" t="s">
+        <v>68</v>
+      </c>
+      <c r="C66" s="2">
+        <v>44359</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E66" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>14</v>
+      </c>
+      <c r="B67" t="s">
+        <v>69</v>
+      </c>
+      <c r="C67" s="2">
+        <v>44348</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E67" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>15</v>
+      </c>
+      <c r="B68" t="s">
+        <v>70</v>
+      </c>
+      <c r="C68" s="2">
+        <v>44344</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E68" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" t="s">
+        <v>71</v>
+      </c>
+      <c r="C69" s="2">
+        <v>44341</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E69" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70" t="s">
+        <v>72</v>
+      </c>
+      <c r="C70" s="2">
+        <v>44567</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E70" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71" t="s">
+        <v>73</v>
+      </c>
+      <c r="C71" s="2">
+        <v>44567</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" t="s">
+        <v>74</v>
+      </c>
+      <c r="C72" s="2">
+        <v>44560</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>20</v>
+      </c>
+      <c r="B73" t="s">
+        <v>75</v>
+      </c>
+      <c r="C73" s="2">
+        <v>44491</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>21</v>
+      </c>
+      <c r="B74" t="s">
+        <v>76</v>
+      </c>
+      <c r="C74" s="2">
+        <v>44469</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>22</v>
+      </c>
+      <c r="B75" t="s">
+        <v>77</v>
+      </c>
+      <c r="C75" s="2">
+        <v>44467</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E75" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>23</v>
+      </c>
+      <c r="B76" t="s">
+        <v>78</v>
+      </c>
+      <c r="C76" s="2">
+        <v>44568</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>24</v>
+      </c>
+      <c r="B77" t="s">
+        <v>79</v>
+      </c>
+      <c r="C77" s="2">
+        <v>44567</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>25</v>
+      </c>
+      <c r="B78" t="s">
+        <v>80</v>
+      </c>
+      <c r="C78" s="2">
+        <v>44567</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>26</v>
+      </c>
+      <c r="B79" t="s">
+        <v>81</v>
+      </c>
+      <c r="C79" s="2">
+        <v>44566</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>27</v>
+      </c>
+      <c r="B80" t="s">
+        <v>82</v>
+      </c>
+      <c r="C80" s="2">
+        <v>44566</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>28</v>
+      </c>
+      <c r="B81" t="s">
+        <v>83</v>
+      </c>
+      <c r="C81" s="2">
+        <v>44566</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>29</v>
+      </c>
+      <c r="B82" t="s">
+        <v>84</v>
+      </c>
+      <c r="C82" s="2">
+        <v>44568</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>30</v>
+      </c>
+      <c r="B83" t="s">
+        <v>85</v>
+      </c>
+      <c r="C83" s="2">
+        <v>44568</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>30</v>
+      </c>
+      <c r="B84" t="s">
+        <v>86</v>
+      </c>
+      <c r="C84" s="2">
+        <v>44568</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>31</v>
+      </c>
+      <c r="B85" t="s">
+        <v>87</v>
+      </c>
+      <c r="C85" s="2">
+        <v>44567</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>32</v>
+      </c>
+      <c r="B86" t="s">
+        <v>88</v>
+      </c>
+      <c r="C86" s="2">
+        <v>44566</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>33</v>
+      </c>
+      <c r="B87" t="s">
+        <v>89</v>
+      </c>
+      <c r="C87" s="2">
+        <v>44566</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
         <v>34</v>
       </c>
-      <c r="E11" t="s">
-        <v>44</v>
+      <c r="B88" t="s">
+        <v>90</v>
+      </c>
+      <c r="C88" s="2">
+        <v>44554</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>35</v>
+      </c>
+      <c r="B89" t="s">
+        <v>91</v>
+      </c>
+      <c r="C89" s="2">
+        <v>44554</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E89" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>36</v>
+      </c>
+      <c r="B90" t="s">
+        <v>92</v>
+      </c>
+      <c r="C90" s="2">
+        <v>44550</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E90" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>37</v>
+      </c>
+      <c r="B91" t="s">
+        <v>93</v>
+      </c>
+      <c r="C91" s="2">
+        <v>44515</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E91" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>38</v>
+      </c>
+      <c r="B92" t="s">
+        <v>94</v>
+      </c>
+      <c r="C92" s="2">
+        <v>44496</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>39</v>
+      </c>
+      <c r="B93" t="s">
+        <v>95</v>
+      </c>
+      <c r="C93" s="2">
+        <v>44494</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -728,6 +2428,88 @@
     <hyperlink ref="D9" r:id="rId8"/>
     <hyperlink ref="D10" r:id="rId9"/>
     <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="D12" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId12"/>
+    <hyperlink ref="D14" r:id="rId13"/>
+    <hyperlink ref="D15" r:id="rId14"/>
+    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D17" r:id="rId16"/>
+    <hyperlink ref="D18" r:id="rId17"/>
+    <hyperlink ref="D19" r:id="rId18"/>
+    <hyperlink ref="D20" r:id="rId19"/>
+    <hyperlink ref="D21" r:id="rId20"/>
+    <hyperlink ref="D22" r:id="rId21"/>
+    <hyperlink ref="D23" r:id="rId22"/>
+    <hyperlink ref="D24" r:id="rId23"/>
+    <hyperlink ref="D25" r:id="rId24"/>
+    <hyperlink ref="D26" r:id="rId25"/>
+    <hyperlink ref="D27" r:id="rId26"/>
+    <hyperlink ref="D28" r:id="rId27"/>
+    <hyperlink ref="D29" r:id="rId28"/>
+    <hyperlink ref="D30" r:id="rId29"/>
+    <hyperlink ref="D31" r:id="rId30"/>
+    <hyperlink ref="D32" r:id="rId31"/>
+    <hyperlink ref="D33" r:id="rId32"/>
+    <hyperlink ref="D34" r:id="rId33"/>
+    <hyperlink ref="D35" r:id="rId34"/>
+    <hyperlink ref="D36" r:id="rId35"/>
+    <hyperlink ref="D37" r:id="rId36"/>
+    <hyperlink ref="D38" r:id="rId37"/>
+    <hyperlink ref="D39" r:id="rId38"/>
+    <hyperlink ref="D40" r:id="rId39"/>
+    <hyperlink ref="D41" r:id="rId40"/>
+    <hyperlink ref="D42" r:id="rId41"/>
+    <hyperlink ref="D43" r:id="rId42"/>
+    <hyperlink ref="D44" r:id="rId43"/>
+    <hyperlink ref="D45" r:id="rId44"/>
+    <hyperlink ref="D46" r:id="rId45"/>
+    <hyperlink ref="D47" r:id="rId46"/>
+    <hyperlink ref="D48" r:id="rId47"/>
+    <hyperlink ref="D49" r:id="rId48"/>
+    <hyperlink ref="D50" r:id="rId49"/>
+    <hyperlink ref="D51" r:id="rId50"/>
+    <hyperlink ref="D52" r:id="rId51"/>
+    <hyperlink ref="D53" r:id="rId52"/>
+    <hyperlink ref="D54" r:id="rId53"/>
+    <hyperlink ref="D55" r:id="rId54"/>
+    <hyperlink ref="D56" r:id="rId55"/>
+    <hyperlink ref="D57" r:id="rId56"/>
+    <hyperlink ref="D58" r:id="rId57"/>
+    <hyperlink ref="D59" r:id="rId58"/>
+    <hyperlink ref="D60" r:id="rId59"/>
+    <hyperlink ref="D61" r:id="rId60"/>
+    <hyperlink ref="D62" r:id="rId61"/>
+    <hyperlink ref="D63" r:id="rId62"/>
+    <hyperlink ref="D64" r:id="rId63"/>
+    <hyperlink ref="D65" r:id="rId64"/>
+    <hyperlink ref="D66" r:id="rId65"/>
+    <hyperlink ref="D67" r:id="rId66"/>
+    <hyperlink ref="D68" r:id="rId67"/>
+    <hyperlink ref="D69" r:id="rId68"/>
+    <hyperlink ref="D70" r:id="rId69"/>
+    <hyperlink ref="D71" r:id="rId70"/>
+    <hyperlink ref="D72" r:id="rId71"/>
+    <hyperlink ref="D73" r:id="rId72"/>
+    <hyperlink ref="D74" r:id="rId73"/>
+    <hyperlink ref="D75" r:id="rId74"/>
+    <hyperlink ref="D76" r:id="rId75"/>
+    <hyperlink ref="D77" r:id="rId76"/>
+    <hyperlink ref="D78" r:id="rId77"/>
+    <hyperlink ref="D79" r:id="rId78"/>
+    <hyperlink ref="D80" r:id="rId79"/>
+    <hyperlink ref="D81" r:id="rId80"/>
+    <hyperlink ref="D82" r:id="rId81"/>
+    <hyperlink ref="D83" r:id="rId82"/>
+    <hyperlink ref="D84" r:id="rId83"/>
+    <hyperlink ref="D85" r:id="rId84"/>
+    <hyperlink ref="D86" r:id="rId85"/>
+    <hyperlink ref="D87" r:id="rId86"/>
+    <hyperlink ref="D88" r:id="rId87"/>
+    <hyperlink ref="D89" r:id="rId88"/>
+    <hyperlink ref="D90" r:id="rId89"/>
+    <hyperlink ref="D91" r:id="rId90"/>
+    <hyperlink ref="D92" r:id="rId91"/>
+    <hyperlink ref="D93" r:id="rId92"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20220110
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="343">
   <si>
     <t>Press Title</t>
   </si>
@@ -49,91 +49,16 @@
     <t>因應春節入境人潮及COVID-19境外移入確診個案增加，指揮中心擴大開設專責病房及調整醫療機構應變策略</t>
   </si>
   <si>
-    <t>網傳「三級警戒微解封的不可思議之處」指揮中心： 原同住家人就不受限制，謠言邏輯誤導且比喻失當，請勿輕信轉傳，造成防疫困擾</t>
-  </si>
-  <si>
-    <t>網傳「政府讓人民施打未受認證且保護力低之國產疫苗」  指揮中心：會把關國產疫苗品質、安全及療效</t>
-  </si>
-  <si>
-    <t>網傳「代工(AZ疫苗)三億劑嫌太多賣不出去」，指揮中心：有心人刻意扭曲語意</t>
-  </si>
-  <si>
-    <t>網傳「臺中太原路復健醫院被徵收為方艙醫院」 指揮中心：假訊息勿轉傳</t>
-  </si>
-  <si>
-    <t>網路販售「新冠病毒快篩試劑」，指揮中心：已觸法，警方偵辦中</t>
-  </si>
-  <si>
-    <t>網現偽冒教育部網站  指揮中心：境外假網頁勿輕信</t>
-  </si>
-  <si>
-    <t>因應結核菌液態培養(MGIT)檢驗試劑暫時性缺貨，為利早期診斷結核病，針對疑似結核病送驗初查痰3套，請務必再進行結核分枝桿菌核酸增幅(NAA)檢驗(疾病管制署致醫界通函第470號)</t>
-  </si>
-  <si>
-    <t>COVID-19專家諮詢會因應變異株流行，更新治療指引藥物適用原則(疾病管制署致醫界通函第469號)</t>
-  </si>
-  <si>
-    <t>因應COVID-19 Omicron變異株威脅，籲請社區定點診所加強發放公費COVID-19家用快篩試劑予高風險民眾(疾病管制署致醫界通函第468號)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COVID-19專家諮詢會參照最新實證與藥物適應症，更新治療指引藥物適用對象並重申制定原則(疾病管制署致醫界通函第467號) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">近期登革熱隱藏期平均超過3日，籲請醫師對具登革熱流行地區旅遊史之疑似病例提高警覺，加強診斷及通報(疾病管制署致醫界通函第466號) </t>
-  </si>
-  <si>
-    <t>10月1日起擴大2歲以上兒童使用丙型干擾素釋放試驗(IGRA)，以提升潛伏結核感染(LTBI)檢驗準確性及守護幼童健康(疾病管制署致醫界通函第465號)</t>
-  </si>
-  <si>
-    <t>111年潛伏結核感染治療HP複方藥品.pdf(另開新視窗)</t>
-  </si>
-  <si>
-    <t>「111年人體測溫用紅外線熱影像儀維護保養」採購案.pdf(另開新視窗)</t>
-  </si>
-  <si>
-    <t>111年細胞培養及分生試劑乙批.pdf(另開新視窗)</t>
-  </si>
-  <si>
-    <t>111年疫情統計分析R系統維護及諮詢服務.pdf(另開新視窗)</t>
-  </si>
-  <si>
-    <t>111-112年 COVID-19疫苗4,000萬劑倉儲物流與配送.pdf(另開新視窗)</t>
-  </si>
-  <si>
-    <t>高屏區管制中心111年國際港埠檢體收送.pdf(另開新視窗)</t>
-  </si>
-  <si>
-    <t>助理研究員(預估缺)</t>
-  </si>
-  <si>
-    <t>師(三)級護理師</t>
-  </si>
-  <si>
-    <t>約聘護理師</t>
-  </si>
-  <si>
-    <t>約用護理師(徵才案號：1521延長公告)</t>
-  </si>
-  <si>
-    <t>約用助理(徵才案號：1522延長公告)</t>
-  </si>
-  <si>
-    <t>111年地方衛生機關防疫業務考評作業手冊</t>
-  </si>
-  <si>
-    <t>公告本署慢性傳染病組約用人員徵才案(徵才案號：0309)初審合格名單及甄試事宜。</t>
-  </si>
-  <si>
-    <t>公告本署公共關係室約用人員徵才案(徵才案號：0708)初審合格名單及甄試事宜。</t>
-  </si>
-  <si>
-    <t>公告本署檢驗及疫苗研製中心約用人員徵才案(徵才案號：1057、1058)初審合格名單及甄試事宜。</t>
-  </si>
-  <si>
-    <t>公告本署師(三)級護理師甄選之口試日程相關事宜(口試名單公告)。</t>
-  </si>
-  <si>
-    <t>公告本署急性傳染病組約用人員徵才案(徵才案號：1105)初審合格名單及甄試事宜。</t>
+    <t>新增3例COVID-19本土確定病例，衛生單位已啟動疫情調查及防治作為</t>
+  </si>
+  <si>
+    <t>新增26例COVID-19確定病例，分別為1例本土及25例境外移入</t>
+  </si>
+  <si>
+    <t>自2022年1月6日起，公費流感疫苗開放全民接種至疫苗用罄</t>
+  </si>
+  <si>
+    <t>針對桃園機場群聚感染案件，指揮中心今日成立前進指揮所協助防疫作為</t>
   </si>
   <si>
     <t>1月5日起至1月31日止，地方政府可提供民眾200元(含)以下衛教品，以提升接種意願</t>
@@ -196,6 +121,135 @@
     <t>12月28日至1月10日維持疫情警戒標準為第二級，請民眾配合跨年大型活動等防疫準備注意事項</t>
   </si>
   <si>
+    <t>新增24例COVID-19確定病例，分別為1例本土及23例境外移入</t>
+  </si>
+  <si>
+    <t>新增18例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>關鍵「疫」戰，感謝有您！指揮中心向COVID-19疫情期間貢獻卓越的第一線防疫英雄致謝！</t>
+  </si>
+  <si>
+    <t>指揮中心外部專家調查小組說明中研院ABSL-3實驗室感染事件初步調查結果</t>
+  </si>
+  <si>
+    <t>指揮中心說明如參與國內臨床試驗計畫，接種未經我國食品藥物管理署核准使用COVID-19疫苗之民眾，後續疫苗接種相關因應方式</t>
+  </si>
+  <si>
+    <t>新增13例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>歡慶佳節，「定期篩檢」是給自己和伴侶最好的禮物</t>
+  </si>
+  <si>
+    <t>春節檢疫專案擇C方案(7+7+7)入境者返家注意事項</t>
+  </si>
+  <si>
+    <t>指揮中心全面檢討防疫旅宿防疫作為，3大強化措施精進管理</t>
+  </si>
+  <si>
+    <t>新增10例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>AstraZeneca疫苗約73.84萬劑將於今(21)日下午抵臺</t>
+  </si>
+  <si>
+    <t>ACIP專家建議，符合COVID-19疫苗接種對象與間隔之民眾，應盡速完成基礎劑接種；已完成基礎劑接種且滿5個月之民眾，應接種追加劑</t>
+  </si>
+  <si>
+    <t>指揮中心說明中研院P3實驗室事件調查進度</t>
+  </si>
+  <si>
+    <t>新增11例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>新增6例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>新增15例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>因應近期疫情，指揮中心啟動防疫旅宿四大強化作為</t>
+  </si>
+  <si>
+    <t>新增12例COVID-19確定病例，分別為1例本土及11例境外移入</t>
+  </si>
+  <si>
+    <t>新增7例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>新增5例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>指揮中心宣布自12月14日至12月27日維持疫情警戒標準為第二級，請民眾持續配合防疫措施</t>
+  </si>
+  <si>
+    <t>指揮中心已全面提供民眾預約接種COVID-19疫苗第一、二劑，及已完整接種疫苗且滿５個月者接種追加劑，請民眾儘速完成二劑疫苗接種，以獲得完整免疫保護力</t>
+  </si>
+  <si>
+    <t>已完整接種COVID-19疫苗且滿5個月之民眾，可前往合約醫療院所接種COVID-19疫苗追加劑</t>
+  </si>
+  <si>
+    <t>疾管署攜手廚神奶爸蔣偉文推廣防疫雙語繪本，一起用繪本陪孩童共同思考正確防疫觀念！</t>
+  </si>
+  <si>
+    <t>「做好檢疫、返臺簡易」，指揮中心提醒旅客返臺前及機場通關應配合事項</t>
+  </si>
+  <si>
+    <t>台積電、鴻海永齡、慈濟三間企業和民間團體捐贈之第十四批BNT疫苗192.35萬劑於今(9)日下午抵臺</t>
+  </si>
+  <si>
+    <t>自111年1月1日起，強化因工作或服務性質具有「接觸不特定人士或無法保持社交距離」之部分場所(域)人員COVID-19疫苗接種規範，以嚴守社區防線</t>
+  </si>
+  <si>
+    <t>指揮中心臺北車站之「莫德納疫苗施打站」將延長開設至12/12，請民眾把握時間多加利用</t>
+  </si>
+  <si>
+    <t>指揮中心再度重申治安機關不會針對接種疫苗之失聯移工進行查處，請各單位依防疫政策辦理</t>
+  </si>
+  <si>
+    <t>自111年1月1日起，強化教育部、經濟部、勞動部、衛生福利部業管之部分場所(域)人員COVID-19疫苗接種規範，請儘速於110年12月17日前完整接種疫苗2劑，以嚴守社區防線</t>
+  </si>
+  <si>
+    <t>指揮中心12/5-12/9於臺北車站大廳開設「莫德納疫苗施打站」，歡迎民眾多加利用</t>
+  </si>
+  <si>
+    <t>新增4例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>目前已全面提供民眾COVID-19疫苗第一、二劑預約接種，請民眾利用「COVID-19公費疫苗預約平臺」、各地方政府衛生局指定或安排的醫療院所或衛生所等管道進行預約</t>
+  </si>
+  <si>
+    <t>因應Omicron變異株疫情，即日起提供已完整接種COVID-19疫苗且滿５個月之民眾，接種COVID-19疫苗追加劑</t>
+  </si>
+  <si>
+    <t>新增17例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>新增8例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>感謝地方政府及醫療院所通力合作，妥善運用疫苗資源，提升國人疫苗涵蓋率</t>
+  </si>
+  <si>
+    <t>疾管署與奧運拳擊國手黃筱雯共同出擊，邀請您一起「戰勝愛滋，分享愛」!</t>
+  </si>
+  <si>
+    <t>12月1日零時起，增列馬拉威、莫三比克、埃及、奈及利亞等4個國家為「重點高風險國家」，入境後須入住集中檢疫所</t>
+  </si>
+  <si>
+    <t>12-17歲青少年第二劑BioNTech COVID-19疫苗接種建議</t>
+  </si>
+  <si>
+    <t>為提升免疫保護力，專家建議接種COVID-19疫苗追加劑</t>
+  </si>
+  <si>
+    <t>指揮中心宣布自11月30日至12月13日維持疫情警戒標準為第二級，並宣布歲末／跨年大型活動防疫準備注意事項，請民眾持續配合</t>
+  </si>
+  <si>
+    <t>新增12例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
     <t>/Bulletin/Detail/QcNPHHjaJVEr-bnW4hG5RQ?typeid=9</t>
   </si>
   <si>
@@ -214,94 +268,16 @@
     <t>/Bulletin/Detail/u0vHFZX2nzlhWBifQl3x5Q?typeid=9</t>
   </si>
   <si>
-    <t>/Bulletin/Detail/ftv6FPFis84j5uHWTq4lNA?typeid=8772</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/PmSCiSjM5YpCUxXqoS81RA?typeid=8772</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/QCmwPRiL1nKrc8-AuqSEGg?typeid=8772</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/IO3F02JMs4pToOM84aXopQ?typeid=8772</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/zjF-6vCLlbYe1RhTXKlq1Q?typeid=8772</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/IU5CMLLt8bQqXWHQhil0Aw?typeid=8772</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/KaqzyT5RqFOuOQFGpEYLgA?typeid=48</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/zUiCR7uM2Ox39wGHOkzhMw?typeid=48</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/tun0Es9fOoIJqDFToylh6Q?typeid=48</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/1pVYYgWzE_U3RlTuctsioQ?typeid=48</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/HU4mCbrzZQlHC-VhwBiJOg?typeid=48</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/DyZ6ZOuk-VLQSHiQ6xhqoQ?typeid=48</t>
-  </si>
-  <si>
-    <t>/Uploads/files/2eca6680-fdde-4a38-934a-6da1c2dd8b8b.pdf</t>
-  </si>
-  <si>
-    <t>/Uploads/files/575633c9-11a3-4d2c-a5df-3bc675a198dc.pdf</t>
-  </si>
-  <si>
-    <t>/Uploads/files/a022ad25-9fb8-433f-a588-a93c1e5f9d9c.pdf</t>
-  </si>
-  <si>
-    <t>/Uploads/files/557f2695-c3ee-4d00-aa33-5d0dc36f7f09.pdf</t>
-  </si>
-  <si>
-    <t>/Uploads/files/a22b63a6-c6cb-463f-940d-26f4c11b17bc.pdf</t>
-  </si>
-  <si>
-    <t>/Uploads/files/0516860c-da1c-4620-ae05-79a01343a4d6.pdf</t>
-  </si>
-  <si>
-    <t>/HireList/Detail?hireId=kLNv1XH1fB8TlCZo6RSNGw</t>
-  </si>
-  <si>
-    <t>/HireList/Detail?hireId=7afE7y_q_0a-FLqnxHIjIA</t>
-  </si>
-  <si>
-    <t>/HireList/Detail?hireId=0i1H55b5Pqk0ahyBe-cr-A</t>
-  </si>
-  <si>
-    <t>/HireList/Detail?hireId=2tmdwtNL8GDuj002O3_QsA</t>
-  </si>
-  <si>
-    <t>/HireList/Detail?hireId=3FDssdDwiCeDzVB2w5R-gA</t>
-  </si>
-  <si>
-    <t>/HireList/Detail?hireId=HnyAaEpJjNTAhTgoRupHfg</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/Y_cTXA-RBSS1MjAEFDP3TQ?typeid=11</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/vN_TxnDuv7GamvGxnZXEdw?typeid=11</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/7UJRpdDRbQNIZWyyEfHdHQ?typeid=11</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/u9ej71cxiu9bJqO0gMxdOQ?typeid=11</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/_EjXyzKBrURN93eoTpH45Q?typeid=11</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/6_WqkhWC-GJV1mcZ8hGpEg?typeid=11</t>
+    <t>/Bulletin/Detail/jK3GN-Hw8x_ELLciTmfwQg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/xR3EWQ6aKrqsQwfI_iNxqg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/oHyBMuXSjeea-EJ0olgdRQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Y4fwruTZG4YQclQTSYPT-w?typeid=9</t>
   </si>
   <si>
     <t>/Bulletin/Detail/Q-xhjZ6c709hJ-9GQXtFFw?typeid=9</t>
@@ -364,6 +340,186 @@
     <t>/Bulletin/Detail/nIdKcbV265_Oy19NRrVK0g?typeid=9</t>
   </si>
   <si>
+    <t>/Bulletin/Detail/E9JqcdOD9YBfOq_fOEruwQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/D9upl4oQF7fRR8BX1H0Gqg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/-GpLgraJhhrmCF_EV5snAg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/DyYwMZYOnDPQaxZXyYkGag?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/U_G8thyYx_NXqs4bt22mLQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/ZRGaGQGvgOVp0sgi7p0Flw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/3PbK6u1juCPF_H5RpSmg1A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/K6-Py9CkPH7F7fbEhkN-cg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/kWxZwn01NkNft8vvuR-8iQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/M936bwIy8h1c3o0JAGx6XQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/OFCGVMPdO7s8EroSL08bnw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/ZCHA5BJcbAHqa3rEfKzgiQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/4ig8Ulsdu5Upgxk7yAoHbw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/L-qJBbrKStZuXh0N0Y1B7A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/DDtX98YMnWlt1E5YooyXig?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/IgdrNGmRzvUV_y1dDQZLbg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/GqrECv8g1A5pcuUsJbNwyA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/xpr8IEBdD6agTmKYO0do_Q?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/ZEZs-BpahQJyNxIgZMvnmw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/g07xJkUnioeBi2K4x_oa8A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/j0Lv5A4_bB5XCnhGvdJYzw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/DF7ogeZZ4Sq2mcsf3p5V1A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/jYSkhkTuIrL1g8h4BnsiPw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/8ZtmGnmnTDndGf1ih_-ZgA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/BawHgYTsb-Ifbw2VpNUErA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/6_2cOpRBTVjg_3-72yJMVQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/XL05Cn8AuiHJYNBfEMlPUA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/ruOWq6GTSZGSOq38yIgd3w?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/PnGZZJOra7MGuKGaHvOMnw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/UN5fQgp3h2gfyNntP6ouCQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/o-9C7vcqy3glqLxfaZr0rA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/fj9M7VB1NY9hkka3hbzqZg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/NI47Ps_FwSzR-S0AKTUsOQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/M6sT3rx4Rd7QcDxcnCG8ow?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/ka15R2rxOSpGsHael2mbNg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/-boqIqRww_Yy5jsG6ykh4A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Cw2WizvTzxs1dNf94r8Fnw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/leTuUMjsTGLW2_z9xHKGtA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/UTOmrhMe_NCgvE6ng0eQpQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/DkHH9jmlqsuArel0Ge54ig?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/XIxEY8HS7u87sxrY5rsZcw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/uZUdiaR1R7nr_G3N1VnVNQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Nw8YySH5kTUhHqnmT5ZVDg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/QyP53F_Wz5w2aH-FyMZoYA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/j64gUcFiy8FFvnjgoM5oyw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/F8-1SIJFEYKojfzKvCdPlQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Np-A0yrPBcpPrd8Kd2z18A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/798cb1f2X8khkCiLzskCRA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/TejSFjyPpHPOxcpKU26DyQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/GrUNWEYBePWBA55X5f08Fg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/qfSGTQPpNsErzyNcZmWsvg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/K4mTgO4hBZ97ER1dRHGqxQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/VVem5ruoxZhiPBFveSPiLQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/li9brSynHWZJlsVyo8ePTA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/HWZBo7OcNi_zzoXb5_g2SA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/22wN1aouBR921VG4dFhDmA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/m00G4Iadc5c7bts6_BIahw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/g3P2I2f95J6p71e1KnOaaQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/ANy77Zi3gOROMqIijYiUbQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/l5TWIq4FmR_R3yAuW40-iA?typeid=9</t>
+  </si>
+  <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/QcNPHHjaJVEr-bnW4hG5RQ?typeid=9</t>
   </si>
   <si>
@@ -382,94 +538,16 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/u0vHFZX2nzlhWBifQl3x5Q?typeid=9</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/ftv6FPFis84j5uHWTq4lNA?typeid=8772</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/PmSCiSjM5YpCUxXqoS81RA?typeid=8772</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/QCmwPRiL1nKrc8-AuqSEGg?typeid=8772</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/IO3F02JMs4pToOM84aXopQ?typeid=8772</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/zjF-6vCLlbYe1RhTXKlq1Q?typeid=8772</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/IU5CMLLt8bQqXWHQhil0Aw?typeid=8772</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/KaqzyT5RqFOuOQFGpEYLgA?typeid=48</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/zUiCR7uM2Ox39wGHOkzhMw?typeid=48</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/tun0Es9fOoIJqDFToylh6Q?typeid=48</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/1pVYYgWzE_U3RlTuctsioQ?typeid=48</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/HU4mCbrzZQlHC-VhwBiJOg?typeid=48</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/DyZ6ZOuk-VLQSHiQ6xhqoQ?typeid=48</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Uploads/files/2eca6680-fdde-4a38-934a-6da1c2dd8b8b.pdf</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Uploads/files/575633c9-11a3-4d2c-a5df-3bc675a198dc.pdf</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Uploads/files/a022ad25-9fb8-433f-a588-a93c1e5f9d9c.pdf</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Uploads/files/557f2695-c3ee-4d00-aa33-5d0dc36f7f09.pdf</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Uploads/files/a22b63a6-c6cb-463f-940d-26f4c11b17bc.pdf</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Uploads/files/0516860c-da1c-4620-ae05-79a01343a4d6.pdf</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=kLNv1XH1fB8TlCZo6RSNGw</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=7afE7y_q_0a-FLqnxHIjIA</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=0i1H55b5Pqk0ahyBe-cr-A</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=2tmdwtNL8GDuj002O3_QsA</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=3FDssdDwiCeDzVB2w5R-gA</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=HnyAaEpJjNTAhTgoRupHfg</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/Y_cTXA-RBSS1MjAEFDP3TQ?typeid=11</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/vN_TxnDuv7GamvGxnZXEdw?typeid=11</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/7UJRpdDRbQNIZWyyEfHdHQ?typeid=11</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/u9ej71cxiu9bJqO0gMxdOQ?typeid=11</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/_EjXyzKBrURN93eoTpH45Q?typeid=11</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/6_WqkhWC-GJV1mcZ8hGpEg?typeid=11</t>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/jK3GN-Hw8x_ELLciTmfwQg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/xR3EWQ6aKrqsQwfI_iNxqg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/oHyBMuXSjeea-EJ0olgdRQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Y4fwruTZG4YQclQTSYPT-w?typeid=9</t>
   </si>
   <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/Q-xhjZ6c709hJ-9GQXtFFw?typeid=9</t>
@@ -532,34 +610,211 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/nIdKcbV265_Oy19NRrVK0g?typeid=9</t>
   </si>
   <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/E9JqcdOD9YBfOq_fOEruwQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/D9upl4oQF7fRR8BX1H0Gqg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/-GpLgraJhhrmCF_EV5snAg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/DyYwMZYOnDPQaxZXyYkGag?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/U_G8thyYx_NXqs4bt22mLQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/ZRGaGQGvgOVp0sgi7p0Flw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/3PbK6u1juCPF_H5RpSmg1A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/K6-Py9CkPH7F7fbEhkN-cg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/kWxZwn01NkNft8vvuR-8iQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/M936bwIy8h1c3o0JAGx6XQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/OFCGVMPdO7s8EroSL08bnw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/ZCHA5BJcbAHqa3rEfKzgiQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/4ig8Ulsdu5Upgxk7yAoHbw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/L-qJBbrKStZuXh0N0Y1B7A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/DDtX98YMnWlt1E5YooyXig?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/IgdrNGmRzvUV_y1dDQZLbg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/GqrECv8g1A5pcuUsJbNwyA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/xpr8IEBdD6agTmKYO0do_Q?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/ZEZs-BpahQJyNxIgZMvnmw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/g07xJkUnioeBi2K4x_oa8A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/j0Lv5A4_bB5XCnhGvdJYzw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/DF7ogeZZ4Sq2mcsf3p5V1A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/jYSkhkTuIrL1g8h4BnsiPw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/8ZtmGnmnTDndGf1ih_-ZgA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/BawHgYTsb-Ifbw2VpNUErA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/6_2cOpRBTVjg_3-72yJMVQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/XL05Cn8AuiHJYNBfEMlPUA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/ruOWq6GTSZGSOq38yIgd3w?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/PnGZZJOra7MGuKGaHvOMnw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/UN5fQgp3h2gfyNntP6ouCQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/o-9C7vcqy3glqLxfaZr0rA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/fj9M7VB1NY9hkka3hbzqZg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/NI47Ps_FwSzR-S0AKTUsOQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/M6sT3rx4Rd7QcDxcnCG8ow?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/ka15R2rxOSpGsHael2mbNg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/-boqIqRww_Yy5jsG6ykh4A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Cw2WizvTzxs1dNf94r8Fnw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/leTuUMjsTGLW2_z9xHKGtA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/UTOmrhMe_NCgvE6ng0eQpQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/DkHH9jmlqsuArel0Ge54ig?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/XIxEY8HS7u87sxrY5rsZcw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/uZUdiaR1R7nr_G3N1VnVNQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Nw8YySH5kTUhHqnmT5ZVDg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/QyP53F_Wz5w2aH-FyMZoYA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/j64gUcFiy8FFvnjgoM5oyw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/F8-1SIJFEYKojfzKvCdPlQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Np-A0yrPBcpPrd8Kd2z18A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/798cb1f2X8khkCiLzskCRA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/TejSFjyPpHPOxcpKU26DyQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/GrUNWEYBePWBA55X5f08Fg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/qfSGTQPpNsErzyNcZmWsvg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/K4mTgO4hBZ97ER1dRHGqxQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/VVem5ruoxZhiPBFveSPiLQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/li9brSynHWZJlsVyo8ePTA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/HWZBo7OcNi_zzoXb5_g2SA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/22wN1aouBR921VG4dFhDmA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/m00G4Iadc5c7bts6_BIahw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/g3P2I2f95J6p71e1KnOaaQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/ANy77Zi3gOROMqIijYiUbQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/l5TWIq4FmR_R3yAuW40-iA?typeid=9</t>
+  </si>
+  <si>
     <t>發佈日期：2022-01-08\$\@\$中央流行疫情指揮中心今(8)日公布國內新增44例COVID-19確定病例，分別為2例本土個案(案17414-17415)及42例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，本土個案(案17414-17415)分別為本國籍1例男性、1例女性，年齡均為50多歲，均為桃園機場感染事件相關個案；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增42例境外移入個案，性別為25例男性、16例女性、1例調查中，年齡介於未滿10至70多歲，分別自美國(23例)、越南(4例)、法國(2例)、阿根廷、澳大利亞、菲律賓、加拿大、阿拉伯聯合大公國、泰國、巴西、西班牙、印度、義大利及德國(各1例)入境，另有2例調查中，入境日介於去(2021)年12月15日至今(2022)年1月7日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,074,946例新型冠狀病毒肺炎相關通報(含5,055,445例排除)，其中17,302例確診，分別為2,630例境外移入，14,618例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計113例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月8日新增本土COVID-19確診個案表.pdf\$\@\$1月8日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
     <t>發佈日期：2022-01-07\$\@\$中央流行疫情指揮中心今(7)日表示，因應國內發生Omicron變異株本土確診病例，社區感染風險提升，衛生福利部傳染病防治諮詢會預防接種組(ACIP)決議，已接種兩劑COVID-19疫苗且間隔滿12週(84天)以上之滿18歲民眾，應儘速接種1劑COVID-19疫苗追加劑，以提升免疫保護力。\$\@\$指揮中心說明，昨(6)日召開ACIP會議討論COVID-19疫苗接種策略，考量國內外COVID-19疫情升溫，為降低社區傳播風險，專家指出，建議滿18歲以上民眾於完整接種COVID-19疫苗基礎劑12週後，應接種1劑追加劑，以提升個人及群體免疫力。追加劑接種廠牌建議如下：\$\@\$一、以mRNA疫苗(如Moderna、BNT)或蛋白質次單元疫苗(如高端)完成基礎劑：追加劑可以選擇接種Moderna(半劑量)、BNT、高端或AZ疫苗。\$\@\$二、以AZ完成基礎劑：追加劑可選擇接種mRNA或蛋白質次單元疫苗。\$\@\$指揮中心指出，目前國內疫苗庫存充足，將請地方政府衛生局儘速擴充接種量能，符合接種間隔的民眾可透過「COVID-19疫苗防治一網通」( https://antiflu.cdc.gov.tw/Covid19 )或地方政府衛生局公告，查詢鄰近合約醫療院所提供施打之疫苗廠牌及接種時間。\$\@\$*備註：國外接種疫苗者，接種追加劑說明：\$\@\$一、於國外曾接種WHO EUL 之COVID-19疫苗 返國後請先至就近衛生所或健康服務中心補登國外疫苗接種紀錄，並妥善保存國外接種紀錄。\$\@\$二、符合現行追加劑接種間隔者(至少12週)，可攜國外接種紀錄、健保卡或相關身分證明文件，至鄰近COVID-19疫苗合約院所掛號接種。\$\@\$三、如接種非WHO EUL COVID-19疫苗, 視同無效劑次, 可於與最後一劑COVID-19疫苗間隔28天後, 於國內先完成COVID-19疫苗基礎劑接種，再依規定接種追加劑。</t>
   </si>
   <si>
+    <t>發佈日期：2022-01-07\$\@\$中央流行疫情指揮中心今(7)日公布國內新增62例COVID-19確定病例，分別為4例本土個案(案17368-17371)及58例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，本土個案(案17368-17371)分別為本國籍1例男性、3例女性，年齡介於20至50多歲，均為桃園機場感染事件相關個案；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增58例境外移入個案，為29例男性、29例女性，年齡介於10多歲至70多歲，分別自美國(35例)、法國(4例)、英國(3例)、瑞士、越南及印度(各2例)、奧地利、智利、德國、加拿大、愛爾蘭、孟加拉、奈及利亞、墨西哥、西班牙及哥斯大黎加(各1例)入境，入境日介於去(2021)年12月22日至今(2022)年1月6日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,055,274例新型冠狀病毒肺炎相關通報(含5,035,769例排除)，其中17,258例確診，分別為2,588例境外移入，14,616例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另新增2例空號病例(案17271，案17272與舊案重複，改列空號)，累計113例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月7日新增本土COVID-19確診個案表.pdf\$\@\$1月7日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-06\$\@\$中央流行疫情指揮中心今(6)日公布國內新增43例COVID-19確定病例，為昨(5)日公布尚未取號的3例本土個案(案17307-17309)及40例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，案17307-17309為本國籍女性，年齡介於50至60多歲，皆已接種2劑疫苗，為案17230、案17238、案17239及案17266同職場工作人員；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增40例境外移入個案，為20例男性、20例女性，年齡介於未滿5歲至70多歲，分別自美國(24例，案17267、案17270、案17273-17275、案17277-17282、案17284-17289、案17291-17292、案17300、案17302、案17304-17306)、印度(3例，案17290、案17296、案17303)、巴拿馬(2例，案17271-17272)、荷蘭(案17268)、阿拉伯聯合大公國(2例，案17283、案17301)、加拿大(案17269)、菲律賓(案17276)、義大利(案17293)、英國(案17295)、中國(案17298)及法國(案17299)入境，另有2例(案17294、案17297)調查中，入境日介於去(2021)年12月26日至今(2022)年1月5日；詳如新聞稿附件。\$\@\$另去年12月31日公布之案17127境外移入病例經疫調後改判為本土病例，為案17073之相關感染。\$\@\$指揮中心統計，截至目前國內累計5,036,659例新型冠狀病毒肺炎相關通報(含5,016,638例排除)，其中17,198例確診，分別為2,532例境外移入，14,612例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月6日新增境外移入COVID-19確診個案表.pdf\$\@\$1月6日新增本土COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-06\$\@\$中央流行疫情指揮中心今(6)日表示，考量目前國際COVID-19疫情嚴峻，請長者及其他 COVID-19感染後容易產生嚴重併發症之族群，儘速完成COVID-19疫苗基礎劑接種，提升保護力。\$\@\$指揮中心表示，目前我國75歲以上長者第1劑接種率僅約73%，第2劑接種率僅約67%，仍需再積極提升，為維護長者及風險族群健康，降低因感染COVID-19造成之重症、住院或死亡風險，家中長輩如尚未接種COVID-19疫苗第1、2劑，請於其身體狀況較穩定時，協助陪同至各地方政府衛生局安排或指定之合約醫療院所接種。\$\@\$指揮中心說明，疫苗接種後可能發生副作用，通常輕微並於數天內消失，並隨年齡層增加而減少，若擔心接種疫苗後所產生之副作用，可先與醫師討論，經諮詢評估選擇合適的疫苗接種。\$\@\$指揮中心表示，若為行動不便者，各地方政府衛生局亦設有到宅接種服務，有需求者可向各地方政府衛生局洽詢。另為鼓勵18歲以上尚未接種第1劑、第2劑COVID-19疫苗接種者儘速踴躍前往接種，於2022年1月5日至1月31日前接種COVID-19疫苗者，可獲得地方政府發放之200元(含)以下衛教品，鼓勵民眾儘速接種，獲得保護力。\$\@\$指揮中心提醒，依我國衛生福利部傳染病防治諮詢會預防接種組(ACIP)建議，接種COVID-19疫苗應與流感疫苗等其他疫苗間隔至少7天，亦請民眾前往接種COVID-19疫苗前，應備妥健保卡或其他可證明身分之證件，如為接種第2劑COVID-19疫苗者，請記得攜帶「COVID-19疫苗接種紀錄卡」，並於接種前評估時，說明過往疫苗接種史，以利醫生評估。另近期天氣多變，對於近期身體具狀況或慢性病情不穩定者，請於身體狀況較穩定後就近前往接種。接種後亦請多加留意身體狀況，多喝水多休息，亦請家人協助注意，如有持續發燒超過48小時、嚴重過敏反應如呼吸困難、氣喘、眩暈、心跳加速、全身紅疹等不適症狀，應儘速就醫釐清病因。</t>
+  </si>
+  <si>
     <t>發佈日期：2022-01-06\$\@\$中央流行疫情指揮中心今(6)日表示，因應國際COVID-19疫情嚴峻及Omicron新型變異株威脅，考量春節入境人潮且近期COVID-19境外移入確診個案增加，為確保國內醫療院所對疫情的因應及保全醫療量能，即日起調整醫療機構醫療應變作為，說明如下：\$\@\$一、全國專責病房及負壓隔離病房調整收治病人條件，專責病房僅收治疑似或確診COVID-19病人；負壓隔離病室則以收治疑似或確診COVID-19及其他空氣傳染之法定傳染病病人為原則，清空非必要(如非空氣傳染防護隔離治療)入住於負壓隔離病房的病人。\$\@\$二、臺北市、新北市、基隆市、桃園市之應變醫院，於3日內恢復開設急性一般病床總數之20%作為專責病房(開設床數含負壓隔離病床)，收治疑似或確診個案。\$\@\$三、臺北市、新北市、基隆市、宜蘭縣、桃園市、新竹市、新竹縣及苗栗縣之急性一般病床總數500床以上之急救責任醫院，於3日內恢復開設急性一般病床總數之5%作為專責病房(開設床數含負壓隔離病床)，收治疑似或確診個案。\$\@\$四、專責病房收治疑似或確診COVID-19病人應以一人一室為原則(家人、同住者、同行者等如均為確診個案且知情同意，得兩人一室)，並有適當動線規劃，分流分艙安置住院病人；落實固定照護團隊與服務區塊化，避免人員頻繁輪替或跨單位工作；配置適當且固定之工作人員(含清潔人員、傳送人員及照顧服務員等)，以防範院內感染傳播風險。\$\@\$指揮中心呼籲醫療機構落實感染管制、強化門禁管制及工作人員健康監測、加強員工使用適當個人防護裝備，以預防並降低醫院群聚感染風險。由於Omicron新型變異株可能造成突破性感染，降低疫苗之保護力，指揮中心籲請可接種追加劑疫苗之醫院工作人員儘速接種追加劑疫苗，以確保人員健康安全。指揮中心將持續監測國內外疫情發展，確實掌握病床數及相關醫療資源分配，滾動修正相關應變策略，完善醫療照護體系，確保醫療量能充足以因應疫情。</t>
   </si>
   <si>
-    <t>發佈日期：2021-07-10\$\@\$中央流行疫情指揮中心今（10）日表示，近日有網友散布「三級警戒微解封的不可思議之處，新冠肺炎病毒只會攻擊家人」等訊息，相關內容多有誤導，且在錯誤基礎上進行不當類比，指揮中心再次強調，相關防疫指引已清楚說明，原本同住家人可以繼續維持生活，相關指引都是針對日常非同住者間的行為互動加以規範，呼籲民眾勿輕信或隨意散播、轉傳錯誤訊息，造成防疫困擾。\$\@\$指揮中心指出，有關7月13號以後針對部分場所將適度鬆綁，但仍須遵守防疫相關指引及規範，而此波疫情中，不少個案均為家戶群聚感染，由於室內密切接觸風險較高，因此對於室內社交人數須有較嚴格規範，但不包含原本同住的家人，也無需限制同住家人不能在家打麻將、看電影、吃飯等。 圖片 附件\$\@\$0710指揮中心：勿輕信「三級警戒微解封的不可思議之處」之網傳.jpg</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-06-13\$\@\$近日有網友在臉書FB以自製圖文方式散布「政府讓人民施打未受認證且保護力低之國產疫苗」、「國產疫苗的中和抗體效價比國外疫苗差」、「國產疫苗為什麼不向國際提出緊急授權」，中央流行疫情指揮中心(下稱指揮中心)今（13）日嚴正澄清表示，目前國產疫苗臨床試驗尚在進行中，最終結果須等廠商提出EUA 申請，經專家會議審查疫苗的製程管控、藥毒理試驗及臨床試驗結果，在緊急公衛的需求下，確認疫苗使用效益大於風險，才會核准緊急授權使用。\$\@\$指揮中心指出，目前國產疫苗廠商皆已積極規劃，以取得國際認證為目標。國產疫苗需經食藥署和專家會議嚴謹審查，在緊急公衛需求，並確認效益大於風險，才會核准緊急授權使用。此外，各家廠牌的疫苗所使用的檢驗實驗室及檢驗方式不同且無協和，無法直接由各實驗室產生數值進行比較。國產疫苗仍需等廠商提出申請，經過中央主管機關嚴格把關及審查通過後，確認品質、安全、療效後，品質沒有問題，疫苗方可供民眾施打。\$\@\$指揮中心再次提醒，民眾接獲來源不明的訊息時，應先進行查證，切勿隨意散播、轉傳，以免觸法。 圖片 附件\$\@\$0613網傳「政府讓人民施打未受認證且保護力低之國產疫苗」-1.jpg\$\@\$0613網傳「政府讓人民施打未受認證且保護力低之國產疫苗」-2.jpg</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-06-12\$\@\$中央流行疫情指揮中心今(12)日嚴正澄清，近日於社群平台流傳「代工三億劑嫌太多賣不出去」等訊息，指揮中心於6月10日記者會已公開說明，與AstraZeneca原廠洽談授權製造事宜時，我方提出可年產一億劑之規劃，但原廠要求需年產三億劑，經評估，對我方產能過於沉重，並無以「賣不出去」為由拒絕原廠授權製造，卻被有心人刻意扭曲語意。此圖文與事實不符，指揮中心特此澄清。\$\@\$指揮中心重申，防疫相關資訊應以中央流行疫情指揮中心公布內容為主。提醒民眾，收到來路不明訊息多加留意、查證，切勿轉傳散播。詳情請上官網查詢 (http://at.cdc.tw/Q7S2Vt)。 圖片 附件\$\@\$20210612澄清.jpg</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-05-25\$\@\$中央流行疫情指揮中心今(25)日表示，近日網路出現偽冒教育部網站，杜撰「全國各級學校因應疫情停課時程資訊」等訊息，意圖造成民眾困惑，此為境外假網頁不實訊息，請民眾勿輕信。\$\@\$指揮中心副指揮官陳宗彥表示，該網站假冒教育部傳達不實防疫訊息，刑事警察局已成立專案小組偵辦，經調查其為境外IP。\$\@\$指揮中心指出，教育部全球資訊網正確的網址是https://www.edu.tw/ ，民眾收到任何連結時，可以先觀察連結網址，是否跟官方網址一樣。例如，教育部官方網址的網域，就會是「edu.tw」結尾。\$\@\$指揮中心強調，散播假訊息構成犯罪，會被判處最高三年有期徒刑或併科三百萬元罰金。提醒民眾，收到來路不明訊息多加留意、查證，切勿轉傳散播，以免觸法。 圖片 附件\$\@\$0525指揮中心指出，網路出現偽冒教育部網站並杜撰假訊息，請民眾勿輕信.jpg\$\@\$勿散播不實訊息，以免觸法受罰.jpg</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-06\$\@\$為提供結核病患即時診斷，疾病管制署結核病診治指引自104年已加重結核分枝桿菌核酸增幅(nucleic acid amplification, NAA)檢驗於診斷結核病之角色。NAA檢驗具快速、高敏感度及高特異性，可大幅縮短傳統培養檢驗方法所需等待結果時間，有利及早診斷及治療結核病。\$\@\$因應近期結核菌液態培養(MGIT)檢驗發生添加劑(營養劑併抑制細菌生長的抗生素成分)供貨短缺情形，為避免延遲發現疑似結核病個案，依本署110年12月24日「衛生福利部傳染病防治諮詢會(結核病防治組)」會議決議，於供貨短缺期間，對於社區型肺炎尚未通報結核病者，於診斷送驗3套初查痰執行塗片耐酸性染色鏡檢(Acid fast stain)及分枝桿菌培養時，其中1套請務必同時開立NAA檢驗。另考量實驗室短期內MGIT痰培養試劑有限，對於管理中的結核病患追蹤複查痰，請採1套進行培養檢驗，暫時避免重複送驗檢體，此因應作為停止施行時間將於缺貨狀況緩解後再函週知。\$\@\$有關「結核病診治指引」可至疾病管制署全球資訊網(https://www.cdc.gov.tw)&gt;傳染病與防疫專題&gt;傳染病介紹&gt;第三類定傳染病&gt;結核病&gt;重要指引及教材項下查閱。\$\@\$感謝您與我們共同維護全民的健康安全。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-12-24\$\@\$一、考評單位：衛生福利部疾病管制署。\$\@\$二、考評目的：客觀衡量地方政府衛生局111年防疫業務之施政績效。\$\@\$三、受評機關：地方政府衛生局。\$\@\$四、受評期間：111年1月至12月\$\@\$五、考評架構與權重：9項考評指標，共計200分。\$\@\$六、考評方式：\$\@\$(一)   防疫業務相關管理系統之統計結果及書面考核。\$\@\$本手冊考評指標資料，如須受評機關提供始得評分者，請於112年1月13日前備函逕送考評執行單位進行評核。\$\@\$考評單位於指定日期前完成分數統計及成績評定。\$\@\$考評單位完成考評並請地方政府衛生局確認後，於111年3月17日前將考評結果送衛生福利部綜合規劃司備查。\$\@\$(二)   考評單位得視需要辦理實地查核。 附件\$\@\$111年地方衛生機關業務考評作業手冊-防疫類.pdf\$\@\$111年地方衛生機關業務考評作業手冊-防疫類.docx</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-12-20\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$公共關係室\$\@\$約用公關助理\$\@\$(徵才案號：0708)\$\@\$(計5名)\$\@\$王○琴(F22546****)\$\@\$李○怡(A22422****)\$\@\$李○達(F12468****)\$\@\$鍾○婷(T22347****)\$\@\$廖○儀(T22036****)\$\@\$二、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一)口試：\$\@\$1、報到時間：110年12月30日星期四09:50~10:00，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署1樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：10:00~11:30。\$\@\$(二)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(三)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於110年12月29日下午5點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3823)，俾利安排應試座位。\$\@\$(四)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(五)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
+    <t>發佈日期：2022-01-05\$\@\$中央流行疫情指揮中心今(5)日公布國內新增3例COVID-19本土確定病例(尚未取號)，為擴大採檢清潔外包人員，於今日晚間檢驗陽性。\$\@\$指揮中心表示，3名個案均為女性，年齡分別為1例50多歲及2例60多歲，Ct值分別為33.8、23.4及19.5，為案17230、案17238、案17239及17266同職場工作人員，相關疫情調查、接觸者匡列及防治工作刻正進行中。\$\@\$指揮中心說明，因應桃園機場感染事件，指揮中心於第一時間針對外包清潔人員進行擴大採檢，已匡列861人，截至今日晚間，已有4例陽性（案17266及前述3例陽性）、855例陰性、1例檢驗中、1例待採檢。總計清潔外包人員已確診共7人（案17230、案17238-17239、17266、及前述3例）。\$\@\$指揮中心說明，因應今日晚間新增3位本土確診病例，前進指揮所立即啟動緊急作為如下：\$\@\$1. 針對清潔外包公司航廈夜班人員共93人，全數送集中檢疫所集中隔離。\$\@\$2. 該公司其餘未隔離員工，共768人，明後兩日（1月6日-1月7日）每日以家用快篩自我檢測，並彙整報告提供前進指揮所。1月8日將再度安排全員PCR檢驗。\$\@\$3. 已責成外包清潔公司嚴格確實執行員工健康監測，確保員工健康，以及早處理可能事件。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-05\$\@\$中央流行疫情指揮中心今(5)日公布國內新增26例COVID-19確定病例，分別為1例(案17266)本土及25例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，案17266為本國籍50多歲女性，已接種2劑莫德納疫苗(為突破性感染)，與案17230、案17238及案17239為同職場工作人員，曾與前述個案搭乘同路線交通車，原定於今(2022)年1月5日採檢，1月3日出現乾咳、喉嚨不適等症狀，1月4日自行前往採檢站採檢後於今日確診，相關疫情調查、接觸者匡列及防治工作刻正進行中。\$\@\$指揮中心表示，今日新增25例境外移入個案，為12例男性、13例女性，年齡介於未滿5歲至70多歲，分別自美國(12例，案17241-17243、案17245、案17250、案17252、案17254、案17256-17259、案17265)、法國(3例，案17244、案17246、案17253)、丹麥(案17247)、英國(17248)、玻利維亞(案17249)、德國(案17251)、史瓦帝尼王國(案17255)、澳洲(案17260)、巴拿馬(2例，案17261-17262)、瑞典(案17263)及印尼(案17264)入境，入境日介於去(2021)年11月14日至今(2022)年1月4日；詳如新聞稿附件。\$\@\$另1月2日公布之案17181境外移入病例經疫調後改判為本土病例，為案16941之相關感染。\$\@\$指揮中心統計，截至目前國內累計5,017,456例新型冠狀病毒肺炎相關通報(含4,998,328例排除)，其中17,155例確診，分別為2,493例境外移入，14,608例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月5日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-05\$\@\$疾管署今(5)日宣布，為提升疫苗接種人口涵蓋率，發揮疫苗最大效益，自2022年1月6日起，公費流感疫苗擴大提供全國6個月以上尚未接種之民眾接種，至疫苗用罄為止，疾管署呼籲尚未接種的計畫對象，尤其是65歲以上長者、學齡前幼兒及醫事人員等重點族群儘快接種，以保障自身及周遭人員的健康。\$\@\$疾管署表示，2021年度公費流感疫苗分2階段施打，除50至64歲無高風險慢性病成人於第二階段11月15日開打外，其於對象均為10月1日開打。截至2022年1月4日，公費疫苗總接種數約562萬劑，整體疫苗使用率逾91.9%，剩餘量約49萬劑；目前全國約有3,700餘家合約院所(含部分衛生所)提供接種服務，建議民眾可先透過各地方政府衛生局網頁、疾管署流感防治一網通(https://antiflu.cdc.gov.tw/)、疾管家或1922防疫諮詢專線，查詢鄰近合約院所名單，並向合約院所預約，以確保可施打到疫苗。\$\@\$另公費流感疫苗接種期間，COVID-19疫苗接種作業持續進行，依衛生福利部傳染病防治諮詢會預防接種組專家建議，2種疫苗接種間隔應至少7天，避免發生疫苗接種不良事件無法釐清。疾管署提醒民眾於預約或接種前主動告知疫苗接種史，合約院所應於接種區建立動線分流，並請相關工作人員於接種前落實檢核接種紀錄，接種後於健保卡黏貼流感疫苗接種貼紙。\$\@\$疾管署提醒，國內流感疫情仍處低點尚未進入流行期，民眾可儘速接種，以於流感疫情達高峰前獲得足夠保護力。近期氣溫偏低，為防範流感及COVID-19疫情雙重衝擊，民眾除接種疫苗，應養成良好衛生習慣，出現類流感症狀儘速戴口罩就醫，並在家休息，減少病毒傳播機會。如有流感疫苗或流感防治相關疑問，可至疾管署全球資訊網(https://www.cdc.gov.tw)，或撥打免付費防疫專線1922(或0800-001922)洽詢。</t>
   </si>
   <si>
     <t>發佈日期：2022-01-04\$\@\$中央流行疫情指揮中心今(4)日表示，為加速國人完成2劑接種，提升尚未接種第1、2劑COVID-19疫苗民眾之接種意願，各地方政府自2022年1月5日至1月31日前，可提供18歲以上民眾200元(含)以下衛教品，以鼓勵民眾踴躍完成接種2劑COVID-19疫苗，儘速獲得完整免疫保護力。\$\@\$指揮中心表示，截至2022年1月3日為止，我國COVID-19疫苗第一劑接種率約80%，第二劑接種率約69%，為因應國際疫情持續嚴峻及Omicron新型變異株之威脅增加，接種涵蓋率仍須再提升，目前COVID-19疫苗由地方政府衛生局指定/安排之合約醫療院所或衛生所進行接種，鼓勵尚未接種過任何1劑COVID-19疫苗及符合接種間隔但尚未完成2劑COVID-19疫苗接種之民眾，請儘速前往COVID-19疫苗合約醫療院所接種。\$\@\$指揮中心說明，目前國內各廠牌COVID-19疫苗供應充分，民眾可至衛生福利部疾病管制署全球資訊網，「COVID-19疫苗接種院所單元」（https://www.cdc.gov.tw/Category/List/u4l1b_gHhf9WDjhEtRmRRw），運用「COVID-19接種院所地圖」及各地方政府衛生局公告之COVID-19疫苗接種合約醫療院所以及車站等隨到隨打疫苗接種站，就近前往接種。\$\@\$指揮中心提醒， 18歲至未滿20歲民眾，如自行前往接種，請持家長簽具之意願同意書。若由家長陪同前往接種，請本人與家長於現場共同簽署意願同意書。另依衛生福利部傳染病防治諮詢會預防接種組(ACIP)建議，接種COVID-19疫苗應與流感疫苗等其他疫苗間隔至少7天，亦請民眾前往接種COVID-19疫苗前，應備妥健保卡或其他可證明身分之證件，如為接種第2劑COVID-19疫苗者亦請攜帶「COVID-19疫苗接種紀錄卡」，並於接種前評估時說明過往疫苗接種史，以利醫生評估。</t>
@@ -574,16 +829,22 @@
     <t>發佈日期：2022-01-03\$\@\$中央流行疫情指揮中心今(3)日公布國內新增25例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增25例境外移入個案，為9例男性、16例女性，年齡介於未滿5歲至70多歲，分別自美國(15例，案17182-17183、案17186-17191、案17196-17197、案17199、案17201-17203、案17205)、土耳其(4例，案17192-17195)、德國(案17184)、加拿大(案17185)、義大利(案17198)、菲律賓(案17200)、亞美尼亞(案17204)及千里達及托巴哥(案17206)入境，入境日介於去(2021)年12月19日至今(2022)年1月1日；詳如新聞稿附件。\$\@\$另去年12月28日及12月30日公布之2例(案17058、案17099)境外移入病例經疫調後改判為本土病例，為案17085之相關感染。\$\@\$指揮中心統計，截至目前國內累計4,982,263例新型冠狀病毒肺炎相關通報(含4,962,860例排除)，其中17,095例確診，分別為2,439例境外移入，14,602例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月3日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
+    <t>發佈日期：2022-01-02\$\@\$中央流行疫情指揮中心今(2)日公布國內新增20例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增20例境外移入個案，為10例男性、10例女性，年齡介於未滿5歲至60多歲，分別自美國(11例，案17162-17163、17165-17166、案17168、案17170、案17172、案17174-17175、案17179-17180)、加拿大(案17164)、澳大利亞(案17167)、英國(2例，案17169、案17177)、越南(案17171)、沙烏地阿拉伯(案17173)、泰國(案17176)、希臘(案17178)及中國(案17181)，入境日介於去(2021)年12月12日至12月31日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,972,057例新型冠狀病毒肺炎相關通報(含4,951,828例排除)，其中17,070例確診，分別為2,416例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月2日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
     <t>發佈日期：2022-01-01\$\@\$中央流行疫情指揮中心今(1)日公布國內新增21例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增21例境外移入個案，為15例男性、6例女性，年齡介於20多歲至70多歲，分別自美國(9例，案17141、案17148、案17149、案17151、案17154、案17156、案17159-17161)、越南(6例，案17142、案17145、案17147、案17150、案17152、案17153)、埃及(案17143)、寮國(案17144)、瓜地馬拉(案17146)、羅馬尼亞(案17155)、烏克蘭(案17157)及德國(案17158)入境，入境日介於去(2021)年12月17日至12月31日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,961,497例新型冠狀病毒肺炎相關通報(含4,942,271例排除)，其中17,050例確診，分別為2,396例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月1日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
     <t>發佈日期：2021-12-31\$\@\$中央流行疫情指揮中心今(31)日公布國內新增41例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增41例境外移入個案，為16例男性、25例女性，年齡介於20多歲至70多歲，分別自美國(14例，案17104-17106、案17112、案17113、案17115、案17116、案17118-17122、案17131、案17139)、菲律賓(2例，案17125、案17132)、法國(2例，案17117、案17124)、義大利(案17114)、肯亞(案17123)、喀麥隆(案17126)、瑞士(案17127)、印度(案17128)、阿拉伯聯合大公國(案17129)、烏克蘭(案17130)、越南(案17133)及柬埔寨(案17138)入境，另14例(案17100-17103、案17107-17111、案17134-17137、案17140)調查中，入境日介於今(2021)年12月16日至12月30日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,946,919例新型冠狀病毒肺炎相關通報(含4,927,473例排除)，其中17,029例確診，分別為2,375例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月31日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
+    <t>發佈日期：2021-12-31\$\@\$中央流行疫情指揮中心今(31)日表示，指揮中心均秉持防疫優先之原則進行各項防疫工作，有關中國大陸國台辦針對臺灣防疫之錯誤發言內容，相關澄清說明如下：\$\@\$一、鑒於兩岸往來頻繁，為掌握疫情狀況，向來致力與中國大陸保持資訊交流，我方自108年12月31日至110年12月28日，與中國大陸透過正式管道就 COVID-19 疫情往來資訊包括陸方提供我方疫情資訊286次，我方提供陸方包括個案大陸旅遊史等資訊共50次。另我方洽詢陸方疫情訊息計85次，陸方回覆我方疫情資訊21次，而陸方洽詢我方疫情訊息29次，我方回覆陸方疫情資訊28次。陸方電話洽我方聯絡疫情資訊7次，我方電話洽陸方聯絡疫情資訊8次。此外，陸方提供我方技術文件共計12次。相關數據都有文件紀錄可查數，國台辦提供數據有與事實不符之處。\$\@\$二、為與國際分享、交換衛生、防疫經驗，我國均積極爭取參與世界衛生組織相關會議，自2009年至2021年，共向WHO申請參加220場技術性會議，但僅77場獲邀出席。\$\@\$三、為守護國人健康，我國政府一直多方洽談COVID-19疫苗購買，在BioNTech疫苗取得上，為尊重BioNTech原廠疫苗商業代理權劃分，BioNTech 疫苗係由台積電、鴻海／永齡基金會、慈濟基金會三捐贈方委託裕利醫藥公司，向原廠代理商復星實業公司（香港復星）有償購買，在基於「原廠製造、原廠標籤、直送臺灣」三原則的共識，全部無償捐贈政府統籌運用，對於捐贈單位出錢、出力，無私付出，不應被扭曲抹殺。\$\@\$指揮中心強調，疫情尚未止息，人民健康福祉為先。兩岸應互助合作，防疫優先，才能維護兩岸民眾健康。</t>
+  </si>
+  <si>
     <t>發佈日期：2021-12-30\$\@\$衛生福利部疾病管制署今（30）日公布「受聘僱外國人健康檢查管理辦法」部分條文修正案，並預訂於111年1月1日實施。本次修法重點包括「修正移工申請結核病都治條件」及「防疫期間調整移工健檢期限之法源依據」等事項，確保社區防疫安全。\$\@\$疾管署說明，結核病為結核桿菌感染所造成的慢性傳染病，目前抗結核藥物效果良好，連續服藥14天後的傳染力可大幅下降；透過移工主動配合、雇主支持，再加上結核病都治關懷員等衛生單位人員持續關心移工確實規則服藥，幾乎可以痊癒，且治療期間亦可正常工作與生活作息；此外，罹患結核病之移工若於國內完成治療，除能避免疾病持續傳播，維護員工健康外，亦不影響雇主勞動力需求。本辦法修正後，移工確診為肺結核、結核性肋膜炎（多重抗藥性結核病個案除外）或漢生病，且本人同意留臺配合按規治療者，雇主應於收受診斷證明書之次日起15日內，檢具「診斷證明書」及「受聘僱外國人接受衛生單位安排都治服務同意書」送縣市政府衛生局申請都治服務，共同落實社區防疫。\$\@\$疾管署指出，本辦法另增訂「中央流行疫情指揮中心成立期間，中央衛生主管機關得依國內疫情防治所需，調整移工健檢期限」及「自聘僱許可生效日起滿6、18及30個月之日與最近一次健檢日間隔未滿3個月者，免辦該次定期健檢」等規定；且回溯至自110年5月19日施行，以避免部分移工需於短期間內重複健檢，並能兼顧防疫安全。\$\@\$為利雇主（仲介）能瞭解本辦法修正後實務作業，疾病管制署提供「移工罹患結核病申請留臺治療」宣導海報、「認識結核病的問與答」多國語言宣導單張及宣導影片等相關衛教素材，並建置於該署全球資訊網（http://www.cdc.gov.tw ； 首頁&gt;國際旅遊與健康&gt;外國人健康管理&gt;受聘僱外國人健檢&gt;最新消息）供下載瀏覽。</t>
   </si>
   <si>
-    <t>發佈日期：2021-12-30\$\@\$中央流行疫情指揮中心今（30）日表示，由於國際疫情嚴峻及Omicron新型變異株之威脅日益擴散，近期入境人數及COVID-19境外移入個案增加，為強化社區監測，自明(2022)年1月1日起擴大辦理COVID-19社區加強監測方案，全國由86家定點診所發放公費COVID-19家用快篩試劑增加至272家，由各縣市人口數較多之鄉鎮市區基層診所協助發放試劑，因COVID-19症狀與一般感冒相似，提醒民眾如有出現呼吸道症狀，可多加前往該等診所，由醫師評估發放試劑後自行檢驗。\$\@\$指揮中心說明，今(2021)年8月30日起規劃推動COVID-19社區加強監測方案，迄今已發放1萬餘劑公費COVID-19家用快篩試劑，考量近期COVID-19社區傳播風險提升，為提高民眾取得公費家用快篩試劑可近性與及早發現自身感染之可能，將自明年1月1日起於全國21個縣市增加至272個診所試劑發放點，診所名單詳如新聞稿附件。\$\@\$指揮中心呼籲，現值呼吸道病毒活躍期，請民眾多加留意自身健康，如出現呼吸道症狀，可前往本計畫定點診所；民眾如為2歲以上出現呼吸道症狀的病患至公費快篩試劑發放診所掛號就醫，經醫師評估後發放試劑及注意事項說明單張，如為2歲以下幼兒的陪同看診者，亦由醫師評估後發放。民眾領取試劑後，請配合依注意事項說明內容儘速採檢，並至線上(https://forms.gle/8gh7Kb3ZkYE5aArW7)填寫試劑領取診所名稱及快篩結果等資料，此為匿名方式收集，無須擔心個人資料外洩情形。\$\@\$指揮中心提醒，如居家快篩檢驗為陽性時，請勿慌張並儘速至鄰近的社區採檢院所( https://reurl.cc/MArG1L )進一步PCR檢驗。民眾前往社區採檢院所時，請戴好口罩、勿搭乘大眾運輸工具，對於使用過之採檢器材請用塑膠袋密封包好，並攜帶至社區採檢院所，交予院所人員處理。 附件\$\@\$附件-配合辦理發放公費COVID-19家用快篩試劑社區定點診所名單.pdf</t>
+    <t>發佈日期：2021-12-30\$\@\$中央流行疫情指揮中心今(30)日公布國內新增24例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增24例境外移入個案，為11例男性、13例女性，年齡介於10多歲至60多歲，分別自美國(12例，案17076、案17078-17080、案17082-17083、案17085、案17088、案17090、案17094、案17096)、越南(2例，案17077、案17098)、英國(案17081)、尼加拉瓜(案17084)、奈及利亞(案17086)、加拿大(案17087)、阿拉伯聯合大公國(案17089)、法國(3例，17091-17093)、泰國(案17095)、海地(案17097)及日本(案17099)入境，入境日介於今(2021)年12月14日至12月28日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,932,261例新型冠狀病毒肺炎相關通報(含4,912,670例排除)，其中16,988例確診，分別為2,334例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月30日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
     <t>發佈日期：2021-12-30\$\@\$中央流行疫情指揮中心今(30)日表示，台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的第十五批BNT疫苗93.83萬劑，已於今日上午順利運抵桃園國際機場，並在完成通關程序後，直接運送至指定冷儲物流中心進行後續檢驗封緘作業。\$\@\$指揮中心說明，由台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的BNT疫苗1,500萬劑，目前共計到貨1333.62萬劑，分別為首批9月2日93萬劑、第二批9月9日91萬劑、第三批9月30日54萬劑、第四批10月1日67萬劑、第五批10月4日27萬劑、第六批10月7日88.92萬劑、第七批10月8日88.92萬劑、第八批10月14日82.7萬劑、第九批10月28日90.21萬劑、第十批10月29日91.03萬劑、第十一批11月5日87.17萬劑、第十二批11月12日92.66萬劑、第十三批11月25日93.83萬劑、第十四批12月9日192.35萬劑，以及本批93.83萬劑。本批疫苗效期至2022年3月28日，將由指揮中心統籌運用，儘速提供民眾接種。\$\@\$對於台積電、鴻海暨永齡基金會、慈濟基金會三間企業和民間團體積極協助，提供更多的疫苗讓民眾接種，加速提升臺灣疫苗覆蓋率，指揮中心再次表達由衷的謝意。</t>
@@ -595,31 +856,193 @@
     <t>發佈日期：2021-12-28\$\@\$中央流行疫情指揮中心今(28)日公布國內新增19例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增19例境外移入個案，為9例男性、10例女性，年齡介於未滿10歲至80多歲，分別自美國(8例，案17043、案17045-17049、案17051、案17056)、瑞士(案17044)、寮國(案17050)、越南(案17052)、柬埔寨(案17053)、加拿大(2例，案17054、案17061)、哈薩克(案17055)、香港(案17057)、中國(案17058)及阿根廷(2例，案17059、案17060)入境，入境日介於今(2021)年12月14日至12月26日；詳如新聞稿附件。\$\@\$指揮中心統計，累計4,901,375例新型冠狀病毒肺炎相關通報(含4,882,616例排除)，其中16,950例確診，分別為2,296例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月28日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
+    <t>發佈日期：2021-12-27\$\@\$中央流行疫情指揮中心今(27)日表示，歐盟執委會於今(110)年12月21日宣布我國正式加入「歐盟數位新冠證明」系統。歐盟數位新冠證明為世界性標準之一，國際成員國多且最早用於國際旅行，為使我國民眾能加速入境歐盟等國家，指揮中心將於12月28日上午8時開放我國「數位新冠病毒健康證明」供國人下載使用。\$\@\$指揮中心說明，由於歐盟為世界重要國際聯盟，「歐盟數位新冠證明」系統目前已有60國加入，包括27個歐盟會員國、33個非歐盟會員國(統計至2021/12/22止)。另，美國已公開接受旅客持歐盟數位新冠證明供入境查驗，國際航空運輸協會(IATA)之數位新冠證明亦與之互通，故持我國數位證明於國際旅行己不限上述的60國。\$\@\$指揮中心指出，我國「疫苗接種數位證明」或「檢驗結果數位證明」之資料欄位、數位簽章、防偽機制、個人資料保護、QR Code顯示與電子驗證等均依照歐盟標準，尤其是個人資料保護完全依據歐盟一般資料保護規則之最小使用、自行攜帶、可被遺忘等原則，請國人安心使用。\$\@\$指揮中心表示，本項數位證明的內容屬於個人資料保護法定義的敏感性資料，身分確認的方式相對繁瑣。本數位證明提供所有於國內接種疫苗或進行PCR檢驗者自行下載，初期限持有有效護照者，申請方式以電腦或手機直接上網辦理，網址為：https://dvc.mohw.gov.tw（將於12月28日上午8時開放），或在衛福部官網取得連結，三個步驟即可取得證明：\$\@\$一、確認身分：\$\@\$(一)國人：(1)身分證號+健保卡號+有效護照號碼；(2) FIDO(為安全且便利的生物辨識方式，提供指紋或臉部辨識登入)+有效護照號碼；(3)自然人憑證+有效護照號碼。三種方式擇一。\$\@\$(二)外來人口：(1)統一證號+健保卡號；(2) 統一證號+入出境證號；(3) 統一證號+護照號碼。三種方式擇一。\$\@\$二、選擇項目：選擇「疫苗接種數位證明」或「檢驗結果數位證明」。\$\@\$三、取得證明：於申請成功畫面點選「下載/列印 數位證明」，檔案格式為PDF，提醒要先保存於行動裝置或電腦硬碟中，再視個人需要列印紙本。無列印設備但又有列印需求者，可於申請成功畫面選擇超商並點選「取得超商列印碼」，系統將產製超商取件條碼或取件編號，請自行攜至超商付費列印。\$\@\$指揮中心提醒，實際使用時，出示紙本或行動載具中的QR code都是可接受的方法，查驗人員掃瞄QR code後會出現不同顏色的號誌表達接受與否。但各國或不同場所仍可能有不同方式驗證，請民眾特別提醒留意。本數位證明優先提供民眾出國使用，至於國內何時開放使用，再由疫情指揮中心另行發布。詳細系統操作方式可以參考衛生福利部官網數位證明專區( https://covid19.mohw.gov.tw/ch/np-5345-205.html )。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-27\$\@\$中央流行疫情指揮中心今(27)日表示，因應近期COVID-19全球疫情升溫，Omicron等新興變異株於全球迅速擴散，上週(12/20-12/26)境外移入病例數新增109例，較前一次(12/13-12/19)新增62例，上升76%，且Omicron變異株增加迅速，截至今日已累計34例，感染國家以美國及英國較多，加以我國已檢出多起境外移入病例為突破性感染，經評估國際間採認之入境前檢驗報告多以採檢日計算，故為確保航空防疫安全，自2022年1月4日零時起(啟程日)，旅客搭機前應檢附之COVID-19核酸檢驗報告調整為「2日內」報告，報告起計日由原「報告日」改以「採檢日」為基準，並以啟程地表定航班時間（不含搭機當日）往前推2個「日曆日」計算，請旅客搭機前務必確認PCR檢驗報告符合以上規範。\$\@\$指揮中心說明，旅客所持「2日內COVID-19核酸檢驗報告」請符合下列規範：\$\@\$1. 以英文、中文或中英對照版本為原則。\$\@\$2. 該報告可為紙本(正本/影本)或電子報告書形式。\$\@\$3. 需採分子生物學核酸檢測，且應可審核登機者之護照姓名、出生年月日(或護照號碼)、疾病名稱、採檢日及報告日、核酸檢驗方法（包括PCR、Real-Time PCR及RT-PCR等）及判讀結果等。\$\@\$4. 血清免疫學檢驗抗原或抗體，非屬核酸檢測，未符合本措施規範之條件。\$\@\$對於違反前述規定之旅客，抵臺時將依傳染病防治法第58條、第69條規定及衛生福利部公告裁罰基準，處新臺幣一萬元至十五萬元罰鍰。\$\@\$指揮中心強調，適逢春節前返鄉人潮，請旅客返臺必須事先瞭解並配合我國現行入境檢疫規定，及在臺檢疫期間應遵守之防疫措施，共同維護國內社區安全。</t>
+  </si>
+  <si>
     <t>發佈日期：2021-12-27\$\@\$中央流行疫情指揮中心今(27)日表示，近期考量國內整體疫情趨緩及配合疫苗接種政策，為兼顧國內產業用人需求及移工工作權益，因此適度鬆綁管制措施，自110年12月27日起，移工轉換新雇主及同一雇主調派移工變更工作地點，如移工已完整接種COVID-19疫苗，無須再事前安排移工檢驗PCR，但雇主及移工仍應落實指揮中心及勞動部規定的相關防疫措施。\$\@\$指揮中心表示，鼓勵在臺移工接種疫苗，以提升疫苗覆蓋率，降低群聚感染可能性。另取消PCR相關規定後，雇主仍應依規定落實強化宿舍管理、分艙分流、健康監測等其他防疫規定，若未落實防疫，仍將依就業服務法相關規定，處新臺幣6萬至30萬元罰鍰及不予核發接續聘僱許可。另雇主如委託仲介公司辦理移工生活照顧，因仲介公司未善盡受任事務，違反防疫措施，將依仲介公司違反就業服務法規定，處新臺幣6萬元以上至30萬元以下罰鍰。</t>
   </si>
   <si>
+    <t>發佈日期：2021-12-27\$\@\$中央流行疫情指揮中心今(27)日表示，鑒於國際疫情持續嚴峻及Omicron新型變異株之威脅增加，並考量住院陪病特殊需求，已於12月24日發函周知全國醫療院所，調整醫院門禁管制及強化住院病人之陪病者COVID-19疫苗接種規範，相關調整說明如下：\$\@\$1. 陪病人數：\$\@\$(1) 每名住院病人之陪病人數維持以1人為原則。\$\@\$(2) 若病人為兒童(12歲以下)、老人(65歲以上)、身心障礙、或經醫療機構評估有必要者等特殊情形，陪病人數上限得為2人，惟每名住院病人之陪病者公費篩檢仍為1名。\$\@\$2. 篩檢規定：\$\@\$(1) 完成疫苗應接種劑次達14天(含)以上之陪病者，得免除入院篩檢及每週定期篩檢。\$\@\$(2) 未完成疫苗應接種劑次達14天(含)以上之陪病者，自明(111)年1月1日起，入院進行公費篩檢(每名住院病人之陪病者限1名公費)，且每週定期進行自費篩檢；自明年2月1日起，入院篩檢改為自費篩檢，且每週定期進行自費篩檢。\$\@\$3. 篩檢方式：\$\@\$(1) 公費篩檢方式為抗原快篩或PCR核酸檢驗二者擇一，或同時執行；自費篩檢方式為抗原快篩(含家用快篩)或PCR核酸檢驗。\$\@\$(2) 若為「確定病例符合檢驗解除隔離條件且距發病日3個月內」，得免除前述篩檢。\$\@\$指揮中心提醒，由於醫院屬於高感染傳播風險場域，為降低疾病在院內傳播風險，籲請民眾儘速完成完整疫苗接種。於疫情期間儘量避免不必要的陪病或探病，建議以視訊或電話方式替代實地探視，若仍有陪病或探病需要，應配合實名登記及院方相關管理措施。陪(探)病人員須不具COVID-19相關症狀，亦未曾接觸確診個案或具相關公共場所活動史；且進入醫療機構務必全程佩戴口罩、遵循呼吸道衛生與咳嗽禮節、落實手部衛生，以降低交互感染風險，保障自身及病人安全。</t>
+  </si>
+  <si>
     <t>發佈日期：2021-12-27\$\@\$中央流行疫情指揮中心今(27)日公布國內新增16例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增16例境外移入個案，為12例男性、4例女性，年齡介於10多歲至60多歲，分別自美國(8例，案17027-案17028、案17031、案17033-案17037)、越南(案17029)、匈牙利(案17030)、哈薩克(案17032)、菲律賓(案17038)、寮國(案17039)、英國(案17040)、德國(案17041)及印尼(案17042)入境，入境日介於今(2021)年12月12日至12月26日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,884,004例新型冠狀病毒肺炎相關通報(含4,864,380例排除)，其中16,931例確診，分別為2,277例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月27日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-07\$\@\$中央流行疫情指揮中心今(7)日公布國內新增62例COVID-19確定病例，分別為4例本土個案(案17368-17371)及58例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，本土個案(案17368-17371)分別為本國籍1例男性、3例女性，年齡介於20至50多歲，均為桃園機場感染事件相關個案；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增58例境外移入個案，為29例男性、29例女性，年齡介於10多歲至70多歲，分別自美國(35例)、法國(4例)、英國(3例)、瑞士、越南及印度(各2例)、奧地利、智利、德國、加拿大、愛爾蘭、孟加拉、奈及利亞、墨西哥、西班牙及哥斯大黎加(各1例)入境，入境日介於去(2021)年12月22日至今(2022)年1月6日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,055,274例新型冠狀病毒肺炎相關通報(含5,035,769例排除)，其中17,258例確診，分別為2,588例境外移入，14,616例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另新增2例空號病例(案17271，案17272與舊案重複，改列空號)，累計113例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月7日新增本土COVID-19確診個案表.pdf\$\@\$1月7日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-06\$\@\$中央流行疫情指揮中心今(6)日表示，考量目前國際COVID-19疫情嚴峻，請長者及其他 COVID-19感染後容易產生嚴重併發症之族群，儘速完成COVID-19疫苗基礎劑接種，提升保護力。\$\@\$指揮中心表示，目前我國75歲以上長者第1劑接種率僅約73%，第2劑接種率僅約67%，仍需再積極提升，為維護長者及風險族群健康，降低因感染COVID-19造成之重症、住院或死亡風險，家中長輩如尚未接種COVID-19疫苗第1、2劑，請於其身體狀況較穩定時，協助陪同至各地方政府衛生局安排或指定之合約醫療院所接種。\$\@\$指揮中心說明，疫苗接種後可能發生副作用，通常輕微並於數天內消失，並隨年齡層增加而減少，若擔心接種疫苗後所產生之副作用，可先與醫師討論，經諮詢評估選擇合適的疫苗接種。\$\@\$指揮中心表示，若為行動不便者，各地方政府衛生局亦設有到宅接種服務，有需求者可向各地方政府衛生局洽詢。另為鼓勵18歲以上尚未接種第1劑、第2劑COVID-19疫苗接種者儘速踴躍前往接種，於2022年1月5日至1月31日前接種COVID-19疫苗者，可獲得地方政府發放之200元(含)以下衛教品，鼓勵民眾儘速接種，獲得保護力。\$\@\$指揮中心提醒，依我國衛生福利部傳染病防治諮詢會預防接種組(ACIP)建議，接種COVID-19疫苗應與流感疫苗等其他疫苗間隔至少7天，亦請民眾前往接種COVID-19疫苗前，應備妥健保卡或其他可證明身分之證件，如為接種第2劑COVID-19疫苗者，請記得攜帶「COVID-19疫苗接種紀錄卡」，並於接種前評估時，說明過往疫苗接種史，以利醫生評估。另近期天氣多變，對於近期身體具狀況或慢性病情不穩定者，請於身體狀況較穩定後就近前往接種。接種後亦請多加留意身體狀況，多喝水多休息，亦請家人協助注意，如有持續發燒超過48小時、嚴重過敏反應如呼吸困難、氣喘、眩暈、心跳加速、全身紅疹等不適症狀，應儘速就醫釐清病因。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-06-01\$\@\$中央流行疫情指揮中心今(1)日指出，近日有網友在通訊軟體LINE散布「臺中市太原路復健醫院被徵收為方艙醫院」，臺中市政府衛生局已澄清為不實訊息，請民眾勿再轉傳與散布，以免觸法遭罰。\$\@\$指揮中心表示，臺中市政府已對外澄清，此復健醫院近期進行搬遷作業，是為了提升醫療品質，正以BOT方式規劃市立綜合醫院，並非徵用作為方艙醫院。\$\@\$指揮中心副指揮官陳宗彥指出，因應疫情變化，各地方政府規劃應變醫院及專責醫院收治患者，民眾接獲來源不明的訊息時，應先進行查證，切勿隨意散播、轉傳，以免觸法。\$\@\$指揮中心重申，防疫相關資訊應以中央流行疫情指揮中心公布內容為主，散播假訊息構成犯罪，會被判處最高三年有期徒刑或併科三百萬元罰金。提醒民眾，收到來路不明訊息多加留意、查證，切勿轉傳散播，以免觸法。詳情請上官網查詢(http://at.cdc.tw/Q7S2Vt)。 圖片 附件\$\@\$網傳「臺中市太原路復健醫院被徵收為方艙醫院」為不實訊息勿轉傳.jpg\$\@\$勿散播不實訊息，以免觸法受罰.jpg</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-05-28\$\@\$近期國內疫情升溫，警方發現網路上有不肖人士販售「新冠病毒快篩試劑」，中央流行疫情指揮中心副指揮官陳宗彥今(28)日表示，擅自在網路販售新冠病毒檢驗試劑等第三級醫療器材已違反「醫療器材管理法」，目前警方已進行偵辦，提醒民眾切勿購買檢測，除有效性及檢測結果正確性均無法確認外，還可能危害自身健康。\$\@\$指揮中心指出，新冠病毒檢驗試劑是第三級醫療器材，依據「醫療器材管理法」規定，只有醫療器材商及藥局可以販賣，且國內並未開放可使用通訊方式在網路、電話、社群媒體等販售。\$\@\$指揮中心強調，不肖人士在網路擅自販售專案核准的新冠病毒檢驗試劑已違「醫療器材管理法」，會被罰3萬以上100萬以下罰鍰，如果民眾發現有類似狀況，可打1919專線或是向地方衛生局檢舉。 圖片 附件\$\@\$0528網路販售「新冠病毒快篩試劑」已觸法，警方偵辦中.jpg\$\@\$勿散播不實訊息，以免觸法受罰.jpg</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-09-28\$\@\$各位醫界朋友，您好：\$\@\$我國現行潛伏結核感染(LTBI)檢驗方式依受檢者年齡區分，未滿5歲以皮膚結核菌素試驗(TST)，5歲(含)以上抽血執行丙型干擾素釋放試驗(IGRA)。經參考世界衛生組織(WHO)、美國兒科醫學會(AAP)及國內臨床兒科醫師建議，並考量國際間已有相關研究指出IGRA可適用於2歲以上兒童，爰自本(110)年10月1日起擴大IGRA適用對象至2歲(含)以上兒童。\$\@\$IGRA檢驗方式較TST可減少兒童接種卡介苗造成的偽陽性結果，避免因環境非結核分枝桿菌(NTM)或卡介苗造成的TST增強效應(booster effect)，提升檢驗準確性，及早給予治療。倘2歲(含)至未滿5歲兒童無法執行IGRA檢驗，得維持使用TST方式。另，考量2歲以下因缺乏相關實證資料故暫不建議使用IGRA檢驗，仍維持TST方式檢測。\$\@\$此外，考量未滿5歲之結核病接觸者發病風險高，應於指標個案確診後儘速完成胸部X光攝影及LTBI檢驗，其中陽性者排除活動性結核病後應提供LTBI治療；陰性者可能處於LTBI空窗期，請LTBI合作醫師先提供預防性治療(prophylaxis)，俟接觸者與指標個案終止有效暴露滿8週後之LTBI檢驗結果，再決定是否停止預防性治療或完成LTBI治療，以降低發病風險。有關LTBI檢驗與治療資訊，請參考疾病管制署全球資訊網(https://www.cdc.gov.tw)&gt;傳染病與防疫專題&gt;傳染病介紹&gt;第三類法定傳染病&gt;結核病&gt;治療照護&gt;潛伏結核感染專區。\$\@\$感謝您與我們共同守護民眾的健康。 附件\$\@\$附件1-110年IGRA檢驗適用對象擴大至2歲以上兒童問答集.pdf\$\@\$附件2-未滿5歲結核病接觸者LTBI檢驗流程建議.pdf\$\@\$附件3-結核病接觸者就醫轉介單更新版.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-12-24\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$慢性傳染病組\$\@\$約用助理\$\@\$(徵才案號：0309)\$\@\$(計3名)\$\@\$林○萱(B22260****)\$\@\$陳○瑜(Q22389****)\$\@\$陳○君(F22674****)\$\@\$二、實作、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一)實作：\$\@\$1、報到時間：111年1月7日星期五13:20。\$\@\$2、報到地點：衛生福利部疾病管制署1樓(臺北市中正區林森南路6號)。\$\@\$3、實作時間：13:40~15:10。實作開始鈴響(13:40)未到者，喪失應考資格。\$\@\$(二)口試：\$\@\$1、報到時間：111年1月7日星期五15:20，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署1樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：15:30~16:30。\$\@\$(三)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(四)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於111年1月6日下午5點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3823)，俾利安排應試座位。\$\@\$(五)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(六)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。\$\@\$三、試場規則：\$\@\$(一)第一試為實作測驗，題型為資料串接統計分析，應試者得自行攜帶筆記型電腦，並預先安裝欲於測驗時使用的統計分析軟體(可選擇使用SAS、R、Excel等其他統計分析軟體)；未自行攜帶筆記型電腦者，則由本署提供公務電腦於測驗時使用(僅具Excel功能且無法安裝軟體)。\$\@\$(二)測驗中途不容許離場，並於考試時間過半後始得離場，離場後不得再進入試場。\$\@\$(三)測驗期間不允許上網、隨身攜帶手機(含智慧手環)、行動網卡、無線網路分享器等電子用品，並請關閉網路、手機、聲音及振動(含鬧鐘)，考試過程中如有上網、發出聲音及震動，均喪失應考資格。\$\@\$(四)個人用品(如書包等)置於考場前後，桌面上僅可放置必要文具(墊板須為透明；水杯、飲料亦禁止放置)。\$\@\$(五)有下列各款情事之一者，予以扣考並不予計分或不得繼續應考：\$\@\$1、冒名頂替。\$\@\$2、持用偽造或變造之證件。\$\@\$3、互換座位或試卷。\$\@\$4、傳遞文稿、參考資料、書寫有關文字之物件或有關信號。\$\@\$5、夾帶書籍文件。\$\@\$6、故意不繳交試卷或破壞試卷彌封。\$\@\$7、在桌椅、文具或肢體上或其他處所，書寫有關文字。\$\@\$8、電子通訊舞弊行為。\$\@\$9、窺視他人試卷、答案卷、作答結果或互相交談。\$\@\$10、在答案卷上書寫姓名、座號或其他不應有之文字、標記或自備稿紙書寫。\$\@\$11、其他破壞試場秩序事項。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-11-15\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$檢驗及疫苗研製中心\$\@\$約用助理\$\@\$(徵才案號：1057)\$\@\$(計3名)\$\@\$張○睿(I10045****)\$\@\$方○媃(Q22405****)\$\@\$洪○貞(E22306****)\$\@\$檢驗及疫苗研製中心\$\@\$約用研究助理\$\@\$(徵才案號：1058)\$\@\$(計4名)\$\@\$蘇○瑜(A22867****)\$\@\$李○志(P12320****)\$\@\$陳○均(F23000****)\$\@\$陳○君(C22130****)\$\@\$二、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一)口試：\$\@\$1、報到時間：110年11月25日星期四08:50~09:00，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署7樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：09:00~11:00。\$\@\$(二)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(三)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於110年11月24日下午3點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3823)，俾利安排應試座位。\$\@\$(四)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(五)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
+    <t>發佈日期：2021-12-27\$\@\$因應國際間新變異株Omicron威脅，中央流行疫情指揮中心與相關單位溝通及評估後於今(27)日宣布，今(2021)年12月28日至明(2022)年1月10日維持疫情警戒標準為第二級，並維持相關措施及規定如下：\$\@\$一、維持現行戴口罩規定，外出時應全程佩戴口罩，但符合以下情形，得免戴口罩(本次未調整)：\$\@\$(一)下列場合得免戴口罩，但應隨身攜帶口罩，且如本身有相關症狀或與不特定對象無法保持社交距離時，仍應戴口罩：\$\@\$1.於室內外從事運動、唱歌時。\$\@\$2.於室內外拍攝個人/團體照時。\$\@\$3.單人或多人進行直播、錄影、主持、報導、致詞、演講、講課等談話性質工作或活動之正式拍攝或進行時。\$\@\$4.農林漁牧工作者於空曠處(如：田間、魚塭、山林)工作。\$\@\$5.於山林(含森林遊樂區)、海濱活動。\$\@\$6.於溫/冷泉、烤箱、水療設施、三溫暖、蒸氣室、水域活動等易使口罩潮濕之場合。\$\@\$(二)外出時有飲食需求，得免戴口罩。\$\@\$(三)於指揮中心或主管機關指定之場所或活動，如符合相關防疫措施，得暫時脫下口罩。\$\@\$二、營業場所及公共場域維持應遵守實聯制、量體溫、加強環境清消、員工健康管理、確診事件即時應變。\$\@\$指揮中心強調，歲末年終將近，請民眾配合歲末/跨年大型活動防疫準備注意事項：\$\@\$一、主辦單位應遵守指揮中心二級警戒公告措施、地方政府大型活動相關防疫規定：\$\@\$(一)主辦單位應於活動場域提供足量手部清消用品、提高公共廁所之消毒頻率並設有醫療應變措施。\$\@\$(二)除指定販賣區外，場內不得販售飲食。\$\@\$(三)室內活動不得販售無座位票，須落實實聯制，規劃固定入口，且於入口處進行體溫量測及手部消毒。\$\@\$二、活動期間應全程佩戴口罩，除補充水分外，禁止飲食。\$\@\$(一)除主持、表演及致詞人員得於正式拍攝或進行時免戴口罩，其餘人員及參加活動者不適用飲食(補充水分除外)、拍照等得免戴口罩之例外情形。\$\@\$(二)主辦單位經地方政府同意，得設置專屬飲食區域供民眾脫口罩飲食，該區域須落實實聯制、入口體溫量測及手部消毒，並不得邊走邊吃，亦不開放試吃。\$\@\$(三)違反以上規定、經工作人員勸導不聽者，由地方政府依傳染病防治法裁罰。\$\@\$三、居家檢疫、居家隔離、(加強)自主健康管理者，及有發燒、呼吸道症狀、腹瀉、嗅味覺異常等疑似症狀之民眾(包括表演者及活動工作人員)，不得參加相關活動。違反者將從重處罰。\$\@\$指揮中心將視國內外疫情及實際執行狀況，適時機動調整防疫措施，強化邊境監測及防疫作為。籲請民眾應落實個人防護措施，主動積極配合各項防疫規範，以兼顧防疫與生活品質。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-26\$\@\$中央流行疫情指揮中心今(26)日公布國內新增24例COVID-19確定病例，分別為1例本土及23例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增1例本土病例(案17026)，為30多歲本國籍男性，未接種過COVID-19疫苗，今(2021)年12月25日因有陪病需求至醫院採檢，於今日確診( Ct值34.1，二採PCR檢驗陰性)，血清檢驗IgM陰性，IgG陽性，研判為非近期感染。目前已匡列接觸者14人，3人列居家隔離，6人列自主健康管理，5人列自我健康監測，其餘接觸者匡列中。衛生單位刻正進行疫情調查及防治工作，以釐清感染源。\$\@\$指揮中心表示，今日新增23例境外移入個案，為13例男性、10例女性，年齡介於10多歲至70多歲，分別自美國(10例，案17003-17009、案17022-17023、案17025)、哈薩克(11例，案17010-17019、案17024)、喀麥隆(案17020)及南非(案17021)，入境日介於今(2021)年12月19日至12月24日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,873,578例新型冠狀病毒肺炎相關通報(含4,853,506例排除)，其中16,915例確診，分別為2,261例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月26日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-25\$\@\$中央流行疫情指揮中心今(25)日公布國內新增18例COVID-19移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增18例境外移入個案，為15例男性、3例女性，年齡介於10多歲至60多歲，分別自美國(6例，案16985、案16990-16992、案17000、案17001)、越南(6例，案16986-16988、案16996、案16997、案16999)、柬埔寨(案16989)、法國(案16993)、巴基斯坦(案16994)、義大利(案16995)、阿拉伯聯合大公國(案16998)及荷蘭(案17002)，入境日介於今(2021)年12月10日至12月23日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,860,998例新型冠狀病毒肺炎相關通報(含4,841,748例排除)，其中16,891例確診，分別為2,238例境外移入，14,599例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月25日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-25\$\@\$為感謝2021年我國COVID-19本土疫情期間，眾多醫護防疫人員、醫療院所、專業學協會與防疫旅館，不畏辛勞、挺身抗疫，幫助國家快速彌平疫情、恢復民生經濟，中央流行疫情指揮中心今（25）日於衛生福利部大禮堂舉行 COVID-19「關鍵『疫』戰，感謝有您」頒獎典禮，向疫情期間貢獻卓越的第一線防疫英雄致謝，同時發表紀錄我國抗疫重症照護關鍵的「COVID-19重症照護關鍵紀實」專書。\$\@\$本次頒獎典禮由指揮中心指揮官陳時中親自頒發獎項，共計頒發79座獎座予疫情期間防疫有功之單位，包含COVID-19本土疫情期間 （本年5月12日至7月14日）收治確診者超過1,000住院人日之醫院（平均每日照顧16位確診者）、收住高感染風險族群的加強型防疫旅館、派駐前往防疫旅館提供專業醫療的主責醫院、加強版集中檢疫所主責醫院，以及提供專業諮詢之相關專業公學協會；陳指揮官同時頒發感謝狀予134位貢獻良多的防疫專家，包含傳染病防治醫療網指揮官、緊急醫療網執行長、中央流行疫情指揮中心專家諮詢小組、COVID-19重症個案臨床處置專家諮詢小組暨研討會專家、COVID-19感染管制與防治策略研討會專家，以及COVID-19疫苗與心血管疾病臨床處置研討會專家。\$\@\$指揮中心指出，我國於本年5月發生COVID-19本土疫情，重症與死亡個案增加，為加強公共衛生及醫療從業人員針對COVID-19重症個案之照護能力及品質，指揮中心緊急成立「COVID-19重症個案臨床處置專家諮詢小組」，邀請臺大醫院新竹分院余忠仁院長擔任召集人，率領22位委員建立重症個案處置諮詢平臺，規劃辦理COVID-19系列線上直播研討會以及COVID-19重症個案臨床處置線上病例諮詢討論會議，並擷取前述講座與諮詢會議之重要關鍵及實務經驗，彙整成「COVID-19重症照護關鍵紀實」專書，亦於本次頒獎典禮同步發表，以期相關領域專業人員精進臨床照護知能，作為未來疫情防治之參考。\$\@\$指揮中心表示，頒獎典禮中亦同步播放「關鍵『疫』戰，感謝有您」感謝與回顧影片，紀錄我國貢獻卓越的第一線防疫英雄堅守崗位、抗疫不懈的過程，共同回顧與感謝防疫英雄於抗疫期間守護國人健康的點點滴滴，同時也藉由國立臺灣大學醫學院杏林管弦樂團的音樂饗宴，象徵防疫的薪火相傳，生生不息！</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-24\$\@\$中央流行疫情指揮中心今(24)日表示，昨(23)日召開生物安全專家調查小組會議，針對中研院提供動物生物安全第三等級(Animal Biosafety Level 3, ABSL-3)實驗室內部調查報告，以及調查小組先前進行中研院相關人員訪談紀錄與實驗室內部監控影帶及資料，討論造成實驗室感染之可能原因。經初步調查結果如下：\$\@\$一、ABSL-3實驗室人員進行實驗操作時，未依規定穿著C級防護裝備(包括連身型防護衣、N95口罩、雙層手套、護目鏡及鞋套等)；並且在穿脫個人防護裝備(Personal Protective Equipment, PPE)以及使用生物安全櫃(Biosafety cabinet, BSC)方面，皆未遵守該實驗室訂定之標準作業程序(Standard Operating Procedures, SOP)。\$\@\$二、生物安全會未依「感染性生物材料管理辦法」規定，每年落實對實驗室辦理內部稽核；亦未追蹤ABSL-3實驗室之新進人員相關訓練考核完成情形。\$\@\$三、實驗室人員需再加強教育訓練，並落實訓練後考核機制，以及辦理個人防護裝備之實體演練，確認人員對於個人防護裝備穿脫的認知程度。\$\@\$四、另有部分調查細節尚待釐清，將請中研院再提供該實驗室人員進出實驗室之電子紀錄、監控影帶以及工作紀錄等，予調查小組確認。\$\@\$指揮中心說明，調查小組將於釐清相關事實後，完成最終調查報告，屆時再由指揮官統一對外說明。另對於中研院未依「感染性生物材料管理辦法」規定，落實單位內部生物安全事務之監督及管理情事，將於彙整相關違規事實後，依傳染病防治法第34條及第69條規定，對中研院進行裁處，從重處以最高罰鍰新臺幣十五萬元。\$\@\$指揮中心提醒，國內持有、使用、輸出入、保存及處分第2級危險群以上病原體及生物毒素之設置單位，單位生物安全主管及生物安全會，應依法落實對單位內部生物安全事務之監督及管理，以確保所屬實驗室之生物安全無虞。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-24\$\@\$中央流行疫情指揮中心今(24)日公布國內新增20例COVID-19移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增20例境外移入個案，為14例男性、6例女性，年齡介於10多歲至60多歲，分別自美國(7例，案16965、案16967、案16968、案16970、案16977、案16982、案16983)、越南(3例，案16971、案16979、案16980)、菲律賓(2例，案16973、案16974)、泰國(案16966)、德國(案16969)、馬來西亞(案16972)、印尼(案16975)、新加坡(案16976)、加拿大(案16978)、立陶宛(案16984)及日本(案16981)，入境日介於今(2021)年11月21日至12月22日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,844,559例新型冠狀病毒肺炎相關通報(含4,825,692例排除)，其中16,873例確診，分別為2,220例境外移入，14,599例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月24日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-23\$\@\$中央流行疫情指揮中心今(23)日表示，衛生福利部傳染病防治諮詢會預防接種組(ACIP)建議，考量目前國內部分民眾加入COVID-19疫苗臨床試驗計畫，ACIP參酌各國疫苗接種政策，建議該類民眾如後續有疫苗接種需求，可與臨床試驗研究單位討論後，經醫師評估接種其他國內核准之COVID-19疫苗，並建議與最後一劑試驗COVID-19疫苗間隔28天。\$\@\$指揮中心說明，由於國際疫情持續嚴峻及Omicron新型變異株之威脅增加，為積極防範社區傳播風險，自明(2022)年1月1日起，強化因工作或服務性質具有「接觸不特定人士或無法保持社交距離」之部分場所(域)人員COVID-19疫苗接種規範，如經醫師評估且開立不建議施打COVID-19疫苗證明，或個人因素無法施打者，可每週1次自費抗原快篩(含家用快篩)或PCR檢驗。另參與臨床試驗之民眾工作性質，如屬於「接觸不特定人士或無法保持社交距離」之對象，可與臨床試驗計畫單位討論後續疫苗接種，以及以自費抗原快篩(含家用快篩)或PCR檢驗取代疫苗接種證明等事宜。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-23\$\@\$中央流行疫情指揮中心今(23)日公布國內新增13例COVID-19移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增13例境外移入個案，為8例男性、5例女性，年齡介於10多歲至60多歲，分別自美國(10例，案16952-16954、案16956-16962)、多明尼加(案16955)、俄羅斯(案16963)、烏克蘭(案16964)，入境日介於今(2021)年12月7日至12月22日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,829,258例新型冠狀病毒肺炎相關通報(含4,810,401例排除)，其中16,853例確診，分別為2,200例境外移入，14,599例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月23日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-22\$\@\$疾病管制署今(22)日表示，迎接耶誕及新年到來，共度歡樂時光的同時，除落實防疫新生活及個人防護措施，也不忘互相提醒為「愛」篩檢，「定期篩檢」就是送給自己與伴侶最好的禮物。疾管署「愛滋自我篩檢 網路訂購超商取貨 期間限定免運費活動」自今(2021)年12月23日起開跑，至明(2022)年1月31日止，只要支付200元即可訂購愛滋自我篩檢試劑(免運費)，歡迎民眾把握機會、掌握自身健康！\$\@\$疾管署說明，為鼓勵民眾瞭解自身健康狀況，今年透過「愛滋自我篩檢計畫」已提供4萬7,000多人次篩檢服務，民眾上網登錄檢驗結果陽性率為0.5%，計畫受到廣大迴響，其中網路訂購超商取貨為民眾喜愛通路之一，有超過7成民眾使用。民眾可至疾管署自我篩檢網站預訂，選擇鄰近超商通路，支付200元試劑費及45元物流費取得自我篩檢試劑。假期將至，疾管署於12月23日推出「自我篩檢 網路訂購超商取貨 期間限定免運費活動」，民眾僅需支付試劑費用即可獲得篩檢試劑，寄送試劑的外包裝不會有任何標示內容物和寄送廠商名稱，充分保障隱私。\$\@\$此外，也可就近前往合作民間團體、衛生局(所)等411個實體服務點，或利用54臺自動服務機，支付200元費用後直接取得篩檢試劑，相關服務內容及試劑提供地點資訊可至疾管署自我篩檢計畫網頁(https://hiva.cdc.gov.tw/Selftest/)查詢。若初步檢驗呈陽性，即使沒有不適，請儘速至愛滋指定醫事機構進一步確認檢驗，疾管署補助當次就醫掛號費及部分負擔，並退還200元試劑費用。衛生局及相關民間團體也提供篩檢諮詢及篩檢陽性個案轉介或陪伴就醫等服務，如有需求可多加利用。\$\@\$疾管署提醒，若發生性行為應主動要求對方或自己全程使用保險套，並搭配水性潤滑液，以保護自己，降低感染風險。疾管署再次呼籲，有性行為者，建議至少進行1次愛滋篩檢，有不安全性行為者，建議每年至少進行1次篩檢，若有感染風險行為(如與人共用針具、多重性伴侶、合併使用成癮性藥物、感染性病等)，建議每3至6個月篩檢1次，以了解自身健康狀況。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-22\$\@\$中央流行疫情指揮中心今(22)日公布國內新增14例COVID-19移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增14例境外移入個案，為9例男性、5例女性，年齡介於20多歲至40多歲，分別自美國(5例，案16938、案16941-16942、案16946、案16950)、義大利(案16939)、印尼(案16940)、波蘭(案16943)、英國(案16944)、柬埔寨(案16945)、越南(3例，案16947、案16949、案16951)，餘1例調查中(案16948)，入境日介於今(2021)年10月7日至12月19日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,813,164例新型冠狀病毒肺炎相關通報(含4,794,827例排除)，其中16,840例確診，分別為2,187例境外移入，14,599例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。 2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月22日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-21\$\@\$中央流行疫情指揮中心今(21)日表示，本(2021)年12月14日起入境擇定春節檢疫專案C方案之民眾，將自12月21日起陸續期滿168小時，凡經檢疫第6天PCR檢測陰性及返家居家檢疫環境與條件均符合規定者，請全程佩戴口罩，搭乘地方政府安排之防疫車輛，返家接續後7天在家居家檢疫，並配合以下檢測措施：\$\@\$一、檢疫期間第10天(Day 10)以家用快篩檢測1次，並配合健康關懷回報結果。\$\@\$二、在家居家檢疫期滿前(Day 13-14)進行PCR檢測1次。\$\@\$三、檢疫期滿後，自主健康管理期間第6至7天(Day 20-21)以家用快篩檢測1次，並以雙向簡訊回復篩檢結果。\$\@\$指揮中心再次提醒，在居家檢疫期間，應留在家中，禁止外出，亦不得出境或出國，確實遵守「防範嚴重特殊傳染性肺炎入境健康聲明暨居家檢疫通知書(春節檢疫專案)」所載規定，並呼籲返家後7天係採1人1室之檢疫者，其同戶內同住者(非居家檢疫者)應共同遵守以下加強暨自主健康管理相關規定及檢測措施，包括：\$\@\$一、於檢疫者返家第3天、第7天各進行1次自費家用快篩，並以雙向簡訊回報結果。\$\@\$二、檢疫者返家檢疫同住期間加強自主健康管理7天，檢疫者檢疫期滿後，接續一起自主健康管理7天。\$\@\$三、自主健康管理期間之規定：\$\@\$(一)    每日早/晚各量體溫一次、詳實記錄體溫、健康狀況及活動史，並配合雙向簡訊回報健康狀況。\$\@\$(二)    避免出入無法保持社交距離，或容易近距離接觸不特定人之場所。\$\@\$(三)    禁止從事近距離或群聚型之活動。\$\@\$(四)    外出時全程佩戴口罩及保持社交距離。\$\@\$(五)    若出現相關症狀，應主動與當地衛生局聯繫，或撥1922，依指示方式就醫。\$\@\$四、加強自主健康管理期間，除遵守上開規定外，應同時遵守下列規定：\$\@\$(一)    不可與自國外入境家人共用房間、衛浴，亦不可同處、共食。\$\@\$(二)    僅能從事固定且有限度之活動，且不可搭乘大眾運輸，禁止至人潮擁擠場所。\$\@\$(三)    落實實名制，須記錄每日活動，且應全程佩戴口罩及保持社交距離。\$\@\$指揮中心強調，檢疫措施是控制疫情的必要防線之一，請民眾務必遵守檢疫期間相關事項，如有違反規定，依法最高可處新臺幣100萬元罰鍰。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-21\$\@\$中央流行疫情指揮中心今(21)日表示，防疫旅宿為國內疫情控制關鍵，經追蹤調查近期兩起群聚事件結果，為提升民眾入住安全品質，降低社區傳播風險，全面檢討防疫旅宿防疫作為，即刻啟動防疫旅宿3大強化措施，嚴守社區防線：\$\@\$一、建立防疫旅宿疑似COVID-19群聚事件之偵測與應變作業，以即時掌握可能相關個案，啟動防治作為：\$\@\$(一) 建立及早偵測防疫旅宿發生疑似群聚事件之策略及可運用資料。\$\@\$(二) 懷疑可能有疑似群聚事件階段之應變作為。\$\@\$(三) 已研判確認發生疑似群聚事件階段之應變作為。\$\@\$二、增修「COVID-19因應指引：防疫旅宿設置及管理」：\$\@\$針對本次群聚事件進行檢討分析，並針對環境、人員等設置與管理之可能風險，與相關專家討論後納入指引；並請地方政府加強落實防疫旅館每月查核作業。\$\@\$三、防疫旅宿訪視輔導與全面查核：\$\@\$(一) 請地方政府於111/1/3前完成全面查核，並可邀請勞動部勞動及職業安全衛生研究所代表或所推薦之通風空調領域專家共同參與，檢視防疫旅宿通風空調運作情形，對於查核結果有須改善之事項，儘速輔導並複查至改善完成。\$\@\$(二) 由感染管制、公共衛生、空調等領域專家組成查核團隊，預計自110/12/27啟動防疫旅宿訪視輔導作業，將曾發生群聚、高於75%入住率、採分層收住等事項之防疫旅宿列為優先訪視輔導對象，並提出改善建議。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-21\$\@\$中央流行疫情指揮中心今(21)日公布國內新增10例COVID-19移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增10例境外移入個案，為5例男性、5例女性，年齡介於20多歲至50多歲，分別自哥倫比亞(案16928)、美國(2例，案16929、案16937)、柬埔寨(案16930)、越南(案16931)、英國(3例，案16932、案16934-16935)、印尼(2例，案16933、案16936)，入境日介於今(2021)年11月22日至12月19日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,794,007例新型冠狀病毒肺炎相關通報(含4,775,550例排除)，其中16,826例確診，分別為2,173例境外移入，14,599例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月21日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-21\$\@\$中央流行疫情指揮中心今(21)日表示，AstraZeneca疫苗約73.84萬劑預定於今日下午抵達桃園國際機場，待完成通關程序後，直接運送至指定冷儲物流中心進行後續檢驗封緘作業，再提供COVID-19接種計畫所列實施對象接種。\$\@\$指揮中心指出，該中心係於去(2020)年10月30日與臺灣阿斯特捷利康公司簽署1,000萬劑COVID-19疫苗供應合約，截至目前總計已超過853萬劑到貨，分別為3月3日11.7萬劑、7月7日62.6萬劑、7月15日56萬劑、7月27日58.2萬劑、8月12日52.4萬劑、8月27日26.5萬劑、8月31日59.5萬劑、9月10日45.8萬劑、9月17日64萬劑、9月30日65.6萬劑、10月13日136萬劑、11月4日14.2萬劑、11月6日59.4萬劑、11月19日67.6萬劑，及本次提供第十五批73.84萬疫苗。本次提供的疫苗係為多劑型包裝(每瓶10人份)，需存放於2-8℃的環境，本批效期至2022年4月30日。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-20\$\@\$中央流行疫情指揮中心今(20)日表示，昨(19)日衛生福利部傳染病防治諮詢會預防接種組(ACIP)專家會議決議，經評估國內外疫情風險、國內疫苗供應現況並參酌各國疫苗接種政策，調整及建議COVID-19疫苗接種作業如下：\$\@\$(一)已接種基礎劑(primary series)第一劑COVID-19疫苗之民眾，經醫師評估符合接種間隔後，第二劑可選擇我國食品藥物管理署核准之接種任一廠牌COVID-19疫苗。\$\@\$(二)經醫師評估有免疫不全或免疫力低下且病情穩定之12歲以上民眾，應接種基礎加強劑(additional dose)，其與第二劑COVID-19疫苗間隔至少28天，建議優先接種mRNA疫苗(如Moderna、BNT)或次單位蛋白質疫苗(如高端)。\$\@\$(三)已完成基礎劑接種且間隔滿5個月之18歲以上民眾，應接種追加劑(Booster dose)，建議優先接種mRNA疫苗(如Moderna、BNT)或次單位蛋白質疫苗(如高端)，以獲得充足之免疫保護力。\$\@\$指揮中心說明，會議中專家參酌國內外臨床研究與試驗結果及各國接種策略指出，目前經衛生福利部食品藥物管理署核准專案輸入或製造之COVID-19疫苗，均需至少完成兩劑接種。由於目前國內各廠牌COVID-19疫苗供應充足，世界衛生組織(World Health Organization, WHO)、歐盟及各國亦多採用基礎劑可混打策略，民眾經醫師評估後，可選擇同廠牌疫苗或混打，以提升疫苗接種完成率。\$\@\$另ACIP專家檢視目前現有文獻及臨床試驗結果後表示，免疫不全以及免疫力低下病人即使完成2劑COVID-19疫苗接種，多無法獲得足夠的免疫保護力，爰建議12歲以上經醫師評估病情穩定之下列對象，應接種第3劑基礎加強劑，其間隔與第二劑COVID-19疫苗至少28天，建議優先接種全劑量mRNA疫苗(如Moderna、BNT)或次單位蛋白質疫苗(如高端)：\$\@\$(一)目前正進行或1年內曾接受免疫抑制治療之癌症患者\$\@\$(二)器官移植患者/幹細胞移植患者\$\@\$(三)中度/嚴重先天性免疫不全患者\$\@\$(四)血液透析患者\$\@\$(五)HIV陽性患者\$\@\$(六)目前正使用高度免疫抑制藥物者\$\@\$(七)過去6個月內接受化學治療或放射線治療者\$\@\$(八)其他經醫師評估因免疫不全或免疫力低下，可接種基礎加強劑者\$\@\$基於Omicron變異株疫情於各國持續升溫，ACIP專家表示雖然目前尚無證據顯示感染Omicron變異株後會增加重症、住院或死亡之風險，惟此變異株會可能造成突破性感染(Breakthrough infection)，降低疫苗之保護力，加速傳播，即使曾經感染過其他COVID-19基因型痊癒者，亦可能感染Omicron變異株。對此ACIP專家亦表示，目前就國際間臨床試驗報告、監測及相關文獻均指出，完成基礎劑接種後，疫苗保護力會隨接種時間消退，建議滿18歲以上民眾於完成基礎劑接種後，應接種追加劑。而依據目前國內外研究數據顯示，無論基礎劑接種何種廠牌COVID-19疫苗，國內追加劑建議優先接種Moderna COVID-19疫苗半劑量(50微毫克)、BioNTech COVID-19疫苗全劑量或次單位蛋白質疫苗(如高端)全劑量，以提升免疫保護力。\$\@\$指揮中心提醒，前述政策訂於12月24日開始實施，施行細節將於近日函知各地方政府衛生局轉轄內COVID-19疫苗接種合約院所。指揮中心呼籲，符合接種資格之民眾，請儘速前往COVID-19疫苗合約醫療院所完成接種，加強免疫保護。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-20\$\@\$中央流行疫情指揮中心今(20)日表示，有關中研院P3實驗室內部調查報告，該院已依指揮中心要求期限於昨(19)日晚間送達指揮中心。報告書中說明事發經過、院方應變措施、感染途徑調查、院方整體調查結果與根本原因分析、責任檢討與未來改進事項；其中針對人員訪談、11月中下旬監視器錄影檔、實驗室使用紀錄表等調查發現，確認具有以下三項感染暴露風險因子：\$\@\$一、實驗操作區與非操作區均存在環境汙染。於實驗動物操作時，未於生物安全櫃中進行。髒墊料直接置於未封口的袋子、也未放置於加蓋的容器中。\$\@\$二、個案及其他實驗室人員均曾僅穿著一般防護裝備(未戴N95口罩、雙層手套、護目鏡或面罩)執行實驗。\$\@\$三、個案於脫除防護裝備過程先行脫口罩。\$\@\$根據以上感染暴露風險因子，中研院研判感染途徑可能有三種：\$\@\$一、呼吸道直接暴露受汙染的墊料粉塵、染疫動物受刺激而引發噴飛沫或氣膠的環境。\$\@\$二、手套表面因直接操作染疫動物被汙染，於脫卸防護裝備程序先誤脫口罩時，接觸臉部口鼻等部位而感染。\$\@\$三、防護裝備外層在操作區遭帶有病毒之物體表面汙染，於脫卸防護裝備程序先誤脫口罩時，使口鼻暴露於脫卸過程而感染。\$\@\$此外，中研院亦針對：(1)新進人員教育訓練與操作指導；(2)實驗室SOP操作；(3)實驗操作過程監控；(4)個人防護裝備穿卸流程；(5)意外事故通報流程；(6)動物科學應用審核管理規範及感染性生物材料之使用管控；(7)本次染疫事件成因的系統性問題等七大面向，進行制度面及執行面的回顧檢討，並說明若最終調查認定確有違反規定，將依據人員身分別處理責任歸屬及處分。中研院並提出未來將成立P3實驗室綜合檢討委員會，確實改進P3實驗室的管理運作級生物安全監督查核機制。\$\@\$指揮中心說明，該中心已於12月17日及19日派員訪談中研院該P3實驗室主管、工作人員、及中研院生安會主委，並於今日上午提交訪談結果及中研院內部調查報告予外部專家調查小組，且安排於本週四開會進行審視及討論，預計兩週內提出外部專家小組調查結論及建議；另亦將依傳染病防治法第34條、第69條及感染性生物材料管理辦法第25條規定，對中研院進行裁處，最高可處十五萬元罰鍰，並限期令其改善，屆期未改善者，按次處罰之，並於生物安全疑慮解除前，要求該P3實驗室停止使用或處分相關感染性生物材料。另依前開管理辦法第29條規定，於生物安全疑慮解除，經該院生安會確認後，報疾管署同意後，始得再行使用或處分相關感染性生物材料。\$\@\$指揮中心另指出，除中研院基因體研究中心P3實驗室已另案調查，其餘國內11家操作新冠病毒之P3實驗室均已於12/17查核完畢，未發現重大缺失。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-20\$\@\$中央流行疫情指揮中心今(20)日公布國內新增11例COVID-19移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增11例境外移入個案，為7例男性、4例女性，年齡介於10多歲至50多歲，分別自義大利(案16917)、美國(5例，案16918-16920、案16922、案16926)、德國(案16921)、法國(案16923)、巴西(案16924)、越南(案16925)及菲律賓(案16927)入境，入境日介於今(2021)年12月5日至12月19日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,774,769例新型冠狀病毒肺炎相關通報(含4,756,108例排除)，其中16,816例確診，分別為2,163例境外移入，14,599例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月20日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-19\$\@\$中央流行疫情指揮中心今(19)日公布國內新增6例COVID-19境外移入確定病例；另確診個案中新增1例死亡。\$\@\$指揮中心說明，今日新增6例境外移入個案，為3例男性、3例女性，年齡介於10多歲至40多歲，分別自美國(案16911)、加拿大(案16912)、英國(2例，案16913、案16915)、越南(案16914)及奈及利亞(案16916)入境，入境日介於今(2021)年12月5日至12月17日；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增1例死亡個案(案4397)，為60多歲本國籍男性，具慢性病史；5月22日因發燒就醫採檢，5月23日住院隔離治療，5月24日確診，7月2日解除隔離，12月1日死亡。\$\@\$指揮中心統計，截至目前國內累計4,763,385例新型冠狀病毒肺炎相關通報(含4,744,216例排除)，其中16,805例確診，分別為2,152例境外移入，14,599例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月19日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-18\$\@\$中央流行疫情指揮中心今(18)日公布國內新增13例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增13例境外移入個案，為6例男性、7例女性，年齡介於10多歲至60多歲，分別自越南(4例，案16898、案16900、案16904、案16906)、英國(3例，案16899、案16905、案16908)、美國(2例，案16903、16910)、西班牙(案16901)、柬埔寨(案16902)、菲律賓(案16907)及新加坡(案16909)入境，入境日介於今(2021)年12月3日至12月17日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,747,250例新型冠狀病毒肺炎相關通報(含4,727,825例排除)，其中16,799例確診，分別為2,146例境外移入，14,599例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；累計111例移除為空號。2020年起累計849例COVID-19死亡病例，其中837例本土，個案居住縣市分布為新北市412例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月18日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-16\$\@\$中央流行疫情指揮中心今(16)日表示，因應案16851於今(2021)年12月11日自主健康管理期間確診，指揮中心與地方衛生局立即展開相關調查，包括擴大回溯追蹤、擴大採檢、現場勘查、病毒定序等，發現同防疫旅宿同樓層之案16768、16841、16851、16856病毒S基因序列相同，初步研判可能為一起防疫旅宿相關感染事件。\$\@\$指揮中心說明，考量防疫旅宿為國內疫情控制關鍵，指揮中心即刻啟動防疫旅宿四大強化作為，多管齊下，嚴守社區防線：\$\@\$一、強化監測作為，增加春節檢疫專案3項方案篩檢次數及查核與違規裁處：\$\@\$(一) 3方案均於入境時、檢疫第3、7、10、14及第21天(自主健康管理期間第6-7天)進行PCR檢驗或公費快篩(詳附件)。\$\@\$(二) 居家檢疫期間加強查核，違反規定者將加重裁處。\$\@\$二、防疫旅宿防疫措施查核：邀集感控專家針對防疫旅宿進行全面查核，指導與協助防疫旅宿落實防疫管理措施。\$\@\$三、防疫旅宿通風空調檢視：請勞動部勞動及職業安全衛生研究所協助全面檢視防疫旅宿之通風空調換氣情形，並提供改善建議。\$\@\$四、加強有症狀通報：檢疫期間有症狀均要進行PCR採檢，以確實掌握可能個案。 附件\$\@\$1216-春節檢疫專案篩檢次數調整.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-16\$\@\$中央流行疫情指揮中心今(16)日公布國內新增12例COVID-19確定病例，分別為1例本土及11例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增1例本土病例(案16882)，為80多歲本國籍女性，已接種2劑AZ疫苗，今(2021)年12月15日因腹痛、發燒等症狀就醫並採檢，於今日確診( Ct值39.9)，血清檢驗N蛋白抗體陽性，研判為舊案。目前已匡列接觸者2人，列居家隔離，其餘接觸者匡列中。衛生單位刻正進行疫情調查及防治，以釐清感染源。\$\@\$指揮中心表示，今日新增11例境外移入個案，為4例男性、7例女性，年齡介於10多歲至50多歲，分別自美國(案16871)、柬埔寨(3例，案16872、案16878、案16879)、菲律賓(2例，案16873、案16876)、英國(案16874)、越南(2例，案16875、案16877)、泰國(案16880)、蒙古(案16881)入境，入境日介於11月21日至12月14日，皆持有搭機前3日內檢驗陰性報告；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,710,205例新型冠狀病毒肺炎相關通報(含4,689,895例排除)，其中16,771例確診，分別為2,125例境外移入，14,592例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計849例COVID-19死亡病例，其中837例本土，個案居住縣市分布為新北市412例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月16日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-15\$\@\$中央流行疫情指揮中心今(15)日公布國內新增7例COVID-19境外移入確定病例；另確診個案中新增1例死亡。\$\@\$指揮中心說明，今日新增7例境外移入個案，為6例男性、1例女性，年齡介於20多歲至40多歲，分別自菲律賓(3例，案16864、案16866、案16867)、澳大利亞(案16865)、印尼(案16868)及美國(案16870)入境，餘1例調查中(案16869)，入境日介於今(2021)年11月30日至12月5日；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增1例死亡個案(案10511)，為50多歲本國籍男性，具慢性病史及相關活動接觸史；6月3日採檢為陽性，6月4日因呼吸喘住院隔離治療，6月5日確診，8月14日解除隔離，11月19日死亡。\$\@\$指揮中心統計，截至目前國內累計4,690,800例新型冠狀病毒肺炎相關通報(含4,672,174例排除)，其中16,759例確診，分別為2,114例境外移入，14,591例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；累計111例移除為空號。2020年起累計849例COVID-19死亡病例，其中837例本土，個案居住縣市分布為新北市412例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月15日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-14\$\@\$中央流行疫情指揮中心今(14)日公布國內新增10例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增10例境外移入個案，為6例男性、4例女性，年齡介於10多歲至50多歲，分別自美國(2例，案16854、案16855)、香港(案16856)、孟加拉(案16857)、越南(2例，案16858、案16863)、柬埔寨(案16859)、菲律賓(案16860)、阿拉伯聯合大公國(案16861)及印尼(案16862)入境，入境日介於今(2021)年11月26日至12月12日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,672,651例新型冠狀病毒肺炎相關通報(含4,655,350例排除)，其中16,752例確診，分別為2,107例境外移入，14,591例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另累計111例移除為空號。2020年起累計848例COVID-19死亡病例，其中836例本土，個案居住縣市分布為新北市412例、臺北市321例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月14日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-13\$\@\$中央流行疫情指揮中心今(13)日公布國內新增5例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增5例境外移入個案，為4例男性、1例女性，年齡介於10多歲至40多歲，分別自越南(2例，案16849、案16853)、英國(案16850)、中國(案16851)及馬來西亞(案16852)入境，入境日介於今(2021)年11月20日至12月10日，皆持有搭機前3日內檢驗陰性報告；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,657,395例新型冠狀病毒肺炎相關通報(含4,639,667例排除)，其中16,742例確診，分別為2,097例境外移入，14,591例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另累計111例移除為空號。2020年起累計848例COVID-19死亡病例，其中836例本土，個案居住縣市分布為新北市412例、臺北市321例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月13日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-13\$\@\$因應國際間新變異株Omicron威脅，中央流行疫情指揮中心經與相關單位溝通討論及評估後，於今(13)日宣布，自今(2021)年12月14日至12月27日維持疫情警戒標準為第二級，並維持相關措施及規定如下：\$\@\$一、維持現行戴口罩規定，外出時應全程佩戴口罩，但符合以下情形，得免戴口罩(本次未調整)：\$\@\$(一)下列場合得免戴口罩，但應隨身攜帶口罩，且如本身有相關症狀或與不特定對象無法保持社交距離時，仍應戴口罩：\$\@\$1.於室內外從事運動、唱歌時。\$\@\$2.於室內外拍攝個人/團體照時。\$\@\$3.單人或多人進行直播、錄影、主持、報導、致詞、演講、講課等談話性質工作或活動之正式拍攝或進行時。\$\@\$4.農林漁牧工作者於空曠處(如：田間、魚塭、山林)工作。\$\@\$5.於山林(含森林遊樂區)、海濱活動。\$\@\$6.於溫/冷泉、烤箱、水療設施、三溫暖、蒸氣室、水域活動等易使口罩潮濕之場合。\$\@\$(二)外出時有飲食需求，得免戴口罩。\$\@\$(三)於指揮中心或主管機關指定之場所或活動，如符合相關防疫措施，得暫時脫下口罩。\$\@\$二、營業場所及公共場域維持應遵守實聯制、量體溫、加強環境清消、員工健康管理、確診事件即時應變。\$\@\$指揮中心將視國內外疫情及實際執行狀況，適時機動調整防疫措施，強化邊境監測及防疫作為。籲請民眾應落實個人防護措施，主動積極配合各項防疫規範，以兼顧防疫與生活品質。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-13\$\@\$中央流行疫情指揮中心今(13)日表示，目前已全面提供「AZ、莫德納、BNT、高端共4種疫苗第一、二劑」、「已接種第一劑AZ疫苗，第二劑混打BNT或莫德納疫苗」以及「完整接種COVID-19疫苗且滿5個月，追加接種第三劑莫德納」之接種服務，請民眾儘速透過「COVID-19公費疫苗預約平臺」（https://1922.gov.tw/ ，以下簡稱預約平臺）或各地方政府指定合約醫療院所/衛生所預約接種。\$\@\$其中，預約平臺第18期規劃提供BNT疫苗預約，相關對象及期程說明如下：\$\@\$一、符合資格對象，12月13日上午6時前已意願登記(含混打)民眾，且符合下列任一條件：\$\@\$(一) BNT第一劑：12歲以上民眾[即2009/12/16(含)前出生]。\$\@\$(二) BNT第二劑：11月18日(含)前已接種BNT第一劑18歲以上民眾[即2003/12/31(含)前出生]。\$\@\$(三)已接種第一劑AZ，第二劑混打BNT疫苗：10月21日(含)前已接種AZ第一劑18歲以上民眾[即2003/12/16(含)前出生]。\$\@\$二、預約時程：12月14日上午10時至12月15日中午12時。\$\@\$三、施打時程：12月16日至12月22日。\$\@\$指揮中心說明，上述符合資格對象將於12月13日下午2時起，陸續收到提醒簡訊，請記得依預約時間進行預約；預約當日如遇啟動流量管制亦請配合依序排隊耐心等候預約。後續將視疫苗供應期程調整接種場次，籲請民眾屆時準時前往接種。\$\@\$指揮中心強調，各廠牌疫苗均可至各地方政府衛生局合約醫療院所預約接種，且衛生福利部所屬醫院、國軍退除役官兵輔導委員會所屬醫院及國防部所屬醫院，亦增開週一至週五夜間門診，提供莫德納疫苗接種服務，請民眾多加利用，並呼籲民眾儘速完成二劑疫苗接種，以獲得完整免疫保護力。\$\@\$指揮中心提醒，10月1日起亦開始接種流感疫苗，依我國衛生福利部傳染病防治諮詢會預防接種組(ACIP)建議，接種流感疫苗應與COVID-19疫苗間隔至少7天，請民眾前往接種COVID-19第二劑疫苗前，應備妥「COVID-19疫苗接種紀錄卡」及健保卡，並於接種前評估時說明過往疫苗接種史，以利醫生評估。另未滿18歲對象，請由家長(或法定代理人、監護人及關係人等)陪同前往合約醫療院所或接種站接種，並由本人與家長於現場共同簽署意願同意書；18歲至未滿20歲民眾，如自行前往接種，請持家長簽具之意願同意書，若由家長陪同前往接種，請本人與家長於現場共同簽署意願同意書。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-12\$\@\$中央流行疫情指揮中心今(12)日公布國內新增6例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增6例境外移入個案，為5例男性、1例女性，年齡介於10多歲至20多歲，分別自美國(2例，案16843、案16844)、柬埔寨(案16845)、馬來西亞(案16846)、菲律賓(案16847)及印尼(案16848)入境，入境日介於今(2021)年11月26日至12月10日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,646,270例新型冠狀病毒肺炎相關通報(含4,628,598例排除)，其中16,737例確診，分別為2,092例境外移入，14,591例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計848例COVID-19死亡病例，其中836例本土，個案居住縣市分布為新北市412例、臺北市321例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月12日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-11\$\@\$中央流行疫情指揮中心今(11)日公布國內新增10例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增10例境外移入個案，為7例男性、3例女性，年齡介於10多歲至70多歲，分別自美國(案16833)、柬埔寨(2例，案16834、案16835)、印尼(案16836)、緬甸(案16837)、越南(3例，案16838-16840)、中國(案16841)及蒙古(案16842)入境，入境日介於今(2021)年11月19日至12月9日，皆持有搭機前3日內檢驗陰性報告；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,632,446例新型冠狀病毒肺炎相關通報(含4,614,110例排除)，其中16,731例確診，分別為2,086例境外移入，14,591例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另累計111例移除為空號。2020年起累計848例COVID-19死亡病例，其中836例本土，個案居住縣市分布為新北市412例、臺北市321例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月11日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-10\$\@\$中央流行疫情指揮中心今(10)日表示，因應國內新增本土確定病例，為降低社區感染及傳播風險，呼籲已接種兩劑COVID-19疫苗且滿5個月之民眾，可前往追加接種第三劑莫德納COVID-19疫苗，提升免疫保護力。依目前各國核准及我國衛生福利部傳染病防治諮詢會預防接種組(ACIP)建議，莫德納追加劑接種劑量為50微毫克(依目前劑型，注射量為0.25ml)。\$\@\$指揮中心說明，目前各廠牌COVID-19疫苗接種後之免疫保護力會隨時間下降，加上COVID-19病毒變異株具免疫逃脫之特性，即使完整接種兩劑疫苗後，仍可能因免疫保護力不足導致突破性感染(breakthrough infection)，建議符合接種間隔之民眾可接種追加劑，特別是醫護人員、防疫工作人員、第一線高感染風險工作人員、65歲以上長者、長照機構住民與工作者及容易感染與疾病嚴重風險者。民眾除可透過各地方政府衛生局合約醫療院所預約接種，亦可多利用衛生福利部所屬醫院、國軍退除役官兵輔導委員會所屬醫院、及國防部所屬醫院於週一至週五增設之夜間門診。指揮中心提醒民眾前往接種時，應備妥「COVID-19疫苗接種紀錄卡」及健保卡，並於接種前評估時說明過往疫苗接種史，以利醫生評估。\$\@\$指揮中心指出，昨(9)日屆期之莫德納 COVID-19疫苗已全數用罄，指揮中心特別感謝地方政府及醫療院所通力合作，積極調度，有效運用疫苗資源。截至本年12月10日止，我國COVID-19疫苗第一劑涵蓋率為78.55%，第二劑涵蓋率為63.25%，呼籲尚未接種第一劑或完整接種之民眾應儘速接種。\$\@\$指揮中心表示，為提供民眾更便利的疫苗接種服務，指揮中心自12月5日起協調臺北車站場地及三軍總醫院、三軍總醫院松山分院與衛生福利部臺北醫院醫療人力，提供莫德納COVID-19疫苗第一劑及第二劑接種服務，截至12月9日已接種12,760人次。臺北車站接種站服務期間至12月12日止，服務時間為每日下午1時至晚上8時，尚未接種第一劑或二劑疫苗之民眾可多加利用。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-09\$\@\$中央流行疫情指揮中心今(9)日公布國內新增1例COVID-19本土確定病例(案16816)，為本國籍20多歲女性，曾任中央研究院基因體研究中心實驗室研究人員，近期無出入境紀錄，已接種2劑莫德納疫苗。個案於11月中旬工作過程曾接觸過病原，當下並無症狀；11月26日開始出現輕微咳嗽，12月4日咳嗽加劇，12月8日出現嗅、味覺異常，就醫採檢後，於今日確診。\$\@\$指揮中心說明，因應本例本土確定病例，指揮中心已初步匡列相關接觸者共85人，均安排於集中檢疫所隔離，並進行採檢，其中1人為陰性，其餘接觸者持續匡列中。指揮中心進一步說明，在接獲醫院通報個案後，隨即安排疾病管制署防疫醫師、同仁至該實驗室進行調查，同時由專家諮詢小組張上淳召集人到場指導並召開會議，針對疫情及防治作為進行討論，採取措施包括：\$\@\$一、個案所屬實驗室暫停使用，同樓層人員全數居家隔離。\$\@\$二、調閱實驗室進出紀錄及錄影帶，以掌握可能接觸者及瞭解運作情形。\$\@\$三、實驗室全棟人員12月10日停止上班，且於9日起自我健康監測，如有不適症狀立即聯絡衛生單位。\$\@\$四、要求中央研究院10日內提出調查檢討報告，指揮中心將派生物安全專家調查小組前往該實驗室進行調查。\$\@\$指揮中心進一步指出，依照該中心所訂定的「新型冠狀病毒(SARS-CoV-2)之實驗室生物安全指引」，請各實驗室務必落實及查核相關規定，也提醒相關人員，注意下列事項，確保自身安全：\$\@\$一、有關從事SARS-CoV-2檢驗研究相關實驗室之工作人員，應落實健康監測。\$\@\$二、如實驗室工作人員出現疑似感染症狀，應主動通報實驗室主管並儘速就醫評估，並於就醫時主動告知醫師相關暴露風險。\$\@\$三、操作SARS-CoV-2檢驗研究相關實驗室工作人員，應儘速完成COVID-19疫苗接種。\$\@\$四、各設置單位之生物安全會應落實實驗室工作人員之健康監測管理。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-09\$\@\$衛生福利部疾病管制署今(9)日表示，為響應雙語國家政策，自2019年起，每年推出一套4本中英文防疫雙語繪本「CHELSEA AND FRIENDS小喜與朋友們」，至今(2021)年共推出三套12個主題，利用中英文對照、淺顯易懂的單字及故事劇情，讓小朋友在學習常見的傳染病，如COVID-19、登革熱、腸病毒、流感等知識中，一起學習英文。\$\@\$疾管署說明，今年是以狂犬病、日本腦炎、破傷風及結核病等傳染病為主題，設計4本中英文雙語繪本，除了中英文雙語繪本外，也製作了新型A型流感、腸病毒中英文防疫兒歌動畫影片4支；系列繪本及兒歌動畫，都是透過主角「小喜」與好朋友之間的故事，深入淺出地引導讀者認識疾病症狀與預防方法，大人、小孩在閱讀繪本及學習兒歌的過程中，能共同學習與思考正確防疫觀念。\$\@\$疾管署也指出，隨著民眾對傳染病相關議題越來越關注，今年特別邀請廚神奶爸蔣偉文擔任防疫大使，拍攝宣導短片《「廚神奶爸」防疫繪話通》，與民眾分享親子共讀及歌唱的樂趣，也向民眾呼籲勤洗手、戴口罩、及按時接種疫苗等防疫措施對幼兒預防傳染病的重要性。育有兩子的蔣偉文在影片中與小朋友安安一起閱讀雙語繪本「汪！汪！」，以說故事方式，搭配中英語對話互動，讓家長知道如何輕鬆、自然與孩子共讀，寓教於樂學習防疫知識；此外，影片中還有一起學唱「新型A型流感」雙語防疫兒歌動畫，藉由簡單的歌詞讓小孩記得基本的預防方法。\$\@\$身為防疫大使的蔣偉文也透露，防疫雙語繪本與兒歌不僅故事畫風有趣，容易吸引小孩注意，讓小孩在閱讀繪本與歌唱過程中，提升對傳染病認知並學習豐富的英文單字，大力推薦給家中有幼兒的父母親。\$\@\$本系列套書可透過國家書店、五南書店購買；防疫兒歌動畫影片，可於疾管署全球資訊網宣導專區（https://reurl.cc/m9yaLj），選擇新型A型流感或腸病毒主題之影片分類下觀看；《「廚神奶爸」防疫繪話通》也可至相同宣導專區，選擇狂犬病或新型A型流感主題之影片分類下觀看。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-09\$\@\$中央流行疫情指揮中心今(9)日表示，因應國際疫情變化難測、新興變異株頻傳，並考量國際間COVID-19病毒核酸(PCR)檢測可近性已大幅增加，為確保航空防疫安全，自2021年12月14日起，調整「3日內」PCR報告日為啟程地表定航班時間往前推3個「日曆日」計算，不排除當地國定假日、例假日，請旅客搭機前務必確認PCR檢驗報告符合規範。\$\@\$指揮中心指出，春節檢疫措施專案將於下週二(12月14日)上路，預期將湧現返鄉人潮，提醒12月14日至明(2022)年2月14日期間自國外返臺旅客，必須瞭解及配合以下三步驟，事先做好檢疫，返臺將更簡易：\$\@\$第一步、事前，應準備資料：\$\@\$旅客請依照選擇的春節檢疫方案(方案A：入住防疫旅宿完成檢疫期14天及接續自主健康管理7天、方案B：10天入住防疫旅宿+4天在家居家檢疫+7天自主健康管理、方案C：7天自費入住集中檢疫所或防疫旅宿+7天在家居家檢疫+7天自主健康管理)，備妥相關資料及可上網的個人手機；其中無論選擇哪個方案，全部旅客均需準備「搭機前三日內COVID-19病毒核酸(PCR)檢驗報告」和「防疫旅宿訂房證明(全部旅客)」；如為選擇方案C者，須增加準備「完整疫苗接種證明」；此外，若為選擇方案B/方案C旅客，且於隔離檢疫最後4天/7天需返家，並符合以一人一室方式進行在家檢疫者(同住家人須已完整COVID-19疫苗接種且滿14天)，應事前取得同戶內同住家人之姓名、身分證字號、電話等個人資訊，以利線上申報。\$\@\$第二步、搭機前，應完成線上申報：\$\@\$旅客請於航班抵臺前48小時內至「入境檢疫系統」( https://hdhq.mohw.gov.tw/ )完成線上申報，於國外機場報到(check-in)時，出示已完成線上申報之「啟程地申報證明」手機畫面，並隨身攜帶前述證明文件，以供航空公司進行搭機前檢視作業。\$\@\$第三步、抵臺時，應依現場引導順利通關：\$\@\$旅客下機後，請打開手機確認收到簡訊，於機場通關時依序出示線上檢疫憑證及前述證明文件；於完成證照查驗及提領行李，再取快篩試劑(選擇方案A、方案C者)、並配合深喉唾液採檢後，儘速搭乘防疫車輛前往檢疫地點，完成14天檢疫。\$\@\$指揮中心強調，邊境管制為防範COVID-19疫情的重要關鍵，交通主管機關已通知各航空公司應主動通知訂票旅客配合上述規定及落實外站檢視把關；也籲請入境旅客務必配合上述規範及相關檢疫措施，共同維護國內防疫安全。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-09\$\@\$中央流行疫情指揮中心今(9)日公布國內新增16例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增16例境外移入個案，為11例男性、5例女性，年齡介於10多歲至50多歲，分別自美國(案16800)、越南(7例，案16801-16802、案16806、案16809-16812)、西班牙(案16803)、英國(2例，案16804-16805)、菲律賓(2例，案16807、案16815)及印尼(3例，案16808、案16813-16814)入境，入境日介於今(2021)年11月25日至12月7日，皆持有搭機前3日內檢驗陰性報告；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,600,226例新型冠狀病毒肺炎相關通報(含4,582,236例排除)，其中16,704例確診，分別為2,060例境外移入，14,590例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計848例COVID-19死亡病例，其中836例本土，個案居住縣市分布為新北市412例、臺北市321例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月9日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-09\$\@\$中央流行疫情指揮中心今(9)日表示，台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的第十四批BNT疫苗192.35萬劑，預計於今日下午運抵桃園國際機場，並在完成通關程序後，直接運送至指定冷儲物流中心進行後續檢驗封緘作業。\$\@\$指揮中心說明，由台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的BNT疫苗1,500萬劑，目前共計到貨1239.79萬劑，分別為首批9月2日93萬劑、第二批9月9日91萬劑、第三批9月30日54萬劑、第四批10月1日67萬劑、第五批10月4日27萬劑、第六批10月7日88.92萬劑、第七批10月8日88.92萬劑、第八批10月14日82.7萬劑、第九批10月28日90.21萬劑、第十批10月29日91.03萬劑、第十一批11月5日87.17萬劑、第十二批11月12日92.66萬劑、第十三批11月25日93.83萬劑，以及本批192.35萬劑。本批疫苗效期至2022年3月25日，將由指揮中心統籌運用，儘速提供民眾接種。\$\@\$對於台積電、鴻海暨永齡基金會、慈濟基金會三間企業和民間團體積極協助，提供更多的疫苗讓民眾接種，加速提升臺灣疫苗覆蓋率，指揮中心再次表達由衷的謝意。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-08\$\@\$中央流行疫情指揮中心今(8)日表示，由於國際疫情持續嚴峻及Omicron新型變異株之威脅增加，考量國內COVID-19疫苗接種量能尚屬充足，為積極防範社區傳播風險，自111年1月1日起，中央各部會及地方政府權管場所場域之工作人員及從業人員，屬於維持醫療及防疫量能者、高接觸風險工作者、維持國家安全及社會機能正常運作者(即COVID-19公費疫苗接種對象第1、2、3、7類對象)，以及矯正機關、殯葬場所工作人員等(詳如附件)，因工作或服務性質具有「接觸不特定人士或無法保持社交距離」之特性，將強化上述人員COVID-19疫苗接種規範，共同維護國人健康安全。規範原則如下：\$\@\$一、上述中央各部會及地方政府權管場所場域工作人員/從業人員皆應接種COVID-19疫苗2劑且滿14天（最晚應於110年12月17日前接種第2劑疫苗）；新進人員於首次服務前，倘未完整接種2劑疫苗且滿14天，應提供自費3日內抗原快篩(含家用快篩)或PCR檢驗陰性證明。\$\@\$二、倘人員曾為COVID-19確診個案，且持有3個月內由衛生機關開立之解除隔離通知書者，可暫免檢具COVID-19疫苗接種證明，惟應於解除隔離滿3個月後，儘速完整接種COVID-19疫苗，新進人員並應於首次服務前，提供自費3日內PCR檢驗陰性證明。\$\@\$三、倘人員經醫師評估且開立不建議施打COVID-19疫苗證明或個人因素無法施打者，須每週1次自費抗原快篩(含家用快篩)或PCR檢驗陰性後，始得提供服務，新進人員並應於首次服務前，增加1次自費3日內PCR檢驗陰性證明。\$\@\$指揮中心強調，為確保相關場所場域人員自111年1月1日起皆能符合上開規範，各相關部會及地方政府將加強督導，請相關場所場域鼓勵未完整COVID-19疫苗接種之工作人員及從業人員，儘速於110年12月17日前完整接種2劑疫苗。 附件\$\@\$附件-各部會業管場所場域之工作及從業人員於110年12月17日前完整接種2劑疫苗清單.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-08\$\@\$中央流行疫情指揮中心今(8)日公布國內新增5例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增5例境外移入個案，為3例男性、2例女性，年齡介於20多歲至70多歲，分別自印尼(2例，案16795、案16796)、菲律賓(案16797)及衣索比亞(2例，案16798、案16799)入境，入境日介於今(2021)年11月19日至11月24日，皆持有搭機前3日內檢驗陰性報告；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,583,889例新型冠狀病毒肺炎相關通報(含4,566,149例排除)，其中16,688例確診，分別為2,044例境外移入，14,590例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另累計111例移除為空號。2020年起累計848例COVID-19死亡病例，其中836例本土，個案居住縣市分布為新北市412例、臺北市321例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月8日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-08\$\@\$中央流行疫情指揮中心今(8)日表示，為因應Omicron變異株疫情，以及提供民眾更便利的疫苗接種服務，指揮中心自今(2021)年12月5日起在臺北車站開設「莫德納疫苗施打站」，由於民眾接種踴躍，除原三軍總醫院松山分院醫護人力外，已於12月6日起再協調三軍總醫院及衛生福利部臺北醫院醫療人力增設2個施打處，截至12月7日止，累計接種5,623人次。為擴大接種服務，符合民眾接種需求，該接種站將延長服務時間至12月12日止，持續在每日下午1時至晚上8時，於車站大廳西側迴廊、車站大廳及東側迴廊，共3個施打處提供莫德納疫苗接種服務；可接種對象不限本國籍民眾，外國籍人士亦可接種，民眾無需預約，隨到隨打，完成接種者即可獲得1份禮品。\$\@\$指揮中心另說明，昨(7)日屆效之莫德納疫苗皆已用完，此外，約有4萬劑解凍後28天之莫德納疫苗即將於12月12日到期；為使資源有效運用，並為提升民眾莫德納疫苗第一劑、第二劑施打意願，各縣市至12月21日止，均可提供接種疫苗之宣導品，以鼓勵民眾踴躍接種莫德納疫苗。\$\@\$指揮中心強調，除設置施打站外，並已協調衛生福利部所屬醫院、國軍退除役官兵輔導委員會所屬醫院、及國防部所屬醫院，增開週一至週五夜間門診，提供莫德納疫苗接種服務；另其餘廠牌COVID-19疫苗亦可透過「COVID-19公費疫苗預約平臺」、或各地方政府衛生局合約醫療院所預約接種。呼籲民眾把握機會儘速完成二劑疫苗接種，以獲得完整免疫保護力。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-07\$\@\$中央流行疫情指揮中心今(7)日表示，有關媒體報導新竹縣一名失聯移工接種疫苗被捕一事，指揮中心說明如下：\$\@\$一、指揮中心指出，為提高全國疫苗覆蓋率，指揮中心與地方衛生局設置接種站，提供民眾(含外籍人士)便利接種，針對失聯移工配合政策出面接種疫苗，昨(6)日記者會再度重申，治安機關不會針對失聯移工進行查處，因此，已通知各治安機關依指揮中心之防疫政策辦理。\$\@\$二、指揮中心強調，逾期停(居)留外來人口申請接種疫苗所提供之基本資料，不會作為治安機關查處依據；現階段，各治安機關均應以防疫為首要任務，請各治安機關務必配合。\$\@\$三、指揮中心重申，為確保臺灣社區防疫安全網，勞政、衛政、警政及移民等各機關，應確實配合指揮中心防疫政策辦理。各機關請依內政部移民署「安心接種疫苗專案」之不通報、不查處、不收費及不管制等四項作為，鼓勵逾期停(居)留外來人口出面接種疫苗，共同維護臺灣的防疫安全。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-07\$\@\$中央流行疫情指揮中心今(7)日公布國內新增21例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增21例境外移入個案，為8例男性、13例女性，年齡介於20多歲至60多歲，分別自貝里斯(案16774)、美國(2例，案16775、案16777)、印尼(10例，案16776、案16778-16779、案16781-16782、案16789-16790、案16792-16794)、越南(案16780)、新加坡(5例，案16783-16787)、柬埔寨(案16788)及菲律賓(案16791)入境，入境日介於今(2021)年10月29日至12月5日，皆持有搭機前3日內檢驗陰性報告；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,565,572例新型冠狀病毒肺炎相關通報(含4,547,856例排除)，其中16,683例確診，分別為2,039例境外移入，14,590例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另累計111例移除為空號。2020年起累計848例COVID-19死亡病例，其中836例本土，個案居住縣市分布為新北市412例、臺北市321例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月7日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-05\$\@\$中央流行疫情指揮中心今(5)日表示，考量目前國內已持續提升COVID-19疫苗接種量能，為積極防範國際疫情嚴峻及新型變異株威脅，降低社區傳播風險，自111年1月1日起，教育部、經濟部、勞動部及衛生福利部業管之部分場所(域)防疫指引(如附表)將強化COVID-19疫苗接種規範，以嚴守社區防線。規範原則如下：\$\@\$一、所有工作人員/從業人員皆應接種COVID-19疫苗2劑且滿14天，復業及新進人員於首次服務前，應同時提供自費3日內抗原快篩(含家用快篩)或PCR檢驗陰性證明。\$\@\$二、倘人員曾為COVID-19確診個案，且持有3個月內由衛生機關開立之解除隔離通知書者，可暫免檢具COVID-19疫苗接種證明。惟於首次服務前，仍應提供自費3日內PCR檢驗陰性證明，並應於解除隔離滿3個月後，儘速完整COVID-19疫苗接種。\$\@\$三、倘人員經醫師評估且開立不建議施打COVID-19疫苗證明或個人因素無法施打者，於首次服務前，應提供自費3日內PCR檢驗陰性證明，後續須每週1次自費抗原快篩(含家用快篩)或PCR檢驗陰性後，始得提供服務。\$\@\$指揮中心強調，為確保相關場所(域)人員自111年1月1日起能符合上開規範，請相關場所(域)鼓勵未完整COVID-19疫苗接種之工作人員及從業人員，儘速於110年12月17日前完整接種疫苗2劑。各相關部會亦將加強查核，倘場所(域)尚有未完整COVID-19疫苗接種之人員，業者須限期改善，並依各主管機關所訂之防疫指引規定辦理。 附件\$\@\$附件-訂有COVID-19疫苗接種規定之防疫指引.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-05\$\@\$中央流行疫情指揮中心今(5)日表示，為因應Omicron變異株疫情，以及提供民眾更便利的疫苗接種服務，指揮中心已協調臺北車站場地及三軍總醫院松山分院醫療人力，自即日起至12月9日止，每日下午1時至晚上8時，於車站大廳西側迴廊開設「莫德納疫苗施打站」，不限本國籍民眾，外國籍人士亦可接種，民眾無需預約，隨到隨打，完成接種者還可獲得禮品1份。\$\@\$指揮中心說明，臺北車站「莫德納疫苗施打站」可接種對象如下：\$\@\$一、18歲以上有意願接種莫德納疫苗第一劑者。\$\@\$二、已接種莫德納疫苗第一劑間隔滿4週以上者。\$\@\$三、已接種AZ疫苗第一劑間隔滿8週以上者。\$\@\$指揮中心指出，經考量臺北火車站為臺鐵、高鐵及臺北捷運三鐵共構，地理位置便利，出入人潮眾多，為方便即時提供民眾接種服務，提升疫苗之可近性，故選擇該站做為莫德納疫苗施打站，歡迎民眾踴躍多加利用。\$\@\$指揮中心強調，除設置施打站外，並已協調衛生福利部所屬醫院、國軍退除役官兵輔導委員會所屬醫院、及國防部所屬醫院，增開週一至週五夜間門診，提供莫德納疫苗接種服務；另其餘廠牌COVID-19疫苗亦可透過「COVID-19公費疫苗預約平臺」、或各地方政府衛生局合約醫療院所預約接種。呼籲民眾把握機會儘速完成二劑疫苗接種，以獲得完整免疫保護力。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-05\$\@\$中央流行疫情指揮中心今(5)日公布國內新增4例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增4例境外移入個案，為3例男性、1例女性，年齡介於20多歲至60多歲，分別自美國(案16760)、越南(案16761)、寮國(案16762)及印尼(案16763)入境，入境日介於今(2021)年11月18日至12月3日，皆持有搭機前3日內檢驗陰性報告；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,536,780例新型冠狀病毒肺炎相關通報(含4,518,083例排除)，其中16,652例確診，分別為2,008例境外移入，14,590例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另累計111例移除為空號。2020年起累計848例COVID-19死亡病例，其中836例本土，個案居住縣市分布為新北市412例、臺北市321例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月5日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-04\$\@\$中央流行疫情指揮中心今(4)日公布國內新增11例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增11例境外移入個案，為5例男性、6例女性，年齡介於未滿5歲至50多歲，分別自美國(2例，案16749、案16759)、新加坡(案16750)、越南(2例，案16751、16755)、印尼(5例，案16752- 16754、案16757-16758)及柬埔寨(案16756)入境，入境日介於今(2021)年11月19日至12月2日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,523,528例新型冠狀病毒肺炎相關通報(含4,504,860例排除)，其中16,648例確診，分別為2,004例境外移入，14,590例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另累計111例移除為空號。2020年起累計848例COVID-19死亡病例，其中836例本土，個案居住縣市分布為新北市412例、臺北市321例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月4日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-04\$\@\$中央流行疫情指揮中心今(4)日表示，目前已全面提供民眾BNT疫苗、AZ疫苗、莫德納疫苗以及高端疫苗等四種COVID-19疫苗預約接種，為方便民眾接種疫苗，除「COVID-19公費疫苗預約平臺」（https://1922.gov.tw/ ，以下簡稱預約平臺）外，指揮中心已開放各地方政府指定/安排合約醫療院所或衛生所，提供AZ、莫德納、BNT、高端共4種疫苗第一、二劑，及已接種第一劑AZ疫苗，第二劑混打BNT或莫德納疫苗之接種服務。\$\@\$其中，預約平臺第17期規劃提供BNT疫苗及AZ疫苗預約，相關對象及期程說明如下：\$\@\$一、 符合資格對象，今(2021)年12月5日上午6時前已意願登記/混打意願登記民眾，且符合下列任一條件：\$\@\$(一) BNT第一劑：12歲以上民眾[即2009/12/9(含)前出生]。\$\@\$(二) BNT第二劑：11月11日(含)前已接種BNT第一劑18歲以上民眾[即2003/12/31(含)前出生]。\$\@\$(三) AZ第一劑：18歲以上民眾[即2003/12/9(含)前出生]。\$\@\$(四) AZ第二劑/第二劑混打BNT疫苗：10月14日(含)前已接種AZ第一劑18歲以上民眾[即2003/12/9(含)前出生]。\$\@\$二、 預約分流時程：\$\@\$(一) BNT 疫苗：12月6日上午10時至12月7日中午12時。\$\@\$(二) AZ疫苗：12月6日下午2時至12月7日中午12時。\$\@\$三、 施打時程：12月9日至12月15日。\$\@\$指揮中心說明，預約平臺對象將於12月5日下午2時起，陸續收到提醒簡訊，請記得依預約分流時間進行預約；如為已接種第一劑AZ疫苗之民眾，請依欲選擇之第二劑疫苗種類分流時間，進行預約；預約當日如遇啟動流量管制亦請配合依序排隊耐心等候預約。後續將視疫苗供應期程調整接種場次，籲請民眾屆時準時前往接種。\$\@\$指揮中心提醒，由於10月1日起亦開始接種流感疫苗，依我國衛生福利部傳染病防治諮詢會預防接種組(ACIP)建議，接種流感疫苗應與COVID-19疫苗間隔至少7天，請民眾前往接種COVID-19第二劑疫苗前，應備妥「COVID-19疫苗接種紀錄卡」及健保卡，並於接種前評估時說明過往疫苗接種史，以利醫生評估。\$\@\$此外，未滿18歲對象，請由家長(或法定代理人、監護人及關係人等)陪同前往合約醫療院所或接種站接種，並由本人與家長於現場共同簽署意願同意書；18歲至未滿20歲民眾，如自行前往接種，請持家長簽具之意願同意書，若由家長陪同前往接種，請本人與家長於現場共同簽署意願同意書。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-03\$\@\$中央流行疫情指揮中心今(3)日公布國內新增11例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增11例境外移入個案，為4例男性、7例女性，年齡介於20多歲至40多歲，分別自美國(案16738)、土耳其(案16739)、印尼(4例，案16740-案16742、案16745)、西班牙(案16743)、義大利(案16744)、韓國(案16746)、英國(案16747)及越南(案16748)入境，入境日介於今(2021)年10月24日至12月1日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,507,035例新型冠狀病毒肺炎相關通報(含4,488,710例排除)，其中16,637例確診，分別為1,993例境外移入，14,590例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另累計111例移除為空號。2020年起累計848例COVID-19死亡病例，其中836例本土，個案居住縣市分布為新北市412例、臺北市321例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月3日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-02\$\@\$中央流行疫情指揮中心今(2)日表示，COVID-19變異株Omicron於各國迅速傳播，為積極因應COVID-19病毒變異株對於國內防疫造成之威脅，確保醫療及防疫量能，自即日起提供已完整接種COVID-19疫苗且滿5個月之民眾，追加接種第三劑COVID-19疫苗。\$\@\$指揮中心提醒，目前提供接種之追加劑為莫德納 COVID-19疫苗，依各國核准及接種建議，接種劑量為50微毫克(基礎劑之一半劑量，依目前劑型，注射量為0.25ml)。\$\@\$指揮中心說明，截至今日，已完整接種COVID-19疫苗(不論廠牌)且間隔滿５個月者[即本(2021)年7月2日(含)前已完整接種]，約4.8萬人，依我國COVID-19疫苗接種政策歷程，多為「COVID-19公費疫苗優先接種順序」第一類至第三類對象，包括醫護人員、防疫工作人員、第一線高感染風險工作人員等。為確保高感染風險對象儘速接種第三劑，建議優先接種符合間隔之醫護人員、第一線高感染風險工作人員(包括航空機組員、港埠工作人員、防疫旅宿工作人員等)及因公出國人員；其餘符合間隔之民眾，亦可視感染風險及接種意願，經醫師評估後接種。\$\@\$指揮中心指出，本年11月28日我國「衛生福利部傳染病防治諮詢會預防接種組(ACIP)」專家會議即建議，高風險對象追加接種第三劑COVID-19疫苗，其他18歲以上民眾可評估自身感染風險以及接種意願，經醫師評估後接種；而會中專家亦表示，如遇特殊情況，第二劑與第三劑間隔可縮短至5個月。\$\@\$為因應農曆年節返臺人潮，指揮中心評估國際疫情風險及國內疫苗供應現況，調整第二劑及第三劑間隔為5個月，並自即日起開始提供接種，以及早建立高感染風險人員之免疫保護力。\$\@\$指揮中心強調，目前各國對於追加劑接種廠牌尚無明確建議，惟依據已開始接種追加劑國家之接種現況，以腺病毒載體COVID-19疫苗(包括AstraZeneca 及 Janssen COVID-19 Vaccine)為基礎劑者，可以莫德納 COVID-19疫苗做為追加劑，接種劑量為莫德納 COVID-19疫苗基礎劑之一半劑量。另依據莫德納原廠建議，疫苗瓶裝之膠塞(vial stopper)，每瓶入針不得超過20次，以避免影響疫苗品質，爰若該瓶疫苗開瓶已接種20人劑後，疫苗即丟棄不使用。\$\@\$指揮中心呼籲，為提升COVID-19疫苗接種可近性，指揮中心已協調國軍醫院、衛福部所屬醫院、及退輔會所屬醫療機構即日起加開夜間門診，提供COVID-19疫苗接種服務。民眾除可透過「COVID-19公費疫苗預約平臺」預約接種，亦可至前述院所，或各地方政府衛生局合約醫療院所預約接種。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-02\$\@\$中央流行疫情指揮中心今(2)日公布國內新增17例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增17例境外移入個案，為16例男性、1例女性，年齡介於10多歲至50多歲，分別自美國(2例，案16721、案16736)、波蘭(案16722) 、菲律賓(案16723) 、印尼(6例，案16724-16728、案16737)、緬甸(案16729)、阿拉伯聯合大公國(案16730)、馬來西亞(案16731)、越南(2例，案16732、案16733)、英國(案16734)及義大利(案16735)入境，入境日介於今(2021)年11月17日至11月30日，皆持有搭機前3日內檢驗陰性報告；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,491,850例新型冠狀病毒肺炎相關通報(含4,473,526例排除)，其中16,626例確診，分別為1,982例境外移入，14,590例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另累計111例移除為空號。2020年起累計848例COVID-19死亡病例，其中836例本土，個案居住縣市分布為新北市412例、臺北市321例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月2日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-01\$\@\$中央流行疫情指揮中心今(1)日公布國內新增8例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增8例境外移入個案，為5例男性、3例女性，年齡介於10多歲至40多歲，分別自印尼(5例，案16713、案16716-16718、案16720)、加拿大(案16714)、美國(案16715)及柬埔寨(案16719)入境，入境日介於今(2021)年11月17日至11月29日，皆持有搭機前3日內檢驗陰性報告；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,475,425例新型冠狀病毒肺炎相關通報(含4,457,677例排除)，其中16,609例確診，分別為1,965例境外移入，14,590例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計848例COVID-19死亡病例，其中836例本土，個案居住縣市分布為新北市412例、臺北市321例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月1日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-01\$\@\$中央流行疫情指揮中心今(1)日表示，今(2021)年11月6日晚間抵臺之AstraZeneca COVID-19疫苗第十三批59.4萬劑AstraZeneca COVID-19疫苗，經衛生福利部食品藥物管理署檢驗合格後封緘放行，於11月15日配送至各地方政府衛生局提供民眾接種，已於昨日用罄。指揮中心特別感謝地方政府及醫療院所通力合作，積極調度疫苗，提升國內疫苗涵蓋率。\$\@\$指揮中心表示，截至本年12月1日止，我國COVID-19疫苗第一劑涵蓋率為77.93%，第二劑涵蓋率為56.80%，劑次人口比為134.74 (劑/每百人)。指揮中心再次感謝參與疫苗接種計畫之所有工作人員，包括醫護人員、衛生工作人員、協助運送之航空機組員、疫苗倉儲物流人員等，以及願意前往接種疫苗之每一位民眾。指揮中心將持續推動COVID-19疫苗接種計畫，提升國人疫苗涵蓋率，確保國內防疫安全。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-11-30\$\@\$中央流行疫情指揮中心今(30)日公布國內新增5例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增5例境外移入個案，為5例男性，年齡介於20多歲至40多歲，分別自捷克(案16708)、澳大利亞(3案，案16709-16711)及荷蘭(案16712)入境，入境日介於今(2021)年11月15日至11月29日，皆持有搭機前3日內檢驗陰性報告；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,456,652例新型冠狀病毒肺炎相關通報(含4,438,954例排除)，其中16,601例確診，分別為1,957例境外移入，14,590例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計848例COVID-19死亡病例，其中836例本土，個案居住縣市分布為新北市412例、臺北市321例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$11月30日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-11-30\$\@\$響應聯合國愛滋病規劃署(UNAIDS) 2021世界愛滋病日宣導主題「End inequalities. End AIDS. End pandemics.」，疾管署以「戰勝愛滋，分享愛」作為今年宣導主軸，邀請奧運拳擊國手黃筱雯拍攝宣導影片，透過自身戰勝人生難題之故事，呼籲民眾勇於接受愛滋篩檢，正視愛滋議題，並結合時下流行的網路宣傳平台，推出首支Instagram (IG)濾鏡及Facebook大頭貼特效框活動，邀請民眾一起使用IG濾鏡與Facebook大頭貼特效框，共同響應世界愛滋病日活動，一同關注愛滋防治議題。\$\@\$「戰勝愛滋，分享愛」宣導影片呈現奧運拳擊國手黃筱雯在賽場上面臨挑戰從自我懷疑到正視後戰勝挑戰的心路歷程，鼓勵民眾要正視愛滋議題、勇於接受愛滋篩檢，若感染愛滋病毒也應及早接受治療、達到病毒量測不到之狀態。\$\@\$疾管署持續結合相關部會、地方政府、醫療機關及民間團體等各界資源，全面推動各項愛滋防治工作，我國愛滋疫情自2018年起，已連續4年呈現下降趨勢，2021年截至11月24日新通報感染人數為1,139人，與2020年同期相較亦下降11%。此外，UNAIDS訂定之2020年達成「90-90-90」目標（90%感染者知道自己之感染狀態、90%感染者有服藥、90%服藥之感染者病毒量達測不到），全球達成值為「84-87-90」，我國則為「90-93-95」。並自2022年起推動「2030年消除愛滋第一期計畫(2022-2026)」，以達UNAIDS下一階段「95-95-95」目標努力。\$\@\$同時呼籲各界築起戰勝愛滋之4道防線：\$\@\$第1道-安全性行為：落實性行為時，全程正確使用保險套及水性潤滑液。\$\@\$第2道-暴露愛滋病毒前預防性投藥(PrEP)：感染風險族群在暴露於感染愛滋風險前，透過服用藥物，讓體內有足夠的藥物濃度以預防愛滋病毒感染，保護效果可達90%以上。\$\@\$第3道-定期篩檢愛滋：可藉由疾管署提供之多元篩檢管道，包括自我篩檢或匿名篩檢，鼓勵有性行為者，至少進行1次篩檢；有無套性行為者，每年至少進行1次篩檢；若有感染風險行為(如多重性伴侶、合併使用成癮性藥物、感染性病等) ，每3至6個月篩檢1次。\$\@\$第4道-及早治療，控制病毒量：診斷即刻治療，使感染者維持在病毒量測不到狀態，可預防透過性行為傳播，亦大大降低社區傳染風險。\$\@\$更多相關資訊，可透過疾管家Line@於本年12月1日上線之「性健康友善資源地圖」或疾病管制署全球資訊網(https://www.cdc.gov.tw)查詢。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-11-29\$\@\$中央流行疫情指揮中心今(29)日表示，為因應新型變異株Omicron於全球日益擴散且其傳播力強，考量馬拉威、莫三比克、埃及、奈及利亞等4國已有個案輸入他國，且評估其國內疫情有擴散趨勢，研判風險較高，自今(2021)年12月1日零時(航機抵臺時間)起，增列前述4國為「重點高風險國家」，如過去14天有前述4國旅遊史(含轉機)者，入境後均應至集中檢疫所進行14天檢疫，且配合專案採檢(到所、期滿)及續行7天自主健康管理(第6-7天公費家用快篩1次)，上述旅客不需支付集中檢疫所及採檢費用，亦不適用7+7+7、10+4+7之春節專案。此外，國籍航空公司機組員若自「重點高風險國家」航線航班(含轉機)返臺後，應入住防疫旅宿或符合規定之公司宿舍檢疫14天，且配合入境、檢疫期滿進行PCR檢測，並續行7天自主健康管理。\$\@\$指揮中心指出，現行「重點高風險國家」為南非、波札那、納米比亞、賴索托、史瓦帝尼、辛巴威及本次新增馬拉威、莫三比克、埃及、奈及利亞，共10國。\$\@\$指揮中心強調，邊境管制為防範COVID-19疫情的重要關鍵，入境旅客抵臺時應主動配合邊境檢疫措施，並依指揮中心規定的交通方式前往檢疫地點及配合後續防疫相關措施。落實全民共同抗疫，將疫情阻絕於境外，以降低該病毒進入我國社區之風險。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-11-29\$\@\$中央流行疫情指揮中心今(29)日公布國內新增8例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增8例境外移入個案，為7例男性、1例女性，年齡介於10多歲至60多歲，分別自越南(4例，案16700-16703)、印尼(案16704)、柬埔寨(2案，案16705、16706)及美國(案16707)入境，入境日介於今(2021)年11月15日至11月26日，皆持有搭機前3日內檢驗陰性報告；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,439,574例新型冠狀病毒肺炎相關通報(含4,421,667例排除)，其中16,596例確診，分別為1,952例境外移入，14,590例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計848例COVID-19死亡病例，其中836例本土，個案居住縣市分布為新北市412例、臺北市321例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$11月29日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-11-29\$\@\$中央流行疫情指揮中心今(29)日表示，昨(28)日經我國「衛生福利部傳染病防治諮詢會預防接種組(ACIP)」專家會議討論，為提升社區群體免疫力，確保國內防疫安全，國人應按時程接種第二劑COVID-19疫苗，並建議已接種第1劑BioNTech COVID-19疫苗(以下簡稱BNT疫苗)且無發生嚴重不良反應之12-17歲青少年族群，接種第2劑BNT疫苗，並建議兩劑間隔12週以上。後續將由指揮中心與地方政府衛生局規劃安排於校園接種。\$\@\$指揮中心指出，會中經專家審慎檢視各國青少年族群COVID-19感染、傳播與重症風險、mRNA COVID-19疫苗(包括BNT 及Moderna)接種策略、疫苗接種後心肌炎發生率與相關文獻，並分析國內青少年接種BNT疫苗後心肌炎/心包膜炎發生率、個案病程與恢復情形，雖然mRNA疫苗接種後發生之心肌炎/心包膜炎，可能與疫苗接種有關，惟考量COVID-19病毒變異株持續於國際間流行，且農曆春節即將到來，為降低境外移入個案造成國內社區流行之風險，應積極提升各類對象第二劑接種率，提升群體免疫力，故建議12-17歲青少年完成兩劑BNT疫苗接種。另評估現行雖尚無研究證實兩劑接種間隔與接種疫苗後心肌炎/心包膜炎發生率之關聯性，然依據目前疫苗間隔與保護力實證研究結果，及英國、歐盟、加拿大等國之監測與建議，專家建議12-17歲青少年兩劑BNT疫苗間隔為12週以上。\$\@\$指揮中心說明，依據各國上市後監測數據，接種BNT疫苗會出現極罕見的心肌炎/心包膜炎病例，這些病例主要發生在接種後14天內，亦有極少數個案發生於接種後2週至4週間；接種第二劑後發生心肌炎/心包膜炎之比率高於第一劑，且年輕男性發生比例較女性以及其他男性年齡層高。指揮中心特別提醒，民眾於接種BNT疫苗後28天內，如出現下列任一疑似心肌炎或心包膜炎的症狀，包括胸痛、胸口壓迫感或不適、心悸(心跳不規則、跳拍或「顫動」)、暈厥（昏厥）、呼吸急促、運動耐受不良（例如走幾步路就會很喘、沒有力氣爬樓梯）等，應立即就醫。並於就醫時告知醫師相關症狀、症狀發生時間、疫苗接種時間，以做為診斷參考。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-11-29\$\@\$中央流行疫情指揮中心今(29)日表示，昨(28)日我國「衛生福利部傳染病防治諮詢會預防接種組(ACIP)」專家會議建議，考量COVID-19疫苗接種後之免疫保護力可能隨時間下降，為積極因應COVID-19病毒變異株對於國內防疫造成之威脅，降低COVID-19疫苗感染與感染後重症風險，建議已完成2劑COVID-19疫苗接種之65歲以上長者、長照機構住民與工作者、醫護人員、防疫工作人員、第一線高感染風險工作人員及容易感染與疾病嚴重風險者(即COVID-19疫苗公費接種對象第九類)，應於第二劑COVID-19疫苗接種6個月後，追加接種第三劑COVID-19疫苗，其他滿18歲以上民眾可以評估自身感染風險以及接種意願，經醫師評估後接種第三劑COVID-19疫苗，提升保護力。\$\@\$指揮中心說明，會中經專家檢視目前國外COVID-19疫苗接種後保護力追蹤情形及各國追加劑接種政策與接種實務作業，評估雖完成兩劑COVID-19疫苗後可以快速提升免疫保護力，有效預防COVID-19病毒感染、及感染後重症與死亡風險，惟疫苗保護力會隨著接種時間逐續下降，加以COVID-19病毒不斷變異，即便完成兩劑疫苗後，仍有突破性感染(breakthrough infection)之風險，故建議完成兩劑疫苗接種之民眾，應於第二劑接種6個月後，追加接種第三劑COVID-19疫苗。\$\@\$指揮中心指出，目前國外各國對於追加劑接種廠牌尚無明確建議，指揮中心將持續收集國內外相關臨床實驗與研究數據以及各國接種建議，並視國內疫苗接種與供應情形，規劃接種作業後，再提供民眾進行接種。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-11-29\$\@\$國內疫情趨緩且穩定控制，中央流行疫情指揮中心經與相關單位溝通討論及評估後，於今(29)日宣布，自今(2021)年11月30日至12月13日維持疫情警戒標準為第二級，並維持相關措施及規定如下：\$\@\$一、維持現行戴口罩規定，外出時應全程佩戴口罩，但符合以下情形，得免戴口罩(本次未調整)：\$\@\$(一)下列場合得免戴口罩，但應隨身攜帶口罩，且如本身有相關症狀或與不特定對象無法保持社交距離時，仍應戴口罩：\$\@\$1.於室內外從事運動、唱歌時。\$\@\$2.於室內外拍攝個人/團體照時。\$\@\$3.單人或多人進行直播、錄影、主持、報導、致詞、演講、講課等談話性質工作或活動之正式拍攝或進行時。\$\@\$4.農林漁牧工作者於空曠處(如：田間、魚塭、山林)工作。\$\@\$5.於山林(含森林遊樂區)、海濱活動。\$\@\$6.於溫/冷泉、烤箱、水療設施、三溫暖、蒸氣室、水域活動等易使口罩潮濕之場合。\$\@\$(二)外出時有飲食需求，得免戴口罩。\$\@\$(三)於指揮中心或主管機關指定之場所或活動，如符合相關防疫措施，得暫時脫下口罩。\$\@\$二、營業場所及公共場域維持應遵守實聯制、量體溫、加強環境清消、員工健康管理、確診事件即時應變。\$\@\$指揮中心指出，因應國際間新變異株Omicron威脅，相關大型活動具有人潮擁擠、長時間且近距離接觸不特定人士的特性，仍應維持嚴格防疫管理並加嚴裁處，請主辦單位及民眾務必遵守下列防疫準備注意事項：\$\@\$一、主辦單位應遵守指揮中心二級警戒公告措施、地方政府大型活動相關防疫規定：\$\@\$(一)主辦單位應於活動場域提供足量手部清消用品、提高公共廁所之消毒頻率並設有醫療應變措施。\$\@\$(二)除指定販賣區外，場內不得販售飲食。\$\@\$(三)室內活動不得販售無座位票，須落實實聯制，規劃固定入口，且於入口處進行體溫量測及手部消毒。\$\@\$二、活動期間應全程佩戴口罩，除補充水分外，禁止飲食。\$\@\$(一)除主持、表演及致詞人員得於正式拍攝或進行時免戴口罩，其餘人員及參加活動者不適用飲食(補充水分除外)、拍照等得免戴口罩之例外情形。\$\@\$(二)主辦單位經地方政府同意，得設置專屬飲食區域供民眾脫口罩飲食，該區域須落實實聯制、入口體溫量測及手部消毒，並不得邊走邊吃，亦不開放試吃。\$\@\$(三)違反以上規定、經工作人員勸導不聽者，由地方政府依傳染病防治法裁罰。\$\@\$三、居家檢疫、居家隔離、(加強)自主健康管理者，及有發燒、呼吸道症狀、腹瀉、嗅味覺異常等疑似症狀之民眾(包括表演者及活動工作人員)，不得參加相關活動。違反者將從重處罰。\$\@\$指揮中心將視國內外疫情及實際執行狀況，適時機動調整防疫措施，強化邊境監測及防疫作為。籲請民眾應落實個人防護措施，主動積極配合各項防疫措施，以兼顧防疫與生活品質。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-11-28\$\@\$中央流行疫情指揮中心今(28)日公布國內新增10例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增10例境外移入個案，為7例男性、3例女性，年齡介於10多歲至30多歲，分別自美國(案16690)、越南(4例，案16691、案16692、案16697、案16699)、印尼(3案，案16693、案16696、案16698)、阿拉伯聯合大公國(案16694)及菲律賓(案16695)入境，入境日介於今(2021)年11月25日至11月26日，皆持有搭機前3日內檢驗陰性報告；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,426,033例新型冠狀病毒肺炎相關通報(含4,407,812例排除)，其中16,588例確診，分別為1,944例境外移入，14,590例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另累計111例移除為空號。2020年起累計848例COVID-19死亡病例，其中836例本土，個案居住縣市分布為新北市412例、臺北市321例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$11月28日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-11-27\$\@\$中央流行疫情指揮中心今(27)日公布國內新增12例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增12例境外移入個案，為8例男性、4例女性，年齡介於10多歲至60多歲，分別自衣索比亞(3例，案16678-16680)、印尼(4例、案16681-16684)、越南(2例，案16685-16686)、印度(案16687)、美國(案16688)及韓國(案16689)入境，入境日介於今(2021)年11月12日至11月25日，皆持有搭機前3日內檢驗陰性報告；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,411,374例新型冠狀病毒肺炎相關通報(含4,393,040例排除)，其中16,578例確診，分別為1,934例境外移入，14,590例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另累計111例移除為空號。2020年起累計848例COVID-19死亡病例，其中836例本土，個案居住縣市分布為新北市412例、臺北市321例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$11月27日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
 </sst>
 </file>
@@ -994,7 +1417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1022,16 +1445,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2">
         <v>44569</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>116</v>
+        <v>168</v>
       </c>
       <c r="E2" t="s">
-        <v>172</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1039,16 +1462,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C3" s="2">
         <v>44568</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>117</v>
+        <v>169</v>
       </c>
       <c r="E3" t="s">
-        <v>173</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1056,13 +1479,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="C4" s="2">
         <v>44568</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>118</v>
+        <v>170</v>
+      </c>
+      <c r="E4" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1070,13 +1496,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="C5" s="2">
         <v>44567</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>119</v>
+        <v>171</v>
+      </c>
+      <c r="E5" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1084,13 +1513,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C6" s="2">
         <v>44567</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>120</v>
+        <v>172</v>
+      </c>
+      <c r="E6" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1098,16 +1530,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="C7" s="2">
         <v>44567</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>121</v>
+        <v>173</v>
       </c>
       <c r="E7" t="s">
-        <v>174</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1115,16 +1547,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="C8" s="2">
-        <v>44387</v>
+        <v>44566</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>122</v>
+        <v>174</v>
       </c>
       <c r="E8" t="s">
-        <v>175</v>
+        <v>264</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1132,16 +1564,16 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="C9" s="2">
-        <v>44360</v>
+        <v>44566</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>123</v>
+        <v>175</v>
       </c>
       <c r="E9" t="s">
-        <v>176</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1149,16 +1581,16 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="C10" s="2">
-        <v>44359</v>
+        <v>44566</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>124</v>
+        <v>176</v>
       </c>
       <c r="E10" t="s">
-        <v>177</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1166,13 +1598,13 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="C11" s="2">
-        <v>44348</v>
+        <v>44565</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>125</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1180,13 +1612,16 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="C12" s="2">
-        <v>44344</v>
+        <v>44565</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>126</v>
+        <v>178</v>
+      </c>
+      <c r="E12" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1194,16 +1629,16 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="C13" s="2">
-        <v>44341</v>
+        <v>44565</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>127</v>
+        <v>179</v>
       </c>
       <c r="E13" t="s">
-        <v>178</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1211,16 +1646,16 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C14" s="2">
-        <v>44567</v>
+        <v>44564</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>128</v>
+        <v>180</v>
       </c>
       <c r="E14" t="s">
-        <v>179</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1228,13 +1663,16 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="C15" s="2">
-        <v>44567</v>
+        <v>44564</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>129</v>
+        <v>181</v>
+      </c>
+      <c r="E15" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1242,13 +1680,16 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="C16" s="2">
-        <v>44560</v>
+        <v>44563</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>130</v>
+        <v>182</v>
+      </c>
+      <c r="E16" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1256,13 +1697,16 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="C17" s="2">
-        <v>44491</v>
+        <v>44562</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>131</v>
+        <v>183</v>
+      </c>
+      <c r="E17" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1270,13 +1714,16 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="C18" s="2">
-        <v>44469</v>
+        <v>44561</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>132</v>
+        <v>184</v>
+      </c>
+      <c r="E18" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1284,13 +1731,16 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="C19" s="2">
-        <v>44467</v>
+        <v>44561</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>133</v>
+        <v>185</v>
+      </c>
+      <c r="E19" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1298,13 +1748,16 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="C20" s="2">
-        <v>44568</v>
+        <v>44560</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>134</v>
+        <v>186</v>
+      </c>
+      <c r="E20" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1312,13 +1765,13 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="C21" s="2">
-        <v>44567</v>
+        <v>44560</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>135</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1326,13 +1779,16 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="C22" s="2">
-        <v>44567</v>
+        <v>44560</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>136</v>
+        <v>188</v>
+      </c>
+      <c r="E22" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1340,13 +1796,16 @@
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="C23" s="2">
-        <v>44566</v>
+        <v>44560</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>137</v>
+        <v>189</v>
+      </c>
+      <c r="E23" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1354,13 +1813,16 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="C24" s="2">
-        <v>44566</v>
+        <v>44559</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>138</v>
+        <v>190</v>
+      </c>
+      <c r="E24" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1368,13 +1830,16 @@
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="C25" s="2">
-        <v>44566</v>
+        <v>44558</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>139</v>
+        <v>191</v>
+      </c>
+      <c r="E25" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1382,13 +1847,16 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="C26" s="2">
-        <v>44568</v>
+        <v>44557</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>140</v>
+        <v>192</v>
+      </c>
+      <c r="E26" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1396,145 +1864,169 @@
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="C27" s="2">
-        <v>44568</v>
+        <v>44557</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>141</v>
+        <v>193</v>
+      </c>
+      <c r="E27" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="C28" s="2">
-        <v>44568</v>
+        <v>44557</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>142</v>
+        <v>194</v>
+      </c>
+      <c r="E28" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="C29" s="2">
-        <v>44567</v>
+        <v>44557</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>143</v>
+        <v>195</v>
+      </c>
+      <c r="E29" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="C30" s="2">
-        <v>44566</v>
+        <v>44557</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>144</v>
+        <v>196</v>
+      </c>
+      <c r="E30" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="C31" s="2">
-        <v>44566</v>
+        <v>44557</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>145</v>
+        <v>197</v>
+      </c>
+      <c r="E31" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C32" s="2">
-        <v>44554</v>
+        <v>44556</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>146</v>
+        <v>198</v>
       </c>
       <c r="E32" t="s">
-        <v>180</v>
+        <v>286</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="C33" s="2">
-        <v>44554</v>
+        <v>44555</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>147</v>
+        <v>199</v>
+      </c>
+      <c r="E33" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="C34" s="2">
-        <v>44550</v>
+        <v>44555</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>148</v>
+        <v>200</v>
       </c>
       <c r="E34" t="s">
-        <v>181</v>
+        <v>288</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C35" s="2">
-        <v>44515</v>
+        <v>44554</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>149</v>
+        <v>201</v>
+      </c>
+      <c r="E35" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="C36" s="2">
-        <v>44496</v>
+        <v>44554</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>150</v>
+        <v>202</v>
+      </c>
+      <c r="E36" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1542,13 +2034,16 @@
         <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="C37" s="2">
-        <v>44494</v>
+        <v>44553</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>151</v>
+        <v>203</v>
+      </c>
+      <c r="E37" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1556,16 +2051,16 @@
         <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="C38" s="2">
-        <v>44565</v>
+        <v>44553</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>152</v>
+        <v>204</v>
       </c>
       <c r="E38" t="s">
-        <v>182</v>
+        <v>292</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1573,847 +2068,891 @@
         <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C39" s="2">
-        <v>44565</v>
+        <v>44552</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>153</v>
+        <v>205</v>
       </c>
       <c r="E39" t="s">
-        <v>183</v>
+        <v>293</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="C40" s="2">
-        <v>44564</v>
+        <v>44552</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>154</v>
+        <v>206</v>
       </c>
       <c r="E40" t="s">
-        <v>184</v>
+        <v>294</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="C41" s="2">
-        <v>44564</v>
+        <v>44551</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>155</v>
+        <v>207</v>
       </c>
       <c r="E41" t="s">
-        <v>185</v>
+        <v>295</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="C42" s="2">
-        <v>44563</v>
+        <v>44551</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>156</v>
+        <v>208</v>
+      </c>
+      <c r="E42" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="C43" s="2">
-        <v>44562</v>
+        <v>44551</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>157</v>
+        <v>209</v>
       </c>
       <c r="E43" t="s">
-        <v>186</v>
+        <v>297</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="C44" s="2">
-        <v>44561</v>
+        <v>44551</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>158</v>
+        <v>210</v>
       </c>
       <c r="E44" t="s">
-        <v>187</v>
+        <v>298</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="C45" s="2">
-        <v>44561</v>
+        <v>44550</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>159</v>
+        <v>211</v>
+      </c>
+      <c r="E45" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="C46" s="2">
-        <v>44560</v>
+        <v>44550</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>160</v>
+        <v>212</v>
       </c>
       <c r="E46" t="s">
-        <v>188</v>
+        <v>300</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="C47" s="2">
-        <v>44560</v>
+        <v>44550</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>161</v>
+        <v>213</v>
       </c>
       <c r="E47" t="s">
-        <v>189</v>
+        <v>301</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="C48" s="2">
-        <v>44560</v>
+        <v>44549</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>162</v>
+        <v>214</v>
+      </c>
+      <c r="E48" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B49" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="C49" s="2">
-        <v>44560</v>
+        <v>44548</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>163</v>
+        <v>215</v>
       </c>
       <c r="E49" t="s">
-        <v>190</v>
+        <v>303</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="C50" s="2">
-        <v>44559</v>
+        <v>44547</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="E50" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="C51" s="2">
-        <v>44558</v>
+        <v>44546</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>165</v>
+        <v>217</v>
       </c>
       <c r="E51" t="s">
-        <v>192</v>
+        <v>304</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="C52" s="2">
-        <v>44557</v>
+        <v>44546</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>166</v>
+        <v>218</v>
+      </c>
+      <c r="E52" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="C53" s="2">
-        <v>44557</v>
+        <v>44545</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>167</v>
+        <v>219</v>
+      </c>
+      <c r="E53" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B54" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="C54" s="2">
-        <v>44557</v>
+        <v>44544</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>168</v>
+        <v>220</v>
       </c>
       <c r="E54" t="s">
-        <v>193</v>
+        <v>307</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="C55" s="2">
-        <v>44557</v>
+        <v>44543</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>169</v>
+        <v>221</v>
+      </c>
+      <c r="E55" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="C56" s="2">
-        <v>44557</v>
+        <v>44543</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>170</v>
+        <v>222</v>
       </c>
       <c r="E56" t="s">
-        <v>194</v>
+        <v>309</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="C57" s="2">
-        <v>44557</v>
+        <v>44543</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>171</v>
+        <v>223</v>
+      </c>
+      <c r="E57" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="B58" t="s">
-        <v>60</v>
+        <v>134</v>
       </c>
       <c r="C58" s="2">
-        <v>44569</v>
+        <v>44542</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>116</v>
+        <v>224</v>
       </c>
       <c r="E58" t="s">
-        <v>172</v>
+        <v>311</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="B59" t="s">
-        <v>61</v>
+        <v>135</v>
       </c>
       <c r="C59" s="2">
-        <v>44568</v>
+        <v>44541</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>117</v>
+        <v>225</v>
+      </c>
+      <c r="E59" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>62</v>
+        <v>136</v>
       </c>
       <c r="C60" s="2">
-        <v>44568</v>
+        <v>44540</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>118</v>
+        <v>226</v>
       </c>
       <c r="E60" t="s">
-        <v>195</v>
+        <v>313</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B61" t="s">
-        <v>63</v>
+        <v>137</v>
       </c>
       <c r="C61" s="2">
-        <v>44567</v>
+        <v>44540</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>119</v>
+        <v>227</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B62" t="s">
-        <v>64</v>
+        <v>138</v>
       </c>
       <c r="C62" s="2">
-        <v>44567</v>
+        <v>44539</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>120</v>
+        <v>228</v>
       </c>
       <c r="E62" t="s">
-        <v>196</v>
+        <v>314</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="B63" t="s">
-        <v>65</v>
+        <v>139</v>
       </c>
       <c r="C63" s="2">
-        <v>44567</v>
+        <v>44539</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>121</v>
+        <v>229</v>
       </c>
       <c r="E63" t="s">
-        <v>174</v>
+        <v>315</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="B64" t="s">
-        <v>66</v>
+        <v>140</v>
       </c>
       <c r="C64" s="2">
-        <v>44387</v>
+        <v>44539</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>122</v>
+        <v>230</v>
+      </c>
+      <c r="E64" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B65" t="s">
-        <v>67</v>
+        <v>141</v>
       </c>
       <c r="C65" s="2">
-        <v>44360</v>
+        <v>44539</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>123</v>
+        <v>231</v>
       </c>
       <c r="E65" t="s">
-        <v>176</v>
+        <v>317</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="B66" t="s">
-        <v>68</v>
+        <v>142</v>
       </c>
       <c r="C66" s="2">
-        <v>44359</v>
+        <v>44539</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>124</v>
+        <v>232</v>
       </c>
       <c r="E66" t="s">
-        <v>177</v>
+        <v>318</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="B67" t="s">
-        <v>69</v>
+        <v>143</v>
       </c>
       <c r="C67" s="2">
-        <v>44348</v>
+        <v>44538</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>125</v>
+        <v>233</v>
       </c>
       <c r="E67" t="s">
-        <v>197</v>
+        <v>319</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="B68" t="s">
-        <v>70</v>
+        <v>144</v>
       </c>
       <c r="C68" s="2">
-        <v>44344</v>
+        <v>44538</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>126</v>
+        <v>234</v>
       </c>
       <c r="E68" t="s">
-        <v>198</v>
+        <v>320</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="B69" t="s">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="C69" s="2">
-        <v>44341</v>
+        <v>44538</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>127</v>
+        <v>235</v>
       </c>
       <c r="E69" t="s">
-        <v>178</v>
+        <v>321</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="B70" t="s">
-        <v>72</v>
+        <v>146</v>
       </c>
       <c r="C70" s="2">
-        <v>44567</v>
+        <v>44537</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>128</v>
+        <v>236</v>
       </c>
       <c r="E70" t="s">
-        <v>179</v>
+        <v>322</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B71" t="s">
-        <v>73</v>
+        <v>147</v>
       </c>
       <c r="C71" s="2">
-        <v>44567</v>
+        <v>44537</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>129</v>
+        <v>237</v>
+      </c>
+      <c r="E71" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B72" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="C72" s="2">
-        <v>44560</v>
+        <v>44536</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>130</v>
+        <v>238</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="B73" t="s">
-        <v>75</v>
+        <v>149</v>
       </c>
       <c r="C73" s="2">
-        <v>44491</v>
+        <v>44535</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>131</v>
+        <v>239</v>
+      </c>
+      <c r="E73" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B74" t="s">
-        <v>76</v>
+        <v>150</v>
       </c>
       <c r="C74" s="2">
-        <v>44469</v>
+        <v>44535</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>132</v>
+        <v>240</v>
+      </c>
+      <c r="E74" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="B75" t="s">
-        <v>77</v>
+        <v>151</v>
       </c>
       <c r="C75" s="2">
-        <v>44467</v>
+        <v>44535</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>133</v>
+        <v>241</v>
       </c>
       <c r="E75" t="s">
-        <v>199</v>
+        <v>326</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="B76" t="s">
-        <v>78</v>
+        <v>152</v>
       </c>
       <c r="C76" s="2">
-        <v>44568</v>
+        <v>44534</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>134</v>
+        <v>242</v>
+      </c>
+      <c r="E76" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B77" t="s">
-        <v>79</v>
+        <v>153</v>
       </c>
       <c r="C77" s="2">
-        <v>44567</v>
+        <v>44534</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>135</v>
+        <v>243</v>
+      </c>
+      <c r="E77" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="B78" t="s">
-        <v>80</v>
+        <v>154</v>
       </c>
       <c r="C78" s="2">
-        <v>44567</v>
+        <v>44533</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>136</v>
+        <v>244</v>
+      </c>
+      <c r="E78" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="B79" t="s">
-        <v>81</v>
+        <v>155</v>
       </c>
       <c r="C79" s="2">
-        <v>44566</v>
+        <v>44532</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>137</v>
+        <v>245</v>
+      </c>
+      <c r="E79" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="B80" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
       <c r="C80" s="2">
-        <v>44566</v>
+        <v>44532</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>138</v>
+        <v>246</v>
+      </c>
+      <c r="E80" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="B81" t="s">
-        <v>83</v>
+        <v>157</v>
       </c>
       <c r="C81" s="2">
-        <v>44566</v>
+        <v>44531</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>139</v>
+        <v>247</v>
+      </c>
+      <c r="E81" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="B82" t="s">
-        <v>84</v>
+        <v>158</v>
       </c>
       <c r="C82" s="2">
-        <v>44568</v>
+        <v>44531</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>140</v>
+        <v>248</v>
+      </c>
+      <c r="E82" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B83" t="s">
-        <v>85</v>
+        <v>159</v>
       </c>
       <c r="C83" s="2">
-        <v>44568</v>
+        <v>44530</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>141</v>
+        <v>249</v>
+      </c>
+      <c r="E83" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="B84" t="s">
-        <v>86</v>
+        <v>160</v>
       </c>
       <c r="C84" s="2">
-        <v>44568</v>
+        <v>44530</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>142</v>
+        <v>250</v>
+      </c>
+      <c r="E84" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="B85" t="s">
-        <v>87</v>
+        <v>161</v>
       </c>
       <c r="C85" s="2">
-        <v>44567</v>
+        <v>44529</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>143</v>
+        <v>251</v>
+      </c>
+      <c r="E85" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="B86" t="s">
-        <v>88</v>
+        <v>162</v>
       </c>
       <c r="C86" s="2">
-        <v>44566</v>
+        <v>44529</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>144</v>
+        <v>252</v>
+      </c>
+      <c r="E86" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="B87" t="s">
-        <v>89</v>
+        <v>163</v>
       </c>
       <c r="C87" s="2">
-        <v>44566</v>
+        <v>44529</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>145</v>
+        <v>253</v>
+      </c>
+      <c r="E87" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="B88" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
       <c r="C88" s="2">
-        <v>44554</v>
+        <v>44529</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>146</v>
+        <v>254</v>
+      </c>
+      <c r="E88" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="B89" t="s">
-        <v>91</v>
+        <v>165</v>
       </c>
       <c r="C89" s="2">
-        <v>44554</v>
+        <v>44529</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>147</v>
+        <v>255</v>
       </c>
       <c r="E89" t="s">
-        <v>200</v>
+        <v>340</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B90" t="s">
-        <v>92</v>
+        <v>166</v>
       </c>
       <c r="C90" s="2">
-        <v>44550</v>
+        <v>44528</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>148</v>
+        <v>256</v>
       </c>
       <c r="E90" t="s">
-        <v>181</v>
+        <v>341</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="B91" t="s">
-        <v>93</v>
+        <v>167</v>
       </c>
       <c r="C91" s="2">
-        <v>44515</v>
+        <v>44527</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>149</v>
+        <v>257</v>
       </c>
       <c r="E91" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
-      <c r="A92" t="s">
-        <v>38</v>
-      </c>
-      <c r="B92" t="s">
-        <v>94</v>
-      </c>
-      <c r="C92" s="2">
-        <v>44496</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5">
-      <c r="A93" t="s">
-        <v>39</v>
-      </c>
-      <c r="B93" t="s">
-        <v>95</v>
-      </c>
-      <c r="C93" s="2">
-        <v>44494</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>151</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -2508,8 +3047,6 @@
     <hyperlink ref="D89" r:id="rId88"/>
     <hyperlink ref="D90" r:id="rId89"/>
     <hyperlink ref="D91" r:id="rId90"/>
-    <hyperlink ref="D92" r:id="rId91"/>
-    <hyperlink ref="D93" r:id="rId92"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20220122
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -31,6 +31,9 @@
     <t>Page Content</t>
   </si>
   <si>
+    <t>新增130例COVID-19確定病例，分別為82例本土及48例境外移入</t>
+  </si>
+  <si>
     <t>新增68例COVID-19確定病例，分別為23例本土及45例境外移入</t>
   </si>
   <si>
@@ -58,7 +61,10 @@
     <t>新增66例COVID-19確定病例，分別為17例本土及49例境外移入</t>
   </si>
   <si>
-    <t>新增65例COVID-19確定病例，分別為17例本土及48例境外移入</t>
+    <t>COVID-19公費疫苗預約平台自1月18日起，提供已完整接種兩劑COVID-19疫苗滿12週且滿18歲以上民眾，預約接種追加劑</t>
+  </si>
+  <si>
+    <t>新增51例COVID-19確定病例，分別為10例本土及41例境外移入</t>
   </si>
   <si>
     <t>新增78例COVID-19確定病例，分別為6例本土及72例境外移入</t>
@@ -115,10 +121,7 @@
     <t>新增62例COVID-19確定病例，分別為4例本土及58例境外移入</t>
   </si>
   <si>
-    <t>新增43例COVID-19確定病例，分別為3例本土及40例境外移入</t>
-  </si>
-  <si>
-    <t>呼籲長者及其他 COVID-19感染後容易產生嚴重併發症之族群，儘速完成疫苗基礎劑接種</t>
+    <t>/Bulletin/Detail/5MtrgzOJApOSjivffWLWRw?typeid=9</t>
   </si>
   <si>
     <t>/Bulletin/Detail/cdBM6ZsvZ-djQZ8je9OYkg?typeid=9</t>
@@ -148,7 +151,10 @@
     <t>/Bulletin/Detail/5XT_6l4aNN_OQfb208cYtg?typeid=9</t>
   </si>
   <si>
-    <t>/Bulletin/Detail/rkvMm-Hng9jJHKRdCEXvDg?typeid=9</t>
+    <t>/Bulletin/Detail/sKXQ2hw4AvLbte5bgT1zPQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/yryfZDzFpd5okqzaJbqiFw?typeid=9</t>
   </si>
   <si>
     <t>/Bulletin/Detail/u_qQ9mEWekb8f6zoUpXeKA?typeid=9</t>
@@ -205,10 +211,7 @@
     <t>/Bulletin/Detail/szV5W2pK70cBBVpTxxghzw?typeid=9</t>
   </si>
   <si>
-    <t>/Bulletin/Detail/09VZRAwn1bOg97wX7spbLw?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/Vwd8It8AE16rPEuotcXK9Q?typeid=9</t>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/5MtrgzOJApOSjivffWLWRw?typeid=9</t>
   </si>
   <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/cdBM6ZsvZ-djQZ8je9OYkg?typeid=9</t>
@@ -238,7 +241,10 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/5XT_6l4aNN_OQfb208cYtg?typeid=9</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/rkvMm-Hng9jJHKRdCEXvDg?typeid=9</t>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/sKXQ2hw4AvLbte5bgT1zPQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/yryfZDzFpd5okqzaJbqiFw?typeid=9</t>
   </si>
   <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/u_qQ9mEWekb8f6zoUpXeKA?typeid=9</t>
@@ -295,10 +301,7 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/szV5W2pK70cBBVpTxxghzw?typeid=9</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/09VZRAwn1bOg97wX7spbLw?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/Vwd8It8AE16rPEuotcXK9Q?typeid=9</t>
+    <t>發佈日期：2022-01-22\$\@\$中央流行疫情指揮中心今(22)日公布國內新增130例COVID-19確定病例，分別為82例本土個案及48例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為12例男性、70例女性，年齡介於未滿10歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為29例男性、19例女性，年齡介於未滿5歲至70多歲，分別自美國(13例)、加拿大及新加坡(各4例)、菲律賓(3例)、印度、土耳其及香港(各2例)、奧地利、奈及利亞、義大利、柬埔寨、德國、越南及巴西(各1例)移入；另11例調查中。入境日介於去(2021)年12月31日至今(2022)年1月21日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,418,957例新型冠狀病毒肺炎相關通報(含5,400,086例排除)，其中18,238例確診，分別為3,331例境外移入，14,853例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案18182，再次採檢為陰性，改判排除)，累計117例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月22日新增本土COVID-19確診個案表.pdf\$\@\$1月22日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
     <t>發佈日期：2022-01-21\$\@\$中央流行疫情指揮中心今(21)日公布國內新增68例COVID-19確定病例，分別為23例本土個案及45例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為10例男性、13例女性，年齡介於未滿10歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為20例男性、24例女性及1例調查中，年齡介於未滿5歲至70多歲，分別自美國(17例)、菲律賓(4例)、越南及以色列(各3例)、加拿大(2例)、波蘭、澳大利亞、韓國、新加坡、瑞典、俄羅斯、英國及愛爾蘭(各1例)移入；另8例調查中。入境日介於今(2022)年1月5日至1月20日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,394,042例新型冠狀病毒肺炎相關通報(含5,375,246例排除)，其中18,109例確診，分別為3,283例境外移入，14,772例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計116例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月21日新增本土COVID-19確診個案表.pdf\$\@\$1月21日新增境外移入COVID-19確診個案表.pdf</t>
@@ -328,7 +331,10 @@
     <t>發佈日期：2022-01-18\$\@\$中央流行疫情指揮中心今(18)日公布國內新增66例COVID-19確定病例，分別為17例本土個案及49例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為10例男性、7例女性，年齡介於未滿5歲至60多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為33例男性、16例女性，年齡介於未滿10歲至60多歲，分別自美國(21例)、越南(5例)、加拿大(4例)、英國(3例)、法國(2例)、愛爾蘭、西班牙、瑞典、菲律賓、波蘭、墨西哥及巴拿馬(各1例)移入；另7例調查中。入境日介於今(2022)年1月3日至1月17日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,306,453例新型冠狀病毒肺炎相關通報(含5,287,815例排除)，其中17,951例確診，分別為3,171例境外移入，14,726例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計115例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月18日新增本土COVID-19確診個案表.pdf\$\@\$1月18日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-17\$\@\$中央流行疫情指揮中心今(17)日公布國內新增65例COVID-19確定病例，分別為17例本土個案及48例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為8例男性、9例女性，年齡介於未滿5歲至60多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為28例男性、20例女性，年齡介於未滿10歲至50多歲，分別自美國(28例)、菲律賓(2例)、法國、愛爾蘭、荷蘭、哥斯大黎加、加拿大、丹麥及德國(各1例)移入；另11例調查中。入境日介於今(2022)年1月2日至1月16日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,278,363例新型冠狀病毒肺炎相關通報(含5,258,762例排除)，其中17,885例確診，分別為3,122例境外移入，14,709例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計115例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月17日新增本土COVID-19確診個案表.pdf\$\@\$1月17日新增境外移入COVID-19確診個案表.pdf</t>
+    <t>發佈日期：2022-01-16\$\@\$中央流行疫情指揮中心今( 16 )日表示，因應國內本土疫情升溫，目前提供民眾於各地方政府衛生局安排/指定之合約醫療院所預約接種或隨到隨打接種站進行接種。為提供民眾多元疫苗預約管道選擇，以加速提升民眾免疫保護力，COVID-19公費疫苗預約平台(下稱預約平台)，持續於第20期提供「已完整接種兩劑COVID-19疫苗滿12週且滿18歲以上」民眾，預約接種疫苗追加劑。如已於各地方政府衛生局安排/指定之合約醫療院所完成預約之民眾，請依原已預約時段前往接種，無須再於預約平台重複預約。\$\@\$預約平台相關對象及期程說明如下：\$\@\$一、施打時程：1月24日至1月30日。\$\@\$二、符合資格對象：110年11月7日(含)前已完整接種兩劑疫苗且間隔滿12週之18歲以上民眾[即2004/1/30(含)前出生]預約接種疫苗追加劑。\$\@\$三、預約分流時程：\$\@\$(一)65歲以上：1月18日上午10時至1月22日中午12時。\$\@\$(二)50歲-64歲：1月18日中午12時至1月22日中午12時。\$\@\$(三)18歲-49歲：1月18日下午2時至1月22日中午12時。\$\@\$指揮中心提醒，民眾可於預約時段至預約平台進行預約資格查詢，不再另發送預約提醒簡訊，符合資格民眾請記得於預約時間進行預約，預約當日如遇啟動流量管制亦請配合依序排隊耐心等候預約，亦可持「COVID-19疫苗接種紀錄卡」(小黃卡)逕至各地方政府指定/安排合約醫療院所或衛生所預約接種，或所設置之隨到隨打接種站接種。\$\@\$指揮中心說明，BNT、Moderna都屬mRNA疫苗，兩者保護效果相當，請符合預約資格且有意願接種但尚未完成預約者，如欲選擇的疫苗接種點額滿，可選擇另一種疫苗接種，以儘速獲得追加保護。\$\@\$指揮中心表示，預約平台第20期僅提供民眾預約接種疫苗追加劑，若有第一劑或第二劑疫苗接種需求之民眾，請持COVID-19疫苗接種紀錄卡(小黃卡)至各地方政府指定/安排合約醫療院所或衛生所預約接種，或所設置之隨到隨打接種站接種。至1月31日止，可由地方政府衛生局提供200元(含)以下衛教品，以提升接種意願。\$\@\$指揮中心提醒，請民眾前往接種COVID-19疫苗前，應備妥「COVID-19疫苗接種紀錄卡」(小黃卡)及健保卡，並經醫生評估過往疫苗接種史及檢核接種紀錄後，提供民眾疫苗接種。另18歲至未滿20歲民眾，如自行前往接種，請持家長簽具之意願同意書，若由家長陪同前往接種，請本人與家長於現場共同簽署意願同意書。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-16\$\@\$中央流行疫情指揮中心今(16)日公布國內新增51例COVID-19確定病例，分別為10例本土個案及41例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為2例男性、6例女性、2例調查中，年齡介於10多歲至50多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為25例男性、16例女性，年齡介於10歲至80多歲，分別自美國(14例)、墨西哥、印度、菲律賓、澳大利亞、越南及柬埔寨(各2例)、丹麥、法國、加拿大、印尼、英國(各1例)移入；另10例調查中。入境日介於去(2021)年12月22日至今(2022)年1月15日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,257,161例新型冠狀病毒肺炎相關通報(含5,236,654例排除)，其中17,820例確診，分別為3,074例境外移入，14,692例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案17765)，累計115例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月16日新增境外移入COVID-19確診個案表.pdf\$\@\$1月16日新增本土COVID-19確診個案表.pdf</t>
   </si>
   <si>
     <t>發佈日期：2022-01-15\$\@\$中央流行疫情指揮中心今(15)日公布國內新增78例COVID-19確定病例，分別為6例本土個案及72例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為2例男性、4例女性，年齡介於10多歲至30多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為38例男性、31例女性、3例調查中，年齡介於未滿5歲至60多歲，分別自美國(23例)、加拿大(10例)、印尼及越南(各3例)、法國及澳大利亞(各2例)、新加坡及德國(各1例)移入；另27例調查中。入境日介於去(2021)年11月4日至今(2022)年1月14日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,233,163例新型冠狀病毒肺炎相關通報(含5,213,414例排除)，其中17,769例確診，分別為3,033例境外移入，14,682例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案17765)，累計115例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月15日新增境外移入COVID-19確診個案表.pdf\$\@\$1月15日新增本土COVID-19確診個案表.pdf</t>
@@ -383,12 +389,6 @@
   </si>
   <si>
     <t>發佈日期：2022-01-07\$\@\$中央流行疫情指揮中心今(7)日公布國內新增62例COVID-19確定病例，分別為4例本土個案(案17368-17371)及58例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，本土個案(案17368-17371)分別為本國籍1例男性、3例女性，年齡介於20至50多歲，均為桃園機場感染事件相關個案；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增58例境外移入個案，為29例男性、29例女性，年齡介於10多歲至70多歲，分別自美國(35例)、法國(4例)、英國(3例)、瑞士、越南及印度(各2例)、奧地利、智利、德國、加拿大、愛爾蘭、孟加拉、奈及利亞、墨西哥、西班牙及哥斯大黎加(各1例)入境，入境日介於去(2021)年12月22日至今(2022)年1月6日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,055,274例新型冠狀病毒肺炎相關通報(含5,035,769例排除)，其中17,258例確診，分別為2,588例境外移入，14,616例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另新增2例空號病例(案17271，案17272與舊案重複，改列空號)，累計113例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月7日新增本土COVID-19確診個案表.pdf\$\@\$1月7日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-06\$\@\$中央流行疫情指揮中心今(6)日公布國內新增43例COVID-19確定病例，為昨(5)日公布尚未取號的3例本土個案(案17307-17309)及40例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，案17307-17309為本國籍女性，年齡介於50至60多歲，皆已接種2劑疫苗，為案17230、案17238、案17239及案17266同職場工作人員；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增40例境外移入個案，為20例男性、20例女性，年齡介於未滿5歲至70多歲，分別自美國(24例，案17267、案17270、案17273-17275、案17277-17282、案17284-17289、案17291-17292、案17300、案17302、案17304-17306)、印度(3例，案17290、案17296、案17303)、巴拿馬(2例，案17271-17272)、荷蘭(案17268)、阿拉伯聯合大公國(2例，案17283、案17301)、加拿大(案17269)、菲律賓(案17276)、義大利(案17293)、英國(案17295)、中國(案17298)及法國(案17299)入境，另有2例(案17294、案17297)調查中，入境日介於去(2021)年12月26日至今(2022)年1月5日；詳如新聞稿附件。\$\@\$另去年12月31日公布之案17127境外移入病例經疫調後改判為本土病例，為案17073之相關感染。\$\@\$指揮中心統計，截至目前國內累計5,036,659例新型冠狀病毒肺炎相關通報(含5,016,638例排除)，其中17,198例確診，分別為2,532例境外移入，14,612例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月6日新增境外移入COVID-19確診個案表.pdf\$\@\$1月6日新增本土COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-06\$\@\$中央流行疫情指揮中心今(6)日表示，考量目前國際COVID-19疫情嚴峻，請長者及其他 COVID-19感染後容易產生嚴重併發症之族群，儘速完成COVID-19疫苗基礎劑接種，提升保護力。\$\@\$指揮中心表示，目前我國75歲以上長者第1劑接種率僅約73%，第2劑接種率僅約67%，仍需再積極提升，為維護長者及風險族群健康，降低因感染COVID-19造成之重症、住院或死亡風險，家中長輩如尚未接種COVID-19疫苗第1、2劑，請於其身體狀況較穩定時，協助陪同至各地方政府衛生局安排或指定之合約醫療院所接種。\$\@\$指揮中心說明，疫苗接種後可能發生副作用，通常輕微並於數天內消失，並隨年齡層增加而減少，若擔心接種疫苗後所產生之副作用，可先與醫師討論，經諮詢評估選擇合適的疫苗接種。\$\@\$指揮中心表示，若為行動不便者，各地方政府衛生局亦設有到宅接種服務，有需求者可向各地方政府衛生局洽詢。另為鼓勵18歲以上尚未接種第1劑、第2劑COVID-19疫苗接種者儘速踴躍前往接種，於2022年1月5日至1月31日前接種COVID-19疫苗者，可獲得地方政府發放之200元(含)以下衛教品，鼓勵民眾儘速接種，獲得保護力。\$\@\$指揮中心提醒，依我國衛生福利部傳染病防治諮詢會預防接種組(ACIP)建議，接種COVID-19疫苗應與流感疫苗等其他疫苗間隔至少7天，亦請民眾前往接種COVID-19疫苗前，應備妥健保卡或其他可證明身分之證件，如為接種第2劑COVID-19疫苗者，請記得攜帶「COVID-19疫苗接種紀錄卡」，並於接種前評估時，說明過往疫苗接種史，以利醫生評估。另近期天氣多變，對於近期身體具狀況或慢性病情不穩定者，請於身體狀況較穩定後就近前往接種。接種後亦請多加留意身體狀況，多喝水多休息，亦請家人協助注意，如有持續發燒超過48小時、嚴重過敏反應如呼吸困難、氣喘、眩暈、心跳加速、全身紅疹等不適症狀，應儘速就醫釐清病因。</t>
   </si>
 </sst>
 </file>
@@ -794,7 +794,7 @@
         <v>35</v>
       </c>
       <c r="C2" s="2">
-        <v>44582</v>
+        <v>44583</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>65</v>
@@ -828,7 +828,7 @@
         <v>37</v>
       </c>
       <c r="C4" s="2">
-        <v>44581</v>
+        <v>44582</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>67</v>
@@ -896,7 +896,7 @@
         <v>41</v>
       </c>
       <c r="C8" s="2">
-        <v>44580</v>
+        <v>44581</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>71</v>
@@ -930,7 +930,7 @@
         <v>43</v>
       </c>
       <c r="C10" s="2">
-        <v>44579</v>
+        <v>44580</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>73</v>
@@ -947,7 +947,7 @@
         <v>44</v>
       </c>
       <c r="C11" s="2">
-        <v>44578</v>
+        <v>44579</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>74</v>
@@ -964,7 +964,7 @@
         <v>45</v>
       </c>
       <c r="C12" s="2">
-        <v>44576</v>
+        <v>44577</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>75</v>
@@ -981,7 +981,7 @@
         <v>46</v>
       </c>
       <c r="C13" s="2">
-        <v>44575</v>
+        <v>44577</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>76</v>
@@ -998,7 +998,7 @@
         <v>47</v>
       </c>
       <c r="C14" s="2">
-        <v>44575</v>
+        <v>44576</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>77</v>
@@ -1015,7 +1015,7 @@
         <v>48</v>
       </c>
       <c r="C15" s="2">
-        <v>44574</v>
+        <v>44575</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>78</v>
@@ -1032,7 +1032,7 @@
         <v>49</v>
       </c>
       <c r="C16" s="2">
-        <v>44574</v>
+        <v>44575</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>79</v>
@@ -1049,7 +1049,7 @@
         <v>50</v>
       </c>
       <c r="C17" s="2">
-        <v>44573</v>
+        <v>44574</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>80</v>
@@ -1066,7 +1066,7 @@
         <v>51</v>
       </c>
       <c r="C18" s="2">
-        <v>44573</v>
+        <v>44574</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>81</v>
@@ -1083,7 +1083,7 @@
         <v>52</v>
       </c>
       <c r="C19" s="2">
-        <v>44572</v>
+        <v>44573</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>82</v>
@@ -1100,7 +1100,7 @@
         <v>53</v>
       </c>
       <c r="C20" s="2">
-        <v>44571</v>
+        <v>44573</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>83</v>
@@ -1117,7 +1117,7 @@
         <v>54</v>
       </c>
       <c r="C21" s="2">
-        <v>44571</v>
+        <v>44572</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>84</v>
@@ -1151,7 +1151,7 @@
         <v>56</v>
       </c>
       <c r="C23" s="2">
-        <v>44570</v>
+        <v>44571</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>86</v>
@@ -1168,7 +1168,7 @@
         <v>57</v>
       </c>
       <c r="C24" s="2">
-        <v>44570</v>
+        <v>44571</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>87</v>
@@ -1219,7 +1219,7 @@
         <v>60</v>
       </c>
       <c r="C27" s="2">
-        <v>44569</v>
+        <v>44570</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>90</v>
@@ -1236,7 +1236,7 @@
         <v>61</v>
       </c>
       <c r="C28" s="2">
-        <v>44568</v>
+        <v>44570</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>91</v>
@@ -1253,7 +1253,7 @@
         <v>62</v>
       </c>
       <c r="C29" s="2">
-        <v>44568</v>
+        <v>44569</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>92</v>
@@ -1270,7 +1270,7 @@
         <v>63</v>
       </c>
       <c r="C30" s="2">
-        <v>44567</v>
+        <v>44568</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>93</v>
@@ -1287,7 +1287,7 @@
         <v>64</v>
       </c>
       <c r="C31" s="2">
-        <v>44567</v>
+        <v>44568</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20220123
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="199">
   <si>
     <t>Press Title</t>
   </si>
@@ -61,6 +61,9 @@
     <t>新增66例COVID-19確定病例，分別為17例本土及49例境外移入</t>
   </si>
   <si>
+    <t>新增65例COVID-19確定病例，分別為17例本土及48例境外移入</t>
+  </si>
+  <si>
     <t>COVID-19公費疫苗預約平台自1月18日起，提供已完整接種兩劑COVID-19疫苗滿12週且滿18歲以上民眾，預約接種追加劑</t>
   </si>
   <si>
@@ -121,6 +124,63 @@
     <t>新增62例COVID-19確定病例，分別為4例本土及58例境外移入</t>
   </si>
   <si>
+    <t>新增43例COVID-19確定病例，分別為3例本土及40例境外移入</t>
+  </si>
+  <si>
+    <t>呼籲長者及其他 COVID-19感染後容易產生嚴重併發症之族群，儘速完成疫苗基礎劑接種</t>
+  </si>
+  <si>
+    <t>因應春節入境人潮及COVID-19境外移入確診個案增加，指揮中心擴大開設專責病房及調整醫療機構應變策略</t>
+  </si>
+  <si>
+    <t>新增3例COVID-19本土確定病例，衛生單位已啟動疫情調查及防治作為</t>
+  </si>
+  <si>
+    <t>新增26例COVID-19確定病例，分別為1例本土及25例境外移入</t>
+  </si>
+  <si>
+    <t>自2022年1月6日起，公費流感疫苗開放全民接種至疫苗用罄</t>
+  </si>
+  <si>
+    <t>針對桃園機場群聚感染案件，指揮中心今日成立前進指揮所協助防疫作為</t>
+  </si>
+  <si>
+    <t>1月5日起至1月31日止，地方政府可提供民眾200元(含)以下衛教品，以提升接種意願</t>
+  </si>
+  <si>
+    <t>新增34例COVID-19確定病例，分別為4例本土及30例境外移入</t>
+  </si>
+  <si>
+    <t>新增1例COVID-19本土確定病例，衛生單位已啟動疫情調查及防治作為</t>
+  </si>
+  <si>
+    <t>新增25例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>新增20例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>新增21例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>新增41例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>指揮中心重申，兩岸應以防疫優先，才能維護兩岸民眾健康</t>
+  </si>
+  <si>
+    <t>受聘僱外國人健康檢查管理辦法部分條文修正案自111年1月1日起實施，確保社區防疫安全</t>
+  </si>
+  <si>
+    <t>指揮中心增加公費COVID-19家用快篩試劑發放點，早期偵測，防範病毒進入社區</t>
+  </si>
+  <si>
+    <t>新增24例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>台積電、鴻海永齡、慈濟三間企業和民間團體捐贈之第十五批BNT疫苗93.83萬劑於今(30)日上午抵臺</t>
+  </si>
+  <si>
     <t>/Bulletin/Detail/5MtrgzOJApOSjivffWLWRw?typeid=9</t>
   </si>
   <si>
@@ -151,6 +211,9 @@
     <t>/Bulletin/Detail/5XT_6l4aNN_OQfb208cYtg?typeid=9</t>
   </si>
   <si>
+    <t>/Bulletin/Detail/rkvMm-Hng9jJHKRdCEXvDg?typeid=9</t>
+  </si>
+  <si>
     <t>/Bulletin/Detail/sKXQ2hw4AvLbte5bgT1zPQ?typeid=9</t>
   </si>
   <si>
@@ -211,6 +274,63 @@
     <t>/Bulletin/Detail/szV5W2pK70cBBVpTxxghzw?typeid=9</t>
   </si>
   <si>
+    <t>/Bulletin/Detail/09VZRAwn1bOg97wX7spbLw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Vwd8It8AE16rPEuotcXK9Q?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/u0vHFZX2nzlhWBifQl3x5Q?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/jK3GN-Hw8x_ELLciTmfwQg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/xR3EWQ6aKrqsQwfI_iNxqg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/oHyBMuXSjeea-EJ0olgdRQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Y4fwruTZG4YQclQTSYPT-w?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Q-xhjZ6c709hJ-9GQXtFFw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/NQf6AVY3GBaKX9pYZ5jA3Q?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/8XzxB5KZNJhy0ITApU7wWg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/wPYoUO5Fv8bYEL0fGvlwrw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/7wbCdR_N1PJc783mP_mtlQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/mj5H52pb8ivr0RcjQ-N9cw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/L32CQqYyDVXO-DF7hgHyAQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/pr-CblnPk9vL2ApdEOo_dQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/jOxiIwl9CpcNJxP8dckk6A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/ijxgB4PqNSwT9jxZQotXIQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/AjUkrlWXkxOqou5W9tgVpw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/WIMrcWpPk8g16xjOZR_e4g?typeid=9</t>
+  </si>
+  <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/5MtrgzOJApOSjivffWLWRw?typeid=9</t>
   </si>
   <si>
@@ -241,6 +361,9 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/5XT_6l4aNN_OQfb208cYtg?typeid=9</t>
   </si>
   <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/rkvMm-Hng9jJHKRdCEXvDg?typeid=9</t>
+  </si>
+  <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/sKXQ2hw4AvLbte5bgT1zPQ?typeid=9</t>
   </si>
   <si>
@@ -301,6 +424,63 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/szV5W2pK70cBBVpTxxghzw?typeid=9</t>
   </si>
   <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/09VZRAwn1bOg97wX7spbLw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Vwd8It8AE16rPEuotcXK9Q?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/u0vHFZX2nzlhWBifQl3x5Q?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/jK3GN-Hw8x_ELLciTmfwQg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/xR3EWQ6aKrqsQwfI_iNxqg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/oHyBMuXSjeea-EJ0olgdRQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Y4fwruTZG4YQclQTSYPT-w?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Q-xhjZ6c709hJ-9GQXtFFw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/NQf6AVY3GBaKX9pYZ5jA3Q?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/8XzxB5KZNJhy0ITApU7wWg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/wPYoUO5Fv8bYEL0fGvlwrw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/7wbCdR_N1PJc783mP_mtlQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/mj5H52pb8ivr0RcjQ-N9cw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/L32CQqYyDVXO-DF7hgHyAQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/pr-CblnPk9vL2ApdEOo_dQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/jOxiIwl9CpcNJxP8dckk6A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/ijxgB4PqNSwT9jxZQotXIQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/AjUkrlWXkxOqou5W9tgVpw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/WIMrcWpPk8g16xjOZR_e4g?typeid=9</t>
+  </si>
+  <si>
     <t>發佈日期：2022-01-22\$\@\$中央流行疫情指揮中心今(22)日公布國內新增130例COVID-19確定病例，分別為82例本土個案及48例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為12例男性、70例女性，年齡介於未滿10歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為29例男性、19例女性，年齡介於未滿5歲至70多歲，分別自美國(13例)、加拿大及新加坡(各4例)、菲律賓(3例)、印度、土耳其及香港(各2例)、奧地利、奈及利亞、義大利、柬埔寨、德國、越南及巴西(各1例)移入；另11例調查中。入境日介於去(2021)年12月31日至今(2022)年1月21日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,418,957例新型冠狀病毒肺炎相關通報(含5,400,086例排除)，其中18,238例確診，分別為3,331例境外移入，14,853例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案18182，再次採檢為陰性，改判排除)，累計117例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月22日新增本土COVID-19確診個案表.pdf\$\@\$1月22日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
@@ -331,6 +511,9 @@
     <t>發佈日期：2022-01-18\$\@\$中央流行疫情指揮中心今(18)日公布國內新增66例COVID-19確定病例，分別為17例本土個案及49例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為10例男性、7例女性，年齡介於未滿5歲至60多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為33例男性、16例女性，年齡介於未滿10歲至60多歲，分別自美國(21例)、越南(5例)、加拿大(4例)、英國(3例)、法國(2例)、愛爾蘭、西班牙、瑞典、菲律賓、波蘭、墨西哥及巴拿馬(各1例)移入；另7例調查中。入境日介於今(2022)年1月3日至1月17日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,306,453例新型冠狀病毒肺炎相關通報(含5,287,815例排除)，其中17,951例確診，分別為3,171例境外移入，14,726例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計115例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月18日新增本土COVID-19確診個案表.pdf\$\@\$1月18日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
+    <t>發佈日期：2022-01-17\$\@\$中央流行疫情指揮中心今(17)日公布國內新增65例COVID-19確定病例，分別為17例本土個案及48例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為8例男性、9例女性，年齡介於未滿5歲至60多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為28例男性、20例女性，年齡介於未滿10歲至50多歲，分別自美國(28例)、菲律賓(2例)、法國、愛爾蘭、荷蘭、哥斯大黎加、加拿大、丹麥及德國(各1例)移入；另11例調查中。入境日介於今(2022)年1月2日至1月16日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,278,363例新型冠狀病毒肺炎相關通報(含5,258,762例排除)，其中17,885例確診，分別為3,122例境外移入，14,709例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計115例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月17日新增本土COVID-19確診個案表.pdf\$\@\$1月17日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
     <t>發佈日期：2022-01-16\$\@\$中央流行疫情指揮中心今( 16 )日表示，因應國內本土疫情升溫，目前提供民眾於各地方政府衛生局安排/指定之合約醫療院所預約接種或隨到隨打接種站進行接種。為提供民眾多元疫苗預約管道選擇，以加速提升民眾免疫保護力，COVID-19公費疫苗預約平台(下稱預約平台)，持續於第20期提供「已完整接種兩劑COVID-19疫苗滿12週且滿18歲以上」民眾，預約接種疫苗追加劑。如已於各地方政府衛生局安排/指定之合約醫療院所完成預約之民眾，請依原已預約時段前往接種，無須再於預約平台重複預約。\$\@\$預約平台相關對象及期程說明如下：\$\@\$一、施打時程：1月24日至1月30日。\$\@\$二、符合資格對象：110年11月7日(含)前已完整接種兩劑疫苗且間隔滿12週之18歲以上民眾[即2004/1/30(含)前出生]預約接種疫苗追加劑。\$\@\$三、預約分流時程：\$\@\$(一)65歲以上：1月18日上午10時至1月22日中午12時。\$\@\$(二)50歲-64歲：1月18日中午12時至1月22日中午12時。\$\@\$(三)18歲-49歲：1月18日下午2時至1月22日中午12時。\$\@\$指揮中心提醒，民眾可於預約時段至預約平台進行預約資格查詢，不再另發送預約提醒簡訊，符合資格民眾請記得於預約時間進行預約，預約當日如遇啟動流量管制亦請配合依序排隊耐心等候預約，亦可持「COVID-19疫苗接種紀錄卡」(小黃卡)逕至各地方政府指定/安排合約醫療院所或衛生所預約接種，或所設置之隨到隨打接種站接種。\$\@\$指揮中心說明，BNT、Moderna都屬mRNA疫苗，兩者保護效果相當，請符合預約資格且有意願接種但尚未完成預約者，如欲選擇的疫苗接種點額滿，可選擇另一種疫苗接種，以儘速獲得追加保護。\$\@\$指揮中心表示，預約平台第20期僅提供民眾預約接種疫苗追加劑，若有第一劑或第二劑疫苗接種需求之民眾，請持COVID-19疫苗接種紀錄卡(小黃卡)至各地方政府指定/安排合約醫療院所或衛生所預約接種，或所設置之隨到隨打接種站接種。至1月31日止，可由地方政府衛生局提供200元(含)以下衛教品，以提升接種意願。\$\@\$指揮中心提醒，請民眾前往接種COVID-19疫苗前，應備妥「COVID-19疫苗接種紀錄卡」(小黃卡)及健保卡，並經醫生評估過往疫苗接種史及檢核接種紀錄後，提供民眾疫苗接種。另18歲至未滿20歲民眾，如自行前往接種，請持家長簽具之意願同意書，若由家長陪同前往接種，請本人與家長於現場共同簽署意願同意書。</t>
   </si>
   <si>
@@ -340,9 +523,6 @@
     <t>發佈日期：2022-01-15\$\@\$中央流行疫情指揮中心今(15)日公布國內新增78例COVID-19確定病例，分別為6例本土個案及72例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為2例男性、4例女性，年齡介於10多歲至30多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為38例男性、31例女性、3例調查中，年齡介於未滿5歲至60多歲，分別自美國(23例)、加拿大(10例)、印尼及越南(各3例)、法國及澳大利亞(各2例)、新加坡及德國(各1例)移入；另27例調查中。入境日介於去(2021)年11月4日至今(2022)年1月14日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,233,163例新型冠狀病毒肺炎相關通報(含5,213,414例排除)，其中17,769例確診，分別為3,033例境外移入，14,682例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案17765)，累計115例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月15日新增境外移入COVID-19確診個案表.pdf\$\@\$1月15日新增本土COVID-19確診個案表.pdf</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-14\$\@\$中央流行疫情指揮中心今(14)日公布國內新增68例COVID-19確定病例，分別為11例本土個案及57例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為8例男性、3例女性，年齡介於未滿5歲至50多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為25例男性、24例女性、8例調查中，年齡介於未滿5歲至70多歲，分別自美國(17例)、加拿大(5例)、菲律賓(4例)、澳大利亞、波蘭及越南(各3例)、印尼、丹麥、法國、葡萄牙、巴西、土耳其及瑞典(各1例)移入；另15例調查中。入境日介於去(2021)年12月31日至今(2022)年1月13日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,210,348例新型冠狀病毒肺炎相關通報(含5,190,844例排除)，其中17,692例確診，分別為2,962例境外移入，14,676例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計114例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月14日新增境外移入COVID-19確診個案表.pdf\$\@\$1月14日新增本土COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
     <t>發佈日期：2022-01-14\$\@\$中央流行疫情指揮中心今( 14 )日表示，因應國內本土疫情升溫，目前提供民眾於各地方政府指定/安排合約醫療院所或衛生所預約接種，或所設置之隨到隨打接種站接種COVID-19疫苗。為提供民眾多元疫苗預約管道選擇，以加速提升民眾免疫保護力，將於1月15日開放COVID-19公費疫苗預約平台，於第19期提供「已完整接種兩劑COVID-19疫苗滿12週且滿18歲以上」民眾預約接種疫苗追加劑。如已於各地方政府指定/安排合約醫療院所或衛生所完成預約之民眾，請依原已預約時段前往接種，無須再於預約平台重複預約。\$\@\$預約平台相關對象及期程說明如下：\$\@\$一、施打時程：1月17日至1月23日。\$\@\$二、符合資格對象：2021年10月31日前已完整接種兩劑疫苗且間隔滿12週之18歲以上民眾[即2004/1/23(含)前出生]，預約接種疫苗追加劑。\$\@\$三、預約分流時程：\$\@\$(一)65歲以上：1月15日上午10時至1月16日中午12時。\$\@\$(二)50歲-64歲：1月15日中午12時至1月16日中午12時。\$\@\$(三)18歲-49歲：1月15日下午2時至1月16日中午12時。\$\@\$指揮中心說明，民眾可於1月14日下午2時起至預約平台進行預約資格查詢，不再另發送預約提醒簡訊。符合資格民眾請記得於預約時間進行預約，預約當日如遇啟動流量管制，請配合依序排隊、耐心等候。若符合本期資格但未能預約成功者，請於下週下一期平台開放時再行預約。符合本期資格但未預約成功、以及有第一劑或第二劑疫苗接種需求之民眾，可持「COVID-19疫苗接種紀錄卡」(小黃卡)逕至各地方政府指定/安排合約醫療院所或衛生所預約接種，或所設置之隨到隨打接種站接種。\$\@\$指揮中心提醒，請民眾前往接種COVID-19疫苗前，應備妥「COVID-19疫苗接種紀錄卡」及健保卡，並經醫生評估過往疫苗接種史及檢核接種紀錄後，提供民眾疫苗接種。另18歲至未滿20歲民眾，如自行前往接種，請持家長簽具之意願同意書，若由家長陪同前往接種，請本人與家長於現場共同簽署意願同意書。</t>
   </si>
   <si>
@@ -367,9 +547,6 @@
     <t>發佈日期：2022-01-10\$\@\$中央流行疫情指揮中心今(10)日表示，Omicron變異株於全球迅速擴散，近期境外移入確診數大增，為降低COVID-19威脅國內社區防疫安全，自今(2022)年1月11日零時起(航班表定抵臺時間)，調整入境旅客檢疫措施如下，請旅客務必配合：\$\@\$搭乘歐美、中東及紐澳等航線長程航班旅客，於抵臺時進行落地公費採檢及快速核酸檢驗，檢驗結果陰性者接續入境通關程序，且應搭乘防疫車輛前往防疫旅宿/集中檢疫所完成檢疫；檢驗結果陽性者，指派專人完成證照查驗後，由空側搭乘救護車後送專責醫院。\$\@\$指揮中心再次強調，適逢春節前返鄉人潮，請旅客返臺必須事先瞭解，並主動配合我國現行入境檢疫規定，並依指揮中心規定的交通方式前往檢疫地點，同時遵守檢疫期間各項檢疫、防疫措施，共同維護國內社區安全。</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-10\$\@\$中央流行疫情指揮中心今(10)日公布國內新增32例COVID-19確定病例，分別為6例本土個案及26例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為2例男性、4例女性，年齡介於未滿10歲至40多歲；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增境外移入個案為14例男性、12例女性，年齡介於未滿5歲至70多歲，分別自美國(11例)、印尼及緬甸(各2例)、尼泊爾、比利時、冰島、厄瓜多、英國、義大利、菲律賓、丹麥、南非、法國及芬蘭(各1例)移入。入境日介於去(2021)年12月26日至今(2022)年1月9日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,119,134例新型冠狀病毒肺炎相關通報(含5,099,767例排除)，其中17,393例確診，分別為2,704例境外移入，14,635例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案17462)，累計114例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月10日新增境外移入COVID-19確診個案表.pdf\$\@\$1月10日新增本土COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
     <t>發佈日期：2022-01-09\$\@\$中央流行疫情指揮中心今(9)日表示，因應國內發生Omicron變異株本土確診病例，社區傳播風險提升，為確保醫療機構對疫情的因應及保全醫療量能，自即日起調整以下醫療應變作為，說明如下：\$\@\$一、探病管制：臺北市、新北市、基隆市、桃園市之醫院除例外情形外，禁止探病。符合例外情形經醫院同意探病者，應出具探視日前3天內抗原快篩或PCR檢測陰性證明。探病者為完成疫苗基礎劑應接種劑次達14天(含)以上者，以公費篩檢；未完成者，以自費篩檢。探病者若為確定病例符合檢驗解除隔離條件且距發病日3個月內，得免除篩檢。\$\@\$二、住院病人及陪病者入院篩檢：臺北市、新北市、基隆市、桃園市之醫院或入住前14天內居住於臺北市、新北市、基隆市、桃園市之住院病人及陪病者，無論有無完成疫苗基礎劑應接種劑次達14天(含)以上，預定(非緊急)住院者，於入院前3日內公費篩檢；緊急需住院者，於入住病房前公費篩檢。住院病人及陪病者若為確定病例符合檢驗解除隔離條件且距發病日3個月內，得免除篩檢。\$\@\$三、住院病人之陪病者管理：臺北市、新北市、基隆市、桃園市之醫院，陪病人數以1人為原則。陪病者須不具COVID-19相關症狀，亦未曾接觸確診個案或具相關公共場所活動史。\$\@\$四、醫療照護人員管理：專責病房之醫療照護人員應完成COVID-19疫苗基礎劑應接種劑次達14天(含)以上；可接種追加劑疫苗者，於111年2月1日前應完成接種，未完成者應評估調整職務內容。桃園市之醫院所有單位(除專責病房) 醫療照護人員，未完成疫苗基礎劑應接種劑次達14天(含)以上者，每週定期進行公費篩檢。\$\@\$指揮中心呼籲，醫療機構務必落實執行醫療應變措施，強化感染管制，提高警覺，加強通報採檢，並鼓勵可接種追加劑疫苗之醫院工作人員儘速接種追加劑疫苗，以確保人員健康安全，共同嚴守醫療防線。指揮中心將持續監測國內外疫情發展，滾動修正相關應變策略，完善醫療照護體系，確保醫療量能充足以因應疫情。</t>
   </si>
   <si>
@@ -389,6 +566,51 @@
   </si>
   <si>
     <t>發佈日期：2022-01-07\$\@\$中央流行疫情指揮中心今(7)日公布國內新增62例COVID-19確定病例，分別為4例本土個案(案17368-17371)及58例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，本土個案(案17368-17371)分別為本國籍1例男性、3例女性，年齡介於20至50多歲，均為桃園機場感染事件相關個案；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增58例境外移入個案，為29例男性、29例女性，年齡介於10多歲至70多歲，分別自美國(35例)、法國(4例)、英國(3例)、瑞士、越南及印度(各2例)、奧地利、智利、德國、加拿大、愛爾蘭、孟加拉、奈及利亞、墨西哥、西班牙及哥斯大黎加(各1例)入境，入境日介於去(2021)年12月22日至今(2022)年1月6日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,055,274例新型冠狀病毒肺炎相關通報(含5,035,769例排除)，其中17,258例確診，分別為2,588例境外移入，14,616例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另新增2例空號病例(案17271，案17272與舊案重複，改列空號)，累計113例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月7日新增本土COVID-19確診個案表.pdf\$\@\$1月7日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-06\$\@\$中央流行疫情指揮中心今(6)日公布國內新增43例COVID-19確定病例，為昨(5)日公布尚未取號的3例本土個案(案17307-17309)及40例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，案17307-17309為本國籍女性，年齡介於50至60多歲，皆已接種2劑疫苗，為案17230、案17238、案17239及案17266同職場工作人員；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增40例境外移入個案，為20例男性、20例女性，年齡介於未滿5歲至70多歲，分別自美國(24例，案17267、案17270、案17273-17275、案17277-17282、案17284-17289、案17291-17292、案17300、案17302、案17304-17306)、印度(3例，案17290、案17296、案17303)、巴拿馬(2例，案17271-17272)、荷蘭(案17268)、阿拉伯聯合大公國(2例，案17283、案17301)、加拿大(案17269)、菲律賓(案17276)、義大利(案17293)、英國(案17295)、中國(案17298)及法國(案17299)入境，另有2例(案17294、案17297)調查中，入境日介於去(2021)年12月26日至今(2022)年1月5日；詳如新聞稿附件。\$\@\$另去年12月31日公布之案17127境外移入病例經疫調後改判為本土病例，為案17073之相關感染。\$\@\$指揮中心統計，截至目前國內累計5,036,659例新型冠狀病毒肺炎相關通報(含5,016,638例排除)，其中17,198例確診，分別為2,532例境外移入，14,612例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月6日新增境外移入COVID-19確診個案表.pdf\$\@\$1月6日新增本土COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-06\$\@\$中央流行疫情指揮中心今(6)日表示，考量目前國際COVID-19疫情嚴峻，請長者及其他 COVID-19感染後容易產生嚴重併發症之族群，儘速完成COVID-19疫苗基礎劑接種，提升保護力。\$\@\$指揮中心表示，目前我國75歲以上長者第1劑接種率僅約73%，第2劑接種率僅約67%，仍需再積極提升，為維護長者及風險族群健康，降低因感染COVID-19造成之重症、住院或死亡風險，家中長輩如尚未接種COVID-19疫苗第1、2劑，請於其身體狀況較穩定時，協助陪同至各地方政府衛生局安排或指定之合約醫療院所接種。\$\@\$指揮中心說明，疫苗接種後可能發生副作用，通常輕微並於數天內消失，並隨年齡層增加而減少，若擔心接種疫苗後所產生之副作用，可先與醫師討論，經諮詢評估選擇合適的疫苗接種。\$\@\$指揮中心表示，若為行動不便者，各地方政府衛生局亦設有到宅接種服務，有需求者可向各地方政府衛生局洽詢。另為鼓勵18歲以上尚未接種第1劑、第2劑COVID-19疫苗接種者儘速踴躍前往接種，於2022年1月5日至1月31日前接種COVID-19疫苗者，可獲得地方政府發放之200元(含)以下衛教品，鼓勵民眾儘速接種，獲得保護力。\$\@\$指揮中心提醒，依我國衛生福利部傳染病防治諮詢會預防接種組(ACIP)建議，接種COVID-19疫苗應與流感疫苗等其他疫苗間隔至少7天，亦請民眾前往接種COVID-19疫苗前，應備妥健保卡或其他可證明身分之證件，如為接種第2劑COVID-19疫苗者，請記得攜帶「COVID-19疫苗接種紀錄卡」，並於接種前評估時，說明過往疫苗接種史，以利醫生評估。另近期天氣多變，對於近期身體具狀況或慢性病情不穩定者，請於身體狀況較穩定後就近前往接種。接種後亦請多加留意身體狀況，多喝水多休息，亦請家人協助注意，如有持續發燒超過48小時、嚴重過敏反應如呼吸困難、氣喘、眩暈、心跳加速、全身紅疹等不適症狀，應儘速就醫釐清病因。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-06\$\@\$中央流行疫情指揮中心今(6)日表示，因應國際COVID-19疫情嚴峻及Omicron新型變異株威脅，考量春節入境人潮且近期COVID-19境外移入確診個案增加，為確保國內醫療院所對疫情的因應及保全醫療量能，即日起調整醫療機構醫療應變作為，說明如下：\$\@\$一、全國專責病房及負壓隔離病房調整收治病人條件，專責病房僅收治疑似或確診COVID-19病人；負壓隔離病室則以收治疑似或確診COVID-19及其他空氣傳染之法定傳染病病人為原則，清空非必要(如非空氣傳染防護隔離治療)入住於負壓隔離病房的病人。\$\@\$二、臺北市、新北市、基隆市、桃園市之應變醫院，於3日內恢復開設急性一般病床總數之20%作為專責病房(開設床數含負壓隔離病床)，收治疑似或確診個案。\$\@\$三、臺北市、新北市、基隆市、宜蘭縣、桃園市、新竹市、新竹縣及苗栗縣之急性一般病床總數500床以上之急救責任醫院，於3日內恢復開設急性一般病床總數之5%作為專責病房(開設床數含負壓隔離病床)，收治疑似或確診個案。\$\@\$四、專責病房收治疑似或確診COVID-19病人應以一人一室為原則(家人、同住者、同行者等如均為確診個案且知情同意，得兩人一室)，並有適當動線規劃，分流分艙安置住院病人；落實固定照護團隊與服務區塊化，避免人員頻繁輪替或跨單位工作；配置適當且固定之工作人員(含清潔人員、傳送人員及照顧服務員等)，以防範院內感染傳播風險。\$\@\$指揮中心呼籲醫療機構落實感染管制、強化門禁管制及工作人員健康監測、加強員工使用適當個人防護裝備，以預防並降低醫院群聚感染風險。由於Omicron新型變異株可能造成突破性感染，降低疫苗之保護力，指揮中心籲請可接種追加劑疫苗之醫院工作人員儘速接種追加劑疫苗，以確保人員健康安全。指揮中心將持續監測國內外疫情發展，確實掌握病床數及相關醫療資源分配，滾動修正相關應變策略，完善醫療照護體系，確保醫療量能充足以因應疫情。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-05\$\@\$中央流行疫情指揮中心今(5)日公布國內新增26例COVID-19確定病例，分別為1例(案17266)本土及25例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，案17266為本國籍50多歲女性，已接種2劑莫德納疫苗(為突破性感染)，與案17230、案17238及案17239為同職場工作人員，曾與前述個案搭乘同路線交通車，原定於今(2022)年1月5日採檢，1月3日出現乾咳、喉嚨不適等症狀，1月4日自行前往採檢站採檢後於今日確診，相關疫情調查、接觸者匡列及防治工作刻正進行中。\$\@\$指揮中心表示，今日新增25例境外移入個案，為12例男性、13例女性，年齡介於未滿5歲至70多歲，分別自美國(12例，案17241-17243、案17245、案17250、案17252、案17254、案17256-17259、案17265)、法國(3例，案17244、案17246、案17253)、丹麥(案17247)、英國(17248)、玻利維亞(案17249)、德國(案17251)、史瓦帝尼王國(案17255)、澳洲(案17260)、巴拿馬(2例，案17261-17262)、瑞典(案17263)及印尼(案17264)入境，入境日介於去(2021)年11月14日至今(2022)年1月4日；詳如新聞稿附件。\$\@\$另1月2日公布之案17181境外移入病例經疫調後改判為本土病例，為案16941之相關感染。\$\@\$指揮中心統計，截至目前國內累計5,017,456例新型冠狀病毒肺炎相關通報(含4,998,328例排除)，其中17,155例確診，分別為2,493例境外移入，14,608例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月5日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-04\$\@\$中央流行疫情指揮中心今(4)日表示，為因應桃園機場群聚感染案件，陳時中指揮官於今日下午協同醫療應變組王必勝副組長、桃園市政府衛生局王文彥局長、衛生福利部疾病管制署北區管制中心及機場公司航運中心工作人員，實地進行入境旅客動線勘查，評估釐清風險，檢視第一線人員防護裝備及消毒情形，並啟動下列防疫作為：\$\@\$一、 成立前進指揮所，由醫療應變組王必勝副組長擔任指揮官，統籌指揮相關防疫工作，進行跨單位溝通協調，並評估各單位現場作業風險，提出相關改善計畫。\$\@\$二、 針對高風險旅客(14天內有症狀)之入境動線，重新釐清評估風險，避免與其他民眾、工作人員接觸，降低傳播可能性。\$\@\$三、 配合桃園市政府衛生局採檢規劃「擴大、快速」戰略概念，擴大評估可能有在個案活動地(如清潔的廁所)活動之其他人員，快速進行相關篩檢。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-04\$\@\$中央流行疫情指揮中心今(4)日公布國內新增34例COVID-19確定病例，分別為4例(案17230、案17238-17240)本土及30例境外移入，其中案17230為昨(3)日公布之尚未取號本土個案；另確診個案中無新增死亡。\$\@\$指揮中心表示，案17238-17240為本國籍，1例男性、2例女性，年齡均為50多歲，皆已接種2劑疫苗，為案17230接觸者。案17238及案17239均為同職場工作人員，通勤時搭乘同班交通車，案17239於1月1日起陸續出現疲倦、咳嗽、流鼻水症狀；案17240為防疫計程車司機，1月1日出現咳嗽症狀，3人經衛生單位安排採檢後於今日確診，相關疫情調查、接觸者匡列及防治工作刻正進行中。\$\@\$指揮中心表示，今日新增30例境外移入個案，為16例男性、14例女性，年齡介於未滿5歲至70多歲，分別自美國(22例，案17207、案17210-17219、案17221、案17223-17228、案17231-17232、案17235-17236)、法國(案17208)、挪威(案17209)、南非(案17220)、阿拉伯聯合大公國(案17222)、英國(案17229)、波蘭(案17234)及烏茲別克(案17237)入境，另1例(案17233)調查中，入境日介於去(2021)年11月20日至今(2022)年1月3日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,998,949例新型冠狀病毒肺炎相關通報(含4,979,641例排除)，其中17,129例確診，分別為2,469例境外移入，14,606例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月4日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-03\$\@\$中央流行疫情指揮中心今(3)日公布國內新增1例COVID-19本土確定病例(尚未取號)，為本國籍40多歲女性，任機場停車場清潔人員，近期無出入境紀錄，已接種2劑AZ疫苗。個案於今(2022)年1/2出現發燒、畏寒、咳嗽、流鼻水、喉嚨痛等症狀，並於今日進行快篩，結果為陽性，同時採檢後確診。桃園市政府衛生局即刻啟動疫情調查，並立即通知同住家人就讀之兩校，分別預防性停課一天。\$\@\$指揮中心說明，桃園市政府在接獲醫院通報個案後，已通知個案家人就讀之兩校，分別預防性停課一天。並立即針對6名家人，已於今晚完成採檢，並以急件進行核酸檢驗，檢驗結果確認均為陰性，請兩校師生及家長不需擔憂。並對於個案之工作場域相關接觸者，現正擴大匡列採檢中，包括召回數百名防疫計程車司機將漏夜進行採檢，及針對個案所服務工作場域將進行清消。\$\@\$指揮中心進一步說明，個案另曾於去(2021)年12/30、12/31兩日上午9時至12時有至忠貞市場(中壢前龍街路段)擺攤賣小孩耳環、公仔、髪圈等，衛生單位將針對該市場進行疫調及接觸者匡列，並進行清消作業。\$\@\$指揮中心呼籲，民眾若曾於該段時間出入該場所，應請進行自我健康監測，若於1/14前出現發燒、上呼吸道、腹瀉、嗅味覺異常等症狀，應佩戴醫用口罩，儘速至社區採檢站或各指定採檢院所，接受採檢及評估。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-03\$\@\$中央流行疫情指揮中心今(3)日公布國內新增25例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增25例境外移入個案，為9例男性、16例女性，年齡介於未滿5歲至70多歲，分別自美國(15例，案17182-17183、案17186-17191、案17196-17197、案17199、案17201-17203、案17205)、土耳其(4例，案17192-17195)、德國(案17184)、加拿大(案17185)、義大利(案17198)、菲律賓(案17200)、亞美尼亞(案17204)及千里達及托巴哥(案17206)入境，入境日介於去(2021)年12月19日至今(2022)年1月1日；詳如新聞稿附件。\$\@\$另去年12月28日及12月30日公布之2例(案17058、案17099)境外移入病例經疫調後改判為本土病例，為案17085之相關感染。\$\@\$指揮中心統計，截至目前國內累計4,982,263例新型冠狀病毒肺炎相關通報(含4,962,860例排除)，其中17,095例確診，分別為2,439例境外移入，14,602例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月3日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-02\$\@\$中央流行疫情指揮中心今(2)日公布國內新增20例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增20例境外移入個案，為10例男性、10例女性，年齡介於未滿5歲至60多歲，分別自美國(11例，案17162-17163、17165-17166、案17168、案17170、案17172、案17174-17175、案17179-17180)、加拿大(案17164)、澳大利亞(案17167)、英國(2例，案17169、案17177)、越南(案17171)、沙烏地阿拉伯(案17173)、泰國(案17176)、希臘(案17178)及中國(案17181)，入境日介於去(2021)年12月12日至12月31日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,972,057例新型冠狀病毒肺炎相關通報(含4,951,828例排除)，其中17,070例確診，分別為2,416例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月2日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-01\$\@\$中央流行疫情指揮中心今(1)日公布國內新增21例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增21例境外移入個案，為15例男性、6例女性，年齡介於20多歲至70多歲，分別自美國(9例，案17141、案17148、案17149、案17151、案17154、案17156、案17159-17161)、越南(6例，案17142、案17145、案17147、案17150、案17152、案17153)、埃及(案17143)、寮國(案17144)、瓜地馬拉(案17146)、羅馬尼亞(案17155)、烏克蘭(案17157)及德國(案17158)入境，入境日介於去(2021)年12月17日至12月31日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,961,497例新型冠狀病毒肺炎相關通報(含4,942,271例排除)，其中17,050例確診，分別為2,396例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月1日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-31\$\@\$中央流行疫情指揮中心今(31)日公布國內新增41例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增41例境外移入個案，為16例男性、25例女性，年齡介於20多歲至70多歲，分別自美國(14例，案17104-17106、案17112、案17113、案17115、案17116、案17118-17122、案17131、案17139)、菲律賓(2例，案17125、案17132)、法國(2例，案17117、案17124)、義大利(案17114)、肯亞(案17123)、喀麥隆(案17126)、瑞士(案17127)、印度(案17128)、阿拉伯聯合大公國(案17129)、烏克蘭(案17130)、越南(案17133)及柬埔寨(案17138)入境，另14例(案17100-17103、案17107-17111、案17134-17137、案17140)調查中，入境日介於今(2021)年12月16日至12月30日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,946,919例新型冠狀病毒肺炎相關通報(含4,927,473例排除)，其中17,029例確診，分別為2,375例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月31日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-31\$\@\$中央流行疫情指揮中心今(31)日表示，指揮中心均秉持防疫優先之原則進行各項防疫工作，有關中國大陸國台辦針對臺灣防疫之錯誤發言內容，相關澄清說明如下：\$\@\$一、鑒於兩岸往來頻繁，為掌握疫情狀況，向來致力與中國大陸保持資訊交流，我方自108年12月31日至110年12月28日，與中國大陸透過正式管道就 COVID-19 疫情往來資訊包括陸方提供我方疫情資訊286次，我方提供陸方包括個案大陸旅遊史等資訊共50次。另我方洽詢陸方疫情訊息計85次，陸方回覆我方疫情資訊21次，而陸方洽詢我方疫情訊息29次，我方回覆陸方疫情資訊28次。陸方電話洽我方聯絡疫情資訊7次，我方電話洽陸方聯絡疫情資訊8次。此外，陸方提供我方技術文件共計12次。相關數據都有文件紀錄可查數，國台辦提供數據有與事實不符之處。\$\@\$二、為與國際分享、交換衛生、防疫經驗，我國均積極爭取參與世界衛生組織相關會議，自2009年至2021年，共向WHO申請參加220場技術性會議，但僅77場獲邀出席。\$\@\$三、為守護國人健康，我國政府一直多方洽談COVID-19疫苗購買，在BioNTech疫苗取得上，為尊重BioNTech原廠疫苗商業代理權劃分，BioNTech 疫苗係由台積電、鴻海／永齡基金會、慈濟基金會三捐贈方委託裕利醫藥公司，向原廠代理商復星實業公司（香港復星）有償購買，在基於「原廠製造、原廠標籤、直送臺灣」三原則的共識，全部無償捐贈政府統籌運用，對於捐贈單位出錢、出力，無私付出，不應被扭曲抹殺。\$\@\$指揮中心強調，疫情尚未止息，人民健康福祉為先。兩岸應互助合作，防疫優先，才能維護兩岸民眾健康。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-30\$\@\$衛生福利部疾病管制署今（30）日公布「受聘僱外國人健康檢查管理辦法」部分條文修正案，並預訂於111年1月1日實施。本次修法重點包括「修正移工申請結核病都治條件」及「防疫期間調整移工健檢期限之法源依據」等事項，確保社區防疫安全。\$\@\$疾管署說明，結核病為結核桿菌感染所造成的慢性傳染病，目前抗結核藥物效果良好，連續服藥14天後的傳染力可大幅下降；透過移工主動配合、雇主支持，再加上結核病都治關懷員等衛生單位人員持續關心移工確實規則服藥，幾乎可以痊癒，且治療期間亦可正常工作與生活作息；此外，罹患結核病之移工若於國內完成治療，除能避免疾病持續傳播，維護員工健康外，亦不影響雇主勞動力需求。本辦法修正後，移工確診為肺結核、結核性肋膜炎（多重抗藥性結核病個案除外）或漢生病，且本人同意留臺配合按規治療者，雇主應於收受診斷證明書之次日起15日內，檢具「診斷證明書」及「受聘僱外國人接受衛生單位安排都治服務同意書」送縣市政府衛生局申請都治服務，共同落實社區防疫。\$\@\$疾管署指出，本辦法另增訂「中央流行疫情指揮中心成立期間，中央衛生主管機關得依國內疫情防治所需，調整移工健檢期限」及「自聘僱許可生效日起滿6、18及30個月之日與最近一次健檢日間隔未滿3個月者，免辦該次定期健檢」等規定；且回溯至自110年5月19日施行，以避免部分移工需於短期間內重複健檢，並能兼顧防疫安全。\$\@\$為利雇主（仲介）能瞭解本辦法修正後實務作業，疾病管制署提供「移工罹患結核病申請留臺治療」宣導海報、「認識結核病的問與答」多國語言宣導單張及宣導影片等相關衛教素材，並建置於該署全球資訊網（http://www.cdc.gov.tw ； 首頁&gt;國際旅遊與健康&gt;外國人健康管理&gt;受聘僱外國人健檢&gt;最新消息）供下載瀏覽。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-30\$\@\$中央流行疫情指揮中心今(30)日公布國內新增24例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增24例境外移入個案，為11例男性、13例女性，年齡介於10多歲至60多歲，分別自美國(12例，案17076、案17078-17080、案17082-17083、案17085、案17088、案17090、案17094、案17096)、越南(2例，案17077、案17098)、英國(案17081)、尼加拉瓜(案17084)、奈及利亞(案17086)、加拿大(案17087)、阿拉伯聯合大公國(案17089)、法國(3例，17091-17093)、泰國(案17095)、海地(案17097)及日本(案17099)入境，入境日介於今(2021)年12月14日至12月28日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,932,261例新型冠狀病毒肺炎相關通報(含4,912,670例排除)，其中16,988例確診，分別為2,334例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月30日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-30\$\@\$中央流行疫情指揮中心今(30)日表示，台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的第十五批BNT疫苗93.83萬劑，已於今日上午順利運抵桃園國際機場，並在完成通關程序後，直接運送至指定冷儲物流中心進行後續檢驗封緘作業。\$\@\$指揮中心說明，由台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的BNT疫苗1,500萬劑，目前共計到貨1333.62萬劑，分別為首批9月2日93萬劑、第二批9月9日91萬劑、第三批9月30日54萬劑、第四批10月1日67萬劑、第五批10月4日27萬劑、第六批10月7日88.92萬劑、第七批10月8日88.92萬劑、第八批10月14日82.7萬劑、第九批10月28日90.21萬劑、第十批10月29日91.03萬劑、第十一批11月5日87.17萬劑、第十二批11月12日92.66萬劑、第十三批11月25日93.83萬劑、第十四批12月9日192.35萬劑，以及本批93.83萬劑。本批疫苗效期至2022年3月28日，將由指揮中心統籌運用，儘速提供民眾接種。\$\@\$對於台積電、鴻海暨永齡基金會、慈濟基金會三間企業和民間團體積極協助，提供更多的疫苗讓民眾接種，加速提升臺灣疫苗覆蓋率，指揮中心再次表達由衷的謝意。</t>
   </si>
 </sst>
 </file>
@@ -763,7 +985,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -791,16 +1013,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="C2" s="2">
         <v>44583</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -808,16 +1030,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="C3" s="2">
         <v>44582</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="E3" t="s">
-        <v>96</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -825,16 +1047,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C4" s="2">
         <v>44582</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="E4" t="s">
-        <v>97</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -842,16 +1064,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C5" s="2">
         <v>44581</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="E5" t="s">
-        <v>98</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -859,16 +1081,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C6" s="2">
         <v>44581</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
       <c r="E6" t="s">
-        <v>99</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -876,16 +1098,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C7" s="2">
         <v>44581</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="E7" t="s">
-        <v>100</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -893,16 +1115,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C8" s="2">
         <v>44581</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -910,16 +1132,16 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="C9" s="2">
         <v>44580</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="E9" t="s">
-        <v>102</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -927,16 +1149,16 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="C10" s="2">
         <v>44580</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="E10" t="s">
-        <v>103</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -944,16 +1166,16 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C11" s="2">
         <v>44579</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="E11" t="s">
-        <v>104</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -961,16 +1183,16 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C12" s="2">
-        <v>44577</v>
+        <v>44578</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="E12" t="s">
-        <v>105</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -978,16 +1200,16 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="C13" s="2">
         <v>44577</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="E13" t="s">
-        <v>106</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -995,16 +1217,16 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="C14" s="2">
-        <v>44576</v>
+        <v>44577</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>77</v>
+        <v>117</v>
       </c>
       <c r="E14" t="s">
-        <v>107</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1012,16 +1234,16 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="C15" s="2">
-        <v>44575</v>
+        <v>44576</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="E15" t="s">
-        <v>108</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1029,16 +1251,13 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="C16" s="2">
         <v>44575</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1046,16 +1265,16 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C17" s="2">
-        <v>44574</v>
+        <v>44575</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="E17" t="s">
-        <v>110</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1063,16 +1282,16 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="C18" s="2">
         <v>44574</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>81</v>
+        <v>121</v>
       </c>
       <c r="E18" t="s">
-        <v>111</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1080,16 +1299,16 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="C19" s="2">
-        <v>44573</v>
+        <v>44574</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="E19" t="s">
-        <v>112</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1097,16 +1316,16 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="C20" s="2">
         <v>44573</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
       <c r="E20" t="s">
-        <v>113</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1114,16 +1333,16 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="C21" s="2">
-        <v>44572</v>
+        <v>44573</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="E21" t="s">
-        <v>114</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1131,16 +1350,16 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="C22" s="2">
-        <v>44571</v>
+        <v>44572</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="E22" t="s">
-        <v>115</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1148,16 +1367,16 @@
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="C23" s="2">
         <v>44571</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="E23" t="s">
-        <v>116</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1165,16 +1384,16 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C24" s="2">
         <v>44571</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="E24" t="s">
-        <v>117</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1182,16 +1401,13 @@
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="C25" s="2">
-        <v>44570</v>
+        <v>44571</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1199,16 +1415,16 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="C26" s="2">
         <v>44570</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="E26" t="s">
-        <v>119</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1216,16 +1432,16 @@
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C27" s="2">
         <v>44570</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="E27" t="s">
-        <v>120</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1233,16 +1449,16 @@
         <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="C28" s="2">
         <v>44570</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E28" t="s">
-        <v>121</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1250,16 +1466,16 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="C29" s="2">
-        <v>44569</v>
+        <v>44570</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>92</v>
+        <v>132</v>
       </c>
       <c r="E29" t="s">
-        <v>122</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1267,16 +1483,16 @@
         <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C30" s="2">
-        <v>44568</v>
+        <v>44569</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>93</v>
+        <v>133</v>
       </c>
       <c r="E30" t="s">
-        <v>123</v>
+        <v>181</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1284,16 +1500,344 @@
         <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="C31" s="2">
         <v>44568</v>
       </c>
       <c r="D31" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E31" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="2">
+        <v>44568</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="2">
+        <v>44567</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="2">
+        <v>44567</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="2">
+        <v>44567</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="2">
+        <v>44566</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="2">
+        <v>44566</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E37" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" s="2">
+        <v>44566</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="2">
+        <v>44565</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E39" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="2">
+        <v>44565</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" t="s">
         <v>94</v>
       </c>
-      <c r="E31" t="s">
-        <v>124</v>
+      <c r="C41" s="2">
+        <v>44565</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" s="2">
+        <v>44564</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E42" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="2">
+        <v>44564</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E43" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" s="2">
+        <v>44563</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E44" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="2">
+        <v>44562</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E45" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" s="2">
+        <v>44561</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E46" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" s="2">
+        <v>44561</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E47" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" s="2">
+        <v>44560</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E48" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" s="2">
+        <v>44560</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="2">
+        <v>44560</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E50" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" t="s">
+        <v>104</v>
+      </c>
+      <c r="C51" s="2">
+        <v>44560</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E51" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -1328,6 +1872,26 @@
     <hyperlink ref="D29" r:id="rId28"/>
     <hyperlink ref="D30" r:id="rId29"/>
     <hyperlink ref="D31" r:id="rId30"/>
+    <hyperlink ref="D32" r:id="rId31"/>
+    <hyperlink ref="D33" r:id="rId32"/>
+    <hyperlink ref="D34" r:id="rId33"/>
+    <hyperlink ref="D35" r:id="rId34"/>
+    <hyperlink ref="D36" r:id="rId35"/>
+    <hyperlink ref="D37" r:id="rId36"/>
+    <hyperlink ref="D38" r:id="rId37"/>
+    <hyperlink ref="D39" r:id="rId38"/>
+    <hyperlink ref="D40" r:id="rId39"/>
+    <hyperlink ref="D41" r:id="rId40"/>
+    <hyperlink ref="D42" r:id="rId41"/>
+    <hyperlink ref="D43" r:id="rId42"/>
+    <hyperlink ref="D44" r:id="rId43"/>
+    <hyperlink ref="D45" r:id="rId44"/>
+    <hyperlink ref="D46" r:id="rId45"/>
+    <hyperlink ref="D47" r:id="rId46"/>
+    <hyperlink ref="D48" r:id="rId47"/>
+    <hyperlink ref="D49" r:id="rId48"/>
+    <hyperlink ref="D50" r:id="rId49"/>
+    <hyperlink ref="D51" r:id="rId50"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20220124
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="263">
   <si>
     <t>Press Title</t>
   </si>
@@ -31,6 +31,24 @@
     <t>Page Content</t>
   </si>
   <si>
+    <t>全國醫院即日起除例外情形，停止開放探病，並調整住院病人、陪(探)病者及醫療照護人員篩檢及疫苗接種等相關規定</t>
+  </si>
+  <si>
+    <t>因應國內COVID-19疫情發展，指揮中心1/24起調整全國住宿式長照機構訪客及新進住民管理等應變措施</t>
+  </si>
+  <si>
+    <t>為降低醫療量能負擔，首批我國採購之COVID-19口服抗病毒藥Molnupiravir抵臺，提供具重症風險因子之輕中度確診個案治療使用</t>
+  </si>
+  <si>
+    <t>新增51例COVID-19確定病例，分別為15例本土及36例境外移入</t>
+  </si>
+  <si>
+    <t>1月25日至2月7日維持第二級疫情警戒標準，並調整相關規定，請民眾自主落實防疫措施，共同維護國內社區安全</t>
+  </si>
+  <si>
+    <t>新增89例COVID-19確定病例，分別為52例本土及37例境外移入</t>
+  </si>
+  <si>
     <t>新增130例COVID-19確定病例，分別為82例本土及48例境外移入</t>
   </si>
   <si>
@@ -43,21 +61,6 @@
     <t>因應帛琉近期疫情，指揮中心說明相關檢疫應變措施</t>
   </si>
   <si>
-    <t>1月21日上午8時「數位新冠病毒健康證明」開放國內使用</t>
-  </si>
-  <si>
-    <t>自1月21日起，前往部分休閒娛樂場所應配合出示完整接種COVID-19疫苗紀錄</t>
-  </si>
-  <si>
-    <t>新增37例COVID-19確定病例，分別為13例本土及24例境外移入</t>
-  </si>
-  <si>
-    <t>自1月20日零時起，增列印度及東南亞航線航班旅客於落地時採驗，檢驗結果陽性後送醫院或集中檢疫所/加強版防疫旅宿</t>
-  </si>
-  <si>
-    <t>新增54例COVID-19確定病例，分別為10例本土及44例境外移入</t>
-  </si>
-  <si>
     <t>新增66例COVID-19確定病例，分別為17例本土及49例境外移入</t>
   </si>
   <si>
@@ -103,21 +106,6 @@
     <t>新增32例COVID-19確定病例，分別為6例本土及26例境外移入</t>
   </si>
   <si>
-    <t>因應國內發生Omicron變異株本土確診病例，指揮中心自即日起調整醫院陪(探)病管制及醫療照護人員管理等醫療應變措施</t>
-  </si>
-  <si>
-    <t>指揮中心即日起調整北北基桃住宿式長照機構訪客及新進住民管理等COVID-19應變措施</t>
-  </si>
-  <si>
-    <t>1月9日至24日維持第二級疫情警戒標準，並調整相關規定，請民眾持續配合防疫措施</t>
-  </si>
-  <si>
-    <t>新增60例COVID-19確定病例，分別為11例本土及49例境外移入</t>
-  </si>
-  <si>
-    <t>新增44例COVID-19確定病例，分別為2例本土及42例境外移入</t>
-  </si>
-  <si>
     <t>即日起請已接種兩劑COVID-19疫苗且滿12週並滿18歲民眾，儘速接種疫苗追加劑</t>
   </si>
   <si>
@@ -181,6 +169,93 @@
     <t>台積電、鴻海永齡、慈濟三間企業和民間團體捐贈之第十五批BNT疫苗93.83萬劑於今(30)日上午抵臺</t>
   </si>
   <si>
+    <t>新增14例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>新增19例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>為因應我國民眾能加速入境歐盟等國家，我國「數位新冠病毒健康證明」於12月28日上午8時開放下載</t>
+  </si>
+  <si>
+    <t>因應國際Omicron變異株疫情迅速擴散，指揮中心入境旅客PCR檢驗報告調整為「2日內」報告並改以「採檢日」為計算基準</t>
+  </si>
+  <si>
+    <t>關鍵「疫」戰，感謝有您！指揮中心向COVID-19疫情期間貢獻卓越的第一線防疫英雄致謝！</t>
+  </si>
+  <si>
+    <t>指揮中心外部專家調查小組說明中研院ABSL-3實驗室感染事件初步調查結果</t>
+  </si>
+  <si>
+    <t>指揮中心說明如參與國內臨床試驗計畫，接種未經我國食品藥物管理署核准使用COVID-19疫苗之民眾，後續疫苗接種相關因應方式</t>
+  </si>
+  <si>
+    <t>新增13例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>歡慶佳節，「定期篩檢」是給自己和伴侶最好的禮物</t>
+  </si>
+  <si>
+    <t>春節檢疫專案擇C方案(7+7+7)入境者返家注意事項</t>
+  </si>
+  <si>
+    <t>指揮中心全面檢討防疫旅宿防疫作為，3大強化措施精進管理</t>
+  </si>
+  <si>
+    <t>新增10例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>ACIP專家建議，符合COVID-19疫苗接種對象與間隔之民眾，應盡速完成基礎劑接種；已完成基礎劑接種且滿5個月之民眾，應接種追加劑</t>
+  </si>
+  <si>
+    <t>指揮中心說明中研院P3實驗室事件調查進度</t>
+  </si>
+  <si>
+    <t>新增11例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>新增6例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>新增15例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>因應近期疫情，指揮中心啟動防疫旅宿四大強化作為</t>
+  </si>
+  <si>
+    <t>新增12例COVID-19確定病例，分別為1例本土及11例境外移入</t>
+  </si>
+  <si>
+    <t>新增7例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>新增5例COVID-19境外移入確定病例</t>
+  </si>
+  <si>
+    <t>指揮中心宣布自12月14日至12月27日維持疫情警戒標準為第二級，請民眾持續配合防疫措施</t>
+  </si>
+  <si>
+    <t>指揮中心已全面提供民眾預約接種COVID-19疫苗第一、二劑，及已完整接種疫苗且滿５個月者接種追加劑，請民眾儘速完成二劑疫苗接種，以獲得完整免疫保護力</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/kVDslqExqB7BSiqJuFzXCg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/cU2pYInOEJ4NOhg-uOH5Zg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/yxiRZA3J-EAjVZ3CcK4n9Q?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Eg5gZrriSQBA--KxcspeTg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/y6MiRdu9X-y3kAs1UrXvng?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/RpwW0PpibHaRFJpatPM1HA?typeid=9</t>
+  </si>
+  <si>
     <t>/Bulletin/Detail/5MtrgzOJApOSjivffWLWRw?typeid=9</t>
   </si>
   <si>
@@ -193,21 +268,6 @@
     <t>/Bulletin/Detail/lVU_tRUutNI667QAZYcj7g?typeid=9</t>
   </si>
   <si>
-    <t>/Bulletin/Detail/mAWzcQcUVI2XPmIdtic3jg?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/VSnz3gIu4mKSTrTFXHqIzQ?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/X5oSF1tnbyvV8_Nfrl31lg?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/Mhpv_WBf9Gw4pLB1hMe1hg?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/uomdnhoUoWvMFa8ce4zYMQ?typeid=9</t>
-  </si>
-  <si>
     <t>/Bulletin/Detail/5XT_6l4aNN_OQfb208cYtg?typeid=9</t>
   </si>
   <si>
@@ -253,21 +313,6 @@
     <t>/Bulletin/Detail/BLTzFri3lYiciwF15SmVqg?typeid=9</t>
   </si>
   <si>
-    <t>/Bulletin/Detail/jrbh2wkghEi4QBYwD6WRew?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/q7Jr3KpXpoIPMblJUG49zQ?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/_g-303qhIANyJ29lbGiXYQ?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/NPmLr1LSFi4UCOINnkDDiw?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/QcNPHHjaJVEr-bnW4hG5RQ?typeid=9</t>
-  </si>
-  <si>
     <t>/Bulletin/Detail/DViInYHA83okHIasbqONZQ?typeid=9</t>
   </si>
   <si>
@@ -331,6 +376,105 @@
     <t>/Bulletin/Detail/WIMrcWpPk8g16xjOZR_e4g?typeid=9</t>
   </si>
   <si>
+    <t>/Bulletin/Detail/uC2CvyAZKpXLB4pbfUDEwA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Vr-xa_jxF7CS4mlKHSpHgw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/-rE5uMCRLrzdP16Sf7m5UA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/_VRX4ciyxXBAZZrWlce-FQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/-GpLgraJhhrmCF_EV5snAg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/DyYwMZYOnDPQaxZXyYkGag?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/U_G8thyYx_NXqs4bt22mLQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/ZRGaGQGvgOVp0sgi7p0Flw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/3PbK6u1juCPF_H5RpSmg1A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/K6-Py9CkPH7F7fbEhkN-cg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/kWxZwn01NkNft8vvuR-8iQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/M936bwIy8h1c3o0JAGx6XQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/OFCGVMPdO7s8EroSL08bnw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/ZCHA5BJcbAHqa3rEfKzgiQ?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/L-qJBbrKStZuXh0N0Y1B7A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/DDtX98YMnWlt1E5YooyXig?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/IgdrNGmRzvUV_y1dDQZLbg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/GqrECv8g1A5pcuUsJbNwyA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/xpr8IEBdD6agTmKYO0do_Q?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/ZEZs-BpahQJyNxIgZMvnmw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/g07xJkUnioeBi2K4x_oa8A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/j0Lv5A4_bB5XCnhGvdJYzw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/DF7ogeZZ4Sq2mcsf3p5V1A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/jYSkhkTuIrL1g8h4BnsiPw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/8ZtmGnmnTDndGf1ih_-ZgA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/BawHgYTsb-Ifbw2VpNUErA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/6_2cOpRBTVjg_3-72yJMVQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/kVDslqExqB7BSiqJuFzXCg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/cU2pYInOEJ4NOhg-uOH5Zg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/yxiRZA3J-EAjVZ3CcK4n9Q?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Eg5gZrriSQBA--KxcspeTg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/y6MiRdu9X-y3kAs1UrXvng?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/RpwW0PpibHaRFJpatPM1HA?typeid=9</t>
+  </si>
+  <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/5MtrgzOJApOSjivffWLWRw?typeid=9</t>
   </si>
   <si>
@@ -343,21 +487,6 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/lVU_tRUutNI667QAZYcj7g?typeid=9</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/mAWzcQcUVI2XPmIdtic3jg?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/VSnz3gIu4mKSTrTFXHqIzQ?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/X5oSF1tnbyvV8_Nfrl31lg?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/Mhpv_WBf9Gw4pLB1hMe1hg?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/uomdnhoUoWvMFa8ce4zYMQ?typeid=9</t>
-  </si>
-  <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/5XT_6l4aNN_OQfb208cYtg?typeid=9</t>
   </si>
   <si>
@@ -403,21 +532,6 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/BLTzFri3lYiciwF15SmVqg?typeid=9</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/jrbh2wkghEi4QBYwD6WRew?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/q7Jr3KpXpoIPMblJUG49zQ?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/_g-303qhIANyJ29lbGiXYQ?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/NPmLr1LSFi4UCOINnkDDiw?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/QcNPHHjaJVEr-bnW4hG5RQ?typeid=9</t>
-  </si>
-  <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/DViInYHA83okHIasbqONZQ?typeid=9</t>
   </si>
   <si>
@@ -481,93 +595,126 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/WIMrcWpPk8g16xjOZR_e4g?typeid=9</t>
   </si>
   <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/uC2CvyAZKpXLB4pbfUDEwA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Vr-xa_jxF7CS4mlKHSpHgw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/-rE5uMCRLrzdP16Sf7m5UA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/_VRX4ciyxXBAZZrWlce-FQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/-GpLgraJhhrmCF_EV5snAg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/DyYwMZYOnDPQaxZXyYkGag?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/U_G8thyYx_NXqs4bt22mLQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/ZRGaGQGvgOVp0sgi7p0Flw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/3PbK6u1juCPF_H5RpSmg1A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/K6-Py9CkPH7F7fbEhkN-cg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/kWxZwn01NkNft8vvuR-8iQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/M936bwIy8h1c3o0JAGx6XQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/OFCGVMPdO7s8EroSL08bnw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/ZCHA5BJcbAHqa3rEfKzgiQ?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/L-qJBbrKStZuXh0N0Y1B7A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/DDtX98YMnWlt1E5YooyXig?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/IgdrNGmRzvUV_y1dDQZLbg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/GqrECv8g1A5pcuUsJbNwyA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/xpr8IEBdD6agTmKYO0do_Q?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/ZEZs-BpahQJyNxIgZMvnmw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/g07xJkUnioeBi2K4x_oa8A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/j0Lv5A4_bB5XCnhGvdJYzw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/DF7ogeZZ4Sq2mcsf3p5V1A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/jYSkhkTuIrL1g8h4BnsiPw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/8ZtmGnmnTDndGf1ih_-ZgA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/BawHgYTsb-Ifbw2VpNUErA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/6_2cOpRBTVjg_3-72yJMVQ?typeid=9</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-24\$\@\$中央流行疫情指揮中心今(24)日表示，因應近期國內發生數名本土COVID-19確定病例，為防範COVID-19於住宿式長照機構內傳播風險，即日(1/24)起調整全國住宿式長照機構COVID-19應變措施，重點說明如下：\$\@\$一、訪客管理：除例外情形暫停探視。例外情形經機構同意可探視者，應出具訪視前3天內採檢之自費篩檢陰性證明。\$\@\$二、新進住民管理：新進住民不論是否已完成COVID-19疫苗接種，須配合以下兩項措施，包括：\$\@\$(一)均須出具入住機構前3天內採檢之自費篩檢陰性證明；\$\@\$(二)依機構人員完成COVID-19疫苗應接種劑次14天以上比率，採取對應之管制措施：\$\@\$1.如為工作人員達90%以上且住民達80%以上之機構，自入住機構次日起14天內避免參加團體活動；\$\@\$2.如為工作人員未達90%或住民未達80%之機構，則自入住次日起隔離14天，或自入住次日起隔離7天，於第7天進行自費篩檢，陰性者可解除隔離，但仍須避免參加團體活動，之後於第14天再進行1次自費篩檢。\$\@\$指揮中心將持續監測國內外疫情發展，滾動修正相關應變策略。請各類住宿式長照機構務必落實執行「第2級疫情警戒期間住宿式長照機構COVID-19強化管制措施」及指揮中心公布之COVID-19相關措施指引，並鼓勵完整接種COVID-19疫苗基礎劑12週後之機構工作人員與住民儘速接種1劑追加劑疫苗，以提升個人及群體免疫力，確保工作人員及住民健康安全。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-24\$\@\$中央流行疫情指揮中心今(24)日表示，我國向美商默沙東公司採購之COVID-19口服抗病毒藥Molnupiravir，首批2,016人份療程已於今日清晨運抵臺灣，將於完成通關程序後儘速配撥，提供具有重症風險因子之輕中度COVID-19個案治療使用，降低醫療量能負擔。\$\@\$指揮中心指出，依據國際研究顯示，新冠病毒感染患者輕症比率大約佔8成左右，但其中約9％的患者可能惡化為重症，主要的風險因子包括65歲以上長者、肥胖、慢性腎病、心血管疾病/高血壓、慢性肺疾、免疫抑制疾病/免疫抑制治療等影響免疫功能之疾病，以及懷孕等，且其病程演化迅速，甚至導致死亡。截至本(111)年1月24日監測資料，國內輕中度COVID-19確診病例約佔所有確診個案84%，死亡病例數佔確診病例4.6%。\$\@\$指揮中心說明，Molnupiravir之療效及安全性已有部分證據支持，美國FDA及國際間已陸續發布緊急使用授權(EUA)核准於臨床使用，以治療輕度至中度SARS-CoV-2感染且有重症危險因子之高風險患者，降低個案轉為重症需住院之風險，我國衛福部食藥署亦於今年1月13日同意依據藥事法第48條之2規定，核准其專案輸入。\$\@\$指揮中心進一步說明，經諮詢專家意見，已將該藥物之使用建議納入我國「新型冠狀病毒(SARS-CoV-2)感染臨床處置暫行指引」，並採購儲備5,040人份療程，規劃分批配撥至集中檢疫所/加強版防疫專責旅宿之主責醫院，經醫師評估治療效益與風險，並充分告知後，給予符合條件個案治療。\$\@\$指揮中心表示，全球疫情持續嚴峻，Omicron變異株擴及多國，對國內公共衛生及醫療量能構成威脅，指揮中心將持續密切關注國際COVID-19口服抗病毒藥物之研發使用情形，積極儲備適當藥物供國內個案治療使用。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-24\$\@\$中央流行疫情指揮中心今(24)日公布國內新增51例COVID-19確定病例，分別為15例本土個案及36例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為10例男性、5例女性，年齡介於10多歲至50多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為21例男性、15例女性，年齡介於未滿5歲至70多歲，分別自美國(20例)、帛琉及印尼(各2例)、香港、越南、荷蘭、海地、菲律賓、多明尼加及比利時(各1例)移入；另5例調查中。入境日介於今(2022)年1月9日至1月23日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,463,663例新型冠狀病毒肺炎相關通報(含5,444,547例排除)，其中18,376例確診，分別為3,404例境外移入，14,918例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計119例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月24日新增本土COVID-19確診個案表.pdf\$\@\$1月24日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-23\$\@\$中央流行疫情指揮中心今(23)日公布國內新增89例COVID-19確定病例，分別為52例本土個案及37例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為32例男性、20例女性，年齡介於未滿5歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為17例男性、20例女性，年齡介於未滿10歲至60多歲，分別自美國(12例)、法國(3例)、英國(2例)、丹麥、印度、烏克蘭、菲律賓、土耳其、澳大利亞(各1例)移入；另14例調查中。入境日介於今(2022)年1月8日至1月22日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,441,110例新型冠狀病毒肺炎相關通報(含5,422,031例排除)，其中18,325例確診，分別為3,368例境外移入，14,903例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增2例空號病例(案17934、案17970，再次採檢為陰性改判排除)，累計119例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月23日新增境外移入COVID-19確診個案表.pdf\$\@\$1月23日新增本土COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
     <t>發佈日期：2022-01-22\$\@\$中央流行疫情指揮中心今(22)日公布國內新增130例COVID-19確定病例，分別為82例本土個案及48例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為12例男性、70例女性，年齡介於未滿10歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為29例男性、19例女性，年齡介於未滿5歲至70多歲，分別自美國(13例)、加拿大及新加坡(各4例)、菲律賓(3例)、印度、土耳其及香港(各2例)、奧地利、奈及利亞、義大利、柬埔寨、德國、越南及巴西(各1例)移入；另11例調查中。入境日介於去(2021)年12月31日至今(2022)年1月21日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,418,957例新型冠狀病毒肺炎相關通報(含5,400,086例排除)，其中18,238例確診，分別為3,331例境外移入，14,853例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案18182，再次採檢為陰性，改判排除)，累計117例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月22日新增本土COVID-19確診個案表.pdf\$\@\$1月22日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-21\$\@\$中央流行疫情指揮中心今(21)日公布國內新增68例COVID-19確定病例，分別為23例本土個案及45例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為10例男性、13例女性，年齡介於未滿10歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為20例男性、24例女性及1例調查中，年齡介於未滿5歲至70多歲，分別自美國(17例)、菲律賓(4例)、越南及以色列(各3例)、加拿大(2例)、波蘭、澳大利亞、韓國、新加坡、瑞典、俄羅斯、英國及愛爾蘭(各1例)移入；另8例調查中。入境日介於今(2022)年1月5日至1月20日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,394,042例新型冠狀病毒肺炎相關通報(含5,375,246例排除)，其中18,109例確診，分別為3,283例境外移入，14,772例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計116例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月21日新增本土COVID-19確診個案表.pdf\$\@\$1月21日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-21\$\@\$中央流行疫情指揮中心今(21)日表示，台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的第十六批BNT疫苗99.45萬劑，已於今日上午順利運抵桃園國際機場，並在完成通關程序後，直接運送至指定冷儲物流中心進行後續檢驗封緘作業。\$\@\$指揮中心說明，由台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的BNT疫苗1,500萬劑，目前共計到貨1433.07萬劑，分別為首批9月2日93萬劑、第二批9月9日91萬劑、第三批9月30日54萬劑、第四批10月1日67萬劑、第五批10月4日27萬劑、第六批10月7日88.92萬劑、第七批10月8日88.92萬劑、第八批10月14日82.7萬劑、第九批10月28日90.21萬劑、第十批10月29日91.03萬劑、第十一批11月5日87.17萬劑、第十二批11月12日92.66萬劑、第十三批11月25日93.83萬劑、第十四批12月9日192.35萬劑、第十五批12月30日93.83萬劑，以及本批99.45萬劑。本批疫苗效期至2022年5月25日，將由指揮中心統籌運用，儘速提供民眾接種。\$\@\$對於台積電、鴻海暨永齡基金會、慈濟基金會三間企業和民間團體積極協助，提供更多的疫苗讓民眾接種，加速提升臺灣疫苗覆蓋率，指揮中心再次表達由衷的謝意。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-20\$\@\$中央流行疫情指揮中心今(20)日表示，鑒於帛琉疫情升溫，為確保社區防疫安全，自帛琉來臺旅客，除搭機前須持二日內核酸檢測報告外，入境仍依現行作法，採綠色專屬通道，並強化相關入境採檢及檢疫措施，請赴帛琉或自帛琉抵臺旅客，務必配合當地及回臺相關防疫及檢疫措施，以保障國內社區安全。\$\@\$指揮中心指出，強化入境採檢及檢疫措施將自今(2022)年1月22日(含)起實施，入境旅客公費入住集中檢疫所實施5天檢疫，接續加強自主健康管理9天，再進行一般自主健康管理7天，並配合入境時(集中檢疫所採檢)、第5天及第13至14天進行PCR檢測，第8天、第11天及一般自主健康管理期滿(第20至21天)以家用快篩試劑各檢測1次。另提醒旅客於到訪帛琉期間，請務必落實自我健康監測，並確實遵守指揮中心及帛國的防疫措施，如佩戴口罩、勤洗手及保持社交距離等規範，以維護自身的健康安全。\$\@\$指揮中心說明，針對1月22日分別有旅遊團啟程至帛琉，以及自帛琉入境旅客，請儘速辦理下列事項：\$\@\$(一) 駐帛琉共和國大使館將持續提供當地疫情風險資訊予交通部觀光局，以利旅行社向旅客宣達該國疫情風險，以及須配合的防疫措施（包括從事醫療照護工作人員，於加強自主健康管理期間不得上班）。\$\@\$(二) 為確保赴帛琉旅客瞭解當地疫情風險，駐帛琉共和國大使館亦將於機場加強宣導。\$\@\$(三) 有關自帛琉入境之14名旅客(含後送轉診病人)，將請駐帛琉共和國大使館轉達調整後的防疫措施，並請醫療應變組瞭解後送轉診病人的就醫需求，以利預先調度。\$\@\$此外，外交部已調整帛琉旅遊警示為「提醒注意」，並將召集交通部與駐帛琉共和國大使館共同研商合理的退費機制。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-20\$\@\$中央流行疫情指揮中心今(20)日表示，我國「數位新冠病毒健康證明」自去(110)年12月28日上線後已核發超過26萬份。考量國內外疫情升溫，各界建議及需求，指揮中心將於今(111)年1月21日上午8時開放「數位新冠病毒健康證明」供國內使用，共計三大功能：所有在國內接種者皆可下載、符合歐盟規範的查驗程式，可驗證60國的證明、提供具實名制的APP作為證明載具。\$\@\$指揮中心指出，原本下載限持有效護照者，現以戶口名簿的戶號取代，民眾可以電腦或手機上網申辦「數位新冠病毒健康證明」（ https://dvc.mohw.gov.tw ），注意事項說明如下：\$\@\$一、確認身分：\$\@\$(一)國人：(1)身分證號+健保卡號+戶口名簿戶號；(2) FIDO；(3)自然人憑證。三種方式擇一。\$\@\$(二)外來人口：(1)統一證號+健保卡號；(2) 統一證號+入出境證號；(3) 統一證號+護照號碼。三種方式擇一。\$\@\$二、選擇項目：選擇「疫苗接種數位證明」或「檢驗結果數位證明」。\$\@\$三、取得證明：於申請成功畫面點選「下載/列印 數位證明」，檔案格式為PDF，提醒要先保存於行動裝置或電腦硬碟中，再視個人需要列印紙本。無列印設備但又有列印需求者，可於申請成功畫面選擇超商並點選「取得超商列印碼」，系統將產製超商取件條碼或取件編號，請自行攜碼至超商付費列印。\$\@\$此次僅變更確認身分方式，方便未持有護照者下載。具有效護照民眾申辦數位證明時仍會產出護照號碼，未來不必為出國另行下載；不具有效護照民眾者護照號碼欄位顯示為「Not Issued」。\$\@\$「數位新冠病毒健康證明」查驗程式係網頁形式（ https://dvc.mohw.gov.tw/verifier-web ），不需下載安裝，民眾也可在衛福部官網取得連結，該網頁不會保留受查驗者的個資，符合歐盟GDPR，使用步驟如下：\$\@\$一、前往網站：使用具備相機及網頁瀏覽器的手機、電腦等，開啟瀏覽器前往上述網址。\$\@\$二、同意隱私權聲明、允許取用相機權限。\$\@\$三、不退出查驗網頁且不中斷網路者，可續使用並維持最新功能，退出或中斷者可重新上網更新。\$\@\$查驗程式以顏色、圖示及文字顯示查驗結果，綠色、打勾為通過，紅色、打叉為不通過，黃色、三角驚嘆號為待確認狀態（包括：接種不完整、效期不符、非我國同意的疫苗或檢驗等），不合規格的QR code則會出現解析錯誤的訊息。驗證程式個人基本資料僅會顯示姓名及出生年月日，如需嚴格確認是否為本人持有，建議仍需搭配其它身分證件。由於我國已是歐盟數位新冠證明(EU-DCC)的成員，故本查驗程式也可查證持同樣規格由其它國家發行的疫苗、核酸檢驗數位證明，及部分有發行康復證明的國家。\$\@\$指揮中心提醒，依據世界衛生組織(WHO)規範，疫苗證明可採紙本或數位方式，檢驗陰性或康復證明亦可做為健康證明，數位證明僅是方式之一，民眾有多元方式可提供各場所查驗。\$\@\$另外，指揮中心亦已備有標準的應用軟體介接程式(API)供國內具實名制功能的APP介接取得民眾自己的數位證明，並以APP為載具。發行或管理APP者，確認符合個資法及GDPR、身分驗證強度不低於本數位證明平臺，且APP後臺不得留存數位證明，請向指揮中心正式申請。\$\@\$為更新原有版本的功能，申辦平台預計今年1月20日下午5時至次(21)日上午8時停止服務進行更版，有急需出國使用者，請先提前下載。詳細下戴及驗證系統操作方式可以參考衛生福利部官網數位證明專區( https://covid19.mohw.gov.tw/ch/np-5345-205.html )。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-20\$\@\$中央流行疫情指揮中心今(20)日表示，因應Omicron新型變異株之威脅，且國內本土疫情尚未平息，存在社區傳播風險，自今(2022)年1月21日起，民眾前往「歌廳、舞廳、夜總會、俱樂部、酒家、酒吧、酒店(廊)、理容院(觀光理髮、視聽理容)及特種咖啡茶室、夜店、舞場、三溫暖」等休閒娛樂場所時，應配合出示完整接種COVID-19疫苗紀錄，始得入內活動消費。接種紀錄除出示「紙本疫苗接種卡」外，亦可使用「健保快易通」或「數位新冠病毒健康證明」提供檢視。\$\@\$指揮中心說明，上述休閒娛樂場所具有接觸不特定人及無法保持社交距離之特性，COVID-19傳播風險相對較高，為降低於場所消費期間接觸染疫之風險，強化場所之防疫管理措施，除維持該等場所工作人員皆應接種COVID-19疫苗2劑且滿14天，未完整接種者，應每週定期篩檢陰性，始得提供服務外，自1月21日起調整民眾前往消費時，須配合出示完整接種COVID-19疫苗2劑且滿14天紀錄，始得進場，請民眾務必配合，也請業者落實查核，使顧客安心消費，同時保護員工健康安全。\$\@\$指揮中心另指出，針對醫院及住宿式長照機構等現行已有針對COVID-19疫苗接種情形進行規範之場域，請民眾依規定，配合出示COVID-19疫苗紀錄，接種紀錄同樣可使用「紙本疫苗接種卡」、「健保快易通」或「數位新冠病毒健康證明」提供檢視。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-20\$\@\$中央流行疫情指揮中心今(20)日公布國內新增37例COVID-19確定病例，分別為13例本土個案及24例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為5例男性、8例女性，年齡介於未滿5歲至80多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為13例男性、11例女性，年齡介於10多歲至50多歲，分別自美國(10例)、越南(3例)、法國及澳大利亞(各2例)、巴拉圭及沙烏地阿拉伯(各1例)移入；另5例調查中。入境日介於今(2022)年1月5日至1月19日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,363,205例新型冠狀病毒肺炎相關通報(含5,344,301例排除)，其中18,041例確診，分別為3,238例境外移入，14,749例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案18119，再次採檢為陰性，改判排除)，累計116例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月20日新增境外移入COVID-19確診個案表.pdf\$\@\$1月20日新增本土COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-19\$\@\$中央流行疫情指揮中心今(19)日表示，鑒於印度、東南亞疫情持續升溫，為及時防堵疫情，自今(2022)年1月20日零時起(航班表定抵臺時間)，增列印度及東南亞(菲律賓、柬埔寨、泰國、越南、緬甸、印尼、馬來西亞、新加坡)航線航班旅客，於抵臺時進行落地公費採檢及快速核酸檢驗，檢驗結果陰性者接續入境通關程序，且應搭乘防疫車輛前往防疫旅宿/集中檢疫所完成檢疫；檢驗結果陽性者，指派專人完成證照查驗後，由空側後送醫院或集中檢疫所/加強版防疫旅宿。\$\@\$指揮中心指出，旅客抵臺時須進行「落地採驗」之航班為歐美、中東、紐澳及本次新增之印度、東南亞航線航班，籲請旅客配合入境檢疫作業。\$\@\$指揮中心再次強調，邊境管制為防範COVID-19疫情之重要關鍵，入境旅客抵臺時應主動配合邊境檢疫措施，並依指揮中心規定的交通方式前往檢疫地點，同時遵守檢疫期間各項檢疫、防疫措施，落實全民共同抗疫，以維護國內社區安全。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-19\$\@\$中央流行疫情指揮中心今(19)日公布國內新增54例COVID-19確定病例，分別為10例本土個案及44例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為5例男性，5例女性，年齡介於未滿10歲至60多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為16例男性、24例女性、4例調查中，年齡介於未滿5歲至70多歲，分別自美國(10例)、菲律賓(6例)、阿拉伯聯合大公國(3例)、法國、西班牙及澳大利亞(各2例)、柬埔寨、韓國、英國、厄瓜多及印度(各1例)移入；另14例調查中。入境日介於去(2021)年12月29日至今(2022)年1月18日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,336,346例新型冠狀病毒肺炎相關通報(含5,317,735例排除)，其中18,005例確診，分別為3,214例境外移入，14,737例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計115例移除為空號。另今年1月6日公布之案17298境外移入病例，經病毒定序及疫調後改判為本土病例。 2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月19日新增境外移入COVID-19確診個案表.pdf\$\@\$1月19日新增本土COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-18\$\@\$中央流行疫情指揮中心今(18)日公布國內新增66例COVID-19確定病例，分別為17例本土個案及49例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為10例男性、7例女性，年齡介於未滿5歲至60多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為33例男性、16例女性，年齡介於未滿10歲至60多歲，分別自美國(21例)、越南(5例)、加拿大(4例)、英國(3例)、法國(2例)、愛爾蘭、西班牙、瑞典、菲律賓、波蘭、墨西哥及巴拿馬(各1例)移入；另7例調查中。入境日介於今(2022)年1月3日至1月17日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,306,453例新型冠狀病毒肺炎相關通報(含5,287,815例排除)，其中17,951例確診，分別為3,171例境外移入，14,726例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計115例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月18日新增本土COVID-19確診個案表.pdf\$\@\$1月18日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
     <t>發佈日期：2022-01-17\$\@\$中央流行疫情指揮中心今(17)日公布國內新增65例COVID-19確定病例，分別為17例本土個案及48例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為8例男性、9例女性，年齡介於未滿5歲至60多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為28例男性、20例女性，年齡介於未滿10歲至50多歲，分別自美國(28例)、菲律賓(2例)、法國、愛爾蘭、荷蘭、哥斯大黎加、加拿大、丹麥及德國(各1例)移入；另11例調查中。入境日介於今(2022)年1月2日至1月16日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,278,363例新型冠狀病毒肺炎相關通報(含5,258,762例排除)，其中17,885例確診，分別為3,122例境外移入，14,709例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計115例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月17日新增本土COVID-19確診個案表.pdf\$\@\$1月17日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-16\$\@\$中央流行疫情指揮中心今( 16 )日表示，因應國內本土疫情升溫，目前提供民眾於各地方政府衛生局安排/指定之合約醫療院所預約接種或隨到隨打接種站進行接種。為提供民眾多元疫苗預約管道選擇，以加速提升民眾免疫保護力，COVID-19公費疫苗預約平台(下稱預約平台)，持續於第20期提供「已完整接種兩劑COVID-19疫苗滿12週且滿18歲以上」民眾，預約接種疫苗追加劑。如已於各地方政府衛生局安排/指定之合約醫療院所完成預約之民眾，請依原已預約時段前往接種，無須再於預約平台重複預約。\$\@\$預約平台相關對象及期程說明如下：\$\@\$一、施打時程：1月24日至1月30日。\$\@\$二、符合資格對象：110年11月7日(含)前已完整接種兩劑疫苗且間隔滿12週之18歲以上民眾[即2004/1/30(含)前出生]預約接種疫苗追加劑。\$\@\$三、預約分流時程：\$\@\$(一)65歲以上：1月18日上午10時至1月22日中午12時。\$\@\$(二)50歲-64歲：1月18日中午12時至1月22日中午12時。\$\@\$(三)18歲-49歲：1月18日下午2時至1月22日中午12時。\$\@\$指揮中心提醒，民眾可於預約時段至預約平台進行預約資格查詢，不再另發送預約提醒簡訊，符合資格民眾請記得於預約時間進行預約，預約當日如遇啟動流量管制亦請配合依序排隊耐心等候預約，亦可持「COVID-19疫苗接種紀錄卡」(小黃卡)逕至各地方政府指定/安排合約醫療院所或衛生所預約接種，或所設置之隨到隨打接種站接種。\$\@\$指揮中心說明，BNT、Moderna都屬mRNA疫苗，兩者保護效果相當，請符合預約資格且有意願接種但尚未完成預約者，如欲選擇的疫苗接種點額滿，可選擇另一種疫苗接種，以儘速獲得追加保護。\$\@\$指揮中心表示，預約平台第20期僅提供民眾預約接種疫苗追加劑，若有第一劑或第二劑疫苗接種需求之民眾，請持COVID-19疫苗接種紀錄卡(小黃卡)至各地方政府指定/安排合約醫療院所或衛生所預約接種，或所設置之隨到隨打接種站接種。至1月31日止，可由地方政府衛生局提供200元(含)以下衛教品，以提升接種意願。\$\@\$指揮中心提醒，請民眾前往接種COVID-19疫苗前，應備妥「COVID-19疫苗接種紀錄卡」(小黃卡)及健保卡，並經醫生評估過往疫苗接種史及檢核接種紀錄後，提供民眾疫苗接種。另18歲至未滿20歲民眾，如自行前往接種，請持家長簽具之意願同意書，若由家長陪同前往接種，請本人與家長於現場共同簽署意願同意書。</t>
-  </si>
-  <si>
     <t>發佈日期：2022-01-16\$\@\$中央流行疫情指揮中心今(16)日公布國內新增51例COVID-19確定病例，分別為10例本土個案及41例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為2例男性、6例女性、2例調查中，年齡介於10多歲至50多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為25例男性、16例女性，年齡介於10歲至80多歲，分別自美國(14例)、墨西哥、印度、菲律賓、澳大利亞、越南及柬埔寨(各2例)、丹麥、法國、加拿大、印尼、英國(各1例)移入；另10例調查中。入境日介於去(2021)年12月22日至今(2022)年1月15日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,257,161例新型冠狀病毒肺炎相關通報(含5,236,654例排除)，其中17,820例確診，分別為3,074例境外移入，14,692例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案17765)，累計115例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月16日新增境外移入COVID-19確診個案表.pdf\$\@\$1月16日新增本土COVID-19確診個案表.pdf</t>
   </si>
   <si>
     <t>發佈日期：2022-01-15\$\@\$中央流行疫情指揮中心今(15)日公布國內新增78例COVID-19確定病例，分別為6例本土個案及72例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為2例男性、4例女性，年齡介於10多歲至30多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為38例男性、31例女性、3例調查中，年齡介於未滿5歲至60多歲，分別自美國(23例)、加拿大(10例)、印尼及越南(各3例)、法國及澳大利亞(各2例)、新加坡及德國(各1例)移入；另27例調查中。入境日介於去(2021)年11月4日至今(2022)年1月14日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,233,163例新型冠狀病毒肺炎相關通報(含5,213,414例排除)，其中17,769例確診，分別為3,033例境外移入，14,682例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案17765)，累計115例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月15日新增境外移入COVID-19確診個案表.pdf\$\@\$1月15日新增本土COVID-19確診個案表.pdf</t>
   </si>
   <si>
+    <t>發佈日期：2022-01-14\$\@\$中央流行疫情指揮中心今(14)日公布國內新增68例COVID-19確定病例，分別為11例本土個案及57例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為8例男性、3例女性，年齡介於未滿5歲至50多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為25例男性、24例女性、8例調查中，年齡介於未滿5歲至70多歲，分別自美國(17例)、加拿大(5例)、菲律賓(4例)、澳大利亞、波蘭及越南(各3例)、印尼、丹麥、法國、葡萄牙、巴西、土耳其及瑞典(各1例)移入；另15例調查中。入境日介於去(2021)年12月31日至今(2022)年1月13日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,210,348例新型冠狀病毒肺炎相關通報(含5,190,844例排除)，其中17,692例確診，分別為2,962例境外移入，14,676例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計114例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月14日新增境外移入COVID-19確診個案表.pdf\$\@\$1月14日新增本土COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
     <t>發佈日期：2022-01-14\$\@\$中央流行疫情指揮中心今( 14 )日表示，因應國內本土疫情升溫，目前提供民眾於各地方政府指定/安排合約醫療院所或衛生所預約接種，或所設置之隨到隨打接種站接種COVID-19疫苗。為提供民眾多元疫苗預約管道選擇，以加速提升民眾免疫保護力，將於1月15日開放COVID-19公費疫苗預約平台，於第19期提供「已完整接種兩劑COVID-19疫苗滿12週且滿18歲以上」民眾預約接種疫苗追加劑。如已於各地方政府指定/安排合約醫療院所或衛生所完成預約之民眾，請依原已預約時段前往接種，無須再於預約平台重複預約。\$\@\$預約平台相關對象及期程說明如下：\$\@\$一、施打時程：1月17日至1月23日。\$\@\$二、符合資格對象：2021年10月31日前已完整接種兩劑疫苗且間隔滿12週之18歲以上民眾[即2004/1/23(含)前出生]，預約接種疫苗追加劑。\$\@\$三、預約分流時程：\$\@\$(一)65歲以上：1月15日上午10時至1月16日中午12時。\$\@\$(二)50歲-64歲：1月15日中午12時至1月16日中午12時。\$\@\$(三)18歲-49歲：1月15日下午2時至1月16日中午12時。\$\@\$指揮中心說明，民眾可於1月14日下午2時起至預約平台進行預約資格查詢，不再另發送預約提醒簡訊。符合資格民眾請記得於預約時間進行預約，預約當日如遇啟動流量管制，請配合依序排隊、耐心等候。若符合本期資格但未能預約成功者，請於下週下一期平台開放時再行預約。符合本期資格但未預約成功、以及有第一劑或第二劑疫苗接種需求之民眾，可持「COVID-19疫苗接種紀錄卡」(小黃卡)逕至各地方政府指定/安排合約醫療院所或衛生所預約接種，或所設置之隨到隨打接種站接種。\$\@\$指揮中心提醒，請民眾前往接種COVID-19疫苗前，應備妥「COVID-19疫苗接種紀錄卡」及健保卡，並經醫生評估過往疫苗接種史及檢核接種紀錄後，提供民眾疫苗接種。另18歲至未滿20歲民眾，如自行前往接種，請持家長簽具之意願同意書，若由家長陪同前往接種，請本人與家長於現場共同簽署意願同意書。</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-13\$\@\$中央流行疫情指揮中心今(13)日公布國內新增65例COVID-19確定病例，分別為14例本土個案及51例境外移入；另確診個案中新增1例死亡。\$\@\$指揮中心表示，今日新增本土個案為3例男性、11例女性，年齡介於未滿10歲至60多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為17例男性、28例女性、6例調查中，年齡介於未滿5歲至70多歲，分別自美國(28例)、越南(3例)、法國、澳大利亞、菲律賓及英國(各2例)、阿拉伯聯合大公國、哥斯大黎加、瓜地馬拉、印尼、德國、孟加拉、丹麥、印度及義大利(各1例)移入；另3例調查中。入境日介於去(2021)年12月29日至今(2022)年1月12日；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增1例死亡個案(案16906)，為50多歲本國籍男性，具慢性病史；去年12月於越南確診，當月17日由國際緊急醫療專機從越南接運返國住院隔離治療，今年1月9日死亡。\$\@\$指揮中心統計，截至目前國內累計5,187,725例新型冠狀病毒肺炎相關通報(含5,168,285例排除)，其中17,624例確診，分別為2,905例境外移入，14,665例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計114例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月13日新增本土COVID-19確診個案表.pdf\$\@\$1月13日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
     <t>發佈日期：2022-01-13\$\@\$中央流行疫情指揮中心今(13)日表示，AstraZeneca疫苗約146.15萬劑預定於今日下午抵達桃園國際機場，待完成通關程序後，直接運送至指定冷儲物流中心進行後續檢驗封緘作業，再提供COVID-19接種計畫所列實施對象接種。\$\@\$指揮中心指出，該中心係於2020年10月30日與臺灣阿斯特捷利康公司簽署1,000萬劑COVID-19疫苗供應合約，截至今日1,000萬劑已全數到貨，分別為 2021年3月3日11.71萬劑、7月7日62.65萬劑、7月15日56.07萬劑、7月27日58.2萬劑、8月12日52.48萬劑、8月27日26.5萬劑、8月31日59.55萬劑、9月10日45.84萬劑、9月17日64.15萬劑、9月30日65.68萬劑、10月13日136.08萬劑、11月4日14.25萬劑、11月6日59.41萬劑、11月19日67.57萬劑、12月21日73.84萬劑，及本次提供第十六批146.15萬劑疫苗。本次提供的疫苗係為多劑型包裝(每瓶10人份)，需存放於2-8℃的環境，本批效期至2022年5月31日。</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-12\$\@\$中央流行疫情指揮中心今(12)日晚間公布國內新增9例COVID-19本土確定病例(均尚未取號，Ct值介於18.2-26.5)，分別為2例男性、7例女性，年齡介於20多歲至50多歲，均為本日匡列接觸者擴大採檢之中壢區某銀行員工(案17630之同職場工作人員)。目前該銀行員工及其家人、親友及近距離接觸者，已經全部隔離，衛生局正漏夜進行調查並持續擴大匡列相關接觸者進行採檢作業，並針對個案服務工作場域進行清消。\$\@\$指揮中心說明，桃園市政府衛生局已於中壢區中正公園、中路公園、龍岡採檢站、中壢區黎明公園、北區客家會館、自強活動中心、東興社區活動中心等處開設社區採檢站，呼籲若民眾曾於今(2022)年1月4日至12日期間至中壢聯邦銀行健行分行洽公、與行員有接觸，或與附近社區足跡有重疊，應請進行自我健康監測，若於1月26日前出現發燒、上呼吸道、腹瀉、嗅味覺異常等症狀，應佩戴醫用口罩，儘速至社區採檢站或各指定採檢院所，接受採檢及評估。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-12\$\@\$中央流行疫情指揮中心今(12)日公布國內新增96例COVID-19確定病例，分別為4例本土個案及92例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為2例男性、2例女性，年齡介於20多歲至60多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為25例男性、27例女性、40例調查中，年齡介於未滿5歲至70多歲，分別自美國(34例)、越南、澳大利亞及菲律賓(各4例)、阿拉伯聯合大公國(2例)、德國、法國及英國(各1例)移入；另41例調查中。入境日介於去(2021)年12月28日至今(2022)年1月11日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,164,612例新型冠狀病毒肺炎相關通報(含5,145,758例排除)，其中17,559例確診，分別為2,854例境外移入，14,651例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計114例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月12日新增本土COVID-19確診個案表.pdf\$\@\$1月12日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
     <t>發佈日期：2022-01-11\$\@\$中央流行疫情指揮中心今(11)日公布國內新增70例COVID-19確定病例，分別為12例本土個案及58例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為6例男性、6例女性，年齡介於未滿5歲至60多歲；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增境外移入個案為27例男性、31例女性，年齡介於未滿5歲至70多歲，分別自美國(27例)、英國(4例)、印尼、菲律賓及澳大利亞(各3例)、阿拉伯聯合大公國、比利時及加拿大(各2例)、卡達、德國、柬埔寨、泰國、哥斯大黎加、中國、愛爾蘭、越南、西班牙及巴西(各1例)移入，另2例調查中。入境日介於去(2021)年12月9日至今(2022)年1月10日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,137,738例新型冠狀病毒肺炎相關通報(含5,118,167例排除)，其中17,463例確診，分別為2,762例境外移入，14,647例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計114例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月11日新增境外移入COVID-19確診個案表.pdf\$\@\$1月11日新增本土COVID-19確診個案表.pdf</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-10\$\@\$中央流行疫情指揮中心今(10)日表示，南非、波札那、納米比亞、賴索托、史瓦帝尼、辛巴威、馬拉威、莫三比克、埃及及奈及利亞等10國原列為以Omicron變異株為主的「重點高風險國家」名單，目前我國已累積對該變異株的防疫經驗，指揮中心經檢討及評估後，宣布將上述10國自「重點高風險國家」名單移除，並適用目前已加嚴之第三級流行地區來臺旅客的入境檢疫措施。\$\@\$指揮中心指出，我國去(2021)年11月底及12月初為因應Omicron變異株，實施「重點高風險國家」來臺旅客管制措施，迄今已逾一個月，截至1月7日已執行162位旅客專案集中檢疫，累計篩檢出2例Omicron變異株病例。指揮中心將持續監視國際疫情，如經監測發現新興(emerging)變異株可能對我國防疫造成重大威脅時，將再重啟「重點高風險國家」來臺旅客專案管制措施。\$\@\$指揮中心說明，國際COVID-19疫情持續，我國已加嚴邊境檢疫措施，自第三級流行地區所有入境旅客搭機來臺前應取得「表定航班時間(Flight schedule time)前2日內COVID-19核酸檢驗報告」，且事前安排檢疫居所(僅限防疫旅宿或自費集中檢疫所)，旅客抵臺後皆須配合採深喉唾液，進行PCR檢測，並搭乘防疫車隊前往檢疫居所，接續完成14天檢疫，旅客應於入境後的檢疫及自主健康管理期間，配合進行6次PCR檢驗或公費快篩。此外，長程航班抵臺的旅客應於機場落地採檢及進行快速核酸檢驗，陽性者由空側搭乘救護車後送專責醫院。\$\@\$指揮中心表示，如旅客於本措施宣布實施前已完成航班機票預訂，且有改訂防疫旅宿的困難，仍可自費至集中檢疫所檢疫14天，或撥打1922防疫專線，並提供航班訂票證明，由本中心協助安排至集中檢疫所自費檢疫。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-10\$\@\$中央流行疫情指揮中心今(10)日表示，Omicron變異株於全球迅速擴散，近期境外移入確診數大增，為降低COVID-19威脅國內社區防疫安全，自今(2022)年1月11日零時起(航班表定抵臺時間)，調整入境旅客檢疫措施如下，請旅客務必配合：\$\@\$搭乘歐美、中東及紐澳等航線長程航班旅客，於抵臺時進行落地公費採檢及快速核酸檢驗，檢驗結果陰性者接續入境通關程序，且應搭乘防疫車輛前往防疫旅宿/集中檢疫所完成檢疫；檢驗結果陽性者，指派專人完成證照查驗後，由空側搭乘救護車後送專責醫院。\$\@\$指揮中心再次強調，適逢春節前返鄉人潮，請旅客返臺必須事先瞭解，並主動配合我國現行入境檢疫規定，並依指揮中心規定的交通方式前往檢疫地點，同時遵守檢疫期間各項檢疫、防疫措施，共同維護國內社區安全。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-09\$\@\$中央流行疫情指揮中心今(9)日表示，因應國內發生Omicron變異株本土確診病例，社區傳播風險提升，為確保醫療機構對疫情的因應及保全醫療量能，自即日起調整以下醫療應變作為，說明如下：\$\@\$一、探病管制：臺北市、新北市、基隆市、桃園市之醫院除例外情形外，禁止探病。符合例外情形經醫院同意探病者，應出具探視日前3天內抗原快篩或PCR檢測陰性證明。探病者為完成疫苗基礎劑應接種劑次達14天(含)以上者，以公費篩檢；未完成者，以自費篩檢。探病者若為確定病例符合檢驗解除隔離條件且距發病日3個月內，得免除篩檢。\$\@\$二、住院病人及陪病者入院篩檢：臺北市、新北市、基隆市、桃園市之醫院或入住前14天內居住於臺北市、新北市、基隆市、桃園市之住院病人及陪病者，無論有無完成疫苗基礎劑應接種劑次達14天(含)以上，預定(非緊急)住院者，於入院前3日內公費篩檢；緊急需住院者，於入住病房前公費篩檢。住院病人及陪病者若為確定病例符合檢驗解除隔離條件且距發病日3個月內，得免除篩檢。\$\@\$三、住院病人之陪病者管理：臺北市、新北市、基隆市、桃園市之醫院，陪病人數以1人為原則。陪病者須不具COVID-19相關症狀，亦未曾接觸確診個案或具相關公共場所活動史。\$\@\$四、醫療照護人員管理：專責病房之醫療照護人員應完成COVID-19疫苗基礎劑應接種劑次達14天(含)以上；可接種追加劑疫苗者，於111年2月1日前應完成接種，未完成者應評估調整職務內容。桃園市之醫院所有單位(除專責病房) 醫療照護人員，未完成疫苗基礎劑應接種劑次達14天(含)以上者，每週定期進行公費篩檢。\$\@\$指揮中心呼籲，醫療機構務必落實執行醫療應變措施，強化感染管制，提高警覺，加強通報採檢，並鼓勵可接種追加劑疫苗之醫院工作人員儘速接種追加劑疫苗，以確保人員健康安全，共同嚴守醫療防線。指揮中心將持續監測國內外疫情發展，滾動修正相關應變策略，完善醫療照護體系，確保醫療量能充足以因應疫情。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-09\$\@\$中央流行疫情指揮中心今(9)日表示，因應桃園國際機場群聚感染SARS-CoV-2病毒Omicron變異株並引發社區感染事件，為防範COVID-19於住宿式長照機構內傳播風險，即日起調整臺北市、新北市、基隆市、桃園市住宿式長照機構COVID-19應變措施，重點說明如下：\$\@\$一、訪客管理：除例外情形暫停探視。例外情形經機構同意可探視者，應出具訪視前3天內採檢之自費篩檢陰性證明。\$\@\$二、新進住民管理：新進住民不論是否已完成COVID-19疫苗接種，\$\@\$(一)均須出具入住機構前3天內採檢之自費篩檢陰性證明；\$\@\$(二)依機構人員完成COVID-19疫苗應接種劑次14天以上比率，採取對應之管制措施：\$\@\$1.如為工作人員達90%以上且住民達80%以上之機構，自入住機構次日起14天內避免參加團體活動；\$\@\$2.如為工作人員未達90%或住民未達80%之機構，則自入住次日起隔離14天，或自入住次日起隔離7天，於第7天進行自費篩檢，陰性者可解除隔離，但仍須避免參加團體活動，之後於第14天再進行1次自費篩檢。\$\@\$指揮中心將持續監測國內外疫情發展，滾動修正相關應變策略。請各類住宿式長照機構務必落實執行「第2級疫情警戒期間住宿式長照機構COVID-19強化管制措施」及指揮中心公布之COVID-19相關措施指引，並鼓勵完整接種COVID-19疫苗基礎劑12週後之機構工作人員與住民儘速接種1劑追加劑疫苗，以提升個人及群體免疫力，確保工作人員及住民健康安全。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-09\$\@\$因應國際間新變異株Omicron威脅，中央流行疫情指揮中心與相關單位溝通及評估後於今(9)日宣布，今(2022)年1月9日至1月24日維持疫情警戒標準為第二級，調整或維持相關措施及規定如下：\$\@\$一、戴口罩規定加嚴，除下列少數例外情形，外出全程佩戴口罩：\$\@\$(一)運動、唱歌、拍照及直播、錄影、主持、報導、致詞、演講、講課等談話性質工作或活動之正式拍攝或進行時，恢復為須戴口罩。\$\@\$(二)下列場合得免戴口罩，但應隨身攜帶口罩，且如本身有相關症狀或與不特定對象無法保持社交距離時，仍應戴口罩：\$\@\$1.農林漁牧工作者於空曠處(如：田間、魚塭、山林)工作。\$\@\$2.於山林(含森林遊樂區)、海濱活動。\$\@\$3.於溫/冷泉、烤箱、水療設施、三溫暖、蒸氣室、水域活動等易使口罩潮濕之場合。\$\@\$(三)外出時有飲食需求，得免戴口罩。\$\@\$(四)於指揮中心或主管機關指定之場所或活動(例如：藝文表演/劇組/電視主播等演出人員正式拍攝演出時、運動競賽之參賽選手及裁判於比賽期間等)，如符合指揮中心或主管機關之相關防疫措施，得暫時脫下口罩。\$\@\$二、營業場所及公共場域(含交通運輸)應嚴格遵守：實聯制、量體溫、加強環境淸消、員工健康管理、確診事件即時應變。\$\@\$三、賣場、超市、市場加強人流管制：室內空間至少1.5米/人(2.25平方米/人)，室外空間至少1米/人(1平方米/人)；不開放試吃。\$\@\$四、餐飮場所：落實實聯制、量體溫、提供洗手設備及消毒用品；宴席不得逐桌敬酒敬茶。\$\@\$指揮中心將視國內外疫情及實際執行狀況，適時機動調整防疫措施，強化邊境監測及防疫作為，籲請民眾應落實個人防護措施，主動積極配合各項防疫規範，以兼顧防疫與生活品質。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-09\$\@\$中央流行疫情指揮中心今(9)日公布國內新增60例COVID-19確定病例，分別為11例本土個案及49例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為5例男性、6例女性，年齡介於未滿5歲至60多歲；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增境外移入個案為29例男性、20例女性，年齡介於未滿5歲至70多歲，分別自美國(30例)、越南(5例)、加拿大(4例)、印度及菲律賓(各2例)、德國、新加坡、英國、奧地利及法國(各1例)移入；另1例調查中。入境日介於去(2021)年12月25日至今(2022)年1月8日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,095,065例新型冠狀病毒肺炎相關通報(含5,075,047例排除)，其中17,362例確診，分別為2,679例境外移入，14,629例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計113例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。\$\@\$(目前網站維護中，相關新聞稿附件請至衛生福利部網站上查詢：https://www.mohw.gov.tw/cp-5264-65480-1.html (另開新頁)) 附件\$\@\$1月9日新增境外移入COVID-19確診個案表.pdf\$\@\$1月9日新增本土COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-08\$\@\$中央流行疫情指揮中心今(8)日公布國內新增44例COVID-19確定病例，分別為2例本土個案(案17414-17415)及42例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，本土個案(案17414-17415)分別為本國籍1例男性、1例女性，年齡均為50多歲，均為桃園機場感染事件相關個案；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增42例境外移入個案，性別為25例男性、16例女性、1例調查中，年齡介於未滿10至70多歲，分別自美國(23例)、越南(4例)、法國(2例)、阿根廷、澳大利亞、菲律賓、加拿大、阿拉伯聯合大公國、泰國、巴西、西班牙、印度、義大利及德國(各1例)入境，另有2例調查中，入境日介於去(2021)年12月15日至今(2022)年1月7日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,074,946例新型冠狀病毒肺炎相關通報(含5,055,445例排除)，其中17,302例確診，分別為2,630例境外移入，14,618例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計113例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月8日新增本土COVID-19確診個案表.pdf\$\@\$1月8日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
     <t>發佈日期：2022-01-07\$\@\$中央流行疫情指揮中心今(7)日表示，因應國內發生Omicron變異株本土確診病例，社區感染風險提升，衛生福利部傳染病防治諮詢會預防接種組(ACIP)決議，已接種兩劑COVID-19疫苗且間隔滿12週(84天)以上之滿18歲民眾，應儘速接種1劑COVID-19疫苗追加劑，以提升免疫保護力。\$\@\$指揮中心說明，昨(6)日召開ACIP會議討論COVID-19疫苗接種策略，考量國內外COVID-19疫情升溫，為降低社區傳播風險，專家指出，建議滿18歲以上民眾於完整接種COVID-19疫苗基礎劑12週後，應接種1劑追加劑，以提升個人及群體免疫力。追加劑接種廠牌建議如下：\$\@\$一、以mRNA疫苗(如Moderna、BNT)或蛋白質次單元疫苗(如高端)完成基礎劑：追加劑可以選擇接種Moderna(半劑量)、BNT、高端或AZ疫苗。\$\@\$二、以AZ完成基礎劑：追加劑可選擇接種mRNA或蛋白質次單元疫苗。\$\@\$指揮中心指出，目前國內疫苗庫存充足，將請地方政府衛生局儘速擴充接種量能，符合接種間隔的民眾可透過「COVID-19疫苗防治一網通」( https://antiflu.cdc.gov.tw/Covid19 )或地方政府衛生局公告，查詢鄰近合約醫療院所提供施打之疫苗廠牌及接種時間。\$\@\$*備註：國外接種疫苗者，接種追加劑說明：\$\@\$一、於國外曾接種WHO EUL 之COVID-19疫苗 返國後請先至就近衛生所或健康服務中心補登國外疫苗接種紀錄，並妥善保存國外接種紀錄。\$\@\$二、符合現行追加劑接種間隔者(至少12週)，可攜國外接種紀錄、健保卡或相關身分證明文件，至鄰近COVID-19疫苗合約院所掛號接種。\$\@\$三、如接種非WHO EUL COVID-19疫苗, 視同無效劑次, 可於與最後一劑COVID-19疫苗間隔28天後, 於國內先完成COVID-19疫苗基礎劑接種，再依規定接種追加劑。</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-07\$\@\$中央流行疫情指揮中心今(7)日公布國內新增62例COVID-19確定病例，分別為4例本土個案(案17368-17371)及58例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，本土個案(案17368-17371)分別為本國籍1例男性、3例女性，年齡介於20至50多歲，均為桃園機場感染事件相關個案；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增58例境外移入個案，為29例男性、29例女性，年齡介於10多歲至70多歲，分別自美國(35例)、法國(4例)、英國(3例)、瑞士、越南及印度(各2例)、奧地利、智利、德國、加拿大、愛爾蘭、孟加拉、奈及利亞、墨西哥、西班牙及哥斯大黎加(各1例)入境，入境日介於去(2021)年12月22日至今(2022)年1月6日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,055,274例新型冠狀病毒肺炎相關通報(含5,035,769例排除)，其中17,258例確診，分別為2,588例境外移入，14,616例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另新增2例空號病例(案17271，案17272與舊案重複，改列空號)，累計113例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月7日新增本土COVID-19確診個案表.pdf\$\@\$1月7日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
     <t>發佈日期：2022-01-06\$\@\$中央流行疫情指揮中心今(6)日公布國內新增43例COVID-19確定病例，為昨(5)日公布尚未取號的3例本土個案(案17307-17309)及40例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，案17307-17309為本國籍女性，年齡介於50至60多歲，皆已接種2劑疫苗，為案17230、案17238、案17239及案17266同職場工作人員；詳如新聞稿附件。\$\@\$指揮中心表示，今日新增40例境外移入個案，為20例男性、20例女性，年齡介於未滿5歲至70多歲，分別自美國(24例，案17267、案17270、案17273-17275、案17277-17282、案17284-17289、案17291-17292、案17300、案17302、案17304-17306)、印度(3例，案17290、案17296、案17303)、巴拿馬(2例，案17271-17272)、荷蘭(案17268)、阿拉伯聯合大公國(2例，案17283、案17301)、加拿大(案17269)、菲律賓(案17276)、義大利(案17293)、英國(案17295)、中國(案17298)及法國(案17299)入境，另有2例(案17294、案17297)調查中，入境日介於去(2021)年12月26日至今(2022)年1月5日；詳如新聞稿附件。\$\@\$另去年12月31日公布之案17127境外移入病例經疫調後改判為本土病例，為案17073之相關感染。\$\@\$指揮中心統計，截至目前國內累計5,036,659例新型冠狀病毒肺炎相關通報(含5,016,638例排除)，其中17,198例確診，分別為2,532例境外移入，14,612例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月6日新增境外移入COVID-19確診個案表.pdf\$\@\$1月6日新增本土COVID-19確診個案表.pdf</t>
   </si>
   <si>
@@ -580,7 +727,10 @@
     <t>發佈日期：2022-01-05\$\@\$中央流行疫情指揮中心今(5)日公布國內新增26例COVID-19確定病例，分別為1例(案17266)本土及25例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，案17266為本國籍50多歲女性，已接種2劑莫德納疫苗(為突破性感染)，與案17230、案17238及案17239為同職場工作人員，曾與前述個案搭乘同路線交通車，原定於今(2022)年1月5日採檢，1月3日出現乾咳、喉嚨不適等症狀，1月4日自行前往採檢站採檢後於今日確診，相關疫情調查、接觸者匡列及防治工作刻正進行中。\$\@\$指揮中心表示，今日新增25例境外移入個案，為12例男性、13例女性，年齡介於未滿5歲至70多歲，分別自美國(12例，案17241-17243、案17245、案17250、案17252、案17254、案17256-17259、案17265)、法國(3例，案17244、案17246、案17253)、丹麥(案17247)、英國(17248)、玻利維亞(案17249)、德國(案17251)、史瓦帝尼王國(案17255)、澳洲(案17260)、巴拿馬(2例，案17261-17262)、瑞典(案17263)及印尼(案17264)入境，入境日介於去(2021)年11月14日至今(2022)年1月4日；詳如新聞稿附件。\$\@\$另1月2日公布之案17181境外移入病例經疫調後改判為本土病例，為案16941之相關感染。\$\@\$指揮中心統計，截至目前國內累計5,017,456例新型冠狀病毒肺炎相關通報(含4,998,328例排除)，其中17,155例確診，分別為2,493例境外移入，14,608例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月5日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-04\$\@\$中央流行疫情指揮中心今(4)日表示，為因應桃園機場群聚感染案件，陳時中指揮官於今日下午協同醫療應變組王必勝副組長、桃園市政府衛生局王文彥局長、衛生福利部疾病管制署北區管制中心及機場公司航運中心工作人員，實地進行入境旅客動線勘查，評估釐清風險，檢視第一線人員防護裝備及消毒情形，並啟動下列防疫作為：\$\@\$一、 成立前進指揮所，由醫療應變組王必勝副組長擔任指揮官，統籌指揮相關防疫工作，進行跨單位溝通協調，並評估各單位現場作業風險，提出相關改善計畫。\$\@\$二、 針對高風險旅客(14天內有症狀)之入境動線，重新釐清評估風險，避免與其他民眾、工作人員接觸，降低傳播可能性。\$\@\$三、 配合桃園市政府衛生局採檢規劃「擴大、快速」戰略概念，擴大評估可能有在個案活動地(如清潔的廁所)活動之其他人員，快速進行相關篩檢。</t>
+    <t>發佈日期：2022-01-05\$\@\$疾管署今(5)日宣布，為提升疫苗接種人口涵蓋率，發揮疫苗最大效益，自2022年1月6日起，公費流感疫苗擴大提供全國6個月以上尚未接種之民眾接種，至疫苗用罄為止，疾管署呼籲尚未接種的計畫對象，尤其是65歲以上長者、學齡前幼兒及醫事人員等重點族群儘快接種，以保障自身及周遭人員的健康。\$\@\$疾管署表示，2021年度公費流感疫苗分2階段施打，除50至64歲無高風險慢性病成人於第二階段11月15日開打外，其於對象均為10月1日開打。截至2022年1月4日，公費疫苗總接種數約562萬劑，整體疫苗使用率逾91.9%，剩餘量約49萬劑；目前全國約有3,700餘家合約院所(含部分衛生所)提供接種服務，建議民眾可先透過各地方政府衛生局網頁、疾管署流感防治一網通(https://antiflu.cdc.gov.tw/)、疾管家或1922防疫諮詢專線，查詢鄰近合約院所名單，並向合約院所預約，以確保可施打到疫苗。\$\@\$另公費流感疫苗接種期間，COVID-19疫苗接種作業持續進行，依衛生福利部傳染病防治諮詢會預防接種組專家建議，2種疫苗接種間隔應至少7天，避免發生疫苗接種不良事件無法釐清。疾管署提醒民眾於預約或接種前主動告知疫苗接種史，合約院所應於接種區建立動線分流，並請相關工作人員於接種前落實檢核接種紀錄，接種後於健保卡黏貼流感疫苗接種貼紙。\$\@\$疾管署提醒，國內流感疫情仍處低點尚未進入流行期，民眾可儘速接種，以於流感疫情達高峰前獲得足夠保護力。近期氣溫偏低，為防範流感及COVID-19疫情雙重衝擊，民眾除接種疫苗，應養成良好衛生習慣，出現類流感症狀儘速戴口罩就醫，並在家休息，減少病毒傳播機會。如有流感疫苗或流感防治相關疑問，可至疾管署全球資訊網(https://www.cdc.gov.tw)，或撥打免付費防疫專線1922(或0800-001922)洽詢。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-04\$\@\$中央流行疫情指揮中心今(4)日表示，為加速國人完成2劑接種，提升尚未接種第1、2劑COVID-19疫苗民眾之接種意願，各地方政府自2022年1月5日至1月31日前，可提供18歲以上民眾200元(含)以下衛教品，以鼓勵民眾踴躍完成接種2劑COVID-19疫苗，儘速獲得完整免疫保護力。\$\@\$指揮中心表示，截至2022年1月3日為止，我國COVID-19疫苗第一劑接種率約80%，第二劑接種率約69%，為因應國際疫情持續嚴峻及Omicron新型變異株之威脅增加，接種涵蓋率仍須再提升，目前COVID-19疫苗由地方政府衛生局指定/安排之合約醫療院所或衛生所進行接種，鼓勵尚未接種過任何1劑COVID-19疫苗及符合接種間隔但尚未完成2劑COVID-19疫苗接種之民眾，請儘速前往COVID-19疫苗合約醫療院所接種。\$\@\$指揮中心說明，目前國內各廠牌COVID-19疫苗供應充分，民眾可至衛生福利部疾病管制署全球資訊網，「COVID-19疫苗接種院所單元」（https://www.cdc.gov.tw/Category/List/u4l1b_gHhf9WDjhEtRmRRw），運用「COVID-19接種院所地圖」及各地方政府衛生局公告之COVID-19疫苗接種合約醫療院所以及車站等隨到隨打疫苗接種站，就近前往接種。\$\@\$指揮中心提醒， 18歲至未滿20歲民眾，如自行前往接種，請持家長簽具之意願同意書。若由家長陪同前往接種，請本人與家長於現場共同簽署意願同意書。另依衛生福利部傳染病防治諮詢會預防接種組(ACIP)建議，接種COVID-19疫苗應與流感疫苗等其他疫苗間隔至少7天，亦請民眾前往接種COVID-19疫苗前，應備妥健保卡或其他可證明身分之證件，如為接種第2劑COVID-19疫苗者亦請攜帶「COVID-19疫苗接種紀錄卡」，並於接種前評估時說明過往疫苗接種史，以利醫生評估。</t>
   </si>
   <si>
     <t>發佈日期：2022-01-04\$\@\$中央流行疫情指揮中心今(4)日公布國內新增34例COVID-19確定病例，分別為4例(案17230、案17238-17240)本土及30例境外移入，其中案17230為昨(3)日公布之尚未取號本土個案；另確診個案中無新增死亡。\$\@\$指揮中心表示，案17238-17240為本國籍，1例男性、2例女性，年齡均為50多歲，皆已接種2劑疫苗，為案17230接觸者。案17238及案17239均為同職場工作人員，通勤時搭乘同班交通車，案17239於1月1日起陸續出現疲倦、咳嗽、流鼻水症狀；案17240為防疫計程車司機，1月1日出現咳嗽症狀，3人經衛生單位安排採檢後於今日確診，相關疫情調查、接觸者匡列及防治工作刻正進行中。\$\@\$指揮中心表示，今日新增30例境外移入個案，為16例男性、14例女性，年齡介於未滿5歲至70多歲，分別自美國(22例，案17207、案17210-17219、案17221、案17223-17228、案17231-17232、案17235-17236)、法國(案17208)、挪威(案17209)、南非(案17220)、阿拉伯聯合大公國(案17222)、英國(案17229)、波蘭(案17234)及烏茲別克(案17237)入境，另1例(案17233)調查中，入境日介於去(2021)年11月20日至今(2022)年1月3日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,998,949例新型冠狀病毒肺炎相關通報(含4,979,641例排除)，其中17,129例確診，分別為2,469例境外移入，14,606例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月4日新增境外移入COVID-19確診個案表.pdf</t>
@@ -589,28 +739,70 @@
     <t>發佈日期：2022-01-03\$\@\$中央流行疫情指揮中心今(3)日公布國內新增1例COVID-19本土確定病例(尚未取號)，為本國籍40多歲女性，任機場停車場清潔人員，近期無出入境紀錄，已接種2劑AZ疫苗。個案於今(2022)年1/2出現發燒、畏寒、咳嗽、流鼻水、喉嚨痛等症狀，並於今日進行快篩，結果為陽性，同時採檢後確診。桃園市政府衛生局即刻啟動疫情調查，並立即通知同住家人就讀之兩校，分別預防性停課一天。\$\@\$指揮中心說明，桃園市政府在接獲醫院通報個案後，已通知個案家人就讀之兩校，分別預防性停課一天。並立即針對6名家人，已於今晚完成採檢，並以急件進行核酸檢驗，檢驗結果確認均為陰性，請兩校師生及家長不需擔憂。並對於個案之工作場域相關接觸者，現正擴大匡列採檢中，包括召回數百名防疫計程車司機將漏夜進行採檢，及針對個案所服務工作場域將進行清消。\$\@\$指揮中心進一步說明，個案另曾於去(2021)年12/30、12/31兩日上午9時至12時有至忠貞市場(中壢前龍街路段)擺攤賣小孩耳環、公仔、髪圈等，衛生單位將針對該市場進行疫調及接觸者匡列，並進行清消作業。\$\@\$指揮中心呼籲，民眾若曾於該段時間出入該場所，應請進行自我健康監測，若於1/14前出現發燒、上呼吸道、腹瀉、嗅味覺異常等症狀，應佩戴醫用口罩，儘速至社區採檢站或各指定採檢院所，接受採檢及評估。</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-03\$\@\$中央流行疫情指揮中心今(3)日公布國內新增25例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增25例境外移入個案，為9例男性、16例女性，年齡介於未滿5歲至70多歲，分別自美國(15例，案17182-17183、案17186-17191、案17196-17197、案17199、案17201-17203、案17205)、土耳其(4例，案17192-17195)、德國(案17184)、加拿大(案17185)、義大利(案17198)、菲律賓(案17200)、亞美尼亞(案17204)及千里達及托巴哥(案17206)入境，入境日介於去(2021)年12月19日至今(2022)年1月1日；詳如新聞稿附件。\$\@\$另去年12月28日及12月30日公布之2例(案17058、案17099)境外移入病例經疫調後改判為本土病例，為案17085之相關感染。\$\@\$指揮中心統計，截至目前國內累計4,982,263例新型冠狀病毒肺炎相關通報(含4,962,860例排除)，其中17,095例確診，分別為2,439例境外移入，14,602例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月3日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
     <t>發佈日期：2022-01-02\$\@\$中央流行疫情指揮中心今(2)日公布國內新增20例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增20例境外移入個案，為10例男性、10例女性，年齡介於未滿5歲至60多歲，分別自美國(11例，案17162-17163、17165-17166、案17168、案17170、案17172、案17174-17175、案17179-17180)、加拿大(案17164)、澳大利亞(案17167)、英國(2例，案17169、案17177)、越南(案17171)、沙烏地阿拉伯(案17173)、泰國(案17176)、希臘(案17178)及中國(案17181)，入境日介於去(2021)年12月12日至12月31日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,972,057例新型冠狀病毒肺炎相關通報(含4,951,828例排除)，其中17,070例確診，分別為2,416例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月2日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-01\$\@\$中央流行疫情指揮中心今(1)日公布國內新增21例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增21例境外移入個案，為15例男性、6例女性，年齡介於20多歲至70多歲，分別自美國(9例，案17141、案17148、案17149、案17151、案17154、案17156、案17159-17161)、越南(6例，案17142、案17145、案17147、案17150、案17152、案17153)、埃及(案17143)、寮國(案17144)、瓜地馬拉(案17146)、羅馬尼亞(案17155)、烏克蘭(案17157)及德國(案17158)入境，入境日介於去(2021)年12月17日至12月31日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,961,497例新型冠狀病毒肺炎相關通報(含4,942,271例排除)，其中17,050例確診，分別為2,396例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月1日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
     <t>發佈日期：2021-12-31\$\@\$中央流行疫情指揮中心今(31)日公布國內新增41例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增41例境外移入個案，為16例男性、25例女性，年齡介於20多歲至70多歲，分別自美國(14例，案17104-17106、案17112、案17113、案17115、案17116、案17118-17122、案17131、案17139)、菲律賓(2例，案17125、案17132)、法國(2例，案17117、案17124)、義大利(案17114)、肯亞(案17123)、喀麥隆(案17126)、瑞士(案17127)、印度(案17128)、阿拉伯聯合大公國(案17129)、烏克蘭(案17130)、越南(案17133)及柬埔寨(案17138)入境，另14例(案17100-17103、案17107-17111、案17134-17137、案17140)調查中，入境日介於今(2021)年12月16日至12月30日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,946,919例新型冠狀病毒肺炎相關通報(含4,927,473例排除)，其中17,029例確診，分別為2,375例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月31日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
     <t>發佈日期：2021-12-31\$\@\$中央流行疫情指揮中心今(31)日表示，指揮中心均秉持防疫優先之原則進行各項防疫工作，有關中國大陸國台辦針對臺灣防疫之錯誤發言內容，相關澄清說明如下：\$\@\$一、鑒於兩岸往來頻繁，為掌握疫情狀況，向來致力與中國大陸保持資訊交流，我方自108年12月31日至110年12月28日，與中國大陸透過正式管道就 COVID-19 疫情往來資訊包括陸方提供我方疫情資訊286次，我方提供陸方包括個案大陸旅遊史等資訊共50次。另我方洽詢陸方疫情訊息計85次，陸方回覆我方疫情資訊21次，而陸方洽詢我方疫情訊息29次，我方回覆陸方疫情資訊28次。陸方電話洽我方聯絡疫情資訊7次，我方電話洽陸方聯絡疫情資訊8次。此外，陸方提供我方技術文件共計12次。相關數據都有文件紀錄可查數，國台辦提供數據有與事實不符之處。\$\@\$二、為與國際分享、交換衛生、防疫經驗，我國均積極爭取參與世界衛生組織相關會議，自2009年至2021年，共向WHO申請參加220場技術性會議，但僅77場獲邀出席。\$\@\$三、為守護國人健康，我國政府一直多方洽談COVID-19疫苗購買，在BioNTech疫苗取得上，為尊重BioNTech原廠疫苗商業代理權劃分，BioNTech 疫苗係由台積電、鴻海／永齡基金會、慈濟基金會三捐贈方委託裕利醫藥公司，向原廠代理商復星實業公司（香港復星）有償購買，在基於「原廠製造、原廠標籤、直送臺灣」三原則的共識，全部無償捐贈政府統籌運用，對於捐贈單位出錢、出力，無私付出，不應被扭曲抹殺。\$\@\$指揮中心強調，疫情尚未止息，人民健康福祉為先。兩岸應互助合作，防疫優先，才能維護兩岸民眾健康。</t>
   </si>
   <si>
-    <t>發佈日期：2021-12-30\$\@\$衛生福利部疾病管制署今（30）日公布「受聘僱外國人健康檢查管理辦法」部分條文修正案，並預訂於111年1月1日實施。本次修法重點包括「修正移工申請結核病都治條件」及「防疫期間調整移工健檢期限之法源依據」等事項，確保社區防疫安全。\$\@\$疾管署說明，結核病為結核桿菌感染所造成的慢性傳染病，目前抗結核藥物效果良好，連續服藥14天後的傳染力可大幅下降；透過移工主動配合、雇主支持，再加上結核病都治關懷員等衛生單位人員持續關心移工確實規則服藥，幾乎可以痊癒，且治療期間亦可正常工作與生活作息；此外，罹患結核病之移工若於國內完成治療，除能避免疾病持續傳播，維護員工健康外，亦不影響雇主勞動力需求。本辦法修正後，移工確診為肺結核、結核性肋膜炎（多重抗藥性結核病個案除外）或漢生病，且本人同意留臺配合按規治療者，雇主應於收受診斷證明書之次日起15日內，檢具「診斷證明書」及「受聘僱外國人接受衛生單位安排都治服務同意書」送縣市政府衛生局申請都治服務，共同落實社區防疫。\$\@\$疾管署指出，本辦法另增訂「中央流行疫情指揮中心成立期間，中央衛生主管機關得依國內疫情防治所需，調整移工健檢期限」及「自聘僱許可生效日起滿6、18及30個月之日與最近一次健檢日間隔未滿3個月者，免辦該次定期健檢」等規定；且回溯至自110年5月19日施行，以避免部分移工需於短期間內重複健檢，並能兼顧防疫安全。\$\@\$為利雇主（仲介）能瞭解本辦法修正後實務作業，疾病管制署提供「移工罹患結核病申請留臺治療」宣導海報、「認識結核病的問與答」多國語言宣導單張及宣導影片等相關衛教素材，並建置於該署全球資訊網（http://www.cdc.gov.tw ； 首頁&gt;國際旅遊與健康&gt;外國人健康管理&gt;受聘僱外國人健檢&gt;最新消息）供下載瀏覽。</t>
+    <t>發佈日期：2021-12-30\$\@\$中央流行疫情指揮中心今（30）日表示，由於國際疫情嚴峻及Omicron新型變異株之威脅日益擴散，近期入境人數及COVID-19境外移入個案增加，為強化社區監測，自明(2022)年1月1日起擴大辦理COVID-19社區加強監測方案，全國由86家定點診所發放公費COVID-19家用快篩試劑增加至272家，由各縣市人口數較多之鄉鎮市區基層診所協助發放試劑，因COVID-19症狀與一般感冒相似，提醒民眾如有出現呼吸道症狀，可多加前往該等診所，由醫師評估發放試劑後自行檢驗。\$\@\$指揮中心說明，今(2021)年8月30日起規劃推動COVID-19社區加強監測方案，迄今已發放1萬餘劑公費COVID-19家用快篩試劑，考量近期COVID-19社區傳播風險提升，為提高民眾取得公費家用快篩試劑可近性與及早發現自身感染之可能，將自明年1月1日起於全國21個縣市增加至272個診所試劑發放點，診所名單詳如新聞稿附件。\$\@\$指揮中心呼籲，現值呼吸道病毒活躍期，請民眾多加留意自身健康，如出現呼吸道症狀，可前往本計畫定點診所；民眾如為2歲以上出現呼吸道症狀的病患至公費快篩試劑發放診所掛號就醫，經醫師評估後發放試劑及注意事項說明單張，如為2歲以下幼兒的陪同看診者，亦由醫師評估後發放。民眾領取試劑後，請配合依注意事項說明內容儘速採檢，並至線上(https://forms.gle/8gh7Kb3ZkYE5aArW7)填寫試劑領取診所名稱及快篩結果等資料，此為匿名方式收集，無須擔心個人資料外洩情形。\$\@\$指揮中心提醒，如居家快篩檢驗為陽性時，請勿慌張並儘速至鄰近的社區採檢院所( https://reurl.cc/MArG1L )進一步PCR檢驗。民眾前往社區採檢院所時，請戴好口罩、勿搭乘大眾運輸工具，對於使用過之採檢器材請用塑膠袋密封包好，並攜帶至社區採檢院所，交予院所人員處理。 附件\$\@\$附件-配合辦理發放公費COVID-19家用快篩試劑社區定點診所名單.pdf</t>
   </si>
   <si>
     <t>發佈日期：2021-12-30\$\@\$中央流行疫情指揮中心今(30)日公布國內新增24例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增24例境外移入個案，為11例男性、13例女性，年齡介於10多歲至60多歲，分別自美國(12例，案17076、案17078-17080、案17082-17083、案17085、案17088、案17090、案17094、案17096)、越南(2例，案17077、案17098)、英國(案17081)、尼加拉瓜(案17084)、奈及利亞(案17086)、加拿大(案17087)、阿拉伯聯合大公國(案17089)、法國(3例，17091-17093)、泰國(案17095)、海地(案17097)及日本(案17099)入境，入境日介於今(2021)年12月14日至12月28日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,932,261例新型冠狀病毒肺炎相關通報(含4,912,670例排除)，其中16,988例確診，分別為2,334例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月30日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
     <t>發佈日期：2021-12-30\$\@\$中央流行疫情指揮中心今(30)日表示，台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的第十五批BNT疫苗93.83萬劑，已於今日上午順利運抵桃園國際機場，並在完成通關程序後，直接運送至指定冷儲物流中心進行後續檢驗封緘作業。\$\@\$指揮中心說明，由台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的BNT疫苗1,500萬劑，目前共計到貨1333.62萬劑，分別為首批9月2日93萬劑、第二批9月9日91萬劑、第三批9月30日54萬劑、第四批10月1日67萬劑、第五批10月4日27萬劑、第六批10月7日88.92萬劑、第七批10月8日88.92萬劑、第八批10月14日82.7萬劑、第九批10月28日90.21萬劑、第十批10月29日91.03萬劑、第十一批11月5日87.17萬劑、第十二批11月12日92.66萬劑、第十三批11月25日93.83萬劑、第十四批12月9日192.35萬劑，以及本批93.83萬劑。本批疫苗效期至2022年3月28日，將由指揮中心統籌運用，儘速提供民眾接種。\$\@\$對於台積電、鴻海暨永齡基金會、慈濟基金會三間企業和民間團體積極協助，提供更多的疫苗讓民眾接種，加速提升臺灣疫苗覆蓋率，指揮中心再次表達由衷的謝意。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-28\$\@\$中央流行疫情指揮中心今(28)日公布國內新增19例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增19例境外移入個案，為9例男性、10例女性，年齡介於未滿10歲至80多歲，分別自美國(8例，案17043、案17045-17049、案17051、案17056)、瑞士(案17044)、寮國(案17050)、越南(案17052)、柬埔寨(案17053)、加拿大(2例，案17054、案17061)、哈薩克(案17055)、香港(案17057)、中國(案17058)及阿根廷(2例，案17059、案17060)入境，入境日介於今(2021)年12月14日至12月26日；詳如新聞稿附件。\$\@\$指揮中心統計，累計4,901,375例新型冠狀病毒肺炎相關通報(含4,882,616例排除)，其中16,950例確診，分別為2,296例境外移入，14,600例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月28日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-27\$\@\$中央流行疫情指揮中心今(27)日表示，歐盟執委會於今(110)年12月21日宣布我國正式加入「歐盟數位新冠證明」系統。歐盟數位新冠證明為世界性標準之一，國際成員國多且最早用於國際旅行，為使我國民眾能加速入境歐盟等國家，指揮中心將於12月28日上午8時開放我國「數位新冠病毒健康證明」供國人下載使用。\$\@\$指揮中心說明，由於歐盟為世界重要國際聯盟，「歐盟數位新冠證明」系統目前已有60國加入，包括27個歐盟會員國、33個非歐盟會員國(統計至2021/12/22止)。另，美國已公開接受旅客持歐盟數位新冠證明供入境查驗，國際航空運輸協會(IATA)之數位新冠證明亦與之互通，故持我國數位證明於國際旅行己不限上述的60國。\$\@\$指揮中心指出，我國「疫苗接種數位證明」或「檢驗結果數位證明」之資料欄位、數位簽章、防偽機制、個人資料保護、QR Code顯示與電子驗證等均依照歐盟標準，尤其是個人資料保護完全依據歐盟一般資料保護規則之最小使用、自行攜帶、可被遺忘等原則，請國人安心使用。\$\@\$指揮中心表示，本項數位證明的內容屬於個人資料保護法定義的敏感性資料，身分確認的方式相對繁瑣。本數位證明提供所有於國內接種疫苗或進行PCR檢驗者自行下載，初期限持有有效護照者，申請方式以電腦或手機直接上網辦理，網址為：https://dvc.mohw.gov.tw（將於12月28日上午8時開放），或在衛福部官網取得連結，三個步驟即可取得證明：\$\@\$一、確認身分：\$\@\$(一)國人：(1)身分證號+健保卡號+有效護照號碼；(2) FIDO(為安全且便利的生物辨識方式，提供指紋或臉部辨識登入)+有效護照號碼；(3)自然人憑證+有效護照號碼。三種方式擇一。\$\@\$(二)外來人口：(1)統一證號+健保卡號；(2) 統一證號+入出境證號；(3) 統一證號+護照號碼。三種方式擇一。\$\@\$二、選擇項目：選擇「疫苗接種數位證明」或「檢驗結果數位證明」。\$\@\$三、取得證明：於申請成功畫面點選「下載/列印 數位證明」，檔案格式為PDF，提醒要先保存於行動裝置或電腦硬碟中，再視個人需要列印紙本。無列印設備但又有列印需求者，可於申請成功畫面選擇超商並點選「取得超商列印碼」，系統將產製超商取件條碼或取件編號，請自行攜至超商付費列印。\$\@\$指揮中心提醒，實際使用時，出示紙本或行動載具中的QR code都是可接受的方法，查驗人員掃瞄QR code後會出現不同顏色的號誌表達接受與否。但各國或不同場所仍可能有不同方式驗證，請民眾特別提醒留意。本數位證明優先提供民眾出國使用，至於國內何時開放使用，再由疫情指揮中心另行發布。詳細系統操作方式可以參考衛生福利部官網數位證明專區( https://covid19.mohw.gov.tw/ch/np-5345-205.html )。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-27\$\@\$中央流行疫情指揮中心今(27)日表示，因應近期COVID-19全球疫情升溫，Omicron等新興變異株於全球迅速擴散，上週(12/20-12/26)境外移入病例數新增109例，較前一次(12/13-12/19)新增62例，上升76%，且Omicron變異株增加迅速，截至今日已累計34例，感染國家以美國及英國較多，加以我國已檢出多起境外移入病例為突破性感染，經評估國際間採認之入境前檢驗報告多以採檢日計算，故為確保航空防疫安全，自2022年1月4日零時起(啟程日)，旅客搭機前應檢附之COVID-19核酸檢驗報告調整為「2日內」報告，報告起計日由原「報告日」改以「採檢日」為基準，並以啟程地表定航班時間（不含搭機當日）往前推2個「日曆日」計算，請旅客搭機前務必確認PCR檢驗報告符合以上規範。\$\@\$指揮中心說明，旅客所持「2日內COVID-19核酸檢驗報告」請符合下列規範：\$\@\$1. 以英文、中文或中英對照版本為原則。\$\@\$2. 該報告可為紙本(正本/影本)或電子報告書形式。\$\@\$3. 需採分子生物學核酸檢測，且應可審核登機者之護照姓名、出生年月日(或護照號碼)、疾病名稱、採檢日及報告日、核酸檢驗方法（包括PCR、Real-Time PCR及RT-PCR等）及判讀結果等。\$\@\$4. 血清免疫學檢驗抗原或抗體，非屬核酸檢測，未符合本措施規範之條件。\$\@\$對於違反前述規定之旅客，抵臺時將依傳染病防治法第58條、第69條規定及衛生福利部公告裁罰基準，處新臺幣一萬元至十五萬元罰鍰。\$\@\$指揮中心強調，適逢春節前返鄉人潮，請旅客返臺必須事先瞭解並配合我國現行入境檢疫規定，及在臺檢疫期間應遵守之防疫措施，共同維護國內社區安全。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-24\$\@\$中央流行疫情指揮中心今(24)日公布國內新增20例COVID-19移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增20例境外移入個案，為14例男性、6例女性，年齡介於10多歲至60多歲，分別自美國(7例，案16965、案16967、案16968、案16970、案16977、案16982、案16983)、越南(3例，案16971、案16979、案16980)、菲律賓(2例，案16973、案16974)、泰國(案16966)、德國(案16969)、馬來西亞(案16972)、印尼(案16975)、新加坡(案16976)、加拿大(案16978)、立陶宛(案16984)及日本(案16981)，入境日介於今(2021)年11月21日至12月22日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,844,559例新型冠狀病毒肺炎相關通報(含4,825,692例排除)，其中16,873例確診，分別為2,220例境外移入，14,599例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月24日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-23\$\@\$中央流行疫情指揮中心今(23)日公布國內新增13例COVID-19移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增13例境外移入個案，為8例男性、5例女性，年齡介於10多歲至60多歲，分別自美國(10例，案16952-16954、案16956-16962)、多明尼加(案16955)、俄羅斯(案16963)、烏克蘭(案16964)，入境日介於今(2021)年12月7日至12月22日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,829,258例新型冠狀病毒肺炎相關通報(含4,810,401例排除)，其中16,853例確診，分別為2,200例境外移入，14,599例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月23日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-22\$\@\$疾病管制署今(22)日表示，迎接耶誕及新年到來，共度歡樂時光的同時，除落實防疫新生活及個人防護措施，也不忘互相提醒為「愛」篩檢，「定期篩檢」就是送給自己與伴侶最好的禮物。疾管署「愛滋自我篩檢 網路訂購超商取貨 期間限定免運費活動」自今(2021)年12月23日起開跑，至明(2022)年1月31日止，只要支付200元即可訂購愛滋自我篩檢試劑(免運費)，歡迎民眾把握機會、掌握自身健康！\$\@\$疾管署說明，為鼓勵民眾瞭解自身健康狀況，今年透過「愛滋自我篩檢計畫」已提供4萬7,000多人次篩檢服務，民眾上網登錄檢驗結果陽性率為0.5%，計畫受到廣大迴響，其中網路訂購超商取貨為民眾喜愛通路之一，有超過7成民眾使用。民眾可至疾管署自我篩檢網站預訂，選擇鄰近超商通路，支付200元試劑費及45元物流費取得自我篩檢試劑。假期將至，疾管署於12月23日推出「自我篩檢 網路訂購超商取貨 期間限定免運費活動」，民眾僅需支付試劑費用即可獲得篩檢試劑，寄送試劑的外包裝不會有任何標示內容物和寄送廠商名稱，充分保障隱私。\$\@\$此外，也可就近前往合作民間團體、衛生局(所)等411個實體服務點，或利用54臺自動服務機，支付200元費用後直接取得篩檢試劑，相關服務內容及試劑提供地點資訊可至疾管署自我篩檢計畫網頁(https://hiva.cdc.gov.tw/Selftest/)查詢。若初步檢驗呈陽性，即使沒有不適，請儘速至愛滋指定醫事機構進一步確認檢驗，疾管署補助當次就醫掛號費及部分負擔，並退還200元試劑費用。衛生局及相關民間團體也提供篩檢諮詢及篩檢陽性個案轉介或陪伴就醫等服務，如有需求可多加利用。\$\@\$疾管署提醒，若發生性行為應主動要求對方或自己全程使用保險套，並搭配水性潤滑液，以保護自己，降低感染風險。疾管署再次呼籲，有性行為者，建議至少進行1次愛滋篩檢，有不安全性行為者，建議每年至少進行1次篩檢，若有感染風險行為(如與人共用針具、多重性伴侶、合併使用成癮性藥物、感染性病等)，建議每3至6個月篩檢1次，以了解自身健康狀況。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-22\$\@\$中央流行疫情指揮中心今(22)日公布國內新增14例COVID-19移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增14例境外移入個案，為9例男性、5例女性，年齡介於20多歲至40多歲，分別自美國(5例，案16938、案16941-16942、案16946、案16950)、義大利(案16939)、印尼(案16940)、波蘭(案16943)、英國(案16944)、柬埔寨(案16945)、越南(3例，案16947、案16949、案16951)，餘1例調查中(案16948)，入境日介於今(2021)年10月7日至12月19日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,813,164例新型冠狀病毒肺炎相關通報(含4,794,827例排除)，其中16,840例確診，分別為2,187例境外移入，14,599例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。 2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月22日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-21\$\@\$中央流行疫情指揮中心今(21)日表示，本(2021)年12月14日起入境擇定春節檢疫專案C方案之民眾，將自12月21日起陸續期滿168小時，凡經檢疫第6天PCR檢測陰性及返家居家檢疫環境與條件均符合規定者，請全程佩戴口罩，搭乘地方政府安排之防疫車輛，返家接續後7天在家居家檢疫，並配合以下檢測措施：\$\@\$一、檢疫期間第10天(Day 10)以家用快篩檢測1次，並配合健康關懷回報結果。\$\@\$二、在家居家檢疫期滿前(Day 13-14)進行PCR檢測1次。\$\@\$三、檢疫期滿後，自主健康管理期間第6至7天(Day 20-21)以家用快篩檢測1次，並以雙向簡訊回復篩檢結果。\$\@\$指揮中心再次提醒，在居家檢疫期間，應留在家中，禁止外出，亦不得出境或出國，確實遵守「防範嚴重特殊傳染性肺炎入境健康聲明暨居家檢疫通知書(春節檢疫專案)」所載規定，並呼籲返家後7天係採1人1室之檢疫者，其同戶內同住者(非居家檢疫者)應共同遵守以下加強暨自主健康管理相關規定及檢測措施，包括：\$\@\$一、於檢疫者返家第3天、第7天各進行1次自費家用快篩，並以雙向簡訊回報結果。\$\@\$二、檢疫者返家檢疫同住期間加強自主健康管理7天，檢疫者檢疫期滿後，接續一起自主健康管理7天。\$\@\$三、自主健康管理期間之規定：\$\@\$(一)    每日早/晚各量體溫一次、詳實記錄體溫、健康狀況及活動史，並配合雙向簡訊回報健康狀況。\$\@\$(二)    避免出入無法保持社交距離，或容易近距離接觸不特定人之場所。\$\@\$(三)    禁止從事近距離或群聚型之活動。\$\@\$(四)    外出時全程佩戴口罩及保持社交距離。\$\@\$(五)    若出現相關症狀，應主動與當地衛生局聯繫，或撥1922，依指示方式就醫。\$\@\$四、加強自主健康管理期間，除遵守上開規定外，應同時遵守下列規定：\$\@\$(一)    不可與自國外入境家人共用房間、衛浴，亦不可同處、共食。\$\@\$(二)    僅能從事固定且有限度之活動，且不可搭乘大眾運輸，禁止至人潮擁擠場所。\$\@\$(三)    落實實名制，須記錄每日活動，且應全程佩戴口罩及保持社交距離。\$\@\$指揮中心強調，檢疫措施是控制疫情的必要防線之一，請民眾務必遵守檢疫期間相關事項，如有違反規定，依法最高可處新臺幣100萬元罰鍰。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-21\$\@\$中央流行疫情指揮中心今(21)日表示，防疫旅宿為國內疫情控制關鍵，經追蹤調查近期兩起群聚事件結果，為提升民眾入住安全品質，降低社區傳播風險，全面檢討防疫旅宿防疫作為，即刻啟動防疫旅宿3大強化措施，嚴守社區防線：\$\@\$一、建立防疫旅宿疑似COVID-19群聚事件之偵測與應變作業，以即時掌握可能相關個案，啟動防治作為：\$\@\$(一) 建立及早偵測防疫旅宿發生疑似群聚事件之策略及可運用資料。\$\@\$(二) 懷疑可能有疑似群聚事件階段之應變作為。\$\@\$(三) 已研判確認發生疑似群聚事件階段之應變作為。\$\@\$二、增修「COVID-19因應指引：防疫旅宿設置及管理」：\$\@\$針對本次群聚事件進行檢討分析，並針對環境、人員等設置與管理之可能風險，與相關專家討論後納入指引；並請地方政府加強落實防疫旅館每月查核作業。\$\@\$三、防疫旅宿訪視輔導與全面查核：\$\@\$(一) 請地方政府於111/1/3前完成全面查核，並可邀請勞動部勞動及職業安全衛生研究所代表或所推薦之通風空調領域專家共同參與，檢視防疫旅宿通風空調運作情形，對於查核結果有須改善之事項，儘速輔導並複查至改善完成。\$\@\$(二) 由感染管制、公共衛生、空調等領域專家組成查核團隊，預計自110/12/27啟動防疫旅宿訪視輔導作業，將曾發生群聚、高於75%入住率、採分層收住等事項之防疫旅宿列為優先訪視輔導對象，並提出改善建議。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-21\$\@\$中央流行疫情指揮中心今(21)日公布國內新增10例COVID-19移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增10例境外移入個案，為5例男性、5例女性，年齡介於20多歲至50多歲，分別自哥倫比亞(案16928)、美國(2例，案16929、案16937)、柬埔寨(案16930)、越南(案16931)、英國(3例，案16932、案16934-16935)、印尼(2例，案16933、案16936)，入境日介於今(2021)年11月22日至12月19日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,794,007例新型冠狀病毒肺炎相關通報(含4,775,550例排除)，其中16,826例確診，分別為2,173例境外移入，14,599例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月21日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-20\$\@\$中央流行疫情指揮中心今(20)日表示，昨(19)日衛生福利部傳染病防治諮詢會預防接種組(ACIP)專家會議決議，經評估國內外疫情風險、國內疫苗供應現況並參酌各國疫苗接種政策，調整及建議COVID-19疫苗接種作業如下：\$\@\$(一)已接種基礎劑(primary series)第一劑COVID-19疫苗之民眾，經醫師評估符合接種間隔後，第二劑可選擇我國食品藥物管理署核准之接種任一廠牌COVID-19疫苗。\$\@\$(二)經醫師評估有免疫不全或免疫力低下且病情穩定之12歲以上民眾，應接種基礎加強劑(additional dose)，其與第二劑COVID-19疫苗間隔至少28天，建議優先接種mRNA疫苗(如Moderna、BNT)或次單位蛋白質疫苗(如高端)。\$\@\$(三)已完成基礎劑接種且間隔滿5個月之18歲以上民眾，應接種追加劑(Booster dose)，建議優先接種mRNA疫苗(如Moderna、BNT)或次單位蛋白質疫苗(如高端)，以獲得充足之免疫保護力。\$\@\$指揮中心說明，會議中專家參酌國內外臨床研究與試驗結果及各國接種策略指出，目前經衛生福利部食品藥物管理署核准專案輸入或製造之COVID-19疫苗，均需至少完成兩劑接種。由於目前國內各廠牌COVID-19疫苗供應充足，世界衛生組織(World Health Organization, WHO)、歐盟及各國亦多採用基礎劑可混打策略，民眾經醫師評估後，可選擇同廠牌疫苗或混打，以提升疫苗接種完成率。\$\@\$另ACIP專家檢視目前現有文獻及臨床試驗結果後表示，免疫不全以及免疫力低下病人即使完成2劑COVID-19疫苗接種，多無法獲得足夠的免疫保護力，爰建議12歲以上經醫師評估病情穩定之下列對象，應接種第3劑基礎加強劑，其間隔與第二劑COVID-19疫苗至少28天，建議優先接種全劑量mRNA疫苗(如Moderna、BNT)或次單位蛋白質疫苗(如高端)：\$\@\$(一)目前正進行或1年內曾接受免疫抑制治療之癌症患者\$\@\$(二)器官移植患者/幹細胞移植患者\$\@\$(三)中度/嚴重先天性免疫不全患者\$\@\$(四)血液透析患者\$\@\$(五)HIV陽性患者\$\@\$(六)目前正使用高度免疫抑制藥物者\$\@\$(七)過去6個月內接受化學治療或放射線治療者\$\@\$(八)其他經醫師評估因免疫不全或免疫力低下，可接種基礎加強劑者\$\@\$基於Omicron變異株疫情於各國持續升溫，ACIP專家表示雖然目前尚無證據顯示感染Omicron變異株後會增加重症、住院或死亡之風險，惟此變異株會可能造成突破性感染(Breakthrough infection)，降低疫苗之保護力，加速傳播，即使曾經感染過其他COVID-19基因型痊癒者，亦可能感染Omicron變異株。對此ACIP專家亦表示，目前就國際間臨床試驗報告、監測及相關文獻均指出，完成基礎劑接種後，疫苗保護力會隨接種時間消退，建議滿18歲以上民眾於完成基礎劑接種後，應接種追加劑。而依據目前國內外研究數據顯示，無論基礎劑接種何種廠牌COVID-19疫苗，國內追加劑建議優先接種Moderna COVID-19疫苗半劑量(50微毫克)、BioNTech COVID-19疫苗全劑量或次單位蛋白質疫苗(如高端)全劑量，以提升免疫保護力。\$\@\$指揮中心提醒，前述政策訂於12月24日開始實施，施行細節將於近日函知各地方政府衛生局轉轄內COVID-19疫苗接種合約院所。指揮中心呼籲，符合接種資格之民眾，請儘速前往COVID-19疫苗合約醫療院所完成接種，加強免疫保護。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-20\$\@\$中央流行疫情指揮中心今(20)日表示，有關中研院P3實驗室內部調查報告，該院已依指揮中心要求期限於昨(19)日晚間送達指揮中心。報告書中說明事發經過、院方應變措施、感染途徑調查、院方整體調查結果與根本原因分析、責任檢討與未來改進事項；其中針對人員訪談、11月中下旬監視器錄影檔、實驗室使用紀錄表等調查發現，確認具有以下三項感染暴露風險因子：\$\@\$一、實驗操作區與非操作區均存在環境汙染。於實驗動物操作時，未於生物安全櫃中進行。髒墊料直接置於未封口的袋子、也未放置於加蓋的容器中。\$\@\$二、個案及其他實驗室人員均曾僅穿著一般防護裝備(未戴N95口罩、雙層手套、護目鏡或面罩)執行實驗。\$\@\$三、個案於脫除防護裝備過程先行脫口罩。\$\@\$根據以上感染暴露風險因子，中研院研判感染途徑可能有三種：\$\@\$一、呼吸道直接暴露受汙染的墊料粉塵、染疫動物受刺激而引發噴飛沫或氣膠的環境。\$\@\$二、手套表面因直接操作染疫動物被汙染，於脫卸防護裝備程序先誤脫口罩時，接觸臉部口鼻等部位而感染。\$\@\$三、防護裝備外層在操作區遭帶有病毒之物體表面汙染，於脫卸防護裝備程序先誤脫口罩時，使口鼻暴露於脫卸過程而感染。\$\@\$此外，中研院亦針對：(1)新進人員教育訓練與操作指導；(2)實驗室SOP操作；(3)實驗操作過程監控；(4)個人防護裝備穿卸流程；(5)意外事故通報流程；(6)動物科學應用審核管理規範及感染性生物材料之使用管控；(7)本次染疫事件成因的系統性問題等七大面向，進行制度面及執行面的回顧檢討，並說明若最終調查認定確有違反規定，將依據人員身分別處理責任歸屬及處分。中研院並提出未來將成立P3實驗室綜合檢討委員會，確實改進P3實驗室的管理運作級生物安全監督查核機制。\$\@\$指揮中心說明，該中心已於12月17日及19日派員訪談中研院該P3實驗室主管、工作人員、及中研院生安會主委，並於今日上午提交訪談結果及中研院內部調查報告予外部專家調查小組，且安排於本週四開會進行審視及討論，預計兩週內提出外部專家小組調查結論及建議；另亦將依傳染病防治法第34條、第69條及感染性生物材料管理辦法第25條規定，對中研院進行裁處，最高可處十五萬元罰鍰，並限期令其改善，屆期未改善者，按次處罰之，並於生物安全疑慮解除前，要求該P3實驗室停止使用或處分相關感染性生物材料。另依前開管理辦法第29條規定，於生物安全疑慮解除，經該院生安會確認後，報疾管署同意後，始得再行使用或處分相關感染性生物材料。\$\@\$指揮中心另指出，除中研院基因體研究中心P3實驗室已另案調查，其餘國內11家操作新冠病毒之P3實驗室均已於12/17查核完畢，未發現重大缺失。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-20\$\@\$中央流行疫情指揮中心今(20)日公布國內新增11例COVID-19移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增11例境外移入個案，為7例男性、4例女性，年齡介於10多歲至50多歲，分別自義大利(案16917)、美國(5例，案16918-16920、案16922、案16926)、德國(案16921)、法國(案16923)、巴西(案16924)、越南(案16925)及菲律賓(案16927)入境，入境日介於今(2021)年12月5日至12月19日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,774,769例新型冠狀病毒肺炎相關通報(含4,756,108例排除)，其中16,816例確診，分別為2,163例境外移入，14,599例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計111例移除為空號。2020年起累計850例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月20日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-16\$\@\$中央流行疫情指揮中心今(16)日表示，因應案16851於今(2021)年12月11日自主健康管理期間確診，指揮中心與地方衛生局立即展開相關調查，包括擴大回溯追蹤、擴大採檢、現場勘查、病毒定序等，發現同防疫旅宿同樓層之案16768、16841、16851、16856病毒S基因序列相同，初步研判可能為一起防疫旅宿相關感染事件。\$\@\$指揮中心說明，考量防疫旅宿為國內疫情控制關鍵，指揮中心即刻啟動防疫旅宿四大強化作為，多管齊下，嚴守社區防線：\$\@\$一、強化監測作為，增加春節檢疫專案3項方案篩檢次數及查核與違規裁處：\$\@\$(一) 3方案均於入境時、檢疫第3、7、10、14及第21天(自主健康管理期間第6-7天)進行PCR檢驗或公費快篩(詳附件)。\$\@\$(二) 居家檢疫期間加強查核，違反規定者將加重裁處。\$\@\$二、防疫旅宿防疫措施查核：邀集感控專家針對防疫旅宿進行全面查核，指導與協助防疫旅宿落實防疫管理措施。\$\@\$三、防疫旅宿通風空調檢視：請勞動部勞動及職業安全衛生研究所協助全面檢視防疫旅宿之通風空調換氣情形，並提供改善建議。\$\@\$四、加強有症狀通報：檢疫期間有症狀均要進行PCR採檢，以確實掌握可能個案。 附件\$\@\$1216-春節檢疫專案篩檢次數調整.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-14\$\@\$中央流行疫情指揮中心今(14)日公布國內新增10例COVID-19境外移入確定病例；另確診個案中無新增死亡。\$\@\$指揮中心說明，今日新增10例境外移入個案，為6例男性、4例女性，年齡介於10多歲至50多歲，分別自美國(2例，案16854、案16855)、香港(案16856)、孟加拉(案16857)、越南(2例，案16858、案16863)、柬埔寨(案16859)、菲律賓(案16860)、阿拉伯聯合大公國(案16861)及印尼(案16862)入境，入境日介於今(2021)年11月26日至12月12日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計4,672,651例新型冠狀病毒肺炎相關通報(含4,655,350例排除)，其中16,752例確診，分別為2,107例境外移入，14,591例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另累計111例移除為空號。2020年起累計848例COVID-19死亡病例，其中836例本土，個案居住縣市分布為新北市412例、臺北市321例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另12例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$12月14日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-13\$\@\$中央流行疫情指揮中心今(13)日表示，目前已全面提供「AZ、莫德納、BNT、高端共4種疫苗第一、二劑」、「已接種第一劑AZ疫苗，第二劑混打BNT或莫德納疫苗」以及「完整接種COVID-19疫苗且滿5個月，追加接種第三劑莫德納」之接種服務，請民眾儘速透過「COVID-19公費疫苗預約平臺」（https://1922.gov.tw/ ，以下簡稱預約平臺）或各地方政府指定合約醫療院所/衛生所預約接種。\$\@\$其中，預約平臺第18期規劃提供BNT疫苗預約，相關對象及期程說明如下：\$\@\$一、符合資格對象，12月13日上午6時前已意願登記(含混打)民眾，且符合下列任一條件：\$\@\$(一) BNT第一劑：12歲以上民眾[即2009/12/16(含)前出生]。\$\@\$(二) BNT第二劑：11月18日(含)前已接種BNT第一劑18歲以上民眾[即2003/12/31(含)前出生]。\$\@\$(三)已接種第一劑AZ，第二劑混打BNT疫苗：10月21日(含)前已接種AZ第一劑18歲以上民眾[即2003/12/16(含)前出生]。\$\@\$二、預約時程：12月14日上午10時至12月15日中午12時。\$\@\$三、施打時程：12月16日至12月22日。\$\@\$指揮中心說明，上述符合資格對象將於12月13日下午2時起，陸續收到提醒簡訊，請記得依預約時間進行預約；預約當日如遇啟動流量管制亦請配合依序排隊耐心等候預約。後續將視疫苗供應期程調整接種場次，籲請民眾屆時準時前往接種。\$\@\$指揮中心強調，各廠牌疫苗均可至各地方政府衛生局合約醫療院所預約接種，且衛生福利部所屬醫院、國軍退除役官兵輔導委員會所屬醫院及國防部所屬醫院，亦增開週一至週五夜間門診，提供莫德納疫苗接種服務，請民眾多加利用，並呼籲民眾儘速完成二劑疫苗接種，以獲得完整免疫保護力。\$\@\$指揮中心提醒，10月1日起亦開始接種流感疫苗，依我國衛生福利部傳染病防治諮詢會預防接種組(ACIP)建議，接種流感疫苗應與COVID-19疫苗間隔至少7天，請民眾前往接種COVID-19第二劑疫苗前，應備妥「COVID-19疫苗接種紀錄卡」及健保卡，並於接種前評估時說明過往疫苗接種史，以利醫生評估。另未滿18歲對象，請由家長(或法定代理人、監護人及關係人等)陪同前往合約醫療院所或接種站接種，並由本人與家長於現場共同簽署意願同意書；18歲至未滿20歲民眾，如自行前往接種，請持家長簽具之意願同意書，若由家長陪同前往接種，請本人與家長於現場共同簽署意願同意書。</t>
   </si>
 </sst>
 </file>
@@ -985,7 +1177,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1013,16 +1205,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="C2" s="2">
-        <v>44583</v>
+        <v>44585</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1030,16 +1219,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="C3" s="2">
-        <v>44582</v>
+        <v>44585</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>106</v>
+        <v>148</v>
       </c>
       <c r="E3" t="s">
-        <v>156</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1047,16 +1236,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="C4" s="2">
-        <v>44582</v>
+        <v>44585</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>107</v>
+        <v>149</v>
       </c>
       <c r="E4" t="s">
-        <v>157</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1064,16 +1253,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="C5" s="2">
-        <v>44581</v>
+        <v>44585</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>108</v>
+        <v>150</v>
       </c>
       <c r="E5" t="s">
-        <v>158</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1081,16 +1270,13 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="C6" s="2">
-        <v>44581</v>
+        <v>44585</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E6" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1098,16 +1284,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="C7" s="2">
-        <v>44581</v>
+        <v>44584</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>110</v>
+        <v>152</v>
       </c>
       <c r="E7" t="s">
-        <v>160</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1115,16 +1301,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="C8" s="2">
-        <v>44581</v>
+        <v>44583</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="E8" t="s">
-        <v>161</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1132,16 +1318,13 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C9" s="2">
-        <v>44580</v>
+        <v>44582</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E9" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1149,16 +1332,13 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="C10" s="2">
-        <v>44580</v>
+        <v>44582</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E10" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1166,16 +1346,13 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C11" s="2">
-        <v>44579</v>
+        <v>44581</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E11" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1183,16 +1360,13 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="C12" s="2">
-        <v>44578</v>
+        <v>44579</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E12" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1200,16 +1374,16 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="C13" s="2">
-        <v>44577</v>
+        <v>44578</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>116</v>
+        <v>158</v>
       </c>
       <c r="E13" t="s">
-        <v>166</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1217,16 +1391,13 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="C14" s="2">
         <v>44577</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E14" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1234,16 +1405,16 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C15" s="2">
-        <v>44576</v>
+        <v>44577</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>118</v>
+        <v>160</v>
       </c>
       <c r="E15" t="s">
-        <v>168</v>
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1251,13 +1422,16 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="C16" s="2">
-        <v>44575</v>
+        <v>44576</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>119</v>
+        <v>161</v>
+      </c>
+      <c r="E16" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1265,16 +1439,16 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="C17" s="2">
         <v>44575</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>120</v>
+        <v>162</v>
       </c>
       <c r="E17" t="s">
-        <v>169</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1282,16 +1456,16 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="C18" s="2">
-        <v>44574</v>
+        <v>44575</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
       <c r="E18" t="s">
-        <v>170</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1299,16 +1473,13 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="C19" s="2">
         <v>44574</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E19" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1316,16 +1487,16 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="C20" s="2">
-        <v>44573</v>
+        <v>44574</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>123</v>
+        <v>165</v>
       </c>
       <c r="E20" t="s">
-        <v>172</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1333,511 +1504,1113 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="C21" s="2">
         <v>44573</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E21" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C22" s="2">
-        <v>44572</v>
+        <v>44575</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="E22" t="s">
-        <v>174</v>
+        <v>228</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="C23" s="2">
-        <v>44571</v>
+        <v>44575</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
       <c r="E23" t="s">
-        <v>175</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C24" s="2">
-        <v>44571</v>
+        <v>44574</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E24" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="C25" s="2">
-        <v>44571</v>
+        <v>44574</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>128</v>
+        <v>165</v>
+      </c>
+      <c r="E25" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="C26" s="2">
-        <v>44570</v>
+        <v>44573</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E26" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C27" s="2">
-        <v>44570</v>
+        <v>44573</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E27" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="C28" s="2">
-        <v>44570</v>
+        <v>44572</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>131</v>
+        <v>168</v>
       </c>
       <c r="E28" t="s">
-        <v>179</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="C29" s="2">
-        <v>44570</v>
+        <v>44571</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E29" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="C30" s="2">
-        <v>44569</v>
+        <v>44571</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E30" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="C31" s="2">
-        <v>44568</v>
+        <v>44571</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E31" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="C32" s="2">
         <v>44568</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>135</v>
+        <v>172</v>
       </c>
       <c r="E32" t="s">
-        <v>183</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C33" s="2">
-        <v>44567</v>
+        <v>44568</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E33" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="C34" s="2">
         <v>44567</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>137</v>
+        <v>174</v>
       </c>
       <c r="E34" t="s">
-        <v>185</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="C35" s="2">
         <v>44567</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="E35" t="s">
-        <v>186</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="C36" s="2">
-        <v>44566</v>
+        <v>44567</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>139</v>
+        <v>176</v>
+      </c>
+      <c r="E36" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="C37" s="2">
         <v>44566</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="E37" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="C38" s="2">
         <v>44566</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>141</v>
+        <v>178</v>
+      </c>
+      <c r="E38" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="C39" s="2">
-        <v>44565</v>
+        <v>44566</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="E39" t="s">
-        <v>188</v>
+        <v>237</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="C40" s="2">
         <v>44565</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>143</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="C41" s="2">
         <v>44565</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>144</v>
+        <v>181</v>
       </c>
       <c r="E41" t="s">
-        <v>189</v>
+        <v>238</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="C42" s="2">
-        <v>44564</v>
+        <v>44566</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E42" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C43" s="2">
-        <v>44564</v>
+        <v>44566</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>146</v>
+        <v>178</v>
       </c>
       <c r="E43" t="s">
-        <v>191</v>
+        <v>236</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="C44" s="2">
-        <v>44563</v>
+        <v>44566</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>147</v>
+        <v>179</v>
       </c>
       <c r="E44" t="s">
-        <v>192</v>
+        <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C45" s="2">
-        <v>44562</v>
+        <v>44565</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E45" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="C46" s="2">
-        <v>44561</v>
+        <v>44565</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>149</v>
+        <v>181</v>
       </c>
       <c r="E46" t="s">
-        <v>194</v>
+        <v>238</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="C47" s="2">
-        <v>44561</v>
+        <v>44565</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>150</v>
+        <v>182</v>
       </c>
       <c r="E47" t="s">
-        <v>195</v>
+        <v>239</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B48" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="C48" s="2">
-        <v>44560</v>
+        <v>44564</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>151</v>
+        <v>183</v>
       </c>
       <c r="E48" t="s">
-        <v>196</v>
+        <v>240</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B49" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="C49" s="2">
-        <v>44560</v>
+        <v>44564</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>152</v>
+        <v>184</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B50" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="C50" s="2">
-        <v>44560</v>
+        <v>44563</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>153</v>
+        <v>185</v>
       </c>
       <c r="E50" t="s">
-        <v>197</v>
+        <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" t="s">
+        <v>113</v>
+      </c>
+      <c r="C51" s="2">
+        <v>44562</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" s="2">
+        <v>44561</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E52" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53" t="s">
+        <v>115</v>
+      </c>
+      <c r="C53" s="2">
+        <v>44561</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E53" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" s="2">
+        <v>44560</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55" t="s">
+        <v>117</v>
+      </c>
+      <c r="C55" s="2">
+        <v>44560</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E55" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>49</v>
+      </c>
+      <c r="B56" t="s">
+        <v>118</v>
+      </c>
+      <c r="C56" s="2">
+        <v>44560</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E56" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>50</v>
+      </c>
+      <c r="B57" t="s">
+        <v>119</v>
+      </c>
+      <c r="C57" s="2">
+        <v>44560</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E57" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>51</v>
+      </c>
+      <c r="B58" t="s">
+        <v>120</v>
+      </c>
+      <c r="C58" s="2">
+        <v>44559</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>52</v>
+      </c>
+      <c r="B59" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" s="2">
+        <v>44558</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E59" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>53</v>
+      </c>
+      <c r="B60" t="s">
+        <v>122</v>
+      </c>
+      <c r="C60" s="2">
+        <v>44557</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E60" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
         <v>54</v>
       </c>
-      <c r="B51" t="s">
-        <v>104</v>
-      </c>
-      <c r="C51" s="2">
-        <v>44560</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="B61" t="s">
+        <v>123</v>
+      </c>
+      <c r="C61" s="2">
+        <v>44557</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E61" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>55</v>
+      </c>
+      <c r="B62" t="s">
+        <v>124</v>
+      </c>
+      <c r="C62" s="2">
+        <v>44555</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>56</v>
+      </c>
+      <c r="B63" t="s">
+        <v>125</v>
+      </c>
+      <c r="C63" s="2">
+        <v>44554</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>198</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>43</v>
+      </c>
+      <c r="B64" t="s">
+        <v>126</v>
+      </c>
+      <c r="C64" s="2">
+        <v>44554</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E64" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>57</v>
+      </c>
+      <c r="B65" t="s">
+        <v>127</v>
+      </c>
+      <c r="C65" s="2">
+        <v>44553</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>58</v>
+      </c>
+      <c r="B66" t="s">
+        <v>128</v>
+      </c>
+      <c r="C66" s="2">
+        <v>44553</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E66" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>59</v>
+      </c>
+      <c r="B67" t="s">
+        <v>129</v>
+      </c>
+      <c r="C67" s="2">
+        <v>44552</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E67" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>51</v>
+      </c>
+      <c r="B68" t="s">
+        <v>130</v>
+      </c>
+      <c r="C68" s="2">
+        <v>44552</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="E68" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>60</v>
+      </c>
+      <c r="B69" t="s">
+        <v>131</v>
+      </c>
+      <c r="C69" s="2">
+        <v>44551</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="E69" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>61</v>
+      </c>
+      <c r="B70" t="s">
+        <v>132</v>
+      </c>
+      <c r="C70" s="2">
+        <v>44551</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E70" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>62</v>
+      </c>
+      <c r="B71" t="s">
+        <v>133</v>
+      </c>
+      <c r="C71" s="2">
+        <v>44551</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E71" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>63</v>
+      </c>
+      <c r="B72" t="s">
+        <v>134</v>
+      </c>
+      <c r="C72" s="2">
+        <v>44550</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E72" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>64</v>
+      </c>
+      <c r="B73" t="s">
+        <v>135</v>
+      </c>
+      <c r="C73" s="2">
+        <v>44550</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E73" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>65</v>
+      </c>
+      <c r="B74" t="s">
+        <v>136</v>
+      </c>
+      <c r="C74" s="2">
+        <v>44550</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E74" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75" t="s">
+        <v>137</v>
+      </c>
+      <c r="C75" s="2">
+        <v>44549</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>58</v>
+      </c>
+      <c r="B76" t="s">
+        <v>138</v>
+      </c>
+      <c r="C76" s="2">
+        <v>44548</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>67</v>
+      </c>
+      <c r="B77" t="s">
+        <v>139</v>
+      </c>
+      <c r="C77" s="2">
+        <v>44547</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>68</v>
+      </c>
+      <c r="B78" t="s">
+        <v>140</v>
+      </c>
+      <c r="C78" s="2">
+        <v>44546</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E78" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>69</v>
+      </c>
+      <c r="B79" t="s">
+        <v>141</v>
+      </c>
+      <c r="C79" s="2">
+        <v>44546</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>70</v>
+      </c>
+      <c r="B80" t="s">
+        <v>142</v>
+      </c>
+      <c r="C80" s="2">
+        <v>44545</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>62</v>
+      </c>
+      <c r="B81" t="s">
+        <v>143</v>
+      </c>
+      <c r="C81" s="2">
+        <v>44544</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E81" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>66</v>
+      </c>
+      <c r="B82" t="s">
+        <v>137</v>
+      </c>
+      <c r="C82" s="2">
+        <v>44549</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>58</v>
+      </c>
+      <c r="B83" t="s">
+        <v>138</v>
+      </c>
+      <c r="C83" s="2">
+        <v>44548</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>67</v>
+      </c>
+      <c r="B84" t="s">
+        <v>139</v>
+      </c>
+      <c r="C84" s="2">
+        <v>44547</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>68</v>
+      </c>
+      <c r="B85" t="s">
+        <v>140</v>
+      </c>
+      <c r="C85" s="2">
+        <v>44546</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E85" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>69</v>
+      </c>
+      <c r="B86" t="s">
+        <v>141</v>
+      </c>
+      <c r="C86" s="2">
+        <v>44546</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>70</v>
+      </c>
+      <c r="B87" t="s">
+        <v>142</v>
+      </c>
+      <c r="C87" s="2">
+        <v>44545</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>62</v>
+      </c>
+      <c r="B88" t="s">
+        <v>143</v>
+      </c>
+      <c r="C88" s="2">
+        <v>44544</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="E88" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>71</v>
+      </c>
+      <c r="B89" t="s">
+        <v>144</v>
+      </c>
+      <c r="C89" s="2">
+        <v>44543</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>72</v>
+      </c>
+      <c r="B90" t="s">
+        <v>145</v>
+      </c>
+      <c r="C90" s="2">
+        <v>44543</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>73</v>
+      </c>
+      <c r="B91" t="s">
+        <v>146</v>
+      </c>
+      <c r="C91" s="2">
+        <v>44543</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E91" t="s">
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -1892,6 +2665,46 @@
     <hyperlink ref="D49" r:id="rId48"/>
     <hyperlink ref="D50" r:id="rId49"/>
     <hyperlink ref="D51" r:id="rId50"/>
+    <hyperlink ref="D52" r:id="rId51"/>
+    <hyperlink ref="D53" r:id="rId52"/>
+    <hyperlink ref="D54" r:id="rId53"/>
+    <hyperlink ref="D55" r:id="rId54"/>
+    <hyperlink ref="D56" r:id="rId55"/>
+    <hyperlink ref="D57" r:id="rId56"/>
+    <hyperlink ref="D58" r:id="rId57"/>
+    <hyperlink ref="D59" r:id="rId58"/>
+    <hyperlink ref="D60" r:id="rId59"/>
+    <hyperlink ref="D61" r:id="rId60"/>
+    <hyperlink ref="D62" r:id="rId61"/>
+    <hyperlink ref="D63" r:id="rId62"/>
+    <hyperlink ref="D64" r:id="rId63"/>
+    <hyperlink ref="D65" r:id="rId64"/>
+    <hyperlink ref="D66" r:id="rId65"/>
+    <hyperlink ref="D67" r:id="rId66"/>
+    <hyperlink ref="D68" r:id="rId67"/>
+    <hyperlink ref="D69" r:id="rId68"/>
+    <hyperlink ref="D70" r:id="rId69"/>
+    <hyperlink ref="D71" r:id="rId70"/>
+    <hyperlink ref="D72" r:id="rId71"/>
+    <hyperlink ref="D73" r:id="rId72"/>
+    <hyperlink ref="D74" r:id="rId73"/>
+    <hyperlink ref="D75" r:id="rId74"/>
+    <hyperlink ref="D76" r:id="rId75"/>
+    <hyperlink ref="D77" r:id="rId76"/>
+    <hyperlink ref="D78" r:id="rId77"/>
+    <hyperlink ref="D79" r:id="rId78"/>
+    <hyperlink ref="D80" r:id="rId79"/>
+    <hyperlink ref="D81" r:id="rId80"/>
+    <hyperlink ref="D82" r:id="rId81"/>
+    <hyperlink ref="D83" r:id="rId82"/>
+    <hyperlink ref="D84" r:id="rId83"/>
+    <hyperlink ref="D85" r:id="rId84"/>
+    <hyperlink ref="D86" r:id="rId85"/>
+    <hyperlink ref="D87" r:id="rId86"/>
+    <hyperlink ref="D88" r:id="rId87"/>
+    <hyperlink ref="D89" r:id="rId88"/>
+    <hyperlink ref="D90" r:id="rId89"/>
+    <hyperlink ref="D91" r:id="rId90"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20220126
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="154">
   <si>
     <t>Press Title</t>
   </si>
@@ -31,6 +31,12 @@
     <t>Page Content</t>
   </si>
   <si>
+    <t>新增92例COVID-19確定病例，分別為46例本土及46例境外移入</t>
+  </si>
+  <si>
+    <t>鑑於帛琉近期疫情快速上升，1月25日起提升旅遊疫情建議至第三級警告 (Warning)</t>
+  </si>
+  <si>
     <t>指揮中心公布COVID-19自費核酸檢驗指定機構農曆春節連假期間服務資訊</t>
   </si>
   <si>
@@ -43,12 +49,6 @@
     <t>今(2022)年第一批採購Moderna疫苗151.21萬劑於今(25)日下午抵臺</t>
   </si>
   <si>
-    <t>全國醫院即日起除例外情形，停止開放探病，並調整住院病人、陪(探)病者及醫療照護人員篩檢及疫苗接種等相關規定</t>
-  </si>
-  <si>
-    <t>因應國內COVID-19疫情發展，指揮中心1/24起調整全國住宿式長照機構訪客及新進住民管理等應變措施</t>
-  </si>
-  <si>
     <t>網傳「三級警戒微解封的不可思議之處」指揮中心： 原同住家人就不受限制，謠言邏輯誤導且比喻失當，請勿輕信轉傳，造成防疫困擾</t>
   </si>
   <si>
@@ -97,6 +97,9 @@
     <t>約聘技術員</t>
   </si>
   <si>
+    <t>約用助理(徵才案號：1059延長公告)(依身心障礙權益保障法任用身心障礙者)</t>
+  </si>
+  <si>
     <t>技士</t>
   </si>
   <si>
@@ -106,9 +109,6 @@
     <t>約用護理師(徵才案號：1523)</t>
   </si>
   <si>
-    <t>約用助理(徵才案號：1526)</t>
-  </si>
-  <si>
     <t>約聘護理師</t>
   </si>
   <si>
@@ -130,6 +130,12 @@
     <t>公告本署檢驗及疫苗研製中心約用人員徵才案(徵才案號：1057、1058)初審合格名單及甄試事宜。</t>
   </si>
   <si>
+    <t>1月25日至2月7日維持第二級疫情警戒標準，並調整相關規定，請民眾自主落實防疫措施，共同維護國內社區安全</t>
+  </si>
+  <si>
+    <t>新增89例COVID-19確定病例，分別為52例本土及37例境外移入</t>
+  </si>
+  <si>
     <t>新增130例COVID-19確定病例，分別為82例本土及48例境外移入</t>
   </si>
   <si>
@@ -154,10 +160,10 @@
     <t>自1月20日零時起，增列印度及東南亞航線航班旅客於落地時採驗，檢驗結果陽性後送醫院或集中檢疫所/加強版防疫旅宿</t>
   </si>
   <si>
-    <t>新增54例COVID-19確定病例，分別為10例本土及44例境外移入</t>
-  </si>
-  <si>
-    <t>新增66例COVID-19確定病例，分別為17例本土及49例境外移入</t>
+    <t>/Bulletin/Detail/J3ByKlpyULZLtHehAJUa_g?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/w5wAafr4zKG_ZR88_qWdVQ?typeid=9</t>
   </si>
   <si>
     <t>/Bulletin/Detail/xah9AQII8GupFO7uV7kz-Q?typeid=9</t>
@@ -172,12 +178,6 @@
     <t>/Bulletin/Detail/AFuil2ECiqiNku1SmowIGQ?typeid=9</t>
   </si>
   <si>
-    <t>/Bulletin/Detail/kVDslqExqB7BSiqJuFzXCg?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/cU2pYInOEJ4NOhg-uOH5Zg?typeid=9</t>
-  </si>
-  <si>
     <t>/Bulletin/Detail/ftv6FPFis84j5uHWTq4lNA?typeid=8772</t>
   </si>
   <si>
@@ -226,6 +226,9 @@
     <t>/HireList/Detail?hireId=dbhD6saaWV5URglIuc0HhA</t>
   </si>
   <si>
+    <t>/HireList/Detail?hireId=Zqa4DDs0UoZULIvGT10iAA</t>
+  </si>
+  <si>
     <t>/HireList/Detail?hireId=_KGB6fXszZ2udoZvtWhyuw</t>
   </si>
   <si>
@@ -235,9 +238,6 @@
     <t>/HireList/Detail?hireId=4wyEVe65rp-Hr9DETX8n2g</t>
   </si>
   <si>
-    <t>/HireList/Detail?hireId=ndMCl2Q6Sfsq3tUerM6pcw</t>
-  </si>
-  <si>
     <t>/HireList/Detail?hireId=snieuoubdCfzpuQJABGcjA</t>
   </si>
   <si>
@@ -259,6 +259,12 @@
     <t>/Bulletin/Detail/u9ej71cxiu9bJqO0gMxdOQ?typeid=11</t>
   </si>
   <si>
+    <t>/Bulletin/Detail/y6MiRdu9X-y3kAs1UrXvng?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/RpwW0PpibHaRFJpatPM1HA?typeid=9</t>
+  </si>
+  <si>
     <t>/Bulletin/Detail/5MtrgzOJApOSjivffWLWRw?typeid=9</t>
   </si>
   <si>
@@ -283,10 +289,10 @@
     <t>/Bulletin/Detail/Mhpv_WBf9Gw4pLB1hMe1hg?typeid=9</t>
   </si>
   <si>
-    <t>/Bulletin/Detail/uomdnhoUoWvMFa8ce4zYMQ?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/5XT_6l4aNN_OQfb208cYtg?typeid=9</t>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/J3ByKlpyULZLtHehAJUa_g?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/w5wAafr4zKG_ZR88_qWdVQ?typeid=9</t>
   </si>
   <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/xah9AQII8GupFO7uV7kz-Q?typeid=9</t>
@@ -301,12 +307,6 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/AFuil2ECiqiNku1SmowIGQ?typeid=9</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/kVDslqExqB7BSiqJuFzXCg?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/cU2pYInOEJ4NOhg-uOH5Zg?typeid=9</t>
-  </si>
-  <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/ftv6FPFis84j5uHWTq4lNA?typeid=8772</t>
   </si>
   <si>
@@ -355,6 +355,9 @@
     <t>https://www.cdc.gov.tw/HireList/Detail?hireId=dbhD6saaWV5URglIuc0HhA</t>
   </si>
   <si>
+    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=Zqa4DDs0UoZULIvGT10iAA</t>
+  </si>
+  <si>
     <t>https://www.cdc.gov.tw/HireList/Detail?hireId=_KGB6fXszZ2udoZvtWhyuw</t>
   </si>
   <si>
@@ -364,9 +367,6 @@
     <t>https://www.cdc.gov.tw/HireList/Detail?hireId=4wyEVe65rp-Hr9DETX8n2g</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=ndMCl2Q6Sfsq3tUerM6pcw</t>
-  </si>
-  <si>
     <t>https://www.cdc.gov.tw/HireList/Detail?hireId=snieuoubdCfzpuQJABGcjA</t>
   </si>
   <si>
@@ -388,6 +388,12 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/u9ej71cxiu9bJqO0gMxdOQ?typeid=11</t>
   </si>
   <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/y6MiRdu9X-y3kAs1UrXvng?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/RpwW0PpibHaRFJpatPM1HA?typeid=9</t>
+  </si>
+  <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/5MtrgzOJApOSjivffWLWRw?typeid=9</t>
   </si>
   <si>
@@ -412,13 +418,13 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/Mhpv_WBf9Gw4pLB1hMe1hg?typeid=9</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/uomdnhoUoWvMFa8ce4zYMQ?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/5XT_6l4aNN_OQfb208cYtg?typeid=9</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-25\$\@\$中央流行疫情指揮中心今(25)日表示，今年第一批採購Moderna疫苗151.21萬劑，於今日下午抵達桃園國際機場，完成通關程序後，直接運送至指定冷儲物流中心進行後續檢驗封緘作業，再提供COVID-19接種計畫所列實施對象接種。本批效期至2022年4月23日。\$\@\$指揮中心說明，已於2021年7月22日與美國Moderna公司簽署2年共3,500萬劑COVID-19疫苗之供應合約，今年預定供應2,000萬劑疫苗做為基礎劑、基礎加強劑或追加劑使用，以因應SARS-CoV-2變異病毒株之威脅。</t>
+    <t>發佈日期：2022-01-26\$\@\$中央流行疫情指揮中心今(26)日公布國內新增92例COVID-19確定病例，分別為46例本土個案及46例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為24例男性、22例女性，年齡介於未滿5歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為27例男性、19例女性，年齡介於未滿5歲至60多歲，分別自美國(9例)、英國、加拿大及荷蘭(各2例)、馬來西亞、阿拉伯聯合大公國、法國、中國、瑞典、柬埔寨、越南、新加坡(各1例)移入；另23例調查中。入境日介於今(2022)年1月9日至1月25日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,542,669例新型冠狀病毒肺炎相關通報(含5,523,800例排除)，其中18,503例確診，分別為3,475例境外移入，14,974例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計122例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月26日新增本土COVID-19確診個案表.pdf\$\@\$1月26日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-25\$\@\$中央流行疫情指揮中心今(25)日表示，帛琉近期疫情快速上升，近7日每日平均確診數72例，累計651例確診，另昨(24)日公布2例自帛琉境外移入個案。抵帛之美國CDC專家推測可能為感染Omicron株，評估未來一至兩週應為疫情高峰。\$\@\$指揮中心說明，基於國人至當地有感染風險，指揮中心於1月25日起將帛琉之國際旅遊疫情建議等級提升至第三級警告(Warning)，提醒國人應避免至帛琉進行所有非必要旅遊。除基於(醫療)人道或急迫理由必須緊急赴臺之外籍旅客可另行申請外，入境旅客應遵循相關檢疫規定：所有入境旅客，不論身分(本國籍與外國籍人士等)或來臺目的，原則均應檢附「表定航班時間前2日內COVID-19核酸檢驗報告」及預訂「檢疫居所證明」始得搭機來臺，並於抵臺前48小時內預先使用手機上網登入「入境檢疫系統」，填寫健康情形及旅遊史，完成線上健康申報。另自帛返臺旅客與其他國家入境旅客一致，適用春節檢疫專案。\$\@\$指揮中心強調，將嚴密監控疫情變化，隨時調整各項防檢疫措施，相關資訊可至衛生福利部疾病管制署全球資訊網首頁「COVID-19防疫專區-春節檢疫措施專案」(https://www.cdc.gov.tw/Category/MPage/y-WU-wWeGC8M5ihxysmbFw)查閱。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-25\$\@\$中央流行疫情指揮中心於今(25)日表示，為確保農曆春節連假期間COVID-19自費核酸檢驗指定機構檢驗量能，以應民眾出境或出入醫療/照護機構等其他因素檢附COVID-19陰性檢驗證明之需，指揮中心已將農曆春節連假期間提供服務資訊公布於衛生福利部全球資訊網／春節衛福、防疫措施(網址：https://www.mohw.gov.tw/cp-5380-65644-1.html )及衛生福利部疾病管制署全球資訊網／COVID-19防疫專區／醫療照護機構感染管制相關指引／開放民眾自費檢驗COVID-19申請規定項下(網址：https://www.cdc.gov.tw/Category/MPage/I92jtldmxZO_oolFPzP9HQ )，方便民眾上網查閱。另健保署LINE(點此加入：https://line.me/R/ti/p/%40dyk0948w )推出「春節期間自費COV19 PCR這裏找」專區，可以「定位查詢」或「院所名稱」搜尋附近篩檢的醫事服務機構，方便得知收費資訊、採檢模式及時間表、服務網址、電話等資訊。\$\@\$指揮中心說明，為使民眾便於掌握COVID-19自費核酸檢驗資訊，指揮中心公布各自費核酸檢驗指定機構於今(2022)年1月29日至2月6日農曆春節連假期間提供服務情形，包括每日提供常規檢驗及快速檢驗之採檢時間、收費情形、採檢模式（如：採網路預約、電話預約、現場報名、固定時間或隨到隨採等）、每日可採檢人數、指定機構服務網址及聯繫電話等。\$\@\$指揮中心進一步說明，目前全國自費核酸檢驗指定機構共216家，其中有187家自費檢驗指定機構於農曆春節期間持續提供自費核酸檢驗服務，開設率達87％。有自費核酸檢驗需求民眾於檢驗前，請務必先行至醫院官方網站或致電詢問及確認相關採檢事宜。\$\@\$指揮中心提醒民眾，因應近期COVID-19全球疫情升溫，Omicron等新興變異株於全球迅速擴散，適逢春節前返鄉人潮，請民眾於檢疫期間及自主健康管理期間應遵守防疫措施。有自費核酸檢驗需求民眾進入醫院請全程配戴口罩，並加強洗手、落實呼吸道衛生與咳嗽禮節，保持良好個人衛生習慣，以保護自身健康及維護國內社區安全。</t>
   </si>
   <si>
     <t>發佈日期：2021-07-10\$\@\$中央流行疫情指揮中心今（10）日表示，近日有網友散布「三級警戒微解封的不可思議之處，新冠肺炎病毒只會攻擊家人」等訊息，相關內容多有誤導，且在錯誤基礎上進行不當類比，指揮中心再次強調，相關防疫指引已清楚說明，原本同住家人可以繼續維持生活，相關指引都是針對日常非同住者間的行為互動加以規範，呼籲民眾勿輕信或隨意散播、轉傳錯誤訊息，造成防疫困擾。\$\@\$指揮中心指出，有關7月13號以後針對部分場所將適度鬆綁，但仍須遵守防疫相關指引及規範，而此波疫情中，不少個案均為家戶群聚感染，由於室內密切接觸風險較高，因此對於室內社交人數須有較嚴格規範，但不包含原本同住的家人，也無需限制同住家人不能在家打麻將、看電影、吃飯等。 圖片 附件\$\@\$0710指揮中心：勿輕信「三級警戒微解封的不可思議之處」之網傳.jpg</t>
@@ -427,13 +433,49 @@
     <t>發佈日期：2021-06-13\$\@\$近日有網友在臉書FB以自製圖文方式散布「政府讓人民施打未受認證且保護力低之國產疫苗」、「國產疫苗的中和抗體效價比國外疫苗差」、「國產疫苗為什麼不向國際提出緊急授權」，中央流行疫情指揮中心(下稱指揮中心)今（13）日嚴正澄清表示，目前國產疫苗臨床試驗尚在進行中，最終結果須等廠商提出EUA 申請，經專家會議審查疫苗的製程管控、藥毒理試驗及臨床試驗結果，在緊急公衛的需求下，確認疫苗使用效益大於風險，才會核准緊急授權使用。\$\@\$指揮中心指出，目前國產疫苗廠商皆已積極規劃，以取得國際認證為目標。國產疫苗需經食藥署和專家會議嚴謹審查，在緊急公衛需求，並確認效益大於風險，才會核准緊急授權使用。此外，各家廠牌的疫苗所使用的檢驗實驗室及檢驗方式不同且無協和，無法直接由各實驗室產生數值進行比較。國產疫苗仍需等廠商提出申請，經過中央主管機關嚴格把關及審查通過後，確認品質、安全、療效後，品質沒有問題，疫苗方可供民眾施打。\$\@\$指揮中心再次提醒，民眾接獲來源不明的訊息時，應先進行查證，切勿隨意散播、轉傳，以免觸法。 圖片 附件\$\@\$0613網傳「政府讓人民施打未受認證且保護力低之國產疫苗」-1.jpg\$\@\$0613網傳「政府讓人民施打未受認證且保護力低之國產疫苗」-2.jpg</t>
   </si>
   <si>
-    <t>發佈日期：2021-06-12\$\@\$中央流行疫情指揮中心今(12)日嚴正澄清，近日於社群平台流傳「代工三億劑嫌太多賣不出去」等訊息，指揮中心於6月10日記者會已公開說明，與AstraZeneca原廠洽談授權製造事宜時，我方提出可年產一億劑之規劃，但原廠要求需年產三億劑，經評估，對我方產能過於沉重，並無以「賣不出去」為由拒絕原廠授權製造，卻被有心人刻意扭曲語意。此圖文與事實不符，指揮中心特此澄清。\$\@\$指揮中心重申，防疫相關資訊應以中央流行疫情指揮中心公布內容為主。提醒民眾，收到來路不明訊息多加留意、查證，切勿轉傳散播。詳情請上官網查詢 (http://at.cdc.tw/Q7S2Vt)。 圖片 附件\$\@\$20210612澄清.jpg</t>
+    <t>發佈日期：2021-06-01\$\@\$中央流行疫情指揮中心今(1)日指出，近日有網友在通訊軟體LINE散布「臺中市太原路復健醫院被徵收為方艙醫院」，臺中市政府衛生局已澄清為不實訊息，請民眾勿再轉傳與散布，以免觸法遭罰。\$\@\$指揮中心表示，臺中市政府已對外澄清，此復健醫院近期進行搬遷作業，是為了提升醫療品質，正以BOT方式規劃市立綜合醫院，並非徵用作為方艙醫院。\$\@\$指揮中心副指揮官陳宗彥指出，因應疫情變化，各地方政府規劃應變醫院及專責醫院收治患者，民眾接獲來源不明的訊息時，應先進行查證，切勿隨意散播、轉傳，以免觸法。\$\@\$指揮中心重申，防疫相關資訊應以中央流行疫情指揮中心公布內容為主，散播假訊息構成犯罪，會被判處最高三年有期徒刑或併科三百萬元罰金。提醒民眾，收到來路不明訊息多加留意、查證，切勿轉傳散播，以免觸法。詳情請上官網查詢(http://at.cdc.tw/Q7S2Vt)。 圖片 附件\$\@\$網傳「臺中市太原路復健醫院被徵收為方艙醫院」為不實訊息勿轉傳.jpg\$\@\$勿散播不實訊息，以免觸法受罰.jpg</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-30\$\@\$各位醫界朋友，您好：\$\@\$鑑於國際COVID-19疫情嚴峻及Omicron新型變異株威脅增加，嚴重特殊傳染性肺炎中央流行疫情指揮中心(下稱指揮中心)邀請各縣市兒科、內科、家醫科、耳鼻喉科及婦產科等有提供診治呼吸道症狀服務之診所/衛生所，自明(2022)年1月1日起加入公費COVID-19家用快篩試劑發放行列，指揮中心感謝基層診所積極守護社區健康的熱誠，並籲請各定點診所醫師針對具呼吸道症狀就醫民眾，加強發放公費COVID-19家用快篩試劑。\$\@\$指揮中心於今(2021)年8月30日起啟動前揭計畫，全國共計18個縣市86家診所/衛生所參加，迄今已發放1萬餘劑公費COVID-19家用快篩試劑，於有效監測下均無發現陽性個案。為提升民眾取用COVID-19家用快篩試劑可近性及擴大監測，自明年1月1日起增加至21個縣市272家診所/衛生所參與。\$\@\$由於國內現處於流感季節且COVID-19症狀與上呼吸道感染症狀相似，指揮中心籲請定點診所針對出現呼吸道症狀就醫民眾，加強發放公費COVID-19家用快篩試劑，尤可對於幼兒及其陪病家屬加強評估發放；另請診所衛教民眾試劑使用流程及注意事項、提醒民眾匿名填寫線上問卷以回報快篩結果等資料，並將發放民眾資料登錄於疾病管制署系統中。\$\@\$該計畫相關內容公布於疾病管制署全球資訊網 (http://www.cdc.gov.tw) COVID-19防疫專區&gt;臺灣社交距離APP及採檢地圖&gt;COVID-19社區加強監測方案，歡迎查閱。\$\@\$感謝您與我們共同維護全民的健康安全。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-10-22\$\@\$各位醫界朋友，您好：\$\@\$我國新型冠狀病毒(SARS-CoV-2)感染臨床處置暫行指引建議可依照病患病程與嚴重度，對不需用氧且有重症風險因子之病患給予單株抗體，需用氧病患則除dexamethasone外可併用免疫調節劑tocilizumab或baricitinib。鑒於近期國際間藥物使用建議與國內適應症均有更新，經COVID-19專家諮詢會議更新建議如下：\$\@\$1.複合單株抗體Casirivimab + imdevimab或Bamlanivimab + etesevimab。適用對象為\$\@\$― 具以下任一風險因子，未使用氧氣且於發病十天內之≧12歲且體重≧40公斤病患；\$\@\$― 風險因子包括：年齡 ≧ 65歲、糖尿病、慢性腎病、心血管疾病（含高血壓）、慢性肺疾、BMI ≧25（或12-17歲兒童BMI超過同齡第85百分位）、懷孕、其他影響免疫功能之疾病或已知重症風險因子等。\$\@\$目前實證顯示上述兩種複合單株抗體對國內現今主要檢出之Delta與Alpha變異株均有效，但由於體外試驗顯示Bamlanivimab + etesevimab可能無法有效中和包括Beta、Gamma、Delta plus與Mu變異株，建議臨床醫師使用時需考量流行狀況與參閱最新版「SARS-CoV-2之藥物使用實證摘要」附表。\$\@\$另參考WHO最新公布治療建議，於診治指引註解中新增「隨機對照研究顯示對血清抗體陰性之嚴重肺炎以上程度病患，除標準治療外，給予casirivimab 4000mg + imdevimab 4000mg 可降低死亡率」。\$\@\$2.Remdesivir適用對象為嚴重肺炎以上（未使用吸氧治療下的SpO2 ≦ 94%、需使用吸氧治療、需使用高流量氧氣或非侵襲性呼吸器但未插管）病患。另於診治指引註解中新增「若住院病患胸部X光片顯示肺炎，雖未達重症標準且不符合單株抗體適用條件，仍可申請使用remdesivir」。但由於目前尚無併用單株抗體之效益與安全性資料，目前仍暫不建議remdesivir與單株抗體同時併用。\$\@\$由於近日媒體報導ivermectin用於治療COVID-19一事，經專家委員審視國際文獻，發現ivermectin相關臨床試驗研究證據力等級低，且部分研究涉及科學誠信，其中亦有發表論文被撤回之情形，統合分析結果顯示目前證據不支持ivermectin可用於治療或預防COVID-19，WHO及歐美等具公信力之治療指引均不建議使用於COVID-19之治療。為確保國人健康，我國診治指引治療藥物建議係根據最高等級實證基礎制訂，參考目前各方面之資料，仍不建議ivermectin納入我國診治指引之治療建議藥物。\$\@\$「嚴重特殊傳染性肺炎」之診療相關資訊將隨時依防疫需求與最新文獻證據更新並公布於疾病管制署全球資訊網(http://www.cdc.gov.tw)。\$\@\$感謝您與我們共同維護全民的健康安全。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-13\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$急性傳染病組\$\@\$約用助理\$\@\$(徵才案號：1106，含延長公告)\$\@\$(計1名)\$\@\$張○純(A22889****)\$\@\$二、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一) 口試：\$\@\$1、報到時間：111年01月17日星期一15:20~15:30，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署7樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：16:40~17:10。\$\@\$(二)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(三)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於111年01月17日上午10點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3823)，俾利安排應試座位。\$\@\$(四)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(五)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-12\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$檢疫組\$\@\$約用助理\$\@\$(徵才案號：0507)\$\@\$(計4名)\$\@\$陳○涵(A22534****)\$\@\$張○純(A22889****)\$\@\$林○翔(S12427****)\$\@\$謝○樺(K12260****)\$\@\$二、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一) 口試：\$\@\$1、報到時間：111年01月17日星期一15:20~15:30，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署7樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：15:30~16:40。\$\@\$(二)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(三)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於111年01月17日上午10點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3864)，俾利安排應試座位。\$\@\$(四)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(五)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-24\$\@\$中央流行疫情指揮中心今(24)日表示，因應國際疫情嚴峻，且國內發生新變異株Omicron感染事件，經指揮中心與相關單位溝通及評估後於今日宣布，今(2022)年1月25日至2月7日維持疫情警戒標準為第二級，調整或維持相關措施及規定如下：\$\@\$一、維持加嚴之戴口罩規定，除少數例外情形，外出全程佩戴口罩：\$\@\$(一)運動、唱歌、拍照及直播、錄影、主持、報導、致詞、演講、講課等談話性質工作或活動之正式拍攝或進行時，恢復為須戴口罩。\$\@\$(二)下列場合得免戴口罩，但應隨身攜帶口罩，且如本身有相關症狀或與不特定對象無法保持社交距離時，仍應戴口罩：\$\@\$1. 農林漁牧工作者於空曠處(如：田間、魚塭、山林)工作。\$\@\$2. 於山林(含森林遊樂區)、海濱活動。\$\@\$3. 於溫/冷泉、烤箱、水療設施、三溫暖、蒸氣室、水域活動等易使口罩潮濕之場合。\$\@\$(三)外出時有飲食需求，得免戴口罩。\$\@\$(四)於指揮中心或主管機關指定之場所或活動(例如：藝文表演/劇組/電視主播等演出人員正式拍攝演出時、運動競賽之參賽選手及裁判於比賽期間等)，如符合指揮中心或主管機關之相關防疫措施，得暫時脫下口罩。\$\@\$二、營業場所及公共場域(含交通運輸)應嚴格遵守：實聯制、量體溫、加強環境淸消、員工健康管理、確診事件即時應變。\$\@\$三、高鐵、臺鐵、公路客運、船舶(固定餐飲區除外)、國內航班：於運具內（車廂、船舶、航空器）禁止飲食。\$\@\$四、賣場、超市、市場加強人流管制：室內空間至少1.5米/人(2.25平方米/人)，室外空間至少1米/人(1平方米/人)；不開放試吃。\$\@\$五、宗教場所、宗教集會活動：依內政部規定之防疫措施辦理。\$\@\$六、餐飮場所：嚴格落實實聯制、量體溫、提供洗手設備及消毒用品；宴席不得逐桌敬酒敬茶；違反者依法裁處並限期改善，未完成改善者，不得提供內用服務。\$\@\$指揮中心呼籲，防疫工作人人有責，請民眾自主落實防疫措施，維持個人衛生好習慣，戴口罩、勤洗手、保持社交距離；出入公共場域落實實聯制、體溫量測等，降低病毒傳播風險，保護自己也保護他人，共同維護國內社區安全。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-23\$\@\$中央流行疫情指揮中心今(23)日公布國內新增89例COVID-19確定病例，分別為52例本土個案及37例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為32例男性、20例女性，年齡介於未滿5歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為17例男性、20例女性，年齡介於未滿10歲至60多歲，分別自美國(12例)、法國(3例)、英國(2例)、丹麥、印度、烏克蘭、菲律賓、土耳其、澳大利亞(各1例)移入；另14例調查中。入境日介於今(2022)年1月8日至1月22日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,441,110例新型冠狀病毒肺炎相關通報(含5,422,031例排除)，其中18,325例確診，分別為3,368例境外移入，14,903例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增2例空號病例(案17934、案17970，再次採檢為陰性改判排除)，累計119例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月23日新增境外移入COVID-19確診個案表.pdf\$\@\$1月23日新增本土COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-22\$\@\$中央流行疫情指揮中心今(22)日公布國內新增130例COVID-19確定病例，分別為82例本土個案及48例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為12例男性、70例女性，年齡介於未滿10歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為29例男性、19例女性，年齡介於未滿5歲至70多歲，分別自美國(13例)、加拿大及新加坡(各4例)、菲律賓(3例)、印度、土耳其及香港(各2例)、奧地利、奈及利亞、義大利、柬埔寨、德國、越南及巴西(各1例)移入；另11例調查中。入境日介於去(2021)年12月31日至今(2022)年1月21日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,418,957例新型冠狀病毒肺炎相關通報(含5,400,086例排除)，其中18,238例確診，分別為3,331例境外移入，14,853例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案18182，再次採檢為陰性，改判排除)，累計117例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月22日新增本土COVID-19確診個案表.pdf\$\@\$1月22日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-21\$\@\$中央流行疫情指揮中心今(21)日公布國內新增68例COVID-19確定病例，分別為23例本土個案及45例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為10例男性、13例女性，年齡介於未滿10歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為20例男性、24例女性及1例調查中，年齡介於未滿5歲至70多歲，分別自美國(17例)、菲律賓(4例)、越南及以色列(各3例)、加拿大(2例)、波蘭、澳大利亞、韓國、新加坡、瑞典、俄羅斯、英國及愛爾蘭(各1例)移入；另8例調查中。入境日介於今(2022)年1月5日至1月20日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,394,042例新型冠狀病毒肺炎相關通報(含5,375,246例排除)，其中18,109例確診，分別為3,283例境外移入，14,772例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計116例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月21日新增本土COVID-19確診個案表.pdf\$\@\$1月21日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
     <t>發佈日期：2022-01-21\$\@\$中央流行疫情指揮中心今(21)日表示，台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的第十六批BNT疫苗99.45萬劑，已於今日上午順利運抵桃園國際機場，並在完成通關程序後，直接運送至指定冷儲物流中心進行後續檢驗封緘作業。\$\@\$指揮中心說明，由台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的BNT疫苗1,500萬劑，目前共計到貨1433.07萬劑，分別為首批9月2日93萬劑、第二批9月9日91萬劑、第三批9月30日54萬劑、第四批10月1日67萬劑、第五批10月4日27萬劑、第六批10月7日88.92萬劑、第七批10月8日88.92萬劑、第八批10月14日82.7萬劑、第九批10月28日90.21萬劑、第十批10月29日91.03萬劑、第十一批11月5日87.17萬劑、第十二批11月12日92.66萬劑、第十三批11月25日93.83萬劑、第十四批12月9日192.35萬劑、第十五批12月30日93.83萬劑，以及本批99.45萬劑。本批疫苗效期至2022年5月25日，將由指揮中心統籌運用，儘速提供民眾接種。\$\@\$對於台積電、鴻海暨永齡基金會、慈濟基金會三間企業和民間團體積極協助，提供更多的疫苗讓民眾接種，加速提升臺灣疫苗覆蓋率，指揮中心再次表達由衷的謝意。</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-20\$\@\$中央流行疫情指揮中心今(20)日公布國內新增37例COVID-19確定病例，分別為13例本土個案及24例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為5例男性、8例女性，年齡介於未滿5歲至80多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為13例男性、11例女性，年齡介於10多歲至50多歲，分別自美國(10例)、越南(3例)、法國及澳大利亞(各2例)、巴拉圭及沙烏地阿拉伯(各1例)移入；另5例調查中。入境日介於今(2022)年1月5日至1月19日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,363,205例新型冠狀病毒肺炎相關通報(含5,344,301例排除)，其中18,041例確診，分別為3,238例境外移入，14,749例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案18119，再次採檢為陰性，改判排除)，累計116例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月20日新增境外移入COVID-19確診個案表.pdf\$\@\$1月20日新增本土COVID-19確診個案表.pdf</t>
+    <t>發佈日期：2022-01-20\$\@\$中央流行疫情指揮中心今(20)日表示，鑒於帛琉疫情升溫，為確保社區防疫安全，自帛琉來臺旅客，除搭機前須持二日內核酸檢測報告外，入境仍依現行作法，採綠色專屬通道，並強化相關入境採檢及檢疫措施，請赴帛琉或自帛琉抵臺旅客，務必配合當地及回臺相關防疫及檢疫措施，以保障國內社區安全。\$\@\$指揮中心指出，強化入境採檢及檢疫措施將自今(2022)年1月22日(含)起實施，入境旅客公費入住集中檢疫所實施5天檢疫，接續加強自主健康管理9天，再進行一般自主健康管理7天，並配合入境時(集中檢疫所採檢)、第5天及第13至14天進行PCR檢測，第8天、第11天及一般自主健康管理期滿(第20至21天)以家用快篩試劑各檢測1次。另提醒旅客於到訪帛琉期間，請務必落實自我健康監測，並確實遵守指揮中心及帛國的防疫措施，如佩戴口罩、勤洗手及保持社交距離等規範，以維護自身的健康安全。\$\@\$指揮中心說明，針對1月22日分別有旅遊團啟程至帛琉，以及自帛琉入境旅客，請儘速辦理下列事項：\$\@\$(一) 駐帛琉共和國大使館將持續提供當地疫情風險資訊予交通部觀光局，以利旅行社向旅客宣達該國疫情風險，以及須配合的防疫措施（包括從事醫療照護工作人員，於加強自主健康管理期間不得上班）。\$\@\$(二) 為確保赴帛琉旅客瞭解當地疫情風險，駐帛琉共和國大使館亦將於機場加強宣導。\$\@\$(三) 有關自帛琉入境之14名旅客(含後送轉診病人)，將請駐帛琉共和國大使館轉達調整後的防疫措施，並請醫療應變組瞭解後送轉診病人的就醫需求，以利預先調度。\$\@\$此外，外交部已調整帛琉旅遊警示為「提醒注意」，並將召集交通部與駐帛琉共和國大使館共同研商合理的退費機制。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-20\$\@\$中央流行疫情指揮中心今(20)日表示，我國「數位新冠病毒健康證明」自去(110)年12月28日上線後已核發超過26萬份。考量國內外疫情升溫，各界建議及需求，指揮中心將於今(111)年1月21日上午8時開放「數位新冠病毒健康證明」供國內使用，共計三大功能：所有在國內接種者皆可下載、符合歐盟規範的查驗程式，可驗證60國的證明、提供具實名制的APP作為證明載具。\$\@\$指揮中心指出，原本下載限持有效護照者，現以戶口名簿的戶號取代，民眾可以電腦或手機上網申辦「數位新冠病毒健康證明」（ https://dvc.mohw.gov.tw ），注意事項說明如下：\$\@\$一、確認身分：\$\@\$(一)國人：(1)身分證號+健保卡號+戶口名簿戶號；(2) FIDO；(3)自然人憑證。三種方式擇一。\$\@\$(二)外來人口：(1)統一證號+健保卡號；(2) 統一證號+入出境證號；(3) 統一證號+護照號碼。三種方式擇一。\$\@\$二、選擇項目：選擇「疫苗接種數位證明」或「檢驗結果數位證明」。\$\@\$三、取得證明：於申請成功畫面點選「下載/列印 數位證明」，檔案格式為PDF，提醒要先保存於行動裝置或電腦硬碟中，再視個人需要列印紙本。無列印設備但又有列印需求者，可於申請成功畫面選擇超商並點選「取得超商列印碼」，系統將產製超商取件條碼或取件編號，請自行攜碼至超商付費列印。\$\@\$此次僅變更確認身分方式，方便未持有護照者下載。具有效護照民眾申辦數位證明時仍會產出護照號碼，未來不必為出國另行下載；不具有效護照民眾者護照號碼欄位顯示為「Not Issued」。\$\@\$「數位新冠病毒健康證明」查驗程式係網頁形式（ https://dvc.mohw.gov.tw/verifier-web ），不需下載安裝，民眾也可在衛福部官網取得連結，該網頁不會保留受查驗者的個資，符合歐盟GDPR，使用步驟如下：\$\@\$一、前往網站：使用具備相機及網頁瀏覽器的手機、電腦等，開啟瀏覽器前往上述網址。\$\@\$二、同意隱私權聲明、允許取用相機權限。\$\@\$三、不退出查驗網頁且不中斷網路者，可續使用並維持最新功能，退出或中斷者可重新上網更新。\$\@\$查驗程式以顏色、圖示及文字顯示查驗結果，綠色、打勾為通過，紅色、打叉為不通過，黃色、三角驚嘆號為待確認狀態（包括：接種不完整、效期不符、非我國同意的疫苗或檢驗等），不合規格的QR code則會出現解析錯誤的訊息。驗證程式個人基本資料僅會顯示姓名及出生年月日，如需嚴格確認是否為本人持有，建議仍需搭配其它身分證件。由於我國已是歐盟數位新冠證明(EU-DCC)的成員，故本查驗程式也可查證持同樣規格由其它國家發行的疫苗、核酸檢驗數位證明，及部分有發行康復證明的國家。\$\@\$指揮中心提醒，依據世界衛生組織(WHO)規範，疫苗證明可採紙本或數位方式，檢驗陰性或康復證明亦可做為健康證明，數位證明僅是方式之一，民眾有多元方式可提供各場所查驗。\$\@\$另外，指揮中心亦已備有標準的應用軟體介接程式(API)供國內具實名制功能的APP介接取得民眾自己的數位證明，並以APP為載具。發行或管理APP者，確認符合個資法及GDPR、身分驗證強度不低於本數位證明平臺，且APP後臺不得留存數位證明，請向指揮中心正式申請。\$\@\$為更新原有版本的功能，申辦平台預計今年1月20日下午5時至次(21)日上午8時停止服務進行更版，有急需出國使用者，請先提前下載。詳細下戴及驗證系統操作方式可以參考衛生福利部官網數位證明專區( https://covid19.mohw.gov.tw/ch/np-5345-205.html )。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-20\$\@\$中央流行疫情指揮中心今(20)日表示，因應Omicron新型變異株之威脅，且國內本土疫情尚未平息，存在社區傳播風險，自今(2022)年1月21日起，民眾前往「歌廳、舞廳、夜總會、俱樂部、酒家、酒吧、酒店(廊)、理容院(觀光理髮、視聽理容)及特種咖啡茶室、夜店、舞場、三溫暖」等休閒娛樂場所時，應配合出示完整接種COVID-19疫苗紀錄，始得入內活動消費。接種紀錄除出示「紙本疫苗接種卡」外，亦可使用「健保快易通」或「數位新冠病毒健康證明」提供檢視。\$\@\$指揮中心說明，上述休閒娛樂場所具有接觸不特定人及無法保持社交距離之特性，COVID-19傳播風險相對較高，為降低於場所消費期間接觸染疫之風險，強化場所之防疫管理措施，除維持該等場所工作人員皆應接種COVID-19疫苗2劑且滿14天，未完整接種者，應每週定期篩檢陰性，始得提供服務外，自1月21日起調整民眾前往消費時，須配合出示完整接種COVID-19疫苗2劑且滿14天紀錄，始得進場，請民眾務必配合，也請業者落實查核，使顧客安心消費，同時保護員工健康安全。\$\@\$指揮中心另指出，針對醫院及住宿式長照機構等現行已有針對COVID-19疫苗接種情形進行規範之場域，請民眾依規定，配合出示COVID-19疫苗紀錄，接種紀錄同樣可使用「紙本疫苗接種卡」、「健保快易通」或「數位新冠病毒健康證明」提供檢視。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-25\$\@\$中央流行疫情指揮中心今(25)日公布國內新增38例COVID-19確定病例，分別為13例本土個案及25例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為4例男性、9例女性，年齡介於未滿5歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為8例男性、17例女性，年齡介於10多歲至70多歲，分別自加拿大(5例)、美國、泰國及印度(各3例)、日本(2例)、奈及利亞、瑞典及中國(各1例)移入；另6例調查中。入境日介於今(2022)年1月11日至1月24日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,501,288例新型冠狀病毒肺炎相關通報(含5,482,563例排除)，其中18,411例確診，分別為3,429例境外移入，14,928例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增3例空號病例(案18216-18218，再次採檢為陰性，改判排除)，累計122例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月25日新增本土COVID-19確診個案表.pdf\$\@\$1月25日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-25\$\@\$中央流行疫情指揮中心今(25)日表示，因應國內本土疫情升溫，目前已提供民眾於各地方政府衛生局安排/指定之合約醫療院所預約或至隨到隨打接種站方式接種COVID-19疫苗。為提供多元疫苗預約管道，加速提升民眾免疫保護力，COVID-19公費疫苗預約平臺（https://1922.gov.tw/ ，以下簡稱預約平臺）第21期將提供「已完整接種兩劑COVID-19疫苗滿12週且滿18歲以上」民眾，預約接種疫苗追加劑。另請已於各地方政府衛生局安排/指定之合約醫療院所完成預約之民眾，請依原已預約時段前往接種，無需再於預約平臺重複預約。\$\@\$預約平臺相關對象及期程說明如下：\$\@\$一、施打時程：2月7日至2月13日。\$\@\$二、符合資格對象：2021年11月21日前已完整接種兩劑疫苗且間隔滿12週之18歲以上民眾[即2004/2/13(含)前出生]預約接種疫苗追加劑。\$\@\$三、預約分流時程：\$\@\$(一)65歲以上：1月26日上午10時至1月27日下午4時。\$\@\$(二)50歲-64歲：1月26日中午12時至1月27日下午4時。\$\@\$(三)18歲-49歲：1月26日下午2時至1月27日下午4時。\$\@\$指揮中心說明，民眾可於1月25日下午2時起於預約平臺進行預約資格查詢，不再另發送預約提醒簡訊，符合資格民眾請記得於預約時間進行預約，預約當日如遇啟動流量管制亦請配合依序排隊耐心等候預約。\$\@\$指揮中心指出，預約平臺第21期僅提供民眾預約接種疫苗追加劑，民眾若有第一、二劑或基礎加強劑接種需求，請持接種紀錄(小黃卡)至各地方政府指定/安排合約醫療院所或衛生所預約接種，或所設置之隨到隨打接種站接種。前述醫療院所資訊，可至疾管署全球資訊網( https://www.cdc.gov.tw/ ) COVID-19疫苗接種院所項下，利用「COVID-19疫苗接種院所」或「COVID-19疫苗接種院所地圖」，依各地方政府衛生局提供資訊連結預約接種。\$\@\$指揮中心提醒，請民眾前往接種COVID-19疫苗前，應備妥「COVID-19疫苗接種紀錄卡」及健保卡，並經醫生評估過往疫苗接種史及檢核接種紀錄後，提供民眾疫苗接種。另18歲至未滿20歲民眾，如自行前往接種，請持家長簽具之意願同意書，若由家長陪同前往接種，請本人與家長於現場共同簽署意願同意書。</t>
   </si>
 </sst>
 </file>
@@ -839,10 +881,13 @@
         <v>48</v>
       </c>
       <c r="C2" s="2">
-        <v>44586</v>
+        <v>44587</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>91</v>
+      </c>
+      <c r="E2" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -858,6 +903,9 @@
       <c r="D3" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="E3" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
@@ -872,6 +920,9 @@
       <c r="D4" s="3" t="s">
         <v>93</v>
       </c>
+      <c r="E4" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
@@ -886,9 +937,6 @@
       <c r="D5" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E5" t="s">
-        <v>134</v>
-      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
@@ -898,7 +946,7 @@
         <v>52</v>
       </c>
       <c r="C6" s="2">
-        <v>44585</v>
+        <v>44586</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>95</v>
@@ -912,7 +960,7 @@
         <v>53</v>
       </c>
       <c r="C7" s="2">
-        <v>44585</v>
+        <v>44586</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>96</v>
@@ -932,7 +980,7 @@
         <v>97</v>
       </c>
       <c r="E8" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -949,7 +997,7 @@
         <v>98</v>
       </c>
       <c r="E9" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -965,9 +1013,6 @@
       <c r="D10" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E10" t="s">
-        <v>137</v>
-      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
@@ -982,6 +1027,9 @@
       <c r="D11" s="3" t="s">
         <v>100</v>
       </c>
+      <c r="E11" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
@@ -1052,8 +1100,11 @@
       <c r="D16" s="3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1066,8 +1117,11 @@
       <c r="D17" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1081,7 +1135,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1095,7 +1149,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1109,7 +1163,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1123,7 +1177,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1137,7 +1191,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1151,7 +1205,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1159,13 +1213,13 @@
         <v>70</v>
       </c>
       <c r="C24" s="2">
-        <v>44585</v>
+        <v>44586</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1173,13 +1227,13 @@
         <v>71</v>
       </c>
       <c r="C25" s="2">
-        <v>44583</v>
+        <v>44585</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1187,13 +1241,13 @@
         <v>72</v>
       </c>
       <c r="C26" s="2">
-        <v>44582</v>
+        <v>44583</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1201,13 +1255,13 @@
         <v>73</v>
       </c>
       <c r="C27" s="2">
-        <v>44581</v>
+        <v>44582</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1221,7 +1275,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1234,8 +1288,11 @@
       <c r="D29" s="3" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1248,8 +1305,11 @@
       <c r="D30" s="3" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1263,7 +1323,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1313,10 +1373,13 @@
         <v>81</v>
       </c>
       <c r="C35" s="2">
-        <v>44583</v>
+        <v>44585</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>124</v>
+      </c>
+      <c r="E35" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1327,10 +1390,13 @@
         <v>82</v>
       </c>
       <c r="C36" s="2">
-        <v>44582</v>
+        <v>44584</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>125</v>
+      </c>
+      <c r="E36" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1341,13 +1407,13 @@
         <v>83</v>
       </c>
       <c r="C37" s="2">
-        <v>44582</v>
+        <v>44583</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>126</v>
       </c>
       <c r="E37" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1358,10 +1424,13 @@
         <v>84</v>
       </c>
       <c r="C38" s="2">
-        <v>44581</v>
+        <v>44582</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>127</v>
+      </c>
+      <c r="E38" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1372,10 +1441,13 @@
         <v>85</v>
       </c>
       <c r="C39" s="2">
-        <v>44581</v>
+        <v>44582</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>128</v>
+      </c>
+      <c r="E39" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1391,6 +1463,9 @@
       <c r="D40" s="3" t="s">
         <v>129</v>
       </c>
+      <c r="E40" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
@@ -1406,7 +1481,7 @@
         <v>130</v>
       </c>
       <c r="E41" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1417,10 +1492,13 @@
         <v>88</v>
       </c>
       <c r="C42" s="2">
-        <v>44580</v>
+        <v>44581</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>131</v>
+      </c>
+      <c r="E42" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1431,7 +1509,7 @@
         <v>89</v>
       </c>
       <c r="C43" s="2">
-        <v>44580</v>
+        <v>44581</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>132</v>
@@ -1445,7 +1523,7 @@
         <v>90</v>
       </c>
       <c r="C44" s="2">
-        <v>44579</v>
+        <v>44580</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>133</v>
@@ -1459,10 +1537,13 @@
         <v>48</v>
       </c>
       <c r="C45" s="2">
-        <v>44586</v>
+        <v>44587</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>91</v>
+      </c>
+      <c r="E45" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1478,6 +1559,9 @@
       <c r="D46" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="E46" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
@@ -1492,6 +1576,9 @@
       <c r="D47" s="3" t="s">
         <v>93</v>
       </c>
+      <c r="E47" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
@@ -1507,7 +1594,7 @@
         <v>94</v>
       </c>
       <c r="E48" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1518,10 +1605,13 @@
         <v>52</v>
       </c>
       <c r="C49" s="2">
-        <v>44585</v>
+        <v>44586</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>95</v>
+      </c>
+      <c r="E49" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1532,7 +1622,7 @@
         <v>53</v>
       </c>
       <c r="C50" s="2">
-        <v>44585</v>
+        <v>44586</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>96</v>
@@ -1552,7 +1642,7 @@
         <v>97</v>
       </c>
       <c r="E51" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1569,7 +1659,7 @@
         <v>98</v>
       </c>
       <c r="E52" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1585,9 +1675,6 @@
       <c r="D53" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E53" t="s">
-        <v>137</v>
-      </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
@@ -1602,6 +1689,9 @@
       <c r="D54" s="3" t="s">
         <v>100</v>
       </c>
+      <c r="E54" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
@@ -1672,6 +1762,9 @@
       <c r="D59" s="3" t="s">
         <v>105</v>
       </c>
+      <c r="E59" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
@@ -1686,6 +1779,9 @@
       <c r="D60" s="3" t="s">
         <v>106</v>
       </c>
+      <c r="E60" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
@@ -1743,7 +1839,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
         <v>25</v>
       </c>
@@ -1757,7 +1853,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>26</v>
       </c>
@@ -1771,7 +1867,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>27</v>
       </c>
@@ -1779,13 +1875,13 @@
         <v>70</v>
       </c>
       <c r="C67" s="2">
-        <v>44585</v>
+        <v>44586</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>28</v>
       </c>
@@ -1793,13 +1889,13 @@
         <v>71</v>
       </c>
       <c r="C68" s="2">
-        <v>44583</v>
+        <v>44585</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>29</v>
       </c>
@@ -1807,13 +1903,13 @@
         <v>72</v>
       </c>
       <c r="C69" s="2">
-        <v>44582</v>
+        <v>44583</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>30</v>
       </c>
@@ -1821,13 +1917,13 @@
         <v>73</v>
       </c>
       <c r="C70" s="2">
-        <v>44581</v>
+        <v>44582</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>31</v>
       </c>
@@ -1841,7 +1937,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>32</v>
       </c>
@@ -1854,8 +1950,11 @@
       <c r="D72" s="3" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="73" spans="1:4">
+      <c r="E72" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>33</v>
       </c>
@@ -1868,8 +1967,11 @@
       <c r="D73" s="3" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="74" spans="1:4">
+      <c r="E73" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>34</v>
       </c>
@@ -1883,7 +1985,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>35</v>
       </c>
@@ -1897,7 +1999,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>36</v>
       </c>
@@ -1911,7 +2013,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20220127
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="166">
   <si>
     <t>Press Title</t>
   </si>
@@ -31,6 +31,15 @@
     <t>Page Content</t>
   </si>
   <si>
+    <t>新增64例COVID-19確定病例，分別為21例本土及43例境外移入</t>
+  </si>
+  <si>
+    <t>指揮中心公布「COVID-19疫情期間民眾假期生活防疫指引」，籲請民眾主動落實防疫措施，平安過好年</t>
+  </si>
+  <si>
+    <t>台積電、鴻海永齡、慈濟三間企業和民間團體捐贈之第十七批BNT疫苗91.84萬劑於今(27)日上午抵臺</t>
+  </si>
+  <si>
     <t>新增92例COVID-19確定病例，分別為46例本土及46例境外移入</t>
   </si>
   <si>
@@ -49,6 +58,39 @@
     <t>今(2022)年第一批採購Moderna疫苗151.21萬劑於今(25)日下午抵臺</t>
   </si>
   <si>
+    <t>全國醫院即日起除例外情形，停止開放探病，並調整住院病人、陪(探)病者及醫療照護人員篩檢及疫苗接種等相關規定</t>
+  </si>
+  <si>
+    <t>因應國內COVID-19疫情發展，指揮中心1/24起調整全國住宿式長照機構訪客及新進住民管理等應變措施</t>
+  </si>
+  <si>
+    <t>為降低醫療量能負擔，首批我國採購之COVID-19口服抗病毒藥Molnupiravir抵臺，提供具重症風險因子之輕中度確診個案治療使用</t>
+  </si>
+  <si>
+    <t>新增51例COVID-19確定病例，分別為15例本土及36例境外移入</t>
+  </si>
+  <si>
+    <t>1月25日至2月7日維持第二級疫情警戒標準，並調整相關規定，請民眾自主落實防疫措施，共同維護國內社區安全</t>
+  </si>
+  <si>
+    <t>新增89例COVID-19確定病例，分別為52例本土及37例境外移入</t>
+  </si>
+  <si>
+    <t>新增130例COVID-19確定病例，分別為82例本土及48例境外移入</t>
+  </si>
+  <si>
+    <t>新增68例COVID-19確定病例，分別為23例本土及45例境外移入</t>
+  </si>
+  <si>
+    <t>台積電、鴻海永齡、慈濟三間企業和民間團體捐贈之第十六批BNT疫苗99.45萬劑於今(21)日上午抵臺</t>
+  </si>
+  <si>
+    <t>因應帛琉近期疫情，指揮中心說明相關檢疫應變措施</t>
+  </si>
+  <si>
+    <t>1月21日上午8時「數位新冠病毒健康證明」開放國內使用</t>
+  </si>
+  <si>
     <t>網傳「三級警戒微解封的不可思議之處」指揮中心： 原同住家人就不受限制，謠言邏輯誤導且比喻失當，請勿輕信轉傳，造成防疫困擾</t>
   </si>
   <si>
@@ -67,6 +109,9 @@
     <t>網現偽冒教育部網站  指揮中心：境外假網頁勿輕信</t>
   </si>
   <si>
+    <t>SARS-CoV-2感染臨床處置暫行指引新增口服抗病毒藥物使用建議(疾病管制署致醫界通函第471號)</t>
+  </si>
+  <si>
     <t>因應結核菌液態培養(MGIT)檢驗試劑暫時性缺貨，為利早期診斷結核病，針對疑似結核病送驗初查痰3套，請務必再進行結核分枝桿菌核酸增幅(NAA)檢驗(疾病管制署致醫界通函第470號)</t>
   </si>
   <si>
@@ -82,9 +127,6 @@
     <t xml:space="preserve">近期登革熱隱藏期平均超過3日，籲請醫師對具登革熱流行地區旅遊史之疑似病例提高警覺，加強診斷及通報(疾病管制署致醫界通函第466號) </t>
   </si>
   <si>
-    <t>10月1日起擴大2歲以上兒童使用丙型干擾素釋放試驗(IGRA)，以提升潛伏結核感染(LTBI)檢驗準確性及守護幼童健康(疾病管制署致醫界通函第465號)</t>
-  </si>
-  <si>
     <t>111-112年 COVID-19疫苗4,000萬劑倉儲物流與配送.pdf(另開新視窗)</t>
   </si>
   <si>
@@ -94,24 +136,24 @@
     <t>衛生福利部疾病管制署臺北區管制中心公告.zip(檔案下載)</t>
   </si>
   <si>
+    <t>約聘護理師</t>
+  </si>
+  <si>
+    <t>約用護理師(徵才案號：1527)</t>
+  </si>
+  <si>
+    <t>約用助理(徵才案號：1528)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">約聘護理師(英檢初級) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">約聘護理師(英檢中級) </t>
+  </si>
+  <si>
     <t>約聘技術員</t>
   </si>
   <si>
-    <t>約用助理(徵才案號：1059延長公告)(依身心障礙權益保障法任用身心障礙者)</t>
-  </si>
-  <si>
-    <t>技士</t>
-  </si>
-  <si>
-    <t>約用助理(徵才案號：1424)</t>
-  </si>
-  <si>
-    <t>約用護理師(徵才案號：1523)</t>
-  </si>
-  <si>
-    <t>約聘護理師</t>
-  </si>
-  <si>
     <t>公告本署急性傳染病組約用人員徵才案(徵才案號：1106，含延長公告)初審合格名單及甄試事宜。</t>
   </si>
   <si>
@@ -130,34 +172,13 @@
     <t>公告本署檢驗及疫苗研製中心約用人員徵才案(徵才案號：1057、1058)初審合格名單及甄試事宜。</t>
   </si>
   <si>
-    <t>1月25日至2月7日維持第二級疫情警戒標準，並調整相關規定，請民眾自主落實防疫措施，共同維護國內社區安全</t>
-  </si>
-  <si>
-    <t>新增89例COVID-19確定病例，分別為52例本土及37例境外移入</t>
-  </si>
-  <si>
-    <t>新增130例COVID-19確定病例，分別為82例本土及48例境外移入</t>
-  </si>
-  <si>
-    <t>新增68例COVID-19確定病例，分別為23例本土及45例境外移入</t>
-  </si>
-  <si>
-    <t>台積電、鴻海永齡、慈濟三間企業和民間團體捐贈之第十六批BNT疫苗99.45萬劑於今(21)日上午抵臺</t>
-  </si>
-  <si>
-    <t>因應帛琉近期疫情，指揮中心說明相關檢疫應變措施</t>
-  </si>
-  <si>
-    <t>1月21日上午8時「數位新冠病毒健康證明」開放國內使用</t>
-  </si>
-  <si>
-    <t>自1月21日起，前往部分休閒娛樂場所應配合出示完整接種COVID-19疫苗紀錄</t>
-  </si>
-  <si>
-    <t>新增37例COVID-19確定病例，分別為13例本土及24例境外移入</t>
-  </si>
-  <si>
-    <t>自1月20日零時起，增列印度及東南亞航線航班旅客於落地時採驗，檢驗結果陽性後送醫院或集中檢疫所/加強版防疫旅宿</t>
+    <t>/Bulletin/Detail/AaV2iREpabJ8syXu4450Rw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/2j_qY-s9J756z6DLeBTe0A?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/hngtwbSDMW8all0kUhN0sQ?typeid=9</t>
   </si>
   <si>
     <t>/Bulletin/Detail/J3ByKlpyULZLtHehAJUa_g?typeid=9</t>
@@ -178,6 +199,39 @@
     <t>/Bulletin/Detail/AFuil2ECiqiNku1SmowIGQ?typeid=9</t>
   </si>
   <si>
+    <t>/Bulletin/Detail/kVDslqExqB7BSiqJuFzXCg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/cU2pYInOEJ4NOhg-uOH5Zg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/yxiRZA3J-EAjVZ3CcK4n9Q?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Eg5gZrriSQBA--KxcspeTg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/y6MiRdu9X-y3kAs1UrXvng?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/RpwW0PpibHaRFJpatPM1HA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/5MtrgzOJApOSjivffWLWRw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/cdBM6ZsvZ-djQZ8je9OYkg?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/b9lBPQefAZUsMqqaIrGSDw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/lVU_tRUutNI667QAZYcj7g?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/mAWzcQcUVI2XPmIdtic3jg?typeid=9</t>
+  </si>
+  <si>
     <t>/Bulletin/Detail/ftv6FPFis84j5uHWTq4lNA?typeid=8772</t>
   </si>
   <si>
@@ -196,6 +250,9 @@
     <t>/Bulletin/Detail/IU5CMLLt8bQqXWHQhil0Aw?typeid=8772</t>
   </si>
   <si>
+    <t>/Bulletin/Detail/7LF3_zX-27ttBkfVRsjlqA?typeid=48</t>
+  </si>
+  <si>
     <t>/Bulletin/Detail/KaqzyT5RqFOuOQFGpEYLgA?typeid=48</t>
   </si>
   <si>
@@ -211,9 +268,6 @@
     <t>/Bulletin/Detail/HU4mCbrzZQlHC-VhwBiJOg?typeid=48</t>
   </si>
   <si>
-    <t>/Bulletin/Detail/DyZ6ZOuk-VLQSHiQ6xhqoQ?typeid=48</t>
-  </si>
-  <si>
     <t>/Uploads/files/a22b63a6-c6cb-463f-940d-26f4c11b17bc.pdf</t>
   </si>
   <si>
@@ -223,24 +277,24 @@
     <t>/Uploads/files/716583a9-c090-42d4-90dd-9afcbccbf4f4.zip</t>
   </si>
   <si>
+    <t>/HireList/Detail?hireId=0nPPV437nrsZtDlmACTqig</t>
+  </si>
+  <si>
+    <t>/HireList/Detail?hireId=qtKOuJxyY69hM91fhqIGwQ</t>
+  </si>
+  <si>
+    <t>/HireList/Detail?hireId=is3mwnpA6TueQWq1SHoKdQ</t>
+  </si>
+  <si>
+    <t>/HireList/Detail?hireId=vYAPhNrdpYAXFjtQ855W3w</t>
+  </si>
+  <si>
+    <t>/HireList/Detail?hireId=ZpDrALR1adV__qi1GWCyKg</t>
+  </si>
+  <si>
     <t>/HireList/Detail?hireId=dbhD6saaWV5URglIuc0HhA</t>
   </si>
   <si>
-    <t>/HireList/Detail?hireId=Zqa4DDs0UoZULIvGT10iAA</t>
-  </si>
-  <si>
-    <t>/HireList/Detail?hireId=_KGB6fXszZ2udoZvtWhyuw</t>
-  </si>
-  <si>
-    <t>/HireList/Detail?hireId=t6WVEcGVeOruE_eDkYXJxA</t>
-  </si>
-  <si>
-    <t>/HireList/Detail?hireId=4wyEVe65rp-Hr9DETX8n2g</t>
-  </si>
-  <si>
-    <t>/HireList/Detail?hireId=snieuoubdCfzpuQJABGcjA</t>
-  </si>
-  <si>
     <t>/Bulletin/Detail/yYmtcBLADf7DiN6l-Qsljw?typeid=11</t>
   </si>
   <si>
@@ -259,34 +313,13 @@
     <t>/Bulletin/Detail/u9ej71cxiu9bJqO0gMxdOQ?typeid=11</t>
   </si>
   <si>
-    <t>/Bulletin/Detail/y6MiRdu9X-y3kAs1UrXvng?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/RpwW0PpibHaRFJpatPM1HA?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/5MtrgzOJApOSjivffWLWRw?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/cdBM6ZsvZ-djQZ8je9OYkg?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/b9lBPQefAZUsMqqaIrGSDw?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/lVU_tRUutNI667QAZYcj7g?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/mAWzcQcUVI2XPmIdtic3jg?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/VSnz3gIu4mKSTrTFXHqIzQ?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/X5oSF1tnbyvV8_Nfrl31lg?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/Mhpv_WBf9Gw4pLB1hMe1hg?typeid=9</t>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/AaV2iREpabJ8syXu4450Rw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/2j_qY-s9J756z6DLeBTe0A?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/hngtwbSDMW8all0kUhN0sQ?typeid=9</t>
   </si>
   <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/J3ByKlpyULZLtHehAJUa_g?typeid=9</t>
@@ -307,6 +340,39 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/AFuil2ECiqiNku1SmowIGQ?typeid=9</t>
   </si>
   <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/kVDslqExqB7BSiqJuFzXCg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/cU2pYInOEJ4NOhg-uOH5Zg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/yxiRZA3J-EAjVZ3CcK4n9Q?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Eg5gZrriSQBA--KxcspeTg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/y6MiRdu9X-y3kAs1UrXvng?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/RpwW0PpibHaRFJpatPM1HA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/5MtrgzOJApOSjivffWLWRw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/cdBM6ZsvZ-djQZ8je9OYkg?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/b9lBPQefAZUsMqqaIrGSDw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/lVU_tRUutNI667QAZYcj7g?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/mAWzcQcUVI2XPmIdtic3jg?typeid=9</t>
+  </si>
+  <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/ftv6FPFis84j5uHWTq4lNA?typeid=8772</t>
   </si>
   <si>
@@ -325,6 +391,9 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/IU5CMLLt8bQqXWHQhil0Aw?typeid=8772</t>
   </si>
   <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/7LF3_zX-27ttBkfVRsjlqA?typeid=48</t>
+  </si>
+  <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/KaqzyT5RqFOuOQFGpEYLgA?typeid=48</t>
   </si>
   <si>
@@ -340,9 +409,6 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/HU4mCbrzZQlHC-VhwBiJOg?typeid=48</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/DyZ6ZOuk-VLQSHiQ6xhqoQ?typeid=48</t>
-  </si>
-  <si>
     <t>https://www.cdc.gov.tw/Uploads/files/a22b63a6-c6cb-463f-940d-26f4c11b17bc.pdf</t>
   </si>
   <si>
@@ -352,24 +418,24 @@
     <t>https://www.cdc.gov.tw/Uploads/files/716583a9-c090-42d4-90dd-9afcbccbf4f4.zip</t>
   </si>
   <si>
+    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=0nPPV437nrsZtDlmACTqig</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=qtKOuJxyY69hM91fhqIGwQ</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=is3mwnpA6TueQWq1SHoKdQ</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=vYAPhNrdpYAXFjtQ855W3w</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=ZpDrALR1adV__qi1GWCyKg</t>
+  </si>
+  <si>
     <t>https://www.cdc.gov.tw/HireList/Detail?hireId=dbhD6saaWV5URglIuc0HhA</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=Zqa4DDs0UoZULIvGT10iAA</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=_KGB6fXszZ2udoZvtWhyuw</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=t6WVEcGVeOruE_eDkYXJxA</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=4wyEVe65rp-Hr9DETX8n2g</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=snieuoubdCfzpuQJABGcjA</t>
-  </si>
-  <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/yYmtcBLADf7DiN6l-Qsljw?typeid=11</t>
   </si>
   <si>
@@ -388,52 +454,46 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/u9ej71cxiu9bJqO0gMxdOQ?typeid=11</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/y6MiRdu9X-y3kAs1UrXvng?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/RpwW0PpibHaRFJpatPM1HA?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/5MtrgzOJApOSjivffWLWRw?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/cdBM6ZsvZ-djQZ8je9OYkg?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/b9lBPQefAZUsMqqaIrGSDw?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/lVU_tRUutNI667QAZYcj7g?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/mAWzcQcUVI2XPmIdtic3jg?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/VSnz3gIu4mKSTrTFXHqIzQ?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/X5oSF1tnbyvV8_Nfrl31lg?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/Mhpv_WBf9Gw4pLB1hMe1hg?typeid=9</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-26\$\@\$中央流行疫情指揮中心今(26)日公布國內新增92例COVID-19確定病例，分別為46例本土個案及46例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為24例男性、22例女性，年齡介於未滿5歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為27例男性、19例女性，年齡介於未滿5歲至60多歲，分別自美國(9例)、英國、加拿大及荷蘭(各2例)、馬來西亞、阿拉伯聯合大公國、法國、中國、瑞典、柬埔寨、越南、新加坡(各1例)移入；另23例調查中。入境日介於今(2022)年1月9日至1月25日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,542,669例新型冠狀病毒肺炎相關通報(含5,523,800例排除)，其中18,503例確診，分別為3,475例境外移入，14,974例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計122例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月26日新增本土COVID-19確診個案表.pdf\$\@\$1月26日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-25\$\@\$中央流行疫情指揮中心今(25)日表示，帛琉近期疫情快速上升，近7日每日平均確診數72例，累計651例確診，另昨(24)日公布2例自帛琉境外移入個案。抵帛之美國CDC專家推測可能為感染Omicron株，評估未來一至兩週應為疫情高峰。\$\@\$指揮中心說明，基於國人至當地有感染風險，指揮中心於1月25日起將帛琉之國際旅遊疫情建議等級提升至第三級警告(Warning)，提醒國人應避免至帛琉進行所有非必要旅遊。除基於(醫療)人道或急迫理由必須緊急赴臺之外籍旅客可另行申請外，入境旅客應遵循相關檢疫規定：所有入境旅客，不論身分(本國籍與外國籍人士等)或來臺目的，原則均應檢附「表定航班時間前2日內COVID-19核酸檢驗報告」及預訂「檢疫居所證明」始得搭機來臺，並於抵臺前48小時內預先使用手機上網登入「入境檢疫系統」，填寫健康情形及旅遊史，完成線上健康申報。另自帛返臺旅客與其他國家入境旅客一致，適用春節檢疫專案。\$\@\$指揮中心強調，將嚴密監控疫情變化，隨時調整各項防檢疫措施，相關資訊可至衛生福利部疾病管制署全球資訊網首頁「COVID-19防疫專區-春節檢疫措施專案」(https://www.cdc.gov.tw/Category/MPage/y-WU-wWeGC8M5ihxysmbFw)查閱。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-25\$\@\$中央流行疫情指揮中心於今(25)日表示，為確保農曆春節連假期間COVID-19自費核酸檢驗指定機構檢驗量能，以應民眾出境或出入醫療/照護機構等其他因素檢附COVID-19陰性檢驗證明之需，指揮中心已將農曆春節連假期間提供服務資訊公布於衛生福利部全球資訊網／春節衛福、防疫措施(網址：https://www.mohw.gov.tw/cp-5380-65644-1.html )及衛生福利部疾病管制署全球資訊網／COVID-19防疫專區／醫療照護機構感染管制相關指引／開放民眾自費檢驗COVID-19申請規定項下(網址：https://www.cdc.gov.tw/Category/MPage/I92jtldmxZO_oolFPzP9HQ )，方便民眾上網查閱。另健保署LINE(點此加入：https://line.me/R/ti/p/%40dyk0948w )推出「春節期間自費COV19 PCR這裏找」專區，可以「定位查詢」或「院所名稱」搜尋附近篩檢的醫事服務機構，方便得知收費資訊、採檢模式及時間表、服務網址、電話等資訊。\$\@\$指揮中心說明，為使民眾便於掌握COVID-19自費核酸檢驗資訊，指揮中心公布各自費核酸檢驗指定機構於今(2022)年1月29日至2月6日農曆春節連假期間提供服務情形，包括每日提供常規檢驗及快速檢驗之採檢時間、收費情形、採檢模式（如：採網路預約、電話預約、現場報名、固定時間或隨到隨採等）、每日可採檢人數、指定機構服務網址及聯繫電話等。\$\@\$指揮中心進一步說明，目前全國自費核酸檢驗指定機構共216家，其中有187家自費檢驗指定機構於農曆春節期間持續提供自費核酸檢驗服務，開設率達87％。有自費核酸檢驗需求民眾於檢驗前，請務必先行至醫院官方網站或致電詢問及確認相關採檢事宜。\$\@\$指揮中心提醒民眾，因應近期COVID-19全球疫情升溫，Omicron等新興變異株於全球迅速擴散，適逢春節前返鄉人潮，請民眾於檢疫期間及自主健康管理期間應遵守防疫措施。有自費核酸檢驗需求民眾進入醫院請全程配戴口罩，並加強洗手、落實呼吸道衛生與咳嗽禮節，保持良好個人衛生習慣，以保護自身健康及維護國內社區安全。</t>
+    <t>發佈日期：2022-01-27\$\@\$中央流行疫情指揮中心今(27)日公布國內新增64例COVID-19確定病例，分別為21例本土個案及43例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為11例男性、10例女性，年齡介於未滿5歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為21例男性、22例女性，年齡介於未滿5歲至60多歲，分別自美國(14例)、印度(3例)、越南、印尼、英國及法國(各2例)、衣索比亞、坦尚尼亞、新加坡、土耳其、菲律賓、南非、芬蘭、日本(各1例)移入；另10例調查中。入境日介於去(2021)年5月2日至今(2022)年1月26日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,581,517例新型冠狀病毒肺炎相關通報(含5,562,679例排除)，其中18,566例確診，分別為3,518例境外移入，14,994例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案18418，再次採檢為陰性，改判排除)，累計123例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月27日新增本土COVID-19確診個案表.pdf\$\@\$1月27日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-27\$\@\$中央流行疫情指揮中心今(27)日表示，因應Omicron新型變異株威脅持續，且國內本土疫情尚未平息，考量春節連假期間團聚交流、遊憩活動頻繁，社區傳播的風險提高，指揮中心特別訂定「COVID-19疫情期間民眾假期生活防疫指引」，提醒民眾在享受春節連假時光時，主動落實防疫措施，平安過好年。\$\@\$指揮中心指出，春節連假期間落實勤洗手、呼吸道衛生與咳嗽禮節等良好個人衛生習慣尤為重要；若民眾本身或家人屬於慢性病患者、老年人、孕婦、體重過重、嬰幼兒等免疫力比較不好的族群，更易受感染及感染後病症較為嚴重，請符合接種條件者，儘速完整接種疫苗，獲得保護力，同時也應儘量避免參加可能密集接觸不特定人的聚會或活動，及前往人潮聚集、密閉空間或通風不良的公共場所。另民眾如果要探視上述免疫力較差的對象，建議雙方皆已完整接種疫苗，而探視者也要確認自身沒有身體不適症狀，且近期沒有參加密集接觸不特定人的聚會或活動，再行當面探視，探視時雙方都應佩戴口罩，以降低感染傳播的機會；否則建議使用電話或視訊方式取代。\$\@\$指揮中心呼籲，連假期間外出活動，儘量選擇前往開放且沒有人群擁擠的地方，並遵循疫情警戒期間外出全程佩戴口罩、與不特定人保持適當社交距離(室內1.5公尺、室外1公尺)、落實實聯制、體溫監測等防疫規範，親友聚餐也儘量控制人數，並遵守餐飲防疫措施。外出時可攜帶乾洗手用品隨時保持手部清潔，並準備備用口罩以便替換，返回住所時，要確實執行手部衛生。如果出現發燒、呼吸道症狀、腹瀉或嗅、味覺異常時，應佩戴口罩，儘速就醫，不要搭乘大眾運輸工具及前往其他公共場所。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-27\$\@\$中央流行疫情指揮中心今(27)日表示，台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的第十七批BNT疫苗91.84萬劑，已於今日上午順利運抵桃園國際機場，並在完成通關程序後，直接運送至指定冷儲物流中心進行後續檢驗封緘作業。\$\@\$指揮中心說明，由台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的1500萬劑BNT疫苗已全數到貨，總計1,524.91萬劑，多贈送24.91萬劑，分別為首批9月2日93萬劑、第二批9月9日91萬劑、第三批9月30日54萬劑、第四批10月1日67萬劑、第五批10月4日27萬劑、第六批10月7日88.92萬劑、第七批10月8日88.92萬劑、第八批10月14日82.7萬劑、第九批10月28日90.21萬劑、第十批10月29日91.03萬劑、第十一批11月5日87.17萬劑、第十二批11月12日92.66萬劑、第十三批11月25日93.83萬劑、第十四批12月9日192.35萬劑、第十五批12月30日93.83萬劑，第十六批1月21日99.45萬，以及本批91.84萬劑。本批疫苗效期至2022年5月25日，將由指揮中心統籌運用，儘速提供民眾接種。\$\@\$對於台積電、鴻海暨永齡基金會、慈濟基金會三間企業和民間團體積極協助，提供更多的疫苗讓民眾接種，加速提升臺灣疫苗覆蓋率，指揮中心再次表達由衷的謝意。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-25\$\@\$中央流行疫情指揮中心今(25)日公布國內新增38例COVID-19確定病例，分別為13例本土個案及25例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為4例男性、9例女性，年齡介於未滿5歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為8例男性、17例女性，年齡介於10多歲至70多歲，分別自加拿大(5例)、美國、泰國及印度(各3例)、日本(2例)、奈及利亞、瑞典及中國(各1例)移入；另6例調查中。入境日介於今(2022)年1月11日至1月24日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,501,288例新型冠狀病毒肺炎相關通報(含5,482,563例排除)，其中18,411例確診，分別為3,429例境外移入，14,928例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增3例空號病例(案18216-18218，再次採檢為陰性，改判排除)，累計122例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月25日新增本土COVID-19確診個案表.pdf\$\@\$1月25日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-25\$\@\$中央流行疫情指揮中心今(25)日表示，因應國內本土疫情升溫，目前已提供民眾於各地方政府衛生局安排/指定之合約醫療院所預約或至隨到隨打接種站方式接種COVID-19疫苗。為提供多元疫苗預約管道，加速提升民眾免疫保護力，COVID-19公費疫苗預約平臺（https://1922.gov.tw/ ，以下簡稱預約平臺）第21期將提供「已完整接種兩劑COVID-19疫苗滿12週且滿18歲以上」民眾，預約接種疫苗追加劑。另請已於各地方政府衛生局安排/指定之合約醫療院所完成預約之民眾，請依原已預約時段前往接種，無需再於預約平臺重複預約。\$\@\$預約平臺相關對象及期程說明如下：\$\@\$一、施打時程：2月7日至2月13日。\$\@\$二、符合資格對象：2021年11月21日前已完整接種兩劑疫苗且間隔滿12週之18歲以上民眾[即2004/2/13(含)前出生]預約接種疫苗追加劑。\$\@\$三、預約分流時程：\$\@\$(一)65歲以上：1月26日上午10時至1月27日下午4時。\$\@\$(二)50歲-64歲：1月26日中午12時至1月27日下午4時。\$\@\$(三)18歲-49歲：1月26日下午2時至1月27日下午4時。\$\@\$指揮中心說明，民眾可於1月25日下午2時起於預約平臺進行預約資格查詢，不再另發送預約提醒簡訊，符合資格民眾請記得於預約時間進行預約，預約當日如遇啟動流量管制亦請配合依序排隊耐心等候預約。\$\@\$指揮中心指出，預約平臺第21期僅提供民眾預約接種疫苗追加劑，民眾若有第一、二劑或基礎加強劑接種需求，請持接種紀錄(小黃卡)至各地方政府指定/安排合約醫療院所或衛生所預約接種，或所設置之隨到隨打接種站接種。前述醫療院所資訊，可至疾管署全球資訊網( https://www.cdc.gov.tw/ ) COVID-19疫苗接種院所項下，利用「COVID-19疫苗接種院所」或「COVID-19疫苗接種院所地圖」，依各地方政府衛生局提供資訊連結預約接種。\$\@\$指揮中心提醒，請民眾前往接種COVID-19疫苗前，應備妥「COVID-19疫苗接種紀錄卡」及健保卡，並經醫生評估過往疫苗接種史及檢核接種紀錄後，提供民眾疫苗接種。另18歲至未滿20歲民眾，如自行前往接種，請持家長簽具之意願同意書，若由家長陪同前往接種，請本人與家長於現場共同簽署意願同意書。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-24\$\@\$中央流行疫情指揮中心今(24)日公布國內新增51例COVID-19確定病例，分別為15例本土個案及36例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為10例男性、5例女性，年齡介於10多歲至50多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為21例男性、15例女性，年齡介於未滿5歲至70多歲，分別自美國(20例)、帛琉及印尼(各2例)、香港、越南、荷蘭、海地、菲律賓、多明尼加及比利時(各1例)移入；另5例調查中。入境日介於今(2022)年1月9日至1月23日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,463,663例新型冠狀病毒肺炎相關通報(含5,444,547例排除)，其中18,376例確診，分別為3,404例境外移入，14,918例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計119例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月24日新增本土COVID-19確診個案表.pdf\$\@\$1月24日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-24\$\@\$中央流行疫情指揮中心今(24)日表示，因應國際疫情嚴峻，且國內發生新變異株Omicron感染事件，經指揮中心與相關單位溝通及評估後於今日宣布，今(2022)年1月25日至2月7日維持疫情警戒標準為第二級，調整或維持相關措施及規定如下：\$\@\$一、維持加嚴之戴口罩規定，除少數例外情形，外出全程佩戴口罩：\$\@\$(一)運動、唱歌、拍照及直播、錄影、主持、報導、致詞、演講、講課等談話性質工作或活動之正式拍攝或進行時，恢復為須戴口罩。\$\@\$(二)下列場合得免戴口罩，但應隨身攜帶口罩，且如本身有相關症狀或與不特定對象無法保持社交距離時，仍應戴口罩：\$\@\$1. 農林漁牧工作者於空曠處(如：田間、魚塭、山林)工作。\$\@\$2. 於山林(含森林遊樂區)、海濱活動。\$\@\$3. 於溫/冷泉、烤箱、水療設施、三溫暖、蒸氣室、水域活動等易使口罩潮濕之場合。\$\@\$(三)外出時有飲食需求，得免戴口罩。\$\@\$(四)於指揮中心或主管機關指定之場所或活動(例如：藝文表演/劇組/電視主播等演出人員正式拍攝演出時、運動競賽之參賽選手及裁判於比賽期間等)，如符合指揮中心或主管機關之相關防疫措施，得暫時脫下口罩。\$\@\$二、營業場所及公共場域(含交通運輸)應嚴格遵守：實聯制、量體溫、加強環境淸消、員工健康管理、確診事件即時應變。\$\@\$三、高鐵、臺鐵、公路客運、船舶(固定餐飲區除外)、國內航班：於運具內（車廂、船舶、航空器）禁止飲食。\$\@\$四、賣場、超市、市場加強人流管制：室內空間至少1.5米/人(2.25平方米/人)，室外空間至少1米/人(1平方米/人)；不開放試吃。\$\@\$五、宗教場所、宗教集會活動：依內政部規定之防疫措施辦理。\$\@\$六、餐飮場所：嚴格落實實聯制、量體溫、提供洗手設備及消毒用品；宴席不得逐桌敬酒敬茶；違反者依法裁處並限期改善，未完成改善者，不得提供內用服務。\$\@\$指揮中心呼籲，防疫工作人人有責，請民眾自主落實防疫措施，維持個人衛生好習慣，戴口罩、勤洗手、保持社交距離；出入公共場域落實實聯制、體溫量測等，降低病毒傳播風險，保護自己也保護他人，共同維護國內社區安全。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-23\$\@\$中央流行疫情指揮中心今(23)日公布國內新增89例COVID-19確定病例，分別為52例本土個案及37例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為32例男性、20例女性，年齡介於未滿5歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為17例男性、20例女性，年齡介於未滿10歲至60多歲，分別自美國(12例)、法國(3例)、英國(2例)、丹麥、印度、烏克蘭、菲律賓、土耳其、澳大利亞(各1例)移入；另14例調查中。入境日介於今(2022)年1月8日至1月22日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,441,110例新型冠狀病毒肺炎相關通報(含5,422,031例排除)，其中18,325例確診，分別為3,368例境外移入，14,903例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增2例空號病例(案17934、案17970，再次採檢為陰性改判排除)，累計119例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月23日新增境外移入COVID-19確診個案表.pdf\$\@\$1月23日新增本土COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-22\$\@\$中央流行疫情指揮中心今(22)日公布國內新增130例COVID-19確定病例，分別為82例本土個案及48例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為12例男性、70例女性，年齡介於未滿10歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為29例男性、19例女性，年齡介於未滿5歲至70多歲，分別自美國(13例)、加拿大及新加坡(各4例)、菲律賓(3例)、印度、土耳其及香港(各2例)、奧地利、奈及利亞、義大利、柬埔寨、德國、越南及巴西(各1例)移入；另11例調查中。入境日介於去(2021)年12月31日至今(2022)年1月21日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,418,957例新型冠狀病毒肺炎相關通報(含5,400,086例排除)，其中18,238例確診，分別為3,331例境外移入，14,853例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案18182，再次採檢為陰性，改判排除)，累計117例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月22日新增本土COVID-19確診個案表.pdf\$\@\$1月22日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-21\$\@\$中央流行疫情指揮中心今(21)日公布國內新增68例COVID-19確定病例，分別為23例本土個案及45例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為10例男性、13例女性，年齡介於未滿10歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為20例男性、24例女性及1例調查中，年齡介於未滿5歲至70多歲，分別自美國(17例)、菲律賓(4例)、越南及以色列(各3例)、加拿大(2例)、波蘭、澳大利亞、韓國、新加坡、瑞典、俄羅斯、英國及愛爾蘭(各1例)移入；另8例調查中。入境日介於今(2022)年1月5日至1月20日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,394,042例新型冠狀病毒肺炎相關通報(含5,375,246例排除)，其中18,109例確診，分別為3,283例境外移入，14,772例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計116例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月21日新增本土COVID-19確診個案表.pdf\$\@\$1月21日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-20\$\@\$中央流行疫情指揮中心今(20)日表示，我國「數位新冠病毒健康證明」自去(110)年12月28日上線後已核發超過26萬份。考量國內外疫情升溫，各界建議及需求，指揮中心將於今(111)年1月21日上午8時開放「數位新冠病毒健康證明」供國內使用，共計三大功能：所有在國內接種者皆可下載、符合歐盟規範的查驗程式，可驗證60國的證明、提供具實名制的APP作為證明載具。\$\@\$指揮中心指出，原本下載限持有效護照者，現以戶口名簿的戶號取代，民眾可以電腦或手機上網申辦「數位新冠病毒健康證明」（ https://dvc.mohw.gov.tw ），注意事項說明如下：\$\@\$一、確認身分：\$\@\$(一)國人：(1)身分證號+健保卡號+戶口名簿戶號；(2) FIDO；(3)自然人憑證。三種方式擇一。\$\@\$(二)外來人口：(1)統一證號+健保卡號；(2) 統一證號+入出境證號；(3) 統一證號+護照號碼。三種方式擇一。\$\@\$二、選擇項目：選擇「疫苗接種數位證明」或「檢驗結果數位證明」。\$\@\$三、取得證明：於申請成功畫面點選「下載/列印 數位證明」，檔案格式為PDF，提醒要先保存於行動裝置或電腦硬碟中，再視個人需要列印紙本。無列印設備但又有列印需求者，可於申請成功畫面選擇超商並點選「取得超商列印碼」，系統將產製超商取件條碼或取件編號，請自行攜碼至超商付費列印。\$\@\$此次僅變更確認身分方式，方便未持有護照者下載。具有效護照民眾申辦數位證明時仍會產出護照號碼，未來不必為出國另行下載；不具有效護照民眾者護照號碼欄位顯示為「Not Issued」。\$\@\$「數位新冠病毒健康證明」查驗程式係網頁形式（ https://dvc.mohw.gov.tw/verifier-web ），不需下載安裝，民眾也可在衛福部官網取得連結，該網頁不會保留受查驗者的個資，符合歐盟GDPR，使用步驟如下：\$\@\$一、前往網站：使用具備相機及網頁瀏覽器的手機、電腦等，開啟瀏覽器前往上述網址。\$\@\$二、同意隱私權聲明、允許取用相機權限。\$\@\$三、不退出查驗網頁且不中斷網路者，可續使用並維持最新功能，退出或中斷者可重新上網更新。\$\@\$查驗程式以顏色、圖示及文字顯示查驗結果，綠色、打勾為通過，紅色、打叉為不通過，黃色、三角驚嘆號為待確認狀態（包括：接種不完整、效期不符、非我國同意的疫苗或檢驗等），不合規格的QR code則會出現解析錯誤的訊息。驗證程式個人基本資料僅會顯示姓名及出生年月日，如需嚴格確認是否為本人持有，建議仍需搭配其它身分證件。由於我國已是歐盟數位新冠證明(EU-DCC)的成員，故本查驗程式也可查證持同樣規格由其它國家發行的疫苗、核酸檢驗數位證明，及部分有發行康復證明的國家。\$\@\$指揮中心提醒，依據世界衛生組織(WHO)規範，疫苗證明可採紙本或數位方式，檢驗陰性或康復證明亦可做為健康證明，數位證明僅是方式之一，民眾有多元方式可提供各場所查驗。\$\@\$另外，指揮中心亦已備有標準的應用軟體介接程式(API)供國內具實名制功能的APP介接取得民眾自己的數位證明，並以APP為載具。發行或管理APP者，確認符合個資法及GDPR、身分驗證強度不低於本數位證明平臺，且APP後臺不得留存數位證明，請向指揮中心正式申請。\$\@\$為更新原有版本的功能，申辦平台預計今年1月20日下午5時至次(21)日上午8時停止服務進行更版，有急需出國使用者，請先提前下載。詳細下戴及驗證系統操作方式可以參考衛生福利部官網數位證明專區( https://covid19.mohw.gov.tw/ch/np-5345-205.html )。</t>
   </si>
   <si>
     <t>發佈日期：2021-07-10\$\@\$中央流行疫情指揮中心今（10）日表示，近日有網友散布「三級警戒微解封的不可思議之處，新冠肺炎病毒只會攻擊家人」等訊息，相關內容多有誤導，且在錯誤基礎上進行不當類比，指揮中心再次強調，相關防疫指引已清楚說明，原本同住家人可以繼續維持生活，相關指引都是針對日常非同住者間的行為互動加以規範，呼籲民眾勿輕信或隨意散播、轉傳錯誤訊息，造成防疫困擾。\$\@\$指揮中心指出，有關7月13號以後針對部分場所將適度鬆綁，但仍須遵守防疫相關指引及規範，而此波疫情中，不少個案均為家戶群聚感染，由於室內密切接觸風險較高，因此對於室內社交人數須有較嚴格規範，但不包含原本同住的家人，也無需限制同住家人不能在家打麻將、看電影、吃飯等。 圖片 附件\$\@\$0710指揮中心：勿輕信「三級警戒微解封的不可思議之處」之網傳.jpg</t>
   </si>
   <si>
-    <t>發佈日期：2021-06-13\$\@\$近日有網友在臉書FB以自製圖文方式散布「政府讓人民施打未受認證且保護力低之國產疫苗」、「國產疫苗的中和抗體效價比國外疫苗差」、「國產疫苗為什麼不向國際提出緊急授權」，中央流行疫情指揮中心(下稱指揮中心)今（13）日嚴正澄清表示，目前國產疫苗臨床試驗尚在進行中，最終結果須等廠商提出EUA 申請，經專家會議審查疫苗的製程管控、藥毒理試驗及臨床試驗結果，在緊急公衛的需求下，確認疫苗使用效益大於風險，才會核准緊急授權使用。\$\@\$指揮中心指出，目前國產疫苗廠商皆已積極規劃，以取得國際認證為目標。國產疫苗需經食藥署和專家會議嚴謹審查，在緊急公衛需求，並確認效益大於風險，才會核准緊急授權使用。此外，各家廠牌的疫苗所使用的檢驗實驗室及檢驗方式不同且無協和，無法直接由各實驗室產生數值進行比較。國產疫苗仍需等廠商提出申請，經過中央主管機關嚴格把關及審查通過後，確認品質、安全、療效後，品質沒有問題，疫苗方可供民眾施打。\$\@\$指揮中心再次提醒，民眾接獲來源不明的訊息時，應先進行查證，切勿隨意散播、轉傳，以免觸法。 圖片 附件\$\@\$0613網傳「政府讓人民施打未受認證且保護力低之國產疫苗」-1.jpg\$\@\$0613網傳「政府讓人民施打未受認證且保護力低之國產疫苗」-2.jpg</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-06-01\$\@\$中央流行疫情指揮中心今(1)日指出，近日有網友在通訊軟體LINE散布「臺中市太原路復健醫院被徵收為方艙醫院」，臺中市政府衛生局已澄清為不實訊息，請民眾勿再轉傳與散布，以免觸法遭罰。\$\@\$指揮中心表示，臺中市政府已對外澄清，此復健醫院近期進行搬遷作業，是為了提升醫療品質，正以BOT方式規劃市立綜合醫院，並非徵用作為方艙醫院。\$\@\$指揮中心副指揮官陳宗彥指出，因應疫情變化，各地方政府規劃應變醫院及專責醫院收治患者，民眾接獲來源不明的訊息時，應先進行查證，切勿隨意散播、轉傳，以免觸法。\$\@\$指揮中心重申，防疫相關資訊應以中央流行疫情指揮中心公布內容為主，散播假訊息構成犯罪，會被判處最高三年有期徒刑或併科三百萬元罰金。提醒民眾，收到來路不明訊息多加留意、查證，切勿轉傳散播，以免觸法。詳情請上官網查詢(http://at.cdc.tw/Q7S2Vt)。 圖片 附件\$\@\$網傳「臺中市太原路復健醫院被徵收為方艙醫院」為不實訊息勿轉傳.jpg\$\@\$勿散播不實訊息，以免觸法受罰.jpg</t>
+    <t>發佈日期：2021-05-25\$\@\$中央流行疫情指揮中心今(25)日表示，近日網路出現偽冒教育部網站，杜撰「全國各級學校因應疫情停課時程資訊」等訊息，意圖造成民眾困惑，此為境外假網頁不實訊息，請民眾勿輕信。\$\@\$指揮中心副指揮官陳宗彥表示，該網站假冒教育部傳達不實防疫訊息，刑事警察局已成立專案小組偵辦，經調查其為境外IP。\$\@\$指揮中心指出，教育部全球資訊網正確的網址是https://www.edu.tw/ ，民眾收到任何連結時，可以先觀察連結網址，是否跟官方網址一樣。例如，教育部官方網址的網域，就會是「edu.tw」結尾。\$\@\$指揮中心強調，散播假訊息構成犯罪，會被判處最高三年有期徒刑或併科三百萬元罰金。提醒民眾，收到來路不明訊息多加留意、查證，切勿轉傳散播，以免觸法。 圖片 附件\$\@\$0525指揮中心指出，網路出現偽冒教育部網站並杜撰假訊息，請民眾勿輕信.jpg\$\@\$勿散播不實訊息，以免觸法受罰.jpg</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-06\$\@\$為提供結核病患即時診斷，疾病管制署結核病診治指引自104年已加重結核分枝桿菌核酸增幅(nucleic acid amplification, NAA)檢驗於診斷結核病之角色。NAA檢驗具快速、高敏感度及高特異性，可大幅縮短傳統培養檢驗方法所需等待結果時間，有利及早診斷及治療結核病。\$\@\$因應近期結核菌液態培養(MGIT)檢驗發生添加劑(營養劑併抑制細菌生長的抗生素成分)供貨短缺情形，為避免延遲發現疑似結核病個案，依本署110年12月24日「衛生福利部傳染病防治諮詢會(結核病防治組)」會議決議，於供貨短缺期間，對於社區型肺炎尚未通報結核病者，於診斷送驗3套初查痰執行塗片耐酸性染色鏡檢(Acid fast stain)及分枝桿菌培養時，其中1套請務必同時開立NAA檢驗。另考量實驗室短期內MGIT痰培養試劑有限，對於管理中的結核病患追蹤複查痰，請採1套進行培養檢驗，暫時避免重複送驗檢體，此因應作為停止施行時間將於缺貨狀況緩解後再函週知。\$\@\$有關「結核病診治指引」可至疾病管制署全球資訊網(https://www.cdc.gov.tw)&gt;傳染病與防疫專題&gt;傳染病介紹&gt;第三類定傳染病&gt;結核病&gt;重要指引及教材項下查閱。\$\@\$感謝您與我們共同維護全民的健康安全。</t>
   </si>
   <si>
     <t>發佈日期：2021-12-30\$\@\$各位醫界朋友，您好：\$\@\$鑑於國際COVID-19疫情嚴峻及Omicron新型變異株威脅增加，嚴重特殊傳染性肺炎中央流行疫情指揮中心(下稱指揮中心)邀請各縣市兒科、內科、家醫科、耳鼻喉科及婦產科等有提供診治呼吸道症狀服務之診所/衛生所，自明(2022)年1月1日起加入公費COVID-19家用快篩試劑發放行列，指揮中心感謝基層診所積極守護社區健康的熱誠，並籲請各定點診所醫師針對具呼吸道症狀就醫民眾，加強發放公費COVID-19家用快篩試劑。\$\@\$指揮中心於今(2021)年8月30日起啟動前揭計畫，全國共計18個縣市86家診所/衛生所參加，迄今已發放1萬餘劑公費COVID-19家用快篩試劑，於有效監測下均無發現陽性個案。為提升民眾取用COVID-19家用快篩試劑可近性及擴大監測，自明年1月1日起增加至21個縣市272家診所/衛生所參與。\$\@\$由於國內現處於流感季節且COVID-19症狀與上呼吸道感染症狀相似，指揮中心籲請定點診所針對出現呼吸道症狀就醫民眾，加強發放公費COVID-19家用快篩試劑，尤可對於幼兒及其陪病家屬加強評估發放；另請診所衛教民眾試劑使用流程及注意事項、提醒民眾匿名填寫線上問卷以回報快篩結果等資料，並將發放民眾資料登錄於疾病管制署系統中。\$\@\$該計畫相關內容公布於疾病管制署全球資訊網 (http://www.cdc.gov.tw) COVID-19防疫專區&gt;臺灣社交距離APP及採檢地圖&gt;COVID-19社區加強監測方案，歡迎查閱。\$\@\$感謝您與我們共同維護全民的健康安全。</t>
@@ -442,40 +502,16 @@
     <t>發佈日期：2021-10-22\$\@\$各位醫界朋友，您好：\$\@\$我國新型冠狀病毒(SARS-CoV-2)感染臨床處置暫行指引建議可依照病患病程與嚴重度，對不需用氧且有重症風險因子之病患給予單株抗體，需用氧病患則除dexamethasone外可併用免疫調節劑tocilizumab或baricitinib。鑒於近期國際間藥物使用建議與國內適應症均有更新，經COVID-19專家諮詢會議更新建議如下：\$\@\$1.複合單株抗體Casirivimab + imdevimab或Bamlanivimab + etesevimab。適用對象為\$\@\$― 具以下任一風險因子，未使用氧氣且於發病十天內之≧12歲且體重≧40公斤病患；\$\@\$― 風險因子包括：年齡 ≧ 65歲、糖尿病、慢性腎病、心血管疾病（含高血壓）、慢性肺疾、BMI ≧25（或12-17歲兒童BMI超過同齡第85百分位）、懷孕、其他影響免疫功能之疾病或已知重症風險因子等。\$\@\$目前實證顯示上述兩種複合單株抗體對國內現今主要檢出之Delta與Alpha變異株均有效，但由於體外試驗顯示Bamlanivimab + etesevimab可能無法有效中和包括Beta、Gamma、Delta plus與Mu變異株，建議臨床醫師使用時需考量流行狀況與參閱最新版「SARS-CoV-2之藥物使用實證摘要」附表。\$\@\$另參考WHO最新公布治療建議，於診治指引註解中新增「隨機對照研究顯示對血清抗體陰性之嚴重肺炎以上程度病患，除標準治療外，給予casirivimab 4000mg + imdevimab 4000mg 可降低死亡率」。\$\@\$2.Remdesivir適用對象為嚴重肺炎以上（未使用吸氧治療下的SpO2 ≦ 94%、需使用吸氧治療、需使用高流量氧氣或非侵襲性呼吸器但未插管）病患。另於診治指引註解中新增「若住院病患胸部X光片顯示肺炎，雖未達重症標準且不符合單株抗體適用條件，仍可申請使用remdesivir」。但由於目前尚無併用單株抗體之效益與安全性資料，目前仍暫不建議remdesivir與單株抗體同時併用。\$\@\$由於近日媒體報導ivermectin用於治療COVID-19一事，經專家委員審視國際文獻，發現ivermectin相關臨床試驗研究證據力等級低，且部分研究涉及科學誠信，其中亦有發表論文被撤回之情形，統合分析結果顯示目前證據不支持ivermectin可用於治療或預防COVID-19，WHO及歐美等具公信力之治療指引均不建議使用於COVID-19之治療。為確保國人健康，我國診治指引治療藥物建議係根據最高等級實證基礎制訂，參考目前各方面之資料，仍不建議ivermectin納入我國診治指引之治療建議藥物。\$\@\$「嚴重特殊傳染性肺炎」之診療相關資訊將隨時依防疫需求與最新文獻證據更新並公布於疾病管制署全球資訊網(http://www.cdc.gov.tw)。\$\@\$感謝您與我們共同維護全民的健康安全。</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-13\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$急性傳染病組\$\@\$約用助理\$\@\$(徵才案號：1106，含延長公告)\$\@\$(計1名)\$\@\$張○純(A22889****)\$\@\$二、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一) 口試：\$\@\$1、報到時間：111年01月17日星期一15:20~15:30，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署7樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：16:40~17:10。\$\@\$(二)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(三)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於111年01月17日上午10點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3823)，俾利安排應試座位。\$\@\$(四)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(五)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
+    <t>發佈日期：2021-09-30\$\@\$全國醫界朋友，您好：\$\@\$目前正值登革熱流行期，雖然今（110）年截至目前尚無本土病例，但仍有少數境外移入個案，主要來自越南、菲律賓、印尼及柬埔寨。因登革熱部分症狀與COVID-19相似，籲請各位醫師對於出現疑似症狀之就診民眾，如具登革熱流行地區旅遊史，除考量可能為COVID-19外，亦請適時使用登革熱NS1快速診斷試劑，以及時發現疑似病例。目前國內氣候持續高溫且常有午後雷陣雨，易使病媒蚊密度快速上升，流行風險增加，而近期登革熱通報本土病例數上升且隱藏期平均值超過3日，請各位醫師留意出現登革熱疑似症狀病例，提高通報警覺。\$\@\$由於登革熱個案在發病前1天至發病後5天為具傳染性之病毒血症期，因此及早發現病例並採取相關防疫措施，是有效控制登革熱疫情之關鍵。疾病管制署籲請各位醫師提高警覺，如遇有發燒、頭痛、後眼窩痛、肌肉痛、關節痛、骨頭痛、出疹等（部分個案有腹瀉症狀）疑似登革熱症狀之個案，請務必詢問TOCC，且視需要使用登革熱NS1快速診斷試劑，供作臨床診斷參考，有效減少疑似病例就醫次數及縮短隱藏期，以利採取相關防治措施，防範疫情擴散。\$\@\$感謝您與我們共同維護全民的健康安全。</t>
   </si>
   <si>
     <t>發佈日期：2022-01-12\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$檢疫組\$\@\$約用助理\$\@\$(徵才案號：0507)\$\@\$(計4名)\$\@\$陳○涵(A22534****)\$\@\$張○純(A22889****)\$\@\$林○翔(S12427****)\$\@\$謝○樺(K12260****)\$\@\$二、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一) 口試：\$\@\$1、報到時間：111年01月17日星期一15:20~15:30，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署7樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：15:30~16:40。\$\@\$(二)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(三)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於111年01月17日上午10點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3864)，俾利安排應試座位。\$\@\$(四)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(五)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-24\$\@\$中央流行疫情指揮中心今(24)日表示，因應國際疫情嚴峻，且國內發生新變異株Omicron感染事件，經指揮中心與相關單位溝通及評估後於今日宣布，今(2022)年1月25日至2月7日維持疫情警戒標準為第二級，調整或維持相關措施及規定如下：\$\@\$一、維持加嚴之戴口罩規定，除少數例外情形，外出全程佩戴口罩：\$\@\$(一)運動、唱歌、拍照及直播、錄影、主持、報導、致詞、演講、講課等談話性質工作或活動之正式拍攝或進行時，恢復為須戴口罩。\$\@\$(二)下列場合得免戴口罩，但應隨身攜帶口罩，且如本身有相關症狀或與不特定對象無法保持社交距離時，仍應戴口罩：\$\@\$1. 農林漁牧工作者於空曠處(如：田間、魚塭、山林)工作。\$\@\$2. 於山林(含森林遊樂區)、海濱活動。\$\@\$3. 於溫/冷泉、烤箱、水療設施、三溫暖、蒸氣室、水域活動等易使口罩潮濕之場合。\$\@\$(三)外出時有飲食需求，得免戴口罩。\$\@\$(四)於指揮中心或主管機關指定之場所或活動(例如：藝文表演/劇組/電視主播等演出人員正式拍攝演出時、運動競賽之參賽選手及裁判於比賽期間等)，如符合指揮中心或主管機關之相關防疫措施，得暫時脫下口罩。\$\@\$二、營業場所及公共場域(含交通運輸)應嚴格遵守：實聯制、量體溫、加強環境淸消、員工健康管理、確診事件即時應變。\$\@\$三、高鐵、臺鐵、公路客運、船舶(固定餐飲區除外)、國內航班：於運具內（車廂、船舶、航空器）禁止飲食。\$\@\$四、賣場、超市、市場加強人流管制：室內空間至少1.5米/人(2.25平方米/人)，室外空間至少1米/人(1平方米/人)；不開放試吃。\$\@\$五、宗教場所、宗教集會活動：依內政部規定之防疫措施辦理。\$\@\$六、餐飮場所：嚴格落實實聯制、量體溫、提供洗手設備及消毒用品；宴席不得逐桌敬酒敬茶；違反者依法裁處並限期改善，未完成改善者，不得提供內用服務。\$\@\$指揮中心呼籲，防疫工作人人有責，請民眾自主落實防疫措施，維持個人衛生好習慣，戴口罩、勤洗手、保持社交距離；出入公共場域落實實聯制、體溫量測等，降低病毒傳播風險，保護自己也保護他人，共同維護國內社區安全。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-23\$\@\$中央流行疫情指揮中心今(23)日公布國內新增89例COVID-19確定病例，分別為52例本土個案及37例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為32例男性、20例女性，年齡介於未滿5歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為17例男性、20例女性，年齡介於未滿10歲至60多歲，分別自美國(12例)、法國(3例)、英國(2例)、丹麥、印度、烏克蘭、菲律賓、土耳其、澳大利亞(各1例)移入；另14例調查中。入境日介於今(2022)年1月8日至1月22日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,441,110例新型冠狀病毒肺炎相關通報(含5,422,031例排除)，其中18,325例確診，分別為3,368例境外移入，14,903例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增2例空號病例(案17934、案17970，再次採檢為陰性改判排除)，累計119例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月23日新增境外移入COVID-19確診個案表.pdf\$\@\$1月23日新增本土COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-22\$\@\$中央流行疫情指揮中心今(22)日公布國內新增130例COVID-19確定病例，分別為82例本土個案及48例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為12例男性、70例女性，年齡介於未滿10歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為29例男性、19例女性，年齡介於未滿5歲至70多歲，分別自美國(13例)、加拿大及新加坡(各4例)、菲律賓(3例)、印度、土耳其及香港(各2例)、奧地利、奈及利亞、義大利、柬埔寨、德國、越南及巴西(各1例)移入；另11例調查中。入境日介於去(2021)年12月31日至今(2022)年1月21日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,418,957例新型冠狀病毒肺炎相關通報(含5,400,086例排除)，其中18,238例確診，分別為3,331例境外移入，14,853例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案18182，再次採檢為陰性，改判排除)，累計117例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月22日新增本土COVID-19確診個案表.pdf\$\@\$1月22日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-21\$\@\$中央流行疫情指揮中心今(21)日公布國內新增68例COVID-19確定病例，分別為23例本土個案及45例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為10例男性、13例女性，年齡介於未滿10歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為20例男性、24例女性及1例調查中，年齡介於未滿5歲至70多歲，分別自美國(17例)、菲律賓(4例)、越南及以色列(各3例)、加拿大(2例)、波蘭、澳大利亞、韓國、新加坡、瑞典、俄羅斯、英國及愛爾蘭(各1例)移入；另8例調查中。入境日介於今(2022)年1月5日至1月20日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,394,042例新型冠狀病毒肺炎相關通報(含5,375,246例排除)，其中18,109例確診，分別為3,283例境外移入，14,772例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計116例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月21日新增本土COVID-19確診個案表.pdf\$\@\$1月21日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-21\$\@\$中央流行疫情指揮中心今(21)日表示，台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的第十六批BNT疫苗99.45萬劑，已於今日上午順利運抵桃園國際機場，並在完成通關程序後，直接運送至指定冷儲物流中心進行後續檢驗封緘作業。\$\@\$指揮中心說明，由台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的BNT疫苗1,500萬劑，目前共計到貨1433.07萬劑，分別為首批9月2日93萬劑、第二批9月9日91萬劑、第三批9月30日54萬劑、第四批10月1日67萬劑、第五批10月4日27萬劑、第六批10月7日88.92萬劑、第七批10月8日88.92萬劑、第八批10月14日82.7萬劑、第九批10月28日90.21萬劑、第十批10月29日91.03萬劑、第十一批11月5日87.17萬劑、第十二批11月12日92.66萬劑、第十三批11月25日93.83萬劑、第十四批12月9日192.35萬劑、第十五批12月30日93.83萬劑，以及本批99.45萬劑。本批疫苗效期至2022年5月25日，將由指揮中心統籌運用，儘速提供民眾接種。\$\@\$對於台積電、鴻海暨永齡基金會、慈濟基金會三間企業和民間團體積極協助，提供更多的疫苗讓民眾接種，加速提升臺灣疫苗覆蓋率，指揮中心再次表達由衷的謝意。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-20\$\@\$中央流行疫情指揮中心今(20)日表示，鑒於帛琉疫情升溫，為確保社區防疫安全，自帛琉來臺旅客，除搭機前須持二日內核酸檢測報告外，入境仍依現行作法，採綠色專屬通道，並強化相關入境採檢及檢疫措施，請赴帛琉或自帛琉抵臺旅客，務必配合當地及回臺相關防疫及檢疫措施，以保障國內社區安全。\$\@\$指揮中心指出，強化入境採檢及檢疫措施將自今(2022)年1月22日(含)起實施，入境旅客公費入住集中檢疫所實施5天檢疫，接續加強自主健康管理9天，再進行一般自主健康管理7天，並配合入境時(集中檢疫所採檢)、第5天及第13至14天進行PCR檢測，第8天、第11天及一般自主健康管理期滿(第20至21天)以家用快篩試劑各檢測1次。另提醒旅客於到訪帛琉期間，請務必落實自我健康監測，並確實遵守指揮中心及帛國的防疫措施，如佩戴口罩、勤洗手及保持社交距離等規範，以維護自身的健康安全。\$\@\$指揮中心說明，針對1月22日分別有旅遊團啟程至帛琉，以及自帛琉入境旅客，請儘速辦理下列事項：\$\@\$(一) 駐帛琉共和國大使館將持續提供當地疫情風險資訊予交通部觀光局，以利旅行社向旅客宣達該國疫情風險，以及須配合的防疫措施（包括從事醫療照護工作人員，於加強自主健康管理期間不得上班）。\$\@\$(二) 為確保赴帛琉旅客瞭解當地疫情風險，駐帛琉共和國大使館亦將於機場加強宣導。\$\@\$(三) 有關自帛琉入境之14名旅客(含後送轉診病人)，將請駐帛琉共和國大使館轉達調整後的防疫措施，並請醫療應變組瞭解後送轉診病人的就醫需求，以利預先調度。\$\@\$此外，外交部已調整帛琉旅遊警示為「提醒注意」，並將召集交通部與駐帛琉共和國大使館共同研商合理的退費機制。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-20\$\@\$中央流行疫情指揮中心今(20)日表示，我國「數位新冠病毒健康證明」自去(110)年12月28日上線後已核發超過26萬份。考量國內外疫情升溫，各界建議及需求，指揮中心將於今(111)年1月21日上午8時開放「數位新冠病毒健康證明」供國內使用，共計三大功能：所有在國內接種者皆可下載、符合歐盟規範的查驗程式，可驗證60國的證明、提供具實名制的APP作為證明載具。\$\@\$指揮中心指出，原本下載限持有效護照者，現以戶口名簿的戶號取代，民眾可以電腦或手機上網申辦「數位新冠病毒健康證明」（ https://dvc.mohw.gov.tw ），注意事項說明如下：\$\@\$一、確認身分：\$\@\$(一)國人：(1)身分證號+健保卡號+戶口名簿戶號；(2) FIDO；(3)自然人憑證。三種方式擇一。\$\@\$(二)外來人口：(1)統一證號+健保卡號；(2) 統一證號+入出境證號；(3) 統一證號+護照號碼。三種方式擇一。\$\@\$二、選擇項目：選擇「疫苗接種數位證明」或「檢驗結果數位證明」。\$\@\$三、取得證明：於申請成功畫面點選「下載/列印 數位證明」，檔案格式為PDF，提醒要先保存於行動裝置或電腦硬碟中，再視個人需要列印紙本。無列印設備但又有列印需求者，可於申請成功畫面選擇超商並點選「取得超商列印碼」，系統將產製超商取件條碼或取件編號，請自行攜碼至超商付費列印。\$\@\$此次僅變更確認身分方式，方便未持有護照者下載。具有效護照民眾申辦數位證明時仍會產出護照號碼，未來不必為出國另行下載；不具有效護照民眾者護照號碼欄位顯示為「Not Issued」。\$\@\$「數位新冠病毒健康證明」查驗程式係網頁形式（ https://dvc.mohw.gov.tw/verifier-web ），不需下載安裝，民眾也可在衛福部官網取得連結，該網頁不會保留受查驗者的個資，符合歐盟GDPR，使用步驟如下：\$\@\$一、前往網站：使用具備相機及網頁瀏覽器的手機、電腦等，開啟瀏覽器前往上述網址。\$\@\$二、同意隱私權聲明、允許取用相機權限。\$\@\$三、不退出查驗網頁且不中斷網路者，可續使用並維持最新功能，退出或中斷者可重新上網更新。\$\@\$查驗程式以顏色、圖示及文字顯示查驗結果，綠色、打勾為通過，紅色、打叉為不通過，黃色、三角驚嘆號為待確認狀態（包括：接種不完整、效期不符、非我國同意的疫苗或檢驗等），不合規格的QR code則會出現解析錯誤的訊息。驗證程式個人基本資料僅會顯示姓名及出生年月日，如需嚴格確認是否為本人持有，建議仍需搭配其它身分證件。由於我國已是歐盟數位新冠證明(EU-DCC)的成員，故本查驗程式也可查證持同樣規格由其它國家發行的疫苗、核酸檢驗數位證明，及部分有發行康復證明的國家。\$\@\$指揮中心提醒，依據世界衛生組織(WHO)規範，疫苗證明可採紙本或數位方式，檢驗陰性或康復證明亦可做為健康證明，數位證明僅是方式之一，民眾有多元方式可提供各場所查驗。\$\@\$另外，指揮中心亦已備有標準的應用軟體介接程式(API)供國內具實名制功能的APP介接取得民眾自己的數位證明，並以APP為載具。發行或管理APP者，確認符合個資法及GDPR、身分驗證強度不低於本數位證明平臺，且APP後臺不得留存數位證明，請向指揮中心正式申請。\$\@\$為更新原有版本的功能，申辦平台預計今年1月20日下午5時至次(21)日上午8時停止服務進行更版，有急需出國使用者，請先提前下載。詳細下戴及驗證系統操作方式可以參考衛生福利部官網數位證明專區( https://covid19.mohw.gov.tw/ch/np-5345-205.html )。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-20\$\@\$中央流行疫情指揮中心今(20)日表示，因應Omicron新型變異株之威脅，且國內本土疫情尚未平息，存在社區傳播風險，自今(2022)年1月21日起，民眾前往「歌廳、舞廳、夜總會、俱樂部、酒家、酒吧、酒店(廊)、理容院(觀光理髮、視聽理容)及特種咖啡茶室、夜店、舞場、三溫暖」等休閒娛樂場所時，應配合出示完整接種COVID-19疫苗紀錄，始得入內活動消費。接種紀錄除出示「紙本疫苗接種卡」外，亦可使用「健保快易通」或「數位新冠病毒健康證明」提供檢視。\$\@\$指揮中心說明，上述休閒娛樂場所具有接觸不特定人及無法保持社交距離之特性，COVID-19傳播風險相對較高，為降低於場所消費期間接觸染疫之風險，強化場所之防疫管理措施，除維持該等場所工作人員皆應接種COVID-19疫苗2劑且滿14天，未完整接種者，應每週定期篩檢陰性，始得提供服務外，自1月21日起調整民眾前往消費時，須配合出示完整接種COVID-19疫苗2劑且滿14天紀錄，始得進場，請民眾務必配合，也請業者落實查核，使顧客安心消費，同時保護員工健康安全。\$\@\$指揮中心另指出，針對醫院及住宿式長照機構等現行已有針對COVID-19疫苗接種情形進行規範之場域，請民眾依規定，配合出示COVID-19疫苗紀錄，接種紀錄同樣可使用「紙本疫苗接種卡」、「健保快易通」或「數位新冠病毒健康證明」提供檢視。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-25\$\@\$中央流行疫情指揮中心今(25)日公布國內新增38例COVID-19確定病例，分別為13例本土個案及25例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為4例男性、9例女性，年齡介於未滿5歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為8例男性、17例女性，年齡介於10多歲至70多歲，分別自加拿大(5例)、美國、泰國及印度(各3例)、日本(2例)、奈及利亞、瑞典及中國(各1例)移入；另6例調查中。入境日介於今(2022)年1月11日至1月24日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,501,288例新型冠狀病毒肺炎相關通報(含5,482,563例排除)，其中18,411例確診，分別為3,429例境外移入，14,928例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增3例空號病例(案18216-18218，再次採檢為陰性，改判排除)，累計122例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月25日新增本土COVID-19確診個案表.pdf\$\@\$1月25日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-25\$\@\$中央流行疫情指揮中心今(25)日表示，因應國內本土疫情升溫，目前已提供民眾於各地方政府衛生局安排/指定之合約醫療院所預約或至隨到隨打接種站方式接種COVID-19疫苗。為提供多元疫苗預約管道，加速提升民眾免疫保護力，COVID-19公費疫苗預約平臺（https://1922.gov.tw/ ，以下簡稱預約平臺）第21期將提供「已完整接種兩劑COVID-19疫苗滿12週且滿18歲以上」民眾，預約接種疫苗追加劑。另請已於各地方政府衛生局安排/指定之合約醫療院所完成預約之民眾，請依原已預約時段前往接種，無需再於預約平臺重複預約。\$\@\$預約平臺相關對象及期程說明如下：\$\@\$一、施打時程：2月7日至2月13日。\$\@\$二、符合資格對象：2021年11月21日前已完整接種兩劑疫苗且間隔滿12週之18歲以上民眾[即2004/2/13(含)前出生]預約接種疫苗追加劑。\$\@\$三、預約分流時程：\$\@\$(一)65歲以上：1月26日上午10時至1月27日下午4時。\$\@\$(二)50歲-64歲：1月26日中午12時至1月27日下午4時。\$\@\$(三)18歲-49歲：1月26日下午2時至1月27日下午4時。\$\@\$指揮中心說明，民眾可於1月25日下午2時起於預約平臺進行預約資格查詢，不再另發送預約提醒簡訊，符合資格民眾請記得於預約時間進行預約，預約當日如遇啟動流量管制亦請配合依序排隊耐心等候預約。\$\@\$指揮中心指出，預約平臺第21期僅提供民眾預約接種疫苗追加劑，民眾若有第一、二劑或基礎加強劑接種需求，請持接種紀錄(小黃卡)至各地方政府指定/安排合約醫療院所或衛生所預約接種，或所設置之隨到隨打接種站接種。前述醫療院所資訊，可至疾管署全球資訊網( https://www.cdc.gov.tw/ ) COVID-19疫苗接種院所項下，利用「COVID-19疫苗接種院所」或「COVID-19疫苗接種院所地圖」，依各地方政府衛生局提供資訊連結預約接種。\$\@\$指揮中心提醒，請民眾前往接種COVID-19疫苗前，應備妥「COVID-19疫苗接種紀錄卡」及健保卡，並經醫生評估過往疫苗接種史及檢核接種紀錄後，提供民眾疫苗接種。另18歲至未滿20歲民眾，如自行前往接種，請持家長簽具之意願同意書，若由家長陪同前往接種，請本人與家長於現場共同簽署意願同意書。</t>
+    <t>發佈日期：2021-12-24\$\@\$一、考評單位：衛生福利部疾病管制署。\$\@\$二、考評目的：客觀衡量地方政府衛生局111年防疫業務之施政績效。\$\@\$三、受評機關：地方政府衛生局。\$\@\$四、受評期間：111年1月至12月\$\@\$五、考評架構與權重：9項考評指標，共計200分。\$\@\$六、考評方式：\$\@\$(一)   防疫業務相關管理系統之統計結果及書面考核。\$\@\$本手冊考評指標資料，如須受評機關提供始得評分者，請於112年1月13日前備函逕送考評執行單位進行評核。\$\@\$考評單位於指定日期前完成分數統計及成績評定。\$\@\$考評單位完成考評並請地方政府衛生局確認後，於111年3月17日前將考評結果送衛生福利部綜合規劃司備查。\$\@\$(二)   考評單位得視需要辦理實地查核。 附件\$\@\$111年地方衛生機關業務考評作業手冊-防疫類.pdf\$\@\$111年地方衛生機關業務考評作業手冊-防疫類.docx</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-20\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$公共關係室\$\@\$約用公關助理\$\@\$(徵才案號：0708)\$\@\$(計5名)\$\@\$王○琴(F22546****)\$\@\$李○怡(A22422****)\$\@\$李○達(F12468****)\$\@\$鍾○婷(T22347****)\$\@\$廖○儀(T22036****)\$\@\$二、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一)口試：\$\@\$1、報到時間：110年12月30日星期四09:50~10:00，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署1樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：10:00~11:30。\$\@\$(二)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(三)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於110年12月29日下午5點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3823)，俾利安排應試座位。\$\@\$(四)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(五)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
   </si>
 </sst>
 </file>
@@ -850,7 +886,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -878,16 +914,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C2" s="2">
-        <v>44587</v>
+        <v>44588</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="E2" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -895,16 +931,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C3" s="2">
-        <v>44586</v>
+        <v>44588</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E3" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -912,16 +948,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C4" s="2">
-        <v>44586</v>
+        <v>44588</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="E4" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -929,13 +965,13 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C5" s="2">
-        <v>44586</v>
+        <v>44587</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -943,13 +979,13 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C6" s="2">
         <v>44586</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -957,13 +993,13 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C7" s="2">
         <v>44586</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -971,16 +1007,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C8" s="2">
-        <v>44387</v>
+        <v>44586</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="E8" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -988,16 +1024,16 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C9" s="2">
-        <v>44360</v>
+        <v>44586</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E9" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1005,13 +1041,13 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C10" s="2">
-        <v>44359</v>
+        <v>44586</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1019,16 +1055,13 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C11" s="2">
-        <v>44348</v>
+        <v>44585</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E11" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1036,13 +1069,13 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C12" s="2">
-        <v>44344</v>
+        <v>44585</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1050,13 +1083,13 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C13" s="2">
-        <v>44341</v>
+        <v>44585</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1064,13 +1097,16 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C14" s="2">
-        <v>44567</v>
+        <v>44585</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>103</v>
+        <v>111</v>
+      </c>
+      <c r="E14" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1078,13 +1114,16 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C15" s="2">
-        <v>44567</v>
+        <v>44585</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>104</v>
+        <v>112</v>
+      </c>
+      <c r="E15" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1092,16 +1131,16 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C16" s="2">
-        <v>44560</v>
+        <v>44584</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E16" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1109,16 +1148,16 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C17" s="2">
-        <v>44491</v>
+        <v>44583</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E17" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1126,13 +1165,16 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C18" s="2">
-        <v>44469</v>
+        <v>44582</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>107</v>
+        <v>115</v>
+      </c>
+      <c r="E18" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1140,13 +1182,13 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C19" s="2">
-        <v>44467</v>
+        <v>44582</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1154,13 +1196,13 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C20" s="2">
-        <v>44566</v>
+        <v>44581</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1168,863 +1210,511 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C21" s="2">
-        <v>44565</v>
+        <v>44581</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>110</v>
+        <v>118</v>
+      </c>
+      <c r="E21" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="C22" s="2">
-        <v>43264</v>
+        <v>44588</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C23" s="2">
-        <v>44586</v>
+        <v>44588</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
+      </c>
+      <c r="E23" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="C24" s="2">
-        <v>44586</v>
+        <v>44588</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>113</v>
+        <v>101</v>
+      </c>
+      <c r="E24" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C25" s="2">
-        <v>44585</v>
+        <v>44587</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C26" s="2">
-        <v>44583</v>
+        <v>44586</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C27" s="2">
-        <v>44582</v>
+        <v>44586</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C28" s="2">
-        <v>44581</v>
+        <v>44387</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
+      </c>
+      <c r="E28" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C29" s="2">
-        <v>44574</v>
+        <v>44360</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E29" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C30" s="2">
-        <v>44573</v>
+        <v>44359</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E30" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C31" s="2">
-        <v>44554</v>
+        <v>44348</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C32" s="2">
-        <v>44554</v>
+        <v>44344</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C33" s="2">
-        <v>44550</v>
+        <v>44341</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
+      </c>
+      <c r="E33" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C34" s="2">
-        <v>44515</v>
+        <v>44587</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C35" s="2">
-        <v>44585</v>
+        <v>44567</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E35" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C36" s="2">
-        <v>44584</v>
+        <v>44567</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E36" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C37" s="2">
-        <v>44583</v>
+        <v>44560</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E37" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C38" s="2">
-        <v>44582</v>
+        <v>44491</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E38" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C39" s="2">
-        <v>44582</v>
+        <v>44469</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E39" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C40" s="2">
-        <v>44581</v>
+        <v>44566</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E40" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C41" s="2">
-        <v>44581</v>
+        <v>44565</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E41" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C42" s="2">
-        <v>44581</v>
+        <v>43264</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E42" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C43" s="2">
-        <v>44581</v>
+        <v>44588</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C44" s="2">
-        <v>44580</v>
+        <v>44587</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="C45" s="2">
         <v>44587</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E45" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="C46" s="2">
-        <v>44586</v>
+        <v>44587</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E46" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="C47" s="2">
-        <v>44586</v>
+        <v>44587</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E47" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="C48" s="2">
         <v>44586</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E48" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="C49" s="2">
-        <v>44586</v>
+        <v>44574</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E49" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="C50" s="2">
-        <v>44586</v>
+        <v>44573</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>96</v>
+        <v>141</v>
+      </c>
+      <c r="E50" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="C51" s="2">
-        <v>44387</v>
+        <v>44554</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>97</v>
+        <v>142</v>
       </c>
       <c r="E51" t="s">
-        <v>137</v>
+        <v>164</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="C52" s="2">
-        <v>44360</v>
+        <v>44554</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E52" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="C53" s="2">
-        <v>44359</v>
+        <v>44550</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>99</v>
+        <v>144</v>
+      </c>
+      <c r="E53" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="C54" s="2">
-        <v>44348</v>
+        <v>44515</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E54" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" t="s">
-        <v>15</v>
-      </c>
-      <c r="B55" t="s">
-        <v>58</v>
-      </c>
-      <c r="C55" s="2">
-        <v>44344</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" t="s">
-        <v>16</v>
-      </c>
-      <c r="B56" t="s">
-        <v>59</v>
-      </c>
-      <c r="C56" s="2">
-        <v>44341</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" t="s">
-        <v>17</v>
-      </c>
-      <c r="B57" t="s">
-        <v>60</v>
-      </c>
-      <c r="C57" s="2">
-        <v>44567</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" t="s">
-        <v>18</v>
-      </c>
-      <c r="B58" t="s">
-        <v>61</v>
-      </c>
-      <c r="C58" s="2">
-        <v>44567</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59" t="s">
-        <v>62</v>
-      </c>
-      <c r="C59" s="2">
-        <v>44560</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E59" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" t="s">
-        <v>20</v>
-      </c>
-      <c r="B60" t="s">
-        <v>63</v>
-      </c>
-      <c r="C60" s="2">
-        <v>44491</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E60" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" t="s">
-        <v>21</v>
-      </c>
-      <c r="B61" t="s">
-        <v>64</v>
-      </c>
-      <c r="C61" s="2">
-        <v>44469</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" t="s">
-        <v>22</v>
-      </c>
-      <c r="B62" t="s">
-        <v>65</v>
-      </c>
-      <c r="C62" s="2">
-        <v>44467</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" t="s">
-        <v>23</v>
-      </c>
-      <c r="B63" t="s">
-        <v>66</v>
-      </c>
-      <c r="C63" s="2">
-        <v>44566</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" t="s">
-        <v>24</v>
-      </c>
-      <c r="B64" t="s">
-        <v>67</v>
-      </c>
-      <c r="C64" s="2">
-        <v>44565</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" t="s">
-        <v>25</v>
-      </c>
-      <c r="B65" t="s">
-        <v>68</v>
-      </c>
-      <c r="C65" s="2">
-        <v>43264</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" t="s">
-        <v>26</v>
-      </c>
-      <c r="B66" t="s">
-        <v>69</v>
-      </c>
-      <c r="C66" s="2">
-        <v>44586</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" t="s">
-        <v>27</v>
-      </c>
-      <c r="B67" t="s">
-        <v>70</v>
-      </c>
-      <c r="C67" s="2">
-        <v>44586</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" t="s">
-        <v>28</v>
-      </c>
-      <c r="B68" t="s">
-        <v>71</v>
-      </c>
-      <c r="C68" s="2">
-        <v>44585</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" t="s">
-        <v>29</v>
-      </c>
-      <c r="B69" t="s">
-        <v>72</v>
-      </c>
-      <c r="C69" s="2">
-        <v>44583</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" t="s">
-        <v>30</v>
-      </c>
-      <c r="B70" t="s">
-        <v>73</v>
-      </c>
-      <c r="C70" s="2">
-        <v>44582</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" t="s">
-        <v>31</v>
-      </c>
-      <c r="B71" t="s">
-        <v>74</v>
-      </c>
-      <c r="C71" s="2">
-        <v>44581</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72" t="s">
-        <v>32</v>
-      </c>
-      <c r="B72" t="s">
-        <v>75</v>
-      </c>
-      <c r="C72" s="2">
-        <v>44574</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E72" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" t="s">
-        <v>33</v>
-      </c>
-      <c r="B73" t="s">
-        <v>76</v>
-      </c>
-      <c r="C73" s="2">
-        <v>44573</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E73" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
-      <c r="A74" t="s">
-        <v>34</v>
-      </c>
-      <c r="B74" t="s">
-        <v>77</v>
-      </c>
-      <c r="C74" s="2">
-        <v>44554</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
-      <c r="A75" t="s">
-        <v>35</v>
-      </c>
-      <c r="B75" t="s">
-        <v>78</v>
-      </c>
-      <c r="C75" s="2">
-        <v>44554</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" t="s">
-        <v>36</v>
-      </c>
-      <c r="B76" t="s">
-        <v>79</v>
-      </c>
-      <c r="C76" s="2">
-        <v>44550</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="A77" t="s">
-        <v>37</v>
-      </c>
-      <c r="B77" t="s">
-        <v>80</v>
-      </c>
-      <c r="C77" s="2">
-        <v>44515</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2082,29 +1772,6 @@
     <hyperlink ref="D52" r:id="rId51"/>
     <hyperlink ref="D53" r:id="rId52"/>
     <hyperlink ref="D54" r:id="rId53"/>
-    <hyperlink ref="D55" r:id="rId54"/>
-    <hyperlink ref="D56" r:id="rId55"/>
-    <hyperlink ref="D57" r:id="rId56"/>
-    <hyperlink ref="D58" r:id="rId57"/>
-    <hyperlink ref="D59" r:id="rId58"/>
-    <hyperlink ref="D60" r:id="rId59"/>
-    <hyperlink ref="D61" r:id="rId60"/>
-    <hyperlink ref="D62" r:id="rId61"/>
-    <hyperlink ref="D63" r:id="rId62"/>
-    <hyperlink ref="D64" r:id="rId63"/>
-    <hyperlink ref="D65" r:id="rId64"/>
-    <hyperlink ref="D66" r:id="rId65"/>
-    <hyperlink ref="D67" r:id="rId66"/>
-    <hyperlink ref="D68" r:id="rId67"/>
-    <hyperlink ref="D69" r:id="rId68"/>
-    <hyperlink ref="D70" r:id="rId69"/>
-    <hyperlink ref="D71" r:id="rId70"/>
-    <hyperlink ref="D72" r:id="rId71"/>
-    <hyperlink ref="D73" r:id="rId72"/>
-    <hyperlink ref="D74" r:id="rId73"/>
-    <hyperlink ref="D75" r:id="rId74"/>
-    <hyperlink ref="D76" r:id="rId75"/>
-    <hyperlink ref="D77" r:id="rId76"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20220128
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="167">
   <si>
     <t>Press Title</t>
   </si>
@@ -31,6 +31,9 @@
     <t>Page Content</t>
   </si>
   <si>
+    <t>新增71例COVID-19確定病例，分別為27例本土及44例境外移入</t>
+  </si>
+  <si>
     <t>新增64例COVID-19確定病例，分別為21例本土及43例境外移入</t>
   </si>
   <si>
@@ -46,16 +49,94 @@
     <t>鑑於帛琉近期疫情快速上升，1月25日起提升旅遊疫情建議至第三級警告 (Warning)</t>
   </si>
   <si>
-    <t>指揮中心公布COVID-19自費核酸檢驗指定機構農曆春節連假期間服務資訊</t>
-  </si>
-  <si>
-    <t>新增38例COVID-19確定病例，分別為13例本土及25例境外移入</t>
-  </si>
-  <si>
-    <t>COVID-19公費疫苗平臺第21期自1月26日起，提供已完整接種兩劑COVID-19疫苗滿12週且滿18歲以上民眾預約接種疫苗追加劑</t>
-  </si>
-  <si>
-    <t>今(2022)年第一批採購Moderna疫苗151.21萬劑於今(25)日下午抵臺</t>
+    <t>網傳「三級警戒微解封的不可思議之處」指揮中心： 原同住家人就不受限制，謠言邏輯誤導且比喻失當，請勿輕信轉傳，造成防疫困擾</t>
+  </si>
+  <si>
+    <t>網傳「政府讓人民施打未受認證且保護力低之國產疫苗」  指揮中心：會把關國產疫苗品質、安全及療效</t>
+  </si>
+  <si>
+    <t>網傳「代工(AZ疫苗)三億劑嫌太多賣不出去」，指揮中心：有心人刻意扭曲語意</t>
+  </si>
+  <si>
+    <t>網傳「臺中太原路復健醫院被徵收為方艙醫院」 指揮中心：假訊息勿轉傳</t>
+  </si>
+  <si>
+    <t>網路販售「新冠病毒快篩試劑」，指揮中心：已觸法，警方偵辦中</t>
+  </si>
+  <si>
+    <t>網現偽冒教育部網站  指揮中心：境外假網頁勿輕信</t>
+  </si>
+  <si>
+    <t>COVID-19專家諮詢會彙整針對Omicron變異株藥物使用建議(疾病管制署致醫界通函第472號)</t>
+  </si>
+  <si>
+    <t>SARS-CoV-2感染臨床處置暫行指引新增口服抗病毒藥物使用建議(疾病管制署致醫界通函第471號)</t>
+  </si>
+  <si>
+    <t>因應結核菌液態培養(MGIT)檢驗試劑暫時性缺貨，為利早期診斷結核病，針對疑似結核病送驗初查痰3套，請務必再進行結核分枝桿菌核酸增幅(NAA)檢驗(疾病管制署致醫界通函第470號)</t>
+  </si>
+  <si>
+    <t>COVID-19專家諮詢會因應變異株流行，更新治療指引藥物適用原則(疾病管制署致醫界通函第469號)</t>
+  </si>
+  <si>
+    <t>因應COVID-19 Omicron變異株威脅，籲請社區定點診所加強發放公費COVID-19家用快篩試劑予高風險民眾(疾病管制署致醫界通函第468號)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COVID-19專家諮詢會參照最新實證與藥物適應症，更新治療指引藥物適用對象並重申制定原則(疾病管制署致醫界通函第467號) </t>
+  </si>
+  <si>
+    <t>BioNTech COVID-19疫苗750萬劑倉儲物流配送與服務.pdf(另開新視窗)</t>
+  </si>
+  <si>
+    <t>111年藥癮愛滋減害計畫1ml注射用水.pdf(另開新視窗)</t>
+  </si>
+  <si>
+    <t>111年藥癮愛滋減害計畫0.5ml注射針具.pdf(另開新視窗)</t>
+  </si>
+  <si>
+    <t>111年度核酸定序.pdf(另開新視窗)</t>
+  </si>
+  <si>
+    <t>111年限制酶、聚合酵素及核酸分析試劑乙批.pdf(另開新視窗)</t>
+  </si>
+  <si>
+    <t>111年分枝桿菌檢驗用聚合酵素鏈鎖反應機及因應嚴重特殊傳染性肺炎全球大流行疫情採購多功能病毒基因及核酸擴增儀.pdf(另開新視窗)</t>
+  </si>
+  <si>
+    <t>約用助理(徵才案號：1424)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">約聘護理師(英檢初級) </t>
+  </si>
+  <si>
+    <t>約聘護理師</t>
+  </si>
+  <si>
+    <t>約聘技術員</t>
+  </si>
+  <si>
+    <t>約用護理師(徵才案號：1523)</t>
+  </si>
+  <si>
+    <t>約用護理師(徵才案號：1810)(預估缺，自111年2月20日出缺)</t>
+  </si>
+  <si>
+    <t>公告本署疫情中心約用人員徵才案(徵才案號：0605，含延長公告)初審合格名單及甄試事宜。</t>
+  </si>
+  <si>
+    <t>公告本署急性傳染病組約用人員徵才案(徵才案號：1106，含延長公告)初審合格名單及甄試事宜。</t>
+  </si>
+  <si>
+    <t>公告本署檢疫組約用人員徵才案(徵才案號：0507)初審合格名單及甄試事宜。</t>
+  </si>
+  <si>
+    <t>111年地方衛生機關防疫業務考評作業手冊</t>
+  </si>
+  <si>
+    <t>公告本署慢性傳染病組約用人員徵才案(徵才案號：0309)初審合格名單及甄試事宜。</t>
+  </si>
+  <si>
+    <t>公告本署公共關係室約用人員徵才案(徵才案號：0708)初審合格名單及甄試事宜。</t>
   </si>
   <si>
     <t>全國醫院即日起除例外情形，停止開放探病，並調整住院病人、陪(探)病者及醫療照護人員篩檢及疫苗接種等相關規定</t>
@@ -88,88 +169,7 @@
     <t>因應帛琉近期疫情，指揮中心說明相關檢疫應變措施</t>
   </si>
   <si>
-    <t>1月21日上午8時「數位新冠病毒健康證明」開放國內使用</t>
-  </si>
-  <si>
-    <t>網傳「三級警戒微解封的不可思議之處」指揮中心： 原同住家人就不受限制，謠言邏輯誤導且比喻失當，請勿輕信轉傳，造成防疫困擾</t>
-  </si>
-  <si>
-    <t>網傳「政府讓人民施打未受認證且保護力低之國產疫苗」  指揮中心：會把關國產疫苗品質、安全及療效</t>
-  </si>
-  <si>
-    <t>網傳「代工(AZ疫苗)三億劑嫌太多賣不出去」，指揮中心：有心人刻意扭曲語意</t>
-  </si>
-  <si>
-    <t>網傳「臺中太原路復健醫院被徵收為方艙醫院」 指揮中心：假訊息勿轉傳</t>
-  </si>
-  <si>
-    <t>網路販售「新冠病毒快篩試劑」，指揮中心：已觸法，警方偵辦中</t>
-  </si>
-  <si>
-    <t>網現偽冒教育部網站  指揮中心：境外假網頁勿輕信</t>
-  </si>
-  <si>
-    <t>SARS-CoV-2感染臨床處置暫行指引新增口服抗病毒藥物使用建議(疾病管制署致醫界通函第471號)</t>
-  </si>
-  <si>
-    <t>因應結核菌液態培養(MGIT)檢驗試劑暫時性缺貨，為利早期診斷結核病，針對疑似結核病送驗初查痰3套，請務必再進行結核分枝桿菌核酸增幅(NAA)檢驗(疾病管制署致醫界通函第470號)</t>
-  </si>
-  <si>
-    <t>COVID-19專家諮詢會因應變異株流行，更新治療指引藥物適用原則(疾病管制署致醫界通函第469號)</t>
-  </si>
-  <si>
-    <t>因應COVID-19 Omicron變異株威脅，籲請社區定點診所加強發放公費COVID-19家用快篩試劑予高風險民眾(疾病管制署致醫界通函第468號)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COVID-19專家諮詢會參照最新實證與藥物適應症，更新治療指引藥物適用對象並重申制定原則(疾病管制署致醫界通函第467號) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">近期登革熱隱藏期平均超過3日，籲請醫師對具登革熱流行地區旅遊史之疑似病例提高警覺，加強診斷及通報(疾病管制署致醫界通函第466號) </t>
-  </si>
-  <si>
-    <t>111-112年 COVID-19疫苗4,000萬劑倉儲物流與配送.pdf(另開新視窗)</t>
-  </si>
-  <si>
-    <t>111年度病毒、細菌、真菌試驗試劑耗材採購案.pdf(另開新視窗)</t>
-  </si>
-  <si>
-    <t>衛生福利部疾病管制署臺北區管制中心公告.zip(檔案下載)</t>
-  </si>
-  <si>
-    <t>約聘護理師</t>
-  </si>
-  <si>
-    <t>約用護理師(徵才案號：1527)</t>
-  </si>
-  <si>
-    <t>約用助理(徵才案號：1528)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">約聘護理師(英檢初級) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">約聘護理師(英檢中級) </t>
-  </si>
-  <si>
-    <t>約聘技術員</t>
-  </si>
-  <si>
-    <t>公告本署急性傳染病組約用人員徵才案(徵才案號：1106，含延長公告)初審合格名單及甄試事宜。</t>
-  </si>
-  <si>
-    <t>公告本署檢疫組約用人員徵才案(徵才案號：0507)初審合格名單及甄試事宜。</t>
-  </si>
-  <si>
-    <t>111年地方衛生機關防疫業務考評作業手冊</t>
-  </si>
-  <si>
-    <t>公告本署慢性傳染病組約用人員徵才案(徵才案號：0309)初審合格名單及甄試事宜。</t>
-  </si>
-  <si>
-    <t>公告本署公共關係室約用人員徵才案(徵才案號：0708)初審合格名單及甄試事宜。</t>
-  </si>
-  <si>
-    <t>公告本署檢驗及疫苗研製中心約用人員徵才案(徵才案號：1057、1058)初審合格名單及甄試事宜。</t>
+    <t>/Bulletin/Detail/RBLVTwsQ9Z33zCEe0IMd_Q?typeid=9</t>
   </si>
   <si>
     <t>/Bulletin/Detail/AaV2iREpabJ8syXu4450Rw?typeid=9</t>
@@ -187,16 +187,94 @@
     <t>/Bulletin/Detail/w5wAafr4zKG_ZR88_qWdVQ?typeid=9</t>
   </si>
   <si>
-    <t>/Bulletin/Detail/xah9AQII8GupFO7uV7kz-Q?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/Juq0widEV7lcQ05-8Db97g?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/CLDus_S2F3qf0fxYMx5zdw?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/AFuil2ECiqiNku1SmowIGQ?typeid=9</t>
+    <t>/Bulletin/Detail/ftv6FPFis84j5uHWTq4lNA?typeid=8772</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/PmSCiSjM5YpCUxXqoS81RA?typeid=8772</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/QCmwPRiL1nKrc8-AuqSEGg?typeid=8772</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/IO3F02JMs4pToOM84aXopQ?typeid=8772</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/zjF-6vCLlbYe1RhTXKlq1Q?typeid=8772</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/IU5CMLLt8bQqXWHQhil0Aw?typeid=8772</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/u6Aw7NXRRwb50IL0WfPyrQ?typeid=48</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/7LF3_zX-27ttBkfVRsjlqA?typeid=48</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/KaqzyT5RqFOuOQFGpEYLgA?typeid=48</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/zUiCR7uM2Ox39wGHOkzhMw?typeid=48</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/tun0Es9fOoIJqDFToylh6Q?typeid=48</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/1pVYYgWzE_U3RlTuctsioQ?typeid=48</t>
+  </si>
+  <si>
+    <t>/Uploads/files/71a88175-332c-4dbd-89c0-46f431a00711.pdf</t>
+  </si>
+  <si>
+    <t>/Uploads/files/29e64809-274d-4391-aff3-9c3972636971.pdf</t>
+  </si>
+  <si>
+    <t>/Uploads/files/c5bc7d2f-52c2-44a5-aad3-90e3831b8894.pdf</t>
+  </si>
+  <si>
+    <t>/Uploads/files/e7441505-beda-428c-b309-9523e48fe264.pdf</t>
+  </si>
+  <si>
+    <t>/Uploads/files/cf7b95e9-905e-4efa-ba42-bac0227f8070.pdf</t>
+  </si>
+  <si>
+    <t>/Uploads/files/f1db9d43-45f0-46d8-9f13-351b4708e447.pdf</t>
+  </si>
+  <si>
+    <t>/HireList/Detail?hireId=Cb-Wgu1wR-59aNUgonxJEQ</t>
+  </si>
+  <si>
+    <t>/HireList/Detail?hireId=d6UgvUNhaaIk8TkyD-3kOw</t>
+  </si>
+  <si>
+    <t>/HireList/Detail?hireId=0nPPV437nrsZtDlmACTqig</t>
+  </si>
+  <si>
+    <t>/HireList/Detail?hireId=dWXPWipxKvMpkrjCmJ3BvA</t>
+  </si>
+  <si>
+    <t>/HireList/Detail?hireId=4wyEVe65rp-Hr9DETX8n2g</t>
+  </si>
+  <si>
+    <t>/HireList/Detail?hireId=4-owN86iWtEzBDoT5ePd2g</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/30JdGCIgFmMIFaxMbxaOmg?typeid=11</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/yYmtcBLADf7DiN6l-Qsljw?typeid=11</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/4g9LCvtGigoLSDRpd_ZKmg?typeid=11</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/Y_cTXA-RBSS1MjAEFDP3TQ?typeid=11</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/vN_TxnDuv7GamvGxnZXEdw?typeid=11</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/7UJRpdDRbQNIZWyyEfHdHQ?typeid=11</t>
   </si>
   <si>
     <t>/Bulletin/Detail/kVDslqExqB7BSiqJuFzXCg?typeid=9</t>
@@ -229,88 +307,7 @@
     <t>/Bulletin/Detail/lVU_tRUutNI667QAZYcj7g?typeid=9</t>
   </si>
   <si>
-    <t>/Bulletin/Detail/mAWzcQcUVI2XPmIdtic3jg?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/ftv6FPFis84j5uHWTq4lNA?typeid=8772</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/PmSCiSjM5YpCUxXqoS81RA?typeid=8772</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/QCmwPRiL1nKrc8-AuqSEGg?typeid=8772</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/IO3F02JMs4pToOM84aXopQ?typeid=8772</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/zjF-6vCLlbYe1RhTXKlq1Q?typeid=8772</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/IU5CMLLt8bQqXWHQhil0Aw?typeid=8772</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/7LF3_zX-27ttBkfVRsjlqA?typeid=48</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/KaqzyT5RqFOuOQFGpEYLgA?typeid=48</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/zUiCR7uM2Ox39wGHOkzhMw?typeid=48</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/tun0Es9fOoIJqDFToylh6Q?typeid=48</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/1pVYYgWzE_U3RlTuctsioQ?typeid=48</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/HU4mCbrzZQlHC-VhwBiJOg?typeid=48</t>
-  </si>
-  <si>
-    <t>/Uploads/files/a22b63a6-c6cb-463f-940d-26f4c11b17bc.pdf</t>
-  </si>
-  <si>
-    <t>/Uploads/files/ff4bbce0-18e6-4472-b285-83199d1a142d.pdf</t>
-  </si>
-  <si>
-    <t>/Uploads/files/716583a9-c090-42d4-90dd-9afcbccbf4f4.zip</t>
-  </si>
-  <si>
-    <t>/HireList/Detail?hireId=0nPPV437nrsZtDlmACTqig</t>
-  </si>
-  <si>
-    <t>/HireList/Detail?hireId=qtKOuJxyY69hM91fhqIGwQ</t>
-  </si>
-  <si>
-    <t>/HireList/Detail?hireId=is3mwnpA6TueQWq1SHoKdQ</t>
-  </si>
-  <si>
-    <t>/HireList/Detail?hireId=vYAPhNrdpYAXFjtQ855W3w</t>
-  </si>
-  <si>
-    <t>/HireList/Detail?hireId=ZpDrALR1adV__qi1GWCyKg</t>
-  </si>
-  <si>
-    <t>/HireList/Detail?hireId=dbhD6saaWV5URglIuc0HhA</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/yYmtcBLADf7DiN6l-Qsljw?typeid=11</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/4g9LCvtGigoLSDRpd_ZKmg?typeid=11</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/Y_cTXA-RBSS1MjAEFDP3TQ?typeid=11</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/vN_TxnDuv7GamvGxnZXEdw?typeid=11</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/7UJRpdDRbQNIZWyyEfHdHQ?typeid=11</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/u9ej71cxiu9bJqO0gMxdOQ?typeid=11</t>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/RBLVTwsQ9Z33zCEe0IMd_Q?typeid=9</t>
   </si>
   <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/AaV2iREpabJ8syXu4450Rw?typeid=9</t>
@@ -328,16 +325,94 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/w5wAafr4zKG_ZR88_qWdVQ?typeid=9</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/xah9AQII8GupFO7uV7kz-Q?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/Juq0widEV7lcQ05-8Db97g?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/CLDus_S2F3qf0fxYMx5zdw?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/AFuil2ECiqiNku1SmowIGQ?typeid=9</t>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/ftv6FPFis84j5uHWTq4lNA?typeid=8772</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/PmSCiSjM5YpCUxXqoS81RA?typeid=8772</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/QCmwPRiL1nKrc8-AuqSEGg?typeid=8772</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/IO3F02JMs4pToOM84aXopQ?typeid=8772</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/zjF-6vCLlbYe1RhTXKlq1Q?typeid=8772</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/IU5CMLLt8bQqXWHQhil0Aw?typeid=8772</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/u6Aw7NXRRwb50IL0WfPyrQ?typeid=48</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/7LF3_zX-27ttBkfVRsjlqA?typeid=48</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/KaqzyT5RqFOuOQFGpEYLgA?typeid=48</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/zUiCR7uM2Ox39wGHOkzhMw?typeid=48</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/tun0Es9fOoIJqDFToylh6Q?typeid=48</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/1pVYYgWzE_U3RlTuctsioQ?typeid=48</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Uploads/files/71a88175-332c-4dbd-89c0-46f431a00711.pdf</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Uploads/files/29e64809-274d-4391-aff3-9c3972636971.pdf</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Uploads/files/c5bc7d2f-52c2-44a5-aad3-90e3831b8894.pdf</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Uploads/files/e7441505-beda-428c-b309-9523e48fe264.pdf</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Uploads/files/cf7b95e9-905e-4efa-ba42-bac0227f8070.pdf</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Uploads/files/f1db9d43-45f0-46d8-9f13-351b4708e447.pdf</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=Cb-Wgu1wR-59aNUgonxJEQ</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=d6UgvUNhaaIk8TkyD-3kOw</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=0nPPV437nrsZtDlmACTqig</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=dWXPWipxKvMpkrjCmJ3BvA</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=4wyEVe65rp-Hr9DETX8n2g</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=4-owN86iWtEzBDoT5ePd2g</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/30JdGCIgFmMIFaxMbxaOmg?typeid=11</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/yYmtcBLADf7DiN6l-Qsljw?typeid=11</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/4g9LCvtGigoLSDRpd_ZKmg?typeid=11</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/Y_cTXA-RBSS1MjAEFDP3TQ?typeid=11</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/vN_TxnDuv7GamvGxnZXEdw?typeid=11</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/7UJRpdDRbQNIZWyyEfHdHQ?typeid=11</t>
   </si>
   <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/kVDslqExqB7BSiqJuFzXCg?typeid=9</t>
@@ -370,88 +445,7 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/lVU_tRUutNI667QAZYcj7g?typeid=9</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/mAWzcQcUVI2XPmIdtic3jg?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/ftv6FPFis84j5uHWTq4lNA?typeid=8772</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/PmSCiSjM5YpCUxXqoS81RA?typeid=8772</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/QCmwPRiL1nKrc8-AuqSEGg?typeid=8772</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/IO3F02JMs4pToOM84aXopQ?typeid=8772</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/zjF-6vCLlbYe1RhTXKlq1Q?typeid=8772</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/IU5CMLLt8bQqXWHQhil0Aw?typeid=8772</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/7LF3_zX-27ttBkfVRsjlqA?typeid=48</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/KaqzyT5RqFOuOQFGpEYLgA?typeid=48</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/zUiCR7uM2Ox39wGHOkzhMw?typeid=48</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/tun0Es9fOoIJqDFToylh6Q?typeid=48</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/1pVYYgWzE_U3RlTuctsioQ?typeid=48</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/HU4mCbrzZQlHC-VhwBiJOg?typeid=48</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Uploads/files/a22b63a6-c6cb-463f-940d-26f4c11b17bc.pdf</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Uploads/files/ff4bbce0-18e6-4472-b285-83199d1a142d.pdf</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Uploads/files/716583a9-c090-42d4-90dd-9afcbccbf4f4.zip</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=0nPPV437nrsZtDlmACTqig</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=qtKOuJxyY69hM91fhqIGwQ</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=is3mwnpA6TueQWq1SHoKdQ</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=vYAPhNrdpYAXFjtQ855W3w</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=ZpDrALR1adV__qi1GWCyKg</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/HireList/Detail?hireId=dbhD6saaWV5URglIuc0HhA</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/yYmtcBLADf7DiN6l-Qsljw?typeid=11</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/4g9LCvtGigoLSDRpd_ZKmg?typeid=11</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/Y_cTXA-RBSS1MjAEFDP3TQ?typeid=11</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/vN_TxnDuv7GamvGxnZXEdw?typeid=11</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/7UJRpdDRbQNIZWyyEfHdHQ?typeid=11</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/u9ej71cxiu9bJqO0gMxdOQ?typeid=11</t>
+    <t>發佈日期：2022-01-28\$\@\$中央流行疫情指揮中心今(28)日公布國內新增71例COVID-19確定病例，分別為27例本土個案及44例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為8例男性、19例女性，年齡介於未滿10歲至60多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為25例男性、19例女性，年齡介於未滿5歲至70多歲，分別自美國及菲律賓各8例、中國5例、印尼3例、日本、瑞典及越南各2例、孟加拉國、荷蘭、土耳其、英國、奧地利及丹麥各1例移入；另8例調查中。入境日介於今(2022)年1月13日至1月27日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,613,922例新型冠狀病毒肺炎相關通報(含5,594,976例排除)，其中18,634例確診，分別為3,561例境外移入，15,019例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增3例空號病例(案18314境外移入、案18425本土、案18438本土，再次採檢為陰性，共3案研判排除)，累計126例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月28日新增本土COVID-19確診個案表.pdf\$\@\$1月28日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
     <t>發佈日期：2022-01-27\$\@\$中央流行疫情指揮中心今(27)日公布國內新增64例COVID-19確定病例，分別為21例本土個案及43例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為11例男性、10例女性，年齡介於未滿5歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為21例男性、22例女性，年齡介於未滿5歲至60多歲，分別自美國(14例)、印度(3例)、越南、印尼、英國及法國(各2例)、衣索比亞、坦尚尼亞、新加坡、土耳其、菲律賓、南非、芬蘭、日本(各1例)移入；另10例調查中。入境日介於去(2021)年5月2日至今(2022)年1月26日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,581,517例新型冠狀病毒肺炎相關通報(含5,562,679例排除)，其中18,566例確診，分別為3,518例境外移入，14,994例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案18418，再次採檢為陰性，改判排除)，累計123例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月27日新增本土COVID-19確診個案表.pdf\$\@\$1月27日新增境外移入COVID-19確診個案表.pdf</t>
@@ -460,16 +454,52 @@
     <t>發佈日期：2022-01-27\$\@\$中央流行疫情指揮中心今(27)日表示，因應Omicron新型變異株威脅持續，且國內本土疫情尚未平息，考量春節連假期間團聚交流、遊憩活動頻繁，社區傳播的風險提高，指揮中心特別訂定「COVID-19疫情期間民眾假期生活防疫指引」，提醒民眾在享受春節連假時光時，主動落實防疫措施，平安過好年。\$\@\$指揮中心指出，春節連假期間落實勤洗手、呼吸道衛生與咳嗽禮節等良好個人衛生習慣尤為重要；若民眾本身或家人屬於慢性病患者、老年人、孕婦、體重過重、嬰幼兒等免疫力比較不好的族群，更易受感染及感染後病症較為嚴重，請符合接種條件者，儘速完整接種疫苗，獲得保護力，同時也應儘量避免參加可能密集接觸不特定人的聚會或活動，及前往人潮聚集、密閉空間或通風不良的公共場所。另民眾如果要探視上述免疫力較差的對象，建議雙方皆已完整接種疫苗，而探視者也要確認自身沒有身體不適症狀，且近期沒有參加密集接觸不特定人的聚會或活動，再行當面探視，探視時雙方都應佩戴口罩，以降低感染傳播的機會；否則建議使用電話或視訊方式取代。\$\@\$指揮中心呼籲，連假期間外出活動，儘量選擇前往開放且沒有人群擁擠的地方，並遵循疫情警戒期間外出全程佩戴口罩、與不特定人保持適當社交距離(室內1.5公尺、室外1公尺)、落實實聯制、體溫監測等防疫規範，親友聚餐也儘量控制人數，並遵守餐飲防疫措施。外出時可攜帶乾洗手用品隨時保持手部清潔，並準備備用口罩以便替換，返回住所時，要確實執行手部衛生。如果出現發燒、呼吸道症狀、腹瀉或嗅、味覺異常時，應佩戴口罩，儘速就醫，不要搭乘大眾運輸工具及前往其他公共場所。</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-27\$\@\$中央流行疫情指揮中心今(27)日表示，台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的第十七批BNT疫苗91.84萬劑，已於今日上午順利運抵桃園國際機場，並在完成通關程序後，直接運送至指定冷儲物流中心進行後續檢驗封緘作業。\$\@\$指揮中心說明，由台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的1500萬劑BNT疫苗已全數到貨，總計1,524.91萬劑，多贈送24.91萬劑，分別為首批9月2日93萬劑、第二批9月9日91萬劑、第三批9月30日54萬劑、第四批10月1日67萬劑、第五批10月4日27萬劑、第六批10月7日88.92萬劑、第七批10月8日88.92萬劑、第八批10月14日82.7萬劑、第九批10月28日90.21萬劑、第十批10月29日91.03萬劑、第十一批11月5日87.17萬劑、第十二批11月12日92.66萬劑、第十三批11月25日93.83萬劑、第十四批12月9日192.35萬劑、第十五批12月30日93.83萬劑，第十六批1月21日99.45萬，以及本批91.84萬劑。本批疫苗效期至2022年5月25日，將由指揮中心統籌運用，儘速提供民眾接種。\$\@\$對於台積電、鴻海暨永齡基金會、慈濟基金會三間企業和民間團體積極協助，提供更多的疫苗讓民眾接種，加速提升臺灣疫苗覆蓋率，指揮中心再次表達由衷的謝意。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-25\$\@\$中央流行疫情指揮中心今(25)日公布國內新增38例COVID-19確定病例，分別為13例本土個案及25例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為4例男性、9例女性，年齡介於未滿5歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為8例男性、17例女性，年齡介於10多歲至70多歲，分別自加拿大(5例)、美國、泰國及印度(各3例)、日本(2例)、奈及利亞、瑞典及中國(各1例)移入；另6例調查中。入境日介於今(2022)年1月11日至1月24日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,501,288例新型冠狀病毒肺炎相關通報(含5,482,563例排除)，其中18,411例確診，分別為3,429例境外移入，14,928例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增3例空號病例(案18216-18218，再次採檢為陰性，改判排除)，累計122例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月25日新增本土COVID-19確診個案表.pdf\$\@\$1月25日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-25\$\@\$中央流行疫情指揮中心今(25)日表示，因應國內本土疫情升溫，目前已提供民眾於各地方政府衛生局安排/指定之合約醫療院所預約或至隨到隨打接種站方式接種COVID-19疫苗。為提供多元疫苗預約管道，加速提升民眾免疫保護力，COVID-19公費疫苗預約平臺（https://1922.gov.tw/ ，以下簡稱預約平臺）第21期將提供「已完整接種兩劑COVID-19疫苗滿12週且滿18歲以上」民眾，預約接種疫苗追加劑。另請已於各地方政府衛生局安排/指定之合約醫療院所完成預約之民眾，請依原已預約時段前往接種，無需再於預約平臺重複預約。\$\@\$預約平臺相關對象及期程說明如下：\$\@\$一、施打時程：2月7日至2月13日。\$\@\$二、符合資格對象：2021年11月21日前已完整接種兩劑疫苗且間隔滿12週之18歲以上民眾[即2004/2/13(含)前出生]預約接種疫苗追加劑。\$\@\$三、預約分流時程：\$\@\$(一)65歲以上：1月26日上午10時至1月27日下午4時。\$\@\$(二)50歲-64歲：1月26日中午12時至1月27日下午4時。\$\@\$(三)18歲-49歲：1月26日下午2時至1月27日下午4時。\$\@\$指揮中心說明，民眾可於1月25日下午2時起於預約平臺進行預約資格查詢，不再另發送預約提醒簡訊，符合資格民眾請記得於預約時間進行預約，預約當日如遇啟動流量管制亦請配合依序排隊耐心等候預約。\$\@\$指揮中心指出，預約平臺第21期僅提供民眾預約接種疫苗追加劑，民眾若有第一、二劑或基礎加強劑接種需求，請持接種紀錄(小黃卡)至各地方政府指定/安排合約醫療院所或衛生所預約接種，或所設置之隨到隨打接種站接種。前述醫療院所資訊，可至疾管署全球資訊網( https://www.cdc.gov.tw/ ) COVID-19疫苗接種院所項下，利用「COVID-19疫苗接種院所」或「COVID-19疫苗接種院所地圖」，依各地方政府衛生局提供資訊連結預約接種。\$\@\$指揮中心提醒，請民眾前往接種COVID-19疫苗前，應備妥「COVID-19疫苗接種紀錄卡」及健保卡，並經醫生評估過往疫苗接種史及檢核接種紀錄後，提供民眾疫苗接種。另18歲至未滿20歲民眾，如自行前往接種，請持家長簽具之意願同意書，若由家長陪同前往接種，請本人與家長於現場共同簽署意願同意書。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-24\$\@\$中央流行疫情指揮中心今(24)日公布國內新增51例COVID-19確定病例，分別為15例本土個案及36例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為10例男性、5例女性，年齡介於10多歲至50多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為21例男性、15例女性，年齡介於未滿5歲至70多歲，分別自美國(20例)、帛琉及印尼(各2例)、香港、越南、荷蘭、海地、菲律賓、多明尼加及比利時(各1例)移入；另5例調查中。入境日介於今(2022)年1月9日至1月23日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,463,663例新型冠狀病毒肺炎相關通報(含5,444,547例排除)，其中18,376例確診，分別為3,404例境外移入，14,918例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計119例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月24日新增本土COVID-19確診個案表.pdf\$\@\$1月24日新增境外移入COVID-19確診個案表.pdf</t>
+    <t>發佈日期：2022-01-27\$\@\$中央流行疫情指揮中心今(27)日表示，台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的第十七批BNT疫苗91.84萬劑，已於今日上午順利運抵桃園國際機場，並在完成通關程序後，直接運送至指定冷儲物流中心進行後續檢驗封緘作業。\$\@\$指揮中心說明，由台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的1500萬劑BNT疫苗已全數到貨，總計1,520.76萬劑，多送20.76萬劑，分別為首批9月2日93.24萬劑、第二批9月9日91.03萬劑、第三批9月30日54萬劑、第四批10月1日67.27萬劑、第五批10月4日27萬劑、第六批10月7日88.92萬劑、第七批10月8日88.92萬劑、第八批10月14日82.7萬劑、第九批10月28日89.62萬劑、第十批10月29日91.03萬劑、第十一批11月5日83.07萬劑、第十二批11月12日92.66萬劑、第十三批11月25日93.83萬劑、第十四批12月9日192.35萬劑、第十五批12月30日93.83萬劑，第十六批1月21日99.45萬，以及本批91.84萬劑。本批疫苗效期至2022年5月25日，將由指揮中心統籌運用，儘速提供民眾接種。\$\@\$對於台積電、鴻海暨永齡基金會、慈濟基金會三間企業和民間團體積極協助，提供更多的疫苗讓民眾接種，加速提升臺灣疫苗覆蓋率，指揮中心再次表達由衷的謝意。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-26\$\@\$中央流行疫情指揮中心今(26)日公布國內新增92例COVID-19確定病例，分別為46例本土個案及46例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為24例男性、22例女性，年齡介於未滿5歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為27例男性、19例女性，年齡介於未滿5歲至60多歲，分別自美國(9例)、英國、加拿大及荷蘭(各2例)、馬來西亞、阿拉伯聯合大公國、法國、中國、瑞典、柬埔寨、越南、新加坡(各1例)移入；另23例調查中。入境日介於今(2022)年1月9日至1月25日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,542,669例新型冠狀病毒肺炎相關通報(含5,523,800例排除)，其中18,503例確診，分別為3,475例境外移入，14,974例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計122例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月26日新增本土COVID-19確診個案表.pdf\$\@\$1月26日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-25\$\@\$中央流行疫情指揮中心今(25)日表示，帛琉近期疫情快速上升，近7日每日平均確診數72例，累計651例確診，另昨(24)日公布2例自帛琉境外移入個案。抵帛之美國CDC專家推測可能為感染Omicron株，評估未來一至兩週應為疫情高峰。\$\@\$指揮中心說明，基於國人至當地有感染風險，指揮中心於1月25日起將帛琉之國際旅遊疫情建議等級提升至第三級警告(Warning)，提醒國人應避免至帛琉進行所有非必要旅遊。除基於(醫療)人道或急迫理由必須緊急赴臺之外籍旅客可另行申請外，入境旅客應遵循相關檢疫規定：所有入境旅客，不論身分(本國籍與外國籍人士等)或來臺目的，原則均應檢附「表定航班時間前2日內COVID-19核酸檢驗報告」及預訂「檢疫居所證明」始得搭機來臺，並於抵臺前48小時內預先使用手機上網登入「入境檢疫系統」，填寫健康情形及旅遊史，完成線上健康申報。另自帛返臺旅客與其他國家入境旅客一致，適用春節檢疫專案。\$\@\$指揮中心強調，將嚴密監控疫情變化，隨時調整各項防檢疫措施，相關資訊可至衛生福利部疾病管制署全球資訊網首頁「COVID-19防疫專區-春節檢疫措施專案」(https://www.cdc.gov.tw/Category/MPage/y-WU-wWeGC8M5ihxysmbFw)查閱。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-10\$\@\$中央流行疫情指揮中心今（10）日表示，近日有網友散布「三級警戒微解封的不可思議之處，新冠肺炎病毒只會攻擊家人」等訊息，相關內容多有誤導，且在錯誤基礎上進行不當類比，指揮中心再次強調，相關防疫指引已清楚說明，原本同住家人可以繼續維持生活，相關指引都是針對日常非同住者間的行為互動加以規範，呼籲民眾勿輕信或隨意散播、轉傳錯誤訊息，造成防疫困擾。\$\@\$指揮中心指出，有關7月13號以後針對部分場所將適度鬆綁，但仍須遵守防疫相關指引及規範，而此波疫情中，不少個案均為家戶群聚感染，由於室內密切接觸風險較高，因此對於室內社交人數須有較嚴格規範，但不包含原本同住的家人，也無需限制同住家人不能在家打麻將、看電影、吃飯等。 圖片 附件\$\@\$0710指揮中心：勿輕信「三級警戒微解封的不可思議之處」之網傳.jpg</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-13\$\@\$近日有網友在臉書FB以自製圖文方式散布「政府讓人民施打未受認證且保護力低之國產疫苗」、「國產疫苗的中和抗體效價比國外疫苗差」、「國產疫苗為什麼不向國際提出緊急授權」，中央流行疫情指揮中心(下稱指揮中心)今（13）日嚴正澄清表示，目前國產疫苗臨床試驗尚在進行中，最終結果須等廠商提出EUA 申請，經專家會議審查疫苗的製程管控、藥毒理試驗及臨床試驗結果，在緊急公衛的需求下，確認疫苗使用效益大於風險，才會核准緊急授權使用。\$\@\$指揮中心指出，目前國產疫苗廠商皆已積極規劃，以取得國際認證為目標。國產疫苗需經食藥署和專家會議嚴謹審查，在緊急公衛需求，並確認效益大於風險，才會核准緊急授權使用。此外，各家廠牌的疫苗所使用的檢驗實驗室及檢驗方式不同且無協和，無法直接由各實驗室產生數值進行比較。國產疫苗仍需等廠商提出申請，經過中央主管機關嚴格把關及審查通過後，確認品質、安全、療效後，品質沒有問題，疫苗方可供民眾施打。\$\@\$指揮中心再次提醒，民眾接獲來源不明的訊息時，應先進行查證，切勿隨意散播、轉傳，以免觸法。 圖片 附件\$\@\$0613網傳「政府讓人民施打未受認證且保護力低之國產疫苗」-1.jpg\$\@\$0613網傳「政府讓人民施打未受認證且保護力低之國產疫苗」-2.jpg</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-12\$\@\$中央流行疫情指揮中心今(12)日嚴正澄清，近日於社群平台流傳「代工三億劑嫌太多賣不出去」等訊息，指揮中心於6月10日記者會已公開說明，與AstraZeneca原廠洽談授權製造事宜時，我方提出可年產一億劑之規劃，但原廠要求需年產三億劑，經評估，對我方產能過於沉重，並無以「賣不出去」為由拒絕原廠授權製造，卻被有心人刻意扭曲語意。此圖文與事實不符，指揮中心特此澄清。\$\@\$指揮中心重申，防疫相關資訊應以中央流行疫情指揮中心公布內容為主。提醒民眾，收到來路不明訊息多加留意、查證，切勿轉傳散播。詳情請上官網查詢 (http://at.cdc.tw/Q7S2Vt)。 圖片 附件\$\@\$20210612澄清.jpg</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-06-01\$\@\$中央流行疫情指揮中心今(1)日指出，近日有網友在通訊軟體LINE散布「臺中市太原路復健醫院被徵收為方艙醫院」，臺中市政府衛生局已澄清為不實訊息，請民眾勿再轉傳與散布，以免觸法遭罰。\$\@\$指揮中心表示，臺中市政府已對外澄清，此復健醫院近期進行搬遷作業，是為了提升醫療品質，正以BOT方式規劃市立綜合醫院，並非徵用作為方艙醫院。\$\@\$指揮中心副指揮官陳宗彥指出，因應疫情變化，各地方政府規劃應變醫院及專責醫院收治患者，民眾接獲來源不明的訊息時，應先進行查證，切勿隨意散播、轉傳，以免觸法。\$\@\$指揮中心重申，防疫相關資訊應以中央流行疫情指揮中心公布內容為主，散播假訊息構成犯罪，會被判處最高三年有期徒刑或併科三百萬元罰金。提醒民眾，收到來路不明訊息多加留意、查證，切勿轉傳散播，以免觸法。詳情請上官網查詢(http://at.cdc.tw/Q7S2Vt)。 圖片 附件\$\@\$網傳「臺中市太原路復健醫院被徵收為方艙醫院」為不實訊息勿轉傳.jpg\$\@\$勿散播不實訊息，以免觸法受罰.jpg</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-05-28\$\@\$近期國內疫情升溫，警方發現網路上有不肖人士販售「新冠病毒快篩試劑」，中央流行疫情指揮中心副指揮官陳宗彥今(28)日表示，擅自在網路販售新冠病毒檢驗試劑等第三級醫療器材已違反「醫療器材管理法」，目前警方已進行偵辦，提醒民眾切勿購買檢測，除有效性及檢測結果正確性均無法確認外，還可能危害自身健康。\$\@\$指揮中心指出，新冠病毒檢驗試劑是第三級醫療器材，依據「醫療器材管理法」規定，只有醫療器材商及藥局可以販賣，且國內並未開放可使用通訊方式在網路、電話、社群媒體等販售。\$\@\$指揮中心強調，不肖人士在網路擅自販售專案核准的新冠病毒檢驗試劑已違「醫療器材管理法」，會被罰3萬以上100萬以下罰鍰，如果民眾發現有類似狀況，可打1919專線或是向地方衛生局檢舉。 圖片 附件\$\@\$0528網路販售「新冠病毒快篩試劑」已觸法，警方偵辦中.jpg\$\@\$勿散播不實訊息，以免觸法受罰.jpg</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-05-25\$\@\$中央流行疫情指揮中心今(25)日表示，近日網路出現偽冒教育部網站，杜撰「全國各級學校因應疫情停課時程資訊」等訊息，意圖造成民眾困惑，此為境外假網頁不實訊息，請民眾勿輕信。\$\@\$指揮中心副指揮官陳宗彥表示，該網站假冒教育部傳達不實防疫訊息，刑事警察局已成立專案小組偵辦，經調查其為境外IP。\$\@\$指揮中心指出，教育部全球資訊網正確的網址是https://www.edu.tw/ ，民眾收到任何連結時，可以先觀察連結網址，是否跟官方網址一樣。例如，教育部官方網址的網域，就會是「edu.tw」結尾。\$\@\$指揮中心強調，散播假訊息構成犯罪，會被判處最高三年有期徒刑或併科三百萬元罰金。提醒民眾，收到來路不明訊息多加留意、查證，切勿轉傳散播，以免觸法。 圖片 附件\$\@\$0525指揮中心指出，網路出現偽冒教育部網站並杜撰假訊息，請民眾勿輕信.jpg\$\@\$勿散播不實訊息，以免觸法受罰.jpg</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-28\$\@\$各位醫界朋友，您好：\$\@\$全球疫情持續嚴峻，Omicron變異株現已為全球與國內主要流行病毒株，由於其具有多個基因變異位點，可能影響部分治療藥物效果，COVID-19專家諮詢會審視國內外最新實證後，統整對Omicron變異株藥物使用建議如下：\$\@\$1. 不需使用氧氣且具重症風險因子之COVID-19病患：\$\@\$(1)建議可使用remdesivir靜脈注射三日療程，或nirmatrelvir + ritonavir (Paxlovid)口服五日，未住院病患建議優先選擇口服藥物治療。若上述兩種藥物均不適用，則可使用molnupiravir (Lagevrio)口服五日。臨床醫師可評估病患情況後，依本署公告之領用方案及注意事項申請使用；另因缺乏實證與安全性資料，不建議同時併用remdesivir和口服抗病毒藥物。\$\@\$(2)我國目前儲備之兩種複合式anti-SARS-CoV-2單株抗體(casirivimab + imdevimab, bamlanivimab + etesevimab)，因體外試驗顯示對Omicron變異株中和能力大幅下降，可能影響臨床效果，故除非已確認上述單株抗體對患者感染之變異株仍有效，否則不建議使用，使用前務必參閱最新版「新型冠狀病毒（SARS-CoV-2）感染臨床處置暫行指引」中「單株抗體對SARS-CoV-2變異株效果實證」表格。\$\@\$2.需吸氧治療、高流量氧氣、非侵襲性呼吸器或插管病患：\$\@\$目前證據顯示，Omicron變異株不影響dexamethasone、tocilizumab、baricitinib與remdesivir對此類病人之療效，故維持現行治療建議。\$\@\$面對社區疫情，指揮中心提醒臨床醫師提高警覺，對有疑似症狀患者加強採檢，以早期偵測疫情。另目前針對不同嚴重程度COVID-19病患均已有治療藥物可選用，用藥前請參閱最新版「新型冠狀病毒（SARS-CoV-2）感染臨床處置暫行指引」中個別藥物說明。\$\@\$「嚴重特殊傳染性肺炎」之診療相關資訊將隨時依防疫需求與最新文獻證據更新並公布於疾病管制署全球資訊網(http://www.cdc.gov.tw)。\$\@\$感謝您與我們共同維護全民的健康安全。 附件\$\@\$診治指引表四＿我國診治指引對SARS-CoV-2確診病患用藥建議彙整.pdf\$\@\$診治指引表五＿單株抗體對SARS-CoV-2變異株效果實證.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-26\$\@\$各位醫界朋友，您好：\$\@\$為積極因應新型冠狀病毒疾病疫情防疫需求，衛生福利部食品藥物管理署於評估療效、安全性、風險效益與緊急公共衛生需求後，於本(111)年1月12日與1月15日分別核准兩種口服抗病毒藥物專案輸入，經COVID-19專家諮詢會檢視最新實證後，於臨床處置暫行指引中新增口服抗病毒藥物使用建議如下：\$\@\$新增nirmatrelvir + ritonavir(Paxlovid)適用對象為具以下任一重症風險因子，未使用氧氣且於發病五天內之 ≧ 12歲且體重 ≧ 40公斤病患；風險因子包括年齡 ≧ 65歲、糖尿病、慢性腎病、心血管疾病(含高血壓)、慢性肺疾、BMI ≧ 25 (或12-17歲兒童青少年BMI 超過同齡第85百分位)、其他影響免疫功能之疾病或已知重症風險因子者。建議劑量為Nirmatrelvir 300 mg + ritonavir 100 mg 每日兩次口服，療程共五天。使用時須特別注意藥物交互作用及肝腎功能異常時之建議，並確實完成五天療程。\$\@\$新增molnupiravir(Lagevrio)適用對象為具以下任一重症風險因子，未使用氧氣且於發病五天內之 ≧ 18歲病患，且無法使用其他建議藥物者；風險因子包括年齡 ≧ 65歲、糖尿病、慢性腎病、心血管疾病(含高血壓)、慢性肺疾、BMI ≧ 25、其他影響免疫功能之疾病或已知重症風險因子者。建議劑量為molnupiravir 800mg每日兩次口服，療程共五天。\$\@\$目前針對未使用氧氣且具重症風險因子之COVID-19病患，專家諮詢小組建議可使用藥物包括remdesivir、nirmatrelvir + ritonavir與兩種複合式anti-SARS-CoV-2單株抗體(casirivimab + imdevimab, bamlanivimab + etesevimab)，臨床醫師可評估病患病況與變異株流行情形後，依本署公告流程申請使用；若病患不適用上述藥物，則可申請使用molnupiravir。\$\@\$「嚴重特殊傳染性肺炎」之診療相關資訊將隨時依防疫需求與最新文獻證據更新並公布於疾病管制署全球資訊網(http://www.cdc.gov.tw)。\$\@\$感謝您與我們共同維護全民的健康安全。 附件\$\@\$附件1＿新型冠狀病毒（SARS-CoV-2）感染臨床處置暫行指引第十六版.pdf\$\@\$附件2_公費COVID-19治療用口服抗病毒藥物領用方案_1110126制定.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-10-22\$\@\$各位醫界朋友，您好：\$\@\$我國新型冠狀病毒(SARS-CoV-2)感染臨床處置暫行指引建議可依照病患病程與嚴重度，對不需用氧且有重症風險因子之病患給予單株抗體，需用氧病患則除dexamethasone外可併用免疫調節劑tocilizumab或baricitinib。鑒於近期國際間藥物使用建議與國內適應症均有更新，經COVID-19專家諮詢會議更新建議如下：\$\@\$1.複合單株抗體Casirivimab + imdevimab或Bamlanivimab + etesevimab。適用對象為\$\@\$― 具以下任一風險因子，未使用氧氣且於發病十天內之≧12歲且體重≧40公斤病患；\$\@\$― 風險因子包括：年齡 ≧ 65歲、糖尿病、慢性腎病、心血管疾病（含高血壓）、慢性肺疾、BMI ≧25（或12-17歲兒童BMI超過同齡第85百分位）、懷孕、其他影響免疫功能之疾病或已知重症風險因子等。\$\@\$目前實證顯示上述兩種複合單株抗體對國內現今主要檢出之Delta與Alpha變異株均有效，但由於體外試驗顯示Bamlanivimab + etesevimab可能無法有效中和包括Beta、Gamma、Delta plus與Mu變異株，建議臨床醫師使用時需考量流行狀況與參閱最新版「SARS-CoV-2之藥物使用實證摘要」附表。\$\@\$另參考WHO最新公布治療建議，於診治指引註解中新增「隨機對照研究顯示對血清抗體陰性之嚴重肺炎以上程度病患，除標準治療外，給予casirivimab 4000mg + imdevimab 4000mg 可降低死亡率」。\$\@\$2.Remdesivir適用對象為嚴重肺炎以上（未使用吸氧治療下的SpO2 ≦ 94%、需使用吸氧治療、需使用高流量氧氣或非侵襲性呼吸器但未插管）病患。另於診治指引註解中新增「若住院病患胸部X光片顯示肺炎，雖未達重症標準且不符合單株抗體適用條件，仍可申請使用remdesivir」。但由於目前尚無併用單株抗體之效益與安全性資料，目前仍暫不建議remdesivir與單株抗體同時併用。\$\@\$由於近日媒體報導ivermectin用於治療COVID-19一事，經專家委員審視國際文獻，發現ivermectin相關臨床試驗研究證據力等級低，且部分研究涉及科學誠信，其中亦有發表論文被撤回之情形，統合分析結果顯示目前證據不支持ivermectin可用於治療或預防COVID-19，WHO及歐美等具公信力之治療指引均不建議使用於COVID-19之治療。為確保國人健康，我國診治指引治療藥物建議係根據最高等級實證基礎制訂，參考目前各方面之資料，仍不建議ivermectin納入我國診治指引之治療建議藥物。\$\@\$「嚴重特殊傳染性肺炎」之診療相關資訊將隨時依防疫需求與最新文獻證據更新並公布於疾病管制署全球資訊網(http://www.cdc.gov.tw)。\$\@\$感謝您與我們共同維護全民的健康安全。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-28\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$疫情中心\$\@\$約用助理\$\@\$(徵才案號：0605，含延長公告)\$\@\$(計4名)\$\@\$姚○雯(A22649****)\$\@\$盧○淳(A22626****)\$\@\$邱○柔(A22582****)\$\@\$莊○媛(R22426****)\$\@\$二、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一)口試：\$\@\$1、報到時間：111年02月09日星期三15:20~15:30，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署1樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：15:30~17:00。\$\@\$(二)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(三)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於111年02月09日上午10點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3864)，俾利安排應試座位。\$\@\$(四)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(五)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-12\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$檢疫組\$\@\$約用助理\$\@\$(徵才案號：0507)\$\@\$(計4名)\$\@\$陳○涵(A22534****)\$\@\$張○純(A22889****)\$\@\$林○翔(S12427****)\$\@\$謝○樺(K12260****)\$\@\$二、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一) 口試：\$\@\$1、報到時間：111年01月17日星期一15:20~15:30，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署7樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：15:30~16:40。\$\@\$(二)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(三)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於111年01月17日上午10點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3864)，俾利安排應試座位。\$\@\$(四)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(五)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-24\$\@\$一、考評單位：衛生福利部疾病管制署。\$\@\$二、考評目的：客觀衡量地方政府衛生局111年防疫業務之施政績效。\$\@\$三、受評機關：地方政府衛生局。\$\@\$四、受評期間：111年1月至12月\$\@\$五、考評架構與權重：9項考評指標，共計200分。\$\@\$六、考評方式：\$\@\$(一)   防疫業務相關管理系統之統計結果及書面考核。\$\@\$本手冊考評指標資料，如須受評機關提供始得評分者，請於112年1月13日前備函逕送考評執行單位進行評核。\$\@\$考評單位於指定日期前完成分數統計及成績評定。\$\@\$考評單位完成考評並請地方政府衛生局確認後，於111年3月17日前將考評結果送衛生福利部綜合規劃司備查。\$\@\$(二)   考評單位得視需要辦理實地查核。 附件\$\@\$111年地方衛生機關業務考評作業手冊-防疫類.pdf\$\@\$111年地方衛生機關業務考評作業手冊-防疫類.docx</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-24\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$慢性傳染病組\$\@\$約用助理\$\@\$(徵才案號：0309)\$\@\$(計3名)\$\@\$林○萱(B22260****)\$\@\$陳○瑜(Q22389****)\$\@\$陳○君(F22674****)\$\@\$二、實作、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一)實作：\$\@\$1、報到時間：111年1月7日星期五13:20。\$\@\$2、報到地點：衛生福利部疾病管制署1樓(臺北市中正區林森南路6號)。\$\@\$3、實作時間：13:40~15:10。實作開始鈴響(13:40)未到者，喪失應考資格。\$\@\$(二)口試：\$\@\$1、報到時間：111年1月7日星期五15:20，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署1樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：15:30~16:30。\$\@\$(三)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(四)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於111年1月6日下午5點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3823)，俾利安排應試座位。\$\@\$(五)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(六)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。\$\@\$三、試場規則：\$\@\$(一)第一試為實作測驗，題型為資料串接統計分析，應試者得自行攜帶筆記型電腦，並預先安裝欲於測驗時使用的統計分析軟體(可選擇使用SAS、R、Excel等其他統計分析軟體)；未自行攜帶筆記型電腦者，則由本署提供公務電腦於測驗時使用(僅具Excel功能且無法安裝軟體)。\$\@\$(二)測驗中途不容許離場，並於考試時間過半後始得離場，離場後不得再進入試場。\$\@\$(三)測驗期間不允許上網、隨身攜帶手機(含智慧手環)、行動網卡、無線網路分享器等電子用品，並請關閉網路、手機、聲音及振動(含鬧鐘)，考試過程中如有上網、發出聲音及震動，均喪失應考資格。\$\@\$(四)個人用品(如書包等)置於考場前後，桌面上僅可放置必要文具(墊板須為透明；水杯、飲料亦禁止放置)。\$\@\$(五)有下列各款情事之一者，予以扣考並不予計分或不得繼續應考：\$\@\$1、冒名頂替。\$\@\$2、持用偽造或變造之證件。\$\@\$3、互換座位或試卷。\$\@\$4、傳遞文稿、參考資料、書寫有關文字之物件或有關信號。\$\@\$5、夾帶書籍文件。\$\@\$6、故意不繳交試卷或破壞試卷彌封。\$\@\$7、在桌椅、文具或肢體上或其他處所，書寫有關文字。\$\@\$8、電子通訊舞弊行為。\$\@\$9、窺視他人試卷、答案卷、作答結果或互相交談。\$\@\$10、在答案卷上書寫姓名、座號或其他不應有之文字、標記或自備稿紙書寫。\$\@\$11、其他破壞試場秩序事項。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
   </si>
   <si>
     <t>發佈日期：2022-01-24\$\@\$中央流行疫情指揮中心今(24)日表示，因應國際疫情嚴峻，且國內發生新變異株Omicron感染事件，經指揮中心與相關單位溝通及評估後於今日宣布，今(2022)年1月25日至2月7日維持疫情警戒標準為第二級，調整或維持相關措施及規定如下：\$\@\$一、維持加嚴之戴口罩規定，除少數例外情形，外出全程佩戴口罩：\$\@\$(一)運動、唱歌、拍照及直播、錄影、主持、報導、致詞、演講、講課等談話性質工作或活動之正式拍攝或進行時，恢復為須戴口罩。\$\@\$(二)下列場合得免戴口罩，但應隨身攜帶口罩，且如本身有相關症狀或與不特定對象無法保持社交距離時，仍應戴口罩：\$\@\$1. 農林漁牧工作者於空曠處(如：田間、魚塭、山林)工作。\$\@\$2. 於山林(含森林遊樂區)、海濱活動。\$\@\$3. 於溫/冷泉、烤箱、水療設施、三溫暖、蒸氣室、水域活動等易使口罩潮濕之場合。\$\@\$(三)外出時有飲食需求，得免戴口罩。\$\@\$(四)於指揮中心或主管機關指定之場所或活動(例如：藝文表演/劇組/電視主播等演出人員正式拍攝演出時、運動競賽之參賽選手及裁判於比賽期間等)，如符合指揮中心或主管機關之相關防疫措施，得暫時脫下口罩。\$\@\$二、營業場所及公共場域(含交通運輸)應嚴格遵守：實聯制、量體溫、加強環境淸消、員工健康管理、確診事件即時應變。\$\@\$三、高鐵、臺鐵、公路客運、船舶(固定餐飲區除外)、國內航班：於運具內（車廂、船舶、航空器）禁止飲食。\$\@\$四、賣場、超市、市場加強人流管制：室內空間至少1.5米/人(2.25平方米/人)，室外空間至少1米/人(1平方米/人)；不開放試吃。\$\@\$五、宗教場所、宗教集會活動：依內政部規定之防疫措施辦理。\$\@\$六、餐飮場所：嚴格落實實聯制、量體溫、提供洗手設備及消毒用品；宴席不得逐桌敬酒敬茶；違反者依法裁處並限期改善，未完成改善者，不得提供內用服務。\$\@\$指揮中心呼籲，防疫工作人人有責，請民眾自主落實防疫措施，維持個人衛生好習慣，戴口罩、勤洗手、保持社交距離；出入公共場域落實實聯制、體溫量測等，降低病毒傳播風險，保護自己也保護他人，共同維護國內社區安全。</t>
@@ -481,37 +511,10 @@
     <t>發佈日期：2022-01-22\$\@\$中央流行疫情指揮中心今(22)日公布國內新增130例COVID-19確定病例，分別為82例本土個案及48例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為12例男性、70例女性，年齡介於未滿10歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為29例男性、19例女性，年齡介於未滿5歲至70多歲，分別自美國(13例)、加拿大及新加坡(各4例)、菲律賓(3例)、印度、土耳其及香港(各2例)、奧地利、奈及利亞、義大利、柬埔寨、德國、越南及巴西(各1例)移入；另11例調查中。入境日介於去(2021)年12月31日至今(2022)年1月21日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,418,957例新型冠狀病毒肺炎相關通報(含5,400,086例排除)，其中18,238例確診，分別為3,331例境外移入，14,853例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案18182，再次採檢為陰性，改判排除)，累計117例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月22日新增本土COVID-19確診個案表.pdf\$\@\$1月22日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-21\$\@\$中央流行疫情指揮中心今(21)日公布國內新增68例COVID-19確定病例，分別為23例本土個案及45例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為10例男性、13例女性，年齡介於未滿10歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為20例男性、24例女性及1例調查中，年齡介於未滿5歲至70多歲，分別自美國(17例)、菲律賓(4例)、越南及以色列(各3例)、加拿大(2例)、波蘭、澳大利亞、韓國、新加坡、瑞典、俄羅斯、英國及愛爾蘭(各1例)移入；另8例調查中。入境日介於今(2022)年1月5日至1月20日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,394,042例新型冠狀病毒肺炎相關通報(含5,375,246例排除)，其中18,109例確診，分別為3,283例境外移入，14,772例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計116例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月21日新增本土COVID-19確診個案表.pdf\$\@\$1月21日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-20\$\@\$中央流行疫情指揮中心今(20)日表示，我國「數位新冠病毒健康證明」自去(110)年12月28日上線後已核發超過26萬份。考量國內外疫情升溫，各界建議及需求，指揮中心將於今(111)年1月21日上午8時開放「數位新冠病毒健康證明」供國內使用，共計三大功能：所有在國內接種者皆可下載、符合歐盟規範的查驗程式，可驗證60國的證明、提供具實名制的APP作為證明載具。\$\@\$指揮中心指出，原本下載限持有效護照者，現以戶口名簿的戶號取代，民眾可以電腦或手機上網申辦「數位新冠病毒健康證明」（ https://dvc.mohw.gov.tw ），注意事項說明如下：\$\@\$一、確認身分：\$\@\$(一)國人：(1)身分證號+健保卡號+戶口名簿戶號；(2) FIDO；(3)自然人憑證。三種方式擇一。\$\@\$(二)外來人口：(1)統一證號+健保卡號；(2) 統一證號+入出境證號；(3) 統一證號+護照號碼。三種方式擇一。\$\@\$二、選擇項目：選擇「疫苗接種數位證明」或「檢驗結果數位證明」。\$\@\$三、取得證明：於申請成功畫面點選「下載/列印 數位證明」，檔案格式為PDF，提醒要先保存於行動裝置或電腦硬碟中，再視個人需要列印紙本。無列印設備但又有列印需求者，可於申請成功畫面選擇超商並點選「取得超商列印碼」，系統將產製超商取件條碼或取件編號，請自行攜碼至超商付費列印。\$\@\$此次僅變更確認身分方式，方便未持有護照者下載。具有效護照民眾申辦數位證明時仍會產出護照號碼，未來不必為出國另行下載；不具有效護照民眾者護照號碼欄位顯示為「Not Issued」。\$\@\$「數位新冠病毒健康證明」查驗程式係網頁形式（ https://dvc.mohw.gov.tw/verifier-web ），不需下載安裝，民眾也可在衛福部官網取得連結，該網頁不會保留受查驗者的個資，符合歐盟GDPR，使用步驟如下：\$\@\$一、前往網站：使用具備相機及網頁瀏覽器的手機、電腦等，開啟瀏覽器前往上述網址。\$\@\$二、同意隱私權聲明、允許取用相機權限。\$\@\$三、不退出查驗網頁且不中斷網路者，可續使用並維持最新功能，退出或中斷者可重新上網更新。\$\@\$查驗程式以顏色、圖示及文字顯示查驗結果，綠色、打勾為通過，紅色、打叉為不通過，黃色、三角驚嘆號為待確認狀態（包括：接種不完整、效期不符、非我國同意的疫苗或檢驗等），不合規格的QR code則會出現解析錯誤的訊息。驗證程式個人基本資料僅會顯示姓名及出生年月日，如需嚴格確認是否為本人持有，建議仍需搭配其它身分證件。由於我國已是歐盟數位新冠證明(EU-DCC)的成員，故本查驗程式也可查證持同樣規格由其它國家發行的疫苗、核酸檢驗數位證明，及部分有發行康復證明的國家。\$\@\$指揮中心提醒，依據世界衛生組織(WHO)規範，疫苗證明可採紙本或數位方式，檢驗陰性或康復證明亦可做為健康證明，數位證明僅是方式之一，民眾有多元方式可提供各場所查驗。\$\@\$另外，指揮中心亦已備有標準的應用軟體介接程式(API)供國內具實名制功能的APP介接取得民眾自己的數位證明，並以APP為載具。發行或管理APP者，確認符合個資法及GDPR、身分驗證強度不低於本數位證明平臺，且APP後臺不得留存數位證明，請向指揮中心正式申請。\$\@\$為更新原有版本的功能，申辦平台預計今年1月20日下午5時至次(21)日上午8時停止服務進行更版，有急需出國使用者，請先提前下載。詳細下戴及驗證系統操作方式可以參考衛生福利部官網數位證明專區( https://covid19.mohw.gov.tw/ch/np-5345-205.html )。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-07-10\$\@\$中央流行疫情指揮中心今（10）日表示，近日有網友散布「三級警戒微解封的不可思議之處，新冠肺炎病毒只會攻擊家人」等訊息，相關內容多有誤導，且在錯誤基礎上進行不當類比，指揮中心再次強調，相關防疫指引已清楚說明，原本同住家人可以繼續維持生活，相關指引都是針對日常非同住者間的行為互動加以規範，呼籲民眾勿輕信或隨意散播、轉傳錯誤訊息，造成防疫困擾。\$\@\$指揮中心指出，有關7月13號以後針對部分場所將適度鬆綁，但仍須遵守防疫相關指引及規範，而此波疫情中，不少個案均為家戶群聚感染，由於室內密切接觸風險較高，因此對於室內社交人數須有較嚴格規範，但不包含原本同住的家人，也無需限制同住家人不能在家打麻將、看電影、吃飯等。 圖片 附件\$\@\$0710指揮中心：勿輕信「三級警戒微解封的不可思議之處」之網傳.jpg</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-05-25\$\@\$中央流行疫情指揮中心今(25)日表示，近日網路出現偽冒教育部網站，杜撰「全國各級學校因應疫情停課時程資訊」等訊息，意圖造成民眾困惑，此為境外假網頁不實訊息，請民眾勿輕信。\$\@\$指揮中心副指揮官陳宗彥表示，該網站假冒教育部傳達不實防疫訊息，刑事警察局已成立專案小組偵辦，經調查其為境外IP。\$\@\$指揮中心指出，教育部全球資訊網正確的網址是https://www.edu.tw/ ，民眾收到任何連結時，可以先觀察連結網址，是否跟官方網址一樣。例如，教育部官方網址的網域，就會是「edu.tw」結尾。\$\@\$指揮中心強調，散播假訊息構成犯罪，會被判處最高三年有期徒刑或併科三百萬元罰金。提醒民眾，收到來路不明訊息多加留意、查證，切勿轉傳散播，以免觸法。 圖片 附件\$\@\$0525指揮中心指出，網路出現偽冒教育部網站並杜撰假訊息，請民眾勿輕信.jpg\$\@\$勿散播不實訊息，以免觸法受罰.jpg</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-06\$\@\$為提供結核病患即時診斷，疾病管制署結核病診治指引自104年已加重結核分枝桿菌核酸增幅(nucleic acid amplification, NAA)檢驗於診斷結核病之角色。NAA檢驗具快速、高敏感度及高特異性，可大幅縮短傳統培養檢驗方法所需等待結果時間，有利及早診斷及治療結核病。\$\@\$因應近期結核菌液態培養(MGIT)檢驗發生添加劑(營養劑併抑制細菌生長的抗生素成分)供貨短缺情形，為避免延遲發現疑似結核病個案，依本署110年12月24日「衛生福利部傳染病防治諮詢會(結核病防治組)」會議決議，於供貨短缺期間，對於社區型肺炎尚未通報結核病者，於診斷送驗3套初查痰執行塗片耐酸性染色鏡檢(Acid fast stain)及分枝桿菌培養時，其中1套請務必同時開立NAA檢驗。另考量實驗室短期內MGIT痰培養試劑有限，對於管理中的結核病患追蹤複查痰，請採1套進行培養檢驗，暫時避免重複送驗檢體，此因應作為停止施行時間將於缺貨狀況緩解後再函週知。\$\@\$有關「結核病診治指引」可至疾病管制署全球資訊網(https://www.cdc.gov.tw)&gt;傳染病與防疫專題&gt;傳染病介紹&gt;第三類定傳染病&gt;結核病&gt;重要指引及教材項下查閱。\$\@\$感謝您與我們共同維護全民的健康安全。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-12-30\$\@\$各位醫界朋友，您好：\$\@\$鑑於國際COVID-19疫情嚴峻及Omicron新型變異株威脅增加，嚴重特殊傳染性肺炎中央流行疫情指揮中心(下稱指揮中心)邀請各縣市兒科、內科、家醫科、耳鼻喉科及婦產科等有提供診治呼吸道症狀服務之診所/衛生所，自明(2022)年1月1日起加入公費COVID-19家用快篩試劑發放行列，指揮中心感謝基層診所積極守護社區健康的熱誠，並籲請各定點診所醫師針對具呼吸道症狀就醫民眾，加強發放公費COVID-19家用快篩試劑。\$\@\$指揮中心於今(2021)年8月30日起啟動前揭計畫，全國共計18個縣市86家診所/衛生所參加，迄今已發放1萬餘劑公費COVID-19家用快篩試劑，於有效監測下均無發現陽性個案。為提升民眾取用COVID-19家用快篩試劑可近性及擴大監測，自明年1月1日起增加至21個縣市272家診所/衛生所參與。\$\@\$由於國內現處於流感季節且COVID-19症狀與上呼吸道感染症狀相似，指揮中心籲請定點診所針對出現呼吸道症狀就醫民眾，加強發放公費COVID-19家用快篩試劑，尤可對於幼兒及其陪病家屬加強評估發放；另請診所衛教民眾試劑使用流程及注意事項、提醒民眾匿名填寫線上問卷以回報快篩結果等資料，並將發放民眾資料登錄於疾病管制署系統中。\$\@\$該計畫相關內容公布於疾病管制署全球資訊網 (http://www.cdc.gov.tw) COVID-19防疫專區&gt;臺灣社交距離APP及採檢地圖&gt;COVID-19社區加強監測方案，歡迎查閱。\$\@\$感謝您與我們共同維護全民的健康安全。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-10-22\$\@\$各位醫界朋友，您好：\$\@\$我國新型冠狀病毒(SARS-CoV-2)感染臨床處置暫行指引建議可依照病患病程與嚴重度，對不需用氧且有重症風險因子之病患給予單株抗體，需用氧病患則除dexamethasone外可併用免疫調節劑tocilizumab或baricitinib。鑒於近期國際間藥物使用建議與國內適應症均有更新，經COVID-19專家諮詢會議更新建議如下：\$\@\$1.複合單株抗體Casirivimab + imdevimab或Bamlanivimab + etesevimab。適用對象為\$\@\$― 具以下任一風險因子，未使用氧氣且於發病十天內之≧12歲且體重≧40公斤病患；\$\@\$― 風險因子包括：年齡 ≧ 65歲、糖尿病、慢性腎病、心血管疾病（含高血壓）、慢性肺疾、BMI ≧25（或12-17歲兒童BMI超過同齡第85百分位）、懷孕、其他影響免疫功能之疾病或已知重症風險因子等。\$\@\$目前實證顯示上述兩種複合單株抗體對國內現今主要檢出之Delta與Alpha變異株均有效，但由於體外試驗顯示Bamlanivimab + etesevimab可能無法有效中和包括Beta、Gamma、Delta plus與Mu變異株，建議臨床醫師使用時需考量流行狀況與參閱最新版「SARS-CoV-2之藥物使用實證摘要」附表。\$\@\$另參考WHO最新公布治療建議，於診治指引註解中新增「隨機對照研究顯示對血清抗體陰性之嚴重肺炎以上程度病患，除標準治療外，給予casirivimab 4000mg + imdevimab 4000mg 可降低死亡率」。\$\@\$2.Remdesivir適用對象為嚴重肺炎以上（未使用吸氧治療下的SpO2 ≦ 94%、需使用吸氧治療、需使用高流量氧氣或非侵襲性呼吸器但未插管）病患。另於診治指引註解中新增「若住院病患胸部X光片顯示肺炎，雖未達重症標準且不符合單株抗體適用條件，仍可申請使用remdesivir」。但由於目前尚無併用單株抗體之效益與安全性資料，目前仍暫不建議remdesivir與單株抗體同時併用。\$\@\$由於近日媒體報導ivermectin用於治療COVID-19一事，經專家委員審視國際文獻，發現ivermectin相關臨床試驗研究證據力等級低，且部分研究涉及科學誠信，其中亦有發表論文被撤回之情形，統合分析結果顯示目前證據不支持ivermectin可用於治療或預防COVID-19，WHO及歐美等具公信力之治療指引均不建議使用於COVID-19之治療。為確保國人健康，我國診治指引治療藥物建議係根據最高等級實證基礎制訂，參考目前各方面之資料，仍不建議ivermectin納入我國診治指引之治療建議藥物。\$\@\$「嚴重特殊傳染性肺炎」之診療相關資訊將隨時依防疫需求與最新文獻證據更新並公布於疾病管制署全球資訊網(http://www.cdc.gov.tw)。\$\@\$感謝您與我們共同維護全民的健康安全。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-09-30\$\@\$全國醫界朋友，您好：\$\@\$目前正值登革熱流行期，雖然今（110）年截至目前尚無本土病例，但仍有少數境外移入個案，主要來自越南、菲律賓、印尼及柬埔寨。因登革熱部分症狀與COVID-19相似，籲請各位醫師對於出現疑似症狀之就診民眾，如具登革熱流行地區旅遊史，除考量可能為COVID-19外，亦請適時使用登革熱NS1快速診斷試劑，以及時發現疑似病例。目前國內氣候持續高溫且常有午後雷陣雨，易使病媒蚊密度快速上升，流行風險增加，而近期登革熱通報本土病例數上升且隱藏期平均值超過3日，請各位醫師留意出現登革熱疑似症狀病例，提高通報警覺。\$\@\$由於登革熱個案在發病前1天至發病後5天為具傳染性之病毒血症期，因此及早發現病例並採取相關防疫措施，是有效控制登革熱疫情之關鍵。疾病管制署籲請各位醫師提高警覺，如遇有發燒、頭痛、後眼窩痛、肌肉痛、關節痛、骨頭痛、出疹等（部分個案有腹瀉症狀）疑似登革熱症狀之個案，請務必詢問TOCC，且視需要使用登革熱NS1快速診斷試劑，供作臨床診斷參考，有效減少疑似病例就醫次數及縮短隱藏期，以利採取相關防治措施，防範疫情擴散。\$\@\$感謝您與我們共同維護全民的健康安全。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-12\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$檢疫組\$\@\$約用助理\$\@\$(徵才案號：0507)\$\@\$(計4名)\$\@\$陳○涵(A22534****)\$\@\$張○純(A22889****)\$\@\$林○翔(S12427****)\$\@\$謝○樺(K12260****)\$\@\$二、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一) 口試：\$\@\$1、報到時間：111年01月17日星期一15:20~15:30，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署7樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：15:30~16:40。\$\@\$(二)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(三)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於111年01月17日上午10點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3864)，俾利安排應試座位。\$\@\$(四)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(五)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-12-24\$\@\$一、考評單位：衛生福利部疾病管制署。\$\@\$二、考評目的：客觀衡量地方政府衛生局111年防疫業務之施政績效。\$\@\$三、受評機關：地方政府衛生局。\$\@\$四、受評期間：111年1月至12月\$\@\$五、考評架構與權重：9項考評指標，共計200分。\$\@\$六、考評方式：\$\@\$(一)   防疫業務相關管理系統之統計結果及書面考核。\$\@\$本手冊考評指標資料，如須受評機關提供始得評分者，請於112年1月13日前備函逕送考評執行單位進行評核。\$\@\$考評單位於指定日期前完成分數統計及成績評定。\$\@\$考評單位完成考評並請地方政府衛生局確認後，於111年3月17日前將考評結果送衛生福利部綜合規劃司備查。\$\@\$(二)   考評單位得視需要辦理實地查核。 附件\$\@\$111年地方衛生機關業務考評作業手冊-防疫類.pdf\$\@\$111年地方衛生機關業務考評作業手冊-防疫類.docx</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-12-20\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$公共關係室\$\@\$約用公關助理\$\@\$(徵才案號：0708)\$\@\$(計5名)\$\@\$王○琴(F22546****)\$\@\$李○怡(A22422****)\$\@\$李○達(F12468****)\$\@\$鍾○婷(T22347****)\$\@\$廖○儀(T22036****)\$\@\$二、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一)口試：\$\@\$1、報到時間：110年12月30日星期四09:50~10:00，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署1樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：10:00~11:30。\$\@\$(二)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(三)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於110年12月29日下午5點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3823)，俾利安排應試座位。\$\@\$(四)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(五)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
+    <t>發佈日期：2022-01-21\$\@\$中央流行疫情指揮中心今(21)日表示，台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的第十六批BNT疫苗99.45萬劑，已於今日上午順利運抵桃園國際機場，並在完成通關程序後，直接運送至指定冷儲物流中心進行後續檢驗封緘作業。\$\@\$指揮中心說明，由台積電、鴻海暨永齡基金會、慈濟基金會共同捐贈的BNT疫苗1,500萬劑，目前共計到貨1433.07萬劑，分別為首批9月2日93萬劑、第二批9月9日91萬劑、第三批9月30日54萬劑、第四批10月1日67萬劑、第五批10月4日27萬劑、第六批10月7日88.92萬劑、第七批10月8日88.92萬劑、第八批10月14日82.7萬劑、第九批10月28日90.21萬劑、第十批10月29日91.03萬劑、第十一批11月5日87.17萬劑、第十二批11月12日92.66萬劑、第十三批11月25日93.83萬劑、第十四批12月9日192.35萬劑、第十五批12月30日93.83萬劑，以及本批99.45萬劑。本批疫苗效期至2022年5月25日，將由指揮中心統籌運用，儘速提供民眾接種。\$\@\$對於台積電、鴻海暨永齡基金會、慈濟基金會三間企業和民間團體積極協助，提供更多的疫苗讓民眾接種，加速提升臺灣疫苗覆蓋率，指揮中心再次表達由衷的謝意。</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-20\$\@\$中央流行疫情指揮中心今(20)日表示，鑒於帛琉疫情升溫，為確保社區防疫安全，自帛琉來臺旅客，除搭機前須持二日內核酸檢測報告外，入境仍依現行作法，採綠色專屬通道，並強化相關入境採檢及檢疫措施，請赴帛琉或自帛琉抵臺旅客，務必配合當地及回臺相關防疫及檢疫措施，以保障國內社區安全。\$\@\$指揮中心指出，強化入境採檢及檢疫措施將自今(2022)年1月22日(含)起實施，入境旅客公費入住集中檢疫所實施5天檢疫，接續加強自主健康管理9天，再進行一般自主健康管理7天，並配合入境時(集中檢疫所採檢)、第5天及第13至14天進行PCR檢測，第8天、第11天及一般自主健康管理期滿(第20至21天)以家用快篩試劑各檢測1次。另提醒旅客於到訪帛琉期間，請務必落實自我健康監測，並確實遵守指揮中心及帛國的防疫措施，如佩戴口罩、勤洗手及保持社交距離等規範，以維護自身的健康安全。\$\@\$指揮中心說明，針對1月22日分別有旅遊團啟程至帛琉，以及自帛琉入境旅客，請儘速辦理下列事項：\$\@\$(一) 駐帛琉共和國大使館將持續提供當地疫情風險資訊予交通部觀光局，以利旅行社向旅客宣達該國疫情風險，以及須配合的防疫措施（包括從事醫療照護工作人員，於加強自主健康管理期間不得上班）。\$\@\$(二) 為確保赴帛琉旅客瞭解當地疫情風險，駐帛琉共和國大使館亦將於機場加強宣導。\$\@\$(三) 有關自帛琉入境之14名旅客(含後送轉診病人)，將請駐帛琉共和國大使館轉達調整後的防疫措施，並請醫療應變組瞭解後送轉診病人的就醫需求，以利預先調度。\$\@\$此外，外交部已調整帛琉旅遊警示為「提醒注意」，並將召集交通部與駐帛琉共和國大使館共同研商合理的退費機制。</t>
   </si>
 </sst>
 </file>
@@ -886,7 +889,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E54"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -914,16 +917,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2">
-        <v>44588</v>
+        <v>44589</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -931,16 +934,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="2">
         <v>44588</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -948,16 +951,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="2">
         <v>44588</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -965,13 +968,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" s="2">
-        <v>44587</v>
+        <v>44588</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="E5" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -979,13 +985,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2">
-        <v>44586</v>
+        <v>44587</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
+      </c>
+      <c r="E6" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -993,13 +1002,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="2">
         <v>44586</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
+      </c>
+      <c r="E7" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1007,13 +1019,13 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="2">
-        <v>44586</v>
+        <v>44387</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E8" t="s">
         <v>149</v>
@@ -1024,13 +1036,13 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="2">
-        <v>44586</v>
+        <v>44360</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E9" t="s">
         <v>150</v>
@@ -1041,13 +1053,16 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="2">
-        <v>44586</v>
+        <v>44359</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="E10" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1055,13 +1070,16 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" s="2">
-        <v>44585</v>
+        <v>44348</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
+      </c>
+      <c r="E11" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1069,13 +1087,16 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="2">
-        <v>44585</v>
+        <v>44344</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E12" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1083,13 +1104,16 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="2">
-        <v>44585</v>
+        <v>44341</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
+      </c>
+      <c r="E13" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1097,16 +1121,16 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="2">
-        <v>44585</v>
+        <v>44589</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E14" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1114,16 +1138,16 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="2">
-        <v>44585</v>
+        <v>44587</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E15" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1131,16 +1155,13 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="2">
-        <v>44584</v>
+        <v>44567</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E16" t="s">
-        <v>153</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1148,16 +1169,13 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" s="2">
-        <v>44583</v>
+        <v>44567</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E17" t="s">
-        <v>154</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1165,16 +1183,13 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="2">
-        <v>44582</v>
+        <v>44560</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E18" t="s">
-        <v>155</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1182,13 +1197,16 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="2">
-        <v>44582</v>
+        <v>44491</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
+      </c>
+      <c r="E19" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1196,13 +1214,13 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" s="2">
-        <v>44581</v>
+        <v>44589</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1210,511 +1228,962 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="2">
-        <v>44581</v>
+        <v>44589</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E21" t="s">
-        <v>156</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="C22" s="2">
-        <v>44588</v>
+        <v>44589</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="C23" s="2">
-        <v>44588</v>
+        <v>44589</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E23" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C24" s="2">
-        <v>44588</v>
+        <v>44589</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E24" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="C25" s="2">
-        <v>44587</v>
+        <v>44589</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="C26" s="2">
-        <v>44586</v>
+        <v>44589</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="C27" s="2">
-        <v>44586</v>
+        <v>44589</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C28" s="2">
-        <v>44387</v>
+        <v>44588</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E28" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C29" s="2">
-        <v>44360</v>
+        <v>44588</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C30" s="2">
-        <v>44359</v>
+        <v>44588</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C31" s="2">
-        <v>44348</v>
+        <v>44588</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C32" s="2">
-        <v>44344</v>
+        <v>44589</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>123</v>
+        <v>127</v>
+      </c>
+      <c r="E32" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C33" s="2">
-        <v>44341</v>
+        <v>44574</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E33" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C34" s="2">
-        <v>44587</v>
+        <v>44573</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>125</v>
+        <v>129</v>
+      </c>
+      <c r="E34" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C35" s="2">
-        <v>44567</v>
+        <v>44554</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E35" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C36" s="2">
-        <v>44567</v>
+        <v>44554</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>127</v>
+        <v>131</v>
+      </c>
+      <c r="E36" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C37" s="2">
-        <v>44560</v>
+        <v>44550</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E37" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C38" s="2">
-        <v>44491</v>
+        <v>44585</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E38" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C39" s="2">
-        <v>44469</v>
+        <v>44585</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E39" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C40" s="2">
-        <v>44566</v>
+        <v>44585</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C41" s="2">
-        <v>44565</v>
+        <v>44585</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C42" s="2">
-        <v>43264</v>
+        <v>44585</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>133</v>
+        <v>137</v>
+      </c>
+      <c r="E42" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C43" s="2">
-        <v>44588</v>
+        <v>44584</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
+      </c>
+      <c r="E43" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C44" s="2">
-        <v>44587</v>
+        <v>44583</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>135</v>
+        <v>139</v>
+      </c>
+      <c r="E44" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C45" s="2">
-        <v>44587</v>
+        <v>44582</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C46" s="2">
-        <v>44587</v>
+        <v>44582</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>137</v>
+        <v>141</v>
+      </c>
+      <c r="E46" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C47" s="2">
-        <v>44587</v>
+        <v>44581</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>138</v>
+        <v>142</v>
+      </c>
+      <c r="E47" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="C48" s="2">
-        <v>44586</v>
+        <v>44589</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>139</v>
+        <v>97</v>
+      </c>
+      <c r="E48" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="C49" s="2">
-        <v>44574</v>
+        <v>44588</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>140</v>
+        <v>98</v>
+      </c>
+      <c r="E49" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="C50" s="2">
-        <v>44573</v>
+        <v>44588</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>141</v>
+        <v>99</v>
       </c>
       <c r="E50" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>95</v>
+        <v>54</v>
       </c>
       <c r="C51" s="2">
-        <v>44554</v>
+        <v>44588</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>142</v>
+        <v>100</v>
       </c>
       <c r="E51" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>96</v>
+        <v>55</v>
       </c>
       <c r="C52" s="2">
-        <v>44554</v>
+        <v>44587</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>143</v>
+        <v>101</v>
+      </c>
+      <c r="E52" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="B53" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="C53" s="2">
-        <v>44550</v>
+        <v>44586</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
       <c r="E53" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>98</v>
+        <v>57</v>
       </c>
       <c r="C54" s="2">
-        <v>44515</v>
+        <v>44387</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>145</v>
+        <v>103</v>
+      </c>
+      <c r="E54" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" s="2">
+        <v>44360</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E55" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56" s="2">
+        <v>44359</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E56" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" s="2">
+        <v>44348</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E57" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>15</v>
+      </c>
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+      <c r="C58" s="2">
+        <v>44344</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E58" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59" s="2">
+        <v>44341</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E59" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>17</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60" s="2">
+        <v>44589</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E60" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>18</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" s="2">
+        <v>44587</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" s="2">
+        <v>44567</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>20</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63" s="2">
+        <v>44567</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>21</v>
+      </c>
+      <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64" s="2">
+        <v>44560</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>22</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65" s="2">
+        <v>44491</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E65" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>23</v>
+      </c>
+      <c r="B66" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" s="2">
+        <v>44589</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>24</v>
+      </c>
+      <c r="B67" t="s">
+        <v>70</v>
+      </c>
+      <c r="C67" s="2">
+        <v>44589</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>25</v>
+      </c>
+      <c r="B68" t="s">
+        <v>71</v>
+      </c>
+      <c r="C68" s="2">
+        <v>44589</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>26</v>
+      </c>
+      <c r="B69" t="s">
+        <v>72</v>
+      </c>
+      <c r="C69" s="2">
+        <v>44589</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>27</v>
+      </c>
+      <c r="B70" t="s">
+        <v>73</v>
+      </c>
+      <c r="C70" s="2">
+        <v>44589</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>28</v>
+      </c>
+      <c r="B71" t="s">
+        <v>74</v>
+      </c>
+      <c r="C71" s="2">
+        <v>44589</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>29</v>
+      </c>
+      <c r="B72" t="s">
+        <v>75</v>
+      </c>
+      <c r="C72" s="2">
+        <v>44589</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>30</v>
+      </c>
+      <c r="B73" t="s">
+        <v>76</v>
+      </c>
+      <c r="C73" s="2">
+        <v>44589</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>31</v>
+      </c>
+      <c r="B74" t="s">
+        <v>77</v>
+      </c>
+      <c r="C74" s="2">
+        <v>44588</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>32</v>
+      </c>
+      <c r="B75" t="s">
+        <v>78</v>
+      </c>
+      <c r="C75" s="2">
+        <v>44588</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>33</v>
+      </c>
+      <c r="B76" t="s">
+        <v>79</v>
+      </c>
+      <c r="C76" s="2">
+        <v>44588</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>34</v>
+      </c>
+      <c r="B77" t="s">
+        <v>80</v>
+      </c>
+      <c r="C77" s="2">
+        <v>44588</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>35</v>
+      </c>
+      <c r="B78" t="s">
+        <v>81</v>
+      </c>
+      <c r="C78" s="2">
+        <v>44589</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E78" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>36</v>
+      </c>
+      <c r="B79" t="s">
+        <v>82</v>
+      </c>
+      <c r="C79" s="2">
+        <v>44574</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>37</v>
+      </c>
+      <c r="B80" t="s">
+        <v>83</v>
+      </c>
+      <c r="C80" s="2">
+        <v>44573</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E80" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>38</v>
+      </c>
+      <c r="B81" t="s">
+        <v>84</v>
+      </c>
+      <c r="C81" s="2">
+        <v>44554</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E81" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>39</v>
+      </c>
+      <c r="B82" t="s">
+        <v>85</v>
+      </c>
+      <c r="C82" s="2">
+        <v>44554</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E82" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>40</v>
+      </c>
+      <c r="B83" t="s">
+        <v>86</v>
+      </c>
+      <c r="C83" s="2">
+        <v>44550</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1772,6 +2241,35 @@
     <hyperlink ref="D52" r:id="rId51"/>
     <hyperlink ref="D53" r:id="rId52"/>
     <hyperlink ref="D54" r:id="rId53"/>
+    <hyperlink ref="D55" r:id="rId54"/>
+    <hyperlink ref="D56" r:id="rId55"/>
+    <hyperlink ref="D57" r:id="rId56"/>
+    <hyperlink ref="D58" r:id="rId57"/>
+    <hyperlink ref="D59" r:id="rId58"/>
+    <hyperlink ref="D60" r:id="rId59"/>
+    <hyperlink ref="D61" r:id="rId60"/>
+    <hyperlink ref="D62" r:id="rId61"/>
+    <hyperlink ref="D63" r:id="rId62"/>
+    <hyperlink ref="D64" r:id="rId63"/>
+    <hyperlink ref="D65" r:id="rId64"/>
+    <hyperlink ref="D66" r:id="rId65"/>
+    <hyperlink ref="D67" r:id="rId66"/>
+    <hyperlink ref="D68" r:id="rId67"/>
+    <hyperlink ref="D69" r:id="rId68"/>
+    <hyperlink ref="D70" r:id="rId69"/>
+    <hyperlink ref="D71" r:id="rId70"/>
+    <hyperlink ref="D72" r:id="rId71"/>
+    <hyperlink ref="D73" r:id="rId72"/>
+    <hyperlink ref="D74" r:id="rId73"/>
+    <hyperlink ref="D75" r:id="rId74"/>
+    <hyperlink ref="D76" r:id="rId75"/>
+    <hyperlink ref="D77" r:id="rId76"/>
+    <hyperlink ref="D78" r:id="rId77"/>
+    <hyperlink ref="D79" r:id="rId78"/>
+    <hyperlink ref="D80" r:id="rId79"/>
+    <hyperlink ref="D81" r:id="rId80"/>
+    <hyperlink ref="D82" r:id="rId81"/>
+    <hyperlink ref="D83" r:id="rId82"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20220201
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="141">
   <si>
     <t>Press Title</t>
   </si>
@@ -31,6 +31,9 @@
     <t>Page Content</t>
   </si>
   <si>
+    <t>新增60例COVID-19確定病例，分別為16例本土及44例境外移入</t>
+  </si>
+  <si>
     <t>新增55例COVID-19確定病例，分別為17例本土及38例境外移入</t>
   </si>
   <si>
@@ -49,6 +52,15 @@
     <t>早期偵測國內COVID-19病例，指揮中心持續辦理5大加強監測方案，守護民眾健康</t>
   </si>
   <si>
+    <t>新增48例COVID-19確定病例，分別為15例本土及33例境外移入</t>
+  </si>
+  <si>
+    <t>新增71例COVID-19確定病例，分別為27例本土及44例境外移入</t>
+  </si>
+  <si>
+    <t>新增64例COVID-19確定病例，分別為21例本土及43例境外移入</t>
+  </si>
+  <si>
     <t>網傳「三級警戒微解封的不可思議之處」指揮中心： 原同住家人就不受限制，謠言邏輯誤導且比喻失當，請勿輕信轉傳，造成防疫困擾</t>
   </si>
   <si>
@@ -139,6 +151,9 @@
     <t>公告本署公共關係室約用人員徵才案(徵才案號：0708)初審合格名單及甄試事宜。</t>
   </si>
   <si>
+    <t>/Bulletin/Detail/UA4tEKjcDQRpDuAVBXizlA?typeid=9</t>
+  </si>
+  <si>
     <t>/Bulletin/Detail/e8ugss3YuZ7PixzNURmx2A?typeid=9</t>
   </si>
   <si>
@@ -157,6 +172,15 @@
     <t>/Bulletin/Detail/HlZ1sqsij-X-oDNh5dVIFQ?typeid=9</t>
   </si>
   <si>
+    <t>/Bulletin/Detail/ORzh4yZe1qOnSgVMSnIkVw?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/RBLVTwsQ9Z33zCEe0IMd_Q?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/AaV2iREpabJ8syXu4450Rw?typeid=9</t>
+  </si>
+  <si>
     <t>/Bulletin/Detail/ftv6FPFis84j5uHWTq4lNA?typeid=8772</t>
   </si>
   <si>
@@ -247,6 +271,9 @@
     <t>/Bulletin/Detail/7UJRpdDRbQNIZWyyEfHdHQ?typeid=11</t>
   </si>
   <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/UA4tEKjcDQRpDuAVBXizlA?typeid=9</t>
+  </si>
+  <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/e8ugss3YuZ7PixzNURmx2A?typeid=9</t>
   </si>
   <si>
@@ -265,6 +292,15 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/HlZ1sqsij-X-oDNh5dVIFQ?typeid=9</t>
   </si>
   <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/ORzh4yZe1qOnSgVMSnIkVw?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/RBLVTwsQ9Z33zCEe0IMd_Q?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/AaV2iREpabJ8syXu4450Rw?typeid=9</t>
+  </si>
+  <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/ftv6FPFis84j5uHWTq4lNA?typeid=8772</t>
   </si>
   <si>
@@ -355,22 +391,25 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/7UJRpdDRbQNIZWyyEfHdHQ?typeid=11</t>
   </si>
   <si>
+    <t>發佈日期：2022-02-01\$\@\$中央流行疫情指揮中心今(1)日公布國內新增60例COVID-19確定病例，分別為16例本土個案及44例境外移入(7例為航班落地採檢陽性)；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為7例男性、9例女性，年齡介於未滿5歲至60多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為33例男性、11例女性，年齡介於未滿5歲至50多歲，分別自馬來西亞(20例)、美國(6例)、英國(3例)、日本(2例)、波蘭、菲律賓、越南、巴西、印度、巴拿馬、瑞典及法國(各1例)移入；另5例調查中。入境日介於今(2022)年1月17日至1月31日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,684,887例新型冠狀病毒肺炎相關通報(含5,665,865例排除)，其中18,850例確診，分別為3,715例境外移入，15,081例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另累計127例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$2月1日新增本土COVID-19確診個案表.pdf\$\@\$2月1日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
     <t>發佈日期：2022-01-31\$\@\$中央流行疫情指揮中心今(31)日公布國內新增55例COVID-19確定病例，分別為17例本土個案及38例境外移入(20例為航班落地採檢陽性)；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為8例男性、9例女性，年齡介於未滿10歲至80多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為26例男性、12例女性，年齡介於未滿10歲至70多歲，分別自美國(19例)、中國(2例)、厄瓜多、日本、巴拿馬、比利時、韓國、越南及沙烏地阿拉伯各1例移入；另10例調查中。入境日介於今(2022)年1月14日至1月30日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,673,543例新型冠狀病毒肺炎相關通報(含5,654,537例排除)，其中18,790例確診，分別為3,671例境外移入，15,065例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計127例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月31日新增境外移入COVID-19確診個案表.pdf\$\@\$1月31日新增本土COVID-19確診個案表.pdf</t>
   </si>
   <si>
     <t>發佈日期：2022-01-30\$\@\$鑒於近日本土COVID-19個案多具社區活動史，中央流行疫情指揮中心今（30）日再度說明接觸者匡列原則，亦提醒民眾提高警覺，如未被匡列但疑有可能接觸，主動篩檢。\$\@\$指揮中心指出，如有COVID-19確診個案，地方政府衛生單位人員即會依據相關作業流程前往執行疫情調查及接觸者匡列，以釐清相關活動史與接觸者，必要時由警政單位協助調查個案活動軌跡。衛生單位針對確診個案於可傳染期間參與之各項活動，皆會進行詳細疫調，並依接觸時間及有無適當防護之條件等，評估所有可能接觸人員感染風險後，進行接觸者名單匡列，並通知該等人員依循衛生機關規定執行居家隔離、自主健康管理或自我健康監測等各項防疫措施。\$\@\$指揮中心表示，密切接觸者之隔離措施自110年5月16日起即以1人1室為原則，惟經指揮中心專案核定、地方政府報經指揮中心同意或經地方政府衛生單位評估家中環境不適合者(如：居家隔離者無法有獨立的房間及廁所、住家環境有受病毒汙染之虞且難以即時確實清消，可能有環境汙染造成疾病傳播之風險等)，可公費送集中檢疫所隔離。隔離措施為阻絕病毒傳播重要方法，籲請民眾務必配合、遵守相關規範，共同維護社區安全。</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-30\$\@\$疾病管制署表示，冬季為呼吸道傳染病好發季節，且國際COVID-19疫情嚴峻，國內亦有社區感染出現，適逢春節連續假期，特別提醒民眾應主動做好個人衛生防護措施，並留意健康情形，拜年時以拱手取代握手，生病在家休息，防範病毒傳播的風險。\$\@\$依據疾管署監測資料顯示，歷年急診類流感就診人次於農曆春節期間達到高峰；2019至2021年春節期間(除夕至初五)急診類流感就診人次分別為33,122、39,738、 10,234，其中2021年因COVID-19疫情實施各項防疫措施，就診人次較往年為低，惟仍高於平時就診人次。本流感季(去(2021)年10月1日至今(2022)年1月24日)尚無流感併發重症病例；近四週社區呼吸道病毒分離以單純疱疹病毒及腺病毒為多。\$\@\$疾管署指出，春節期間拜年、出入公共場所及聚餐的機會增加，但許多場所不易保持社交距離，或會近距離接觸不特定對象(不認識的人)的特性，有較高感染及傳播風險，請民眾出入公共場域、餐飲場所等，應主動配合各項防疫措施，務必落實戴口罩，實聯制、體溫量測、勤洗手、咳嗽禮節等個人防護工作，以降低感染風險。\$\@\$至於戶外場所(如戶外風景區、遊樂園、夜市、傳統市場等)，建議業者或場所管理單位採用「人數總量管制」方式進行管控，使民眾在場所或活動中能持續、有效地保持社交距離，並請民眾如有發燒或呼吸道症狀等身體不適時，應避免前往上述場所。\$\@\$疾管署提醒，仍在居家檢疫/隔離的民眾，應遵守相關規定，可透過視訊或電話等方式向親友拜年，不可外出。自主健康管理者，應避免出入無法保持社交距離、或容易近距離接觸不特定人士之公共場所，亦禁止從事近距離或群聚型之活動(如聚餐、聚會、公眾集會…等)；如有發燒或咳嗽、流鼻水等呼吸道症狀、身體不適者，應確實佩戴醫用口罩，儘速就醫，且不得搭乘大眾交通運輸工具；就醫時應主動告知接觸史、旅遊史、職業暴露及身邊是否有其他人有類似症狀；返家後亦應佩戴口罩避免外出，與他人交談時應保持1公尺以上距離。\$\@\$疾管署再次呼籲，防疫工作應由自身做起，籲請民眾維持個人防疫好習慣，戴口罩、勤洗手、保持社交距離；出入公共場域落實實聯制、體溫量測等，才能降低病毒傳播風險，保護自己也保護他人，共同維護國內社區安全。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-29\$\@\$中央流行疫情指揮中心今(29)日表示，因應Omicron新型變異株威脅持續，且國內本土疫情尚未平息，及農曆春節期間國人團聚交流頻繁，社區傳播風險提高，呼籲尚未接種第1、2劑COVID-19疫苗之長者及高風險族群，儘速完成接種，以獲得保護力。\$\@\$指揮中心說明，目前我國COVID-19疫苗接種率第1劑約81%、第2劑約74%，惟75歲以上長者第1劑接種率僅約75%、第2劑接種率僅約68%，仍需再積極提升。為維護長者及高風險族群健康，降低因感染COVID-19造成之重症、住院或死亡風險，提醒尚未接種第1、2劑之長者及其他 COVID-19感染後容易產生嚴重併發症之族群，於其身體狀況較穩定時，請家屬協助陪同至各地方政府衛生局安排或指定之合約醫療院所，儘速完成接種。疫苗接種後可能發生副作用，通常輕微且於數天內消失，並隨年齡層增加而減少，擔心副作用者，可先與醫師討論，經諮詢、評估以選擇合適之疫苗接種。\$\@\$指揮中心表示，為鼓勵18歲以上尚未接種1、2劑COVID-19疫苗者儘速前往接種，延長地方政府提供200元(含)以下衛教品之措施至今(2022)年2月28日止，請民眾踴躍前往接種，以獲得保護力。民眾可透過「COVID-19疫苗防治一網通」( https://antiflu.cdc.gov.tw/Covid19 )或地方政府衛生局公告，查詢鄰近合約醫療院所及其可提供接種之疫苗廠牌與時間，就近前往接種。18歲至未滿20歲民眾，如自行前往接種，請持家長簽具之意願同意書；若由家長陪同前往接種，請本人與家長於現場共同簽署意願同意書。\$\@\$指揮中心提醒，依我國衛生福利部傳染病防治諮詢會預防接種組(ACIP)建議，接種COVID-19疫苗應與流感疫苗等其他疫苗間隔至少7天。另請民眾前往接種COVID-19疫苗前，應備妥健保卡或其他可證明身分之證件，如為接種第2劑COVID-19疫苗者，請記得攜帶「COVID-19疫苗接種紀錄卡」，並於接種前評估時，說明過往疫苗接種史，以利醫生評估。近期天氣多變，對於近期身體具狀況或慢性病情不穩定者，請於身體狀況較穩定後就近前往接種，接種後請多加留意身體狀況，多喝水多休息，亦請家人協助注意，如有持續發燒超過48小時、嚴重過敏反應如呼吸困難、氣喘、眩暈、心跳加速、全身紅疹等不適症狀，應儘速就醫釐清病因。</t>
+    <t>發佈日期：2022-01-30\$\@\$中央流行疫情指揮中心今(30)日公布國內新增54例COVID-19確定病例，分別為14例本土個案及40例境外移入(8例為航班落地採檢陽性)；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為6例男性、8例女性，年齡介於未滿10歲至60多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為21例男性、19例女性，年齡介於未滿5歲至60多歲，分別自美國(8例)、英國(5例)、中國(4例)、越南(3例)、柬埔寨(2例)、澳大利亞、香港、法國、日本、南非、菲律賓、加拿大及匈牙利(各1例)移入；另10例調查中。入境日介於今(2022)年1月14日至1月29日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,659,833例新型冠狀病毒肺炎相關通報(含5,640,850例排除)，其中18,735例確診，分別為3,633例境外移入，15,048例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計127例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月30日新增本土COVID-19確診個案表.pdf\$\@\$1月30日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
     <t>發佈日期：2022-01-29\$\@\$中央流行疫情指揮中心今(29)日表示，因應國際COVID-19疫情嚴峻及Omicron等新型變異株於國內社區流行風險，自去(2021)年8月30日起啟動各項COVID-19加強監測方案，及時偵測國內病例阻斷傳播鏈，截至本(2022)年1月22日辦理情形如下：\$\@\$一、社區加強監測：\$\@\$於全國21個縣市共計274家基層定點診所，發放公費COVID-19家用快篩試劑，由醫師評估對於具呼吸道症狀民眾發放試劑，再由民眾居家篩檢及回報快篩結果。累計發放17,834劑，其中1人後續經PCR檢驗研判為確定病例，呼籲民眾如出現呼吸道症狀，請善加利用此機制至公費快篩試劑發放診所掛號就醫。\$\@\$二、國際機場/國際海港特定高風險工作人員重點監測：\$\@\$於桃園、臺北、臺中與高雄等4個國際機場及12處國際商港、工業港及離島兩岸通航(小三通)港口之特定高風險工作人員，每7天以公費家用快篩試劑採檢一次。累計檢測80,456人次，其中2人快篩陽性後經PCR檢驗研判為確定病例。\$\@\$三、廢汙水監測：\$\@\$持續辦理全國汙水SARS-CoV-2病毒監測，由11處監測站累計採檢176件汙水檢體，SARS-CoV-2病毒核酸檢測均為陰性。\$\@\$四、邊境進口冷凍食品包裝監測：\$\@\$持續於邊境採樣檢驗進口冷凍肉品、水產品及水果之內、外包裝，監控進口冷凍食品內、外包裝之SARS-CoV-2病毒污染狀況，累計抽驗30個國家之253批產品，共978件樣品，SARS-CoV-2病毒核酸檢測均為陰性。\$\@\$五、捐血人血清抗體陽性盛行率調查：\$\@\$針對去年4至7月份我國捐血中心捐血人之血液存檔樣本，已完成抽樣5,000支檢體進行抗體檢測，僅1支檢體抗核蛋白(N)抗體及抗棘蛋白(S)抗體檢測結果皆為陽性，陽性率為0.02%，整體自然感染陽性率低，與該區間同年齡層確診率相當，本次調查未發現大量未診斷之潛在病例。\$\@\$指揮中心強調，為因應Omicron新型變異株威脅，及維護國內社區安全，將持續強化邊境與社區監測等各項防疫作為，及早發現可能病例，阻斷傳播鏈，並依據疫情態勢，適度調整加強監測方案。</t>
   </si>
   <si>
-    <t>發佈日期：2021-07-10\$\@\$中央流行疫情指揮中心今（10）日表示，近日有網友散布「三級警戒微解封的不可思議之處，新冠肺炎病毒只會攻擊家人」等訊息，相關內容多有誤導，且在錯誤基礎上進行不當類比，指揮中心再次強調，相關防疫指引已清楚說明，原本同住家人可以繼續維持生活，相關指引都是針對日常非同住者間的行為互動加以規範，呼籲民眾勿輕信或隨意散播、轉傳錯誤訊息，造成防疫困擾。\$\@\$指揮中心指出，有關7月13號以後針對部分場所將適度鬆綁，但仍須遵守防疫相關指引及規範，而此波疫情中，不少個案均為家戶群聚感染，由於室內密切接觸風險較高，因此對於室內社交人數須有較嚴格規範，但不包含原本同住的家人，也無需限制同住家人不能在家打麻將、看電影、吃飯等。 圖片 附件\$\@\$0710指揮中心：勿輕信「三級警戒微解封的不可思議之處」之網傳.jpg</t>
+    <t>發佈日期：2022-01-28\$\@\$中央流行疫情指揮中心今(28)日公布國內新增71例COVID-19確定病例，分別為27例本土個案及44例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為8例男性、19例女性，年齡介於未滿10歲至60多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為25例男性、19例女性，年齡介於未滿5歲至70多歲，分別自美國及菲律賓各8例、中國5例、印尼3例、日本、瑞典及越南各2例、孟加拉國、荷蘭、土耳其、英國、奧地利及丹麥各1例移入；另8例調查中。入境日介於今(2022)年1月13日至1月27日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,613,922例新型冠狀病毒肺炎相關通報(含5,594,976例排除)，其中18,634例確診，分別為3,561例境外移入，15,019例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增3例空號病例(案18314境外移入、案18425本土、案18438本土，再次採檢為陰性，共3案研判排除)，累計126例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月28日新增境外移入COVID-19確診個案表.pdf\$\@\$1月28日新增本土COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-27\$\@\$中央流行疫情指揮中心今(27)日公布國內新增64例COVID-19確定病例，分別為21例本土個案及43例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為11例男性、10例女性，年齡介於未滿5歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為21例男性、22例女性，年齡介於未滿5歲至60多歲，分別自美國(14例)、印度(3例)、越南、印尼、英國及法國(各2例)、衣索比亞、坦尚尼亞、新加坡、土耳其、菲律賓、南非、芬蘭、日本(各1例)移入；另10例調查中。入境日介於去(2021)年5月2日至今(2022)年1月26日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,581,517例新型冠狀病毒肺炎相關通報(含5,562,679例排除)，其中18,566例確診，分別為3,518例境外移入，14,994例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案18418，再次採檢為陰性，改判排除)，累計123例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月27日新增本土COVID-19確診個案表.pdf\$\@\$1月27日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
     <t>發佈日期：2021-06-13\$\@\$近日有網友在臉書FB以自製圖文方式散布「政府讓人民施打未受認證且保護力低之國產疫苗」、「國產疫苗的中和抗體效價比國外疫苗差」、「國產疫苗為什麼不向國際提出緊急授權」，中央流行疫情指揮中心(下稱指揮中心)今（13）日嚴正澄清表示，目前國產疫苗臨床試驗尚在進行中，最終結果須等廠商提出EUA 申請，經專家會議審查疫苗的製程管控、藥毒理試驗及臨床試驗結果，在緊急公衛的需求下，確認疫苗使用效益大於風險，才會核准緊急授權使用。\$\@\$指揮中心指出，目前國產疫苗廠商皆已積極規劃，以取得國際認證為目標。國產疫苗需經食藥署和專家會議嚴謹審查，在緊急公衛需求，並確認效益大於風險，才會核准緊急授權使用。此外，各家廠牌的疫苗所使用的檢驗實驗室及檢驗方式不同且無協和，無法直接由各實驗室產生數值進行比較。國產疫苗仍需等廠商提出申請，經過中央主管機關嚴格把關及審查通過後，確認品質、安全、療效後，品質沒有問題，疫苗方可供民眾施打。\$\@\$指揮中心再次提醒，民眾接獲來源不明的訊息時，應先進行查證，切勿隨意散播、轉傳，以免觸法。 圖片 附件\$\@\$0613網傳「政府讓人民施打未受認證且保護力低之國產疫苗」-1.jpg\$\@\$0613網傳「政府讓人民施打未受認證且保護力低之國產疫苗」-2.jpg</t>
@@ -379,34 +418,19 @@
     <t>發佈日期：2021-06-01\$\@\$中央流行疫情指揮中心今(1)日指出，近日有網友在通訊軟體LINE散布「臺中市太原路復健醫院被徵收為方艙醫院」，臺中市政府衛生局已澄清為不實訊息，請民眾勿再轉傳與散布，以免觸法遭罰。\$\@\$指揮中心表示，臺中市政府已對外澄清，此復健醫院近期進行搬遷作業，是為了提升醫療品質，正以BOT方式規劃市立綜合醫院，並非徵用作為方艙醫院。\$\@\$指揮中心副指揮官陳宗彥指出，因應疫情變化，各地方政府規劃應變醫院及專責醫院收治患者，民眾接獲來源不明的訊息時，應先進行查證，切勿隨意散播、轉傳，以免觸法。\$\@\$指揮中心重申，防疫相關資訊應以中央流行疫情指揮中心公布內容為主，散播假訊息構成犯罪，會被判處最高三年有期徒刑或併科三百萬元罰金。提醒民眾，收到來路不明訊息多加留意、查證，切勿轉傳散播，以免觸法。詳情請上官網查詢(http://at.cdc.tw/Q7S2Vt)。 圖片 附件\$\@\$網傳「臺中市太原路復健醫院被徵收為方艙醫院」為不實訊息勿轉傳.jpg\$\@\$勿散播不實訊息，以免觸法受罰.jpg</t>
   </si>
   <si>
-    <t>發佈日期：2021-05-28\$\@\$近期國內疫情升溫，警方發現網路上有不肖人士販售「新冠病毒快篩試劑」，中央流行疫情指揮中心副指揮官陳宗彥今(28)日表示，擅自在網路販售新冠病毒檢驗試劑等第三級醫療器材已違反「醫療器材管理法」，目前警方已進行偵辦，提醒民眾切勿購買檢測，除有效性及檢測結果正確性均無法確認外，還可能危害自身健康。\$\@\$指揮中心指出，新冠病毒檢驗試劑是第三級醫療器材，依據「醫療器材管理法」規定，只有醫療器材商及藥局可以販賣，且國內並未開放可使用通訊方式在網路、電話、社群媒體等販售。\$\@\$指揮中心強調，不肖人士在網路擅自販售專案核准的新冠病毒檢驗試劑已違「醫療器材管理法」，會被罰3萬以上100萬以下罰鍰，如果民眾發現有類似狀況，可打1919專線或是向地方衛生局檢舉。 圖片 附件\$\@\$0528網路販售「新冠病毒快篩試劑」已觸法，警方偵辦中.jpg\$\@\$勿散播不實訊息，以免觸法受罰.jpg</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-05-25\$\@\$中央流行疫情指揮中心今(25)日表示，近日網路出現偽冒教育部網站，杜撰「全國各級學校因應疫情停課時程資訊」等訊息，意圖造成民眾困惑，此為境外假網頁不實訊息，請民眾勿輕信。\$\@\$指揮中心副指揮官陳宗彥表示，該網站假冒教育部傳達不實防疫訊息，刑事警察局已成立專案小組偵辦，經調查其為境外IP。\$\@\$指揮中心指出，教育部全球資訊網正確的網址是https://www.edu.tw/ ，民眾收到任何連結時，可以先觀察連結網址，是否跟官方網址一樣。例如，教育部官方網址的網域，就會是「edu.tw」結尾。\$\@\$指揮中心強調，散播假訊息構成犯罪，會被判處最高三年有期徒刑或併科三百萬元罰金。提醒民眾，收到來路不明訊息多加留意、查證，切勿轉傳散播，以免觸法。 圖片 附件\$\@\$0525指揮中心指出，網路出現偽冒教育部網站並杜撰假訊息，請民眾勿輕信.jpg\$\@\$勿散播不實訊息，以免觸法受罰.jpg</t>
+    <t>發佈日期：2022-01-28\$\@\$各位醫界朋友，您好：\$\@\$全球疫情持續嚴峻，Omicron變異株現已為全球與國內主要流行病毒株，由於其具有多個基因變異位點，可能影響部分治療藥物效果，COVID-19專家諮詢會審視國內外最新實證後，統整對Omicron變異株藥物使用建議如下：\$\@\$1. 不需使用氧氣且具重症風險因子之COVID-19病患：\$\@\$(1)建議可使用remdesivir靜脈注射三日療程，或nirmatrelvir + ritonavir (Paxlovid)口服五日，未住院病患建議優先選擇口服藥物治療。若上述兩種藥物均不適用，則可使用molnupiravir (Lagevrio)口服五日。臨床醫師可評估病患情況後，依本署公告之領用方案及注意事項申請使用；另因缺乏實證與安全性資料，不建議同時併用remdesivir和口服抗病毒藥物。\$\@\$(2)我國目前儲備之兩種複合式anti-SARS-CoV-2單株抗體(casirivimab + imdevimab, bamlanivimab + etesevimab)，因體外試驗顯示對Omicron變異株中和能力大幅下降，可能影響臨床效果，故除非已確認上述單株抗體對患者感染之變異株仍有效，否則不建議使用，使用前務必參閱最新版「新型冠狀病毒（SARS-CoV-2）感染臨床處置暫行指引」中「單株抗體對SARS-CoV-2變異株效果實證」表格。\$\@\$2.需吸氧治療、高流量氧氣、非侵襲性呼吸器或插管病患：\$\@\$目前證據顯示，Omicron變異株不影響dexamethasone、tocilizumab、baricitinib與remdesivir對此類病人之療效，故維持現行治療建議。\$\@\$面對社區疫情，指揮中心提醒臨床醫師提高警覺，對有疑似症狀患者加強採檢，以早期偵測疫情。另目前針對不同嚴重程度COVID-19病患均已有治療藥物可選用，用藥前請參閱最新版「新型冠狀病毒（SARS-CoV-2）感染臨床處置暫行指引」中個別藥物說明。\$\@\$「嚴重特殊傳染性肺炎」之診療相關資訊將隨時依防疫需求與最新文獻證據更新並公布於疾病管制署全球資訊網(http://www.cdc.gov.tw)。\$\@\$感謝您與我們共同維護全民的健康安全。 附件\$\@\$診治指引表四＿我國診治指引對SARS-CoV-2確診病患用藥建議彙整.pdf\$\@\$診治指引表五＿單株抗體對SARS-CoV-2變異株效果實證.pdf</t>
   </si>
   <si>
     <t>發佈日期：2022-01-26\$\@\$各位醫界朋友，您好：\$\@\$為積極因應新型冠狀病毒疾病疫情防疫需求，衛生福利部食品藥物管理署於評估療效、安全性、風險效益與緊急公共衛生需求後，於本(111)年1月12日與1月15日分別核准兩種口服抗病毒藥物專案輸入，經COVID-19專家諮詢會檢視最新實證後，於臨床處置暫行指引中新增口服抗病毒藥物使用建議如下：\$\@\$新增nirmatrelvir + ritonavir(Paxlovid)適用對象為具以下任一重症風險因子，未使用氧氣且於發病五天內之 ≧ 12歲且體重 ≧ 40公斤病患；風險因子包括年齡 ≧ 65歲、糖尿病、慢性腎病、心血管疾病(含高血壓)、慢性肺疾、BMI ≧ 25 (或12-17歲兒童青少年BMI 超過同齡第85百分位)、其他影響免疫功能之疾病或已知重症風險因子者。建議劑量為Nirmatrelvir 300 mg + ritonavir 100 mg 每日兩次口服，療程共五天。使用時須特別注意藥物交互作用及肝腎功能異常時之建議，並確實完成五天療程。\$\@\$新增molnupiravir(Lagevrio)適用對象為具以下任一重症風險因子，未使用氧氣且於發病五天內之 ≧ 18歲病患，且無法使用其他建議藥物者；風險因子包括年齡 ≧ 65歲、糖尿病、慢性腎病、心血管疾病(含高血壓)、慢性肺疾、BMI ≧ 25、其他影響免疫功能之疾病或已知重症風險因子者。建議劑量為molnupiravir 800mg每日兩次口服，療程共五天。\$\@\$目前針對未使用氧氣且具重症風險因子之COVID-19病患，專家諮詢小組建議可使用藥物包括remdesivir、nirmatrelvir + ritonavir與兩種複合式anti-SARS-CoV-2單株抗體(casirivimab + imdevimab, bamlanivimab + etesevimab)，臨床醫師可評估病患病況與變異株流行情形後，依本署公告流程申請使用；若病患不適用上述藥物，則可申請使用molnupiravir。\$\@\$「嚴重特殊傳染性肺炎」之診療相關資訊將隨時依防疫需求與最新文獻證據更新並公布於疾病管制署全球資訊網(http://www.cdc.gov.tw)。\$\@\$感謝您與我們共同維護全民的健康安全。 附件\$\@\$附件1＿新型冠狀病毒（SARS-CoV-2）感染臨床處置暫行指引第十六版.pdf\$\@\$附件2_公費COVID-19治療用口服抗病毒藥物領用方案_1110126制定.pdf</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-06\$\@\$為提供結核病患即時診斷，疾病管制署結核病診治指引自104年已加重結核分枝桿菌核酸增幅(nucleic acid amplification, NAA)檢驗於診斷結核病之角色。NAA檢驗具快速、高敏感度及高特異性，可大幅縮短傳統培養檢驗方法所需等待結果時間，有利及早診斷及治療結核病。\$\@\$因應近期結核菌液態培養(MGIT)檢驗發生添加劑(營養劑併抑制細菌生長的抗生素成分)供貨短缺情形，為避免延遲發現疑似結核病個案，依本署110年12月24日「衛生福利部傳染病防治諮詢會(結核病防治組)」會議決議，於供貨短缺期間，對於社區型肺炎尚未通報結核病者，於診斷送驗3套初查痰執行塗片耐酸性染色鏡檢(Acid fast stain)及分枝桿菌培養時，其中1套請務必同時開立NAA檢驗。另考量實驗室短期內MGIT痰培養試劑有限，對於管理中的結核病患追蹤複查痰，請採1套進行培養檢驗，暫時避免重複送驗檢體，此因應作為停止施行時間將於缺貨狀況緩解後再函週知。\$\@\$有關「結核病診治指引」可至疾病管制署全球資訊網(https://www.cdc.gov.tw)&gt;傳染病與防疫專題&gt;傳染病介紹&gt;第三類定傳染病&gt;結核病&gt;重要指引及教材項下查閱。\$\@\$感謝您與我們共同維護全民的健康安全。</t>
-  </si>
-  <si>
     <t>發佈日期：2022-01-06\$\@\$各位醫界朋友，您好：\$\@\$新型冠狀病毒(SARS-CoV-2)國際疫情嚴峻，Omicron變異株迅速擴散。由於變異株變異位點可能影響抗SARS-CoV-2單株抗體療效，治療指引自第十五版起新增「單株抗體對SARS-CoV-2變異株效果實證」附表，供臨床醫師用藥時參考。另COVID-19專家諮詢會檢視最新實證後，更新治療指引藥物適用原則如下：\$\@\$新增remdesivir適用對象為具以下任一風險因子，未使用氧氣且於發病七天內之≧12歲且體重≧40公斤病患；風險因子包括年齡≧65歲、糖尿病、慢性腎病、心血管疾病(含高血壓)、慢性肺疾、BMI≧25 (或12–17歲兒童青少年BMI 超過同齡第85百分位)、懷孕、其他影響免疫功能之疾病或已知重症風險因子者。建議劑量為第一天200 mg靜脈注射，第二至三天100 mg，療程共三天。\$\@\$維持現行抗SARS-CoV-2複合單株抗體(Casirivimab + imdevimab或Bamlanivimab + etesevimab)適用對象建議，但由於體外試驗顯示上述兩種抗SARS-CoV-2複合單株抗體可能無法有效中和包括Beta、Gamma、Delta plus、Mu與Omicron變異株，建議臨床醫師使用時需考量流行狀況與參閱指引內最新版「單株抗體對SARS-CoV-2變異株效果實證」附表。\$\@\$面對冬季疫情，指揮中心提醒臨床醫師提高警覺，對有疑似症狀患者加強採檢，以早期偵測疫情。另目前針對不同嚴重程度COVID-19病患均已有治療藥物可選用，可依臨床狀況給予最妥善治療。\$\@\$「嚴重特殊傳染性肺炎」之診療相關資訊將隨時依防疫需求與最新文獻證據更新並公布於疾病管制署全球資訊網(http://www.cdc.gov.tw)。\$\@\$感謝您與我們共同維護全民的健康安全。 附件\$\@\$新型冠狀病毒（SARS-CoV-2）感染臨床處置暫行指引第十五版.pdf\$\@\$附表SARS-CoV-2之藥物使用實證摘要_20211230更新.pdf\$\@\$公費COVID-19治療用單株抗體領用方案.pdf\$\@\$公費COVID-19抗病毒藥劑VEKLURYR領用方案1110106第6版.pdf</t>
   </si>
   <si>
-    <t>發佈日期：2021-12-30\$\@\$各位醫界朋友，您好：\$\@\$鑑於國際COVID-19疫情嚴峻及Omicron新型變異株威脅增加，嚴重特殊傳染性肺炎中央流行疫情指揮中心(下稱指揮中心)邀請各縣市兒科、內科、家醫科、耳鼻喉科及婦產科等有提供診治呼吸道症狀服務之診所/衛生所，自明(2022)年1月1日起加入公費COVID-19家用快篩試劑發放行列，指揮中心感謝基層診所積極守護社區健康的熱誠，並籲請各定點診所醫師針對具呼吸道症狀就醫民眾，加強發放公費COVID-19家用快篩試劑。\$\@\$指揮中心於今(2021)年8月30日起啟動前揭計畫，全國共計18個縣市86家診所/衛生所參加，迄今已發放1萬餘劑公費COVID-19家用快篩試劑，於有效監測下均無發現陽性個案。為提升民眾取用COVID-19家用快篩試劑可近性及擴大監測，自明年1月1日起增加至21個縣市272家診所/衛生所參與。\$\@\$由於國內現處於流感季節且COVID-19症狀與上呼吸道感染症狀相似，指揮中心籲請定點診所針對出現呼吸道症狀就醫民眾，加強發放公費COVID-19家用快篩試劑，尤可對於幼兒及其陪病家屬加強評估發放；另請診所衛教民眾試劑使用流程及注意事項、提醒民眾匿名填寫線上問卷以回報快篩結果等資料，並將發放民眾資料登錄於疾病管制署系統中。\$\@\$該計畫相關內容公布於疾病管制署全球資訊網 (http://www.cdc.gov.tw) COVID-19防疫專區&gt;臺灣社交距離APP及採檢地圖&gt;COVID-19社區加強監測方案，歡迎查閱。\$\@\$感謝您與我們共同維護全民的健康安全。</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-10-22\$\@\$各位醫界朋友，您好：\$\@\$我國新型冠狀病毒(SARS-CoV-2)感染臨床處置暫行指引建議可依照病患病程與嚴重度，對不需用氧且有重症風險因子之病患給予單株抗體，需用氧病患則除dexamethasone外可併用免疫調節劑tocilizumab或baricitinib。鑒於近期國際間藥物使用建議與國內適應症均有更新，經COVID-19專家諮詢會議更新建議如下：\$\@\$1.複合單株抗體Casirivimab + imdevimab或Bamlanivimab + etesevimab。適用對象為\$\@\$― 具以下任一風險因子，未使用氧氣且於發病十天內之≧12歲且體重≧40公斤病患；\$\@\$― 風險因子包括：年齡 ≧ 65歲、糖尿病、慢性腎病、心血管疾病（含高血壓）、慢性肺疾、BMI ≧25（或12-17歲兒童BMI超過同齡第85百分位）、懷孕、其他影響免疫功能之疾病或已知重症風險因子等。\$\@\$目前實證顯示上述兩種複合單株抗體對國內現今主要檢出之Delta與Alpha變異株均有效，但由於體外試驗顯示Bamlanivimab + etesevimab可能無法有效中和包括Beta、Gamma、Delta plus與Mu變異株，建議臨床醫師使用時需考量流行狀況與參閱最新版「SARS-CoV-2之藥物使用實證摘要」附表。\$\@\$另參考WHO最新公布治療建議，於診治指引註解中新增「隨機對照研究顯示對血清抗體陰性之嚴重肺炎以上程度病患，除標準治療外，給予casirivimab 4000mg + imdevimab 4000mg 可降低死亡率」。\$\@\$2.Remdesivir適用對象為嚴重肺炎以上（未使用吸氧治療下的SpO2 ≦ 94%、需使用吸氧治療、需使用高流量氧氣或非侵襲性呼吸器但未插管）病患。另於診治指引註解中新增「若住院病患胸部X光片顯示肺炎，雖未達重症標準且不符合單株抗體適用條件，仍可申請使用remdesivir」。但由於目前尚無併用單株抗體之效益與安全性資料，目前仍暫不建議remdesivir與單株抗體同時併用。\$\@\$由於近日媒體報導ivermectin用於治療COVID-19一事，經專家委員審視國際文獻，發現ivermectin相關臨床試驗研究證據力等級低，且部分研究涉及科學誠信，其中亦有發表論文被撤回之情形，統合分析結果顯示目前證據不支持ivermectin可用於治療或預防COVID-19，WHO及歐美等具公信力之治療指引均不建議使用於COVID-19之治療。為確保國人健康，我國診治指引治療藥物建議係根據最高等級實證基礎制訂，參考目前各方面之資料，仍不建議ivermectin納入我國診治指引之治療建議藥物。\$\@\$「嚴重特殊傳染性肺炎」之診療相關資訊將隨時依防疫需求與最新文獻證據更新並公布於疾病管制署全球資訊網(http://www.cdc.gov.tw)。\$\@\$感謝您與我們共同維護全民的健康安全。</t>
-  </si>
-  <si>
     <t>發佈日期：2022-01-28\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$疫情中心\$\@\$約用助理\$\@\$(徵才案號：0605，含延長公告)\$\@\$(計4名)\$\@\$姚○雯(A22649****)\$\@\$盧○淳(A22626****)\$\@\$邱○柔(A22582****)\$\@\$莊○媛(R22426****)\$\@\$二、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一)口試：\$\@\$1、報到時間：111年02月09日星期三15:20~15:30，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署1樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：15:30~17:00。\$\@\$(二)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(三)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於111年02月09日上午10點前主動以電子郵件或電話通知人事室陳小姐(yuan_c@cdc.gov.tw、電話02-23959825分機3864)，俾利安排應試座位。\$\@\$(四)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(五)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
   </si>
   <si>
     <t>發佈日期：2022-01-13\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$急性傳染病組\$\@\$約用助理\$\@\$(徵才案號：1106，含延長公告)\$\@\$(計1名)\$\@\$張○純(A22889****)\$\@\$二、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一) 口試：\$\@\$1、報到時間：111年01月17日星期一15:20~15:30，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署7樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：16:40~17:10。\$\@\$(二)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(三)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於111年01月17日上午10點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3823)，俾利安排應試座位。\$\@\$(四)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(五)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2021-12-24\$\@\$一、考評單位：衛生福利部疾病管制署。\$\@\$二、考評目的：客觀衡量地方政府衛生局111年防疫業務之施政績效。\$\@\$三、受評機關：地方政府衛生局。\$\@\$四、受評期間：111年1月至12月\$\@\$五、考評架構與權重：9項考評指標，共計200分。\$\@\$六、考評方式：\$\@\$(一)   防疫業務相關管理系統之統計結果及書面考核。\$\@\$本手冊考評指標資料，如須受評機關提供始得評分者，請於112年1月13日前備函逕送考評執行單位進行評核。\$\@\$考評單位於指定日期前完成分數統計及成績評定。\$\@\$考評單位完成考評並請地方政府衛生局確認後，於111年3月17日前將考評結果送衛生福利部綜合規劃司備查。\$\@\$(二)   考評單位得視需要辦理實地查核。 附件\$\@\$111年地方衛生機關業務考評作業手冊-防疫類.pdf\$\@\$111年地方衛生機關業務考評作業手冊-防疫類.docx</t>
   </si>
   <si>
     <t>發佈日期：2021-12-24\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$慢性傳染病組\$\@\$約用助理\$\@\$(徵才案號：0309)\$\@\$(計3名)\$\@\$林○萱(B22260****)\$\@\$陳○瑜(Q22389****)\$\@\$陳○君(F22674****)\$\@\$二、實作、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一)實作：\$\@\$1、報到時間：111年1月7日星期五13:20。\$\@\$2、報到地點：衛生福利部疾病管制署1樓(臺北市中正區林森南路6號)。\$\@\$3、實作時間：13:40~15:10。實作開始鈴響(13:40)未到者，喪失應考資格。\$\@\$(二)口試：\$\@\$1、報到時間：111年1月7日星期五15:20，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署1樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：15:30~16:30。\$\@\$(三)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(四)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於111年1月6日下午5點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3823)，俾利安排應試座位。\$\@\$(五)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(六)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。\$\@\$三、試場規則：\$\@\$(一)第一試為實作測驗，題型為資料串接統計分析，應試者得自行攜帶筆記型電腦，並預先安裝欲於測驗時使用的統計分析軟體(可選擇使用SAS、R、Excel等其他統計分析軟體)；未自行攜帶筆記型電腦者，則由本署提供公務電腦於測驗時使用(僅具Excel功能且無法安裝軟體)。\$\@\$(二)測驗中途不容許離場，並於考試時間過半後始得離場，離場後不得再進入試場。\$\@\$(三)測驗期間不允許上網、隨身攜帶手機(含智慧手環)、行動網卡、無線網路分享器等電子用品，並請關閉網路、手機、聲音及振動(含鬧鐘)，考試過程中如有上網、發出聲音及震動，均喪失應考資格。\$\@\$(四)個人用品(如書包等)置於考場前後，桌面上僅可放置必要文具(墊板須為透明；水杯、飲料亦禁止放置)。\$\@\$(五)有下列各款情事之一者，予以扣考並不予計分或不得繼續應考：\$\@\$1、冒名頂替。\$\@\$2、持用偽造或變造之證件。\$\@\$3、互換座位或試卷。\$\@\$4、傳遞文稿、參考資料、書寫有關文字之物件或有關信號。\$\@\$5、夾帶書籍文件。\$\@\$6、故意不繳交試卷或破壞試卷彌封。\$\@\$7、在桌椅、文具或肢體上或其他處所，書寫有關文字。\$\@\$8、電子通訊舞弊行為。\$\@\$9、窺視他人試卷、答案卷、作答結果或互相交談。\$\@\$10、在答案卷上書寫姓名、座號或其他不應有之文字、標記或自備稿紙書寫。\$\@\$11、其他破壞試場秩序事項。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
@@ -787,7 +811,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -815,16 +839,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2">
-        <v>44592</v>
+        <v>44593</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -832,16 +856,16 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C3" s="2">
-        <v>44591</v>
+        <v>44592</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="E3" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -849,13 +873,16 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C4" s="2">
         <v>44591</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>79</v>
+        <v>87</v>
+      </c>
+      <c r="E4" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -863,16 +890,16 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C5" s="2">
         <v>44591</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -880,16 +907,13 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C6" s="2">
-        <v>44590</v>
+        <v>44591</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -897,16 +921,13 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C7" s="2">
         <v>44590</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -914,16 +935,16 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C8" s="2">
-        <v>44387</v>
+        <v>44590</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="E8" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -931,16 +952,13 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C9" s="2">
-        <v>44360</v>
+        <v>44590</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -948,13 +966,16 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C10" s="2">
-        <v>44359</v>
+        <v>44589</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>85</v>
+        <v>93</v>
+      </c>
+      <c r="E10" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -962,959 +983,556 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C11" s="2">
-        <v>44348</v>
+        <v>44588</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="E11" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C12" s="2">
-        <v>44344</v>
+        <v>44593</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E12" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C13" s="2">
-        <v>44341</v>
+        <v>44592</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E13" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C14" s="2">
-        <v>44589</v>
+        <v>44591</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C15" s="2">
-        <v>44587</v>
+        <v>44591</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E15" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C16" s="2">
-        <v>44567</v>
+        <v>44591</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E16" t="s">
-        <v>124</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C17" s="2">
-        <v>44567</v>
+        <v>44590</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E17" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C18" s="2">
-        <v>44560</v>
+        <v>44387</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E18" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C19" s="2">
-        <v>44491</v>
+        <v>44360</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E19" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C20" s="2">
-        <v>44589</v>
+        <v>44359</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C21" s="2">
-        <v>44589</v>
+        <v>44348</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
+      </c>
+      <c r="E21" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C22" s="2">
-        <v>44589</v>
+        <v>44344</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C23" s="2">
-        <v>44589</v>
+        <v>44341</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C24" s="2">
         <v>44589</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
+      </c>
+      <c r="E24" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C25" s="2">
-        <v>44589</v>
+        <v>44587</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
+      </c>
+      <c r="E25" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C26" s="2">
-        <v>44589</v>
+        <v>44567</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C27" s="2">
-        <v>44589</v>
+        <v>44567</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
+      </c>
+      <c r="E27" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C28" s="2">
-        <v>44588</v>
+        <v>44560</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C29" s="2">
-        <v>44588</v>
+        <v>44491</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C30" s="2">
-        <v>44588</v>
+        <v>44589</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C31" s="2">
-        <v>44588</v>
+        <v>44589</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C32" s="2">
         <v>44589</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E32" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C33" s="2">
-        <v>44574</v>
+        <v>44589</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E33" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C34" s="2">
-        <v>44573</v>
+        <v>44589</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C35" s="2">
-        <v>44554</v>
+        <v>44589</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E35" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C36" s="2">
-        <v>44554</v>
+        <v>44589</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E36" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C37" s="2">
-        <v>44550</v>
+        <v>44589</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E37" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C38" s="2">
-        <v>44592</v>
+        <v>44588</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E38" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="C39" s="2">
-        <v>44591</v>
+        <v>44588</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="C40" s="2">
-        <v>44591</v>
+        <v>44588</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="C41" s="2">
-        <v>44591</v>
+        <v>44588</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="C42" s="2">
-        <v>44590</v>
+        <v>44589</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="E42" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="C43" s="2">
-        <v>44590</v>
+        <v>44574</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>82</v>
+        <v>120</v>
+      </c>
+      <c r="E43" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="C44" s="2">
-        <v>44387</v>
+        <v>44573</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="C45" s="2">
-        <v>44360</v>
+        <v>44554</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E45" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="C46" s="2">
-        <v>44359</v>
+        <v>44554</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>85</v>
+        <v>123</v>
+      </c>
+      <c r="E46" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="C47" s="2">
-        <v>44348</v>
+        <v>44550</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>86</v>
+        <v>124</v>
       </c>
       <c r="E47" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" t="s">
-        <v>15</v>
-      </c>
-      <c r="B48" t="s">
-        <v>51</v>
-      </c>
-      <c r="C48" s="2">
-        <v>44344</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" t="s">
-        <v>16</v>
-      </c>
-      <c r="B49" t="s">
-        <v>52</v>
-      </c>
-      <c r="C49" s="2">
-        <v>44341</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" t="s">
-        <v>17</v>
-      </c>
-      <c r="B50" t="s">
-        <v>53</v>
-      </c>
-      <c r="C50" s="2">
-        <v>44589</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51" t="s">
-        <v>54</v>
-      </c>
-      <c r="C51" s="2">
-        <v>44587</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E51" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" t="s">
-        <v>19</v>
-      </c>
-      <c r="B52" t="s">
-        <v>55</v>
-      </c>
-      <c r="C52" s="2">
-        <v>44567</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E52" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" t="s">
-        <v>20</v>
-      </c>
-      <c r="B53" t="s">
-        <v>56</v>
-      </c>
-      <c r="C53" s="2">
-        <v>44567</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" t="s">
-        <v>21</v>
-      </c>
-      <c r="B54" t="s">
-        <v>57</v>
-      </c>
-      <c r="C54" s="2">
-        <v>44560</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E54" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" t="s">
-        <v>22</v>
-      </c>
-      <c r="B55" t="s">
-        <v>58</v>
-      </c>
-      <c r="C55" s="2">
-        <v>44491</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E55" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" t="s">
-        <v>23</v>
-      </c>
-      <c r="B56" t="s">
-        <v>59</v>
-      </c>
-      <c r="C56" s="2">
-        <v>44589</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" t="s">
-        <v>24</v>
-      </c>
-      <c r="B57" t="s">
-        <v>60</v>
-      </c>
-      <c r="C57" s="2">
-        <v>44589</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" t="s">
-        <v>25</v>
-      </c>
-      <c r="B58" t="s">
-        <v>61</v>
-      </c>
-      <c r="C58" s="2">
-        <v>44589</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" t="s">
-        <v>26</v>
-      </c>
-      <c r="B59" t="s">
-        <v>62</v>
-      </c>
-      <c r="C59" s="2">
-        <v>44589</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" t="s">
-        <v>27</v>
-      </c>
-      <c r="B60" t="s">
-        <v>63</v>
-      </c>
-      <c r="C60" s="2">
-        <v>44589</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" t="s">
-        <v>28</v>
-      </c>
-      <c r="B61" t="s">
-        <v>64</v>
-      </c>
-      <c r="C61" s="2">
-        <v>44589</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" t="s">
-        <v>29</v>
-      </c>
-      <c r="B62" t="s">
-        <v>65</v>
-      </c>
-      <c r="C62" s="2">
-        <v>44589</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" t="s">
-        <v>30</v>
-      </c>
-      <c r="B63" t="s">
-        <v>66</v>
-      </c>
-      <c r="C63" s="2">
-        <v>44589</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" t="s">
-        <v>31</v>
-      </c>
-      <c r="B64" t="s">
-        <v>67</v>
-      </c>
-      <c r="C64" s="2">
-        <v>44588</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" t="s">
-        <v>32</v>
-      </c>
-      <c r="B65" t="s">
-        <v>68</v>
-      </c>
-      <c r="C65" s="2">
-        <v>44588</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" t="s">
-        <v>33</v>
-      </c>
-      <c r="B66" t="s">
-        <v>69</v>
-      </c>
-      <c r="C66" s="2">
-        <v>44588</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" t="s">
-        <v>34</v>
-      </c>
-      <c r="B67" t="s">
-        <v>70</v>
-      </c>
-      <c r="C67" s="2">
-        <v>44588</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" t="s">
-        <v>35</v>
-      </c>
-      <c r="B68" t="s">
-        <v>71</v>
-      </c>
-      <c r="C68" s="2">
-        <v>44589</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E68" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" t="s">
-        <v>36</v>
-      </c>
-      <c r="B69" t="s">
-        <v>72</v>
-      </c>
-      <c r="C69" s="2">
-        <v>44574</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E69" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" t="s">
-        <v>37</v>
-      </c>
-      <c r="B70" t="s">
-        <v>73</v>
-      </c>
-      <c r="C70" s="2">
-        <v>44573</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" t="s">
-        <v>38</v>
-      </c>
-      <c r="B71" t="s">
-        <v>74</v>
-      </c>
-      <c r="C71" s="2">
-        <v>44554</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E71" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
-      <c r="A72" t="s">
-        <v>39</v>
-      </c>
-      <c r="B72" t="s">
-        <v>75</v>
-      </c>
-      <c r="C72" s="2">
-        <v>44554</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E72" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
-      <c r="A73" t="s">
-        <v>40</v>
-      </c>
-      <c r="B73" t="s">
-        <v>76</v>
-      </c>
-      <c r="C73" s="2">
-        <v>44550</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E73" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1965,32 +1583,6 @@
     <hyperlink ref="D45" r:id="rId44"/>
     <hyperlink ref="D46" r:id="rId45"/>
     <hyperlink ref="D47" r:id="rId46"/>
-    <hyperlink ref="D48" r:id="rId47"/>
-    <hyperlink ref="D49" r:id="rId48"/>
-    <hyperlink ref="D50" r:id="rId49"/>
-    <hyperlink ref="D51" r:id="rId50"/>
-    <hyperlink ref="D52" r:id="rId51"/>
-    <hyperlink ref="D53" r:id="rId52"/>
-    <hyperlink ref="D54" r:id="rId53"/>
-    <hyperlink ref="D55" r:id="rId54"/>
-    <hyperlink ref="D56" r:id="rId55"/>
-    <hyperlink ref="D57" r:id="rId56"/>
-    <hyperlink ref="D58" r:id="rId57"/>
-    <hyperlink ref="D59" r:id="rId58"/>
-    <hyperlink ref="D60" r:id="rId59"/>
-    <hyperlink ref="D61" r:id="rId60"/>
-    <hyperlink ref="D62" r:id="rId61"/>
-    <hyperlink ref="D63" r:id="rId62"/>
-    <hyperlink ref="D64" r:id="rId63"/>
-    <hyperlink ref="D65" r:id="rId64"/>
-    <hyperlink ref="D66" r:id="rId65"/>
-    <hyperlink ref="D67" r:id="rId66"/>
-    <hyperlink ref="D68" r:id="rId67"/>
-    <hyperlink ref="D69" r:id="rId68"/>
-    <hyperlink ref="D70" r:id="rId69"/>
-    <hyperlink ref="D71" r:id="rId70"/>
-    <hyperlink ref="D72" r:id="rId71"/>
-    <hyperlink ref="D73" r:id="rId72"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update CDC Press and COVID-19 Statistic on 20220202
</commit_message>
<xml_diff>
--- a/Data/CDC_Press List.xlsx
+++ b/Data/CDC_Press List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="146">
   <si>
     <t>Press Title</t>
   </si>
@@ -31,6 +31,12 @@
     <t>Page Content</t>
   </si>
   <si>
+    <t>新增53例COVID-19確定病例，分別為16例本土及37例境外移入</t>
+  </si>
+  <si>
+    <t>新春佳節務必留意手部衛生與飲食安全，健康過好年</t>
+  </si>
+  <si>
     <t>新增60例COVID-19確定病例，分別為16例本土及44例境外移入</t>
   </si>
   <si>
@@ -55,12 +61,6 @@
     <t>新增48例COVID-19確定病例，分別為15例本土及33例境外移入</t>
   </si>
   <si>
-    <t>新增71例COVID-19確定病例，分別為27例本土及44例境外移入</t>
-  </si>
-  <si>
-    <t>新增64例COVID-19確定病例，分別為21例本土及43例境外移入</t>
-  </si>
-  <si>
     <t>網傳「三級警戒微解封的不可思議之處」指揮中心： 原同住家人就不受限制，謠言邏輯誤導且比喻失當，請勿輕信轉傳，造成防疫困擾</t>
   </si>
   <si>
@@ -151,6 +151,12 @@
     <t>公告本署公共關係室約用人員徵才案(徵才案號：0708)初審合格名單及甄試事宜。</t>
   </si>
   <si>
+    <t>/Bulletin/Detail/-y6ftXoFii-OMVXHXoK4BA?typeid=9</t>
+  </si>
+  <si>
+    <t>/Bulletin/Detail/1NIOMSRYI-ifpReSwxHTiw?typeid=9</t>
+  </si>
+  <si>
     <t>/Bulletin/Detail/UA4tEKjcDQRpDuAVBXizlA?typeid=9</t>
   </si>
   <si>
@@ -175,12 +181,6 @@
     <t>/Bulletin/Detail/ORzh4yZe1qOnSgVMSnIkVw?typeid=9</t>
   </si>
   <si>
-    <t>/Bulletin/Detail/RBLVTwsQ9Z33zCEe0IMd_Q?typeid=9</t>
-  </si>
-  <si>
-    <t>/Bulletin/Detail/AaV2iREpabJ8syXu4450Rw?typeid=9</t>
-  </si>
-  <si>
     <t>/Bulletin/Detail/ftv6FPFis84j5uHWTq4lNA?typeid=8772</t>
   </si>
   <si>
@@ -271,6 +271,12 @@
     <t>/Bulletin/Detail/7UJRpdDRbQNIZWyyEfHdHQ?typeid=11</t>
   </si>
   <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/-y6ftXoFii-OMVXHXoK4BA?typeid=9</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov.tw/Bulletin/Detail/1NIOMSRYI-ifpReSwxHTiw?typeid=9</t>
+  </si>
+  <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/UA4tEKjcDQRpDuAVBXizlA?typeid=9</t>
   </si>
   <si>
@@ -295,12 +301,6 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/ORzh4yZe1qOnSgVMSnIkVw?typeid=9</t>
   </si>
   <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/RBLVTwsQ9Z33zCEe0IMd_Q?typeid=9</t>
-  </si>
-  <si>
-    <t>https://www.cdc.gov.tw/Bulletin/Detail/AaV2iREpabJ8syXu4450Rw?typeid=9</t>
-  </si>
-  <si>
     <t>https://www.cdc.gov.tw/Bulletin/Detail/ftv6FPFis84j5uHWTq4lNA?typeid=8772</t>
   </si>
   <si>
@@ -391,31 +391,31 @@
     <t>https://www.cdc.gov.tw/Bulletin/Detail/7UJRpdDRbQNIZWyyEfHdHQ?typeid=11</t>
   </si>
   <si>
+    <t>發佈日期：2022-02-02\$\@\$中央流行疫情指揮中心今(2)日公布國內新增53例COVID-19確定病例，分別為16例本土個案及37例境外移入(25例為航班落地採檢陽性)；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為6例男性、10例女性，年齡介於未滿10歲至80多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為21例男性、15例女性、1例調查中，年齡介於10多歲至80多歲，分別自美國(6例)、法國及新加坡(各2例)、加拿大、宏都拉斯、馬來西亞、阿拉伯聯合大公國、柬埔寨、日本及克羅埃西亞(各1例)移入；另20例調查中。入境日介於今(2022)年1月18日至2月1日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,694,746例新型冠狀病毒肺炎相關通報(含5,675,621例排除)，其中18,903例確診，分別為3,752例境外移入，15,097例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另累計127例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$2月2日新增本土COVID-19確診個案表.pdf\$\@\$2月2日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
     <t>發佈日期：2022-02-01\$\@\$中央流行疫情指揮中心今(1)日公布國內新增60例COVID-19確定病例，分別為16例本土個案及44例境外移入(7例為航班落地採檢陽性)；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為7例男性、9例女性，年齡介於未滿5歲至60多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為33例男性、11例女性，年齡介於未滿5歲至50多歲，分別自馬來西亞(20例)、美國(6例)、英國(3例)、日本(2例)、波蘭、菲律賓、越南、巴西、印度、巴拿馬、瑞典及法國(各1例)移入；另5例調查中。入境日介於今(2022)年1月17日至1月31日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,684,887例新型冠狀病毒肺炎相關通報(含5,665,865例排除)，其中18,850例確診，分別為3,715例境外移入，15,081例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；另累計127例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$2月1日新增本土COVID-19確診個案表.pdf\$\@\$2月1日新增境外移入COVID-19確診個案表.pdf</t>
   </si>
   <si>
     <t>發佈日期：2022-01-31\$\@\$中央流行疫情指揮中心今(31)日公布國內新增55例COVID-19確定病例，分別為17例本土個案及38例境外移入(20例為航班落地採檢陽性)；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為8例男性、9例女性，年齡介於未滿10歲至80多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為26例男性、12例女性，年齡介於未滿10歲至70多歲，分別自美國(19例)、中國(2例)、厄瓜多、日本、巴拿馬、比利時、韓國、越南及沙烏地阿拉伯各1例移入；另10例調查中。入境日介於今(2022)年1月14日至1月30日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,673,543例新型冠狀病毒肺炎相關通報(含5,654,537例排除)，其中18,790例確診，分別為3,671例境外移入，15,065例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計127例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月31日新增境外移入COVID-19確診個案表.pdf\$\@\$1月31日新增本土COVID-19確診個案表.pdf</t>
   </si>
   <si>
-    <t>發佈日期：2022-01-30\$\@\$鑒於近日本土COVID-19個案多具社區活動史，中央流行疫情指揮中心今（30）日再度說明接觸者匡列原則，亦提醒民眾提高警覺，如未被匡列但疑有可能接觸，主動篩檢。\$\@\$指揮中心指出，如有COVID-19確診個案，地方政府衛生單位人員即會依據相關作業流程前往執行疫情調查及接觸者匡列，以釐清相關活動史與接觸者，必要時由警政單位協助調查個案活動軌跡。衛生單位針對確診個案於可傳染期間參與之各項活動，皆會進行詳細疫調，並依接觸時間及有無適當防護之條件等，評估所有可能接觸人員感染風險後，進行接觸者名單匡列，並通知該等人員依循衛生機關規定執行居家隔離、自主健康管理或自我健康監測等各項防疫措施。\$\@\$指揮中心表示，密切接觸者之隔離措施自110年5月16日起即以1人1室為原則，惟經指揮中心專案核定、地方政府報經指揮中心同意或經地方政府衛生單位評估家中環境不適合者(如：居家隔離者無法有獨立的房間及廁所、住家環境有受病毒汙染之虞且難以即時確實清消，可能有環境汙染造成疾病傳播之風險等)，可公費送集中檢疫所隔離。隔離措施為阻絕病毒傳播重要方法，籲請民眾務必配合、遵守相關規範，共同維護社區安全。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-30\$\@\$中央流行疫情指揮中心今(30)日公布國內新增54例COVID-19確定病例，分別為14例本土個案及40例境外移入(8例為航班落地採檢陽性)；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為6例男性、8例女性，年齡介於未滿10歲至60多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為21例男性、19例女性，年齡介於未滿5歲至60多歲，分別自美國(8例)、英國(5例)、中國(4例)、越南(3例)、柬埔寨(2例)、澳大利亞、香港、法國、日本、南非、菲律賓、加拿大及匈牙利(各1例)移入；另10例調查中。入境日介於今(2022)年1月14日至1月29日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,659,833例新型冠狀病毒肺炎相關通報(含5,640,850例排除)，其中18,735例確診，分別為3,633例境外移入，15,048例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；無新增空號病例，累計127例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月30日新增本土COVID-19確診個案表.pdf\$\@\$1月30日新增境外移入COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-29\$\@\$中央流行疫情指揮中心今(29)日表示，因應國際COVID-19疫情嚴峻及Omicron等新型變異株於國內社區流行風險，自去(2021)年8月30日起啟動各項COVID-19加強監測方案，及時偵測國內病例阻斷傳播鏈，截至本(2022)年1月22日辦理情形如下：\$\@\$一、社區加強監測：\$\@\$於全國21個縣市共計274家基層定點診所，發放公費COVID-19家用快篩試劑，由醫師評估對於具呼吸道症狀民眾發放試劑，再由民眾居家篩檢及回報快篩結果。累計發放17,834劑，其中1人後續經PCR檢驗研判為確定病例，呼籲民眾如出現呼吸道症狀，請善加利用此機制至公費快篩試劑發放診所掛號就醫。\$\@\$二、國際機場/國際海港特定高風險工作人員重點監測：\$\@\$於桃園、臺北、臺中與高雄等4個國際機場及12處國際商港、工業港及離島兩岸通航(小三通)港口之特定高風險工作人員，每7天以公費家用快篩試劑採檢一次。累計檢測80,456人次，其中2人快篩陽性後經PCR檢驗研判為確定病例。\$\@\$三、廢汙水監測：\$\@\$持續辦理全國汙水SARS-CoV-2病毒監測，由11處監測站累計採檢176件汙水檢體，SARS-CoV-2病毒核酸檢測均為陰性。\$\@\$四、邊境進口冷凍食品包裝監測：\$\@\$持續於邊境採樣檢驗進口冷凍肉品、水產品及水果之內、外包裝，監控進口冷凍食品內、外包裝之SARS-CoV-2病毒污染狀況，累計抽驗30個國家之253批產品，共978件樣品，SARS-CoV-2病毒核酸檢測均為陰性。\$\@\$五、捐血人血清抗體陽性盛行率調查：\$\@\$針對去年4至7月份我國捐血中心捐血人之血液存檔樣本，已完成抽樣5,000支檢體進行抗體檢測，僅1支檢體抗核蛋白(N)抗體及抗棘蛋白(S)抗體檢測結果皆為陽性，陽性率為0.02%，整體自然感染陽性率低，與該區間同年齡層確診率相當，本次調查未發現大量未診斷之潛在病例。\$\@\$指揮中心強調，為因應Omicron新型變異株威脅，及維護國內社區安全，將持續強化邊境與社區監測等各項防疫作為，及早發現可能病例，阻斷傳播鏈，並依據疫情態勢，適度調整加強監測方案。</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-28\$\@\$中央流行疫情指揮中心今(28)日公布國內新增71例COVID-19確定病例，分別為27例本土個案及44例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為8例男性、19例女性，年齡介於未滿10歲至60多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為25例男性、19例女性，年齡介於未滿5歲至70多歲，分別自美國及菲律賓各8例、中國5例、印尼3例、日本、瑞典及越南各2例、孟加拉國、荷蘭、土耳其、英國、奧地利及丹麥各1例移入；另8例調查中。入境日介於今(2022)年1月13日至1月27日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,613,922例新型冠狀病毒肺炎相關通報(含5,594,976例排除)，其中18,634例確診，分別為3,561例境外移入，15,019例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增3例空號病例(案18314境外移入、案18425本土、案18438本土，再次採檢為陰性，共3案研判排除)，累計126例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月28日新增境外移入COVID-19確診個案表.pdf\$\@\$1月28日新增本土COVID-19確診個案表.pdf</t>
-  </si>
-  <si>
-    <t>發佈日期：2022-01-27\$\@\$中央流行疫情指揮中心今(27)日公布國內新增64例COVID-19確定病例，分別為21例本土個案及43例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為11例男性、10例女性，年齡介於未滿5歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為21例男性、22例女性，年齡介於未滿5歲至60多歲，分別自美國(14例)、印度(3例)、越南、印尼、英國及法國(各2例)、衣索比亞、坦尚尼亞、新加坡、土耳其、菲律賓、南非、芬蘭、日本(各1例)移入；另10例調查中。入境日介於去(2021)年5月2日至今(2022)年1月26日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,581,517例新型冠狀病毒肺炎相關通報(含5,562,679例排除)，其中18,566例確診，分別為3,518例境外移入，14,994例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案18418，再次採檢為陰性，改判排除)，累計123例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月27日新增本土COVID-19確診個案表.pdf\$\@\$1月27日新增境外移入COVID-19確診個案表.pdf</t>
+    <t>發佈日期：2022-01-29\$\@\$中央流行疫情指揮中心今(29)日公布國內新增48例COVID-19確定病例，分別為15例本土個案及33例境外移入；另確診個案中無新增死亡。\$\@\$指揮中心表示，今日新增本土個案為5例男性、10例女性，年齡介於未滿10歲至70多歲；詳如新聞稿附件。\$\@\$指揮中心說明，今日新增境外移入個案為19例男性、14例女性，年齡介於20多歲至70多歲，分別自美國(9例)、阿拉伯聯合大公國及新加坡(各2例)、日本、中國、澳大利亞、越南、墨西哥及荷蘭(各1例)移入；另14例調查中。入境日介於今(2022)年1月9日至1月28日；詳如新聞稿附件。\$\@\$指揮中心統計，截至目前國內累計5,640,594例新型冠狀病毒肺炎相關通報(含5,621,502例排除)，其中18,681例確診，分別為3,593例境外移入，15,034例本土病例，36例敦睦艦隊、3例航空器感染、1例不明及14例調查中；新增1例空號病例(案18315境外移入病例，再次採檢為陰性，改判排除)，累計127例移除為空號。2020年起累計851例COVID-19死亡病例，其中838例本土，個案居住縣市分布為新北市413例、臺北市322例、基隆市29例、桃園市27例、彰化縣15例、新竹縣13例、臺中市5例、苗栗縣3例、宜蘭縣及花蓮縣各2例，新竹市、南投縣、雲林縣、臺南市、高雄市、屏東縣及臺東縣各1例；另13例為境外移入。\$\@\$指揮中心再次呼籲，民眾應落實手部衛生、咳嗽禮節及佩戴口罩等個人防護措施，減少不必要移動、活動或集會，避免出入人多擁擠的場所，或高感染傳播風險場域，並主動積極配合各項防疫措施，共同嚴守社區防線。 附件\$\@\$1月29日新增本土COVID-19確診個案表.pdf\$\@\$1月29日新增境外移入COVID-19確診個案表.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-07-10\$\@\$中央流行疫情指揮中心今（10）日表示，近日有網友散布「三級警戒微解封的不可思議之處，新冠肺炎病毒只會攻擊家人」等訊息，相關內容多有誤導，且在錯誤基礎上進行不當類比，指揮中心再次強調，相關防疫指引已清楚說明，原本同住家人可以繼續維持生活，相關指引都是針對日常非同住者間的行為互動加以規範，呼籲民眾勿輕信或隨意散播、轉傳錯誤訊息，造成防疫困擾。\$\@\$指揮中心指出，有關7月13號以後針對部分場所將適度鬆綁，但仍須遵守防疫相關指引及規範，而此波疫情中，不少個案均為家戶群聚感染，由於室內密切接觸風險較高，因此對於室內社交人數須有較嚴格規範，但不包含原本同住的家人，也無需限制同住家人不能在家打麻將、看電影、吃飯等。 圖片 附件\$\@\$0710指揮中心：勿輕信「三級警戒微解封的不可思議之處」之網傳.jpg</t>
   </si>
   <si>
     <t>發佈日期：2021-06-13\$\@\$近日有網友在臉書FB以自製圖文方式散布「政府讓人民施打未受認證且保護力低之國產疫苗」、「國產疫苗的中和抗體效價比國外疫苗差」、「國產疫苗為什麼不向國際提出緊急授權」，中央流行疫情指揮中心(下稱指揮中心)今（13）日嚴正澄清表示，目前國產疫苗臨床試驗尚在進行中，最終結果須等廠商提出EUA 申請，經專家會議審查疫苗的製程管控、藥毒理試驗及臨床試驗結果，在緊急公衛的需求下，確認疫苗使用效益大於風險，才會核准緊急授權使用。\$\@\$指揮中心指出，目前國產疫苗廠商皆已積極規劃，以取得國際認證為目標。國產疫苗需經食藥署和專家會議嚴謹審查，在緊急公衛需求，並確認效益大於風險，才會核准緊急授權使用。此外，各家廠牌的疫苗所使用的檢驗實驗室及檢驗方式不同且無協和，無法直接由各實驗室產生數值進行比較。國產疫苗仍需等廠商提出申請，經過中央主管機關嚴格把關及審查通過後，確認品質、安全、療效後，品質沒有問題，疫苗方可供民眾施打。\$\@\$指揮中心再次提醒，民眾接獲來源不明的訊息時，應先進行查證，切勿隨意散播、轉傳，以免觸法。 圖片 附件\$\@\$0613網傳「政府讓人民施打未受認證且保護力低之國產疫苗」-1.jpg\$\@\$0613網傳「政府讓人民施打未受認證且保護力低之國產疫苗」-2.jpg</t>
   </si>
   <si>
-    <t>發佈日期：2021-06-01\$\@\$中央流行疫情指揮中心今(1)日指出，近日有網友在通訊軟體LINE散布「臺中市太原路復健醫院被徵收為方艙醫院」，臺中市政府衛生局已澄清為不實訊息，請民眾勿再轉傳與散布，以免觸法遭罰。\$\@\$指揮中心表示，臺中市政府已對外澄清，此復健醫院近期進行搬遷作業，是為了提升醫療品質，正以BOT方式規劃市立綜合醫院，並非徵用作為方艙醫院。\$\@\$指揮中心副指揮官陳宗彥指出，因應疫情變化，各地方政府規劃應變醫院及專責醫院收治患者，民眾接獲來源不明的訊息時，應先進行查證，切勿隨意散播、轉傳，以免觸法。\$\@\$指揮中心重申，防疫相關資訊應以中央流行疫情指揮中心公布內容為主，散播假訊息構成犯罪，會被判處最高三年有期徒刑或併科三百萬元罰金。提醒民眾，收到來路不明訊息多加留意、查證，切勿轉傳散播，以免觸法。詳情請上官網查詢(http://at.cdc.tw/Q7S2Vt)。 圖片 附件\$\@\$網傳「臺中市太原路復健醫院被徵收為方艙醫院」為不實訊息勿轉傳.jpg\$\@\$勿散播不實訊息，以免觸法受罰.jpg</t>
+    <t>發佈日期：2021-06-12\$\@\$中央流行疫情指揮中心今(12)日嚴正澄清，近日於社群平台流傳「代工三億劑嫌太多賣不出去」等訊息，指揮中心於6月10日記者會已公開說明，與AstraZeneca原廠洽談授權製造事宜時，我方提出可年產一億劑之規劃，但原廠要求需年產三億劑，經評估，對我方產能過於沉重，並無以「賣不出去」為由拒絕原廠授權製造，卻被有心人刻意扭曲語意。此圖文與事實不符，指揮中心特此澄清。\$\@\$指揮中心重申，防疫相關資訊應以中央流行疫情指揮中心公布內容為主。提醒民眾，收到來路不明訊息多加留意、查證，切勿轉傳散播。詳情請上官網查詢 (http://at.cdc.tw/Q7S2Vt)。 圖片 附件\$\@\$20210612澄清.jpg</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-05-28\$\@\$近期國內疫情升溫，警方發現網路上有不肖人士販售「新冠病毒快篩試劑」，中央流行疫情指揮中心副指揮官陳宗彥今(28)日表示，擅自在網路販售新冠病毒檢驗試劑等第三級醫療器材已違反「醫療器材管理法」，目前警方已進行偵辦，提醒民眾切勿購買檢測，除有效性及檢測結果正確性均無法確認外，還可能危害自身健康。\$\@\$指揮中心指出，新冠病毒檢驗試劑是第三級醫療器材，依據「醫療器材管理法」規定，只有醫療器材商及藥局可以販賣，且國內並未開放可使用通訊方式在網路、電話、社群媒體等販售。\$\@\$指揮中心強調，不肖人士在網路擅自販售專案核准的新冠病毒檢驗試劑已違「醫療器材管理法」，會被罰3萬以上100萬以下罰鍰，如果民眾發現有類似狀況，可打1919專線或是向地方衛生局檢舉。 圖片 附件\$\@\$0528網路販售「新冠病毒快篩試劑」已觸法，警方偵辦中.jpg\$\@\$勿散播不實訊息，以免觸法受罰.jpg</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-05-25\$\@\$中央流行疫情指揮中心今(25)日表示，近日網路出現偽冒教育部網站，杜撰「全國各級學校因應疫情停課時程資訊」等訊息，意圖造成民眾困惑，此為境外假網頁不實訊息，請民眾勿輕信。\$\@\$指揮中心副指揮官陳宗彥表示，該網站假冒教育部傳達不實防疫訊息，刑事警察局已成立專案小組偵辦，經調查其為境外IP。\$\@\$指揮中心指出，教育部全球資訊網正確的網址是https://www.edu.tw/ ，民眾收到任何連結時，可以先觀察連結網址，是否跟官方網址一樣。例如，教育部官方網址的網域，就會是「edu.tw」結尾。\$\@\$指揮中心強調，散播假訊息構成犯罪，會被判處最高三年有期徒刑或併科三百萬元罰金。提醒民眾，收到來路不明訊息多加留意、查證，切勿轉傳散播，以免觸法。 圖片 附件\$\@\$0525指揮中心指出，網路出現偽冒教育部網站並杜撰假訊息，請民眾勿輕信.jpg\$\@\$勿散播不實訊息，以免觸法受罰.jpg</t>
   </si>
   <si>
     <t>發佈日期：2022-01-28\$\@\$各位醫界朋友，您好：\$\@\$全球疫情持續嚴峻，Omicron變異株現已為全球與國內主要流行病毒株，由於其具有多個基因變異位點，可能影響部分治療藥物效果，COVID-19專家諮詢會審視國內外最新實證後，統整對Omicron變異株藥物使用建議如下：\$\@\$1. 不需使用氧氣且具重症風險因子之COVID-19病患：\$\@\$(1)建議可使用remdesivir靜脈注射三日療程，或nirmatrelvir + ritonavir (Paxlovid)口服五日，未住院病患建議優先選擇口服藥物治療。若上述兩種藥物均不適用，則可使用molnupiravir (Lagevrio)口服五日。臨床醫師可評估病患情況後，依本署公告之領用方案及注意事項申請使用；另因缺乏實證與安全性資料，不建議同時併用remdesivir和口服抗病毒藥物。\$\@\$(2)我國目前儲備之兩種複合式anti-SARS-CoV-2單株抗體(casirivimab + imdevimab, bamlanivimab + etesevimab)，因體外試驗顯示對Omicron變異株中和能力大幅下降，可能影響臨床效果，故除非已確認上述單株抗體對患者感染之變異株仍有效，否則不建議使用，使用前務必參閱最新版「新型冠狀病毒（SARS-CoV-2）感染臨床處置暫行指引」中「單株抗體對SARS-CoV-2變異株效果實證」表格。\$\@\$2.需吸氧治療、高流量氧氣、非侵襲性呼吸器或插管病患：\$\@\$目前證據顯示，Omicron變異株不影響dexamethasone、tocilizumab、baricitinib與remdesivir對此類病人之療效，故維持現行治療建議。\$\@\$面對社區疫情，指揮中心提醒臨床醫師提高警覺，對有疑似症狀患者加強採檢，以早期偵測疫情。另目前針對不同嚴重程度COVID-19病患均已有治療藥物可選用，用藥前請參閱最新版「新型冠狀病毒（SARS-CoV-2）感染臨床處置暫行指引」中個別藥物說明。\$\@\$「嚴重特殊傳染性肺炎」之診療相關資訊將隨時依防疫需求與最新文獻證據更新並公布於疾病管制署全球資訊網(http://www.cdc.gov.tw)。\$\@\$感謝您與我們共同維護全民的健康安全。 附件\$\@\$診治指引表四＿我國診治指引對SARS-CoV-2確診病患用藥建議彙整.pdf\$\@\$診治指引表五＿單株抗體對SARS-CoV-2變異株效果實證.pdf</t>
@@ -424,13 +424,28 @@
     <t>發佈日期：2022-01-26\$\@\$各位醫界朋友，您好：\$\@\$為積極因應新型冠狀病毒疾病疫情防疫需求，衛生福利部食品藥物管理署於評估療效、安全性、風險效益與緊急公共衛生需求後，於本(111)年1月12日與1月15日分別核准兩種口服抗病毒藥物專案輸入，經COVID-19專家諮詢會檢視最新實證後，於臨床處置暫行指引中新增口服抗病毒藥物使用建議如下：\$\@\$新增nirmatrelvir + ritonavir(Paxlovid)適用對象為具以下任一重症風險因子，未使用氧氣且於發病五天內之 ≧ 12歲且體重 ≧ 40公斤病患；風險因子包括年齡 ≧ 65歲、糖尿病、慢性腎病、心血管疾病(含高血壓)、慢性肺疾、BMI ≧ 25 (或12-17歲兒童青少年BMI 超過同齡第85百分位)、其他影響免疫功能之疾病或已知重症風險因子者。建議劑量為Nirmatrelvir 300 mg + ritonavir 100 mg 每日兩次口服，療程共五天。使用時須特別注意藥物交互作用及肝腎功能異常時之建議，並確實完成五天療程。\$\@\$新增molnupiravir(Lagevrio)適用對象為具以下任一重症風險因子，未使用氧氣且於發病五天內之 ≧ 18歲病患，且無法使用其他建議藥物者；風險因子包括年齡 ≧ 65歲、糖尿病、慢性腎病、心血管疾病(含高血壓)、慢性肺疾、BMI ≧ 25、其他影響免疫功能之疾病或已知重症風險因子者。建議劑量為molnupiravir 800mg每日兩次口服，療程共五天。\$\@\$目前針對未使用氧氣且具重症風險因子之COVID-19病患，專家諮詢小組建議可使用藥物包括remdesivir、nirmatrelvir + ritonavir與兩種複合式anti-SARS-CoV-2單株抗體(casirivimab + imdevimab, bamlanivimab + etesevimab)，臨床醫師可評估病患病況與變異株流行情形後，依本署公告流程申請使用；若病患不適用上述藥物，則可申請使用molnupiravir。\$\@\$「嚴重特殊傳染性肺炎」之診療相關資訊將隨時依防疫需求與最新文獻證據更新並公布於疾病管制署全球資訊網(http://www.cdc.gov.tw)。\$\@\$感謝您與我們共同維護全民的健康安全。 附件\$\@\$附件1＿新型冠狀病毒（SARS-CoV-2）感染臨床處置暫行指引第十六版.pdf\$\@\$附件2_公費COVID-19治療用口服抗病毒藥物領用方案_1110126制定.pdf</t>
   </si>
   <si>
+    <t>發佈日期：2022-01-06\$\@\$為提供結核病患即時診斷，疾病管制署結核病診治指引自104年已加重結核分枝桿菌核酸增幅(nucleic acid amplification, NAA)檢驗於診斷結核病之角色。NAA檢驗具快速、高敏感度及高特異性，可大幅縮短傳統培養檢驗方法所需等待結果時間，有利及早診斷及治療結核病。\$\@\$因應近期結核菌液態培養(MGIT)檢驗發生添加劑(營養劑併抑制細菌生長的抗生素成分)供貨短缺情形，為避免延遲發現疑似結核病個案，依本署110年12月24日「衛生福利部傳染病防治諮詢會(結核病防治組)」會議決議，於供貨短缺期間，對於社區型肺炎尚未通報結核病者，於診斷送驗3套初查痰執行塗片耐酸性染色鏡檢(Acid fast stain)及分枝桿菌培養時，其中1套請務必同時開立NAA檢驗。另考量實驗室短期內MGIT痰培養試劑有限，對於管理中的結核病患追蹤複查痰，請採1套進行培養檢驗，暫時避免重複送驗檢體，此因應作為停止施行時間將於缺貨狀況緩解後再函週知。\$\@\$有關「結核病診治指引」可至疾病管制署全球資訊網(https://www.cdc.gov.tw)&gt;傳染病與防疫專題&gt;傳染病介紹&gt;第三類定傳染病&gt;結核病&gt;重要指引及教材項下查閱。\$\@\$感謝您與我們共同維護全民的健康安全。</t>
+  </si>
+  <si>
     <t>發佈日期：2022-01-06\$\@\$各位醫界朋友，您好：\$\@\$新型冠狀病毒(SARS-CoV-2)國際疫情嚴峻，Omicron變異株迅速擴散。由於變異株變異位點可能影響抗SARS-CoV-2單株抗體療效，治療指引自第十五版起新增「單株抗體對SARS-CoV-2變異株效果實證」附表，供臨床醫師用藥時參考。另COVID-19專家諮詢會檢視最新實證後，更新治療指引藥物適用原則如下：\$\@\$新增remdesivir適用對象為具以下任一風險因子，未使用氧氣且於發病七天內之≧12歲且體重≧40公斤病患；風險因子包括年齡≧65歲、糖尿病、慢性腎病、心血管疾病(含高血壓)、慢性肺疾、BMI≧25 (或12–17歲兒童青少年BMI 超過同齡第85百分位)、懷孕、其他影響免疫功能之疾病或已知重症風險因子者。建議劑量為第一天200 mg靜脈注射，第二至三天100 mg，療程共三天。\$\@\$維持現行抗SARS-CoV-2複合單株抗體(Casirivimab + imdevimab或Bamlanivimab + etesevimab)適用對象建議，但由於體外試驗顯示上述兩種抗SARS-CoV-2複合單株抗體可能無法有效中和包括Beta、Gamma、Delta plus、Mu與Omicron變異株，建議臨床醫師使用時需考量流行狀況與參閱指引內最新版「單株抗體對SARS-CoV-2變異株效果實證」附表。\$\@\$面對冬季疫情，指揮中心提醒臨床醫師提高警覺，對有疑似症狀患者加強採檢，以早期偵測疫情。另目前針對不同嚴重程度COVID-19病患均已有治療藥物可選用，可依臨床狀況給予最妥善治療。\$\@\$「嚴重特殊傳染性肺炎」之診療相關資訊將隨時依防疫需求與最新文獻證據更新並公布於疾病管制署全球資訊網(http://www.cdc.gov.tw)。\$\@\$感謝您與我們共同維護全民的健康安全。 附件\$\@\$新型冠狀病毒（SARS-CoV-2）感染臨床處置暫行指引第十五版.pdf\$\@\$附表SARS-CoV-2之藥物使用實證摘要_20211230更新.pdf\$\@\$公費COVID-19治療用單株抗體領用方案.pdf\$\@\$公費COVID-19抗病毒藥劑VEKLURYR領用方案1110106第6版.pdf</t>
   </si>
   <si>
+    <t>發佈日期：2021-12-30\$\@\$各位醫界朋友，您好：\$\@\$鑑於國際COVID-19疫情嚴峻及Omicron新型變異株威脅增加，嚴重特殊傳染性肺炎中央流行疫情指揮中心(下稱指揮中心)邀請各縣市兒科、內科、家醫科、耳鼻喉科及婦產科等有提供診治呼吸道症狀服務之診所/衛生所，自明(2022)年1月1日起加入公費COVID-19家用快篩試劑發放行列，指揮中心感謝基層診所積極守護社區健康的熱誠，並籲請各定點診所醫師針對具呼吸道症狀就醫民眾，加強發放公費COVID-19家用快篩試劑。\$\@\$指揮中心於今(2021)年8月30日起啟動前揭計畫，全國共計18個縣市86家診所/衛生所參加，迄今已發放1萬餘劑公費COVID-19家用快篩試劑，於有效監測下均無發現陽性個案。為提升民眾取用COVID-19家用快篩試劑可近性及擴大監測，自明年1月1日起增加至21個縣市272家診所/衛生所參與。\$\@\$由於國內現處於流感季節且COVID-19症狀與上呼吸道感染症狀相似，指揮中心籲請定點診所針對出現呼吸道症狀就醫民眾，加強發放公費COVID-19家用快篩試劑，尤可對於幼兒及其陪病家屬加強評估發放；另請診所衛教民眾試劑使用流程及注意事項、提醒民眾匿名填寫線上問卷以回報快篩結果等資料，並將發放民眾資料登錄於疾病管制署系統中。\$\@\$該計畫相關內容公布於疾病管制署全球資訊網 (http://www.cdc.gov.tw) COVID-19防疫專區&gt;臺灣社交距離APP及採檢地圖&gt;COVID-19社區加強監測方案，歡迎查閱。\$\@\$感謝您與我們共同維護全民的健康安全。</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-10-22\$\@\$各位醫界朋友，您好：\$\@\$我國新型冠狀病毒(SARS-CoV-2)感染臨床處置暫行指引建議可依照病患病程與嚴重度，對不需用氧且有重症風險因子之病患給予單株抗體，需用氧病患則除dexamethasone外可併用免疫調節劑tocilizumab或baricitinib。鑒於近期國際間藥物使用建議與國內適應症均有更新，經COVID-19專家諮詢會議更新建議如下：\$\@\$1.複合單株抗體Casirivimab + imdevimab或Bamlanivimab + etesevimab。適用對象為\$\@\$― 具以下任一風險因子，未使用氧氣且於發病十天內之≧12歲且體重≧40公斤病患；\$\@\$― 風險因子包括：年齡 ≧ 65歲、糖尿病、慢性腎病、心血管疾病（含高血壓）、慢性肺疾、BMI ≧25（或12-17歲兒童BMI超過同齡第85百分位）、懷孕、其他影響免疫功能之疾病或已知重症風險因子等。\$\@\$目前實證顯示上述兩種複合單株抗體對國內現今主要檢出之Delta與Alpha變異株均有效，但由於體外試驗顯示Bamlanivimab + etesevimab可能無法有效中和包括Beta、Gamma、Delta plus與Mu變異株，建議臨床醫師使用時需考量流行狀況與參閱最新版「SARS-CoV-2之藥物使用實證摘要」附表。\$\@\$另參考WHO最新公布治療建議，於診治指引註解中新增「隨機對照研究顯示對血清抗體陰性之嚴重肺炎以上程度病患，除標準治療外，給予casirivimab 4000mg + imdevimab 4000mg 可降低死亡率」。\$\@\$2.Remdesivir適用對象為嚴重肺炎以上（未使用吸氧治療下的SpO2 ≦ 94%、需使用吸氧治療、需使用高流量氧氣或非侵襲性呼吸器但未插管）病患。另於診治指引註解中新增「若住院病患胸部X光片顯示肺炎，雖未達重症標準且不符合單株抗體適用條件，仍可申請使用remdesivir」。但由於目前尚無併用單株抗體之效益與安全性資料，目前仍暫不建議remdesivir與單株抗體同時併用。\$\@\$由於近日媒體報導ivermectin用於治療COVID-19一事，經專家委員審視國際文獻，發現ivermectin相關臨床試驗研究證據力等級低，且部分研究涉及科學誠信，其中亦有發表論文被撤回之情形，統合分析結果顯示目前證據不支持ivermectin可用於治療或預防COVID-19，WHO及歐美等具公信力之治療指引均不建議使用於COVID-19之治療。為確保國人健康，我國診治指引治療藥物建議係根據最高等級實證基礎制訂，參考目前各方面之資料，仍不建議ivermectin納入我國診治指引之治療建議藥物。\$\@\$「嚴重特殊傳染性肺炎」之診療相關資訊將隨時依防疫需求與最新文獻證據更新並公布於疾病管制署全球資訊網(http://www.cdc.gov.tw)。\$\@\$感謝您與我們共同維護全民的健康安全。</t>
+  </si>
+  <si>
     <t>發佈日期：2022-01-28\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$疫情中心\$\@\$約用助理\$\@\$(徵才案號：0605，含延長公告)\$\@\$(計4名)\$\@\$姚○雯(A22649****)\$\@\$盧○淳(A22626****)\$\@\$邱○柔(A22582****)\$\@\$莊○媛(R22426****)\$\@\$二、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一)口試：\$\@\$1、報到時間：111年02月09日星期三15:20~15:30，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署1樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：15:30~17:00。\$\@\$(二)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(三)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於111年02月09日上午10點前主動以電子郵件或電話通知人事室陳小姐(yuan_c@cdc.gov.tw、電話02-23959825分機3864)，俾利安排應試座位。\$\@\$(四)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(五)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
   </si>
   <si>
     <t>發佈日期：2022-01-13\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$急性傳染病組\$\@\$約用助理\$\@\$(徵才案號：1106，含延長公告)\$\@\$(計1名)\$\@\$張○純(A22889****)\$\@\$二、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一) 口試：\$\@\$1、報到時間：111年01月17日星期一15:20~15:30，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署7樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：16:40~17:10。\$\@\$(二)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(三)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於111年01月17日上午10點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3823)，俾利安排應試座位。\$\@\$(四)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(五)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2022-01-12\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$檢疫組\$\@\$約用助理\$\@\$(徵才案號：0507)\$\@\$(計4名)\$\@\$陳○涵(A22534****)\$\@\$張○純(A22889****)\$\@\$林○翔(S12427****)\$\@\$謝○樺(K12260****)\$\@\$二、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一) 口試：\$\@\$1、報到時間：111年01月17日星期一15:20~15:30，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署7樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：15:30~16:40。\$\@\$(二)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(三)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於111年01月17日上午10點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3864)，俾利安排應試座位。\$\@\$(四)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(五)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
+  </si>
+  <si>
+    <t>發佈日期：2021-12-24\$\@\$一、考評單位：衛生福利部疾病管制署。\$\@\$二、考評目的：客觀衡量地方政府衛生局111年防疫業務之施政績效。\$\@\$三、受評機關：地方政府衛生局。\$\@\$四、受評期間：111年1月至12月\$\@\$五、考評架構與權重：9項考評指標，共計200分。\$\@\$六、考評方式：\$\@\$(一)   防疫業務相關管理系統之統計結果及書面考核。\$\@\$本手冊考評指標資料，如須受評機關提供始得評分者，請於112年1月13日前備函逕送考評執行單位進行評核。\$\@\$考評單位於指定日期前完成分數統計及成績評定。\$\@\$考評單位完成考評並請地方政府衛生局確認後，於111年3月17日前將考評結果送衛生福利部綜合規劃司備查。\$\@\$(二)   考評單位得視需要辦理實地查核。 附件\$\@\$111年地方衛生機關業務考評作業手冊-防疫類.pdf\$\@\$111年地方衛生機關業務考評作業手冊-防疫類.docx</t>
   </si>
   <si>
     <t>發佈日期：2021-12-24\$\@\$一、 書面審查合格名單：\$\@\$甄選單位(合格人數)\$\@\$合格人員(按報名順序排列)\$\@\$慢性傳染病組\$\@\$約用助理\$\@\$(徵才案號：0309)\$\@\$(計3名)\$\@\$林○萱(B22260****)\$\@\$陳○瑜(Q22389****)\$\@\$陳○君(F22674****)\$\@\$二、實作、口試相關資訊如下，請前揭應試人員預為準備：\$\@\$(一)實作：\$\@\$1、報到時間：111年1月7日星期五13:20。\$\@\$2、報到地點：衛生福利部疾病管制署1樓(臺北市中正區林森南路6號)。\$\@\$3、實作時間：13:40~15:10。實作開始鈴響(13:40)未到者，喪失應考資格。\$\@\$(二)口試：\$\@\$1、報到時間：111年1月7日星期五15:20，未準時報到者，喪失口試資格。\$\@\$2、報到地點：衛生福利部疾病管制署1樓(臺北市中正區林森南路6號)。\$\@\$3、口試時間：15:30~16:30。\$\@\$(三)為因應嚴重特殊傳染性肺炎，本次甄試請依「衛生福利部疾病管制署辦理甄試防疫措施指引(如附件1)」及中央流行疫情指揮中心發布之「具感染風險民眾追蹤管理機制」(如附件2)之相關規定辦理。報到時請繳交健康聲明切結書(如附件3)，並自備口罩全程配戴。進入試場前均需量測體溫，如有發燒(額溫≧37.5°C)，將安排至本署設置之隔離試場應試。\$\@\$(四)應試當日如屬經各級衛生主管機關認定應接受居家隔離者、居家檢疫者，以及屬自主健康管理期間，就醫後經醫院安排採檢，返家後尚未接獲檢驗結果前者，均請配合留在家中(或指定地點)勿至試場；如屬上述附件2「自主健康管理」者，請於111年1月6日下午5點前主動以電子郵件或電話通知人事室林小姐(swlin@cdc.gov.tw、電話02-23959825分機3823)，俾利安排應試座位。\$\@\$(五)應試當日如遇颱風等天然災害，臺灣本島任一縣市有依「天然災害停止上班及上課作業辦法」規定停止上班之情形，則延後辦理口試，並於1週內於公布更改之時間地點，請自行查閱，恕不另行通知。\$\@\$(六)請務必攜帶中華民國國民身分證或有照片之全民健康保險卡正本俾供查驗。\$\@\$三、試場規則：\$\@\$(一)第一試為實作測驗，題型為資料串接統計分析，應試者得自行攜帶筆記型電腦，並預先安裝欲於測驗時使用的統計分析軟體(可選擇使用SAS、R、Excel等其他統計分析軟體)；未自行攜帶筆記型電腦者，則由本署提供公務電腦於測驗時使用(僅具Excel功能且無法安裝軟體)。\$\@\$(二)測驗中途不容許離場，並於考試時間過半後始得離場，離場後不得再進入試場。\$\@\$(三)測驗期間不允許上網、隨身攜帶手機(含智慧手環)、行動網卡、無線網路分享器等電子用品，並請關閉網路、手機、聲音及振動(含鬧鐘)，考試過程中如有上網、發出聲音及震動，均喪失應考資格。\$\@\$(四)個人用品(如書包等)置於考場前後，桌面上僅可放置必要文具(墊板須為透明；水杯、飲料亦禁止放置)。\$\@\$(五)有下列各款情事之一者，予以扣考並不予計分或不得繼續應考：\$\@\$1、冒名頂替。\$\@\$2、持用偽造或變造之證件。\$\@\$3、互換座位或試卷。\$\@\$4、傳遞文稿、參考資料、書寫有關文字之物件或有關信號。\$\@\$5、夾帶書籍文件。\$\@\$6、故意不繳交試卷或破壞試卷彌封。\$\@\$7、在桌椅、文具或肢體上或其他處所，書寫有關文字。\$\@\$8、電子通訊舞弊行為。\$\@\$9、窺視他人試卷、答案卷、作答結果或互相交談。\$\@\$10、在答案卷上書寫姓名、座號或其他不應有之文字、標記或自備稿紙書寫。\$\@\$11、其他破壞試場秩序事項。 附件\$\@\$附件1-衛生福利部疾病管制署辦理甄試防疫措施指引.pdf\$\@\$附件2-具感染風險者追蹤管理機制表-1100514(掛網).pdf\$\@\$附件3-應試健康聲明書.pdf</t>
@@ -842,7 +857,7 @@
         <v>45</v>
       </c>
       <c r="C2" s="2">
-        <v>44593</v>
+        <v>44594</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>85</v>
@@ -859,13 +874,10 @@
         <v>46</v>
       </c>
       <c r="C3" s="2">
-        <v>44592</v>
+        <v>44594</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="E3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -876,13 +888,13 @@
         <v>47</v>
       </c>
       <c r="C4" s="2">
-        <v>44591</v>
+        <v>44593</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>87</v>
       </c>
       <c r="E4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -893,13 +905,13 @@
         <v>48</v>
       </c>
       <c r="C5" s="2">
-        <v>44591</v>
+        <v>44592</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>88</v>
       </c>
       <c r="E5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -924,7 +936,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="2">
-        <v>44590</v>
+        <v>44591</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>90</v>
@@ -938,13 +950,10 @@
         <v>51</v>
       </c>
       <c r="C8" s="2">
-        <v>44590</v>
+        <v>44591</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="E8" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -969,13 +978,10 @@
         <v>53</v>
       </c>
       <c r="C10" s="2">
-        <v>44589</v>
+        <v>44590</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="E10" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -986,13 +992,13 @@
         <v>54</v>
       </c>
       <c r="C11" s="2">
-        <v>44588</v>
+        <v>44590</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>94</v>
       </c>
       <c r="E11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1003,13 +1009,10 @@
         <v>45</v>
       </c>
       <c r="C12" s="2">
-        <v>44593</v>
+        <v>44594</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="E12" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1020,13 +1023,10 @@
         <v>46</v>
       </c>
       <c r="C13" s="2">
-        <v>44592</v>
+        <v>44594</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="E13" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1037,7 +1037,7 @@
         <v>47</v>
       </c>
       <c r="C14" s="2">
-        <v>44591</v>
+        <v>44593</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>87</v>
@@ -1051,13 +1051,13 @@
         <v>48</v>
       </c>
       <c r="C15" s="2">
-        <v>44591</v>
+        <v>44592</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>88</v>
       </c>
       <c r="E15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1082,7 +1082,7 @@
         <v>50</v>
       </c>
       <c r="C17" s="2">
-        <v>44590</v>
+        <v>44591</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>90</v>
@@ -1101,6 +1101,9 @@
       <c r="D18" s="3" t="s">
         <v>95</v>
       </c>
+      <c r="E18" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
@@ -1116,7 +1119,7 @@
         <v>96</v>
       </c>
       <c r="E19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1132,6 +1135,9 @@
       <c r="D20" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="E20" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
@@ -1146,9 +1152,6 @@
       <c r="D21" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E21" t="s">
-        <v>133</v>
-      </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
@@ -1163,6 +1166,9 @@
       <c r="D22" s="3" t="s">
         <v>99</v>
       </c>
+      <c r="E22" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
@@ -1177,6 +1183,9 @@
       <c r="D23" s="3" t="s">
         <v>100</v>
       </c>
+      <c r="E23" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
@@ -1225,6 +1234,9 @@
       <c r="D26" s="3" t="s">
         <v>103</v>
       </c>
+      <c r="E26" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
@@ -1240,7 +1252,7 @@
         <v>104</v>
       </c>
       <c r="E27" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1256,6 +1268,9 @@
       <c r="D28" s="3" t="s">
         <v>105</v>
       </c>
+      <c r="E28" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
@@ -1270,6 +1285,9 @@
       <c r="D29" s="3" t="s">
         <v>106</v>
       </c>
+      <c r="E29" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
@@ -1453,7 +1471,7 @@
         <v>119</v>
       </c>
       <c r="E42" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1470,7 +1488,7 @@
         <v>120</v>
       </c>
       <c r="E43" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1486,6 +1504,9 @@
       <c r="D44" s="3" t="s">
         <v>121</v>
       </c>
+      <c r="E44" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
@@ -1500,6 +1521,9 @@
       <c r="D45" s="3" t="s">
         <v>122</v>
       </c>
+      <c r="E45" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
@@ -1515,7 +1539,7 @@
         <v>123</v>
       </c>
       <c r="E46" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1532,7 +1556,7 @@
         <v>124</v>
       </c>
       <c r="E47" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>